<commit_message>
#86 scene move cell implememnt
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Scene.xlsx
+++ b/ConfigData/Xlsx/Scene.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\fish\Trunk\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="36" windowWidth="18132" windowHeight="8388"/>
   </bookViews>
   <sheets>
     <sheet name="Scene" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="43">
   <si>
     <t>村外小屋</t>
   </si>
@@ -148,6 +148,21 @@
   <si>
     <t>13000001|BornMapId</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TilePath</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>配置</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>default</t>
   </si>
 </sst>
 </file>
@@ -822,74 +837,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -902,9 +849,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:G20" totalsRowShown="0">
-  <autoFilter ref="A1:G20"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:H20" totalsRowShown="0">
+  <autoFilter ref="A1:H20"/>
+  <tableColumns count="8">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
     <tableColumn id="3" name="Level"/>
@@ -912,6 +859,7 @@
     <tableColumn id="5" name="WindowY"/>
     <tableColumn id="6" name="Func"/>
     <tableColumn id="7" name="Url"/>
+    <tableColumn id="8" name="TilePath"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -925,7 +873,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="CAEACD"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1204,21 +1152,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.125" customWidth="1"/>
-    <col min="4" max="5" width="9.75" customWidth="1"/>
-    <col min="6" max="6" width="45.125" customWidth="1"/>
-    <col min="10" max="10" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" customWidth="1"/>
+    <col min="4" max="5" width="9.77734375" customWidth="1"/>
+    <col min="6" max="6" width="45.109375" customWidth="1"/>
+    <col min="10" max="10" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -1240,8 +1188,11 @@
       <c r="G1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -1263,8 +1214,11 @@
       <c r="G2" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H2" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>22</v>
       </c>
@@ -1286,8 +1240,11 @@
       <c r="G3" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H3" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -1309,8 +1266,11 @@
       <c r="G4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>13000002</v>
       </c>
@@ -1329,8 +1289,11 @@
       <c r="G5">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>13000003</v>
       </c>
@@ -1349,8 +1312,11 @@
       <c r="G6">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>13010001</v>
       </c>
@@ -1369,8 +1335,11 @@
       <c r="G7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>13010004</v>
       </c>
@@ -1392,8 +1361,11 @@
       <c r="G8">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>13010005</v>
       </c>
@@ -1415,8 +1387,11 @@
       <c r="G9">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>13010006</v>
       </c>
@@ -1438,8 +1413,11 @@
       <c r="G10">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>13010007</v>
       </c>
@@ -1461,8 +1439,11 @@
       <c r="G11">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>13010008</v>
       </c>
@@ -1481,8 +1462,11 @@
       <c r="G12">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>13010009</v>
       </c>
@@ -1501,8 +1485,11 @@
       <c r="G13">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13010010</v>
       </c>
@@ -1524,8 +1511,11 @@
       <c r="G14">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13010011</v>
       </c>
@@ -1547,8 +1537,11 @@
       <c r="G15">
         <v>11</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>13010012</v>
       </c>
@@ -1567,8 +1560,11 @@
       <c r="G16">
         <v>12</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>13010013</v>
       </c>
@@ -1587,8 +1583,11 @@
       <c r="G17">
         <v>13</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>13010014</v>
       </c>
@@ -1607,8 +1606,11 @@
       <c r="G18">
         <v>14</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>13010015</v>
       </c>
@@ -1627,8 +1629,11 @@
       <c r="G19">
         <v>15</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>13010016</v>
       </c>
@@ -1646,6 +1651,9 @@
       </c>
       <c r="G20">
         <v>16</v>
+      </c>
+      <c r="H20" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
support the warp and quest
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Scene.xlsx
+++ b/ConfigData/Xlsx/Scene.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="44">
   <si>
     <t>村外小屋</t>
   </si>
@@ -163,6 +163,10 @@
   </si>
   <si>
     <t>default</t>
+  </si>
+  <si>
+    <t>home</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1155,7 +1159,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -1267,7 +1271,7 @@
         <v>2</v>
       </c>
       <c r="H4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix the map dark forest terrain
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Scene.xlsx
+++ b/ConfigData/Xlsx/Scene.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="50">
   <si>
     <t>村外小屋</t>
   </si>
@@ -182,6 +182,14 @@
   </si>
   <si>
     <t>42000003;3|42000002;1|42000004;2|42000005;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>42000006;2|42000007;1|42000008;2|42000003;2|42000004;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>darkforest</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1210,7 +1218,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1354,11 +1362,14 @@
       <c r="E5">
         <v>468</v>
       </c>
+      <c r="F5" t="s">
+        <v>48</v>
+      </c>
       <c r="H5">
         <v>3</v>
       </c>
       <c r="I5" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
finish scene quest magnetic
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Scene.xlsx
+++ b/ConfigData/Xlsx/Scene.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -178,18 +178,18 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>42000003;3|42000002;1|42000004;2|42000005;1|42000011;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>42000006;2|42000007;1|42000008;2|42000003;3|42000004;2|42000013;1</t>
+    <t>42000003;3|42000002;1|42000004;2|42000005;1|42000011;1|42000014;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>42000006;2|42000007;1|42000008;2|42000003;3|42000004;2|42000013;1|42000014;1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -888,7 +888,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -963,23 +963,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1015,23 +998,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1211,7 +1177,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
finish some new map
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Scene.xlsx
+++ b/ConfigData/Xlsx/Scene.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
   <si>
     <t>村外小屋</t>
   </si>
@@ -184,6 +184,15 @@
   <si>
     <t>GameUpToNumber;GameThreeBody;GameSeven</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>tatamuviliage</t>
+  </si>
+  <si>
+    <t>smallforest</t>
+  </si>
+  <si>
+    <t>farm</t>
   </si>
 </sst>
 </file>
@@ -1177,7 +1186,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1431,7 +1440,7 @@
         <v>6</v>
       </c>
       <c r="C10">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D10">
         <v>1127</v>
@@ -1443,7 +1452,7 @@
         <v>6</v>
       </c>
       <c r="I10" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.15">
@@ -1515,7 +1524,7 @@
         <v>9</v>
       </c>
       <c r="I13" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.15">
@@ -1587,7 +1596,7 @@
         <v>12</v>
       </c>
       <c r="I16" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
add some new map data
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Scene.xlsx
+++ b/ConfigData/Xlsx/Scene.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="56">
   <si>
     <t>村外小屋</t>
   </si>
@@ -193,6 +193,24 @@
   </si>
   <si>
     <t>farm</t>
+  </si>
+  <si>
+    <t>perse</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>demlock</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>hightower</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>smallhill</t>
+  </si>
+  <si>
+    <t>goldseashore</t>
   </si>
 </sst>
 </file>
@@ -1186,7 +1204,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1406,7 +1424,7 @@
         <v>4</v>
       </c>
       <c r="I8" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.15">
@@ -1429,7 +1447,7 @@
         <v>5</v>
       </c>
       <c r="I9" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.15">
@@ -1478,7 +1496,7 @@
         <v>7</v>
       </c>
       <c r="I11" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.15">
@@ -1547,7 +1565,7 @@
         <v>10</v>
       </c>
       <c r="I14" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
@@ -1619,7 +1637,7 @@
         <v>13</v>
       </c>
       <c r="I17" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
finish 2 new maps
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Scene.xlsx
+++ b/ConfigData/Xlsx/Scene.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="58">
   <si>
     <t>村外小屋</t>
   </si>
@@ -211,6 +211,12 @@
   </si>
   <si>
     <t>goldseashore</t>
+  </si>
+  <si>
+    <t>islandold</t>
+  </si>
+  <si>
+    <t>riverold</t>
   </si>
 </sst>
 </file>
@@ -1204,7 +1210,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1591,7 +1597,7 @@
         <v>11</v>
       </c>
       <c r="I15" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.15">
@@ -1660,7 +1666,7 @@
         <v>14</v>
       </c>
       <c r="I18" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
add 2 new scenes
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Scene.xlsx
+++ b/ConfigData/Xlsx/Scene.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="60">
   <si>
     <t>村外小屋</t>
   </si>
@@ -217,6 +217,14 @@
   </si>
   <si>
     <t>riverold</t>
+  </si>
+  <si>
+    <t>落潮小径</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>月光林地</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -903,8 +911,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:I20" totalsRowShown="0">
-  <autoFilter ref="A1:I20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:I22" totalsRowShown="0">
+  <autoFilter ref="A1:I22"/>
   <tableColumns count="9">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
@@ -1207,10 +1215,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1715,6 +1723,52 @@
         <v>39</v>
       </c>
     </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A21">
+        <v>13010017</v>
+      </c>
+      <c r="B21" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21">
+        <v>31</v>
+      </c>
+      <c r="D21">
+        <v>1038</v>
+      </c>
+      <c r="E21">
+        <v>459</v>
+      </c>
+      <c r="H21">
+        <v>18</v>
+      </c>
+      <c r="I21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A22">
+        <v>13010018</v>
+      </c>
+      <c r="B22" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22">
+        <v>31</v>
+      </c>
+      <c r="D22">
+        <v>723</v>
+      </c>
+      <c r="E22">
+        <v>327</v>
+      </c>
+      <c r="H22">
+        <v>19</v>
+      </c>
+      <c r="I22" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
finish the others mapdata
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Scene.xlsx
+++ b/ConfigData/Xlsx/Scene.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="66">
   <si>
     <t>村外小屋</t>
   </si>
@@ -27,9 +27,6 @@
     <t>昏暗密林</t>
   </si>
   <si>
-    <t>矿坑通道</t>
-  </si>
-  <si>
     <t>精灵之都-卡莱</t>
   </si>
   <si>
@@ -225,6 +222,28 @@
   <si>
     <t>月光林地</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>gerdin</t>
+  </si>
+  <si>
+    <t>fogvalley</t>
+  </si>
+  <si>
+    <t>矿脉山脚</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>riverside</t>
+  </si>
+  <si>
+    <t>orevalley</t>
+  </si>
+  <si>
+    <t>woodviliage</t>
+  </si>
+  <si>
+    <t>moonforest</t>
   </si>
 </sst>
 </file>
@@ -1218,7 +1237,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1232,94 +1251,94 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>31</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" t="s">
         <v>32</v>
       </c>
-      <c r="F1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>33</v>
       </c>
-      <c r="H1" t="s">
-        <v>34</v>
-      </c>
       <c r="I1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="C2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="H2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="I3" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -1334,16 +1353,16 @@
         <v>499</v>
       </c>
       <c r="F4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H4">
         <v>2</v>
       </c>
       <c r="I4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.15">
@@ -1363,13 +1382,13 @@
         <v>468</v>
       </c>
       <c r="F5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H5">
         <v>3</v>
       </c>
       <c r="I5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.15">
@@ -1377,7 +1396,7 @@
         <v>13000003</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>61</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1392,7 +1411,7 @@
         <v>17</v>
       </c>
       <c r="I6" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.15">
@@ -1400,7 +1419,7 @@
         <v>13010001</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -1415,7 +1434,7 @@
         <v>1</v>
       </c>
       <c r="I7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.15">
@@ -1423,7 +1442,7 @@
         <v>13010004</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8">
         <v>11</v>
@@ -1438,7 +1457,7 @@
         <v>4</v>
       </c>
       <c r="I8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.15">
@@ -1446,7 +1465,7 @@
         <v>13010005</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C9">
         <v>11</v>
@@ -1461,7 +1480,7 @@
         <v>5</v>
       </c>
       <c r="I9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.15">
@@ -1469,7 +1488,7 @@
         <v>13010006</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1484,7 +1503,7 @@
         <v>6</v>
       </c>
       <c r="I10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.15">
@@ -1492,7 +1511,7 @@
         <v>13010007</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C11">
         <v>21</v>
@@ -1504,13 +1523,13 @@
         <v>330</v>
       </c>
       <c r="G11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H11">
         <v>7</v>
       </c>
       <c r="I11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.15">
@@ -1518,7 +1537,7 @@
         <v>13010008</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12">
         <v>31</v>
@@ -1533,7 +1552,7 @@
         <v>8</v>
       </c>
       <c r="I12" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.15">
@@ -1541,7 +1560,7 @@
         <v>13010009</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C13">
         <v>21</v>
@@ -1556,7 +1575,7 @@
         <v>9</v>
       </c>
       <c r="I13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.15">
@@ -1564,7 +1583,7 @@
         <v>13010010</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C14">
         <v>21</v>
@@ -1579,7 +1598,7 @@
         <v>10</v>
       </c>
       <c r="I14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
@@ -1587,7 +1606,7 @@
         <v>13010011</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C15">
         <v>21</v>
@@ -1599,13 +1618,13 @@
         <v>300</v>
       </c>
       <c r="G15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H15">
         <v>11</v>
       </c>
       <c r="I15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.15">
@@ -1613,7 +1632,7 @@
         <v>13010012</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16">
         <v>11</v>
@@ -1628,7 +1647,7 @@
         <v>12</v>
       </c>
       <c r="I16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.15">
@@ -1636,7 +1655,7 @@
         <v>13010013</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17">
         <v>11</v>
@@ -1651,7 +1670,7 @@
         <v>13</v>
       </c>
       <c r="I17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.15">
@@ -1659,7 +1678,7 @@
         <v>13010014</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C18">
         <v>21</v>
@@ -1674,7 +1693,7 @@
         <v>14</v>
       </c>
       <c r="I18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.15">
@@ -1682,7 +1701,7 @@
         <v>13010015</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C19">
         <v>31</v>
@@ -1697,7 +1716,7 @@
         <v>15</v>
       </c>
       <c r="I19" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.15">
@@ -1705,7 +1724,7 @@
         <v>13010016</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C20">
         <v>31</v>
@@ -1720,7 +1739,7 @@
         <v>16</v>
       </c>
       <c r="I20" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.15">
@@ -1728,7 +1747,7 @@
         <v>13010017</v>
       </c>
       <c r="B21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C21">
         <v>31</v>
@@ -1743,7 +1762,7 @@
         <v>18</v>
       </c>
       <c r="I21" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.15">
@@ -1751,7 +1770,7 @@
         <v>13010018</v>
       </c>
       <c r="B22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C22">
         <v>31</v>
@@ -1766,7 +1785,7 @@
         <v>19</v>
       </c>
       <c r="I22" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
optimise the function of scenequest
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Scene.xlsx
+++ b/ConfigData/Xlsx/Scene.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="Scene" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="79">
   <si>
     <t>村外小屋</t>
   </si>
@@ -171,18 +171,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>42000003;3|42000002;1|42000004;2|42000005;1|42000011;1|42000014;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>42000006;2|42000007;1|42000008;2|42000003;3|42000004;2|42000013;1|42000014;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>GameUpToNumber;GameThreeBody;GameSeven</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>tatamuviliage</t>
   </si>
   <si>
@@ -244,6 +232,69 @@
   </si>
   <si>
     <t>moonforest</t>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>激活传送门</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QPortal</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>42010003;3|42010002;1|42010004;2|42010005;1|42010011;1</t>
+  </si>
+  <si>
+    <t>42010006;2|42010007;1|42010008;2|42010003;3|42010004;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QCardChange</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>卡牌交换</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>素材商人</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QPiece</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>GameUpToNumber;GameThreeBody</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QMerchant</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QDoctor</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QAngel</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>商人</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>医生</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>天使</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -930,15 +981,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:I22" totalsRowShown="0">
-  <autoFilter ref="A1:I22"/>
-  <tableColumns count="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:O22" totalsRowShown="0">
+  <autoFilter ref="A1:O22"/>
+  <tableColumns count="15">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
     <tableColumn id="3" name="Level"/>
     <tableColumn id="4" name="WindowX"/>
     <tableColumn id="5" name="WindowY"/>
     <tableColumn id="9" name="Quest"/>
+    <tableColumn id="10" name="QPortal"/>
+    <tableColumn id="11" name="QCardChange"/>
+    <tableColumn id="12" name="QPiece"/>
+    <tableColumn id="13" name="QMerchant"/>
+    <tableColumn id="14" name="QDoctor"/>
+    <tableColumn id="15" name="QAngel"/>
     <tableColumn id="6" name="Func"/>
     <tableColumn id="7" name="Url"/>
     <tableColumn id="8" name="TilePath"/>
@@ -1234,22 +1291,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="11.125" customWidth="1"/>
     <col min="4" max="5" width="9.75" customWidth="1"/>
-    <col min="6" max="6" width="67.5" customWidth="1"/>
-    <col min="7" max="7" width="9" customWidth="1"/>
-    <col min="10" max="10" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="58.125" customWidth="1"/>
+    <col min="7" max="12" width="3.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -1269,16 +1325,34 @@
         <v>40</v>
       </c>
       <c r="G1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K1" t="s">
+        <v>74</v>
+      </c>
+      <c r="L1" t="s">
+        <v>75</v>
+      </c>
+      <c r="M1" t="s">
         <v>32</v>
       </c>
-      <c r="H1" t="s">
+      <c r="N1" t="s">
         <v>33</v>
       </c>
-      <c r="I1" t="s">
+      <c r="O1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -1298,16 +1372,34 @@
         <v>42</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>20</v>
       </c>
@@ -1327,16 +1419,34 @@
         <v>41</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="M3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -1353,19 +1463,22 @@
         <v>499</v>
       </c>
       <c r="F4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G4" t="s">
-        <v>46</v>
-      </c>
-      <c r="H4">
+        <v>66</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="M4" t="s">
+        <v>72</v>
+      </c>
+      <c r="N4">
         <v>2</v>
       </c>
-      <c r="I4" t="s">
+      <c r="O4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>13000002</v>
       </c>
@@ -1382,21 +1495,27 @@
         <v>468</v>
       </c>
       <c r="F5" t="s">
-        <v>45</v>
-      </c>
-      <c r="H5">
+        <v>67</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="N5">
         <v>3</v>
       </c>
-      <c r="I5" t="s">
+      <c r="O5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>13000003</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1407,14 +1526,17 @@
       <c r="E6">
         <v>535</v>
       </c>
-      <c r="H6">
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="N6">
         <v>17</v>
       </c>
-      <c r="I6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="O6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>13010001</v>
       </c>
@@ -1430,14 +1552,17 @@
       <c r="E7">
         <v>0</v>
       </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-      <c r="I7" t="s">
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>13010004</v>
       </c>
@@ -1453,14 +1578,17 @@
       <c r="E8">
         <v>238</v>
       </c>
-      <c r="H8">
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="N8">
         <v>4</v>
       </c>
-      <c r="I8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="O8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>13010005</v>
       </c>
@@ -1476,14 +1604,17 @@
       <c r="E9">
         <v>231</v>
       </c>
-      <c r="H9">
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="N9">
         <v>5</v>
       </c>
-      <c r="I9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="O9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>13010006</v>
       </c>
@@ -1499,14 +1630,17 @@
       <c r="E10">
         <v>396</v>
       </c>
-      <c r="H10">
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="N10">
         <v>6</v>
       </c>
-      <c r="I10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="O10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>13010007</v>
       </c>
@@ -1522,17 +1656,20 @@
       <c r="E11">
         <v>330</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="M11" t="s">
         <v>7</v>
       </c>
-      <c r="H11">
+      <c r="N11">
         <v>7</v>
       </c>
-      <c r="I11" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="O11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>13010008</v>
       </c>
@@ -1548,14 +1685,17 @@
       <c r="E12">
         <v>328</v>
       </c>
-      <c r="H12">
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="N12">
         <v>8</v>
       </c>
-      <c r="I12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="O12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>13010009</v>
       </c>
@@ -1571,14 +1711,17 @@
       <c r="E13">
         <v>373</v>
       </c>
-      <c r="H13">
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="N13">
         <v>9</v>
       </c>
-      <c r="I13" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="O13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>13010010</v>
       </c>
@@ -1594,14 +1737,17 @@
       <c r="E14">
         <v>434</v>
       </c>
-      <c r="H14">
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="N14">
         <v>10</v>
       </c>
-      <c r="I14" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="O14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>13010011</v>
       </c>
@@ -1617,17 +1763,20 @@
       <c r="E15">
         <v>300</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="M15" t="s">
         <v>12</v>
       </c>
-      <c r="H15">
+      <c r="N15">
         <v>11</v>
       </c>
-      <c r="I15" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="O15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>13010012</v>
       </c>
@@ -1643,14 +1792,17 @@
       <c r="E16">
         <v>319</v>
       </c>
-      <c r="H16">
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="N16">
         <v>12</v>
       </c>
-      <c r="I16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="O16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>13010013</v>
       </c>
@@ -1666,14 +1818,17 @@
       <c r="E17">
         <v>218</v>
       </c>
-      <c r="H17">
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="N17">
         <v>13</v>
       </c>
-      <c r="I17" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="O17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>13010014</v>
       </c>
@@ -1689,14 +1844,17 @@
       <c r="E18">
         <v>388</v>
       </c>
-      <c r="H18">
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="N18">
         <v>14</v>
       </c>
-      <c r="I18" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="O18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>13010015</v>
       </c>
@@ -1712,14 +1870,17 @@
       <c r="E19">
         <v>411</v>
       </c>
-      <c r="H19">
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="N19">
         <v>15</v>
       </c>
-      <c r="I19" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="O19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>13010016</v>
       </c>
@@ -1735,19 +1896,22 @@
       <c r="E20">
         <v>432</v>
       </c>
-      <c r="H20">
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="N20">
         <v>16</v>
       </c>
-      <c r="I20" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="O20" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>13010017</v>
       </c>
       <c r="B21" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C21">
         <v>31</v>
@@ -1758,19 +1922,22 @@
       <c r="E21">
         <v>459</v>
       </c>
-      <c r="H21">
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="N21">
         <v>18</v>
       </c>
-      <c r="I21" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="O21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>13010018</v>
       </c>
       <c r="B22" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C22">
         <v>31</v>
@@ -1781,11 +1948,14 @@
       <c r="E22">
         <v>327</v>
       </c>
-      <c r="H22">
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="N22">
         <v>19</v>
       </c>
-      <c r="I22" t="s">
-        <v>65</v>
+      <c r="O22" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
support scene event portal, punish and reward support multi times
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Scene.xlsx
+++ b/ConfigData/Xlsx/Scene.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="111">
   <si>
     <t>村外小屋</t>
   </si>
@@ -359,7 +359,43 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>sewer;3|poppyfield;1|river;2|fortune;1|oldtree;1</t>
+    <t>poppyfield;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>poppyfield;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>portal;3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>river;2|fishpool;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trees;3|mushroom;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>mushroom;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>sewer;3|river;2|fortune;1|oldtree;1|poppyfield;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trees;3|grave;1|portal;1|oldtree;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>portal;1|fishpool;1|grave;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>fortune;1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -367,7 +403,11 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>trees;3|grave;1</t>
+    <t>river;2|stone;3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>sandpile;1|stone;2</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1948,7 +1988,7 @@
   <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1956,7 +1996,7 @@
     <col min="1" max="1" width="11.125" customWidth="1"/>
     <col min="2" max="2" width="10.625" customWidth="1"/>
     <col min="3" max="3" width="4.375" customWidth="1"/>
-    <col min="4" max="4" width="48.75" customWidth="1"/>
+    <col min="4" max="4" width="52.875" customWidth="1"/>
     <col min="5" max="10" width="3.125" customWidth="1"/>
     <col min="11" max="11" width="6.625" customWidth="1"/>
     <col min="12" max="12" width="4" customWidth="1"/>
@@ -2126,7 +2166,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="E4" s="9">
         <v>1</v>
@@ -2166,7 +2206,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="E5" s="9">
         <v>1</v>
@@ -2176,7 +2216,9 @@
         <v>1</v>
       </c>
       <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
+      <c r="I5" s="9">
+        <v>1</v>
+      </c>
       <c r="J5" s="9"/>
       <c r="K5" s="9"/>
       <c r="L5" s="9">
@@ -2205,7 +2247,9 @@
       <c r="C6" s="9">
         <v>1</v>
       </c>
-      <c r="D6" s="9"/>
+      <c r="D6" s="9" t="s">
+        <v>110</v>
+      </c>
       <c r="E6" s="9">
         <v>1</v>
       </c>
@@ -2275,13 +2319,17 @@
       <c r="C8" s="9">
         <v>31</v>
       </c>
-      <c r="D8" s="9"/>
+      <c r="D8" s="9" t="s">
+        <v>109</v>
+      </c>
       <c r="E8" s="9">
         <v>1</v>
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
+      <c r="H8" s="9">
+        <v>1</v>
+      </c>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
@@ -2315,7 +2363,9 @@
       <c r="E9" s="9">
         <v>1</v>
       </c>
-      <c r="F9" s="9"/>
+      <c r="F9" s="9">
+        <v>1</v>
+      </c>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
@@ -2381,14 +2431,20 @@
       <c r="C11" s="9">
         <v>31</v>
       </c>
-      <c r="D11" s="9"/>
+      <c r="D11" s="9" t="s">
+        <v>106</v>
+      </c>
       <c r="E11" s="9">
         <v>1</v>
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
+      <c r="H11" s="9">
+        <v>1</v>
+      </c>
+      <c r="I11" s="9">
+        <v>1</v>
+      </c>
       <c r="J11" s="9"/>
       <c r="K11" s="9" t="s">
         <v>7</v>
@@ -2419,7 +2475,9 @@
       <c r="C12" s="9">
         <v>31</v>
       </c>
-      <c r="D12" s="9"/>
+      <c r="D12" s="9" t="s">
+        <v>99</v>
+      </c>
       <c r="E12" s="9">
         <v>1</v>
       </c>
@@ -2427,7 +2485,9 @@
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
+      <c r="J12" s="9">
+        <v>1</v>
+      </c>
       <c r="K12" s="9"/>
       <c r="L12" s="9">
         <v>8</v>
@@ -2455,13 +2515,19 @@
       <c r="C13" s="9">
         <v>31</v>
       </c>
-      <c r="D13" s="9"/>
+      <c r="D13" s="9" t="s">
+        <v>98</v>
+      </c>
       <c r="E13" s="9">
         <v>1</v>
       </c>
-      <c r="F13" s="9"/>
+      <c r="F13" s="9">
+        <v>1</v>
+      </c>
       <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
+      <c r="H13" s="9">
+        <v>1</v>
+      </c>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
       <c r="K13" s="9"/>
@@ -2499,7 +2565,9 @@
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
+      <c r="J14" s="9">
+        <v>1</v>
+      </c>
       <c r="K14" s="9"/>
       <c r="L14" s="9">
         <v>10</v>
@@ -2527,12 +2595,16 @@
       <c r="C15" s="9">
         <v>31</v>
       </c>
-      <c r="D15" s="9"/>
+      <c r="D15" s="9" t="s">
+        <v>107</v>
+      </c>
       <c r="E15" s="9">
         <v>1</v>
       </c>
       <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
+      <c r="G15" s="9">
+        <v>1</v>
+      </c>
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
       <c r="J15" s="9"/>
@@ -2566,7 +2638,7 @@
         <v>4</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="E16" s="9">
         <v>1</v>
@@ -2574,7 +2646,9 @@
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
+      <c r="I16" s="9">
+        <v>1</v>
+      </c>
       <c r="J16" s="9"/>
       <c r="K16" s="9"/>
       <c r="L16" s="9">
@@ -2639,15 +2713,21 @@
       <c r="C18" s="9">
         <v>31</v>
       </c>
-      <c r="D18" s="9"/>
+      <c r="D18" s="9" t="s">
+        <v>101</v>
+      </c>
       <c r="E18" s="9">
         <v>1</v>
       </c>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
+      <c r="I18" s="9">
+        <v>1</v>
+      </c>
+      <c r="J18" s="9">
+        <v>1</v>
+      </c>
       <c r="K18" s="9"/>
       <c r="L18" s="9">
         <v>14</v>
@@ -2675,13 +2755,17 @@
       <c r="C19" s="9">
         <v>31</v>
       </c>
-      <c r="D19" s="9"/>
+      <c r="D19" s="9" t="s">
+        <v>100</v>
+      </c>
       <c r="E19" s="9">
         <v>1</v>
       </c>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
+      <c r="H19" s="9">
+        <v>1</v>
+      </c>
       <c r="I19" s="9"/>
       <c r="J19" s="9"/>
       <c r="K19" s="9"/>
@@ -2745,14 +2829,18 @@
       <c r="C21" s="9">
         <v>31</v>
       </c>
-      <c r="D21" s="9"/>
+      <c r="D21" s="9" t="s">
+        <v>103</v>
+      </c>
       <c r="E21" s="9">
         <v>1</v>
       </c>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
+      <c r="I21" s="9">
+        <v>1</v>
+      </c>
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
       <c r="L21" s="9">
@@ -2781,15 +2869,25 @@
       <c r="C22" s="9">
         <v>31</v>
       </c>
-      <c r="D22" s="9"/>
+      <c r="D22" s="9" t="s">
+        <v>102</v>
+      </c>
       <c r="E22" s="9">
         <v>1</v>
       </c>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
+      <c r="F22" s="9">
+        <v>1</v>
+      </c>
+      <c r="G22" s="9">
+        <v>1</v>
+      </c>
+      <c r="H22" s="9">
+        <v>1</v>
+      </c>
       <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
+      <c r="J22" s="9">
+        <v>1</v>
+      </c>
       <c r="K22" s="9"/>
       <c r="L22" s="9">
         <v>19</v>

</xml_diff>

<commit_message>
finish the function of quest NEXT
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Scene.xlsx
+++ b/ConfigData/Xlsx/Scene.xlsx
@@ -1988,7 +1988,7 @@
   <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2646,9 +2646,7 @@
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
-      <c r="I16" s="9">
-        <v>1</v>
-      </c>
+      <c r="I16" s="9"/>
       <c r="J16" s="9"/>
       <c r="K16" s="9"/>
       <c r="L16" s="9">

</xml_diff>

<commit_message>
finish the ruintown event to test the next function
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Scene.xlsx
+++ b/ConfigData/Xlsx/Scene.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17571"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -363,10 +363,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>poppyfield;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>portal;3</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -403,18 +399,22 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>river;2|stone;3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>sandpile;1|stone;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>poppyfield;1|ruintown1;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>river;2|stone;3||ruintown1;1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1699,7 +1699,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1774,6 +1774,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1809,6 +1826,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1988,7 +2022,7 @@
   <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2166,7 +2200,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E4" s="9">
         <v>1</v>
@@ -2206,7 +2240,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E5" s="9">
         <v>1</v>
@@ -2248,7 +2282,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E6" s="9">
         <v>1</v>
@@ -2320,7 +2354,7 @@
         <v>31</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E8" s="9">
         <v>1</v>
@@ -2432,7 +2466,7 @@
         <v>31</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E11" s="9">
         <v>1</v>
@@ -2476,7 +2510,7 @@
         <v>31</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E12" s="9">
         <v>1</v>
@@ -2516,7 +2550,7 @@
         <v>31</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="E13" s="9">
         <v>1</v>
@@ -2596,7 +2630,7 @@
         <v>31</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E15" s="9">
         <v>1</v>
@@ -2638,7 +2672,7 @@
         <v>4</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E16" s="9">
         <v>1</v>
@@ -2712,7 +2746,7 @@
         <v>31</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E18" s="9">
         <v>1</v>
@@ -2754,7 +2788,7 @@
         <v>31</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E19" s="9">
         <v>1</v>
@@ -2828,7 +2862,7 @@
         <v>31</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E21" s="9">
         <v>1</v>
@@ -2868,7 +2902,7 @@
         <v>31</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E22" s="9">
         <v>1</v>

</xml_diff>

<commit_message>
finish the random quest mechanical
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Scene.xlsx
+++ b/ConfigData/Xlsx/Scene.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="117">
   <si>
     <t>村外小屋</t>
   </si>
@@ -408,13 +408,37 @@
   </si>
   <si>
     <t>river;2|stone;3|ruintown1;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>小概率任务</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QuestRandom</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|treasure;25</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1157,7 +1181,48 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="22">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1646,20 +1711,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1674,32 +1725,33 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:P22" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" tableBorderDxfId="16">
-  <autoFilter ref="A3:P22"/>
-  <tableColumns count="16">
-    <tableColumn id="1" name="Id" dataDxfId="15"/>
-    <tableColumn id="2" name="Name" dataDxfId="14"/>
-    <tableColumn id="3" name="Level" dataDxfId="13"/>
-    <tableColumn id="4" name="Quest" dataDxfId="12"/>
-    <tableColumn id="5" name="QPortal" dataDxfId="11"/>
-    <tableColumn id="6" name="QCardChange" dataDxfId="10"/>
-    <tableColumn id="7" name="QPiece" dataDxfId="9"/>
-    <tableColumn id="8" name="QMerchant" dataDxfId="8"/>
-    <tableColumn id="9" name="QDoctor" dataDxfId="7"/>
-    <tableColumn id="10" name="QAngel" dataDxfId="6"/>
-    <tableColumn id="11" name="Func" dataDxfId="5"/>
-    <tableColumn id="12" name="Url" dataDxfId="4"/>
-    <tableColumn id="13" name="TilePath" dataDxfId="3"/>
-    <tableColumn id="14" name="Icon" dataDxfId="2"/>
-    <tableColumn id="15" name="IconX" dataDxfId="1"/>
-    <tableColumn id="16" name="IconY" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:Q22" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20" tableBorderDxfId="19">
+  <autoFilter ref="A3:Q22"/>
+  <tableColumns count="17">
+    <tableColumn id="1" name="Id" dataDxfId="18"/>
+    <tableColumn id="2" name="Name" dataDxfId="17"/>
+    <tableColumn id="3" name="Level" dataDxfId="16"/>
+    <tableColumn id="4" name="Quest" dataDxfId="15"/>
+    <tableColumn id="17" name="QuestRandom" dataDxfId="0"/>
+    <tableColumn id="5" name="QPortal" dataDxfId="14"/>
+    <tableColumn id="6" name="QCardChange" dataDxfId="13"/>
+    <tableColumn id="7" name="QPiece" dataDxfId="12"/>
+    <tableColumn id="8" name="QMerchant" dataDxfId="11"/>
+    <tableColumn id="9" name="QDoctor" dataDxfId="10"/>
+    <tableColumn id="10" name="QAngel" dataDxfId="9"/>
+    <tableColumn id="11" name="Func" dataDxfId="8"/>
+    <tableColumn id="12" name="Url" dataDxfId="7"/>
+    <tableColumn id="13" name="TilePath" dataDxfId="6"/>
+    <tableColumn id="14" name="Icon" dataDxfId="5"/>
+    <tableColumn id="15" name="IconX" dataDxfId="4"/>
+    <tableColumn id="16" name="IconY" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1774,23 +1826,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1826,23 +1861,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2019,10 +2037,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P22"/>
+  <dimension ref="A1:Q22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2031,15 +2049,16 @@
     <col min="2" max="2" width="10.625" customWidth="1"/>
     <col min="3" max="3" width="4.375" customWidth="1"/>
     <col min="4" max="4" width="52.875" customWidth="1"/>
-    <col min="5" max="10" width="3.125" customWidth="1"/>
-    <col min="11" max="11" width="6.625" customWidth="1"/>
-    <col min="12" max="12" width="4" customWidth="1"/>
-    <col min="13" max="13" width="12.875" customWidth="1"/>
-    <col min="14" max="14" width="7.25" customWidth="1"/>
-    <col min="15" max="16" width="6" customWidth="1"/>
+    <col min="5" max="5" width="16.625" customWidth="1"/>
+    <col min="6" max="11" width="3.125" customWidth="1"/>
+    <col min="12" max="12" width="6.625" customWidth="1"/>
+    <col min="13" max="13" width="4" customWidth="1"/>
+    <col min="14" max="14" width="12.875" customWidth="1"/>
+    <col min="15" max="15" width="7.25" customWidth="1"/>
+    <col min="16" max="17" width="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>20</v>
       </c>
@@ -2052,44 +2071,47 @@
       <c r="D1" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="Q1" s="8" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -2102,8 +2124,8 @@
       <c r="D2" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>58</v>
+      <c r="E2" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>58</v>
@@ -2120,26 +2142,29 @@
       <c r="J2" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="Q2" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A3" s="10" t="s">
         <v>25</v>
       </c>
@@ -2152,44 +2177,47 @@
       <c r="D3" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="F3" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="G3" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="H3" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="I3" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="J3" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="K3" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="L3" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="M3" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="M3" s="10" t="s">
+      <c r="N3" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="N3" s="10" t="s">
+      <c r="O3" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="O3" s="10" t="s">
+      <c r="P3" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="P3" s="10" t="s">
+      <c r="Q3" s="10" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A4" s="9" t="s">
         <v>30</v>
       </c>
@@ -2202,34 +2230,35 @@
       <c r="D4" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="E4" s="9">
-        <v>1</v>
-      </c>
-      <c r="F4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9">
+        <v>1</v>
+      </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
-      <c r="K4" s="9" t="s">
+      <c r="K4" s="9"/>
+      <c r="L4" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="L4" s="9">
+      <c r="M4" s="9">
         <v>2</v>
       </c>
-      <c r="M4" s="9" t="s">
+      <c r="N4" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="N4" s="9" t="s">
+      <c r="O4" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="O4" s="9">
+      <c r="P4" s="9">
         <v>1348</v>
       </c>
-      <c r="P4" s="9">
+      <c r="Q4" s="9">
         <v>611</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A5" s="9">
         <v>13000002</v>
       </c>
@@ -2242,36 +2271,37 @@
       <c r="D5" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="E5" s="9">
-        <v>1</v>
-      </c>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9">
-        <v>1</v>
-      </c>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9">
-        <v>1</v>
-      </c>
-      <c r="J5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9">
+        <v>1</v>
+      </c>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9">
+        <v>1</v>
+      </c>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9">
+        <v>1</v>
+      </c>
       <c r="K5" s="9"/>
-      <c r="L5" s="9">
+      <c r="L5" s="9"/>
+      <c r="M5" s="9">
         <v>3</v>
       </c>
-      <c r="M5" s="9" t="s">
+      <c r="N5" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="N5" s="9" t="s">
+      <c r="O5" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="O5" s="9">
+      <c r="P5" s="9">
         <v>1279</v>
       </c>
-      <c r="P5" s="9">
+      <c r="Q5" s="9">
         <v>571</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A6" s="9">
         <v>13000003</v>
       </c>
@@ -2284,32 +2314,35 @@
       <c r="D6" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="E6" s="9">
-        <v>1</v>
-      </c>
-      <c r="F6" s="9"/>
+      <c r="E6" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="F6" s="9">
+        <v>1</v>
+      </c>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
-      <c r="L6" s="9">
+      <c r="L6" s="9"/>
+      <c r="M6" s="9">
         <v>17</v>
       </c>
-      <c r="M6" s="9" t="s">
+      <c r="N6" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="N6" s="9" t="s">
+      <c r="O6" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="O6" s="9">
+      <c r="P6" s="9">
         <v>1213</v>
       </c>
-      <c r="P6" s="9">
+      <c r="Q6" s="9">
         <v>655</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A7" s="9">
         <v>13010001</v>
       </c>
@@ -2320,30 +2353,31 @@
         <v>0</v>
       </c>
       <c r="D7" s="9"/>
-      <c r="E7" s="9">
-        <v>1</v>
-      </c>
-      <c r="F7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9">
+        <v>1</v>
+      </c>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
-      <c r="L7" s="9">
-        <v>1</v>
-      </c>
-      <c r="M7" s="9" t="s">
+      <c r="L7" s="9"/>
+      <c r="M7" s="9">
+        <v>1</v>
+      </c>
+      <c r="N7" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9">
-        <v>0</v>
-      </c>
+      <c r="O7" s="9"/>
       <c r="P7" s="9">
         <v>0</v>
       </c>
+      <c r="Q7" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A8" s="9">
         <v>13010004</v>
       </c>
@@ -2356,34 +2390,37 @@
       <c r="D8" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="E8" s="9">
-        <v>1</v>
-      </c>
-      <c r="F8" s="9"/>
+      <c r="E8" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="F8" s="9">
+        <v>1</v>
+      </c>
       <c r="G8" s="9"/>
-      <c r="H8" s="9">
-        <v>1</v>
-      </c>
-      <c r="I8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9">
+        <v>1</v>
+      </c>
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
-      <c r="L8" s="9">
+      <c r="L8" s="9"/>
+      <c r="M8" s="9">
         <v>4</v>
       </c>
-      <c r="M8" s="9" t="s">
+      <c r="N8" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="N8" s="9" t="s">
+      <c r="O8" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="O8" s="9">
+      <c r="P8" s="9">
         <v>1148</v>
       </c>
-      <c r="P8" s="9">
+      <c r="Q8" s="9">
         <v>351</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A9" s="9">
         <v>13010005</v>
       </c>
@@ -2394,34 +2431,35 @@
         <v>31</v>
       </c>
       <c r="D9" s="9"/>
-      <c r="E9" s="9">
-        <v>1</v>
-      </c>
+      <c r="E9" s="9"/>
       <c r="F9" s="9">
         <v>1</v>
       </c>
-      <c r="G9" s="9"/>
+      <c r="G9" s="9">
+        <v>1</v>
+      </c>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
-      <c r="L9" s="9">
+      <c r="L9" s="9"/>
+      <c r="M9" s="9">
         <v>5</v>
       </c>
-      <c r="M9" s="9" t="s">
+      <c r="N9" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="N9" s="9" t="s">
+      <c r="O9" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="O9" s="9">
+      <c r="P9" s="9">
         <v>1386</v>
       </c>
-      <c r="P9" s="9">
+      <c r="Q9" s="9">
         <v>339</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A10" s="9">
         <v>13010006</v>
       </c>
@@ -2439,23 +2477,24 @@
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
-      <c r="L10" s="9">
+      <c r="L10" s="9"/>
+      <c r="M10" s="9">
         <v>6</v>
       </c>
-      <c r="M10" s="9" t="s">
+      <c r="N10" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="N10" s="9" t="s">
+      <c r="O10" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="O10" s="9">
+      <c r="P10" s="9">
         <v>1232</v>
       </c>
-      <c r="P10" s="9">
+      <c r="Q10" s="9">
         <v>506</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A11" s="9">
         <v>13010007</v>
       </c>
@@ -2468,38 +2507,41 @@
       <c r="D11" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="E11" s="9">
-        <v>1</v>
-      </c>
-      <c r="F11" s="9"/>
+      <c r="E11" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="F11" s="9">
+        <v>1</v>
+      </c>
       <c r="G11" s="9"/>
-      <c r="H11" s="9">
-        <v>1</v>
-      </c>
+      <c r="H11" s="9"/>
       <c r="I11" s="9">
         <v>1</v>
       </c>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9" t="s">
+      <c r="J11" s="9">
+        <v>1</v>
+      </c>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="L11" s="9">
+      <c r="M11" s="9">
         <v>7</v>
       </c>
-      <c r="M11" s="9" t="s">
+      <c r="N11" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="N11" s="9" t="s">
+      <c r="O11" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="O11" s="9">
+      <c r="P11" s="9">
         <v>1431</v>
       </c>
-      <c r="P11" s="9">
+      <c r="Q11" s="9">
         <v>440</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A12" s="9">
         <v>13010008</v>
       </c>
@@ -2512,34 +2554,37 @@
       <c r="D12" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="E12" s="9">
-        <v>1</v>
-      </c>
-      <c r="F12" s="9"/>
+      <c r="E12" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F12" s="9">
+        <v>1</v>
+      </c>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
-      <c r="J12" s="9">
-        <v>1</v>
-      </c>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9">
+      <c r="J12" s="9"/>
+      <c r="K12" s="9">
+        <v>1</v>
+      </c>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9">
         <v>8</v>
       </c>
-      <c r="M12" s="9" t="s">
+      <c r="N12" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="N12" s="9" t="s">
+      <c r="O12" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="O12" s="9">
+      <c r="P12" s="9">
         <v>1067</v>
       </c>
-      <c r="P12" s="9">
+      <c r="Q12" s="9">
         <v>445</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A13" s="9">
         <v>13010009</v>
       </c>
@@ -2552,36 +2597,39 @@
       <c r="D13" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="E13" s="9">
-        <v>1</v>
+      <c r="E13" s="9" t="s">
+        <v>114</v>
       </c>
       <c r="F13" s="9">
         <v>1</v>
       </c>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9">
-        <v>1</v>
-      </c>
-      <c r="I13" s="9"/>
+      <c r="G13" s="9">
+        <v>1</v>
+      </c>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9">
+        <v>1</v>
+      </c>
       <c r="J13" s="9"/>
       <c r="K13" s="9"/>
-      <c r="L13" s="9">
+      <c r="L13" s="9"/>
+      <c r="M13" s="9">
         <v>9</v>
       </c>
-      <c r="M13" s="9" t="s">
+      <c r="N13" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="N13" s="9" t="s">
+      <c r="O13" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="O13" s="9">
+      <c r="P13" s="9">
         <v>1332</v>
       </c>
-      <c r="P13" s="9">
+      <c r="Q13" s="9">
         <v>484</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A14" s="9">
         <v>13010010</v>
       </c>
@@ -2592,34 +2640,37 @@
         <v>31</v>
       </c>
       <c r="D14" s="9"/>
-      <c r="E14" s="9">
-        <v>1</v>
-      </c>
-      <c r="F14" s="9"/>
+      <c r="E14" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F14" s="9">
+        <v>1</v>
+      </c>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
-      <c r="J14" s="9">
-        <v>1</v>
-      </c>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9">
+      <c r="J14" s="9"/>
+      <c r="K14" s="9">
+        <v>1</v>
+      </c>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9">
         <v>10</v>
       </c>
-      <c r="M14" s="9" t="s">
+      <c r="N14" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="N14" s="9" t="s">
+      <c r="O14" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="O14" s="9">
+      <c r="P14" s="9">
         <v>1441</v>
       </c>
-      <c r="P14" s="9">
+      <c r="Q14" s="9">
         <v>527</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A15" s="9">
         <v>13010011</v>
       </c>
@@ -2632,36 +2683,39 @@
       <c r="D15" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="E15" s="9">
-        <v>1</v>
-      </c>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9">
-        <v>1</v>
-      </c>
-      <c r="H15" s="9"/>
+      <c r="E15" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="F15" s="9">
+        <v>1</v>
+      </c>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9">
+        <v>1</v>
+      </c>
       <c r="I15" s="9"/>
       <c r="J15" s="9"/>
-      <c r="K15" s="9" t="s">
+      <c r="K15" s="9"/>
+      <c r="L15" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="L15" s="9">
+      <c r="M15" s="9">
         <v>11</v>
       </c>
-      <c r="M15" s="9" t="s">
+      <c r="N15" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="N15" s="9" t="s">
+      <c r="O15" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="O15" s="9">
+      <c r="P15" s="9">
         <v>1574</v>
       </c>
-      <c r="P15" s="9">
+      <c r="Q15" s="9">
         <v>373</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A16" s="9">
         <v>13010012</v>
       </c>
@@ -2674,32 +2728,33 @@
       <c r="D16" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="E16" s="9">
-        <v>1</v>
-      </c>
-      <c r="F16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9">
+        <v>1</v>
+      </c>
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
       <c r="J16" s="9"/>
       <c r="K16" s="9"/>
-      <c r="L16" s="9">
+      <c r="L16" s="9"/>
+      <c r="M16" s="9">
         <v>12</v>
       </c>
-      <c r="M16" s="9" t="s">
+      <c r="N16" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="N16" s="9" t="s">
+      <c r="O16" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="O16" s="9">
+      <c r="P16" s="9">
         <v>1251</v>
       </c>
-      <c r="P16" s="9">
+      <c r="Q16" s="9">
         <v>432</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A17" s="9">
         <v>13010013</v>
       </c>
@@ -2710,32 +2765,35 @@
         <v>31</v>
       </c>
       <c r="D17" s="9"/>
-      <c r="E17" s="9">
-        <v>1</v>
-      </c>
-      <c r="F17" s="9"/>
+      <c r="E17" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F17" s="9">
+        <v>1</v>
+      </c>
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
       <c r="J17" s="9"/>
       <c r="K17" s="9"/>
-      <c r="L17" s="9">
+      <c r="L17" s="9"/>
+      <c r="M17" s="9">
         <v>13</v>
       </c>
-      <c r="M17" s="9" t="s">
+      <c r="N17" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="N17" s="9" t="s">
+      <c r="O17" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="O17" s="9">
+      <c r="P17" s="9">
         <v>1250</v>
       </c>
-      <c r="P17" s="9">
+      <c r="Q17" s="9">
         <v>338</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A18" s="9">
         <v>13010014</v>
       </c>
@@ -2748,36 +2806,39 @@
       <c r="D18" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="E18" s="9">
-        <v>1</v>
-      </c>
-      <c r="F18" s="9"/>
+      <c r="E18" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F18" s="9">
+        <v>1</v>
+      </c>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
-      <c r="I18" s="9">
-        <v>1</v>
-      </c>
+      <c r="I18" s="9"/>
       <c r="J18" s="9">
         <v>1</v>
       </c>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9">
+      <c r="K18" s="9">
+        <v>1</v>
+      </c>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9">
         <v>14</v>
       </c>
-      <c r="M18" s="9" t="s">
+      <c r="N18" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="N18" s="9" t="s">
+      <c r="O18" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="O18" s="9">
+      <c r="P18" s="9">
         <v>1550</v>
       </c>
-      <c r="P18" s="9">
+      <c r="Q18" s="9">
         <v>505</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A19" s="9">
         <v>13010015</v>
       </c>
@@ -2790,34 +2851,37 @@
       <c r="D19" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="E19" s="9">
-        <v>1</v>
-      </c>
-      <c r="F19" s="9"/>
+      <c r="E19" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F19" s="9">
+        <v>1</v>
+      </c>
       <c r="G19" s="9"/>
-      <c r="H19" s="9">
-        <v>1</v>
-      </c>
-      <c r="I19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9">
+        <v>1</v>
+      </c>
       <c r="J19" s="9"/>
       <c r="K19" s="9"/>
-      <c r="L19" s="9">
+      <c r="L19" s="9"/>
+      <c r="M19" s="9">
         <v>15</v>
       </c>
-      <c r="M19" s="9" t="s">
+      <c r="N19" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="N19" s="9" t="s">
+      <c r="O19" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="O19" s="9">
+      <c r="P19" s="9">
         <v>1040</v>
       </c>
-      <c r="P19" s="9">
+      <c r="Q19" s="9">
         <v>538</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A20" s="9">
         <v>13010016</v>
       </c>
@@ -2835,23 +2899,24 @@
       <c r="I20" s="9"/>
       <c r="J20" s="9"/>
       <c r="K20" s="9"/>
-      <c r="L20" s="9">
+      <c r="L20" s="9"/>
+      <c r="M20" s="9">
         <v>16</v>
       </c>
-      <c r="M20" s="9" t="s">
+      <c r="N20" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="N20" s="9" t="s">
+      <c r="O20" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="O20" s="9">
+      <c r="P20" s="9">
         <v>919</v>
       </c>
-      <c r="P20" s="9">
+      <c r="Q20" s="9">
         <v>534</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A21" s="9">
         <v>13010017</v>
       </c>
@@ -2864,34 +2929,37 @@
       <c r="D21" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="E21" s="9">
-        <v>1</v>
-      </c>
-      <c r="F21" s="9"/>
+      <c r="E21" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F21" s="9">
+        <v>1</v>
+      </c>
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
-      <c r="I21" s="9">
-        <v>1</v>
-      </c>
-      <c r="J21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9">
+        <v>1</v>
+      </c>
       <c r="K21" s="9"/>
-      <c r="L21" s="9">
+      <c r="L21" s="9"/>
+      <c r="M21" s="9">
         <v>18</v>
       </c>
-      <c r="M21" s="9" t="s">
+      <c r="N21" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="N21" s="9" t="s">
+      <c r="O21" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="O21" s="9">
+      <c r="P21" s="9">
         <v>1149</v>
       </c>
-      <c r="P21" s="9">
+      <c r="Q21" s="9">
         <v>584</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A22" s="9">
         <v>13010018</v>
       </c>
@@ -2904,8 +2972,8 @@
       <c r="D22" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="E22" s="9">
-        <v>1</v>
+      <c r="E22" s="9" t="s">
+        <v>114</v>
       </c>
       <c r="F22" s="9">
         <v>1</v>
@@ -2916,36 +2984,39 @@
       <c r="H22" s="9">
         <v>1</v>
       </c>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9">
-        <v>1</v>
-      </c>
-      <c r="K22" s="9"/>
-      <c r="L22" s="9">
+      <c r="I22" s="9">
+        <v>1</v>
+      </c>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9">
+        <v>1</v>
+      </c>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9">
         <v>19</v>
       </c>
-      <c r="M22" s="9" t="s">
+      <c r="N22" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="N22" s="9" t="s">
+      <c r="O22" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="O22" s="9">
+      <c r="P22" s="9">
         <v>840</v>
       </c>
-      <c r="P22" s="9">
+      <c r="Q22" s="9">
         <v>444</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="E4:J22">
-    <cfRule type="cellIs" dxfId="20" priority="2" operator="equal">
+  <conditionalFormatting sqref="F4:K22">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F4">
-    <cfRule type="cellIs" dxfId="19" priority="1" operator="equal">
+  <conditionalFormatting sqref="G4">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
warp can decide target automatic
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Scene.xlsx
+++ b/ConfigData/Xlsx/Scene.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="120">
   <si>
     <t>村外小屋</t>
   </si>
@@ -432,6 +432,18 @@
   </si>
   <si>
     <t>met;30</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>类型</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Type</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1181,7 +1193,7 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="23">
     <dxf>
       <font>
         <b val="0"/>
@@ -1222,6 +1234,33 @@
           <bgColor theme="0" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1725,14 +1764,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:Q22" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20" tableBorderDxfId="19">
-  <autoFilter ref="A3:Q22"/>
-  <tableColumns count="17">
-    <tableColumn id="1" name="Id" dataDxfId="18"/>
-    <tableColumn id="2" name="Name" dataDxfId="17"/>
-    <tableColumn id="3" name="Level" dataDxfId="16"/>
-    <tableColumn id="4" name="Quest" dataDxfId="15"/>
-    <tableColumn id="17" name="QuestRandom" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:R22" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21" tableBorderDxfId="20">
+  <autoFilter ref="A3:R22"/>
+  <tableColumns count="18">
+    <tableColumn id="1" name="Id" dataDxfId="19"/>
+    <tableColumn id="2" name="Name" dataDxfId="18"/>
+    <tableColumn id="18" name="Type" dataDxfId="0"/>
+    <tableColumn id="3" name="Level" dataDxfId="17"/>
+    <tableColumn id="4" name="Quest" dataDxfId="16"/>
+    <tableColumn id="17" name="QuestRandom" dataDxfId="15"/>
     <tableColumn id="5" name="QPortal" dataDxfId="14"/>
     <tableColumn id="6" name="QCardChange" dataDxfId="13"/>
     <tableColumn id="7" name="QPiece" dataDxfId="12"/>
@@ -2037,28 +2077,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q22"/>
+  <dimension ref="A1:R22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="11.125" customWidth="1"/>
     <col min="2" max="2" width="10.625" customWidth="1"/>
-    <col min="3" max="3" width="4.375" customWidth="1"/>
-    <col min="4" max="4" width="52.875" customWidth="1"/>
-    <col min="5" max="5" width="16.625" customWidth="1"/>
-    <col min="6" max="11" width="3.125" customWidth="1"/>
-    <col min="12" max="12" width="6.625" customWidth="1"/>
-    <col min="13" max="13" width="4" customWidth="1"/>
-    <col min="14" max="14" width="12.875" customWidth="1"/>
-    <col min="15" max="15" width="7.25" customWidth="1"/>
-    <col min="16" max="17" width="6" customWidth="1"/>
+    <col min="3" max="3" width="5.125" customWidth="1"/>
+    <col min="4" max="4" width="4.375" customWidth="1"/>
+    <col min="5" max="5" width="52.875" customWidth="1"/>
+    <col min="6" max="6" width="16.625" customWidth="1"/>
+    <col min="7" max="12" width="3.125" customWidth="1"/>
+    <col min="13" max="13" width="6.625" customWidth="1"/>
+    <col min="14" max="14" width="4" customWidth="1"/>
+    <col min="15" max="15" width="12.875" customWidth="1"/>
+    <col min="16" max="16" width="7.25" customWidth="1"/>
+    <col min="17" max="18" width="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>20</v>
       </c>
@@ -2066,52 +2107,55 @@
         <v>21</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="R1" s="8" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -2119,16 +2163,16 @@
         <v>19</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>58</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>58</v>
@@ -2145,26 +2189,29 @@
       <c r="K2" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="R2" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A3" s="10" t="s">
         <v>25</v>
       </c>
@@ -2172,52 +2219,55 @@
         <v>26</v>
       </c>
       <c r="C3" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="E3" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="F3" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="G3" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="H3" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="I3" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="J3" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="K3" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="L3" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="M3" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="M3" s="10" t="s">
+      <c r="N3" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="N3" s="10" t="s">
+      <c r="O3" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="O3" s="10" t="s">
+      <c r="P3" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="P3" s="10" t="s">
+      <c r="Q3" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="Q3" s="10" t="s">
+      <c r="R3" s="10" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A4" s="9" t="s">
         <v>30</v>
       </c>
@@ -2225,40 +2275,43 @@
         <v>0</v>
       </c>
       <c r="C4" s="9">
-        <v>1</v>
-      </c>
-      <c r="D4" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="9">
+        <v>1</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9">
-        <v>1</v>
-      </c>
-      <c r="G4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9">
+        <v>1</v>
+      </c>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
       <c r="K4" s="9"/>
-      <c r="L4" s="9" t="s">
+      <c r="L4" s="9"/>
+      <c r="M4" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="M4" s="9">
+      <c r="N4" s="9">
         <v>2</v>
       </c>
-      <c r="N4" s="9" t="s">
+      <c r="O4" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="O4" s="9" t="s">
+      <c r="P4" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="P4" s="9">
+      <c r="Q4" s="9">
         <v>1348</v>
       </c>
-      <c r="Q4" s="9">
+      <c r="R4" s="9">
         <v>611</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A5" s="9">
         <v>13000002</v>
       </c>
@@ -2268,40 +2321,43 @@
       <c r="C5" s="9">
         <v>2</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="9">
+        <v>2</v>
+      </c>
+      <c r="E5" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9">
-        <v>1</v>
-      </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9">
-        <v>1</v>
-      </c>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9">
-        <v>1</v>
-      </c>
-      <c r="K5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9">
+        <v>1</v>
+      </c>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9">
+        <v>1</v>
+      </c>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9">
+        <v>1</v>
+      </c>
       <c r="L5" s="9"/>
-      <c r="M5" s="9">
+      <c r="M5" s="9"/>
+      <c r="N5" s="9">
         <v>3</v>
       </c>
-      <c r="N5" s="9" t="s">
+      <c r="O5" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="O5" s="9" t="s">
+      <c r="P5" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="P5" s="9">
+      <c r="Q5" s="9">
         <v>1279</v>
       </c>
-      <c r="Q5" s="9">
+      <c r="R5" s="9">
         <v>571</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A6" s="9">
         <v>13000003</v>
       </c>
@@ -2309,40 +2365,43 @@
         <v>53</v>
       </c>
       <c r="C6" s="9">
-        <v>1</v>
-      </c>
-      <c r="D6" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="9">
+        <v>1</v>
+      </c>
+      <c r="E6" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="F6" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="F6" s="9">
-        <v>1</v>
-      </c>
-      <c r="G6" s="9"/>
+      <c r="G6" s="9">
+        <v>1</v>
+      </c>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
       <c r="L6" s="9"/>
-      <c r="M6" s="9">
+      <c r="M6" s="9"/>
+      <c r="N6" s="9">
         <v>17</v>
       </c>
-      <c r="N6" s="9" t="s">
+      <c r="O6" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="O6" s="9" t="s">
+      <c r="P6" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="P6" s="9">
+      <c r="Q6" s="9">
         <v>1213</v>
       </c>
-      <c r="Q6" s="9">
+      <c r="R6" s="9">
         <v>655</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A7" s="9">
         <v>13010001</v>
       </c>
@@ -2350,34 +2409,37 @@
         <v>2</v>
       </c>
       <c r="C7" s="9">
+        <v>2</v>
+      </c>
+      <c r="D7" s="9">
         <v>0</v>
       </c>
-      <c r="D7" s="9"/>
       <c r="E7" s="9"/>
-      <c r="F7" s="9">
-        <v>1</v>
-      </c>
-      <c r="G7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9">
+        <v>1</v>
+      </c>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
-      <c r="M7" s="9">
-        <v>1</v>
-      </c>
-      <c r="N7" s="9" t="s">
+      <c r="M7" s="9"/>
+      <c r="N7" s="9">
+        <v>1</v>
+      </c>
+      <c r="O7" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="O7" s="9"/>
-      <c r="P7" s="9">
-        <v>0</v>
-      </c>
+      <c r="P7" s="9"/>
       <c r="Q7" s="9">
         <v>0</v>
       </c>
+      <c r="R7" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A8" s="9">
         <v>13010004</v>
       </c>
@@ -2385,42 +2447,45 @@
         <v>3</v>
       </c>
       <c r="C8" s="9">
+        <v>2</v>
+      </c>
+      <c r="D8" s="9">
         <v>31</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="E8" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="F8" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="F8" s="9">
-        <v>1</v>
-      </c>
-      <c r="G8" s="9"/>
+      <c r="G8" s="9">
+        <v>1</v>
+      </c>
       <c r="H8" s="9"/>
-      <c r="I8" s="9">
-        <v>1</v>
-      </c>
-      <c r="J8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9">
+        <v>1</v>
+      </c>
       <c r="K8" s="9"/>
       <c r="L8" s="9"/>
-      <c r="M8" s="9">
+      <c r="M8" s="9"/>
+      <c r="N8" s="9">
         <v>4</v>
       </c>
-      <c r="N8" s="9" t="s">
+      <c r="O8" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="O8" s="9" t="s">
+      <c r="P8" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="P8" s="9">
+      <c r="Q8" s="9">
         <v>1148</v>
       </c>
-      <c r="Q8" s="9">
+      <c r="R8" s="9">
         <v>351</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A9" s="9">
         <v>13010005</v>
       </c>
@@ -2428,38 +2493,41 @@
         <v>4</v>
       </c>
       <c r="C9" s="9">
+        <v>2</v>
+      </c>
+      <c r="D9" s="9">
         <v>31</v>
       </c>
-      <c r="D9" s="9"/>
       <c r="E9" s="9"/>
-      <c r="F9" s="9">
-        <v>1</v>
-      </c>
+      <c r="F9" s="9"/>
       <c r="G9" s="9">
         <v>1</v>
       </c>
-      <c r="H9" s="9"/>
+      <c r="H9" s="9">
+        <v>1</v>
+      </c>
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
       <c r="L9" s="9"/>
-      <c r="M9" s="9">
+      <c r="M9" s="9"/>
+      <c r="N9" s="9">
         <v>5</v>
       </c>
-      <c r="N9" s="9" t="s">
+      <c r="O9" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="O9" s="9" t="s">
+      <c r="P9" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="P9" s="9">
+      <c r="Q9" s="9">
         <v>1386</v>
       </c>
-      <c r="Q9" s="9">
+      <c r="R9" s="9">
         <v>339</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A10" s="9">
         <v>13010006</v>
       </c>
@@ -2467,9 +2535,11 @@
         <v>5</v>
       </c>
       <c r="C10" s="9">
+        <v>1</v>
+      </c>
+      <c r="D10" s="9">
         <v>3</v>
       </c>
-      <c r="D10" s="9"/>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
@@ -2478,23 +2548,24 @@
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
       <c r="L10" s="9"/>
-      <c r="M10" s="9">
+      <c r="M10" s="9"/>
+      <c r="N10" s="9">
         <v>6</v>
       </c>
-      <c r="N10" s="9" t="s">
+      <c r="O10" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="O10" s="9" t="s">
+      <c r="P10" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="P10" s="9">
+      <c r="Q10" s="9">
         <v>1232</v>
       </c>
-      <c r="Q10" s="9">
+      <c r="R10" s="9">
         <v>506</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A11" s="9">
         <v>13010007</v>
       </c>
@@ -2502,46 +2573,49 @@
         <v>6</v>
       </c>
       <c r="C11" s="9">
+        <v>2</v>
+      </c>
+      <c r="D11" s="9">
         <v>31</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="E11" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="F11" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="F11" s="9">
-        <v>1</v>
-      </c>
-      <c r="G11" s="9"/>
+      <c r="G11" s="9">
+        <v>1</v>
+      </c>
       <c r="H11" s="9"/>
-      <c r="I11" s="9">
-        <v>1</v>
-      </c>
+      <c r="I11" s="9"/>
       <c r="J11" s="9">
         <v>1</v>
       </c>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9" t="s">
+      <c r="K11" s="9">
+        <v>1</v>
+      </c>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="M11" s="9">
+      <c r="N11" s="9">
         <v>7</v>
       </c>
-      <c r="N11" s="9" t="s">
+      <c r="O11" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="O11" s="9" t="s">
+      <c r="P11" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="P11" s="9">
+      <c r="Q11" s="9">
         <v>1431</v>
       </c>
-      <c r="Q11" s="9">
+      <c r="R11" s="9">
         <v>440</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A12" s="9">
         <v>13010008</v>
       </c>
@@ -2549,42 +2623,45 @@
         <v>8</v>
       </c>
       <c r="C12" s="9">
+        <v>2</v>
+      </c>
+      <c r="D12" s="9">
         <v>31</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="E12" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="F12" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="F12" s="9">
-        <v>1</v>
-      </c>
-      <c r="G12" s="9"/>
+      <c r="G12" s="9">
+        <v>1</v>
+      </c>
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
-      <c r="K12" s="9">
-        <v>1</v>
-      </c>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9">
+      <c r="K12" s="9"/>
+      <c r="L12" s="9">
+        <v>1</v>
+      </c>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9">
         <v>8</v>
       </c>
-      <c r="N12" s="9" t="s">
+      <c r="O12" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="O12" s="9" t="s">
+      <c r="P12" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="P12" s="9">
+      <c r="Q12" s="9">
         <v>1067</v>
       </c>
-      <c r="Q12" s="9">
+      <c r="R12" s="9">
         <v>445</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A13" s="9">
         <v>13010009</v>
       </c>
@@ -2592,44 +2669,47 @@
         <v>9</v>
       </c>
       <c r="C13" s="9">
+        <v>2</v>
+      </c>
+      <c r="D13" s="9">
         <v>31</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="E13" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="F13" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="F13" s="9">
-        <v>1</v>
-      </c>
       <c r="G13" s="9">
         <v>1</v>
       </c>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9">
-        <v>1</v>
-      </c>
-      <c r="J13" s="9"/>
+      <c r="H13" s="9">
+        <v>1</v>
+      </c>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9">
+        <v>1</v>
+      </c>
       <c r="K13" s="9"/>
       <c r="L13" s="9"/>
-      <c r="M13" s="9">
+      <c r="M13" s="9"/>
+      <c r="N13" s="9">
         <v>9</v>
       </c>
-      <c r="N13" s="9" t="s">
+      <c r="O13" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="O13" s="9" t="s">
+      <c r="P13" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="P13" s="9">
+      <c r="Q13" s="9">
         <v>1332</v>
       </c>
-      <c r="Q13" s="9">
+      <c r="R13" s="9">
         <v>484</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A14" s="9">
         <v>13010010</v>
       </c>
@@ -2637,40 +2717,43 @@
         <v>10</v>
       </c>
       <c r="C14" s="9">
+        <v>2</v>
+      </c>
+      <c r="D14" s="9">
         <v>31</v>
       </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="9"/>
+      <c r="F14" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="F14" s="9">
-        <v>1</v>
-      </c>
-      <c r="G14" s="9"/>
+      <c r="G14" s="9">
+        <v>1</v>
+      </c>
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
-      <c r="K14" s="9">
-        <v>1</v>
-      </c>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9">
+      <c r="K14" s="9"/>
+      <c r="L14" s="9">
+        <v>1</v>
+      </c>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9">
         <v>10</v>
       </c>
-      <c r="N14" s="9" t="s">
+      <c r="O14" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="O14" s="9" t="s">
+      <c r="P14" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="P14" s="9">
+      <c r="Q14" s="9">
         <v>1441</v>
       </c>
-      <c r="Q14" s="9">
+      <c r="R14" s="9">
         <v>527</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A15" s="9">
         <v>13010011</v>
       </c>
@@ -2678,44 +2761,47 @@
         <v>11</v>
       </c>
       <c r="C15" s="9">
+        <v>2</v>
+      </c>
+      <c r="D15" s="9">
         <v>31</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="E15" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="F15" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="F15" s="9">
-        <v>1</v>
-      </c>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9">
-        <v>1</v>
-      </c>
-      <c r="I15" s="9"/>
+      <c r="G15" s="9">
+        <v>1</v>
+      </c>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9">
+        <v>1</v>
+      </c>
       <c r="J15" s="9"/>
       <c r="K15" s="9"/>
-      <c r="L15" s="9" t="s">
+      <c r="L15" s="9"/>
+      <c r="M15" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="M15" s="9">
+      <c r="N15" s="9">
         <v>11</v>
       </c>
-      <c r="N15" s="9" t="s">
+      <c r="O15" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="O15" s="9" t="s">
+      <c r="P15" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="P15" s="9">
+      <c r="Q15" s="9">
         <v>1574</v>
       </c>
-      <c r="Q15" s="9">
+      <c r="R15" s="9">
         <v>373</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A16" s="9">
         <v>13010012</v>
       </c>
@@ -2723,38 +2809,41 @@
         <v>13</v>
       </c>
       <c r="C16" s="9">
+        <v>2</v>
+      </c>
+      <c r="D16" s="9">
         <v>4</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="E16" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9">
-        <v>1</v>
-      </c>
-      <c r="G16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9">
+        <v>1</v>
+      </c>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
       <c r="J16" s="9"/>
       <c r="K16" s="9"/>
       <c r="L16" s="9"/>
-      <c r="M16" s="9">
+      <c r="M16" s="9"/>
+      <c r="N16" s="9">
         <v>12</v>
       </c>
-      <c r="N16" s="9" t="s">
+      <c r="O16" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="O16" s="9" t="s">
+      <c r="P16" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="P16" s="9">
+      <c r="Q16" s="9">
         <v>1251</v>
       </c>
-      <c r="Q16" s="9">
+      <c r="R16" s="9">
         <v>432</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A17" s="9">
         <v>13010013</v>
       </c>
@@ -2762,38 +2851,41 @@
         <v>14</v>
       </c>
       <c r="C17" s="9">
+        <v>2</v>
+      </c>
+      <c r="D17" s="9">
         <v>31</v>
       </c>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9" t="s">
+      <c r="E17" s="9"/>
+      <c r="F17" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="F17" s="9">
-        <v>1</v>
-      </c>
-      <c r="G17" s="9"/>
+      <c r="G17" s="9">
+        <v>1</v>
+      </c>
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
       <c r="J17" s="9"/>
       <c r="K17" s="9"/>
       <c r="L17" s="9"/>
-      <c r="M17" s="9">
+      <c r="M17" s="9"/>
+      <c r="N17" s="9">
         <v>13</v>
       </c>
-      <c r="N17" s="9" t="s">
+      <c r="O17" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="O17" s="9" t="s">
+      <c r="P17" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="P17" s="9">
+      <c r="Q17" s="9">
         <v>1250</v>
       </c>
-      <c r="Q17" s="9">
+      <c r="R17" s="9">
         <v>338</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A18" s="9">
         <v>13010014</v>
       </c>
@@ -2801,44 +2893,47 @@
         <v>15</v>
       </c>
       <c r="C18" s="9">
+        <v>2</v>
+      </c>
+      <c r="D18" s="9">
         <v>31</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="E18" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="F18" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="F18" s="9">
-        <v>1</v>
-      </c>
-      <c r="G18" s="9"/>
+      <c r="G18" s="9">
+        <v>1</v>
+      </c>
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
-      <c r="J18" s="9">
-        <v>1</v>
-      </c>
+      <c r="J18" s="9"/>
       <c r="K18" s="9">
         <v>1</v>
       </c>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9">
+      <c r="L18" s="9">
+        <v>1</v>
+      </c>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9">
         <v>14</v>
       </c>
-      <c r="N18" s="9" t="s">
+      <c r="O18" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="O18" s="9" t="s">
+      <c r="P18" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="P18" s="9">
+      <c r="Q18" s="9">
         <v>1550</v>
       </c>
-      <c r="Q18" s="9">
+      <c r="R18" s="9">
         <v>505</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A19" s="9">
         <v>13010015</v>
       </c>
@@ -2846,42 +2941,45 @@
         <v>16</v>
       </c>
       <c r="C19" s="9">
+        <v>2</v>
+      </c>
+      <c r="D19" s="9">
         <v>31</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="E19" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="F19" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="F19" s="9">
-        <v>1</v>
-      </c>
-      <c r="G19" s="9"/>
+      <c r="G19" s="9">
+        <v>1</v>
+      </c>
       <c r="H19" s="9"/>
-      <c r="I19" s="9">
-        <v>1</v>
-      </c>
-      <c r="J19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9">
+        <v>1</v>
+      </c>
       <c r="K19" s="9"/>
       <c r="L19" s="9"/>
-      <c r="M19" s="9">
+      <c r="M19" s="9"/>
+      <c r="N19" s="9">
         <v>15</v>
       </c>
-      <c r="N19" s="9" t="s">
+      <c r="O19" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="O19" s="9" t="s">
+      <c r="P19" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="P19" s="9">
+      <c r="Q19" s="9">
         <v>1040</v>
       </c>
-      <c r="Q19" s="9">
+      <c r="R19" s="9">
         <v>538</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A20" s="9">
         <v>13010016</v>
       </c>
@@ -2889,9 +2987,11 @@
         <v>17</v>
       </c>
       <c r="C20" s="9">
+        <v>1</v>
+      </c>
+      <c r="D20" s="9">
         <v>31</v>
       </c>
-      <c r="D20" s="9"/>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
@@ -2900,23 +3000,24 @@
       <c r="J20" s="9"/>
       <c r="K20" s="9"/>
       <c r="L20" s="9"/>
-      <c r="M20" s="9">
+      <c r="M20" s="9"/>
+      <c r="N20" s="9">
         <v>16</v>
       </c>
-      <c r="N20" s="9" t="s">
+      <c r="O20" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="O20" s="9" t="s">
+      <c r="P20" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="P20" s="9">
+      <c r="Q20" s="9">
         <v>919</v>
       </c>
-      <c r="Q20" s="9">
+      <c r="R20" s="9">
         <v>534</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A21" s="9">
         <v>13010017</v>
       </c>
@@ -2924,42 +3025,45 @@
         <v>49</v>
       </c>
       <c r="C21" s="9">
+        <v>2</v>
+      </c>
+      <c r="D21" s="9">
         <v>31</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="E21" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="F21" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="F21" s="9">
-        <v>1</v>
-      </c>
-      <c r="G21" s="9"/>
+      <c r="G21" s="9">
+        <v>1</v>
+      </c>
       <c r="H21" s="9"/>
       <c r="I21" s="9"/>
-      <c r="J21" s="9">
-        <v>1</v>
-      </c>
-      <c r="K21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9">
+        <v>1</v>
+      </c>
       <c r="L21" s="9"/>
-      <c r="M21" s="9">
+      <c r="M21" s="9"/>
+      <c r="N21" s="9">
         <v>18</v>
       </c>
-      <c r="N21" s="9" t="s">
+      <c r="O21" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="O21" s="9" t="s">
+      <c r="P21" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="P21" s="9">
+      <c r="Q21" s="9">
         <v>1149</v>
       </c>
-      <c r="Q21" s="9">
+      <c r="R21" s="9">
         <v>584</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A22" s="9">
         <v>13010018</v>
       </c>
@@ -2967,17 +3071,17 @@
         <v>50</v>
       </c>
       <c r="C22" s="9">
+        <v>2</v>
+      </c>
+      <c r="D22" s="9">
         <v>31</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="E22" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="E22" s="9" t="s">
+      <c r="F22" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="F22" s="9">
-        <v>1</v>
-      </c>
       <c r="G22" s="9">
         <v>1</v>
       </c>
@@ -2987,35 +3091,38 @@
       <c r="I22" s="9">
         <v>1</v>
       </c>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9">
-        <v>1</v>
-      </c>
-      <c r="L22" s="9"/>
-      <c r="M22" s="9">
+      <c r="J22" s="9">
+        <v>1</v>
+      </c>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9">
+        <v>1</v>
+      </c>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9">
         <v>19</v>
       </c>
-      <c r="N22" s="9" t="s">
+      <c r="O22" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="O22" s="9" t="s">
+      <c r="P22" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="P22" s="9">
+      <c r="Q22" s="9">
         <v>840</v>
       </c>
-      <c r="Q22" s="9">
+      <c r="R22" s="9">
         <v>444</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="F4:K22">
+  <conditionalFormatting sqref="G4:L22">
     <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4">
+  <conditionalFormatting sqref="H4">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
finish the scenequest aolai
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Scene.xlsx
+++ b/ConfigData/Xlsx/Scene.xlsx
@@ -403,10 +403,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>poppyfield;1|ruintown1;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>river;2|stone;3|ruintown1;1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -456,6 +452,10 @@
   </si>
   <si>
     <t>forestfire;10</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ruintown1;1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -2092,7 +2092,7 @@
   <dimension ref="A1:R22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2119,7 +2119,7 @@
         <v>21</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>22</v>
@@ -2128,7 +2128,7 @@
         <v>37</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>59</v>
@@ -2175,7 +2175,7 @@
         <v>19</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>18</v>
@@ -2184,7 +2184,7 @@
         <v>97</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>58</v>
@@ -2231,7 +2231,7 @@
         <v>26</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>27</v>
@@ -2240,7 +2240,7 @@
         <v>36</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G3" s="11" t="s">
         <v>60</v>
@@ -2340,7 +2340,7 @@
         <v>107</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G5" s="9">
         <v>1</v>
@@ -2388,7 +2388,7 @@
         <v>108</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G6" s="9">
         <v>1</v>
@@ -2467,10 +2467,10 @@
         <v>5</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G8" s="9">
         <v>1</v>
@@ -2596,7 +2596,7 @@
         <v>105</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G11" s="9">
         <v>1</v>
@@ -2646,7 +2646,7 @@
         <v>98</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G12" s="9">
         <v>1</v>
@@ -2689,10 +2689,10 @@
         <v>4</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G13" s="9">
         <v>1</v>
@@ -2738,7 +2738,7 @@
       </c>
       <c r="E14" s="9"/>
       <c r="F14" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G14" s="9">
         <v>1</v>
@@ -2784,7 +2784,7 @@
         <v>106</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G15" s="9">
         <v>1</v>
@@ -2832,7 +2832,7 @@
         <v>104</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G16" s="9">
         <v>1</v>
@@ -2874,7 +2874,7 @@
       </c>
       <c r="E17" s="9"/>
       <c r="F17" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G17" s="9">
         <v>1</v>
@@ -2918,7 +2918,7 @@
         <v>100</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G18" s="9">
         <v>1</v>
@@ -2966,7 +2966,7 @@
         <v>99</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G19" s="9">
         <v>1</v>
@@ -3050,7 +3050,7 @@
         <v>102</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G21" s="9">
         <v>1</v>
@@ -3096,7 +3096,7 @@
         <v>101</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G22" s="9">
         <v>1</v>

</xml_diff>

<commit_message>
add the function of HiddenWay
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Scene.xlsx
+++ b/ConfigData/Xlsx/Scene.xlsx
@@ -375,10 +375,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>mushroom;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>sewer;3|river;2|fortune;1|oldtree;1|poppyfield;1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -387,10 +383,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>portal;1|fishpool;1|grave;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>fortune;1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -403,10 +395,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>river;2|stone;3|ruintown1;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>小概率任务</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -456,6 +444,18 @@
   </si>
   <si>
     <t>ruintown1;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>river;2|stone;3|ruintown1;1|hiddeway;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>portal;1|fishpool;1|grave;2|hiddeway;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>mushroom;1|hiddeway;1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -2092,7 +2092,7 @@
   <dimension ref="A1:R22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2119,7 +2119,7 @@
         <v>21</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>22</v>
@@ -2128,7 +2128,7 @@
         <v>37</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>59</v>
@@ -2175,7 +2175,7 @@
         <v>19</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>18</v>
@@ -2184,7 +2184,7 @@
         <v>97</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>58</v>
@@ -2231,7 +2231,7 @@
         <v>26</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>27</v>
@@ -2240,7 +2240,7 @@
         <v>36</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G3" s="11" t="s">
         <v>60</v>
@@ -2293,7 +2293,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F4" s="9"/>
       <c r="G4" s="9">
@@ -2337,10 +2337,10 @@
         <v>2</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G5" s="9">
         <v>1</v>
@@ -2385,10 +2385,10 @@
         <v>19</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="G6" s="9">
         <v>1</v>
@@ -2467,10 +2467,10 @@
         <v>5</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="G8" s="9">
         <v>1</v>
@@ -2593,10 +2593,10 @@
         <v>7</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>105</v>
+        <v>121</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="G11" s="9">
         <v>1</v>
@@ -2646,7 +2646,7 @@
         <v>98</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="G12" s="9">
         <v>1</v>
@@ -2689,10 +2689,10 @@
         <v>4</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="G13" s="9">
         <v>1</v>
@@ -2738,7 +2738,7 @@
       </c>
       <c r="E14" s="9"/>
       <c r="F14" s="9" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="G14" s="9">
         <v>1</v>
@@ -2781,10 +2781,10 @@
         <v>12</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="G15" s="9">
         <v>1</v>
@@ -2829,10 +2829,10 @@
         <v>3</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="G16" s="9">
         <v>1</v>
@@ -2874,7 +2874,7 @@
       </c>
       <c r="E17" s="9"/>
       <c r="F17" s="9" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="G17" s="9">
         <v>1</v>
@@ -2918,7 +2918,7 @@
         <v>100</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="G18" s="9">
         <v>1</v>
@@ -2966,7 +2966,7 @@
         <v>99</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="G19" s="9">
         <v>1</v>
@@ -3047,10 +3047,10 @@
         <v>18</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>102</v>
+        <v>122</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="G21" s="9">
         <v>1</v>
@@ -3096,7 +3096,7 @@
         <v>101</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="G22" s="9">
         <v>1</v>

</xml_diff>

<commit_message>
finish quest swamp and flowsand
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Scene.xlsx
+++ b/ConfigData/Xlsx/Scene.xlsx
@@ -363,14 +363,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>portal;3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>river;2|fishpool;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>trees;3|mushroom;1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -391,10 +383,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>sandpile;1|stone;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>小概率任务</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -455,7 +443,19 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>mushroom;1|hiddeway;1</t>
+    <t>river;2|fishpool;1|swamp;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>mushroom;1|hiddeway;1|swamp;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>portal;3|sandflow;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>sandpile;1|stone;2|sandflow;2</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -2092,7 +2092,7 @@
   <dimension ref="A1:R22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2119,7 +2119,7 @@
         <v>21</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>22</v>
@@ -2128,7 +2128,7 @@
         <v>37</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>59</v>
@@ -2175,7 +2175,7 @@
         <v>19</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>18</v>
@@ -2184,7 +2184,7 @@
         <v>97</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>58</v>
@@ -2231,7 +2231,7 @@
         <v>26</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>27</v>
@@ -2240,7 +2240,7 @@
         <v>36</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G3" s="11" t="s">
         <v>60</v>
@@ -2293,7 +2293,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F4" s="9"/>
       <c r="G4" s="9">
@@ -2337,10 +2337,10 @@
         <v>2</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G5" s="9">
         <v>1</v>
@@ -2385,10 +2385,10 @@
         <v>19</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="G6" s="9">
         <v>1</v>
@@ -2467,10 +2467,10 @@
         <v>5</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="G8" s="9">
         <v>1</v>
@@ -2593,10 +2593,10 @@
         <v>7</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="G11" s="9">
         <v>1</v>
@@ -2646,7 +2646,7 @@
         <v>98</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G12" s="9">
         <v>1</v>
@@ -2689,10 +2689,10 @@
         <v>4</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G13" s="9">
         <v>1</v>
@@ -2738,7 +2738,7 @@
       </c>
       <c r="E14" s="9"/>
       <c r="F14" s="9" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G14" s="9">
         <v>1</v>
@@ -2781,10 +2781,10 @@
         <v>12</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G15" s="9">
         <v>1</v>
@@ -2829,10 +2829,10 @@
         <v>3</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G16" s="9">
         <v>1</v>
@@ -2874,7 +2874,7 @@
       </c>
       <c r="E17" s="9"/>
       <c r="F17" s="9" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G17" s="9">
         <v>1</v>
@@ -2915,10 +2915,10 @@
         <v>14</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>100</v>
+        <v>119</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G18" s="9">
         <v>1</v>
@@ -2963,10 +2963,10 @@
         <v>16</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>99</v>
+        <v>121</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G19" s="9">
         <v>1</v>
@@ -3047,10 +3047,10 @@
         <v>18</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G21" s="9">
         <v>1</v>
@@ -3093,10 +3093,10 @@
         <v>20</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="G22" s="9">
         <v>1</v>

</xml_diff>

<commit_message>
finish the function of bless system close #97
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Scene.xlsx
+++ b/ConfigData/Xlsx/Scene.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17571"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="126">
   <si>
     <t>村外小屋</t>
   </si>
@@ -415,11 +415,50 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>forestfire;35</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|forestfire;20</t>
+    <t>portal;1|fishpool;1|grave;2|hiddeway;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>river;2|fishpool;1|swamp;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>mushroom;1|hiddeway;1|swamp;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>orehole;1|stone;2|sandflow;2</t>
+  </si>
+  <si>
+    <t>coldwind;3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ruintown1;1|manflower;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trees;3|grave;1|portal;1|oldtree;1|manflower;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>portal;3|sandflow;2|manflower;3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>river;2|stone;3|ruintown1;1|hiddeway;1|manflower;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|witchhome;30</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|treasure;25|witchhome;20</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|forestfire;20|witchhome;40</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -427,45 +466,14 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>portal;1|fishpool;1|grave;2|hiddeway;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>river;2|fishpool;1|swamp;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>mushroom;1|hiddeway;1|swamp;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>orehole;1|stone;2|sandflow;2</t>
-  </si>
-  <si>
-    <t>coldwind;3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ruintown1;1|manflower;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>trees;3|grave;1|portal;1|oldtree;1|manflower;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>portal;3|sandflow;2|manflower;3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>river;2|stone;3|ruintown1;1|hiddeway;1|manflower;2</t>
+    <t>forestfire;35|witchhome;10</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1806,7 +1814,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1881,6 +1889,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1916,6 +1941,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2095,7 +2137,7 @@
   <dimension ref="A1:R22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2343,7 +2385,7 @@
         <v>102</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="G5" s="9">
         <v>1</v>
@@ -2388,7 +2430,7 @@
         <v>19</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>107</v>
@@ -2470,10 +2512,10 @@
         <v>5</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>107</v>
+        <v>122</v>
       </c>
       <c r="G8" s="9">
         <v>1</v>
@@ -2596,7 +2638,7 @@
         <v>7</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F11" s="9" t="s">
         <v>107</v>
@@ -2692,7 +2734,7 @@
         <v>4</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>106</v>
@@ -2832,10 +2874,10 @@
         <v>3</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
       <c r="G16" s="9">
         <v>1</v>
@@ -2876,7 +2918,7 @@
         <v>6</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F17" s="9" t="s">
         <v>106</v>
@@ -2920,10 +2962,10 @@
         <v>14</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>106</v>
+        <v>121</v>
       </c>
       <c r="G18" s="9">
         <v>1</v>
@@ -2968,7 +3010,7 @@
         <v>16</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F19" s="9" t="s">
         <v>106</v>
@@ -3052,7 +3094,7 @@
         <v>18</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F21" s="9" t="s">
         <v>106</v>
@@ -3101,7 +3143,7 @@
         <v>99</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="G22" s="9">
         <v>1</v>

</xml_diff>

<commit_message>
#98 dungeon has a startpos and different random quest method now
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Scene.xlsx
+++ b/ConfigData/Xlsx/Scene.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="150">
   <si>
     <t>村外小屋</t>
   </si>
@@ -159,314 +159,412 @@
     <t>smallforest</t>
   </si>
   <si>
+    <t>perse</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>demlock</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>hightower</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>smallhill</t>
+  </si>
+  <si>
+    <t>goldseashore</t>
+  </si>
+  <si>
+    <t>islandold</t>
+  </si>
+  <si>
+    <t>riverold</t>
+  </si>
+  <si>
+    <t>落潮小径</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>月光林地</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>gerdin</t>
+  </si>
+  <si>
+    <t>fogvalley</t>
+  </si>
+  <si>
+    <t>矿脉山脚</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>riverside</t>
+  </si>
+  <si>
+    <t>woodviliage</t>
+  </si>
+  <si>
+    <t>moonforest</t>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>激活传送门</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QPortal</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QCardChange</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>卡牌交换</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>素材商人</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QPiece</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QMerchant</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QDoctor</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QAngel</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>商人</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>医生</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>天使</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>IconX</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>IconY</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Icon</t>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwxw</t>
+  </si>
+  <si>
+    <t>haml</t>
+  </si>
+  <si>
+    <t>kk</t>
+  </si>
+  <si>
+    <t>dlkxg</t>
+  </si>
+  <si>
+    <t>bstgt</t>
+  </si>
+  <si>
+    <t>ttmc</t>
+  </si>
+  <si>
+    <t>psgc</t>
+  </si>
+  <si>
+    <t>gdh</t>
+  </si>
+  <si>
+    <t>cwyy</t>
+  </si>
+  <si>
+    <t>hjha</t>
+  </si>
+  <si>
+    <t>gdyj</t>
+  </si>
+  <si>
+    <t>xsl</t>
+  </si>
+  <si>
+    <t>llf</t>
+  </si>
+  <si>
+    <t>yjht</t>
+  </si>
+  <si>
+    <t>wg</t>
+  </si>
+  <si>
+    <t>myzc</t>
+  </si>
+  <si>
+    <t>lcxj</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ygld</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>小图标x</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>小图标y</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>图标路径</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>GameUpToNumber;GameThreeBody</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>poppyfield;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trees;3|mushroom;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>sewer;3|river;2|fortune;1|oldtree;1|poppyfield;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>fortune;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>wolfnest;2|gamble;1|fishpool;2|sewer;3|river;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>小概率任务</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QuestRandom</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|treasure;25</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>类型</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Type</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>portal;1|fishpool;1|grave;2|hiddeway;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>river;2|fishpool;1|swamp;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>mushroom;1|hiddeway;1|swamp;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>orehole;1|stone;2|sandflow;2</t>
+  </si>
+  <si>
+    <t>coldwind;3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ruintown1;1|manflower;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trees;3|grave;1|portal;1|oldtree;1|manflower;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>portal;3|sandflow;2|manflower;3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>river;2|stone;3|ruintown1;1|hiddeway;1|manflower;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|witchhome;30</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|treasure;25|witchhome;20</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|forestfire;20|witchhome;40</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>forestfire;10</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>forestfire;35|witchhome;10</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>密林迷宫</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>迷宫深处</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>home</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>orevalley</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>default</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>hightower</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>tatamuviliage</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>perse</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>gerdin</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>farm</t>
-  </si>
-  <si>
-    <t>perse</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>demlock</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>hightower</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>farm</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>goldseashore</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>islandold</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>smallforest</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>smallhill</t>
-  </si>
-  <si>
-    <t>goldseashore</t>
-  </si>
-  <si>
-    <t>islandold</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>riverold</t>
-  </si>
-  <si>
-    <t>落潮小径</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>月光林地</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>gerdin</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>fogvalley</t>
-  </si>
-  <si>
-    <t>矿脉山脚</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>woodviliage</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>riverside</t>
-  </si>
-  <si>
-    <t>orevalley</t>
-  </si>
-  <si>
-    <t>woodviliage</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>moonforest</t>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>激活传送门</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>QPortal</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>QCardChange</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>卡牌交换</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>素材商人</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>QPiece</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>QMerchant</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>QDoctor</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>QAngel</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>商人</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>医生</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>天使</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>IconX</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>IconY</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Icon</t>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>cwxw</t>
-  </si>
-  <si>
-    <t>haml</t>
-  </si>
-  <si>
-    <t>kk</t>
-  </si>
-  <si>
-    <t>dlkxg</t>
-  </si>
-  <si>
-    <t>bstgt</t>
-  </si>
-  <si>
-    <t>ttmc</t>
-  </si>
-  <si>
-    <t>psgc</t>
-  </si>
-  <si>
-    <t>gdh</t>
-  </si>
-  <si>
-    <t>cwyy</t>
-  </si>
-  <si>
-    <t>hjha</t>
-  </si>
-  <si>
-    <t>gdyj</t>
-  </si>
-  <si>
-    <t>xsl</t>
-  </si>
-  <si>
-    <t>llf</t>
-  </si>
-  <si>
-    <t>yjht</t>
-  </si>
-  <si>
-    <t>wg</t>
-  </si>
-  <si>
-    <t>myzc</t>
-  </si>
-  <si>
-    <t>lcxj</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ygld</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>小图标x</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>小图标y</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>图标路径</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>GameUpToNumber;GameThreeBody</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>poppyfield;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>trees;3|mushroom;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>sewer;3|river;2|fortune;1|oldtree;1|poppyfield;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>fortune;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>wolfnest;2|gamble;1|fishpool;2|sewer;3|river;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>小概率任务</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>QuestRandom</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|treasure;25</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>类型</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Type</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>portal;1|fishpool;1|grave;2|hiddeway;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>river;2|fishpool;1|swamp;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>mushroom;1|hiddeway;1|swamp;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>orehole;1|stone;2|sandflow;2</t>
-  </si>
-  <si>
-    <t>coldwind;3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ruintown1;1|manflower;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>trees;3|grave;1|portal;1|oldtree;1|manflower;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>portal;3|sandflow;2|manflower;3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>river;2|stone;3|ruintown1;1|hiddeway;1|manflower;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|witchhome;30</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|treasure;25|witchhome;20</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|forestfire;20|witchhome;40</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>forestfire;10</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>forestfire;35|witchhome;10</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>forestmaze</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>forestinner</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trees;3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trees;3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|forestfire;20</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|forestfire;20</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1787,8 +1885,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:R22" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" tableBorderDxfId="18">
-  <autoFilter ref="A3:R22"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:R24" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" tableBorderDxfId="18">
+  <autoFilter ref="A3:R24"/>
   <tableColumns count="18">
     <tableColumn id="1" name="Id" dataDxfId="17"/>
     <tableColumn id="2" name="Name" dataDxfId="16"/>
@@ -2134,10 +2232,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R22"/>
+  <dimension ref="A1:R24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2150,8 +2248,8 @@
     <col min="6" max="6" width="16.625" customWidth="1"/>
     <col min="7" max="12" width="3.125" customWidth="1"/>
     <col min="13" max="13" width="6.625" customWidth="1"/>
-    <col min="14" max="14" width="4" customWidth="1"/>
-    <col min="15" max="15" width="12.875" customWidth="1"/>
+    <col min="14" max="14" width="9.75" customWidth="1"/>
+    <col min="15" max="15" width="9.5" customWidth="1"/>
     <col min="16" max="16" width="7.25" customWidth="1"/>
     <col min="17" max="18" width="6" customWidth="1"/>
   </cols>
@@ -2164,7 +2262,7 @@
         <v>21</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>22</v>
@@ -2173,25 +2271,25 @@
         <v>37</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J1" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="L1" s="7" t="s">
         <v>68</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>70</v>
       </c>
       <c r="M1" s="6" t="s">
         <v>23</v>
@@ -2203,13 +2301,13 @@
         <v>33</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="R1" s="8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.15">
@@ -2220,46 +2318,46 @@
         <v>19</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>32</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>18</v>
@@ -2276,7 +2374,7 @@
         <v>26</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>27</v>
@@ -2285,25 +2383,25 @@
         <v>36</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I3" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="K3" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="L3" s="11" t="s">
         <v>65</v>
-      </c>
-      <c r="K3" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="L3" s="11" t="s">
-        <v>67</v>
       </c>
       <c r="M3" s="10" t="s">
         <v>28</v>
@@ -2315,13 +2413,13 @@
         <v>31</v>
       </c>
       <c r="P3" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="Q3" s="10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="R3" s="10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.15">
@@ -2338,7 +2436,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F4" s="9"/>
       <c r="G4" s="9">
@@ -2350,16 +2448,16 @@
       <c r="K4" s="9"/>
       <c r="L4" s="9"/>
       <c r="M4" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="N4" s="9">
-        <v>2</v>
+        <v>94</v>
+      </c>
+      <c r="N4" s="9" t="s">
+        <v>126</v>
       </c>
       <c r="O4" s="9" t="s">
         <v>35</v>
       </c>
       <c r="P4" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="Q4" s="9">
         <v>1348</v>
@@ -2382,10 +2480,10 @@
         <v>2</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G5" s="9">
         <v>1</v>
@@ -2400,14 +2498,14 @@
       </c>
       <c r="L5" s="9"/>
       <c r="M5" s="9"/>
-      <c r="N5" s="9">
-        <v>3</v>
+      <c r="N5" s="9" t="s">
+        <v>38</v>
       </c>
       <c r="O5" s="9" t="s">
         <v>38</v>
       </c>
       <c r="P5" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="Q5" s="9">
         <v>1279</v>
@@ -2421,7 +2519,7 @@
         <v>13000003</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" s="9">
         <v>2</v>
@@ -2430,10 +2528,10 @@
         <v>19</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G6" s="9">
         <v>1</v>
@@ -2444,14 +2542,14 @@
       <c r="K6" s="9"/>
       <c r="L6" s="9"/>
       <c r="M6" s="9"/>
-      <c r="N6" s="9">
-        <v>17</v>
+      <c r="N6" s="9" t="s">
+        <v>127</v>
       </c>
       <c r="O6" s="9" t="s">
-        <v>55</v>
+        <v>127</v>
       </c>
       <c r="P6" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="Q6" s="9">
         <v>1213</v>
@@ -2484,19 +2582,15 @@
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
       <c r="M7" s="9"/>
-      <c r="N7" s="9">
-        <v>1</v>
+      <c r="N7" s="9" t="s">
+        <v>128</v>
       </c>
       <c r="O7" s="9" t="s">
         <v>34</v>
       </c>
       <c r="P7" s="9"/>
-      <c r="Q7" s="9">
-        <v>0</v>
-      </c>
-      <c r="R7" s="9">
-        <v>0</v>
-      </c>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A8" s="9">
@@ -2512,10 +2606,10 @@
         <v>5</v>
       </c>
       <c r="E8" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="F8" s="9" t="s">
         <v>120</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>122</v>
       </c>
       <c r="G8" s="9">
         <v>1</v>
@@ -2528,14 +2622,14 @@
       <c r="K8" s="9"/>
       <c r="L8" s="9"/>
       <c r="M8" s="9"/>
-      <c r="N8" s="9">
-        <v>4</v>
+      <c r="N8" s="9" t="s">
+        <v>42</v>
       </c>
       <c r="O8" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P8" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Q8" s="9">
         <v>1148</v>
@@ -2570,14 +2664,14 @@
       <c r="K9" s="9"/>
       <c r="L9" s="9"/>
       <c r="M9" s="9"/>
-      <c r="N9" s="9">
-        <v>5</v>
+      <c r="N9" s="9" t="s">
+        <v>129</v>
       </c>
       <c r="O9" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P9" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Q9" s="9">
         <v>1386</v>
@@ -2608,14 +2702,14 @@
       <c r="K10" s="9"/>
       <c r="L10" s="9"/>
       <c r="M10" s="9"/>
-      <c r="N10" s="9">
-        <v>6</v>
+      <c r="N10" s="9" t="s">
+        <v>130</v>
       </c>
       <c r="O10" s="9" t="s">
         <v>39</v>
       </c>
       <c r="P10" s="9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="Q10" s="9">
         <v>1232</v>
@@ -2638,10 +2732,10 @@
         <v>7</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G11" s="9">
         <v>1</v>
@@ -2658,14 +2752,14 @@
       <c r="M11" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="N11" s="9">
-        <v>7</v>
+      <c r="N11" s="9" t="s">
+        <v>131</v>
       </c>
       <c r="O11" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P11" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="Q11" s="9">
         <v>1431</v>
@@ -2688,10 +2782,10 @@
         <v>15</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G12" s="9">
         <v>1</v>
@@ -2704,14 +2798,14 @@
         <v>1</v>
       </c>
       <c r="M12" s="9"/>
-      <c r="N12" s="9">
-        <v>8</v>
+      <c r="N12" s="9" t="s">
+        <v>132</v>
       </c>
       <c r="O12" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P12" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="Q12" s="9">
         <v>1067</v>
@@ -2734,10 +2828,10 @@
         <v>4</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G13" s="9">
         <v>1</v>
@@ -2752,14 +2846,14 @@
       <c r="K13" s="9"/>
       <c r="L13" s="9"/>
       <c r="M13" s="9"/>
-      <c r="N13" s="9">
-        <v>9</v>
+      <c r="N13" s="9" t="s">
+        <v>134</v>
       </c>
       <c r="O13" s="9" t="s">
-        <v>41</v>
+        <v>133</v>
       </c>
       <c r="P13" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="Q13" s="9">
         <v>1332</v>
@@ -2783,7 +2877,7 @@
       </c>
       <c r="E14" s="9"/>
       <c r="F14" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G14" s="9">
         <v>1</v>
@@ -2796,14 +2890,14 @@
         <v>1</v>
       </c>
       <c r="M14" s="9"/>
-      <c r="N14" s="9">
-        <v>10</v>
+      <c r="N14" s="9" t="s">
+        <v>135</v>
       </c>
       <c r="O14" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P14" s="9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="Q14" s="9">
         <v>1441</v>
@@ -2826,10 +2920,10 @@
         <v>12</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G15" s="9">
         <v>1</v>
@@ -2844,14 +2938,14 @@
       <c r="M15" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="N15" s="9">
-        <v>11</v>
+      <c r="N15" s="9" t="s">
+        <v>136</v>
       </c>
       <c r="O15" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P15" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="Q15" s="9">
         <v>1574</v>
@@ -2874,10 +2968,10 @@
         <v>3</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G16" s="9">
         <v>1</v>
@@ -2888,14 +2982,14 @@
       <c r="K16" s="9"/>
       <c r="L16" s="9"/>
       <c r="M16" s="9"/>
-      <c r="N16" s="9">
-        <v>12</v>
+      <c r="N16" s="9" t="s">
+        <v>137</v>
       </c>
       <c r="O16" s="9" t="s">
         <v>40</v>
       </c>
       <c r="P16" s="9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="Q16" s="9">
         <v>1251</v>
@@ -2918,10 +3012,10 @@
         <v>6</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G17" s="9">
         <v>1</v>
@@ -2932,14 +3026,14 @@
       <c r="K17" s="9"/>
       <c r="L17" s="9"/>
       <c r="M17" s="9"/>
-      <c r="N17" s="9">
-        <v>13</v>
+      <c r="N17" s="9" t="s">
+        <v>138</v>
       </c>
       <c r="O17" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P17" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="Q17" s="9">
         <v>1250</v>
@@ -2962,10 +3056,10 @@
         <v>14</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G18" s="9">
         <v>1</v>
@@ -2980,14 +3074,14 @@
         <v>1</v>
       </c>
       <c r="M18" s="9"/>
-      <c r="N18" s="9">
-        <v>14</v>
+      <c r="N18" s="9" t="s">
+        <v>139</v>
       </c>
       <c r="O18" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P18" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="Q18" s="9">
         <v>1550</v>
@@ -3010,10 +3104,10 @@
         <v>16</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G19" s="9">
         <v>1</v>
@@ -3026,14 +3120,14 @@
       <c r="K19" s="9"/>
       <c r="L19" s="9"/>
       <c r="M19" s="9"/>
-      <c r="N19" s="9">
-        <v>15</v>
+      <c r="N19" s="9" t="s">
+        <v>140</v>
       </c>
       <c r="O19" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P19" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="Q19" s="9">
         <v>1040</v>
@@ -3064,14 +3158,14 @@
       <c r="K20" s="9"/>
       <c r="L20" s="9"/>
       <c r="M20" s="9"/>
-      <c r="N20" s="9">
-        <v>16</v>
+      <c r="N20" s="9" t="s">
+        <v>141</v>
       </c>
       <c r="O20" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="P20" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Q20" s="9">
         <v>919</v>
@@ -3085,7 +3179,7 @@
         <v>13010017</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C21" s="9">
         <v>2</v>
@@ -3094,10 +3188,10 @@
         <v>18</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G21" s="9">
         <v>1</v>
@@ -3110,14 +3204,14 @@
       </c>
       <c r="L21" s="9"/>
       <c r="M21" s="9"/>
-      <c r="N21" s="9">
-        <v>18</v>
+      <c r="N21" s="9" t="s">
+        <v>142</v>
       </c>
       <c r="O21" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="P21" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="Q21" s="9">
         <v>1149</v>
@@ -3131,7 +3225,7 @@
         <v>13010018</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C22" s="9">
         <v>2</v>
@@ -3140,36 +3234,26 @@
         <v>20</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="G22" s="9">
-        <v>1</v>
-      </c>
-      <c r="H22" s="9">
-        <v>1</v>
-      </c>
-      <c r="I22" s="9">
-        <v>1</v>
-      </c>
-      <c r="J22" s="9">
-        <v>1</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
       <c r="K22" s="9"/>
-      <c r="L22" s="9">
-        <v>1</v>
-      </c>
+      <c r="L22" s="9"/>
       <c r="M22" s="9"/>
-      <c r="N22" s="9">
-        <v>19</v>
+      <c r="N22" s="9" t="s">
+        <v>143</v>
       </c>
       <c r="O22" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="P22" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="Q22" s="9">
         <v>840</v>
@@ -3177,10 +3261,82 @@
       <c r="R22" s="9">
         <v>444</v>
       </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A23" s="9">
+        <v>13020001</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C23" s="9">
+        <v>3</v>
+      </c>
+      <c r="D23" s="9">
+        <v>3</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="O23" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="9"/>
+      <c r="R23" s="9"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A24" s="9">
+        <v>13020002</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="C24" s="9">
+        <v>3</v>
+      </c>
+      <c r="D24" s="9">
+        <v>3</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="O24" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="9"/>
+      <c r="R24" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="G4:L22">
+  <conditionalFormatting sqref="G4:L24">
     <cfRule type="cellIs" dxfId="22" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
#98 save the random seed for scene generate
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Scene.xlsx
+++ b/ConfigData/Xlsx/Scene.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="150">
   <si>
     <t>村外小屋</t>
   </si>
@@ -556,15 +556,15 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>trees;3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|forestfire;20</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|forestfire;20</t>
+    <t>副本任务列表</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QuestDungeon</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>forestentry;2|forestentry2;2</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -572,7 +572,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -751,6 +751,13 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="37">
     <fill>
@@ -1232,7 +1239,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1267,6 +1274,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1314,33 +1327,20 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="24">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1680,6 +1680,62 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -1857,20 +1913,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1885,27 +1927,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:R24" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" tableBorderDxfId="18">
-  <autoFilter ref="A3:R24"/>
-  <tableColumns count="18">
-    <tableColumn id="1" name="Id" dataDxfId="17"/>
-    <tableColumn id="2" name="Name" dataDxfId="16"/>
-    <tableColumn id="18" name="Type" dataDxfId="15"/>
-    <tableColumn id="3" name="Level" dataDxfId="14"/>
-    <tableColumn id="4" name="Quest" dataDxfId="13"/>
-    <tableColumn id="17" name="QuestRandom" dataDxfId="12"/>
-    <tableColumn id="5" name="QPortal" dataDxfId="11"/>
-    <tableColumn id="6" name="QCardChange" dataDxfId="10"/>
-    <tableColumn id="7" name="QPiece" dataDxfId="9"/>
-    <tableColumn id="8" name="QMerchant" dataDxfId="8"/>
-    <tableColumn id="9" name="QDoctor" dataDxfId="7"/>
-    <tableColumn id="10" name="QAngel" dataDxfId="6"/>
-    <tableColumn id="11" name="Func" dataDxfId="5"/>
-    <tableColumn id="12" name="Url" dataDxfId="4"/>
-    <tableColumn id="13" name="TilePath" dataDxfId="3"/>
-    <tableColumn id="14" name="Icon" dataDxfId="2"/>
-    <tableColumn id="15" name="IconX" dataDxfId="1"/>
-    <tableColumn id="16" name="IconY" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:S24" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22" tableBorderDxfId="21">
+  <autoFilter ref="A3:S24"/>
+  <tableColumns count="19">
+    <tableColumn id="1" name="Id" dataDxfId="20"/>
+    <tableColumn id="2" name="Name" dataDxfId="19"/>
+    <tableColumn id="18" name="Type" dataDxfId="18"/>
+    <tableColumn id="3" name="Level" dataDxfId="17"/>
+    <tableColumn id="4" name="Quest" dataDxfId="16"/>
+    <tableColumn id="17" name="QuestRandom" dataDxfId="15"/>
+    <tableColumn id="19" name="QuestDungeon" dataDxfId="14"/>
+    <tableColumn id="5" name="QPortal" dataDxfId="13"/>
+    <tableColumn id="6" name="QCardChange" dataDxfId="12"/>
+    <tableColumn id="7" name="QPiece" dataDxfId="11"/>
+    <tableColumn id="8" name="QMerchant" dataDxfId="10"/>
+    <tableColumn id="9" name="QDoctor" dataDxfId="9"/>
+    <tableColumn id="10" name="QAngel" dataDxfId="8"/>
+    <tableColumn id="11" name="Func" dataDxfId="7"/>
+    <tableColumn id="12" name="Url" dataDxfId="6"/>
+    <tableColumn id="13" name="TilePath" dataDxfId="5"/>
+    <tableColumn id="14" name="Icon" dataDxfId="4"/>
+    <tableColumn id="15" name="IconX" dataDxfId="3"/>
+    <tableColumn id="16" name="IconY" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2232,10 +2275,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R24"/>
+  <dimension ref="A1:S24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2246,15 +2289,16 @@
     <col min="4" max="4" width="4.375" customWidth="1"/>
     <col min="5" max="5" width="52.875" customWidth="1"/>
     <col min="6" max="6" width="16.625" customWidth="1"/>
-    <col min="7" max="12" width="3.125" customWidth="1"/>
-    <col min="13" max="13" width="6.625" customWidth="1"/>
-    <col min="14" max="14" width="9.75" customWidth="1"/>
-    <col min="15" max="15" width="9.5" customWidth="1"/>
-    <col min="16" max="16" width="7.25" customWidth="1"/>
-    <col min="17" max="18" width="6" customWidth="1"/>
+    <col min="7" max="7" width="50.875" customWidth="1"/>
+    <col min="8" max="13" width="3.125" customWidth="1"/>
+    <col min="14" max="14" width="6.625" customWidth="1"/>
+    <col min="15" max="15" width="9.75" customWidth="1"/>
+    <col min="16" max="16" width="9.5" customWidth="1"/>
+    <col min="17" max="17" width="7.25" customWidth="1"/>
+    <col min="18" max="19" width="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>20</v>
       </c>
@@ -2273,44 +2317,47 @@
       <c r="F1" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="H1" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="M1" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="R1" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="S1" s="8" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -2329,8 +2376,8 @@
       <c r="F2" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>56</v>
+      <c r="G2" s="2" t="s">
+        <v>95</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>56</v>
@@ -2347,26 +2394,29 @@
       <c r="L2" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>32</v>
       </c>
       <c r="P2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q2" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="S2" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A3" s="10" t="s">
         <v>25</v>
       </c>
@@ -2385,44 +2435,47 @@
       <c r="F3" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="H3" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="I3" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="J3" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="K3" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="L3" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="L3" s="11" t="s">
+      <c r="M3" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="M3" s="10" t="s">
+      <c r="N3" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="N3" s="10" t="s">
+      <c r="O3" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="O3" s="10" t="s">
+      <c r="P3" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="P3" s="10" t="s">
+      <c r="Q3" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="Q3" s="10" t="s">
+      <c r="R3" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="R3" s="10" t="s">
+      <c r="S3" s="10" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A4" s="9" t="s">
         <v>30</v>
       </c>
@@ -2439,34 +2492,35 @@
         <v>98</v>
       </c>
       <c r="F4" s="9"/>
-      <c r="G4" s="9">
+      <c r="G4" s="9"/>
+      <c r="H4" s="9">
         <v>1</v>
       </c>
-      <c r="H4" s="9"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
       <c r="K4" s="9"/>
       <c r="L4" s="9"/>
-      <c r="M4" s="9" t="s">
+      <c r="M4" s="9"/>
+      <c r="N4" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="N4" s="9" t="s">
+      <c r="O4" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="O4" s="9" t="s">
+      <c r="P4" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="P4" s="9" t="s">
+      <c r="Q4" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="Q4" s="9">
+      <c r="R4" s="9">
         <v>1348</v>
       </c>
-      <c r="R4" s="9">
+      <c r="S4" s="9">
         <v>611</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A5" s="9">
         <v>13000002</v>
       </c>
@@ -2485,36 +2539,37 @@
       <c r="F5" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="9"/>
+      <c r="H5" s="9">
         <v>1</v>
       </c>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9">
+      <c r="I5" s="9"/>
+      <c r="J5" s="9">
         <v>1</v>
       </c>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9">
+      <c r="K5" s="9"/>
+      <c r="L5" s="9">
         <v>1</v>
       </c>
-      <c r="L5" s="9"/>
       <c r="M5" s="9"/>
-      <c r="N5" s="9" t="s">
-        <v>38</v>
-      </c>
+      <c r="N5" s="9"/>
       <c r="O5" s="9" t="s">
         <v>38</v>
       </c>
       <c r="P5" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q5" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="Q5" s="9">
+      <c r="R5" s="9">
         <v>1279</v>
       </c>
-      <c r="R5" s="9">
+      <c r="S5" s="9">
         <v>571</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A6" s="9">
         <v>13000003</v>
       </c>
@@ -2533,32 +2588,33 @@
       <c r="F6" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="9"/>
+      <c r="H6" s="9">
         <v>1</v>
       </c>
-      <c r="H6" s="9"/>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
       <c r="L6" s="9"/>
       <c r="M6" s="9"/>
-      <c r="N6" s="9" t="s">
-        <v>127</v>
-      </c>
+      <c r="N6" s="9"/>
       <c r="O6" s="9" t="s">
         <v>127</v>
       </c>
       <c r="P6" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q6" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="Q6" s="9">
+      <c r="R6" s="9">
         <v>1213</v>
       </c>
-      <c r="R6" s="9">
+      <c r="S6" s="9">
         <v>655</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A7" s="9">
         <v>13010001</v>
       </c>
@@ -2573,26 +2629,27 @@
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
-      <c r="G7" s="9">
+      <c r="G7" s="9"/>
+      <c r="H7" s="9">
         <v>1</v>
       </c>
-      <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
       <c r="M7" s="9"/>
-      <c r="N7" s="9" t="s">
+      <c r="N7" s="9"/>
+      <c r="O7" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="O7" s="9" t="s">
+      <c r="P7" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="P7" s="9"/>
       <c r="Q7" s="9"/>
       <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A8" s="9">
         <v>13010004</v>
       </c>
@@ -2611,34 +2668,35 @@
       <c r="F8" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="9"/>
+      <c r="H8" s="9">
         <v>1</v>
       </c>
-      <c r="H8" s="9"/>
       <c r="I8" s="9"/>
-      <c r="J8" s="9">
+      <c r="J8" s="9"/>
+      <c r="K8" s="9">
         <v>1</v>
       </c>
-      <c r="K8" s="9"/>
       <c r="L8" s="9"/>
       <c r="M8" s="9"/>
-      <c r="N8" s="9" t="s">
-        <v>42</v>
-      </c>
+      <c r="N8" s="9"/>
       <c r="O8" s="9" t="s">
         <v>42</v>
       </c>
       <c r="P8" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q8" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="Q8" s="9">
+      <c r="R8" s="9">
         <v>1148</v>
       </c>
-      <c r="R8" s="9">
+      <c r="S8" s="9">
         <v>351</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A9" s="9">
         <v>13010005</v>
       </c>
@@ -2653,34 +2711,35 @@
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
-      <c r="G9" s="9">
-        <v>1</v>
-      </c>
+      <c r="G9" s="9"/>
       <c r="H9" s="9">
         <v>1</v>
       </c>
-      <c r="I9" s="9"/>
+      <c r="I9" s="9">
+        <v>1</v>
+      </c>
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
       <c r="L9" s="9"/>
       <c r="M9" s="9"/>
-      <c r="N9" s="9" t="s">
+      <c r="N9" s="9"/>
+      <c r="O9" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="O9" s="9" t="s">
+      <c r="P9" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="P9" s="9" t="s">
+      <c r="Q9" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="Q9" s="9">
+      <c r="R9" s="9">
         <v>1386</v>
       </c>
-      <c r="R9" s="9">
+      <c r="S9" s="9">
         <v>339</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A10" s="9">
         <v>13010006</v>
       </c>
@@ -2702,23 +2761,24 @@
       <c r="K10" s="9"/>
       <c r="L10" s="9"/>
       <c r="M10" s="9"/>
-      <c r="N10" s="9" t="s">
+      <c r="N10" s="9"/>
+      <c r="O10" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="O10" s="9" t="s">
+      <c r="P10" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="P10" s="9" t="s">
+      <c r="Q10" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="Q10" s="9">
+      <c r="R10" s="9">
         <v>1232</v>
       </c>
-      <c r="R10" s="9">
+      <c r="S10" s="9">
         <v>506</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A11" s="9">
         <v>13010007</v>
       </c>
@@ -2737,38 +2797,39 @@
       <c r="F11" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G11" s="9"/>
+      <c r="H11" s="9">
         <v>1</v>
       </c>
-      <c r="H11" s="9"/>
       <c r="I11" s="9"/>
-      <c r="J11" s="9">
-        <v>1</v>
-      </c>
+      <c r="J11" s="9"/>
       <c r="K11" s="9">
         <v>1</v>
       </c>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9" t="s">
+      <c r="L11" s="9">
+        <v>1</v>
+      </c>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="N11" s="9" t="s">
+      <c r="O11" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="O11" s="9" t="s">
+      <c r="P11" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="P11" s="9" t="s">
+      <c r="Q11" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="Q11" s="9">
+      <c r="R11" s="9">
         <v>1431</v>
       </c>
-      <c r="R11" s="9">
+      <c r="S11" s="9">
         <v>440</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A12" s="9">
         <v>13010008</v>
       </c>
@@ -2787,34 +2848,35 @@
       <c r="F12" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="9"/>
+      <c r="H12" s="9">
         <v>1</v>
       </c>
-      <c r="H12" s="9"/>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
       <c r="K12" s="9"/>
-      <c r="L12" s="9">
+      <c r="L12" s="9"/>
+      <c r="M12" s="9">
         <v>1</v>
       </c>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9" t="s">
+      <c r="N12" s="9"/>
+      <c r="O12" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="O12" s="9" t="s">
+      <c r="P12" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="P12" s="9" t="s">
+      <c r="Q12" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="Q12" s="9">
+      <c r="R12" s="9">
         <v>1067</v>
       </c>
-      <c r="R12" s="9">
+      <c r="S12" s="9">
         <v>445</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A13" s="9">
         <v>13010009</v>
       </c>
@@ -2833,36 +2895,37 @@
       <c r="F13" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="G13" s="9">
-        <v>1</v>
-      </c>
+      <c r="G13" s="9"/>
       <c r="H13" s="9">
         <v>1</v>
       </c>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9">
+      <c r="I13" s="9">
         <v>1</v>
       </c>
-      <c r="K13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9">
+        <v>1</v>
+      </c>
       <c r="L13" s="9"/>
       <c r="M13" s="9"/>
-      <c r="N13" s="9" t="s">
+      <c r="N13" s="9"/>
+      <c r="O13" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="O13" s="9" t="s">
+      <c r="P13" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="P13" s="9" t="s">
+      <c r="Q13" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="Q13" s="9">
+      <c r="R13" s="9">
         <v>1332</v>
       </c>
-      <c r="R13" s="9">
+      <c r="S13" s="9">
         <v>484</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A14" s="9">
         <v>13010010</v>
       </c>
@@ -2879,34 +2942,35 @@
       <c r="F14" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G14" s="9"/>
+      <c r="H14" s="9">
         <v>1</v>
       </c>
-      <c r="H14" s="9"/>
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
       <c r="K14" s="9"/>
-      <c r="L14" s="9">
+      <c r="L14" s="9"/>
+      <c r="M14" s="9">
         <v>1</v>
       </c>
-      <c r="M14" s="9"/>
-      <c r="N14" s="9" t="s">
+      <c r="N14" s="9"/>
+      <c r="O14" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="O14" s="9" t="s">
+      <c r="P14" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="P14" s="9" t="s">
+      <c r="Q14" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="Q14" s="9">
+      <c r="R14" s="9">
         <v>1441</v>
       </c>
-      <c r="R14" s="9">
+      <c r="S14" s="9">
         <v>527</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A15" s="9">
         <v>13010011</v>
       </c>
@@ -2925,36 +2989,37 @@
       <c r="F15" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="G15" s="9">
+      <c r="G15" s="9"/>
+      <c r="H15" s="9">
         <v>1</v>
       </c>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9">
+      <c r="I15" s="9"/>
+      <c r="J15" s="9">
         <v>1</v>
       </c>
-      <c r="J15" s="9"/>
       <c r="K15" s="9"/>
       <c r="L15" s="9"/>
-      <c r="M15" s="9" t="s">
+      <c r="M15" s="9"/>
+      <c r="N15" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="N15" s="9" t="s">
+      <c r="O15" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="O15" s="9" t="s">
+      <c r="P15" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="P15" s="9" t="s">
+      <c r="Q15" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="Q15" s="9">
+      <c r="R15" s="9">
         <v>1574</v>
       </c>
-      <c r="R15" s="9">
+      <c r="S15" s="9">
         <v>373</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A16" s="9">
         <v>13010012</v>
       </c>
@@ -2973,32 +3038,33 @@
       <c r="F16" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="G16" s="9">
+      <c r="G16" s="9"/>
+      <c r="H16" s="9">
         <v>1</v>
       </c>
-      <c r="H16" s="9"/>
       <c r="I16" s="9"/>
       <c r="J16" s="9"/>
       <c r="K16" s="9"/>
       <c r="L16" s="9"/>
       <c r="M16" s="9"/>
-      <c r="N16" s="9" t="s">
+      <c r="N16" s="9"/>
+      <c r="O16" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="O16" s="9" t="s">
+      <c r="P16" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="P16" s="9" t="s">
+      <c r="Q16" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="Q16" s="9">
+      <c r="R16" s="9">
         <v>1251</v>
       </c>
-      <c r="R16" s="9">
+      <c r="S16" s="9">
         <v>432</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A17" s="9">
         <v>13010013</v>
       </c>
@@ -3017,32 +3083,33 @@
       <c r="F17" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="G17" s="9">
+      <c r="G17" s="9"/>
+      <c r="H17" s="9">
         <v>1</v>
       </c>
-      <c r="H17" s="9"/>
       <c r="I17" s="9"/>
       <c r="J17" s="9"/>
       <c r="K17" s="9"/>
       <c r="L17" s="9"/>
       <c r="M17" s="9"/>
-      <c r="N17" s="9" t="s">
+      <c r="N17" s="9"/>
+      <c r="O17" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="O17" s="9" t="s">
+      <c r="P17" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="P17" s="9" t="s">
+      <c r="Q17" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="Q17" s="9">
+      <c r="R17" s="9">
         <v>1250</v>
       </c>
-      <c r="R17" s="9">
+      <c r="S17" s="9">
         <v>338</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A18" s="9">
         <v>13010014</v>
       </c>
@@ -3061,36 +3128,37 @@
       <c r="F18" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="G18" s="9">
+      <c r="G18" s="9"/>
+      <c r="H18" s="9">
         <v>1</v>
       </c>
-      <c r="H18" s="9"/>
       <c r="I18" s="9"/>
       <c r="J18" s="9"/>
-      <c r="K18" s="9">
-        <v>1</v>
-      </c>
+      <c r="K18" s="9"/>
       <c r="L18" s="9">
         <v>1</v>
       </c>
-      <c r="M18" s="9"/>
-      <c r="N18" s="9" t="s">
+      <c r="M18" s="9">
+        <v>1</v>
+      </c>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="O18" s="9" t="s">
+      <c r="P18" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="P18" s="9" t="s">
+      <c r="Q18" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="Q18" s="9">
+      <c r="R18" s="9">
         <v>1550</v>
       </c>
-      <c r="R18" s="9">
+      <c r="S18" s="9">
         <v>505</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A19" s="9">
         <v>13010015</v>
       </c>
@@ -3109,34 +3177,35 @@
       <c r="F19" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="G19" s="9">
+      <c r="G19" s="9"/>
+      <c r="H19" s="9">
         <v>1</v>
       </c>
-      <c r="H19" s="9"/>
       <c r="I19" s="9"/>
-      <c r="J19" s="9">
+      <c r="J19" s="9"/>
+      <c r="K19" s="9">
         <v>1</v>
       </c>
-      <c r="K19" s="9"/>
       <c r="L19" s="9"/>
       <c r="M19" s="9"/>
-      <c r="N19" s="9" t="s">
+      <c r="N19" s="9"/>
+      <c r="O19" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="O19" s="9" t="s">
+      <c r="P19" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="P19" s="9" t="s">
+      <c r="Q19" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="Q19" s="9">
+      <c r="R19" s="9">
         <v>1040</v>
       </c>
-      <c r="R19" s="9">
+      <c r="S19" s="9">
         <v>538</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A20" s="9">
         <v>13010016</v>
       </c>
@@ -3158,23 +3227,24 @@
       <c r="K20" s="9"/>
       <c r="L20" s="9"/>
       <c r="M20" s="9"/>
-      <c r="N20" s="9" t="s">
+      <c r="N20" s="9"/>
+      <c r="O20" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="O20" s="9" t="s">
+      <c r="P20" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="P20" s="9" t="s">
+      <c r="Q20" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="Q20" s="9">
+      <c r="R20" s="9">
         <v>919</v>
       </c>
-      <c r="R20" s="9">
+      <c r="S20" s="9">
         <v>534</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A21" s="9">
         <v>13010017</v>
       </c>
@@ -3193,34 +3263,35 @@
       <c r="F21" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="G21" s="9">
+      <c r="G21" s="9"/>
+      <c r="H21" s="9">
         <v>1</v>
       </c>
-      <c r="H21" s="9"/>
       <c r="I21" s="9"/>
       <c r="J21" s="9"/>
-      <c r="K21" s="9">
+      <c r="K21" s="9"/>
+      <c r="L21" s="9">
         <v>1</v>
       </c>
-      <c r="L21" s="9"/>
       <c r="M21" s="9"/>
-      <c r="N21" s="9" t="s">
+      <c r="N21" s="9"/>
+      <c r="O21" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="O21" s="9" t="s">
+      <c r="P21" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="P21" s="9" t="s">
+      <c r="Q21" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="Q21" s="9">
+      <c r="R21" s="9">
         <v>1149</v>
       </c>
-      <c r="R21" s="9">
+      <c r="S21" s="9">
         <v>584</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A22" s="9">
         <v>13010018</v>
       </c>
@@ -3246,23 +3317,24 @@
       <c r="K22" s="9"/>
       <c r="L22" s="9"/>
       <c r="M22" s="9"/>
-      <c r="N22" s="9" t="s">
+      <c r="N22" s="9"/>
+      <c r="O22" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="O22" s="9" t="s">
+      <c r="P22" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="P22" s="9" t="s">
+      <c r="Q22" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="Q22" s="9">
+      <c r="R22" s="9">
         <v>840</v>
       </c>
-      <c r="R22" s="9">
+      <c r="S22" s="9">
         <v>444</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A23" s="9">
         <v>13020001</v>
       </c>
@@ -3275,30 +3347,31 @@
       <c r="D23" s="9">
         <v>3</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="E23" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="F23" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="G23" s="9"/>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
       <c r="K23" s="9"/>
       <c r="L23" s="9"/>
       <c r="M23" s="9"/>
-      <c r="N23" s="9" t="s">
-        <v>144</v>
-      </c>
+      <c r="N23" s="9"/>
       <c r="O23" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="P23" s="9"/>
+      <c r="P23" s="9" t="s">
+        <v>144</v>
+      </c>
       <c r="Q23" s="9"/>
       <c r="R23" s="9"/>
+      <c r="S23" s="9"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A24" s="9">
         <v>13020002</v>
       </c>
@@ -3311,12 +3384,8 @@
       <c r="D24" s="9">
         <v>3</v>
       </c>
-      <c r="E24" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="F24" s="9" t="s">
-        <v>148</v>
-      </c>
+      <c r="E24" s="12"/>
+      <c r="F24" s="9"/>
       <c r="G24" s="9"/>
       <c r="H24" s="9"/>
       <c r="I24" s="9"/>
@@ -3324,25 +3393,26 @@
       <c r="K24" s="9"/>
       <c r="L24" s="9"/>
       <c r="M24" s="9"/>
-      <c r="N24" s="9" t="s">
-        <v>145</v>
-      </c>
+      <c r="N24" s="9"/>
       <c r="O24" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="P24" s="9"/>
+      <c r="P24" s="9" t="s">
+        <v>145</v>
+      </c>
       <c r="Q24" s="9"/>
       <c r="R24" s="9"/>
+      <c r="S24" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="G4:L24">
-    <cfRule type="cellIs" dxfId="22" priority="2" operator="equal">
+  <conditionalFormatting sqref="H4:M24">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="21" priority="1" operator="equal">
+  <conditionalFormatting sqref="I4">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
finish the revive pos of scene
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Scene.xlsx
+++ b/ConfigData/Xlsx/Scene.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="153">
   <si>
     <t>村外小屋</t>
   </si>
@@ -118,460 +118,472 @@
     <t>Url</t>
   </si>
   <si>
+    <t>TilePath</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>配置</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>home</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Quest</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>任务列表</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>darkforest</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>tatamuviliage</t>
+  </si>
+  <si>
+    <t>smallforest</t>
+  </si>
+  <si>
+    <t>perse</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>demlock</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>hightower</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>smallhill</t>
+  </si>
+  <si>
+    <t>goldseashore</t>
+  </si>
+  <si>
+    <t>islandold</t>
+  </si>
+  <si>
+    <t>riverold</t>
+  </si>
+  <si>
+    <t>落潮小径</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>月光林地</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>gerdin</t>
+  </si>
+  <si>
+    <t>fogvalley</t>
+  </si>
+  <si>
+    <t>矿脉山脚</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>riverside</t>
+  </si>
+  <si>
+    <t>woodviliage</t>
+  </si>
+  <si>
+    <t>moonforest</t>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>激活传送门</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QPortal</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QCardChange</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>卡牌交换</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>素材商人</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QPiece</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QMerchant</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QDoctor</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QAngel</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>商人</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>医生</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>天使</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>IconX</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>IconY</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Icon</t>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwxw</t>
+  </si>
+  <si>
+    <t>haml</t>
+  </si>
+  <si>
+    <t>kk</t>
+  </si>
+  <si>
+    <t>dlkxg</t>
+  </si>
+  <si>
+    <t>bstgt</t>
+  </si>
+  <si>
+    <t>ttmc</t>
+  </si>
+  <si>
+    <t>psgc</t>
+  </si>
+  <si>
+    <t>gdh</t>
+  </si>
+  <si>
+    <t>cwyy</t>
+  </si>
+  <si>
+    <t>hjha</t>
+  </si>
+  <si>
+    <t>gdyj</t>
+  </si>
+  <si>
+    <t>xsl</t>
+  </si>
+  <si>
+    <t>llf</t>
+  </si>
+  <si>
+    <t>yjht</t>
+  </si>
+  <si>
+    <t>wg</t>
+  </si>
+  <si>
+    <t>myzc</t>
+  </si>
+  <si>
+    <t>lcxj</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ygld</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>小图标x</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>小图标y</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>图标路径</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>GameUpToNumber;GameThreeBody</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>poppyfield;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trees;3|mushroom;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>sewer;3|river;2|fortune;1|oldtree;1|poppyfield;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>fortune;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>wolfnest;2|gamble;1|fishpool;2|sewer;3|river;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>小概率任务</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QuestRandom</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|treasure;25</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>类型</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Type</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>portal;1|fishpool;1|grave;2|hiddeway;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>river;2|fishpool;1|swamp;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>mushroom;1|hiddeway;1|swamp;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>orehole;1|stone;2|sandflow;2</t>
+  </si>
+  <si>
+    <t>coldwind;3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ruintown1;1|manflower;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trees;3|grave;1|portal;1|oldtree;1|manflower;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>portal;3|sandflow;2|manflower;3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>river;2|stone;3|ruintown1;1|hiddeway;1|manflower;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|witchhome;30</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|treasure;25|witchhome;20</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|forestfire;20|witchhome;40</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>forestfire;10</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>forestfire;35|witchhome;10</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>密林迷宫</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>迷宫深处</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>home</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>orevalley</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>default</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>hightower</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>tatamuviliage</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>perse</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>gerdin</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>farm</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>farm</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>goldseashore</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>islandold</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>smallforest</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>smallhill</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>riverold</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>fogvalley</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>woodviliage</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>riverside</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>moonforest</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>forestmaze</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>forestinner</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trees;3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>副本任务列表</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QuestDungeon</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>forestentry;2|forestentry2;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>复活地图</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ReviveScene</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>13000001|BornMapId</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>TilePath</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>配置</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>default</t>
-  </si>
-  <si>
-    <t>home</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Quest</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>任务列表</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>darkforest</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>tatamuviliage</t>
-  </si>
-  <si>
-    <t>smallforest</t>
-  </si>
-  <si>
-    <t>perse</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>demlock</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>hightower</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>smallhill</t>
-  </si>
-  <si>
-    <t>goldseashore</t>
-  </si>
-  <si>
-    <t>islandold</t>
-  </si>
-  <si>
-    <t>riverold</t>
-  </si>
-  <si>
-    <t>落潮小径</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>月光林地</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>gerdin</t>
-  </si>
-  <si>
-    <t>fogvalley</t>
-  </si>
-  <si>
-    <t>矿脉山脚</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>riverside</t>
-  </si>
-  <si>
-    <t>woodviliage</t>
-  </si>
-  <si>
-    <t>moonforest</t>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>激活传送门</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>QPortal</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>QCardChange</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>卡牌交换</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>素材商人</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>QPiece</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>QMerchant</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>QDoctor</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>QAngel</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>商人</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>医生</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>天使</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>IconX</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>IconY</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Icon</t>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>cwxw</t>
-  </si>
-  <si>
-    <t>haml</t>
-  </si>
-  <si>
-    <t>kk</t>
-  </si>
-  <si>
-    <t>dlkxg</t>
-  </si>
-  <si>
-    <t>bstgt</t>
-  </si>
-  <si>
-    <t>ttmc</t>
-  </si>
-  <si>
-    <t>psgc</t>
-  </si>
-  <si>
-    <t>gdh</t>
-  </si>
-  <si>
-    <t>cwyy</t>
-  </si>
-  <si>
-    <t>hjha</t>
-  </si>
-  <si>
-    <t>gdyj</t>
-  </si>
-  <si>
-    <t>xsl</t>
-  </si>
-  <si>
-    <t>llf</t>
-  </si>
-  <si>
-    <t>yjht</t>
-  </si>
-  <si>
-    <t>wg</t>
-  </si>
-  <si>
-    <t>myzc</t>
-  </si>
-  <si>
-    <t>lcxj</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ygld</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>小图标x</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>小图标y</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>图标路径</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>GameUpToNumber;GameThreeBody</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>poppyfield;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>trees;3|mushroom;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>sewer;3|river;2|fortune;1|oldtree;1|poppyfield;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>fortune;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>wolfnest;2|gamble;1|fishpool;2|sewer;3|river;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>小概率任务</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>QuestRandom</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|treasure;25</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>类型</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Type</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>portal;1|fishpool;1|grave;2|hiddeway;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>river;2|fishpool;1|swamp;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>mushroom;1|hiddeway;1|swamp;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>orehole;1|stone;2|sandflow;2</t>
-  </si>
-  <si>
-    <t>coldwind;3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ruintown1;1|manflower;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>trees;3|grave;1|portal;1|oldtree;1|manflower;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>portal;3|sandflow;2|manflower;3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>river;2|stone;3|ruintown1;1|hiddeway;1|manflower;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|witchhome;30</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|treasure;25|witchhome;20</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|forestfire;20|witchhome;40</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>forestfire;10</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>forestfire;35|witchhome;10</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>密林迷宫</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>迷宫深处</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>home</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>orevalley</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>default</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>hightower</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>tatamuviliage</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>perse</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>gerdin</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>farm</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>farm</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>goldseashore</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>islandold</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>smallforest</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>smallhill</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>riverold</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>fogvalley</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>woodviliage</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>riverside</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>moonforest</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>forestmaze</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>forestinner</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>trees;3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>副本任务列表</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>QuestDungeon</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>forestentry;2|forestentry2;2</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1327,7 +1339,34 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="25">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1680,8 +1719,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -1927,35 +1964,36 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:S24" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22" tableBorderDxfId="21">
-  <autoFilter ref="A3:S24"/>
-  <tableColumns count="19">
-    <tableColumn id="1" name="Id" dataDxfId="20"/>
-    <tableColumn id="2" name="Name" dataDxfId="19"/>
-    <tableColumn id="18" name="Type" dataDxfId="18"/>
-    <tableColumn id="3" name="Level" dataDxfId="17"/>
-    <tableColumn id="4" name="Quest" dataDxfId="16"/>
-    <tableColumn id="17" name="QuestRandom" dataDxfId="15"/>
-    <tableColumn id="19" name="QuestDungeon" dataDxfId="14"/>
-    <tableColumn id="5" name="QPortal" dataDxfId="13"/>
-    <tableColumn id="6" name="QCardChange" dataDxfId="12"/>
-    <tableColumn id="7" name="QPiece" dataDxfId="11"/>
-    <tableColumn id="8" name="QMerchant" dataDxfId="10"/>
-    <tableColumn id="9" name="QDoctor" dataDxfId="9"/>
-    <tableColumn id="10" name="QAngel" dataDxfId="8"/>
-    <tableColumn id="11" name="Func" dataDxfId="7"/>
-    <tableColumn id="12" name="Url" dataDxfId="6"/>
-    <tableColumn id="13" name="TilePath" dataDxfId="5"/>
-    <tableColumn id="14" name="Icon" dataDxfId="4"/>
-    <tableColumn id="15" name="IconX" dataDxfId="3"/>
-    <tableColumn id="16" name="IconY" dataDxfId="2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:T24" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23" tableBorderDxfId="22">
+  <autoFilter ref="A3:T24"/>
+  <tableColumns count="20">
+    <tableColumn id="1" name="Id" dataDxfId="21"/>
+    <tableColumn id="2" name="Name" dataDxfId="20"/>
+    <tableColumn id="18" name="Type" dataDxfId="19"/>
+    <tableColumn id="3" name="Level" dataDxfId="18"/>
+    <tableColumn id="20" name="ReviveScene" dataDxfId="0"/>
+    <tableColumn id="4" name="Quest" dataDxfId="17"/>
+    <tableColumn id="17" name="QuestRandom" dataDxfId="16"/>
+    <tableColumn id="19" name="QuestDungeon" dataDxfId="15"/>
+    <tableColumn id="5" name="QPortal" dataDxfId="14"/>
+    <tableColumn id="6" name="QCardChange" dataDxfId="13"/>
+    <tableColumn id="7" name="QPiece" dataDxfId="12"/>
+    <tableColumn id="8" name="QMerchant" dataDxfId="11"/>
+    <tableColumn id="9" name="QDoctor" dataDxfId="10"/>
+    <tableColumn id="10" name="QAngel" dataDxfId="9"/>
+    <tableColumn id="11" name="Func" dataDxfId="8"/>
+    <tableColumn id="12" name="Url" dataDxfId="7"/>
+    <tableColumn id="13" name="TilePath" dataDxfId="6"/>
+    <tableColumn id="14" name="Icon" dataDxfId="5"/>
+    <tableColumn id="15" name="IconX" dataDxfId="4"/>
+    <tableColumn id="16" name="IconY" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2030,23 +2068,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2082,23 +2103,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2275,10 +2279,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S24"/>
+  <dimension ref="A1:T24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2287,18 +2291,19 @@
     <col min="2" max="2" width="10.625" customWidth="1"/>
     <col min="3" max="3" width="5.125" customWidth="1"/>
     <col min="4" max="4" width="4.375" customWidth="1"/>
-    <col min="5" max="5" width="52.875" customWidth="1"/>
-    <col min="6" max="6" width="16.625" customWidth="1"/>
-    <col min="7" max="7" width="50.875" customWidth="1"/>
-    <col min="8" max="13" width="3.125" customWidth="1"/>
-    <col min="14" max="14" width="6.625" customWidth="1"/>
-    <col min="15" max="15" width="9.75" customWidth="1"/>
-    <col min="16" max="16" width="9.5" customWidth="1"/>
-    <col min="17" max="17" width="7.25" customWidth="1"/>
-    <col min="18" max="19" width="6" customWidth="1"/>
+    <col min="5" max="5" width="9" customWidth="1"/>
+    <col min="6" max="6" width="52.875" customWidth="1"/>
+    <col min="7" max="7" width="16.625" customWidth="1"/>
+    <col min="8" max="8" width="50.875" customWidth="1"/>
+    <col min="9" max="14" width="3.125" customWidth="1"/>
+    <col min="15" max="15" width="6.625" customWidth="1"/>
+    <col min="16" max="16" width="9.75" customWidth="1"/>
+    <col min="17" max="17" width="9.5" customWidth="1"/>
+    <col min="18" max="18" width="7.25" customWidth="1"/>
+    <col min="19" max="20" width="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>20</v>
       </c>
@@ -2306,58 +2311,61 @@
         <v>21</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>22</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>37</v>
+        <v>149</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>101</v>
+        <v>36</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>57</v>
+        <v>100</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>146</v>
       </c>
       <c r="I1" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="K1" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="J1" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="M1" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="N1" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="M1" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="P1" s="6" t="s">
-        <v>33</v>
-      </c>
       <c r="Q1" s="6" t="s">
-        <v>93</v>
+        <v>32</v>
       </c>
       <c r="R1" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="T1" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="S1" s="8" t="s">
-        <v>92</v>
-      </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -2365,58 +2373,61 @@
         <v>19</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>95</v>
+        <v>150</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>56</v>
+        <v>101</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="N2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="O2" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="P2" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>72</v>
+        <v>31</v>
       </c>
       <c r="R2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="S2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="T2" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A3" s="10" t="s">
         <v>25</v>
       </c>
@@ -2424,60 +2435,63 @@
         <v>26</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>27</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>36</v>
+        <v>151</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>103</v>
+        <v>35</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="H3" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="J3" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="I3" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="J3" s="11" t="s">
+      <c r="K3" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="L3" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="M3" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="L3" s="11" t="s">
+      <c r="N3" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="M3" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="N3" s="10" t="s">
+      <c r="O3" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="O3" s="10" t="s">
+      <c r="P3" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="P3" s="10" t="s">
-        <v>31</v>
-      </c>
       <c r="Q3" s="10" t="s">
-        <v>71</v>
+        <v>30</v>
       </c>
       <c r="R3" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="S3" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="T3" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="S3" s="10" t="s">
-        <v>70</v>
-      </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A4" s="9" t="s">
-        <v>30</v>
+        <v>152</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>0</v>
@@ -2488,39 +2502,42 @@
       <c r="D4" s="9">
         <v>1</v>
       </c>
-      <c r="E4" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="F4" s="9"/>
+      <c r="E4" s="9">
+        <v>13000001</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>97</v>
+      </c>
       <c r="G4" s="9"/>
-      <c r="H4" s="9">
+      <c r="H4" s="9"/>
+      <c r="I4" s="9">
         <v>1</v>
       </c>
-      <c r="I4" s="9"/>
       <c r="J4" s="9"/>
       <c r="K4" s="9"/>
       <c r="L4" s="9"/>
       <c r="M4" s="9"/>
-      <c r="N4" s="9" t="s">
-        <v>94</v>
-      </c>
+      <c r="N4" s="9"/>
       <c r="O4" s="9" t="s">
-        <v>126</v>
+        <v>93</v>
       </c>
       <c r="P4" s="9" t="s">
-        <v>35</v>
+        <v>125</v>
       </c>
       <c r="Q4" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="R4" s="9">
+        <v>34</v>
+      </c>
+      <c r="R4" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="S4" s="9">
         <v>1348</v>
       </c>
-      <c r="S4" s="9">
+      <c r="T4" s="9">
         <v>611</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A5" s="9">
         <v>13000002</v>
       </c>
@@ -2533,48 +2550,51 @@
       <c r="D5" s="9">
         <v>2</v>
       </c>
-      <c r="E5" s="9" t="s">
-        <v>100</v>
+      <c r="E5" s="9">
+        <v>13000001</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9">
+        <v>99</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9">
         <v>1</v>
       </c>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9">
+      <c r="J5" s="9"/>
+      <c r="K5" s="9">
         <v>1</v>
       </c>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9">
+      <c r="L5" s="9"/>
+      <c r="M5" s="9">
         <v>1</v>
       </c>
-      <c r="M5" s="9"/>
       <c r="N5" s="9"/>
-      <c r="O5" s="9" t="s">
-        <v>38</v>
-      </c>
+      <c r="O5" s="9"/>
       <c r="P5" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q5" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="R5" s="9">
+        <v>37</v>
+      </c>
+      <c r="R5" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="S5" s="9">
         <v>1279</v>
       </c>
-      <c r="S5" s="9">
+      <c r="T5" s="9">
         <v>571</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A6" s="9">
         <v>13000003</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6" s="9">
         <v>2</v>
@@ -2582,39 +2602,42 @@
       <c r="D6" s="9">
         <v>19</v>
       </c>
-      <c r="E6" s="9" t="s">
-        <v>113</v>
+      <c r="E6" s="9">
+        <v>13010016</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9">
+        <v>112</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9">
         <v>1</v>
       </c>
-      <c r="I6" s="9"/>
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
       <c r="L6" s="9"/>
       <c r="M6" s="9"/>
       <c r="N6" s="9"/>
-      <c r="O6" s="9" t="s">
-        <v>127</v>
-      </c>
+      <c r="O6" s="9"/>
       <c r="P6" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Q6" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="R6" s="9">
+        <v>126</v>
+      </c>
+      <c r="R6" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="S6" s="9">
         <v>1213</v>
       </c>
-      <c r="S6" s="9">
+      <c r="T6" s="9">
         <v>655</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A7" s="9">
         <v>13010001</v>
       </c>
@@ -2627,29 +2650,32 @@
       <c r="D7" s="9">
         <v>0</v>
       </c>
-      <c r="E7" s="9"/>
+      <c r="E7" s="9">
+        <v>13010006</v>
+      </c>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
-      <c r="H7" s="9">
+      <c r="H7" s="9"/>
+      <c r="I7" s="9">
         <v>1</v>
       </c>
-      <c r="I7" s="9"/>
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
       <c r="M7" s="9"/>
       <c r="N7" s="9"/>
-      <c r="O7" s="9" t="s">
-        <v>128</v>
-      </c>
+      <c r="O7" s="9"/>
       <c r="P7" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q7" s="9"/>
+        <v>127</v>
+      </c>
+      <c r="Q7" s="9" t="s">
+        <v>33</v>
+      </c>
       <c r="R7" s="9"/>
       <c r="S7" s="9"/>
+      <c r="T7" s="9"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A8" s="9">
         <v>13010004</v>
       </c>
@@ -2662,41 +2688,44 @@
       <c r="D8" s="9">
         <v>5</v>
       </c>
-      <c r="E8" s="9" t="s">
-        <v>118</v>
+      <c r="E8" s="9">
+        <v>13010006</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9">
+        <v>117</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9">
         <v>1</v>
       </c>
-      <c r="I8" s="9"/>
       <c r="J8" s="9"/>
-      <c r="K8" s="9">
+      <c r="K8" s="9"/>
+      <c r="L8" s="9">
         <v>1</v>
       </c>
-      <c r="L8" s="9"/>
       <c r="M8" s="9"/>
       <c r="N8" s="9"/>
-      <c r="O8" s="9" t="s">
-        <v>42</v>
-      </c>
+      <c r="O8" s="9"/>
       <c r="P8" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Q8" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="R8" s="9">
+        <v>41</v>
+      </c>
+      <c r="R8" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="S8" s="9">
         <v>1148</v>
       </c>
-      <c r="S8" s="9">
+      <c r="T8" s="9">
         <v>351</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A9" s="9">
         <v>13010005</v>
       </c>
@@ -2709,37 +2738,40 @@
       <c r="D9" s="9">
         <v>8</v>
       </c>
-      <c r="E9" s="9"/>
+      <c r="E9" s="9">
+        <v>13010006</v>
+      </c>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
-      <c r="H9" s="9">
-        <v>1</v>
-      </c>
+      <c r="H9" s="9"/>
       <c r="I9" s="9">
         <v>1</v>
       </c>
-      <c r="J9" s="9"/>
+      <c r="J9" s="9">
+        <v>1</v>
+      </c>
       <c r="K9" s="9"/>
       <c r="L9" s="9"/>
       <c r="M9" s="9"/>
       <c r="N9" s="9"/>
-      <c r="O9" s="9" t="s">
-        <v>129</v>
-      </c>
+      <c r="O9" s="9"/>
       <c r="P9" s="9" t="s">
-        <v>43</v>
+        <v>128</v>
       </c>
       <c r="Q9" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="R9" s="9">
+        <v>42</v>
+      </c>
+      <c r="R9" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="S9" s="9">
         <v>1386</v>
       </c>
-      <c r="S9" s="9">
+      <c r="T9" s="9">
         <v>339</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A10" s="9">
         <v>13010006</v>
       </c>
@@ -2752,7 +2784,9 @@
       <c r="D10" s="9">
         <v>3</v>
       </c>
-      <c r="E10" s="9"/>
+      <c r="E10" s="9">
+        <v>13010006</v>
+      </c>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
@@ -2762,23 +2796,24 @@
       <c r="L10" s="9"/>
       <c r="M10" s="9"/>
       <c r="N10" s="9"/>
-      <c r="O10" s="9" t="s">
-        <v>130</v>
-      </c>
+      <c r="O10" s="9"/>
       <c r="P10" s="9" t="s">
-        <v>39</v>
+        <v>129</v>
       </c>
       <c r="Q10" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="R10" s="9">
+        <v>38</v>
+      </c>
+      <c r="R10" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="S10" s="9">
         <v>1232</v>
       </c>
-      <c r="S10" s="9">
+      <c r="T10" s="9">
         <v>506</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A11" s="9">
         <v>13010007</v>
       </c>
@@ -2791,45 +2826,48 @@
       <c r="D11" s="9">
         <v>7</v>
       </c>
-      <c r="E11" s="9" t="s">
-        <v>110</v>
+      <c r="E11" s="9">
+        <v>13010006</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9">
+        <v>109</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9">
         <v>1</v>
       </c>
-      <c r="I11" s="9"/>
       <c r="J11" s="9"/>
-      <c r="K11" s="9">
-        <v>1</v>
-      </c>
+      <c r="K11" s="9"/>
       <c r="L11" s="9">
         <v>1</v>
       </c>
-      <c r="M11" s="9"/>
-      <c r="N11" s="9" t="s">
+      <c r="M11" s="9">
+        <v>1</v>
+      </c>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="O11" s="9" t="s">
-        <v>131</v>
-      </c>
       <c r="P11" s="9" t="s">
-        <v>41</v>
+        <v>130</v>
       </c>
       <c r="Q11" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="R11" s="9">
+        <v>40</v>
+      </c>
+      <c r="R11" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="S11" s="9">
         <v>1431</v>
       </c>
-      <c r="S11" s="9">
+      <c r="T11" s="9">
         <v>440</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A12" s="9">
         <v>13010008</v>
       </c>
@@ -2842,41 +2880,44 @@
       <c r="D12" s="9">
         <v>15</v>
       </c>
-      <c r="E12" s="9" t="s">
-        <v>96</v>
+      <c r="E12" s="9">
+        <v>13010016</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9">
+        <v>95</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9">
         <v>1</v>
       </c>
-      <c r="I12" s="9"/>
       <c r="J12" s="9"/>
       <c r="K12" s="9"/>
       <c r="L12" s="9"/>
-      <c r="M12" s="9">
+      <c r="M12" s="9"/>
+      <c r="N12" s="9">
         <v>1</v>
       </c>
-      <c r="N12" s="9"/>
-      <c r="O12" s="9" t="s">
-        <v>132</v>
-      </c>
+      <c r="O12" s="9"/>
       <c r="P12" s="9" t="s">
-        <v>50</v>
+        <v>131</v>
       </c>
       <c r="Q12" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="R12" s="9">
+        <v>49</v>
+      </c>
+      <c r="R12" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="S12" s="9">
         <v>1067</v>
       </c>
-      <c r="S12" s="9">
+      <c r="T12" s="9">
         <v>445</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A13" s="9">
         <v>13010009</v>
       </c>
@@ -2889,43 +2930,46 @@
       <c r="D13" s="9">
         <v>4</v>
       </c>
-      <c r="E13" s="9" t="s">
-        <v>115</v>
+      <c r="E13" s="9">
+        <v>13010006</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9">
-        <v>1</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="H13" s="9"/>
       <c r="I13" s="9">
         <v>1</v>
       </c>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9">
+      <c r="J13" s="9">
         <v>1</v>
       </c>
-      <c r="L13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9">
+        <v>1</v>
+      </c>
       <c r="M13" s="9"/>
       <c r="N13" s="9"/>
-      <c r="O13" s="9" t="s">
-        <v>134</v>
-      </c>
+      <c r="O13" s="9"/>
       <c r="P13" s="9" t="s">
         <v>133</v>
       </c>
       <c r="Q13" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="R13" s="9">
+        <v>132</v>
+      </c>
+      <c r="R13" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="S13" s="9">
         <v>1332</v>
       </c>
-      <c r="S13" s="9">
+      <c r="T13" s="9">
         <v>484</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A14" s="9">
         <v>13010010</v>
       </c>
@@ -2938,39 +2982,42 @@
       <c r="D14" s="9">
         <v>10</v>
       </c>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9">
+      <c r="E14" s="9">
+        <v>13010006</v>
+      </c>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9">
         <v>1</v>
       </c>
-      <c r="I14" s="9"/>
       <c r="J14" s="9"/>
       <c r="K14" s="9"/>
       <c r="L14" s="9"/>
-      <c r="M14" s="9">
+      <c r="M14" s="9"/>
+      <c r="N14" s="9">
         <v>1</v>
       </c>
-      <c r="N14" s="9"/>
-      <c r="O14" s="9" t="s">
-        <v>135</v>
-      </c>
+      <c r="O14" s="9"/>
       <c r="P14" s="9" t="s">
-        <v>45</v>
+        <v>134</v>
       </c>
       <c r="Q14" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="R14" s="9">
+        <v>44</v>
+      </c>
+      <c r="R14" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="S14" s="9">
         <v>1441</v>
       </c>
-      <c r="S14" s="9">
+      <c r="T14" s="9">
         <v>527</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A15" s="9">
         <v>13010011</v>
       </c>
@@ -2983,43 +3030,46 @@
       <c r="D15" s="9">
         <v>12</v>
       </c>
-      <c r="E15" s="9" t="s">
-        <v>99</v>
+      <c r="E15" s="9">
+        <v>13010006</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9">
+        <v>98</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9">
         <v>1</v>
       </c>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9">
+      <c r="J15" s="9"/>
+      <c r="K15" s="9">
         <v>1</v>
       </c>
-      <c r="K15" s="9"/>
       <c r="L15" s="9"/>
       <c r="M15" s="9"/>
-      <c r="N15" s="9" t="s">
+      <c r="N15" s="9"/>
+      <c r="O15" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="O15" s="9" t="s">
-        <v>136</v>
-      </c>
       <c r="P15" s="9" t="s">
-        <v>46</v>
+        <v>135</v>
       </c>
       <c r="Q15" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="R15" s="9">
+        <v>45</v>
+      </c>
+      <c r="R15" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="S15" s="9">
         <v>1574</v>
       </c>
-      <c r="S15" s="9">
+      <c r="T15" s="9">
         <v>373</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A16" s="9">
         <v>13010012</v>
       </c>
@@ -3032,39 +3082,42 @@
       <c r="D16" s="9">
         <v>3</v>
       </c>
-      <c r="E16" s="9" t="s">
-        <v>116</v>
+      <c r="E16" s="9">
+        <v>13010006</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9">
+        <v>115</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9">
         <v>1</v>
       </c>
-      <c r="I16" s="9"/>
       <c r="J16" s="9"/>
       <c r="K16" s="9"/>
       <c r="L16" s="9"/>
       <c r="M16" s="9"/>
       <c r="N16" s="9"/>
-      <c r="O16" s="9" t="s">
-        <v>137</v>
-      </c>
+      <c r="O16" s="9"/>
       <c r="P16" s="9" t="s">
-        <v>40</v>
+        <v>136</v>
       </c>
       <c r="Q16" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="R16" s="9">
+        <v>39</v>
+      </c>
+      <c r="R16" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="S16" s="9">
         <v>1251</v>
       </c>
-      <c r="S16" s="9">
+      <c r="T16" s="9">
         <v>432</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A17" s="9">
         <v>13010013</v>
       </c>
@@ -3077,39 +3130,42 @@
       <c r="D17" s="9">
         <v>6</v>
       </c>
-      <c r="E17" s="9" t="s">
-        <v>114</v>
+      <c r="E17" s="9">
+        <v>13010006</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9">
+        <v>113</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9">
         <v>1</v>
       </c>
-      <c r="I17" s="9"/>
       <c r="J17" s="9"/>
       <c r="K17" s="9"/>
       <c r="L17" s="9"/>
       <c r="M17" s="9"/>
       <c r="N17" s="9"/>
-      <c r="O17" s="9" t="s">
-        <v>138</v>
-      </c>
+      <c r="O17" s="9"/>
       <c r="P17" s="9" t="s">
-        <v>44</v>
+        <v>137</v>
       </c>
       <c r="Q17" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="R17" s="9">
+        <v>43</v>
+      </c>
+      <c r="R17" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="S17" s="9">
         <v>1250</v>
       </c>
-      <c r="S17" s="9">
+      <c r="T17" s="9">
         <v>338</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A18" s="9">
         <v>13010014</v>
       </c>
@@ -3122,43 +3178,46 @@
       <c r="D18" s="9">
         <v>14</v>
       </c>
-      <c r="E18" s="9" t="s">
-        <v>111</v>
+      <c r="E18" s="9">
+        <v>13010006</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9">
+        <v>110</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9">
         <v>1</v>
       </c>
-      <c r="I18" s="9"/>
       <c r="J18" s="9"/>
       <c r="K18" s="9"/>
-      <c r="L18" s="9">
-        <v>1</v>
-      </c>
+      <c r="L18" s="9"/>
       <c r="M18" s="9">
         <v>1</v>
       </c>
-      <c r="N18" s="9"/>
-      <c r="O18" s="9" t="s">
-        <v>139</v>
-      </c>
+      <c r="N18" s="9">
+        <v>1</v>
+      </c>
+      <c r="O18" s="9"/>
       <c r="P18" s="9" t="s">
-        <v>47</v>
+        <v>138</v>
       </c>
       <c r="Q18" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="R18" s="9">
+        <v>46</v>
+      </c>
+      <c r="R18" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="S18" s="9">
         <v>1550</v>
       </c>
-      <c r="S18" s="9">
+      <c r="T18" s="9">
         <v>505</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A19" s="9">
         <v>13010015</v>
       </c>
@@ -3171,41 +3230,44 @@
       <c r="D19" s="9">
         <v>16</v>
       </c>
-      <c r="E19" s="9" t="s">
-        <v>117</v>
+      <c r="E19" s="9">
+        <v>13010016</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9">
+        <v>116</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9">
         <v>1</v>
       </c>
-      <c r="I19" s="9"/>
       <c r="J19" s="9"/>
-      <c r="K19" s="9">
+      <c r="K19" s="9"/>
+      <c r="L19" s="9">
         <v>1</v>
       </c>
-      <c r="L19" s="9"/>
       <c r="M19" s="9"/>
       <c r="N19" s="9"/>
-      <c r="O19" s="9" t="s">
-        <v>140</v>
-      </c>
+      <c r="O19" s="9"/>
       <c r="P19" s="9" t="s">
-        <v>51</v>
+        <v>139</v>
       </c>
       <c r="Q19" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="R19" s="9">
+        <v>50</v>
+      </c>
+      <c r="R19" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="S19" s="9">
         <v>1040</v>
       </c>
-      <c r="S19" s="9">
+      <c r="T19" s="9">
         <v>538</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A20" s="9">
         <v>13010016</v>
       </c>
@@ -3218,7 +3280,9 @@
       <c r="D20" s="9">
         <v>16</v>
       </c>
-      <c r="E20" s="9"/>
+      <c r="E20" s="9">
+        <v>13010016</v>
+      </c>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
       <c r="H20" s="9"/>
@@ -3228,28 +3292,29 @@
       <c r="L20" s="9"/>
       <c r="M20" s="9"/>
       <c r="N20" s="9"/>
-      <c r="O20" s="9" t="s">
-        <v>141</v>
-      </c>
+      <c r="O20" s="9"/>
       <c r="P20" s="9" t="s">
-        <v>54</v>
+        <v>140</v>
       </c>
       <c r="Q20" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="R20" s="9">
+        <v>53</v>
+      </c>
+      <c r="R20" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="S20" s="9">
         <v>919</v>
       </c>
-      <c r="S20" s="9">
+      <c r="T20" s="9">
         <v>534</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A21" s="9">
         <v>13010017</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C21" s="9">
         <v>2</v>
@@ -3257,46 +3322,49 @@
       <c r="D21" s="9">
         <v>18</v>
       </c>
-      <c r="E21" s="9" t="s">
-        <v>112</v>
+      <c r="E21" s="9">
+        <v>13010016</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9">
+        <v>111</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9">
         <v>1</v>
       </c>
-      <c r="I21" s="9"/>
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
-      <c r="L21" s="9">
+      <c r="L21" s="9"/>
+      <c r="M21" s="9">
         <v>1</v>
       </c>
-      <c r="M21" s="9"/>
       <c r="N21" s="9"/>
-      <c r="O21" s="9" t="s">
-        <v>142</v>
-      </c>
+      <c r="O21" s="9"/>
       <c r="P21" s="9" t="s">
-        <v>53</v>
+        <v>141</v>
       </c>
       <c r="Q21" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="R21" s="9">
+        <v>52</v>
+      </c>
+      <c r="R21" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="S21" s="9">
         <v>1149</v>
       </c>
-      <c r="S21" s="9">
+      <c r="T21" s="9">
         <v>584</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A22" s="9">
         <v>13010018</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C22" s="9">
         <v>2</v>
@@ -3304,13 +3372,15 @@
       <c r="D22" s="9">
         <v>20</v>
       </c>
-      <c r="E22" s="9" t="s">
-        <v>97</v>
+      <c r="E22" s="9">
+        <v>13010016</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="G22" s="9"/>
+        <v>96</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>120</v>
+      </c>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
@@ -3318,28 +3388,29 @@
       <c r="L22" s="9"/>
       <c r="M22" s="9"/>
       <c r="N22" s="9"/>
-      <c r="O22" s="9" t="s">
-        <v>143</v>
-      </c>
+      <c r="O22" s="9"/>
       <c r="P22" s="9" t="s">
-        <v>55</v>
+        <v>142</v>
       </c>
       <c r="Q22" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="R22" s="9">
+        <v>54</v>
+      </c>
+      <c r="R22" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="S22" s="9">
         <v>840</v>
       </c>
-      <c r="S22" s="9">
+      <c r="T22" s="9">
         <v>444</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A23" s="9">
         <v>13020001</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C23" s="9">
         <v>3</v>
@@ -3347,36 +3418,39 @@
       <c r="D23" s="9">
         <v>3</v>
       </c>
-      <c r="E23" s="13" t="s">
-        <v>149</v>
-      </c>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="H23" s="9"/>
+      <c r="E23" s="9">
+        <v>13000002</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9" t="s">
+        <v>145</v>
+      </c>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
       <c r="K23" s="9"/>
       <c r="L23" s="9"/>
       <c r="M23" s="9"/>
       <c r="N23" s="9"/>
-      <c r="O23" s="9" t="s">
-        <v>144</v>
-      </c>
+      <c r="O23" s="9"/>
       <c r="P23" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="Q23" s="9"/>
+        <v>143</v>
+      </c>
+      <c r="Q23" s="9" t="s">
+        <v>143</v>
+      </c>
       <c r="R23" s="9"/>
       <c r="S23" s="9"/>
+      <c r="T23" s="9"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A24" s="9">
         <v>13020002</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C24" s="9">
         <v>3</v>
@@ -3384,8 +3458,10 @@
       <c r="D24" s="9">
         <v>3</v>
       </c>
-      <c r="E24" s="12"/>
-      <c r="F24" s="9"/>
+      <c r="E24" s="9">
+        <v>13000002</v>
+      </c>
+      <c r="F24" s="12"/>
       <c r="G24" s="9"/>
       <c r="H24" s="9"/>
       <c r="I24" s="9"/>
@@ -3394,25 +3470,26 @@
       <c r="L24" s="9"/>
       <c r="M24" s="9"/>
       <c r="N24" s="9"/>
-      <c r="O24" s="9" t="s">
-        <v>145</v>
-      </c>
+      <c r="O24" s="9"/>
       <c r="P24" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="Q24" s="9"/>
+        <v>144</v>
+      </c>
+      <c r="Q24" s="9" t="s">
+        <v>144</v>
+      </c>
       <c r="R24" s="9"/>
       <c r="S24" s="9"/>
+      <c r="T24" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="H4:M24">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+  <conditionalFormatting sqref="I4:N24">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+  <conditionalFormatting sqref="J4">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
simply made the pursemaze
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Scene.xlsx
+++ b/ConfigData/Xlsx/Scene.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17571"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="162">
   <si>
     <t>村外小屋</t>
   </si>
@@ -589,13 +589,36 @@
   </si>
   <si>
     <t>met;30|icedream;25</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>古城大厅</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>persepalace1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>persepalace2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>persepalace3</t>
+  </si>
+  <si>
+    <t>古城外围</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>古城大殿</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1974,74 +1997,6 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2054,8 +2009,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:T24" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21" tableBorderDxfId="20">
-  <autoFilter ref="A3:T24"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:T27" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21" tableBorderDxfId="20">
+  <autoFilter ref="A3:T27"/>
   <tableColumns count="20">
     <tableColumn id="1" name="Id" dataDxfId="19"/>
     <tableColumn id="2" name="Name" dataDxfId="18"/>
@@ -2083,14 +2038,14 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="CAEACD"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -2158,6 +2113,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2193,6 +2165,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2369,10 +2358,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T24"/>
+  <dimension ref="A1:T27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3573,9 +3562,119 @@
       <c r="S24" s="9"/>
       <c r="T24" s="9"/>
     </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A25" s="14">
+        <v>13020011</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="C25" s="14">
+        <v>3</v>
+      </c>
+      <c r="D25" s="9">
+        <v>8</v>
+      </c>
+      <c r="E25" s="9">
+        <v>13010007</v>
+      </c>
+      <c r="F25" s="12"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q25" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="R25" s="9"/>
+      <c r="S25" s="9"/>
+      <c r="T25" s="9"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A26" s="14">
+        <v>13020012</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="C26" s="14">
+        <v>3</v>
+      </c>
+      <c r="D26" s="9">
+        <v>8</v>
+      </c>
+      <c r="E26" s="9">
+        <v>13010007</v>
+      </c>
+      <c r="F26" s="12"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="9"/>
+      <c r="M26" s="9"/>
+      <c r="N26" s="9"/>
+      <c r="O26" s="9"/>
+      <c r="P26" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q26" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="R26" s="9"/>
+      <c r="S26" s="9"/>
+      <c r="T26" s="9"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A27" s="14">
+        <v>13020013</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="C27" s="14">
+        <v>3</v>
+      </c>
+      <c r="D27" s="9">
+        <v>8</v>
+      </c>
+      <c r="E27" s="9">
+        <v>13010007</v>
+      </c>
+      <c r="F27" s="12"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="9"/>
+      <c r="M27" s="9"/>
+      <c r="N27" s="9"/>
+      <c r="O27" s="9"/>
+      <c r="P27" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q27" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="R27" s="9"/>
+      <c r="S27" s="9"/>
+      <c r="T27" s="9"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="I4:N24">
+  <conditionalFormatting sqref="I4:N27">
     <cfRule type="cellIs" dxfId="24" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
add a new scene chanel. scenequest support time control
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Scene.xlsx
+++ b/ConfigData/Xlsx/Scene.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="161">
   <si>
     <t>村外小屋</t>
   </si>
@@ -27,9 +27,6 @@
     <t>昏暗密林</t>
   </si>
   <si>
-    <t>精灵之都-卡莱</t>
-  </si>
-  <si>
     <t>登拉克峡谷</t>
   </si>
   <si>
@@ -45,581 +42,583 @@
     <t>GameIconsCatch</t>
   </si>
   <si>
+    <t>村外田园</t>
+  </si>
+  <si>
+    <t>黄金海岸</t>
+  </si>
+  <si>
+    <t>孤岛遗迹</t>
+  </si>
+  <si>
+    <t>GameBattleRobot</t>
+  </si>
+  <si>
+    <t>小树林</t>
+  </si>
+  <si>
+    <t>玲珑峰</t>
+  </si>
+  <si>
+    <t>遗迹河滩</t>
+  </si>
+  <si>
+    <t>雾谷</t>
+  </si>
+  <si>
+    <t>木阴之村</t>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>序列</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>名字</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>等级</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>功能列表</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>场景背景</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>Func</t>
+  </si>
+  <si>
+    <t>Url</t>
+  </si>
+  <si>
+    <t>TilePath</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>配置</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>home</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Quest</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>任务列表</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>darkforest</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>tatamuviliage</t>
+  </si>
+  <si>
+    <t>smallforest</t>
+  </si>
+  <si>
+    <t>perse</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>demlock</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>hightower</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>smallhill</t>
+  </si>
+  <si>
+    <t>goldseashore</t>
+  </si>
+  <si>
+    <t>islandold</t>
+  </si>
+  <si>
+    <t>riverold</t>
+  </si>
+  <si>
+    <t>落潮小径</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>月光林地</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>gerdin</t>
+  </si>
+  <si>
+    <t>fogvalley</t>
+  </si>
+  <si>
+    <t>矿脉山脚</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>riverside</t>
+  </si>
+  <si>
+    <t>woodviliage</t>
+  </si>
+  <si>
+    <t>moonforest</t>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>激活传送门</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QPortal</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QCardChange</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>卡牌交换</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>素材商人</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QPiece</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QMerchant</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QDoctor</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QAngel</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>商人</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>医生</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>天使</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>IconX</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>IconY</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Icon</t>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwxw</t>
+  </si>
+  <si>
+    <t>haml</t>
+  </si>
+  <si>
+    <t>kk</t>
+  </si>
+  <si>
+    <t>dlkxg</t>
+  </si>
+  <si>
+    <t>bstgt</t>
+  </si>
+  <si>
+    <t>ttmc</t>
+  </si>
+  <si>
+    <t>psgc</t>
+  </si>
+  <si>
+    <t>gdh</t>
+  </si>
+  <si>
+    <t>cwyy</t>
+  </si>
+  <si>
+    <t>hjha</t>
+  </si>
+  <si>
+    <t>gdyj</t>
+  </si>
+  <si>
+    <t>xsl</t>
+  </si>
+  <si>
+    <t>llf</t>
+  </si>
+  <si>
+    <t>yjht</t>
+  </si>
+  <si>
+    <t>wg</t>
+  </si>
+  <si>
+    <t>myzc</t>
+  </si>
+  <si>
+    <t>lcxj</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ygld</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>小图标x</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>小图标y</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>图标路径</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>GameUpToNumber;GameThreeBody</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>poppyfield;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trees;3|mushroom;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>sewer;3|river;2|fortune;1|oldtree;1|poppyfield;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>fortune;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>wolfnest;2|gamble;1|fishpool;2|sewer;3|river;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>小概率任务</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QuestRandom</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|treasure;25</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>类型</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Type</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>portal;1|fishpool;1|grave;2|hiddeway;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>river;2|fishpool;1|swamp;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>mushroom;1|hiddeway;1|swamp;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>orehole;1|stone;2|sandflow;2</t>
+  </si>
+  <si>
+    <t>coldwind;3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ruintown1;1|manflower;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trees;3|grave;1|portal;1|oldtree;1|manflower;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>portal;3|sandflow;2|manflower;3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>river;2|stone;3|ruintown1;1|hiddeway;1|manflower;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|witchhome;30</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|treasure;25|witchhome;20</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|forestfire;20|witchhome;40</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>forestfire;10</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>forestfire;35|witchhome;10</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>密林迷宫</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>迷宫深处</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>home</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>orevalley</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>hightower</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>tatamuviliage</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>perse</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>gerdin</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>farm</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>farm</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>goldseashore</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>islandold</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>smallforest</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>smallhill</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>riverold</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>fogvalley</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>woodviliage</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>riverside</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>moonforest</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>forestmaze</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>forestinner</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>副本任务列表</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QuestDungeon</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>forestentry;2|forestentry2;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>复活地图</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ReviveScene</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trees;4|manflower;2|portal;1|sandland;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|goblinhome;40</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|goblinhome;30</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>goblinhome;50</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|icedream;25</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>古城大厅</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>persepalace1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>persepalace2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>persepalace3</t>
+  </si>
+  <si>
+    <t>古城外围</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>古城大殿</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>persepalace2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>玲珑峰隧道</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>smallhillchanel</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>格丁湖</t>
-  </si>
-  <si>
-    <t>村外田园</t>
-  </si>
-  <si>
-    <t>黄金海岸</t>
-  </si>
-  <si>
-    <t>孤岛遗迹</t>
-  </si>
-  <si>
-    <t>GameBattleRobot</t>
-  </si>
-  <si>
-    <t>小树林</t>
-  </si>
-  <si>
-    <t>玲珑峰</t>
-  </si>
-  <si>
-    <t>遗迹河滩</t>
-  </si>
-  <si>
-    <t>雾谷</t>
-  </si>
-  <si>
-    <t>木阴之村</t>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>序列</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>名字</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>等级</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>功能列表</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>场景背景</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Id</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Level</t>
-  </si>
-  <si>
-    <t>Func</t>
-  </si>
-  <si>
-    <t>Url</t>
-  </si>
-  <si>
-    <t>TilePath</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>配置</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>default</t>
-  </si>
-  <si>
-    <t>home</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Quest</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>任务列表</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>darkforest</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>tatamuviliage</t>
-  </si>
-  <si>
-    <t>smallforest</t>
-  </si>
-  <si>
-    <t>perse</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>demlock</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>hightower</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>smallhill</t>
-  </si>
-  <si>
-    <t>goldseashore</t>
-  </si>
-  <si>
-    <t>islandold</t>
-  </si>
-  <si>
-    <t>riverold</t>
-  </si>
-  <si>
-    <t>落潮小径</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>月光林地</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>gerdin</t>
-  </si>
-  <si>
-    <t>fogvalley</t>
-  </si>
-  <si>
-    <t>矿脉山脚</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>riverside</t>
-  </si>
-  <si>
-    <t>woodviliage</t>
-  </si>
-  <si>
-    <t>moonforest</t>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>激活传送门</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>QPortal</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>QCardChange</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>卡牌交换</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>素材商人</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>QPiece</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>QMerchant</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>QDoctor</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>QAngel</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>商人</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>医生</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>天使</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>IconX</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>IconY</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Icon</t>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>cwxw</t>
-  </si>
-  <si>
-    <t>haml</t>
-  </si>
-  <si>
-    <t>kk</t>
-  </si>
-  <si>
-    <t>dlkxg</t>
-  </si>
-  <si>
-    <t>bstgt</t>
-  </si>
-  <si>
-    <t>ttmc</t>
-  </si>
-  <si>
-    <t>psgc</t>
-  </si>
-  <si>
-    <t>gdh</t>
-  </si>
-  <si>
-    <t>cwyy</t>
-  </si>
-  <si>
-    <t>hjha</t>
-  </si>
-  <si>
-    <t>gdyj</t>
-  </si>
-  <si>
-    <t>xsl</t>
-  </si>
-  <si>
-    <t>llf</t>
-  </si>
-  <si>
-    <t>yjht</t>
-  </si>
-  <si>
-    <t>wg</t>
-  </si>
-  <si>
-    <t>myzc</t>
-  </si>
-  <si>
-    <t>lcxj</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ygld</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>小图标x</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>小图标y</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>图标路径</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>GameUpToNumber;GameThreeBody</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>poppyfield;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>trees;3|mushroom;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>sewer;3|river;2|fortune;1|oldtree;1|poppyfield;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>fortune;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>wolfnest;2|gamble;1|fishpool;2|sewer;3|river;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>小概率任务</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>QuestRandom</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|treasure;25</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>类型</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Type</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>portal;1|fishpool;1|grave;2|hiddeway;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>river;2|fishpool;1|swamp;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>mushroom;1|hiddeway;1|swamp;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>orehole;1|stone;2|sandflow;2</t>
-  </si>
-  <si>
-    <t>coldwind;3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ruintown1;1|manflower;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>trees;3|grave;1|portal;1|oldtree;1|manflower;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>portal;3|sandflow;2|manflower;3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>river;2|stone;3|ruintown1;1|hiddeway;1|manflower;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|witchhome;30</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|treasure;25|witchhome;20</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|forestfire;20|witchhome;40</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>forestfire;10</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>forestfire;35|witchhome;10</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>密林迷宫</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>迷宫深处</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>home</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>orevalley</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>default</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>hightower</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>tatamuviliage</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>perse</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>gerdin</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>farm</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>farm</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>goldseashore</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>islandold</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>smallforest</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>smallhill</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>riverold</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>fogvalley</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>woodviliage</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>riverside</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>moonforest</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>forestmaze</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>forestinner</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>副本任务列表</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>QuestDungeon</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>forestentry;2|forestentry2;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>复活地图</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ReviveScene</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>13000001|BornMapId</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>trees;4|manflower;2|portal;1|sandland;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|goblinhome;40</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|goblinhome;30</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>goblinhome;50</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|icedream;25</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>古城大厅</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>persepalace1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>persepalace2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>persepalace3</t>
-  </si>
-  <si>
-    <t>古城外围</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>古城大殿</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="22" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -806,8 +805,15 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="38">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1014,6 +1020,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1293,7 +1311,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1337,6 +1355,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1385,6 +1412,20 @@
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="25">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1981,22 +2022,76 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2009,43 +2104,46 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:T27" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21" tableBorderDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:T27" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23" tableBorderDxfId="22">
   <autoFilter ref="A3:T27"/>
+  <sortState ref="A4:T27">
+    <sortCondition ref="A3:A27"/>
+  </sortState>
   <tableColumns count="20">
-    <tableColumn id="1" name="Id" dataDxfId="19"/>
-    <tableColumn id="2" name="Name" dataDxfId="18"/>
-    <tableColumn id="18" name="Type" dataDxfId="17"/>
-    <tableColumn id="3" name="Level" dataDxfId="16"/>
-    <tableColumn id="20" name="ReviveScene" dataDxfId="15"/>
-    <tableColumn id="4" name="Quest" dataDxfId="14"/>
-    <tableColumn id="17" name="QuestRandom" dataDxfId="13"/>
-    <tableColumn id="19" name="QuestDungeon" dataDxfId="12"/>
-    <tableColumn id="5" name="QPortal" dataDxfId="11"/>
-    <tableColumn id="6" name="QCardChange" dataDxfId="10"/>
-    <tableColumn id="7" name="QPiece" dataDxfId="9"/>
-    <tableColumn id="8" name="QMerchant" dataDxfId="8"/>
-    <tableColumn id="9" name="QDoctor" dataDxfId="7"/>
-    <tableColumn id="10" name="QAngel" dataDxfId="6"/>
-    <tableColumn id="11" name="Func" dataDxfId="5"/>
-    <tableColumn id="12" name="Url" dataDxfId="4"/>
-    <tableColumn id="13" name="TilePath" dataDxfId="3"/>
-    <tableColumn id="14" name="Icon" dataDxfId="2"/>
-    <tableColumn id="15" name="IconX" dataDxfId="1"/>
-    <tableColumn id="16" name="IconY" dataDxfId="0"/>
+    <tableColumn id="1" name="Id" dataDxfId="21"/>
+    <tableColumn id="2" name="Name" dataDxfId="20"/>
+    <tableColumn id="18" name="Type" dataDxfId="19"/>
+    <tableColumn id="3" name="Level" dataDxfId="18"/>
+    <tableColumn id="20" name="ReviveScene" dataDxfId="17"/>
+    <tableColumn id="4" name="Quest" dataDxfId="16"/>
+    <tableColumn id="17" name="QuestRandom" dataDxfId="15"/>
+    <tableColumn id="19" name="QuestDungeon" dataDxfId="14"/>
+    <tableColumn id="5" name="QPortal" dataDxfId="13"/>
+    <tableColumn id="6" name="QCardChange" dataDxfId="12"/>
+    <tableColumn id="7" name="QPiece" dataDxfId="11"/>
+    <tableColumn id="8" name="QMerchant" dataDxfId="10"/>
+    <tableColumn id="9" name="QDoctor" dataDxfId="9"/>
+    <tableColumn id="10" name="QAngel" dataDxfId="8"/>
+    <tableColumn id="11" name="Func" dataDxfId="7"/>
+    <tableColumn id="12" name="Url" dataDxfId="6"/>
+    <tableColumn id="13" name="TilePath" dataDxfId="5"/>
+    <tableColumn id="14" name="Icon" dataDxfId="4"/>
+    <tableColumn id="15" name="IconX" dataDxfId="3"/>
+    <tableColumn id="16" name="IconY" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="CAEACD"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -2113,23 +2211,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2165,23 +2246,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2361,7 +2425,7 @@
   <dimension ref="A1:T27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2384,195 +2448,195 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="E1" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="O1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>24</v>
-      </c>
       <c r="Q1" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="S1" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="T1" s="8" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A3" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="E3" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="M3" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="N3" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="O3" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="D3" s="10" t="s">
+      <c r="P3" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="K3" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="L3" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="M3" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="N3" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="O3" s="10" t="s">
+      <c r="Q3" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="P3" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q3" s="10" t="s">
-        <v>30</v>
-      </c>
       <c r="R3" s="10" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="S3" s="10" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="T3" s="10" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A4" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="B4" s="9" t="s">
+      <c r="A4" s="16">
+        <v>13010001</v>
+      </c>
+      <c r="B4" s="16" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="9">
@@ -2585,7 +2649,7 @@
         <v>13000001</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
@@ -2598,16 +2662,16 @@
       <c r="M4" s="9"/>
       <c r="N4" s="9"/>
       <c r="O4" s="9" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="P4" s="9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="Q4" s="9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="R4" s="9" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="S4" s="9">
         <v>1348</v>
@@ -2617,10 +2681,10 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A5" s="9">
-        <v>13000002</v>
-      </c>
-      <c r="B5" s="9" t="s">
+      <c r="A5" s="16">
+        <v>13010002</v>
+      </c>
+      <c r="B5" s="16" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="9">
@@ -2633,10 +2697,10 @@
         <v>13000001</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H5" s="9"/>
       <c r="I5" s="9">
@@ -2653,13 +2717,13 @@
       <c r="N5" s="9"/>
       <c r="O5" s="9"/>
       <c r="P5" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="Q5" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="R5" s="9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="S5" s="9">
         <v>1279</v>
@@ -2669,26 +2733,26 @@
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A6" s="9">
-        <v>13000003</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>51</v>
+      <c r="A6" s="16">
+        <v>13010004</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>2</v>
       </c>
       <c r="C6" s="9">
         <v>2</v>
       </c>
       <c r="D6" s="9">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="E6" s="9">
-        <v>13010016</v>
+        <v>13010006</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="H6" s="9"/>
       <c r="I6" s="9">
@@ -2696,185 +2760,205 @@
       </c>
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
+      <c r="L6" s="9">
+        <v>1</v>
+      </c>
       <c r="M6" s="9"/>
       <c r="N6" s="9"/>
       <c r="O6" s="9"/>
       <c r="P6" s="9" t="s">
-        <v>125</v>
+        <v>38</v>
       </c>
       <c r="Q6" s="9" t="s">
-        <v>125</v>
+        <v>38</v>
       </c>
       <c r="R6" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="S6" s="9">
-        <v>1213</v>
+        <v>1148</v>
       </c>
       <c r="T6" s="9">
-        <v>655</v>
+        <v>351</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A7" s="9">
-        <v>13010001</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>2</v>
+      <c r="A7" s="16">
+        <v>13010005</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>3</v>
       </c>
       <c r="C7" s="9">
         <v>2</v>
       </c>
       <c r="D7" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E7" s="9">
         <v>13010006</v>
       </c>
       <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
+      <c r="G7" s="9" t="s">
+        <v>149</v>
+      </c>
       <c r="H7" s="9"/>
       <c r="I7" s="9">
         <v>1</v>
       </c>
-      <c r="J7" s="9"/>
+      <c r="J7" s="9">
+        <v>1</v>
+      </c>
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
       <c r="M7" s="9"/>
       <c r="N7" s="9"/>
       <c r="O7" s="9"/>
       <c r="P7" s="9" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="Q7" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="R7" s="9"/>
-      <c r="S7" s="9"/>
-      <c r="T7" s="9"/>
+        <v>39</v>
+      </c>
+      <c r="R7" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="S7" s="9">
+        <v>1386</v>
+      </c>
+      <c r="T7" s="9">
+        <v>339</v>
+      </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A8" s="9">
-        <v>13010004</v>
-      </c>
-      <c r="B8" s="9" t="s">
+      <c r="A8" s="16">
+        <v>13010006</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="9">
+        <v>1</v>
+      </c>
+      <c r="D8" s="9">
         <v>3</v>
-      </c>
-      <c r="C8" s="9">
-        <v>2</v>
-      </c>
-      <c r="D8" s="9">
-        <v>5</v>
       </c>
       <c r="E8" s="9">
         <v>13010006</v>
       </c>
-      <c r="F8" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>118</v>
-      </c>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
       <c r="H8" s="9"/>
-      <c r="I8" s="9">
-        <v>1</v>
-      </c>
+      <c r="I8" s="9"/>
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
-      <c r="L8" s="9">
-        <v>1</v>
-      </c>
+      <c r="L8" s="9"/>
       <c r="M8" s="9"/>
       <c r="N8" s="9"/>
       <c r="O8" s="9"/>
       <c r="P8" s="9" t="s">
-        <v>41</v>
+        <v>124</v>
       </c>
       <c r="Q8" s="9" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="R8" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="S8" s="9">
-        <v>1148</v>
+        <v>1232</v>
       </c>
       <c r="T8" s="9">
-        <v>351</v>
+        <v>506</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A9" s="9">
-        <v>13010005</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>4</v>
+      <c r="A9" s="16">
+        <v>13010007</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>5</v>
       </c>
       <c r="C9" s="9">
         <v>2</v>
       </c>
       <c r="D9" s="9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E9" s="9">
         <v>13010006</v>
       </c>
-      <c r="F9" s="9"/>
+      <c r="F9" s="9" t="s">
+        <v>105</v>
+      </c>
       <c r="G9" s="9" t="s">
-        <v>154</v>
+        <v>101</v>
       </c>
       <c r="H9" s="9"/>
       <c r="I9" s="9">
         <v>1</v>
       </c>
-      <c r="J9" s="9">
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9">
         <v>1</v>
       </c>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
+      <c r="M9" s="9">
+        <v>1</v>
+      </c>
       <c r="N9" s="9"/>
-      <c r="O9" s="9"/>
+      <c r="O9" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="P9" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="Q9" s="9" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="R9" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="S9" s="9">
-        <v>1386</v>
+        <v>1431</v>
       </c>
       <c r="T9" s="9">
-        <v>339</v>
+        <v>440</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A10" s="9">
-        <v>13010006</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>5</v>
+      <c r="A10" s="16">
+        <v>13010009</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>7</v>
       </c>
       <c r="C10" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E10" s="9">
         <v>13010006</v>
       </c>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
+      <c r="F10" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>148</v>
+      </c>
       <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
+      <c r="I10" s="9">
+        <v>1</v>
+      </c>
+      <c r="J10" s="9">
+        <v>1</v>
+      </c>
       <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
+      <c r="L10" s="9">
+        <v>1</v>
+      </c>
       <c r="M10" s="9"/>
       <c r="N10" s="9"/>
       <c r="O10" s="9"/>
@@ -2882,39 +2966,37 @@
         <v>128</v>
       </c>
       <c r="Q10" s="9" t="s">
-        <v>38</v>
+        <v>127</v>
       </c>
       <c r="R10" s="9" t="s">
         <v>77</v>
       </c>
       <c r="S10" s="9">
-        <v>1232</v>
+        <v>1332</v>
       </c>
       <c r="T10" s="9">
-        <v>506</v>
+        <v>484</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A11" s="9">
-        <v>13010007</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>6</v>
+      <c r="A11" s="16">
+        <v>13010010</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>8</v>
       </c>
       <c r="C11" s="9">
         <v>2</v>
       </c>
       <c r="D11" s="9">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E11" s="9">
         <v>13010006</v>
       </c>
-      <c r="F11" s="9" t="s">
-        <v>108</v>
-      </c>
+      <c r="F11" s="9"/>
       <c r="G11" s="9" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H11" s="9"/>
       <c r="I11" s="9">
@@ -2922,153 +3004,149 @@
       </c>
       <c r="J11" s="9"/>
       <c r="K11" s="9"/>
-      <c r="L11" s="9">
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9">
         <v>1</v>
       </c>
-      <c r="M11" s="9">
-        <v>1</v>
-      </c>
-      <c r="N11" s="9"/>
-      <c r="O11" s="9" t="s">
-        <v>7</v>
-      </c>
+      <c r="O11" s="9"/>
       <c r="P11" s="9" t="s">
         <v>129</v>
       </c>
       <c r="Q11" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="R11" s="9" t="s">
         <v>78</v>
       </c>
       <c r="S11" s="9">
-        <v>1431</v>
+        <v>1441</v>
       </c>
       <c r="T11" s="9">
-        <v>440</v>
+        <v>527</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A12" s="9">
-        <v>13010008</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>8</v>
+      <c r="A12" s="16">
+        <v>13010011</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>9</v>
       </c>
       <c r="C12" s="9">
         <v>2</v>
       </c>
       <c r="D12" s="9">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E12" s="9">
-        <v>13010016</v>
+        <v>13010006</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>95</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="H12" s="9"/>
       <c r="I12" s="9">
         <v>1</v>
       </c>
       <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
+      <c r="K12" s="9">
+        <v>1</v>
+      </c>
       <c r="L12" s="9"/>
       <c r="M12" s="9"/>
-      <c r="N12" s="9">
-        <v>1</v>
-      </c>
-      <c r="O12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9" t="s">
+        <v>10</v>
+      </c>
       <c r="P12" s="9" t="s">
         <v>130</v>
       </c>
       <c r="Q12" s="9" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="R12" s="9" t="s">
         <v>79</v>
       </c>
       <c r="S12" s="9">
-        <v>1067</v>
+        <v>1574</v>
       </c>
       <c r="T12" s="9">
-        <v>445</v>
+        <v>373</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A13" s="9">
-        <v>13010009</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>9</v>
+      <c r="A13" s="16">
+        <v>13010012</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>11</v>
       </c>
       <c r="C13" s="9">
         <v>2</v>
       </c>
       <c r="D13" s="9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E13" s="9">
         <v>13010006</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>153</v>
+        <v>118</v>
       </c>
       <c r="H13" s="9"/>
       <c r="I13" s="9">
         <v>1</v>
       </c>
-      <c r="J13" s="9">
-        <v>1</v>
-      </c>
+      <c r="J13" s="9"/>
       <c r="K13" s="9"/>
-      <c r="L13" s="9">
-        <v>1</v>
-      </c>
+      <c r="L13" s="9"/>
       <c r="M13" s="9"/>
       <c r="N13" s="9"/>
       <c r="O13" s="9"/>
       <c r="P13" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Q13" s="9" t="s">
-        <v>131</v>
+        <v>36</v>
       </c>
       <c r="R13" s="9" t="s">
         <v>80</v>
       </c>
       <c r="S13" s="9">
-        <v>1332</v>
+        <v>1251</v>
       </c>
       <c r="T13" s="9">
-        <v>484</v>
+        <v>432</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A14" s="9">
-        <v>13010010</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>10</v>
+      <c r="A14" s="16">
+        <v>13010013</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>12</v>
       </c>
       <c r="C14" s="9">
         <v>2</v>
       </c>
       <c r="D14" s="9">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E14" s="9">
         <v>13010006</v>
       </c>
-      <c r="F14" s="9"/>
+      <c r="F14" s="9" t="s">
+        <v>109</v>
+      </c>
       <c r="G14" s="9" t="s">
-        <v>103</v>
+        <v>150</v>
       </c>
       <c r="H14" s="9"/>
       <c r="I14" s="9">
@@ -3078,152 +3156,134 @@
       <c r="K14" s="9"/>
       <c r="L14" s="9"/>
       <c r="M14" s="9"/>
-      <c r="N14" s="9">
-        <v>1</v>
-      </c>
+      <c r="N14" s="9"/>
       <c r="O14" s="9"/>
       <c r="P14" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q14" s="9" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="R14" s="9" t="s">
         <v>81</v>
       </c>
       <c r="S14" s="9">
-        <v>1441</v>
+        <v>1250</v>
       </c>
       <c r="T14" s="9">
-        <v>527</v>
+        <v>338</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A15" s="9">
-        <v>13010011</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>11</v>
+      <c r="A15" s="16">
+        <v>13010014</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>13</v>
       </c>
       <c r="C15" s="9">
         <v>2</v>
       </c>
       <c r="D15" s="9">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E15" s="9">
         <v>13010006</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>152</v>
+        <v>114</v>
       </c>
       <c r="H15" s="9"/>
       <c r="I15" s="9">
         <v>1</v>
       </c>
       <c r="J15" s="9"/>
-      <c r="K15" s="9">
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9">
         <v>1</v>
       </c>
-      <c r="L15" s="9"/>
-      <c r="M15" s="9"/>
-      <c r="N15" s="9"/>
-      <c r="O15" s="9" t="s">
-        <v>12</v>
-      </c>
+      <c r="N15" s="9">
+        <v>1</v>
+      </c>
+      <c r="O15" s="9"/>
       <c r="P15" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="Q15" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="R15" s="9" t="s">
         <v>82</v>
       </c>
       <c r="S15" s="9">
-        <v>1574</v>
+        <v>1550</v>
       </c>
       <c r="T15" s="9">
-        <v>373</v>
+        <v>505</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A16" s="9">
-        <v>13010012</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="9">
+      <c r="A16" s="16">
+        <v>13010015</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="C16" s="15">
         <v>2</v>
       </c>
-      <c r="D16" s="9">
-        <v>3</v>
+      <c r="D16" s="15">
+        <v>6</v>
       </c>
       <c r="E16" s="9">
         <v>13010006</v>
       </c>
-      <c r="F16" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9">
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15">
         <v>1</v>
       </c>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="9"/>
-      <c r="O16" s="9"/>
-      <c r="P16" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="Q16" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="R16" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="S16" s="9">
-        <v>1251</v>
-      </c>
-      <c r="T16" s="9">
-        <v>432</v>
-      </c>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="15"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="15"/>
+      <c r="O16" s="15"/>
+      <c r="P16" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q16" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="R16" s="15"/>
+      <c r="S16" s="15"/>
+      <c r="T16" s="15"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A17" s="9">
-        <v>13010013</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>14</v>
+      <c r="A17" s="17">
+        <v>13010101</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>15</v>
       </c>
       <c r="C17" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D17" s="9">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="E17" s="9">
-        <v>13010006</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>155</v>
-      </c>
+        <v>13010101</v>
+      </c>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
       <c r="H17" s="9"/>
-      <c r="I17" s="9">
-        <v>1</v>
-      </c>
+      <c r="I17" s="9"/>
       <c r="J17" s="9"/>
       <c r="K17" s="9"/>
       <c r="L17" s="9"/>
@@ -3231,42 +3291,42 @@
       <c r="N17" s="9"/>
       <c r="O17" s="9"/>
       <c r="P17" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="Q17" s="9" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="R17" s="9" t="s">
         <v>84</v>
       </c>
       <c r="S17" s="9">
-        <v>1250</v>
+        <v>919</v>
       </c>
       <c r="T17" s="9">
-        <v>338</v>
+        <v>534</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A18" s="9">
-        <v>13010014</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>15</v>
+      <c r="A18" s="17">
+        <v>13010102</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>14</v>
       </c>
       <c r="C18" s="9">
         <v>2</v>
       </c>
       <c r="D18" s="9">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E18" s="9">
-        <v>13010006</v>
+        <v>13010101</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>117</v>
+        <v>148</v>
       </c>
       <c r="H18" s="9"/>
       <c r="I18" s="9">
@@ -3274,51 +3334,49 @@
       </c>
       <c r="J18" s="9"/>
       <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9">
+      <c r="L18" s="9">
         <v>1</v>
       </c>
-      <c r="N18" s="9">
-        <v>1</v>
-      </c>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
       <c r="O18" s="9"/>
       <c r="P18" s="9" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="Q18" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="R18" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="S18" s="9">
-        <v>1550</v>
+        <v>1040</v>
       </c>
       <c r="T18" s="9">
-        <v>505</v>
+        <v>538</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A19" s="9">
-        <v>13010015</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>16</v>
+      <c r="A19" s="17">
+        <v>13010103</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>48</v>
       </c>
       <c r="C19" s="9">
         <v>2</v>
       </c>
       <c r="D19" s="9">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E19" s="9">
-        <v>13010016</v>
+        <v>13010101</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>153</v>
+        <v>101</v>
       </c>
       <c r="H19" s="9"/>
       <c r="I19" s="9">
@@ -3326,164 +3384,170 @@
       </c>
       <c r="J19" s="9"/>
       <c r="K19" s="9"/>
-      <c r="L19" s="9">
-        <v>1</v>
-      </c>
+      <c r="L19" s="9"/>
       <c r="M19" s="9"/>
       <c r="N19" s="9"/>
       <c r="O19" s="9"/>
       <c r="P19" s="9" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="Q19" s="9" t="s">
-        <v>50</v>
+        <v>122</v>
       </c>
       <c r="R19" s="9" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="S19" s="9">
-        <v>1040</v>
+        <v>1213</v>
       </c>
       <c r="T19" s="9">
-        <v>538</v>
+        <v>655</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A20" s="9">
-        <v>13010016</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>17</v>
+      <c r="A20" s="17">
+        <v>13010104</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>44</v>
       </c>
       <c r="C20" s="9">
+        <v>2</v>
+      </c>
+      <c r="D20" s="9">
+        <v>18</v>
+      </c>
+      <c r="E20" s="9">
+        <v>13010101</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9">
         <v>1</v>
       </c>
-      <c r="D20" s="9">
-        <v>16</v>
-      </c>
-      <c r="E20" s="9">
-        <v>13010016</v>
-      </c>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
       <c r="J20" s="9"/>
       <c r="K20" s="9"/>
       <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
+      <c r="M20" s="9">
+        <v>1</v>
+      </c>
       <c r="N20" s="9"/>
       <c r="O20" s="9"/>
       <c r="P20" s="9" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="Q20" s="9" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="R20" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="S20" s="9">
-        <v>919</v>
+        <v>1149</v>
       </c>
       <c r="T20" s="9">
-        <v>534</v>
+        <v>584</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A21" s="9">
-        <v>13010017</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>47</v>
+      <c r="A21" s="17">
+        <v>13010105</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>45</v>
       </c>
       <c r="C21" s="9">
         <v>2</v>
       </c>
       <c r="D21" s="9">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E21" s="9">
-        <v>13010016</v>
+        <v>13010101</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="H21" s="9"/>
-      <c r="I21" s="9">
-        <v>1</v>
-      </c>
+      <c r="I21" s="9"/>
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
       <c r="L21" s="9"/>
-      <c r="M21" s="9">
-        <v>1</v>
-      </c>
+      <c r="M21" s="9"/>
       <c r="N21" s="9"/>
       <c r="O21" s="9"/>
       <c r="P21" s="9" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="Q21" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="R21" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="S21" s="9">
-        <v>1149</v>
+        <v>840</v>
       </c>
       <c r="T21" s="9">
-        <v>584</v>
+        <v>444</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A22" s="9">
-        <v>13010018</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>48</v>
+      <c r="A22" s="17">
+        <v>13010106</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>160</v>
       </c>
       <c r="C22" s="9">
         <v>2</v>
       </c>
       <c r="D22" s="9">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E22" s="9">
         <v>13010016</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>119</v>
+        <v>147</v>
       </c>
       <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
+      <c r="I22" s="9">
+        <v>1</v>
+      </c>
       <c r="J22" s="9"/>
       <c r="K22" s="9"/>
       <c r="L22" s="9"/>
       <c r="M22" s="9"/>
-      <c r="N22" s="9"/>
+      <c r="N22" s="9">
+        <v>1</v>
+      </c>
       <c r="O22" s="9"/>
       <c r="P22" s="9" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="Q22" s="9" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="R22" s="9" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="S22" s="9">
-        <v>840</v>
+        <v>1067</v>
       </c>
       <c r="T22" s="9">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.15">
@@ -3491,7 +3555,7 @@
         <v>13020001</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C23" s="14">
         <v>3</v>
@@ -3503,11 +3567,11 @@
         <v>13000002</v>
       </c>
       <c r="F23" s="13" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="G23" s="9"/>
       <c r="H23" s="9" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
@@ -3517,10 +3581,10 @@
       <c r="N23" s="9"/>
       <c r="O23" s="9"/>
       <c r="P23" s="9" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="Q23" s="9" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="R23" s="9"/>
       <c r="S23" s="9"/>
@@ -3531,7 +3595,7 @@
         <v>13020002</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C24" s="14">
         <v>3</v>
@@ -3553,10 +3617,10 @@
       <c r="N24" s="9"/>
       <c r="O24" s="9"/>
       <c r="P24" s="9" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="Q24" s="9" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="R24" s="9"/>
       <c r="S24" s="9"/>
@@ -3567,7 +3631,7 @@
         <v>13020011</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C25" s="14">
         <v>3</v>
@@ -3581,7 +3645,7 @@
       <c r="F25" s="12"/>
       <c r="G25" s="9"/>
       <c r="H25" s="9" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="I25" s="9"/>
       <c r="J25" s="9"/>
@@ -3591,10 +3655,10 @@
       <c r="N25" s="9"/>
       <c r="O25" s="9"/>
       <c r="P25" s="9" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="Q25" s="9" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="R25" s="9"/>
       <c r="S25" s="9"/>
@@ -3605,7 +3669,7 @@
         <v>13020012</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C26" s="14">
         <v>3</v>
@@ -3627,10 +3691,10 @@
       <c r="N26" s="9"/>
       <c r="O26" s="9"/>
       <c r="P26" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="Q26" s="9" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="R26" s="9"/>
       <c r="S26" s="9"/>
@@ -3641,7 +3705,7 @@
         <v>13020013</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C27" s="14">
         <v>3</v>
@@ -3663,10 +3727,10 @@
       <c r="N27" s="9"/>
       <c r="O27" s="9"/>
       <c r="P27" s="9" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="Q27" s="9" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="R27" s="9"/>
       <c r="S27" s="9"/>
@@ -3675,12 +3739,12 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="I4:N27">
-    <cfRule type="cellIs" dxfId="24" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4">
-    <cfRule type="cellIs" dxfId="23" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
add a new quest event
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Scene.xlsx
+++ b/ConfigData/Xlsx/Scene.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="162">
   <si>
     <t>村外小屋</t>
   </si>
@@ -30,587 +30,592 @@
     <t>登拉克峡谷</t>
   </si>
   <si>
+    <t>塔塔木村</t>
+  </si>
+  <si>
+    <t>珀斯古城</t>
+  </si>
+  <si>
+    <t>GameIconsCatch</t>
+  </si>
+  <si>
+    <t>村外田园</t>
+  </si>
+  <si>
+    <t>黄金海岸</t>
+  </si>
+  <si>
+    <t>孤岛遗迹</t>
+  </si>
+  <si>
+    <t>GameBattleRobot</t>
+  </si>
+  <si>
+    <t>小树林</t>
+  </si>
+  <si>
+    <t>玲珑峰</t>
+  </si>
+  <si>
+    <t>遗迹河滩</t>
+  </si>
+  <si>
+    <t>雾谷</t>
+  </si>
+  <si>
+    <t>木阴之村</t>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>序列</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>名字</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>等级</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>功能列表</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>场景背景</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>Func</t>
+  </si>
+  <si>
+    <t>Url</t>
+  </si>
+  <si>
+    <t>TilePath</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>配置</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>home</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Quest</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>任务列表</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>darkforest</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>tatamuviliage</t>
+  </si>
+  <si>
+    <t>smallforest</t>
+  </si>
+  <si>
+    <t>perse</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>demlock</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>hightower</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>smallhill</t>
+  </si>
+  <si>
+    <t>goldseashore</t>
+  </si>
+  <si>
+    <t>islandold</t>
+  </si>
+  <si>
+    <t>riverold</t>
+  </si>
+  <si>
+    <t>落潮小径</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>月光林地</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>gerdin</t>
+  </si>
+  <si>
+    <t>fogvalley</t>
+  </si>
+  <si>
+    <t>矿脉山脚</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>riverside</t>
+  </si>
+  <si>
+    <t>woodviliage</t>
+  </si>
+  <si>
+    <t>moonforest</t>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>激活传送门</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QPortal</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QCardChange</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>卡牌交换</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>素材商人</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QPiece</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QMerchant</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QDoctor</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QAngel</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>商人</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>医生</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>天使</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>IconX</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>IconY</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Icon</t>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwxw</t>
+  </si>
+  <si>
+    <t>haml</t>
+  </si>
+  <si>
+    <t>kk</t>
+  </si>
+  <si>
+    <t>dlkxg</t>
+  </si>
+  <si>
+    <t>bstgt</t>
+  </si>
+  <si>
+    <t>ttmc</t>
+  </si>
+  <si>
+    <t>psgc</t>
+  </si>
+  <si>
+    <t>gdh</t>
+  </si>
+  <si>
+    <t>cwyy</t>
+  </si>
+  <si>
+    <t>hjha</t>
+  </si>
+  <si>
+    <t>gdyj</t>
+  </si>
+  <si>
+    <t>xsl</t>
+  </si>
+  <si>
+    <t>llf</t>
+  </si>
+  <si>
+    <t>yjht</t>
+  </si>
+  <si>
+    <t>wg</t>
+  </si>
+  <si>
+    <t>myzc</t>
+  </si>
+  <si>
+    <t>lcxj</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ygld</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>小图标x</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>小图标y</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>图标路径</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>GameUpToNumber;GameThreeBody</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>poppyfield;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trees;3|mushroom;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>sewer;3|river;2|fortune;1|oldtree;1|poppyfield;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>fortune;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>wolfnest;2|gamble;1|fishpool;2|sewer;3|river;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>小概率任务</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QuestRandom</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|treasure;25</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>类型</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Type</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>portal;1|fishpool;1|grave;2|hiddeway;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>river;2|fishpool;1|swamp;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>mushroom;1|hiddeway;1|swamp;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>orehole;1|stone;2|sandflow;2</t>
+  </si>
+  <si>
+    <t>coldwind;3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ruintown1;1|manflower;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trees;3|grave;1|portal;1|oldtree;1|manflower;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>portal;3|sandflow;2|manflower;3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>river;2|stone;3|ruintown1;1|hiddeway;1|manflower;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|witchhome;30</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|treasure;25|witchhome;20</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|forestfire;20|witchhome;40</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>forestfire;10</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>forestfire;35|witchhome;10</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>密林迷宫</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>迷宫深处</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>home</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>orevalley</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>hightower</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>tatamuviliage</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>perse</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>gerdin</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>farm</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>farm</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>goldseashore</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>islandold</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>smallforest</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>smallhill</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>riverold</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>fogvalley</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>woodviliage</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>riverside</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>moonforest</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>forestmaze</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>forestinner</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>副本任务列表</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QuestDungeon</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>forestentry;2|forestentry2;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>复活地图</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ReviveScene</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trees;4|manflower;2|portal;1|sandland;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|goblinhome;40</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|goblinhome;30</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>goblinhome;50</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|icedream;25</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>古城大厅</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>persepalace1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>persepalace2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>persepalace3</t>
+  </si>
+  <si>
+    <t>古城外围</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>古城大殿</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>persepalace2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>玲珑峰隧道</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>smallhillchanel</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>格丁湖</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>布萨特高塔</t>
-  </si>
-  <si>
-    <t>塔塔木村</t>
-  </si>
-  <si>
-    <t>珀斯古城</t>
-  </si>
-  <si>
-    <t>GameIconsCatch</t>
-  </si>
-  <si>
-    <t>村外田园</t>
-  </si>
-  <si>
-    <t>黄金海岸</t>
-  </si>
-  <si>
-    <t>孤岛遗迹</t>
-  </si>
-  <si>
-    <t>GameBattleRobot</t>
-  </si>
-  <si>
-    <t>小树林</t>
-  </si>
-  <si>
-    <t>玲珑峰</t>
-  </si>
-  <si>
-    <t>遗迹河滩</t>
-  </si>
-  <si>
-    <t>雾谷</t>
-  </si>
-  <si>
-    <t>木阴之村</t>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>序列</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>名字</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>等级</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>功能列表</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>场景背景</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Id</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Level</t>
-  </si>
-  <si>
-    <t>Func</t>
-  </si>
-  <si>
-    <t>Url</t>
-  </si>
-  <si>
-    <t>TilePath</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>配置</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>home</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Quest</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>任务列表</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>darkforest</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>tatamuviliage</t>
-  </si>
-  <si>
-    <t>smallforest</t>
-  </si>
-  <si>
-    <t>perse</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>demlock</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>hightower</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>smallhill</t>
-  </si>
-  <si>
-    <t>goldseashore</t>
-  </si>
-  <si>
-    <t>islandold</t>
-  </si>
-  <si>
-    <t>riverold</t>
-  </si>
-  <si>
-    <t>落潮小径</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>月光林地</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>gerdin</t>
-  </si>
-  <si>
-    <t>fogvalley</t>
-  </si>
-  <si>
-    <t>矿脉山脚</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>riverside</t>
-  </si>
-  <si>
-    <t>woodviliage</t>
-  </si>
-  <si>
-    <t>moonforest</t>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>激活传送门</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>QPortal</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>QCardChange</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>卡牌交换</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>素材商人</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>QPiece</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>QMerchant</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>QDoctor</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>QAngel</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>商人</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>医生</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>天使</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>IconX</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>IconY</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Icon</t>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>cwxw</t>
-  </si>
-  <si>
-    <t>haml</t>
-  </si>
-  <si>
-    <t>kk</t>
-  </si>
-  <si>
-    <t>dlkxg</t>
-  </si>
-  <si>
-    <t>bstgt</t>
-  </si>
-  <si>
-    <t>ttmc</t>
-  </si>
-  <si>
-    <t>psgc</t>
-  </si>
-  <si>
-    <t>gdh</t>
-  </si>
-  <si>
-    <t>cwyy</t>
-  </si>
-  <si>
-    <t>hjha</t>
-  </si>
-  <si>
-    <t>gdyj</t>
-  </si>
-  <si>
-    <t>xsl</t>
-  </si>
-  <si>
-    <t>llf</t>
-  </si>
-  <si>
-    <t>yjht</t>
-  </si>
-  <si>
-    <t>wg</t>
-  </si>
-  <si>
-    <t>myzc</t>
-  </si>
-  <si>
-    <t>lcxj</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ygld</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>小图标x</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>小图标y</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>图标路径</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>GameUpToNumber;GameThreeBody</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>poppyfield;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>trees;3|mushroom;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>sewer;3|river;2|fortune;1|oldtree;1|poppyfield;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>fortune;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>wolfnest;2|gamble;1|fishpool;2|sewer;3|river;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>小概率任务</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>QuestRandom</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|treasure;25</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>类型</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Type</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>portal;1|fishpool;1|grave;2|hiddeway;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>river;2|fishpool;1|swamp;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>mushroom;1|hiddeway;1|swamp;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>orehole;1|stone;2|sandflow;2</t>
-  </si>
-  <si>
-    <t>coldwind;3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ruintown1;1|manflower;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>trees;3|grave;1|portal;1|oldtree;1|manflower;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>portal;3|sandflow;2|manflower;3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>river;2|stone;3|ruintown1;1|hiddeway;1|manflower;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|witchhome;30</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|treasure;25|witchhome;20</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|forestfire;20|witchhome;40</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>forestfire;10</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>forestfire;35|witchhome;10</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>密林迷宫</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>迷宫深处</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>home</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>orevalley</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>hightower</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>tatamuviliage</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>perse</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>gerdin</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>farm</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>farm</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>goldseashore</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>islandold</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>smallforest</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>smallhill</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>riverold</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>fogvalley</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>woodviliage</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>riverside</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>moonforest</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>forestmaze</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>forestinner</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>副本任务列表</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>QuestDungeon</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>forestentry;2|forestentry2;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>复活地图</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ReviveScene</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>trees;4|manflower;2|portal;1|sandland;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|goblinhome;40</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|goblinhome;30</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>goblinhome;50</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|icedream;25</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>古城大厅</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>persepalace1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>persepalace2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>persepalace3</t>
-  </si>
-  <si>
-    <t>古城外围</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>古城大殿</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>persepalace2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>玲珑峰隧道</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>smallhillchanel</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>格丁湖</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trees;4|manflower;2|portal;1|sandland;2|cliff;2</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -2426,7 +2431,7 @@
   <dimension ref="A1:T27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2449,188 +2454,188 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="O1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="O1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="P1" s="6" t="s">
-        <v>22</v>
-      </c>
       <c r="Q1" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="S1" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="T1" s="8" t="s">
         <v>87</v>
-      </c>
-      <c r="T1" s="8" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="P2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A3" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="C3" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="D3" s="10" t="s">
+      <c r="E3" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="M3" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="N3" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="O3" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="K3" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="L3" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="M3" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="N3" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="O3" s="10" t="s">
+      <c r="P3" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="P3" s="10" t="s">
+      <c r="Q3" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="Q3" s="10" t="s">
-        <v>28</v>
-      </c>
       <c r="R3" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="S3" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="T3" s="10" t="s">
         <v>65</v>
-      </c>
-      <c r="T3" s="10" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.15">
@@ -2650,7 +2655,7 @@
         <v>13010001</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
@@ -2663,16 +2668,16 @@
       <c r="M4" s="9"/>
       <c r="N4" s="9"/>
       <c r="O4" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="P4" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Q4" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R4" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="S4" s="9">
         <v>1348</v>
@@ -2698,10 +2703,10 @@
         <v>13010001</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H5" s="9"/>
       <c r="I5" s="9">
@@ -2718,13 +2723,13 @@
       <c r="N5" s="9"/>
       <c r="O5" s="9"/>
       <c r="P5" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Q5" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R5" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="S5" s="9">
         <v>1279</v>
@@ -2750,10 +2755,10 @@
         <v>13010006</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H6" s="9"/>
       <c r="I6" s="9">
@@ -2768,13 +2773,13 @@
       <c r="N6" s="9"/>
       <c r="O6" s="9"/>
       <c r="P6" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q6" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R6" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="S6" s="9">
         <v>1148</v>
@@ -2788,7 +2793,7 @@
         <v>13010005</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>3</v>
+        <v>160</v>
       </c>
       <c r="C7" s="9">
         <v>2</v>
@@ -2801,7 +2806,7 @@
       </c>
       <c r="F7" s="9"/>
       <c r="G7" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H7" s="9"/>
       <c r="I7" s="9">
@@ -2816,13 +2821,13 @@
       <c r="N7" s="9"/>
       <c r="O7" s="9"/>
       <c r="P7" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="Q7" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="R7" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="S7" s="9">
         <v>1386</v>
@@ -2836,7 +2841,7 @@
         <v>13010006</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8" s="9">
         <v>1</v>
@@ -2858,13 +2863,13 @@
       <c r="N8" s="9"/>
       <c r="O8" s="9"/>
       <c r="P8" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="Q8" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R8" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="S8" s="9">
         <v>1232</v>
@@ -2878,7 +2883,7 @@
         <v>13010007</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C9" s="9">
         <v>2</v>
@@ -2890,10 +2895,10 @@
         <v>13010006</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H9" s="9"/>
       <c r="I9" s="9">
@@ -2909,16 +2914,16 @@
       </c>
       <c r="N9" s="9"/>
       <c r="O9" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P9" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Q9" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R9" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="S9" s="9">
         <v>1431</v>
@@ -2932,7 +2937,7 @@
         <v>13010009</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" s="9">
         <v>2</v>
@@ -2944,10 +2949,10 @@
         <v>13010006</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H10" s="9"/>
       <c r="I10" s="9">
@@ -2964,13 +2969,13 @@
       <c r="N10" s="9"/>
       <c r="O10" s="9"/>
       <c r="P10" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="Q10" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="R10" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="S10" s="9">
         <v>1332</v>
@@ -2984,7 +2989,7 @@
         <v>13010010</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11" s="9">
         <v>2</v>
@@ -2997,7 +3002,7 @@
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H11" s="9"/>
       <c r="I11" s="9">
@@ -3012,13 +3017,13 @@
       </c>
       <c r="O11" s="9"/>
       <c r="P11" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="Q11" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="R11" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="S11" s="9">
         <v>1441</v>
@@ -3032,7 +3037,7 @@
         <v>13010011</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12" s="9">
         <v>2</v>
@@ -3044,10 +3049,10 @@
         <v>13010006</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H12" s="9"/>
       <c r="I12" s="9">
@@ -3061,16 +3066,16 @@
       <c r="M12" s="9"/>
       <c r="N12" s="9"/>
       <c r="O12" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="P12" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="Q12" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R12" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="S12" s="9">
         <v>1574</v>
@@ -3084,7 +3089,7 @@
         <v>13010012</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13" s="9">
         <v>2</v>
@@ -3096,10 +3101,10 @@
         <v>13010006</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H13" s="9"/>
       <c r="I13" s="9">
@@ -3112,13 +3117,13 @@
       <c r="N13" s="9"/>
       <c r="O13" s="9"/>
       <c r="P13" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="Q13" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="R13" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="S13" s="9">
         <v>1251</v>
@@ -3132,7 +3137,7 @@
         <v>13010013</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C14" s="9">
         <v>2</v>
@@ -3144,10 +3149,10 @@
         <v>13010006</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H14" s="9"/>
       <c r="I14" s="9">
@@ -3160,13 +3165,13 @@
       <c r="N14" s="9"/>
       <c r="O14" s="9"/>
       <c r="P14" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Q14" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="R14" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="S14" s="9">
         <v>1250</v>
@@ -3180,7 +3185,7 @@
         <v>13010014</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C15" s="9">
         <v>2</v>
@@ -3192,10 +3197,10 @@
         <v>13010006</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H15" s="9"/>
       <c r="I15" s="9">
@@ -3212,13 +3217,13 @@
       </c>
       <c r="O15" s="9"/>
       <c r="P15" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q15" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R15" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="S15" s="9">
         <v>1550</v>
@@ -3232,7 +3237,7 @@
         <v>13010015</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C16" s="15">
         <v>2</v>
@@ -3256,10 +3261,10 @@
       <c r="N16" s="15"/>
       <c r="O16" s="15"/>
       <c r="P16" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="Q16" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="R16" s="15"/>
       <c r="S16" s="15"/>
@@ -3270,7 +3275,7 @@
         <v>13010101</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17" s="9">
         <v>1</v>
@@ -3292,13 +3297,13 @@
       <c r="N17" s="9"/>
       <c r="O17" s="9"/>
       <c r="P17" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="Q17" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="R17" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="S17" s="9">
         <v>919</v>
@@ -3312,7 +3317,7 @@
         <v>13010102</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C18" s="9">
         <v>2</v>
@@ -3324,10 +3329,10 @@
         <v>13010101</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H18" s="9"/>
       <c r="I18" s="9">
@@ -3342,13 +3347,13 @@
       <c r="N18" s="9"/>
       <c r="O18" s="9"/>
       <c r="P18" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="Q18" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="R18" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="S18" s="9">
         <v>1040</v>
@@ -3362,7 +3367,7 @@
         <v>13010103</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C19" s="9">
         <v>2</v>
@@ -3374,10 +3379,10 @@
         <v>13010101</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H19" s="9"/>
       <c r="I19" s="9">
@@ -3390,13 +3395,13 @@
       <c r="N19" s="9"/>
       <c r="O19" s="9"/>
       <c r="P19" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Q19" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="R19" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="S19" s="9">
         <v>1213</v>
@@ -3410,7 +3415,7 @@
         <v>13010104</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C20" s="9">
         <v>2</v>
@@ -3422,10 +3427,10 @@
         <v>13010101</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H20" s="9"/>
       <c r="I20" s="9">
@@ -3440,13 +3445,13 @@
       <c r="N20" s="9"/>
       <c r="O20" s="9"/>
       <c r="P20" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="Q20" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="R20" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S20" s="9">
         <v>1149</v>
@@ -3460,7 +3465,7 @@
         <v>13010105</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C21" s="9">
         <v>2</v>
@@ -3472,10 +3477,10 @@
         <v>13010101</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H21" s="9"/>
       <c r="I21" s="9"/>
@@ -3486,13 +3491,13 @@
       <c r="N21" s="9"/>
       <c r="O21" s="9"/>
       <c r="P21" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Q21" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="R21" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="S21" s="9">
         <v>840</v>
@@ -3506,7 +3511,7 @@
         <v>13010106</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C22" s="9">
         <v>2</v>
@@ -3518,10 +3523,10 @@
         <v>13010016</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H22" s="9"/>
       <c r="I22" s="9">
@@ -3536,13 +3541,13 @@
       </c>
       <c r="O22" s="9"/>
       <c r="P22" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="Q22" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="R22" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="S22" s="9">
         <v>1067</v>
@@ -3556,7 +3561,7 @@
         <v>13020001</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C23" s="14">
         <v>3</v>
@@ -3568,11 +3573,11 @@
         <v>13010002</v>
       </c>
       <c r="F23" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G23" s="9"/>
       <c r="H23" s="9" t="s">
-        <v>146</v>
+        <v>161</v>
       </c>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
@@ -3582,10 +3587,10 @@
       <c r="N23" s="9"/>
       <c r="O23" s="9"/>
       <c r="P23" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q23" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="R23" s="9"/>
       <c r="S23" s="9"/>
@@ -3596,7 +3601,7 @@
         <v>13020002</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C24" s="14">
         <v>3</v>
@@ -3618,10 +3623,10 @@
       <c r="N24" s="9"/>
       <c r="O24" s="9"/>
       <c r="P24" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q24" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="R24" s="9"/>
       <c r="S24" s="9"/>
@@ -3632,7 +3637,7 @@
         <v>13020011</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C25" s="14">
         <v>3</v>
@@ -3646,7 +3651,7 @@
       <c r="F25" s="12"/>
       <c r="G25" s="9"/>
       <c r="H25" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I25" s="9"/>
       <c r="J25" s="9"/>
@@ -3656,10 +3661,10 @@
       <c r="N25" s="9"/>
       <c r="O25" s="9"/>
       <c r="P25" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Q25" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="R25" s="9"/>
       <c r="S25" s="9"/>
@@ -3670,7 +3675,7 @@
         <v>13020012</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C26" s="14">
         <v>3</v>
@@ -3692,10 +3697,10 @@
       <c r="N26" s="9"/>
       <c r="O26" s="9"/>
       <c r="P26" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="Q26" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="R26" s="9"/>
       <c r="S26" s="9"/>
@@ -3706,7 +3711,7 @@
         <v>13020013</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C27" s="14">
         <v>3</v>
@@ -3728,10 +3733,10 @@
       <c r="N27" s="9"/>
       <c r="O27" s="9"/>
       <c r="P27" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Q27" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="R27" s="9"/>
       <c r="S27" s="9"/>

</xml_diff>

<commit_message>
add some new evemt
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Scene.xlsx
+++ b/ConfigData/Xlsx/Scene.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17766"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="175">
   <si>
     <t>村外小屋</t>
   </si>
@@ -637,25 +637,42 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>trees;4</t>
-  </si>
-  <si>
     <t>forestmaze</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>diarybook;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>stonewords;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>underwater;50</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>diarybook;1|barn;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>mushroom;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>hiddeway;35</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>sandflow;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trees;4|brokehouse;3</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1451,6 +1468,20 @@
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="25">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2047,20 +2078,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2075,39 +2092,39 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:T30" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21" tableBorderDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:T30" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23" tableBorderDxfId="22">
   <autoFilter ref="A3:T30"/>
   <sortState ref="A4:T27">
     <sortCondition ref="A3:A27"/>
   </sortState>
   <tableColumns count="20">
-    <tableColumn id="1" name="Id" dataDxfId="19"/>
-    <tableColumn id="2" name="Name" dataDxfId="18"/>
-    <tableColumn id="18" name="Type" dataDxfId="17"/>
-    <tableColumn id="3" name="Level" dataDxfId="16"/>
-    <tableColumn id="20" name="ReviveScene" dataDxfId="15"/>
-    <tableColumn id="4" name="Quest" dataDxfId="14"/>
-    <tableColumn id="17" name="QuestRandom" dataDxfId="13"/>
-    <tableColumn id="19" name="QuestDungeon" dataDxfId="12"/>
-    <tableColumn id="5" name="QPortal" dataDxfId="11"/>
-    <tableColumn id="6" name="QCardChange" dataDxfId="10"/>
-    <tableColumn id="7" name="QPiece" dataDxfId="9"/>
-    <tableColumn id="8" name="QMerchant" dataDxfId="8"/>
-    <tableColumn id="9" name="QDoctor" dataDxfId="7"/>
-    <tableColumn id="10" name="QAngel" dataDxfId="6"/>
-    <tableColumn id="11" name="Func" dataDxfId="5"/>
-    <tableColumn id="12" name="Url" dataDxfId="4"/>
-    <tableColumn id="13" name="TilePath" dataDxfId="3"/>
-    <tableColumn id="14" name="Icon" dataDxfId="2"/>
-    <tableColumn id="15" name="IconX" dataDxfId="1"/>
-    <tableColumn id="16" name="IconY" dataDxfId="0"/>
+    <tableColumn id="1" name="Id" dataDxfId="21"/>
+    <tableColumn id="2" name="Name" dataDxfId="20"/>
+    <tableColumn id="18" name="Type" dataDxfId="19"/>
+    <tableColumn id="3" name="Level" dataDxfId="18"/>
+    <tableColumn id="20" name="ReviveScene" dataDxfId="17"/>
+    <tableColumn id="4" name="Quest" dataDxfId="16"/>
+    <tableColumn id="17" name="QuestRandom" dataDxfId="15"/>
+    <tableColumn id="19" name="QuestDungeon" dataDxfId="14"/>
+    <tableColumn id="5" name="QPortal" dataDxfId="13"/>
+    <tableColumn id="6" name="QCardChange" dataDxfId="12"/>
+    <tableColumn id="7" name="QPiece" dataDxfId="11"/>
+    <tableColumn id="8" name="QMerchant" dataDxfId="10"/>
+    <tableColumn id="9" name="QDoctor" dataDxfId="9"/>
+    <tableColumn id="10" name="QAngel" dataDxfId="8"/>
+    <tableColumn id="11" name="Func" dataDxfId="7"/>
+    <tableColumn id="12" name="Url" dataDxfId="6"/>
+    <tableColumn id="13" name="TilePath" dataDxfId="5"/>
+    <tableColumn id="14" name="Icon" dataDxfId="4"/>
+    <tableColumn id="15" name="IconX" dataDxfId="3"/>
+    <tableColumn id="16" name="IconY" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2182,6 +2199,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2217,6 +2251,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2395,8 +2446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3213,9 +3264,13 @@
       <c r="E16" s="9">
         <v>13010006</v>
       </c>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
+      <c r="F16" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="H16" s="12"/>
       <c r="I16" s="15">
         <v>1</v>
       </c>
@@ -3553,7 +3608,7 @@
         <v>137</v>
       </c>
       <c r="Q23" s="9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="R23" s="9"/>
       <c r="S23" s="9"/>
@@ -3721,10 +3776,12 @@
       <c r="E28" s="9">
         <v>13010004</v>
       </c>
-      <c r="F28" s="12"/>
+      <c r="F28" s="12" t="s">
+        <v>173</v>
+      </c>
       <c r="G28" s="9"/>
       <c r="H28" s="9" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="I28" s="9"/>
       <c r="J28" s="9"/>
@@ -3760,7 +3817,7 @@
         <v>13010004</v>
       </c>
       <c r="F29" s="12" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
@@ -3798,9 +3855,11 @@
         <v>13010004</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="G30" s="9"/>
+        <v>168</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>172</v>
+      </c>
       <c r="H30" s="9"/>
       <c r="I30" s="9"/>
       <c r="J30" s="9"/>
@@ -3822,12 +3881,12 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="I4:N30">
-    <cfRule type="cellIs" dxfId="24" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4">
-    <cfRule type="cellIs" dxfId="23" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
add the detect system
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Scene.xlsx
+++ b/ConfigData/Xlsx/Scene.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="Scene" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="178">
   <si>
     <t>村外小屋</t>
   </si>
@@ -369,10 +369,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>met;30</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>met;30|treasure;25</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -436,10 +432,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>forestfire;10</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>forestfire;35|witchhome;10</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -564,10 +556,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>met;30|icedream;25</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>古城大厅</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -649,10 +637,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>mushroom;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>hiddeway;35</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -666,6 +650,34 @@
   </si>
   <si>
     <t>underwater;50|earthcrack;60</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>mushroom;1|torch;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>crystalball;55</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>forestfire;10|crystalball;35</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|icedream;25|lighthouse;30</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|lighthouse;60</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|lighthouse;60</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|goblinhome;40|lighthouse;70</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -2447,7 +2459,7 @@
   <dimension ref="A1:T30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2476,13 +2488,13 @@
         <v>18</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>32</v>
@@ -2491,7 +2503,7 @@
         <v>96</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I1" s="7" t="s">
         <v>52</v>
@@ -2538,13 +2550,13 @@
         <v>16</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>90</v>
@@ -2600,13 +2612,13 @@
         <v>23</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>24</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>31</v>
@@ -2615,7 +2627,7 @@
         <v>98</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="I3" s="11" t="s">
         <v>53</v>
@@ -2687,7 +2699,7 @@
         <v>89</v>
       </c>
       <c r="P4" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="Q4" s="9" t="s">
         <v>30</v>
@@ -2722,7 +2734,7 @@
         <v>95</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>116</v>
+        <v>173</v>
       </c>
       <c r="H5" s="9"/>
       <c r="I5" s="9">
@@ -2771,10 +2783,10 @@
         <v>13010006</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H6" s="9"/>
       <c r="I6" s="9">
@@ -2809,7 +2821,7 @@
         <v>13010005</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C7" s="9">
         <v>2</v>
@@ -2822,7 +2834,7 @@
       </c>
       <c r="F7" s="9"/>
       <c r="G7" s="9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H7" s="9"/>
       <c r="I7" s="9">
@@ -2837,7 +2849,7 @@
       <c r="N7" s="9"/>
       <c r="O7" s="9"/>
       <c r="P7" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="Q7" s="9" t="s">
         <v>38</v>
@@ -2879,7 +2891,7 @@
       <c r="N8" s="9"/>
       <c r="O8" s="9"/>
       <c r="P8" s="9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="Q8" s="9" t="s">
         <v>34</v>
@@ -2911,10 +2923,10 @@
         <v>13010006</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H9" s="9"/>
       <c r="I9" s="9">
@@ -2933,7 +2945,7 @@
         <v>5</v>
       </c>
       <c r="P9" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="Q9" s="9" t="s">
         <v>36</v>
@@ -2965,10 +2977,10 @@
         <v>13010006</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H10" s="9"/>
       <c r="I10" s="9">
@@ -2985,10 +2997,10 @@
       <c r="N10" s="9"/>
       <c r="O10" s="9"/>
       <c r="P10" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="Q10" s="9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="R10" s="9" t="s">
         <v>76</v>
@@ -3018,7 +3030,7 @@
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="9" t="s">
-        <v>99</v>
+        <v>176</v>
       </c>
       <c r="H11" s="9"/>
       <c r="I11" s="9">
@@ -3033,7 +3045,7 @@
       </c>
       <c r="O11" s="9"/>
       <c r="P11" s="9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="Q11" s="9" t="s">
         <v>40</v>
@@ -3068,7 +3080,7 @@
         <v>94</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>145</v>
+        <v>177</v>
       </c>
       <c r="H12" s="9"/>
       <c r="I12" s="9">
@@ -3085,7 +3097,7 @@
         <v>9</v>
       </c>
       <c r="P12" s="9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="Q12" s="9" t="s">
         <v>41</v>
@@ -3117,10 +3129,10 @@
         <v>13010006</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H13" s="9"/>
       <c r="I13" s="9">
@@ -3133,7 +3145,7 @@
       <c r="N13" s="9"/>
       <c r="O13" s="9"/>
       <c r="P13" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="Q13" s="9" t="s">
         <v>35</v>
@@ -3165,10 +3177,10 @@
         <v>13010006</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>148</v>
+        <v>174</v>
       </c>
       <c r="H14" s="9"/>
       <c r="I14" s="9">
@@ -3181,7 +3193,7 @@
       <c r="N14" s="9"/>
       <c r="O14" s="9"/>
       <c r="P14" s="9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="Q14" s="9" t="s">
         <v>39</v>
@@ -3213,10 +3225,10 @@
         <v>13010006</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H15" s="9"/>
       <c r="I15" s="9">
@@ -3233,7 +3245,7 @@
       </c>
       <c r="O15" s="9"/>
       <c r="P15" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="Q15" s="9" t="s">
         <v>42</v>
@@ -3253,7 +3265,7 @@
         <v>13010015</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C16" s="15">
         <v>2</v>
@@ -3265,10 +3277,10 @@
         <v>13010006</v>
       </c>
       <c r="F16" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="G16" s="12" t="s">
         <v>170</v>
-      </c>
-      <c r="G16" s="12" t="s">
-        <v>174</v>
       </c>
       <c r="H16" s="12"/>
       <c r="I16" s="15">
@@ -3281,10 +3293,10 @@
       <c r="N16" s="15"/>
       <c r="O16" s="15"/>
       <c r="P16" s="12" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="Q16" s="12" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="R16" s="15"/>
       <c r="S16" s="15"/>
@@ -3317,7 +3329,7 @@
       <c r="N17" s="9"/>
       <c r="O17" s="9"/>
       <c r="P17" s="9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="Q17" s="9" t="s">
         <v>49</v>
@@ -3349,10 +3361,10 @@
         <v>13010101</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H18" s="9"/>
       <c r="I18" s="9">
@@ -3367,7 +3379,7 @@
       <c r="N18" s="9"/>
       <c r="O18" s="9"/>
       <c r="P18" s="9" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="Q18" s="9" t="s">
         <v>46</v>
@@ -3399,10 +3411,10 @@
         <v>13010101</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H19" s="9"/>
       <c r="I19" s="9">
@@ -3415,10 +3427,10 @@
       <c r="N19" s="9"/>
       <c r="O19" s="9"/>
       <c r="P19" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="Q19" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="R19" s="9" t="s">
         <v>70</v>
@@ -3447,10 +3459,10 @@
         <v>13010101</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>99</v>
+        <v>175</v>
       </c>
       <c r="H20" s="9"/>
       <c r="I20" s="9">
@@ -3465,7 +3477,7 @@
       <c r="N20" s="9"/>
       <c r="O20" s="9"/>
       <c r="P20" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="Q20" s="9" t="s">
         <v>48</v>
@@ -3500,7 +3512,7 @@
         <v>92</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H21" s="9"/>
       <c r="I21" s="9"/>
@@ -3511,7 +3523,7 @@
       <c r="N21" s="9"/>
       <c r="O21" s="9"/>
       <c r="P21" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="Q21" s="9" t="s">
         <v>50</v>
@@ -3531,7 +3543,7 @@
         <v>13010106</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C22" s="9">
         <v>2</v>
@@ -3546,7 +3558,7 @@
         <v>91</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H22" s="9"/>
       <c r="I22" s="9">
@@ -3561,7 +3573,7 @@
       </c>
       <c r="O22" s="9"/>
       <c r="P22" s="9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="Q22" s="9" t="s">
         <v>45</v>
@@ -3581,7 +3593,7 @@
         <v>13020001</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C23" s="14">
         <v>3</v>
@@ -3595,7 +3607,7 @@
       <c r="F23" s="13"/>
       <c r="G23" s="9"/>
       <c r="H23" s="9" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
@@ -3605,10 +3617,10 @@
       <c r="N23" s="9"/>
       <c r="O23" s="9"/>
       <c r="P23" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="Q23" s="9" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="R23" s="9"/>
       <c r="S23" s="9"/>
@@ -3619,7 +3631,7 @@
         <v>13020002</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C24" s="14">
         <v>3</v>
@@ -3641,10 +3653,10 @@
       <c r="N24" s="9"/>
       <c r="O24" s="9"/>
       <c r="P24" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="Q24" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="R24" s="9"/>
       <c r="S24" s="9"/>
@@ -3655,7 +3667,7 @@
         <v>13020011</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C25" s="14">
         <v>3</v>
@@ -3669,7 +3681,7 @@
       <c r="F25" s="12"/>
       <c r="G25" s="9"/>
       <c r="H25" s="9" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="I25" s="9"/>
       <c r="J25" s="9"/>
@@ -3679,10 +3691,10 @@
       <c r="N25" s="9"/>
       <c r="O25" s="9"/>
       <c r="P25" s="9" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="Q25" s="9" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="R25" s="9"/>
       <c r="S25" s="9"/>
@@ -3693,7 +3705,7 @@
         <v>13020012</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C26" s="14">
         <v>3</v>
@@ -3715,10 +3727,10 @@
       <c r="N26" s="9"/>
       <c r="O26" s="9"/>
       <c r="P26" s="9" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="Q26" s="9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="R26" s="9"/>
       <c r="S26" s="9"/>
@@ -3729,7 +3741,7 @@
         <v>13020013</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C27" s="14">
         <v>3</v>
@@ -3751,10 +3763,10 @@
       <c r="N27" s="9"/>
       <c r="O27" s="9"/>
       <c r="P27" s="9" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="Q27" s="9" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="R27" s="9"/>
       <c r="S27" s="9"/>
@@ -3765,7 +3777,7 @@
         <v>13020021</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C28" s="14">
         <v>3</v>
@@ -3777,11 +3789,13 @@
         <v>13010004</v>
       </c>
       <c r="F28" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="G28" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="G28" s="9"/>
       <c r="H28" s="9" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="I28" s="9"/>
       <c r="J28" s="9"/>
@@ -3791,10 +3805,10 @@
       <c r="N28" s="9"/>
       <c r="O28" s="9"/>
       <c r="P28" s="9" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="Q28" s="9" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="R28" s="9"/>
       <c r="S28" s="9"/>
@@ -3805,7 +3819,7 @@
         <v>13020022</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C29" s="14">
         <v>3</v>
@@ -3817,9 +3831,11 @@
         <v>13010004</v>
       </c>
       <c r="F29" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="G29" s="9"/>
+        <v>166</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>172</v>
+      </c>
       <c r="H29" s="9"/>
       <c r="I29" s="9"/>
       <c r="J29" s="9"/>
@@ -3829,10 +3845,10 @@
       <c r="N29" s="9"/>
       <c r="O29" s="9"/>
       <c r="P29" s="9" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="Q29" s="9" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="R29" s="9"/>
       <c r="S29" s="9"/>
@@ -3843,7 +3859,7 @@
         <v>13020023</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C30" s="14">
         <v>3</v>
@@ -3855,10 +3871,10 @@
         <v>13010004</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="H30" s="9"/>
       <c r="I30" s="9"/>
@@ -3869,10 +3885,10 @@
       <c r="N30" s="9"/>
       <c r="O30" s="9"/>
       <c r="P30" s="9" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="Q30" s="9" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="R30" s="9"/>
       <c r="S30" s="9"/>

</xml_diff>

<commit_message>
add 2 game based event
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Scene.xlsx
+++ b/ConfigData/Xlsx/Scene.xlsx
@@ -383,30 +383,268 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>coldwind;3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ruintown1;1|manflower;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trees;3|grave;1|portal;1|oldtree;1|manflower;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>portal;3|sandflow;2|manflower;3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>密林迷宫</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>迷宫深处</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>home</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>orevalley</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>hightower</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>tatamuviliage</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>perse</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>gerdin</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>farm</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>farm</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>goldseashore</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>islandold</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>smallforest</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>smallhill</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>riverold</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>fogvalley</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>woodviliage</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>riverside</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>moonforest</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>forestmaze</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>forestinner</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>副本任务列表</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QuestDungeon</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>复活地图</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ReviveScene</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trees;4|manflower;2|portal;1|sandland;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|goblinhome;30</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>古城大厅</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>persepalace1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>persepalace2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>persepalace3</t>
+  </si>
+  <si>
+    <t>古城外围</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>古城大殿</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>persepalace2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>玲珑峰隧道</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>smallhillchanel</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>格丁湖</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>布萨特高塔</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>村落入口</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>村中心</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>议事厅</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>viliage1</t>
+  </si>
+  <si>
+    <t>viliage2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>viliage3</t>
+  </si>
+  <si>
+    <t>trees;4|manflower;2|portal;1|sandland;2|cliff;2|colorpool;1|barn;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>forestmaze</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>hiddeway;35</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trees;4|brokehouse;3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>underwater;50|earthcrack;60</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>forestfire;10|crystalball;35</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|lighthouse;60</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|goblinhome;40|lighthouse;70</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>mushroom;1|torch;1|batcrowd;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|goblinhome;30|gamecook;20</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>wolfnest;2|gamegamble;1|fishpool;2|sewer;3|river;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|treasure;25|gamerobot;20</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>river;2|stone;3|ruintown1;1|hiddeway;1|manflower;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|treasure;25|witchhome;20</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>forestfire;35|witchhome;10</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|icedream;25|lighthouse;30</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|witchhome;30</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>orehole;1|stone;2|sandflow;2</t>
-  </si>
-  <si>
-    <t>coldwind;3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ruintown1;1|manflower;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>trees;3|grave;1|portal;1|oldtree;1|manflower;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>portal;3|sandflow;2|manflower;3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|witchhome;30</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|treasure;25|witchhome;20</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -414,200 +652,19 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>forestfire;35|witchhome;10</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>密林迷宫</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>迷宫深处</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>home</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>orevalley</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>hightower</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>tatamuviliage</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>perse</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>gerdin</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>farm</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>farm</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>goldseashore</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>islandold</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>smallforest</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>smallhill</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>riverold</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>fogvalley</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>woodviliage</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>riverside</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>moonforest</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>forestmaze</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>forestinner</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>副本任务列表</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>QuestDungeon</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>复活地图</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ReviveScene</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>trees;4|manflower;2|portal;1|sandland;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>met;30|goblinhome;40</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>met;30|goblinhome;30</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>goblinhome;50</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>古城大厅</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>persepalace1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>persepalace2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>persepalace3</t>
-  </si>
-  <si>
-    <t>古城外围</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>古城大殿</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>persepalace2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>玲珑峰隧道</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>smallhillchanel</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>格丁湖</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>布萨特高塔</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>村落入口</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>村中心</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>议事厅</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>viliage1</t>
-  </si>
-  <si>
-    <t>viliage2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>viliage3</t>
-  </si>
-  <si>
-    <t>trees;4|manflower;2|portal;1|sandland;2|cliff;2|colorpool;1|barn;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>forestmaze</t>
+    <t>sandflow;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>crystalball;55</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>diarybook;1|barn;1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -615,63 +672,7 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>diarybook;1|barn;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>hiddeway;35</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>sandflow;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>trees;4|brokehouse;3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>underwater;50|earthcrack;60</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>crystalball;55</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>forestfire;10|crystalball;35</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|icedream;25|lighthouse;30</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|lighthouse;60</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|lighthouse;60</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|goblinhome;40|lighthouse;70</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>river;2|stone;3|ruintown1;1|hiddeway;1|manflower;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>mushroom;1|torch;1|batcrowd;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|goblinhome;30|gamecook;20</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>wolfnest;2|gamegamble;1|fishpool;2|sewer;3|river;2</t>
+    <t>goblinhome;50|gamemagicbook;15</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1373,7 +1374,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1411,9 +1412,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
@@ -1473,7 +1471,49 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="29">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2070,20 +2110,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2098,32 +2124,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:T30" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21" tableBorderDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:T30" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27" tableBorderDxfId="26">
   <autoFilter ref="A3:T30"/>
   <sortState ref="A4:T27">
     <sortCondition ref="A3:A27"/>
   </sortState>
   <tableColumns count="20">
-    <tableColumn id="1" name="Id" dataDxfId="19"/>
-    <tableColumn id="2" name="Name" dataDxfId="18"/>
-    <tableColumn id="18" name="Type" dataDxfId="17"/>
-    <tableColumn id="3" name="Level" dataDxfId="16"/>
-    <tableColumn id="20" name="ReviveScene" dataDxfId="15"/>
-    <tableColumn id="4" name="Quest" dataDxfId="14"/>
-    <tableColumn id="17" name="QuestRandom" dataDxfId="13"/>
-    <tableColumn id="19" name="QuestDungeon" dataDxfId="12"/>
-    <tableColumn id="5" name="QPortal" dataDxfId="11"/>
-    <tableColumn id="6" name="QCardChange" dataDxfId="10"/>
-    <tableColumn id="7" name="QPiece" dataDxfId="9"/>
-    <tableColumn id="8" name="QMerchant" dataDxfId="8"/>
-    <tableColumn id="9" name="QDoctor" dataDxfId="7"/>
-    <tableColumn id="10" name="QAngel" dataDxfId="6"/>
-    <tableColumn id="11" name="Func" dataDxfId="5"/>
-    <tableColumn id="12" name="Url" dataDxfId="4"/>
-    <tableColumn id="13" name="TilePath" dataDxfId="3"/>
-    <tableColumn id="14" name="Icon" dataDxfId="2"/>
-    <tableColumn id="15" name="IconX" dataDxfId="1"/>
-    <tableColumn id="16" name="IconY" dataDxfId="0"/>
+    <tableColumn id="1" name="Id" dataDxfId="25"/>
+    <tableColumn id="2" name="Name" dataDxfId="24"/>
+    <tableColumn id="18" name="Type" dataDxfId="23"/>
+    <tableColumn id="3" name="Level" dataDxfId="22"/>
+    <tableColumn id="20" name="ReviveScene" dataDxfId="21"/>
+    <tableColumn id="4" name="Quest" dataDxfId="8"/>
+    <tableColumn id="17" name="QuestRandom" dataDxfId="7"/>
+    <tableColumn id="19" name="QuestDungeon" dataDxfId="6"/>
+    <tableColumn id="5" name="QPortal" dataDxfId="20"/>
+    <tableColumn id="6" name="QCardChange" dataDxfId="19"/>
+    <tableColumn id="7" name="QPiece" dataDxfId="18"/>
+    <tableColumn id="8" name="QMerchant" dataDxfId="17"/>
+    <tableColumn id="9" name="QDoctor" dataDxfId="16"/>
+    <tableColumn id="10" name="QAngel" dataDxfId="15"/>
+    <tableColumn id="11" name="Func" dataDxfId="14"/>
+    <tableColumn id="12" name="Url" dataDxfId="13"/>
+    <tableColumn id="13" name="TilePath" dataDxfId="12"/>
+    <tableColumn id="14" name="Icon" dataDxfId="11"/>
+    <tableColumn id="15" name="IconX" dataDxfId="10"/>
+    <tableColumn id="16" name="IconY" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2453,7 +2479,7 @@
   <dimension ref="A1:T30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2464,7 +2490,7 @@
     <col min="4" max="4" width="4.375" customWidth="1"/>
     <col min="5" max="5" width="9" customWidth="1"/>
     <col min="6" max="6" width="52.875" customWidth="1"/>
-    <col min="7" max="7" width="16.625" customWidth="1"/>
+    <col min="7" max="7" width="23.625" customWidth="1"/>
     <col min="8" max="8" width="50.875" customWidth="1"/>
     <col min="9" max="14" width="3.125" customWidth="1"/>
     <col min="15" max="15" width="6.625" customWidth="1"/>
@@ -2488,7 +2514,7 @@
         <v>17</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>30</v>
@@ -2497,7 +2523,7 @@
         <v>92</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="I1" s="7" t="s">
         <v>50</v>
@@ -2550,7 +2576,7 @@
         <v>13</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>87</v>
@@ -2612,7 +2638,7 @@
         <v>22</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>29</v>
@@ -2621,7 +2647,7 @@
         <v>94</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="I3" s="11" t="s">
         <v>51</v>
@@ -2661,10 +2687,10 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A4" s="16">
+      <c r="A4" s="15">
         <v>13010001</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="15" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="9">
@@ -2691,7 +2717,7 @@
       <c r="N4" s="9"/>
       <c r="O4" s="9"/>
       <c r="P4" s="9" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="Q4" s="9" t="s">
         <v>28</v>
@@ -2707,10 +2733,10 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A5" s="16">
+      <c r="A5" s="15">
         <v>13010002</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="15" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="9">
@@ -2723,10 +2749,10 @@
         <v>13010001</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="H5" s="9"/>
       <c r="I5" s="9">
@@ -2759,10 +2785,10 @@
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A6" s="16">
+      <c r="A6" s="15">
         <v>13010004</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="15" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="9">
@@ -2775,10 +2801,10 @@
         <v>13010006</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>108</v>
+        <v>164</v>
       </c>
       <c r="H6" s="9"/>
       <c r="I6" s="9">
@@ -2809,11 +2835,11 @@
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A7" s="16">
+      <c r="A7" s="15">
         <v>13010005</v>
       </c>
-      <c r="B7" s="16" t="s">
-        <v>151</v>
+      <c r="B7" s="15" t="s">
+        <v>144</v>
       </c>
       <c r="C7" s="9">
         <v>2</v>
@@ -2826,7 +2852,7 @@
       </c>
       <c r="F7" s="9"/>
       <c r="G7" s="9" t="s">
-        <v>140</v>
+        <v>175</v>
       </c>
       <c r="H7" s="9"/>
       <c r="I7" s="9">
@@ -2841,7 +2867,7 @@
       <c r="N7" s="9"/>
       <c r="O7" s="9"/>
       <c r="P7" s="9" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="Q7" s="9" t="s">
         <v>36</v>
@@ -2857,10 +2883,10 @@
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A8" s="16">
+      <c r="A8" s="15">
         <v>13010006</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="15" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="9">
@@ -2883,7 +2909,7 @@
       <c r="N8" s="9"/>
       <c r="O8" s="9"/>
       <c r="P8" s="9" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="Q8" s="9" t="s">
         <v>32</v>
@@ -2899,10 +2925,10 @@
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A9" s="16">
+      <c r="A9" s="15">
         <v>13010007</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="15" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="9">
@@ -2918,7 +2944,7 @@
         <v>99</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>95</v>
+        <v>162</v>
       </c>
       <c r="H9" s="9"/>
       <c r="I9" s="9">
@@ -2935,7 +2961,7 @@
       <c r="N9" s="9"/>
       <c r="O9" s="9"/>
       <c r="P9" s="9" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="Q9" s="9" t="s">
         <v>34</v>
@@ -2951,10 +2977,10 @@
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A10" s="16">
+      <c r="A10" s="15">
         <v>13010009</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="15" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="9">
@@ -2967,10 +2993,10 @@
         <v>13010006</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="H10" s="9"/>
       <c r="I10" s="9">
@@ -2987,10 +3013,10 @@
       <c r="N10" s="9"/>
       <c r="O10" s="9"/>
       <c r="P10" s="9" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="Q10" s="9" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="R10" s="9" t="s">
         <v>74</v>
@@ -3003,10 +3029,10 @@
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A11" s="16">
+      <c r="A11" s="15">
         <v>13010010</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="15" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="9">
@@ -3020,7 +3046,7 @@
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="9" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="H11" s="9"/>
       <c r="I11" s="9">
@@ -3035,7 +3061,7 @@
       </c>
       <c r="O11" s="9"/>
       <c r="P11" s="9" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="Q11" s="9" t="s">
         <v>38</v>
@@ -3051,10 +3077,10 @@
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A12" s="16">
+      <c r="A12" s="15">
         <v>13010011</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="15" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="9">
@@ -3070,7 +3096,7 @@
         <v>91</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="H12" s="9"/>
       <c r="I12" s="9">
@@ -3085,7 +3111,7 @@
       <c r="N12" s="9"/>
       <c r="O12" s="9"/>
       <c r="P12" s="9" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="Q12" s="9" t="s">
         <v>39</v>
@@ -3101,10 +3127,10 @@
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A13" s="16">
+      <c r="A13" s="15">
         <v>13010012</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="15" t="s">
         <v>8</v>
       </c>
       <c r="C13" s="9">
@@ -3117,10 +3143,10 @@
         <v>13010006</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>110</v>
+        <v>165</v>
       </c>
       <c r="H13" s="9"/>
       <c r="I13" s="9">
@@ -3133,7 +3159,7 @@
       <c r="N13" s="9"/>
       <c r="O13" s="9"/>
       <c r="P13" s="9" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="Q13" s="9" t="s">
         <v>33</v>
@@ -3149,10 +3175,10 @@
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A14" s="16">
+      <c r="A14" s="15">
         <v>13010013</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="15" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="9">
@@ -3165,10 +3191,10 @@
         <v>13010006</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H14" s="9"/>
       <c r="I14" s="9">
@@ -3181,7 +3207,7 @@
       <c r="N14" s="9"/>
       <c r="O14" s="9"/>
       <c r="P14" s="9" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="Q14" s="9" t="s">
         <v>37</v>
@@ -3197,10 +3223,10 @@
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A15" s="16">
+      <c r="A15" s="15">
         <v>13010014</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="15" t="s">
         <v>10</v>
       </c>
       <c r="C15" s="9">
@@ -3216,7 +3242,7 @@
         <v>100</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>107</v>
+        <v>167</v>
       </c>
       <c r="H15" s="9"/>
       <c r="I15" s="9">
@@ -3233,7 +3259,7 @@
       </c>
       <c r="O15" s="9"/>
       <c r="P15" s="9" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="Q15" s="9" t="s">
         <v>40</v>
@@ -3249,52 +3275,52 @@
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A16" s="16">
+      <c r="A16" s="15">
         <v>13010015</v>
       </c>
-      <c r="B16" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="C16" s="15">
+      <c r="B16" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="C16" s="14">
         <v>2</v>
       </c>
-      <c r="D16" s="15">
+      <c r="D16" s="14">
         <v>6</v>
       </c>
       <c r="E16" s="9">
         <v>13010006</v>
       </c>
-      <c r="F16" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="G16" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="H16" s="12"/>
-      <c r="I16" s="15">
+      <c r="F16" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="H16" s="9"/>
+      <c r="I16" s="14">
         <v>1</v>
       </c>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="15"/>
-      <c r="O16" s="15"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="14"/>
       <c r="P16" s="12" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="Q16" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="R16" s="15"/>
-      <c r="S16" s="15"/>
-      <c r="T16" s="15"/>
+        <v>142</v>
+      </c>
+      <c r="R16" s="14"/>
+      <c r="S16" s="14"/>
+      <c r="T16" s="14"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A17" s="17">
+      <c r="A17" s="16">
         <v>13010101</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="16" t="s">
         <v>12</v>
       </c>
       <c r="C17" s="9">
@@ -3317,7 +3343,7 @@
       <c r="N17" s="9"/>
       <c r="O17" s="9"/>
       <c r="P17" s="9" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="Q17" s="9" t="s">
         <v>47</v>
@@ -3333,10 +3359,10 @@
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A18" s="17">
+      <c r="A18" s="16">
         <v>13010102</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="16" t="s">
         <v>11</v>
       </c>
       <c r="C18" s="9">
@@ -3349,10 +3375,10 @@
         <v>13010101</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="H18" s="9"/>
       <c r="I18" s="9">
@@ -3367,7 +3393,7 @@
       <c r="N18" s="9"/>
       <c r="O18" s="9"/>
       <c r="P18" s="9" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="Q18" s="9" t="s">
         <v>44</v>
@@ -3383,10 +3409,10 @@
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A19" s="17">
+      <c r="A19" s="16">
         <v>13010103</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="16" t="s">
         <v>45</v>
       </c>
       <c r="C19" s="9">
@@ -3399,7 +3425,7 @@
         <v>13010101</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>102</v>
+        <v>168</v>
       </c>
       <c r="G19" s="9" t="s">
         <v>95</v>
@@ -3415,10 +3441,10 @@
       <c r="N19" s="9"/>
       <c r="O19" s="9"/>
       <c r="P19" s="9" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="Q19" s="9" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="R19" s="9" t="s">
         <v>68</v>
@@ -3431,10 +3457,10 @@
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A20" s="17">
+      <c r="A20" s="16">
         <v>13010104</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="16" t="s">
         <v>41</v>
       </c>
       <c r="C20" s="9">
@@ -3450,7 +3476,7 @@
         <v>101</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="H20" s="9"/>
       <c r="I20" s="9">
@@ -3465,7 +3491,7 @@
       <c r="N20" s="9"/>
       <c r="O20" s="9"/>
       <c r="P20" s="9" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="Q20" s="9" t="s">
         <v>46</v>
@@ -3481,10 +3507,10 @@
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A21" s="17">
+      <c r="A21" s="16">
         <v>13010105</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="16" t="s">
         <v>42</v>
       </c>
       <c r="C21" s="9">
@@ -3500,7 +3526,7 @@
         <v>89</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>109</v>
+        <v>169</v>
       </c>
       <c r="H21" s="9"/>
       <c r="I21" s="9"/>
@@ -3511,7 +3537,7 @@
       <c r="N21" s="9"/>
       <c r="O21" s="9"/>
       <c r="P21" s="9" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="Q21" s="9" t="s">
         <v>48</v>
@@ -3527,11 +3553,11 @@
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A22" s="17">
+      <c r="A22" s="16">
         <v>13010106</v>
       </c>
-      <c r="B22" s="17" t="s">
-        <v>150</v>
+      <c r="B22" s="16" t="s">
+        <v>143</v>
       </c>
       <c r="C22" s="9">
         <v>2</v>
@@ -3546,7 +3572,7 @@
         <v>88</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>138</v>
+        <v>170</v>
       </c>
       <c r="H22" s="9"/>
       <c r="I22" s="9">
@@ -3561,7 +3587,7 @@
       </c>
       <c r="O22" s="9"/>
       <c r="P22" s="9" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="Q22" s="9" t="s">
         <v>43</v>
@@ -3577,13 +3603,13 @@
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A23" s="14">
+      <c r="A23" s="13">
         <v>13020001</v>
       </c>
-      <c r="B23" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="C23" s="14">
+      <c r="B23" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C23" s="13">
         <v>3</v>
       </c>
       <c r="D23" s="9">
@@ -3592,10 +3618,10 @@
       <c r="E23" s="9">
         <v>13010002</v>
       </c>
-      <c r="F23" s="13"/>
+      <c r="F23" s="9"/>
       <c r="G23" s="9"/>
       <c r="H23" s="9" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
@@ -3605,23 +3631,23 @@
       <c r="N23" s="9"/>
       <c r="O23" s="9"/>
       <c r="P23" s="9" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="Q23" s="9" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="R23" s="9"/>
       <c r="S23" s="9"/>
       <c r="T23" s="9"/>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A24" s="14">
+      <c r="A24" s="13">
         <v>13020002</v>
       </c>
-      <c r="B24" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="C24" s="14">
+      <c r="B24" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="C24" s="13">
         <v>3</v>
       </c>
       <c r="D24" s="9">
@@ -3630,7 +3656,7 @@
       <c r="E24" s="9">
         <v>13010002</v>
       </c>
-      <c r="F24" s="12"/>
+      <c r="F24" s="9"/>
       <c r="G24" s="9"/>
       <c r="H24" s="9"/>
       <c r="I24" s="9"/>
@@ -3641,23 +3667,23 @@
       <c r="N24" s="9"/>
       <c r="O24" s="9"/>
       <c r="P24" s="9" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="Q24" s="9" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="R24" s="9"/>
       <c r="S24" s="9"/>
       <c r="T24" s="9"/>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A25" s="14">
+      <c r="A25" s="13">
         <v>13020011</v>
       </c>
-      <c r="B25" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="C25" s="14">
+      <c r="B25" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="C25" s="13">
         <v>3</v>
       </c>
       <c r="D25" s="9">
@@ -3666,10 +3692,10 @@
       <c r="E25" s="9">
         <v>13010007</v>
       </c>
-      <c r="F25" s="12"/>
+      <c r="F25" s="9"/>
       <c r="G25" s="9"/>
       <c r="H25" s="9" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="I25" s="9"/>
       <c r="J25" s="9"/>
@@ -3679,23 +3705,23 @@
       <c r="N25" s="9"/>
       <c r="O25" s="9"/>
       <c r="P25" s="9" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="Q25" s="9" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="R25" s="9"/>
       <c r="S25" s="9"/>
       <c r="T25" s="9"/>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A26" s="14">
+      <c r="A26" s="13">
         <v>13020012</v>
       </c>
-      <c r="B26" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="C26" s="14">
+      <c r="B26" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="C26" s="13">
         <v>3</v>
       </c>
       <c r="D26" s="9">
@@ -3704,7 +3730,7 @@
       <c r="E26" s="9">
         <v>13010007</v>
       </c>
-      <c r="F26" s="12"/>
+      <c r="F26" s="9"/>
       <c r="G26" s="9"/>
       <c r="H26" s="9"/>
       <c r="I26" s="9"/>
@@ -3715,23 +3741,23 @@
       <c r="N26" s="9"/>
       <c r="O26" s="9"/>
       <c r="P26" s="9" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="Q26" s="9" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="R26" s="9"/>
       <c r="S26" s="9"/>
       <c r="T26" s="9"/>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A27" s="14">
+      <c r="A27" s="13">
         <v>13020013</v>
       </c>
-      <c r="B27" s="14" t="s">
-        <v>146</v>
-      </c>
-      <c r="C27" s="14">
+      <c r="B27" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="C27" s="13">
         <v>3</v>
       </c>
       <c r="D27" s="9">
@@ -3740,7 +3766,7 @@
       <c r="E27" s="9">
         <v>13010007</v>
       </c>
-      <c r="F27" s="12"/>
+      <c r="F27" s="9"/>
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
       <c r="I27" s="9"/>
@@ -3751,23 +3777,23 @@
       <c r="N27" s="9"/>
       <c r="O27" s="9"/>
       <c r="P27" s="9" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="Q27" s="9" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="R27" s="9"/>
       <c r="S27" s="9"/>
       <c r="T27" s="9"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A28" s="14">
+      <c r="A28" s="13">
         <v>13020021</v>
       </c>
-      <c r="B28" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="C28" s="14">
+      <c r="B28" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="C28" s="13">
         <v>3</v>
       </c>
       <c r="D28" s="9">
@@ -3776,14 +3802,14 @@
       <c r="E28" s="9">
         <v>13010004</v>
       </c>
-      <c r="F28" s="12" t="s">
-        <v>163</v>
+      <c r="F28" s="9" t="s">
+        <v>171</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="I28" s="9"/>
       <c r="J28" s="9"/>
@@ -3793,23 +3819,23 @@
       <c r="N28" s="9"/>
       <c r="O28" s="9"/>
       <c r="P28" s="9" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="Q28" s="9" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="R28" s="9"/>
       <c r="S28" s="9"/>
       <c r="T28" s="9"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A29" s="14">
+      <c r="A29" s="13">
         <v>13020022</v>
       </c>
-      <c r="B29" s="14" t="s">
-        <v>153</v>
-      </c>
-      <c r="C29" s="14">
+      <c r="B29" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="C29" s="13">
         <v>3</v>
       </c>
       <c r="D29" s="9">
@@ -3818,11 +3844,11 @@
       <c r="E29" s="9">
         <v>13010004</v>
       </c>
-      <c r="F29" s="12" t="s">
-        <v>161</v>
+      <c r="F29" s="9" t="s">
+        <v>173</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="H29" s="9"/>
       <c r="I29" s="9"/>
@@ -3833,23 +3859,23 @@
       <c r="N29" s="9"/>
       <c r="O29" s="9"/>
       <c r="P29" s="9" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="Q29" s="9" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="R29" s="9"/>
       <c r="S29" s="9"/>
       <c r="T29" s="9"/>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A30" s="14">
+      <c r="A30" s="13">
         <v>13020023</v>
       </c>
-      <c r="B30" s="14" t="s">
-        <v>154</v>
-      </c>
-      <c r="C30" s="14">
+      <c r="B30" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="C30" s="13">
         <v>3</v>
       </c>
       <c r="D30" s="9">
@@ -3858,11 +3884,11 @@
       <c r="E30" s="9">
         <v>13010004</v>
       </c>
-      <c r="F30" s="12" t="s">
-        <v>160</v>
+      <c r="F30" s="9" t="s">
+        <v>174</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="H30" s="9"/>
       <c r="I30" s="9"/>
@@ -3873,10 +3899,10 @@
       <c r="N30" s="9"/>
       <c r="O30" s="9"/>
       <c r="P30" s="9" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="Q30" s="9" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="R30" s="9"/>
       <c r="S30" s="9"/>
@@ -3885,13 +3911,18 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="I4:N30">
-    <cfRule type="cellIs" dxfId="24" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4">
-    <cfRule type="cellIs" dxfId="23" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
       <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F4:H30">
+    <cfRule type="containsBlanks" dxfId="3" priority="5">
+      <formula>LEN(TRIM(F4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
enext parms load from excel now.
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Scene.xlsx
+++ b/ConfigData/Xlsx/Scene.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Scene" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -383,10 +383,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>coldwind;3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>portal;3|sandflow;2|manflower;3</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -685,6 +681,10 @@
   </si>
   <si>
     <t>colorpool;1|barn;1|portal;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>coldwind;3|snowhill;2</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -2470,7 +2470,7 @@
   <dimension ref="A1:T30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2505,7 +2505,7 @@
         <v>17</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>30</v>
@@ -2514,7 +2514,7 @@
         <v>92</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I1" s="7" t="s">
         <v>50</v>
@@ -2567,7 +2567,7 @@
         <v>13</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>87</v>
@@ -2629,7 +2629,7 @@
         <v>22</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>29</v>
@@ -2638,7 +2638,7 @@
         <v>94</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I3" s="11" t="s">
         <v>51</v>
@@ -2708,7 +2708,7 @@
       <c r="N4" s="9"/>
       <c r="O4" s="9"/>
       <c r="P4" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="Q4" s="9" t="s">
         <v>28</v>
@@ -2740,10 +2740,10 @@
         <v>13010001</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H5" s="9"/>
       <c r="I5" s="9">
@@ -2792,10 +2792,10 @@
         <v>13010006</v>
       </c>
       <c r="F6" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="G6" s="9" t="s">
         <v>158</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>159</v>
       </c>
       <c r="H6" s="9"/>
       <c r="I6" s="9">
@@ -2830,7 +2830,7 @@
         <v>13010005</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C7" s="9">
         <v>2</v>
@@ -2842,10 +2842,10 @@
         <v>13010006</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H7" s="9"/>
       <c r="I7" s="9">
@@ -2860,7 +2860,7 @@
       <c r="N7" s="9"/>
       <c r="O7" s="9"/>
       <c r="P7" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="Q7" s="9" t="s">
         <v>36</v>
@@ -2902,7 +2902,7 @@
       <c r="N8" s="9"/>
       <c r="O8" s="9"/>
       <c r="P8" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="Q8" s="9" t="s">
         <v>32</v>
@@ -2937,7 +2937,7 @@
         <v>99</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H9" s="9"/>
       <c r="I9" s="9">
@@ -2954,7 +2954,7 @@
       <c r="N9" s="9"/>
       <c r="O9" s="9"/>
       <c r="P9" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Q9" s="9" t="s">
         <v>34</v>
@@ -2986,10 +2986,10 @@
         <v>13010006</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H10" s="9"/>
       <c r="I10" s="9">
@@ -3006,10 +3006,10 @@
       <c r="N10" s="9"/>
       <c r="O10" s="9"/>
       <c r="P10" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Q10" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="R10" s="9" t="s">
         <v>74</v>
@@ -3039,7 +3039,7 @@
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H11" s="9"/>
       <c r="I11" s="9">
@@ -3054,7 +3054,7 @@
       </c>
       <c r="O11" s="9"/>
       <c r="P11" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="Q11" s="9" t="s">
         <v>38</v>
@@ -3089,7 +3089,7 @@
         <v>91</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H12" s="9"/>
       <c r="I12" s="9">
@@ -3104,7 +3104,7 @@
       <c r="N12" s="9"/>
       <c r="O12" s="9"/>
       <c r="P12" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="Q12" s="9" t="s">
         <v>39</v>
@@ -3136,10 +3136,10 @@
         <v>13010006</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H13" s="9"/>
       <c r="I13" s="9">
@@ -3152,7 +3152,7 @@
       <c r="N13" s="9"/>
       <c r="O13" s="9"/>
       <c r="P13" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q13" s="9" t="s">
         <v>33</v>
@@ -3184,10 +3184,10 @@
         <v>13010006</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>102</v>
+        <v>178</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H14" s="9"/>
       <c r="I14" s="9">
@@ -3200,7 +3200,7 @@
       <c r="N14" s="9"/>
       <c r="O14" s="9"/>
       <c r="P14" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="Q14" s="9" t="s">
         <v>37</v>
@@ -3235,7 +3235,7 @@
         <v>100</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H15" s="9"/>
       <c r="I15" s="9">
@@ -3252,7 +3252,7 @@
       </c>
       <c r="O15" s="9"/>
       <c r="P15" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Q15" s="9" t="s">
         <v>40</v>
@@ -3272,7 +3272,7 @@
         <v>13010015</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C16" s="14">
         <v>2</v>
@@ -3284,10 +3284,10 @@
         <v>13010006</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H16" s="9"/>
       <c r="I16" s="14">
@@ -3300,10 +3300,10 @@
       <c r="N16" s="14"/>
       <c r="O16" s="14"/>
       <c r="P16" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q16" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="R16" s="14"/>
       <c r="S16" s="14"/>
@@ -3336,7 +3336,7 @@
       <c r="N17" s="9"/>
       <c r="O17" s="9"/>
       <c r="P17" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="Q17" s="9" t="s">
         <v>47</v>
@@ -3368,10 +3368,10 @@
         <v>13010101</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H18" s="9"/>
       <c r="I18" s="9">
@@ -3386,7 +3386,7 @@
       <c r="N18" s="9"/>
       <c r="O18" s="9"/>
       <c r="P18" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="Q18" s="9" t="s">
         <v>44</v>
@@ -3418,7 +3418,7 @@
         <v>13010101</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G19" s="9" t="s">
         <v>95</v>
@@ -3434,10 +3434,10 @@
       <c r="N19" s="9"/>
       <c r="O19" s="9"/>
       <c r="P19" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="Q19" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="R19" s="9" t="s">
         <v>68</v>
@@ -3469,7 +3469,7 @@
         <v>101</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H20" s="9"/>
       <c r="I20" s="9">
@@ -3484,7 +3484,7 @@
       <c r="N20" s="9"/>
       <c r="O20" s="9"/>
       <c r="P20" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Q20" s="9" t="s">
         <v>46</v>
@@ -3519,7 +3519,7 @@
         <v>89</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H21" s="9"/>
       <c r="I21" s="9"/>
@@ -3530,7 +3530,7 @@
       <c r="N21" s="9"/>
       <c r="O21" s="9"/>
       <c r="P21" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Q21" s="9" t="s">
         <v>48</v>
@@ -3550,7 +3550,7 @@
         <v>13010106</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C22" s="9">
         <v>2</v>
@@ -3565,7 +3565,7 @@
         <v>88</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H22" s="9"/>
       <c r="I22" s="9">
@@ -3580,7 +3580,7 @@
       </c>
       <c r="O22" s="9"/>
       <c r="P22" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Q22" s="9" t="s">
         <v>43</v>
@@ -3600,7 +3600,7 @@
         <v>13020001</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C23" s="13">
         <v>3</v>
@@ -3612,11 +3612,11 @@
         <v>13010002</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G23" s="9"/>
       <c r="H23" s="9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
@@ -3626,10 +3626,10 @@
       <c r="N23" s="9"/>
       <c r="O23" s="9"/>
       <c r="P23" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="Q23" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="R23" s="9"/>
       <c r="S23" s="9"/>
@@ -3640,7 +3640,7 @@
         <v>13020002</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C24" s="13">
         <v>3</v>
@@ -3662,10 +3662,10 @@
       <c r="N24" s="9"/>
       <c r="O24" s="9"/>
       <c r="P24" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="Q24" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="R24" s="9"/>
       <c r="S24" s="9"/>
@@ -3676,7 +3676,7 @@
         <v>13020011</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C25" s="13">
         <v>3</v>
@@ -3698,10 +3698,10 @@
       <c r="N25" s="9"/>
       <c r="O25" s="9"/>
       <c r="P25" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Q25" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="R25" s="9"/>
       <c r="S25" s="9"/>
@@ -3712,7 +3712,7 @@
         <v>13020012</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C26" s="13">
         <v>3</v>
@@ -3734,10 +3734,10 @@
       <c r="N26" s="9"/>
       <c r="O26" s="9"/>
       <c r="P26" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Q26" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="R26" s="9"/>
       <c r="S26" s="9"/>
@@ -3748,7 +3748,7 @@
         <v>13020013</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C27" s="13">
         <v>3</v>
@@ -3770,10 +3770,10 @@
       <c r="N27" s="9"/>
       <c r="O27" s="9"/>
       <c r="P27" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="Q27" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="R27" s="9"/>
       <c r="S27" s="9"/>
@@ -3784,7 +3784,7 @@
         <v>13020021</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C28" s="13">
         <v>3</v>
@@ -3796,13 +3796,13 @@
         <v>13010004</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I28" s="9"/>
       <c r="J28" s="9"/>
@@ -3812,10 +3812,10 @@
       <c r="N28" s="9"/>
       <c r="O28" s="9"/>
       <c r="P28" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="Q28" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="R28" s="9"/>
       <c r="S28" s="9"/>
@@ -3826,7 +3826,7 @@
         <v>13020022</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C29" s="13">
         <v>3</v>
@@ -3838,13 +3838,13 @@
         <v>13010004</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H29" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I29" s="9"/>
       <c r="J29" s="9"/>
@@ -3854,10 +3854,10 @@
       <c r="N29" s="9"/>
       <c r="O29" s="9"/>
       <c r="P29" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="Q29" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="R29" s="9"/>
       <c r="S29" s="9"/>
@@ -3868,7 +3868,7 @@
         <v>13020023</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C30" s="13">
         <v>3</v>
@@ -3880,13 +3880,13 @@
         <v>13010004</v>
       </c>
       <c r="F30" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="H30" s="9" t="s">
         <v>171</v>
-      </c>
-      <c r="G30" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="H30" s="9" t="s">
-        <v>172</v>
       </c>
       <c r="I30" s="9"/>
       <c r="J30" s="9"/>
@@ -3896,10 +3896,10 @@
       <c r="N30" s="9"/>
       <c r="O30" s="9"/>
       <c r="P30" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="Q30" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="R30" s="9"/>
       <c r="S30" s="9"/>

</xml_diff>

<commit_message>
new implement of scene format
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Scene.xlsx
+++ b/ConfigData/Xlsx/Scene.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18229"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="Scene" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="186">
   <si>
     <t>村外小屋</t>
   </si>
@@ -487,25 +487,21 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>persepalace3</t>
+  </si>
+  <si>
+    <t>古城外围</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>古城大殿</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>persepalace2</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>persepalace3</t>
-  </si>
-  <si>
-    <t>古城外围</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>古城大殿</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>persepalace2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>玲珑峰隧道</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -534,77 +530,70 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>viliage2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>viliage3</t>
+  </si>
+  <si>
+    <t>hiddeway;35</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>forestfire;10|crystalball;35</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|lighthouse;60</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|goblinhome;40|lighthouse;70</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|goblinhome;30|gamecook;20</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>wolfnest;2|gamegamble;1|fishpool;2|sewer;3|river;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>forestfire;35|witchhome;10</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|icedream;25|lighthouse;30</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|witchhome;30</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>orehole;1|stone;2|sandflow;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|forestfire;20|witchhome;40</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|goblinhome;40</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>crystalball;55</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trees;3|grave;1|portal;1|oldtree;1|manflower;1|gamerace;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>viliage1</t>
-  </si>
-  <si>
-    <t>viliage2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>viliage3</t>
-  </si>
-  <si>
-    <t>forestmaze</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>hiddeway;35</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>forestfire;10|crystalball;35</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|lighthouse;60</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|goblinhome;40|lighthouse;70</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|goblinhome;30|gamecook;20</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>wolfnest;2|gamegamble;1|fishpool;2|sewer;3|river;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>forestfire;35|witchhome;10</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|icedream;25|lighthouse;30</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|witchhome;30</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>orehole;1|stone;2|sandflow;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|forestfire;20|witchhome;40</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|goblinhome;40</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>crystalball;55</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>trees;3|grave;1|portal;1|oldtree;1|manflower;1|gamerace;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>viliage1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -693,6 +682,38 @@
   </si>
   <si>
     <t>coldwind;3|snowhill;2|snowmountain;2|ropeway;1|iceland;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dgforestmaze</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dgforestinner</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dgpersepalace1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dgpersepalace2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dgpersepalace3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dgviliage1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dgviliage2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dgviliage3</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -2478,7 +2499,7 @@
   <dimension ref="A1:T30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="Q24" sqref="Q24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2748,10 +2769,10 @@
         <v>13010001</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="H5" s="9"/>
       <c r="I5" s="9">
@@ -2800,10 +2821,10 @@
         <v>13010006</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="H6" s="9"/>
       <c r="I6" s="9">
@@ -2838,7 +2859,7 @@
         <v>13010005</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C7" s="9">
         <v>2</v>
@@ -2850,10 +2871,10 @@
         <v>13010006</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="H7" s="9"/>
       <c r="I7" s="9">
@@ -2942,10 +2963,10 @@
         <v>13010006</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="H9" s="9"/>
       <c r="I9" s="9">
@@ -2994,10 +3015,10 @@
         <v>13010006</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="H10" s="9"/>
       <c r="I10" s="9">
@@ -3047,7 +3068,7 @@
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="9" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H11" s="9"/>
       <c r="I11" s="9">
@@ -3094,10 +3115,10 @@
         <v>13010006</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H12" s="9"/>
       <c r="I12" s="9">
@@ -3144,10 +3165,10 @@
         <v>13010006</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H13" s="9"/>
       <c r="I13" s="9">
@@ -3192,10 +3213,10 @@
         <v>13010006</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="H14" s="9"/>
       <c r="I14" s="9">
@@ -3240,10 +3261,10 @@
         <v>13010006</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="H15" s="9"/>
       <c r="I15" s="9">
@@ -3280,7 +3301,7 @@
         <v>13010015</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C16" s="14">
         <v>2</v>
@@ -3292,10 +3313,10 @@
         <v>13010006</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="H16" s="9"/>
       <c r="I16" s="14">
@@ -3308,10 +3329,10 @@
       <c r="N16" s="14"/>
       <c r="O16" s="14"/>
       <c r="P16" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="Q16" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="R16" s="14"/>
       <c r="S16" s="14"/>
@@ -3426,7 +3447,7 @@
         <v>13010101</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="G19" s="9" t="s">
         <v>93</v>
@@ -3477,7 +3498,7 @@
         <v>97</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H20" s="9"/>
       <c r="I20" s="9">
@@ -3527,7 +3548,7 @@
         <v>88</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="H21" s="9"/>
       <c r="I21" s="9"/>
@@ -3558,7 +3579,7 @@
         <v>13010106</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C22" s="9">
         <v>2</v>
@@ -3570,10 +3591,10 @@
         <v>13010016</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="H22" s="9"/>
       <c r="I22" s="9">
@@ -3620,11 +3641,11 @@
         <v>13010002</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G23" s="9"/>
       <c r="H23" s="9" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
@@ -3637,7 +3658,7 @@
         <v>118</v>
       </c>
       <c r="Q23" s="9" t="s">
-        <v>143</v>
+        <v>178</v>
       </c>
       <c r="R23" s="9"/>
       <c r="S23" s="9"/>
@@ -3673,7 +3694,7 @@
         <v>119</v>
       </c>
       <c r="Q24" s="9" t="s">
-        <v>119</v>
+        <v>179</v>
       </c>
       <c r="R24" s="9"/>
       <c r="S24" s="9"/>
@@ -3684,7 +3705,7 @@
         <v>13020011</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C25" s="13">
         <v>3</v>
@@ -3709,7 +3730,7 @@
         <v>127</v>
       </c>
       <c r="Q25" s="9" t="s">
-        <v>127</v>
+        <v>180</v>
       </c>
       <c r="R25" s="9"/>
       <c r="S25" s="9"/>
@@ -3732,7 +3753,7 @@
         <v>13010007</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="G26" s="9"/>
       <c r="H26" s="9"/>
@@ -3744,10 +3765,10 @@
       <c r="N26" s="9"/>
       <c r="O26" s="9"/>
       <c r="P26" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Q26" s="9" t="s">
-        <v>128</v>
+        <v>181</v>
       </c>
       <c r="R26" s="9"/>
       <c r="S26" s="9"/>
@@ -3758,7 +3779,7 @@
         <v>13020013</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C27" s="13">
         <v>3</v>
@@ -3780,10 +3801,10 @@
       <c r="N27" s="9"/>
       <c r="O27" s="9"/>
       <c r="P27" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="Q27" s="9" t="s">
-        <v>129</v>
+        <v>182</v>
       </c>
       <c r="R27" s="9"/>
       <c r="S27" s="9"/>
@@ -3794,7 +3815,7 @@
         <v>13020021</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C28" s="13">
         <v>3</v>
@@ -3806,13 +3827,13 @@
         <v>13010004</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="I28" s="9"/>
       <c r="J28" s="9"/>
@@ -3822,10 +3843,10 @@
       <c r="N28" s="9"/>
       <c r="O28" s="9"/>
       <c r="P28" s="9" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="Q28" s="9" t="s">
-        <v>140</v>
+        <v>183</v>
       </c>
       <c r="R28" s="9"/>
       <c r="S28" s="9"/>
@@ -3836,7 +3857,7 @@
         <v>13020022</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C29" s="13">
         <v>3</v>
@@ -3848,13 +3869,13 @@
         <v>13010004</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="H29" s="9" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="I29" s="9"/>
       <c r="J29" s="9"/>
@@ -3864,10 +3885,10 @@
       <c r="N29" s="9"/>
       <c r="O29" s="9"/>
       <c r="P29" s="9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Q29" s="9" t="s">
-        <v>141</v>
+        <v>184</v>
       </c>
       <c r="R29" s="9"/>
       <c r="S29" s="9"/>
@@ -3878,7 +3899,7 @@
         <v>13020023</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C30" s="13">
         <v>3</v>
@@ -3890,13 +3911,13 @@
         <v>13010004</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="H30" s="9" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="I30" s="9"/>
       <c r="J30" s="9"/>
@@ -3906,10 +3927,10 @@
       <c r="N30" s="9"/>
       <c r="O30" s="9"/>
       <c r="P30" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="Q30" s="9" t="s">
-        <v>142</v>
+        <v>185</v>
       </c>
       <c r="R30" s="9"/>
       <c r="S30" s="9"/>

</xml_diff>

<commit_message>
fix a new task of hiddn quest
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Scene.xlsx
+++ b/ConfigData/Xlsx/Scene.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="187">
   <si>
     <t>村外小屋</t>
   </si>
@@ -714,6 +714,10 @@
   </si>
   <si>
     <t>dgviliage3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>strangeletter1;30</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -721,7 +725,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -911,6 +915,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
@@ -1415,7 +1427,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1465,6 +1477,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="39" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2499,7 +2514,7 @@
   <dimension ref="A1:T30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q24" sqref="Q24"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2725,7 +2740,9 @@
       <c r="F4" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="G4" s="9"/>
+      <c r="G4" s="17" t="s">
+        <v>186</v>
+      </c>
       <c r="H4" s="9"/>
       <c r="I4" s="9">
         <v>1</v>

</xml_diff>

<commit_message>
add a scene quest
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Scene.xlsx
+++ b/ConfigData/Xlsx/Scene.xlsx
@@ -673,10 +673,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>ruintown1;1|manflower;2|cornfield;1|honeyhome;3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>coldwind;3|snowhill;2|snowmountain;2|ropeway;1|iceland;2</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -718,6 +714,10 @@
   </si>
   <si>
     <t>underwater;40|earthcrack;60|stonedoor;15|cavefind1;60</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ruintown1;1|manflower;2|cornfield;1|honeyhome;3|poppyfield;1|river;2|insectstorm;1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -2514,7 +2514,7 @@
   <dimension ref="A1:T30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2741,7 +2741,7 @@
         <v>89</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H4" s="9"/>
       <c r="I4" s="9">
@@ -3032,7 +3032,7 @@
         <v>13010006</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>175</v>
+        <v>186</v>
       </c>
       <c r="G10" s="9" t="s">
         <v>145</v>
@@ -3230,7 +3230,7 @@
         <v>13010006</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G14" s="9" t="s">
         <v>148</v>
@@ -3333,7 +3333,7 @@
         <v>163</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H16" s="9"/>
       <c r="I16" s="14">
@@ -3675,7 +3675,7 @@
         <v>118</v>
       </c>
       <c r="Q23" s="9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="R23" s="9"/>
       <c r="S23" s="9"/>
@@ -3711,7 +3711,7 @@
         <v>119</v>
       </c>
       <c r="Q24" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="R24" s="9"/>
       <c r="S24" s="9"/>
@@ -3747,7 +3747,7 @@
         <v>127</v>
       </c>
       <c r="Q25" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="R25" s="9"/>
       <c r="S25" s="9"/>
@@ -3785,7 +3785,7 @@
         <v>131</v>
       </c>
       <c r="Q26" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="R26" s="9"/>
       <c r="S26" s="9"/>
@@ -3821,7 +3821,7 @@
         <v>128</v>
       </c>
       <c r="Q27" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="R27" s="9"/>
       <c r="S27" s="9"/>
@@ -3863,7 +3863,7 @@
         <v>155</v>
       </c>
       <c r="Q28" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="R28" s="9"/>
       <c r="S28" s="9"/>
@@ -3905,7 +3905,7 @@
         <v>139</v>
       </c>
       <c r="Q29" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="R29" s="9"/>
       <c r="S29" s="9"/>
@@ -3947,7 +3947,7 @@
         <v>140</v>
       </c>
       <c r="Q30" s="9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="R30" s="9"/>
       <c r="S30" s="9"/>

</xml_diff>

<commit_message>
add the tower map and terrain
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Scene.xlsx
+++ b/ConfigData/Xlsx/Scene.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="201">
   <si>
     <t>村外小屋</t>
   </si>
@@ -514,230 +514,265 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>村落入口</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>村中心</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>议事厅</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>viliage2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>viliage3</t>
+  </si>
+  <si>
+    <t>hiddeway;35</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>forestfire;10|crystalball;35</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|lighthouse;60</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|goblinhome;40|lighthouse;70</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|goblinhome;30|gamecook;20</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>wolfnest;2|gamegamble;1|fishpool;2|sewer;3|river;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>forestfire;35|witchhome;10</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|icedream;25|lighthouse;30</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|forestfire;20|witchhome;40</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|goblinhome;40</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>crystalball;55</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trees;3|grave;1|portal;1|oldtree;1|manflower;1|gamerace;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>viliage1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trees;4|manflower;2|sandland;2|cliff;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>colorpool;1|barn;1|portal;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>poppyfield;1|fishpool;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trees;4|sandland;2|potteryroom;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>suntemple;2|potteryroom;2|honeyhome;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>barn;1|diarybook;1|weaponseller;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>river;2|stone;3|ruintown1;1|hiddeway;1|manflower;2|orehole;1|weaponseller;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>mushroom;1|torch;1|batcrowd;2|earthelement;1|snare;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>suntemple;2|grave;2|snare;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|treasure;25|witchhome;20|dyeseller;25</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>shadowprince;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>bossmanwang;1|stonedoor;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>goblinhome;50|gamemagicbook;15|stonedoor;20</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>sandflow;2|brokehouse;2|colordoor;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>coldwind;3|snowhill;2|snowmountain;2|ropeway;1|iceland;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dgforestmaze</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dgforestinner</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dgpersepalace1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dgpersepalace2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dgpersepalace3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dgviliage1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dgviliage2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dgviliage3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>strangeletter1;30</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>underwater;40|earthcrack;60|stonedoor;15|cavefind1;60</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ruintown1;1|manflower;2|cornfield;1|honeyhome;3|poppyfield;1|river;2|insectstorm;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|lighthouse;60|floatbottle;50</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>orehole;1|stone;2|sandflow;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>river;2|fishpool;1|swamp;2|colordoor;1|corsair1;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>suntemple;2|shadowprince;1|colordoor;1|blockway;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>blockway;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|treasure;25|gamerobot;20|dyeseller;30|waterbeast;20</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|witchhome;30|waterbeast;20</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>portal;1|fishpool;1|grave;2|hiddeway;1|snare;2|starve;2|blockway;1|suntemple;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>fortune;1|colordoor;1|waternest;2|ruinpiece;3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>shell;2|waternest;3|sandflow;1|corsair1;1|ruinpiece;3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>布萨特高塔</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>村落入口</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>村中心</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>议事厅</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>viliage2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>viliage3</t>
-  </si>
-  <si>
-    <t>hiddeway;35</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>forestfire;10|crystalball;35</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|lighthouse;60</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|goblinhome;40|lighthouse;70</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|goblinhome;30|gamecook;20</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>wolfnest;2|gamegamble;1|fishpool;2|sewer;3|river;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>forestfire;35|witchhome;10</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|icedream;25|lighthouse;30</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|forestfire;20|witchhome;40</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|goblinhome;40</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>crystalball;55</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>trees;3|grave;1|portal;1|oldtree;1|manflower;1|gamerace;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>viliage1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>trees;4|manflower;2|sandland;2|cliff;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>colorpool;1|barn;1|portal;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>poppyfield;1|fishpool;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>trees;4|sandland;2|potteryroom;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>suntemple;2|potteryroom;2|honeyhome;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>barn;1|diarybook;1|weaponseller;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>river;2|stone;3|ruintown1;1|hiddeway;1|manflower;2|orehole;1|weaponseller;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>mushroom;1|torch;1|batcrowd;2|earthelement;1|snare;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>suntemple;2|grave;2|snare;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|treasure;25|witchhome;20|dyeseller;25</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>shadowprince;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>bossmanwang;1|stonedoor;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>goblinhome;50|gamemagicbook;15|stonedoor;20</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>sandflow;2|brokehouse;2|colordoor;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>coldwind;3|snowhill;2|snowmountain;2|ropeway;1|iceland;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>dgforestmaze</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>dgforestinner</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>dgpersepalace1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>dgpersepalace2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>dgpersepalace3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>dgviliage1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>dgviliage2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>dgviliage3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>strangeletter1;30</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>underwater;40|earthcrack;60|stonedoor;15|cavefind1;60</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ruintown1;1|manflower;2|cornfield;1|honeyhome;3|poppyfield;1|river;2|insectstorm;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|lighthouse;60|floatbottle;50</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>orehole;1|stone;2|sandflow;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>river;2|fishpool;1|swamp;2|colordoor;1|corsair1;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>suntemple;2|shadowprince;1|colordoor;1|blockway;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>blockway;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|treasure;25|gamerobot;20|dyeseller;30|waterbeast;20</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|witchhome;30|waterbeast;20</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>portal;1|fishpool;1|grave;2|hiddeway;1|snare;2|starve;2|blockway;1|suntemple;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>fortune;1|colordoor;1|waternest;2|ruinpiece;3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>shell;2|waternest;3|sandflow;1|corsair1;1|ruinpiece;3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
+    <t>高塔1层</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>tower</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>高塔2层</t>
+  </si>
+  <si>
+    <t>高塔3层</t>
+  </si>
+  <si>
+    <t>高塔4层</t>
+  </si>
+  <si>
+    <t>高塔5层</t>
+  </si>
+  <si>
+    <t>dgtower1</t>
+  </si>
+  <si>
+    <t>dgtower2</t>
+  </si>
+  <si>
+    <t>dgtower3</t>
+  </si>
+  <si>
+    <t>dgtower4</t>
+  </si>
+  <si>
+    <t>dgtower5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -937,6 +972,13 @@
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -1439,7 +1481,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1492,6 +1534,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1539,7 +1590,21 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="28">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2171,32 +2236,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A3:T30" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21" tableBorderDxfId="20">
-  <autoFilter ref="A3:T30" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A3:T35" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23" tableBorderDxfId="22">
+  <autoFilter ref="A3:T35" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState ref="A4:T27">
     <sortCondition ref="A3:A27"/>
   </sortState>
   <tableColumns count="20">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="18"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Type" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Level" dataDxfId="16"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="ReviveScene" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Quest" dataDxfId="14"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="QuestRandom" dataDxfId="13"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="QuestDungeon" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="QPortal" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="QCardChange" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="QPiece" dataDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="QMerchant" dataDxfId="8"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="QDoctor" dataDxfId="7"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="QAngel" dataDxfId="6"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Func" dataDxfId="5"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Url" dataDxfId="4"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="TilePath" dataDxfId="3"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Icon" dataDxfId="2"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="IconX" dataDxfId="1"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="IconY" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="20"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Type" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Level" dataDxfId="18"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="ReviveScene" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Quest" dataDxfId="16"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="QuestRandom" dataDxfId="15"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="QuestDungeon" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="QPortal" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="QCardChange" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="QPiece" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="QMerchant" dataDxfId="10"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="QDoctor" dataDxfId="9"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="QAngel" dataDxfId="8"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Func" dataDxfId="7"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Url" dataDxfId="6"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="TilePath" dataDxfId="5"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Icon" dataDxfId="4"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="IconX" dataDxfId="3"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="IconY" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2523,10 +2588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T30"/>
+  <dimension ref="A1:T35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2753,7 +2818,7 @@
         <v>89</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H4" s="9"/>
       <c r="I4" s="9">
@@ -2798,10 +2863,10 @@
         <v>13010001</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H5" s="9"/>
       <c r="I5" s="9">
@@ -2850,10 +2915,10 @@
         <v>13010006</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H6" s="9"/>
       <c r="I6" s="9">
@@ -2888,7 +2953,7 @@
         <v>13010005</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>135</v>
+        <v>189</v>
       </c>
       <c r="C7" s="9">
         <v>2</v>
@@ -2900,10 +2965,10 @@
         <v>13010006</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H7" s="9"/>
       <c r="I7" s="9">
@@ -2992,10 +3057,10 @@
         <v>13010006</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H9" s="9"/>
       <c r="I9" s="9">
@@ -3044,10 +3109,10 @@
         <v>13010006</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H10" s="9"/>
       <c r="I10" s="9">
@@ -3096,10 +3161,10 @@
         <v>13010006</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H11" s="9"/>
       <c r="I11" s="9">
@@ -3146,10 +3211,10 @@
         <v>13010006</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H12" s="9"/>
       <c r="I12" s="9">
@@ -3196,10 +3261,10 @@
         <v>13010006</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H13" s="9"/>
       <c r="I13" s="9">
@@ -3244,10 +3309,10 @@
         <v>13010006</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H14" s="9"/>
       <c r="I14" s="9">
@@ -3292,10 +3357,10 @@
         <v>13010006</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H15" s="9"/>
       <c r="I15" s="9">
@@ -3344,10 +3409,10 @@
         <v>13010006</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H16" s="9"/>
       <c r="I16" s="14">
@@ -3478,7 +3543,7 @@
         <v>13010101</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G19" s="9" t="s">
         <v>93</v>
@@ -3529,7 +3594,7 @@
         <v>97</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H20" s="9"/>
       <c r="I20" s="9">
@@ -3579,7 +3644,7 @@
         <v>88</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H21" s="9"/>
       <c r="I21" s="9"/>
@@ -3622,10 +3687,10 @@
         <v>13010016</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H22" s="9"/>
       <c r="I22" s="9">
@@ -3672,11 +3737,11 @@
         <v>13010002</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G23" s="9"/>
       <c r="H23" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
@@ -3689,7 +3754,7 @@
         <v>118</v>
       </c>
       <c r="Q23" s="9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="R23" s="9"/>
       <c r="S23" s="9"/>
@@ -3725,7 +3790,7 @@
         <v>119</v>
       </c>
       <c r="Q24" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="R24" s="9"/>
       <c r="S24" s="9"/>
@@ -3748,7 +3813,7 @@
         <v>13010007</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G25" s="9"/>
       <c r="H25" s="9"/>
@@ -3763,7 +3828,7 @@
         <v>127</v>
       </c>
       <c r="Q25" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="R25" s="9"/>
       <c r="S25" s="9"/>
@@ -3786,7 +3851,7 @@
         <v>13010007</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G26" s="9"/>
       <c r="H26" s="9"/>
@@ -3801,7 +3866,7 @@
         <v>131</v>
       </c>
       <c r="Q26" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="R26" s="9"/>
       <c r="S26" s="9"/>
@@ -3837,7 +3902,7 @@
         <v>128</v>
       </c>
       <c r="Q27" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="R27" s="9"/>
       <c r="S27" s="9"/>
@@ -3848,7 +3913,7 @@
         <v>13020021</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C28" s="13">
         <v>3</v>
@@ -3860,13 +3925,13 @@
         <v>13010004</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I28" s="9"/>
       <c r="J28" s="9"/>
@@ -3876,10 +3941,10 @@
       <c r="N28" s="9"/>
       <c r="O28" s="9"/>
       <c r="P28" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="Q28" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="R28" s="9"/>
       <c r="S28" s="9"/>
@@ -3890,7 +3955,7 @@
         <v>13020022</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C29" s="13">
         <v>3</v>
@@ -3902,13 +3967,13 @@
         <v>13010004</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H29" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I29" s="9"/>
       <c r="J29" s="9"/>
@@ -3918,10 +3983,10 @@
       <c r="N29" s="9"/>
       <c r="O29" s="9"/>
       <c r="P29" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q29" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="R29" s="9"/>
       <c r="S29" s="9"/>
@@ -3932,7 +3997,7 @@
         <v>13020023</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C30" s="13">
         <v>3</v>
@@ -3944,13 +4009,13 @@
         <v>13010004</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H30" s="9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I30" s="9"/>
       <c r="J30" s="9"/>
@@ -3960,29 +4025,209 @@
       <c r="N30" s="9"/>
       <c r="O30" s="9"/>
       <c r="P30" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q30" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="R30" s="9"/>
       <c r="S30" s="9"/>
       <c r="T30" s="9"/>
     </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A31" s="18">
+        <v>13020031</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="C31" s="18">
+        <v>3</v>
+      </c>
+      <c r="D31" s="19">
+        <v>10</v>
+      </c>
+      <c r="E31" s="19">
+        <v>13010005</v>
+      </c>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="19"/>
+      <c r="J31" s="19"/>
+      <c r="K31" s="19"/>
+      <c r="L31" s="19"/>
+      <c r="M31" s="19"/>
+      <c r="N31" s="19"/>
+      <c r="O31" s="19"/>
+      <c r="P31" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="Q31" s="19" t="s">
+        <v>196</v>
+      </c>
+      <c r="R31" s="19"/>
+      <c r="S31" s="19"/>
+      <c r="T31" s="19"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A32" s="18">
+        <v>13020032</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="C32" s="18">
+        <v>3</v>
+      </c>
+      <c r="D32" s="19">
+        <v>10</v>
+      </c>
+      <c r="E32" s="19">
+        <v>13010005</v>
+      </c>
+      <c r="F32" s="19"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="19"/>
+      <c r="I32" s="19"/>
+      <c r="J32" s="19"/>
+      <c r="K32" s="19"/>
+      <c r="L32" s="19"/>
+      <c r="M32" s="19"/>
+      <c r="N32" s="19"/>
+      <c r="O32" s="19"/>
+      <c r="P32" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="Q32" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="R32" s="19"/>
+      <c r="S32" s="19"/>
+      <c r="T32" s="19"/>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A33" s="18">
+        <v>13020033</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="C33" s="18">
+        <v>3</v>
+      </c>
+      <c r="D33" s="19">
+        <v>10</v>
+      </c>
+      <c r="E33" s="19">
+        <v>13010005</v>
+      </c>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="19"/>
+      <c r="I33" s="19"/>
+      <c r="J33" s="19"/>
+      <c r="K33" s="19"/>
+      <c r="L33" s="19"/>
+      <c r="M33" s="19"/>
+      <c r="N33" s="19"/>
+      <c r="O33" s="19"/>
+      <c r="P33" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="Q33" s="19" t="s">
+        <v>198</v>
+      </c>
+      <c r="R33" s="20"/>
+      <c r="S33" s="20"/>
+      <c r="T33" s="20"/>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A34" s="18">
+        <v>13020034</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="C34" s="18">
+        <v>3</v>
+      </c>
+      <c r="D34" s="19">
+        <v>10</v>
+      </c>
+      <c r="E34" s="19">
+        <v>13010005</v>
+      </c>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="19"/>
+      <c r="I34" s="19"/>
+      <c r="J34" s="19"/>
+      <c r="K34" s="19"/>
+      <c r="L34" s="19"/>
+      <c r="M34" s="19"/>
+      <c r="N34" s="19"/>
+      <c r="O34" s="19"/>
+      <c r="P34" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="Q34" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="R34" s="20"/>
+      <c r="S34" s="20"/>
+      <c r="T34" s="20"/>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="A35" s="18">
+        <v>13020035</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="C35" s="18">
+        <v>3</v>
+      </c>
+      <c r="D35" s="19">
+        <v>10</v>
+      </c>
+      <c r="E35" s="19">
+        <v>13010005</v>
+      </c>
+      <c r="F35" s="19"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="19"/>
+      <c r="I35" s="19"/>
+      <c r="J35" s="19"/>
+      <c r="K35" s="19"/>
+      <c r="L35" s="19"/>
+      <c r="M35" s="19"/>
+      <c r="N35" s="19"/>
+      <c r="O35" s="19"/>
+      <c r="P35" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="Q35" s="19" t="s">
+        <v>200</v>
+      </c>
+      <c r="R35" s="20"/>
+      <c r="S35" s="20"/>
+      <c r="T35" s="20"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="I4:N30">
-    <cfRule type="cellIs" dxfId="25" priority="4" operator="equal">
+  <conditionalFormatting sqref="I4:N35">
+    <cfRule type="cellIs" dxfId="27" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4">
-    <cfRule type="cellIs" dxfId="24" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F4:H30">
-    <cfRule type="containsBlanks" dxfId="23" priority="5">
+  <conditionalFormatting sqref="F4:H35">
+    <cfRule type="containsBlanks" dxfId="25" priority="5">
       <formula>LEN(TRIM(F4))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
fix the warp data of maze tower
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Scene.xlsx
+++ b/ConfigData/Xlsx/Scene.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="206">
   <si>
     <t>村外小屋</t>
   </si>
@@ -597,182 +597,197 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>suntemple;2|potteryroom;2|honeyhome;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>barn;1|diarybook;1|weaponseller;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>river;2|stone;3|ruintown1;1|hiddeway;1|manflower;2|orehole;1|weaponseller;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>mushroom;1|torch;1|batcrowd;2|earthelement;1|snare;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>suntemple;2|grave;2|snare;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|treasure;25|witchhome;20|dyeseller;25</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>shadowprince;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>bossmanwang;1|stonedoor;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>goblinhome;50|gamemagicbook;15|stonedoor;20</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>sandflow;2|brokehouse;2|colordoor;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>coldwind;3|snowhill;2|snowmountain;2|ropeway;1|iceland;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dgforestmaze</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dgforestinner</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dgpersepalace1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dgpersepalace2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dgpersepalace3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dgviliage1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dgviliage2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dgviliage3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>strangeletter1;30</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>underwater;40|earthcrack;60|stonedoor;15|cavefind1;60</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ruintown1;1|manflower;2|cornfield;1|honeyhome;3|poppyfield;1|river;2|insectstorm;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|lighthouse;60|floatbottle;50</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>orehole;1|stone;2|sandflow;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>river;2|fishpool;1|swamp;2|colordoor;1|corsair1;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>suntemple;2|shadowprince;1|colordoor;1|blockway;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>blockway;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|treasure;25|gamerobot;20|dyeseller;30|waterbeast;20</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|witchhome;30|waterbeast;20</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>portal;1|fishpool;1|grave;2|hiddeway;1|snare;2|starve;2|blockway;1|suntemple;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>fortune;1|colordoor;1|waternest;2|ruinpiece;3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>shell;2|waternest;3|sandflow;1|corsair1;1|ruinpiece;3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>布萨特高塔</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>高塔1层</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>tower</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>高塔2层</t>
+  </si>
+  <si>
+    <t>高塔3层</t>
+  </si>
+  <si>
+    <t>高塔4层</t>
+  </si>
+  <si>
+    <t>高塔5层</t>
+  </si>
+  <si>
+    <t>dgtower1</t>
+  </si>
+  <si>
+    <t>dgtower2</t>
+  </si>
+  <si>
+    <t>dgtower3</t>
+  </si>
+  <si>
+    <t>dgtower4</t>
+  </si>
+  <si>
+    <t>dgtower5</t>
+  </si>
+  <si>
     <t>trees;4|sandland;2|potteryroom;2</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>suntemple;2|potteryroom;2|honeyhome;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>barn;1|diarybook;1|weaponseller;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>river;2|stone;3|ruintown1;1|hiddeway;1|manflower;2|orehole;1|weaponseller;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>mushroom;1|torch;1|batcrowd;2|earthelement;1|snare;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>suntemple;2|grave;2|snare;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|treasure;25|witchhome;20|dyeseller;25</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>shadowprince;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>bossmanwang;1|stonedoor;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>goblinhome;50|gamemagicbook;15|stonedoor;20</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>sandflow;2|brokehouse;2|colordoor;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>coldwind;3|snowhill;2|snowmountain;2|ropeway;1|iceland;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>dgforestmaze</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>dgforestinner</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>dgpersepalace1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>dgpersepalace2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>dgpersepalace3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>dgviliage1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>dgviliage2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>dgviliage3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>strangeletter1;30</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>underwater;40|earthcrack;60|stonedoor;15|cavefind1;60</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ruintown1;1|manflower;2|cornfield;1|honeyhome;3|poppyfield;1|river;2|insectstorm;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|lighthouse;60|floatbottle;50</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>orehole;1|stone;2|sandflow;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>river;2|fishpool;1|swamp;2|colordoor;1|corsair1;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>suntemple;2|shadowprince;1|colordoor;1|blockway;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>blockway;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|treasure;25|gamerobot;20|dyeseller;30|waterbeast;20</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|witchhome;30|waterbeast;20</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>portal;1|fishpool;1|grave;2|hiddeway;1|snare;2|starve;2|blockway;1|suntemple;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>fortune;1|colordoor;1|waternest;2|ruinpiece;3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>shell;2|waternest;3|sandflow;1|corsair1;1|ruinpiece;3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>布萨特高塔</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>高塔1层</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>tower</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>高塔2层</t>
-  </si>
-  <si>
-    <t>高塔3层</t>
-  </si>
-  <si>
-    <t>高塔4层</t>
-  </si>
-  <si>
-    <t>高塔5层</t>
-  </si>
-  <si>
-    <t>dgtower1</t>
-  </si>
-  <si>
-    <t>dgtower2</t>
-  </si>
-  <si>
-    <t>dgtower3</t>
-  </si>
-  <si>
-    <t>dgtower4</t>
-  </si>
-  <si>
-    <t>dgtower5</t>
+    <t>trees;4</t>
+  </si>
+  <si>
+    <t>trees;5</t>
+  </si>
+  <si>
+    <t>trees;6</t>
+  </si>
+  <si>
+    <t>trees;7</t>
+  </si>
+  <si>
+    <t>trees;8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -934,15 +949,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -955,11 +961,12 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <family val="3"/>
+      <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -968,8 +975,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
@@ -1497,52 +1521,52 @@
     <xf numFmtId="0" fontId="19" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="38" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="20" fillId="39" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1590,21 +1614,7 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="28">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="26">
     <dxf>
       <font>
         <b val="0"/>
@@ -2236,32 +2246,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A3:T35" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23" tableBorderDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A3:T35" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21" tableBorderDxfId="20">
   <autoFilter ref="A3:T35" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState ref="A4:T27">
     <sortCondition ref="A3:A27"/>
   </sortState>
   <tableColumns count="20">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="20"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Type" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Level" dataDxfId="18"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="ReviveScene" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Quest" dataDxfId="16"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="QuestRandom" dataDxfId="15"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="QuestDungeon" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="QPortal" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="QCardChange" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="QPiece" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="QMerchant" dataDxfId="10"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="QDoctor" dataDxfId="9"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="QAngel" dataDxfId="8"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Func" dataDxfId="7"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Url" dataDxfId="6"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="TilePath" dataDxfId="5"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Icon" dataDxfId="4"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="IconX" dataDxfId="3"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="IconY" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="18"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Type" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Level" dataDxfId="16"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="ReviveScene" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Quest" dataDxfId="14"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="QuestRandom" dataDxfId="13"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="QuestDungeon" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="QPortal" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="QCardChange" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="QPiece" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="QMerchant" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="QDoctor" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="QAngel" dataDxfId="6"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Func" dataDxfId="5"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Url" dataDxfId="4"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="TilePath" dataDxfId="3"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Icon" dataDxfId="2"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="IconX" dataDxfId="1"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="IconY" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2591,148 +2601,149 @@
   <dimension ref="A1:T35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="11.125" customWidth="1"/>
-    <col min="2" max="2" width="10.625" customWidth="1"/>
-    <col min="3" max="3" width="5.125" customWidth="1"/>
-    <col min="4" max="4" width="4.375" customWidth="1"/>
-    <col min="5" max="5" width="9" customWidth="1"/>
-    <col min="6" max="6" width="52.875" customWidth="1"/>
-    <col min="7" max="7" width="23.625" customWidth="1"/>
-    <col min="8" max="8" width="50.875" customWidth="1"/>
-    <col min="9" max="14" width="3.125" customWidth="1"/>
-    <col min="15" max="15" width="6.625" customWidth="1"/>
-    <col min="16" max="16" width="9.75" customWidth="1"/>
-    <col min="17" max="17" width="9.5" customWidth="1"/>
-    <col min="18" max="18" width="7.25" customWidth="1"/>
-    <col min="19" max="20" width="6" customWidth="1"/>
+    <col min="1" max="1" width="11.125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="10.625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="5.125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="4.375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="9" style="5" customWidth="1"/>
+    <col min="6" max="6" width="52.875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="23.625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="50.875" style="5" customWidth="1"/>
+    <col min="9" max="14" width="3.125" style="5" customWidth="1"/>
+    <col min="15" max="15" width="6.625" style="5" customWidth="1"/>
+    <col min="16" max="16" width="9.75" style="5" customWidth="1"/>
+    <col min="17" max="17" width="9.5" style="5" customWidth="1"/>
+    <col min="18" max="18" width="7.25" style="5" customWidth="1"/>
+    <col min="19" max="20" width="6" style="5" customWidth="1"/>
+    <col min="21" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="N1" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="Q1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="R1" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="S1" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="T1" s="4" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="O2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="P2" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="Q2" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="R2" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="S2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="T2" s="9" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2799,640 +2810,640 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A4" s="15">
+      <c r="A4" s="12">
         <v>13010001</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="13">
         <v>2</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="13">
         <v>1</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="13">
         <v>13010001</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="G4" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9">
+      <c r="G4" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13">
         <v>1</v>
       </c>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9" t="s">
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="Q4" s="9" t="s">
+      <c r="Q4" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="R4" s="9" t="s">
+      <c r="R4" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="S4" s="9">
+      <c r="S4" s="13">
         <v>1348</v>
       </c>
-      <c r="T4" s="9">
+      <c r="T4" s="13">
         <v>611</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A5" s="15">
+      <c r="A5" s="12">
         <v>13010002</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="13">
         <v>2</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="13">
         <v>2</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="13">
         <v>13010001</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9">
+      <c r="H5" s="13"/>
+      <c r="I5" s="13">
         <v>1</v>
       </c>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9">
+      <c r="J5" s="13"/>
+      <c r="K5" s="13">
         <v>1</v>
       </c>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9">
+      <c r="L5" s="13"/>
+      <c r="M5" s="13">
         <v>1</v>
       </c>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="9" t="s">
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="Q5" s="9" t="s">
+      <c r="Q5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="R5" s="9" t="s">
+      <c r="R5" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="S5" s="9">
+      <c r="S5" s="13">
         <v>1279</v>
       </c>
-      <c r="T5" s="9">
+      <c r="T5" s="13">
         <v>571</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A6" s="15">
+      <c r="A6" s="12">
         <v>13010004</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="13">
         <v>2</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="13">
         <v>5</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="13">
         <v>13010006</v>
       </c>
-      <c r="F6" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9">
+      <c r="F6" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13">
         <v>1</v>
       </c>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9">
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13">
         <v>1</v>
       </c>
-      <c r="M6" s="9"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="9" t="s">
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="Q6" s="9" t="s">
+      <c r="Q6" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="R6" s="9" t="s">
+      <c r="R6" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="S6" s="9">
+      <c r="S6" s="13">
         <v>1148</v>
       </c>
-      <c r="T6" s="9">
+      <c r="T6" s="13">
         <v>351</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A7" s="15">
+      <c r="A7" s="12">
         <v>13010005</v>
       </c>
-      <c r="B7" s="15" t="s">
-        <v>189</v>
-      </c>
-      <c r="C7" s="9">
+      <c r="B7" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="C7" s="13">
         <v>2</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="13">
         <v>8</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="13">
         <v>13010006</v>
       </c>
-      <c r="F7" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9">
+      <c r="F7" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13">
         <v>1</v>
       </c>
-      <c r="J7" s="9">
+      <c r="J7" s="13">
         <v>1</v>
       </c>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="9" t="s">
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="Q7" s="9" t="s">
+      <c r="Q7" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="R7" s="9" t="s">
+      <c r="R7" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="S7" s="9">
+      <c r="S7" s="13">
         <v>1386</v>
       </c>
-      <c r="T7" s="9">
+      <c r="T7" s="13">
         <v>339</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A8" s="15">
+      <c r="A8" s="12">
         <v>13010006</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="13">
         <v>1</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="13">
         <v>3</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="13">
         <v>13010006</v>
       </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
-      <c r="P8" s="9" t="s">
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="Q8" s="9" t="s">
+      <c r="Q8" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="R8" s="9" t="s">
+      <c r="R8" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="S8" s="9">
+      <c r="S8" s="13">
         <v>1232</v>
       </c>
-      <c r="T8" s="9">
+      <c r="T8" s="13">
         <v>506</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A9" s="15">
+      <c r="A9" s="12">
         <v>13010007</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="13">
         <v>2</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="13">
         <v>7</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="13">
         <v>13010006</v>
       </c>
-      <c r="F9" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9">
+      <c r="F9" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13">
         <v>1</v>
       </c>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9">
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13">
         <v>1</v>
       </c>
-      <c r="M9" s="9">
+      <c r="M9" s="13">
         <v>1</v>
       </c>
-      <c r="N9" s="9"/>
-      <c r="O9" s="9"/>
-      <c r="P9" s="9" t="s">
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="Q9" s="9" t="s">
+      <c r="Q9" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="R9" s="9" t="s">
+      <c r="R9" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="S9" s="9">
+      <c r="S9" s="13">
         <v>1431</v>
       </c>
-      <c r="T9" s="9">
+      <c r="T9" s="13">
         <v>440</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A10" s="15">
+      <c r="A10" s="12">
         <v>13010009</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="13">
         <v>2</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="13">
         <v>4</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="13">
         <v>13010006</v>
       </c>
-      <c r="F10" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="G10" s="9" t="s">
+      <c r="F10" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="G10" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9">
+      <c r="H10" s="13"/>
+      <c r="I10" s="13">
         <v>1</v>
       </c>
-      <c r="J10" s="9">
+      <c r="J10" s="13">
         <v>1</v>
       </c>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9">
+      <c r="K10" s="13"/>
+      <c r="L10" s="13">
         <v>1</v>
       </c>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="9" t="s">
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="Q10" s="9" t="s">
+      <c r="Q10" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="R10" s="9" t="s">
+      <c r="R10" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="S10" s="9">
+      <c r="S10" s="13">
         <v>1332</v>
       </c>
-      <c r="T10" s="9">
+      <c r="T10" s="13">
         <v>484</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A11" s="15">
+      <c r="A11" s="12">
         <v>13010010</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="13">
         <v>2</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="13">
         <v>13010006</v>
       </c>
-      <c r="F11" s="9" t="s">
-        <v>188</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9">
+      <c r="F11" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13">
         <v>1</v>
       </c>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="9">
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13">
         <v>1</v>
       </c>
-      <c r="O11" s="9"/>
-      <c r="P11" s="9" t="s">
+      <c r="O11" s="13"/>
+      <c r="P11" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="Q11" s="9" t="s">
+      <c r="Q11" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="R11" s="9" t="s">
+      <c r="R11" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="S11" s="9">
+      <c r="S11" s="13">
         <v>1441</v>
       </c>
-      <c r="T11" s="9">
+      <c r="T11" s="13">
         <v>527</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A12" s="15">
+      <c r="A12" s="12">
         <v>13010011</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="13">
         <v>2</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="13">
         <v>12</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="13">
         <v>13010006</v>
       </c>
-      <c r="F12" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="G12" s="9" t="s">
+      <c r="F12" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="G12" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9">
+      <c r="H12" s="13"/>
+      <c r="I12" s="13">
         <v>1</v>
       </c>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9">
+      <c r="J12" s="13"/>
+      <c r="K12" s="13">
         <v>1</v>
       </c>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="9" t="s">
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="13"/>
+      <c r="P12" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="Q12" s="9" t="s">
+      <c r="Q12" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="R12" s="9" t="s">
+      <c r="R12" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="S12" s="9">
+      <c r="S12" s="13">
         <v>1574</v>
       </c>
-      <c r="T12" s="9">
+      <c r="T12" s="13">
         <v>373</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A13" s="15">
+      <c r="A13" s="12">
         <v>13010012</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="13">
         <v>2</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="13">
         <v>3</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="13">
         <v>13010006</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="F13" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="G13" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9">
+      <c r="H13" s="13"/>
+      <c r="I13" s="13">
         <v>1</v>
       </c>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="9" t="s">
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
+      <c r="P13" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="Q13" s="9" t="s">
+      <c r="Q13" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="R13" s="9" t="s">
+      <c r="R13" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="S13" s="9">
+      <c r="S13" s="13">
         <v>1251</v>
       </c>
-      <c r="T13" s="9">
+      <c r="T13" s="13">
         <v>432</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A14" s="15">
+      <c r="A14" s="12">
         <v>13010013</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="13">
         <v>2</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="13">
         <v>6</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="13">
         <v>13010006</v>
       </c>
-      <c r="F14" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="G14" s="9" t="s">
+      <c r="F14" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="G14" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9">
+      <c r="H14" s="13"/>
+      <c r="I14" s="13">
         <v>1</v>
       </c>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="9" t="s">
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
+      <c r="P14" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="Q14" s="9" t="s">
+      <c r="Q14" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="R14" s="9" t="s">
+      <c r="R14" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="S14" s="9">
+      <c r="S14" s="13">
         <v>1250</v>
       </c>
-      <c r="T14" s="9">
+      <c r="T14" s="13">
         <v>338</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A15" s="15">
+      <c r="A15" s="12">
         <v>13010014</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="13">
         <v>2</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="13">
         <v>14</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="13">
         <v>13010006</v>
       </c>
-      <c r="F15" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9">
+      <c r="F15" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13">
         <v>1</v>
       </c>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="9"/>
-      <c r="M15" s="9">
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13">
         <v>1</v>
       </c>
-      <c r="N15" s="9">
+      <c r="N15" s="13">
         <v>1</v>
       </c>
-      <c r="O15" s="9"/>
-      <c r="P15" s="9" t="s">
+      <c r="O15" s="13"/>
+      <c r="P15" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="Q15" s="9" t="s">
+      <c r="Q15" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="R15" s="9" t="s">
+      <c r="R15" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="S15" s="9">
+      <c r="S15" s="13">
         <v>1550</v>
       </c>
-      <c r="T15" s="9">
+      <c r="T15" s="13">
         <v>505</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A16" s="15">
+      <c r="A16" s="12">
         <v>13010015</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="C16" s="14">
+      <c r="C16" s="15">
         <v>2</v>
       </c>
-      <c r="D16" s="14">
+      <c r="D16" s="15">
         <v>6</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="13">
         <v>13010006</v>
       </c>
-      <c r="F16" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="H16" s="9"/>
-      <c r="I16" s="14">
+      <c r="F16" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="H16" s="13"/>
+      <c r="I16" s="15">
         <v>1</v>
       </c>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="14"/>
-      <c r="P16" s="12" t="s">
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="15"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="15"/>
+      <c r="O16" s="15"/>
+      <c r="P16" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="Q16" s="12" t="s">
+      <c r="Q16" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="R16" s="14"/>
-      <c r="S16" s="14"/>
-      <c r="T16" s="14"/>
+      <c r="R16" s="15"/>
+      <c r="S16" s="15"/>
+      <c r="T16" s="15"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A17" s="16">
@@ -3441,38 +3452,38 @@
       <c r="B17" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17" s="13">
         <v>1</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D17" s="13">
         <v>16</v>
       </c>
-      <c r="E17" s="9">
+      <c r="E17" s="13">
         <v>13010101</v>
       </c>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="9"/>
-      <c r="P17" s="9" t="s">
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="13"/>
+      <c r="O17" s="13"/>
+      <c r="P17" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="Q17" s="9" t="s">
+      <c r="Q17" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="R17" s="9" t="s">
+      <c r="R17" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="S17" s="9">
+      <c r="S17" s="13">
         <v>919</v>
       </c>
-      <c r="T17" s="9">
+      <c r="T17" s="13">
         <v>534</v>
       </c>
     </row>
@@ -3483,46 +3494,46 @@
       <c r="B18" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C18" s="13">
         <v>2</v>
       </c>
-      <c r="D18" s="9">
+      <c r="D18" s="13">
         <v>16</v>
       </c>
-      <c r="E18" s="9">
+      <c r="E18" s="13">
         <v>13010101</v>
       </c>
-      <c r="F18" s="9" t="s">
+      <c r="F18" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="G18" s="9" t="s">
+      <c r="G18" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9">
+      <c r="H18" s="13"/>
+      <c r="I18" s="13">
         <v>1</v>
       </c>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9">
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13">
         <v>1</v>
       </c>
-      <c r="M18" s="9"/>
-      <c r="N18" s="9"/>
-      <c r="O18" s="9"/>
-      <c r="P18" s="9" t="s">
+      <c r="M18" s="13"/>
+      <c r="N18" s="13"/>
+      <c r="O18" s="13"/>
+      <c r="P18" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="Q18" s="9" t="s">
+      <c r="Q18" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="R18" s="9" t="s">
+      <c r="R18" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="S18" s="9">
+      <c r="S18" s="13">
         <v>1040</v>
       </c>
-      <c r="T18" s="9">
+      <c r="T18" s="13">
         <v>538</v>
       </c>
     </row>
@@ -3533,44 +3544,44 @@
       <c r="B19" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C19" s="13">
         <v>2</v>
       </c>
-      <c r="D19" s="9">
+      <c r="D19" s="13">
         <v>19</v>
       </c>
-      <c r="E19" s="9">
+      <c r="E19" s="13">
         <v>13010101</v>
       </c>
-      <c r="F19" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="G19" s="9" t="s">
+      <c r="F19" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="G19" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9">
+      <c r="H19" s="13"/>
+      <c r="I19" s="13">
         <v>1</v>
       </c>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="9"/>
-      <c r="O19" s="9"/>
-      <c r="P19" s="9" t="s">
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="13"/>
+      <c r="P19" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="Q19" s="9" t="s">
+      <c r="Q19" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="R19" s="9" t="s">
+      <c r="R19" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="S19" s="9">
+      <c r="S19" s="13">
         <v>1213</v>
       </c>
-      <c r="T19" s="9">
+      <c r="T19" s="13">
         <v>655</v>
       </c>
     </row>
@@ -3581,46 +3592,46 @@
       <c r="B20" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C20" s="13">
         <v>2</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20" s="13">
         <v>18</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E20" s="13">
         <v>13010101</v>
       </c>
-      <c r="F20" s="9" t="s">
+      <c r="F20" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="G20" s="9" t="s">
+      <c r="G20" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9">
+      <c r="H20" s="13"/>
+      <c r="I20" s="13">
         <v>1</v>
       </c>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9">
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13">
         <v>1</v>
       </c>
-      <c r="N20" s="9"/>
-      <c r="O20" s="9"/>
-      <c r="P20" s="9" t="s">
+      <c r="N20" s="13"/>
+      <c r="O20" s="13"/>
+      <c r="P20" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="Q20" s="9" t="s">
+      <c r="Q20" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="R20" s="9" t="s">
+      <c r="R20" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="S20" s="9">
+      <c r="S20" s="13">
         <v>1149</v>
       </c>
-      <c r="T20" s="9">
+      <c r="T20" s="13">
         <v>584</v>
       </c>
     </row>
@@ -3631,42 +3642,42 @@
       <c r="B21" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="9">
+      <c r="C21" s="13">
         <v>2</v>
       </c>
-      <c r="D21" s="9">
+      <c r="D21" s="13">
         <v>20</v>
       </c>
-      <c r="E21" s="9">
+      <c r="E21" s="13">
         <v>13010101</v>
       </c>
-      <c r="F21" s="9" t="s">
+      <c r="F21" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="G21" s="9" t="s">
+      <c r="G21" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
-      <c r="L21" s="9"/>
-      <c r="M21" s="9"/>
-      <c r="N21" s="9"/>
-      <c r="O21" s="9"/>
-      <c r="P21" s="9" t="s">
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="13"/>
+      <c r="O21" s="13"/>
+      <c r="P21" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="Q21" s="9" t="s">
+      <c r="Q21" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="R21" s="9" t="s">
+      <c r="R21" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="S21" s="9">
+      <c r="S21" s="13">
         <v>840</v>
       </c>
-      <c r="T21" s="9">
+      <c r="T21" s="13">
         <v>444</v>
       </c>
     </row>
@@ -3677,369 +3688,369 @@
       <c r="B22" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="C22" s="9">
+      <c r="C22" s="13">
         <v>2</v>
       </c>
-      <c r="D22" s="9">
+      <c r="D22" s="13">
         <v>15</v>
       </c>
-      <c r="E22" s="9">
+      <c r="E22" s="13">
         <v>13010016</v>
       </c>
-      <c r="F22" s="9" t="s">
+      <c r="F22" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="G22" s="9" t="s">
+      <c r="G22" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9">
+      <c r="H22" s="13"/>
+      <c r="I22" s="13">
         <v>1</v>
       </c>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
-      <c r="L22" s="9"/>
-      <c r="M22" s="9"/>
-      <c r="N22" s="9">
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="13">
         <v>1</v>
       </c>
-      <c r="O22" s="9"/>
-      <c r="P22" s="9" t="s">
+      <c r="O22" s="13"/>
+      <c r="P22" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="Q22" s="9" t="s">
+      <c r="Q22" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="R22" s="9" t="s">
+      <c r="R22" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="S22" s="9">
+      <c r="S22" s="13">
         <v>1067</v>
       </c>
-      <c r="T22" s="9">
+      <c r="T22" s="13">
         <v>445</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A23" s="13">
+      <c r="A23" s="17">
         <v>13020001</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="C23" s="13">
+      <c r="C23" s="17">
         <v>3</v>
       </c>
-      <c r="D23" s="9">
+      <c r="D23" s="13">
         <v>3</v>
       </c>
-      <c r="E23" s="9">
+      <c r="E23" s="13">
         <v>13010002</v>
       </c>
-      <c r="F23" s="9" t="s">
+      <c r="F23" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9" t="s">
+      <c r="G23" s="13"/>
+      <c r="H23" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
-      <c r="L23" s="9"/>
-      <c r="M23" s="9"/>
-      <c r="N23" s="9"/>
-      <c r="O23" s="9"/>
-      <c r="P23" s="9" t="s">
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
+      <c r="N23" s="13"/>
+      <c r="O23" s="13"/>
+      <c r="P23" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="Q23" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="R23" s="9"/>
-      <c r="S23" s="9"/>
-      <c r="T23" s="9"/>
+      <c r="Q23" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="R23" s="13"/>
+      <c r="S23" s="13"/>
+      <c r="T23" s="13"/>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A24" s="13">
+      <c r="A24" s="17">
         <v>13020002</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="C24" s="13">
+      <c r="C24" s="17">
         <v>3</v>
       </c>
-      <c r="D24" s="9">
+      <c r="D24" s="13">
         <v>3</v>
       </c>
-      <c r="E24" s="9">
+      <c r="E24" s="13">
         <v>13010002</v>
       </c>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="9"/>
-      <c r="M24" s="9"/>
-      <c r="N24" s="9"/>
-      <c r="O24" s="9"/>
-      <c r="P24" s="9" t="s">
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="13"/>
+      <c r="N24" s="13"/>
+      <c r="O24" s="13"/>
+      <c r="P24" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="Q24" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="R24" s="9"/>
-      <c r="S24" s="9"/>
-      <c r="T24" s="9"/>
+      <c r="Q24" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="R24" s="13"/>
+      <c r="S24" s="13"/>
+      <c r="T24" s="13"/>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A25" s="13">
+      <c r="A25" s="17">
         <v>13020011</v>
       </c>
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="C25" s="13">
+      <c r="C25" s="17">
         <v>3</v>
       </c>
-      <c r="D25" s="9">
+      <c r="D25" s="13">
         <v>8</v>
       </c>
-      <c r="E25" s="9">
+      <c r="E25" s="13">
         <v>13010007</v>
       </c>
-      <c r="F25" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="9"/>
-      <c r="J25" s="9"/>
-      <c r="K25" s="9"/>
-      <c r="L25" s="9"/>
-      <c r="M25" s="9"/>
-      <c r="N25" s="9"/>
-      <c r="O25" s="9"/>
-      <c r="P25" s="9" t="s">
+      <c r="F25" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="13"/>
+      <c r="N25" s="13"/>
+      <c r="O25" s="13"/>
+      <c r="P25" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="Q25" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="R25" s="9"/>
-      <c r="S25" s="9"/>
-      <c r="T25" s="9"/>
+      <c r="Q25" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="R25" s="13"/>
+      <c r="S25" s="13"/>
+      <c r="T25" s="13"/>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A26" s="13">
+      <c r="A26" s="17">
         <v>13020012</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="C26" s="13">
+      <c r="C26" s="17">
         <v>3</v>
       </c>
-      <c r="D26" s="9">
+      <c r="D26" s="13">
         <v>8</v>
       </c>
-      <c r="E26" s="9">
+      <c r="E26" s="13">
         <v>13010007</v>
       </c>
-      <c r="F26" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
-      <c r="J26" s="9"/>
-      <c r="K26" s="9"/>
-      <c r="L26" s="9"/>
-      <c r="M26" s="9"/>
-      <c r="N26" s="9"/>
-      <c r="O26" s="9"/>
-      <c r="P26" s="9" t="s">
+      <c r="F26" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="13"/>
+      <c r="M26" s="13"/>
+      <c r="N26" s="13"/>
+      <c r="O26" s="13"/>
+      <c r="P26" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="Q26" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="R26" s="9"/>
-      <c r="S26" s="9"/>
-      <c r="T26" s="9"/>
+      <c r="Q26" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="R26" s="13"/>
+      <c r="S26" s="13"/>
+      <c r="T26" s="13"/>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A27" s="13">
+      <c r="A27" s="17">
         <v>13020013</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="C27" s="13">
+      <c r="C27" s="17">
         <v>3</v>
       </c>
-      <c r="D27" s="9">
+      <c r="D27" s="13">
         <v>8</v>
       </c>
-      <c r="E27" s="9">
+      <c r="E27" s="13">
         <v>13010007</v>
       </c>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="9"/>
-      <c r="L27" s="9"/>
-      <c r="M27" s="9"/>
-      <c r="N27" s="9"/>
-      <c r="O27" s="9"/>
-      <c r="P27" s="9" t="s">
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="13"/>
+      <c r="N27" s="13"/>
+      <c r="O27" s="13"/>
+      <c r="P27" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="Q27" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="R27" s="9"/>
-      <c r="S27" s="9"/>
-      <c r="T27" s="9"/>
+      <c r="Q27" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="R27" s="13"/>
+      <c r="S27" s="13"/>
+      <c r="T27" s="13"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A28" s="13">
+      <c r="A28" s="17">
         <v>13020021</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="17" t="s">
         <v>135</v>
       </c>
-      <c r="C28" s="13">
+      <c r="C28" s="17">
         <v>3</v>
       </c>
-      <c r="D28" s="9">
+      <c r="D28" s="13">
         <v>5</v>
       </c>
-      <c r="E28" s="9">
+      <c r="E28" s="13">
         <v>13010004</v>
       </c>
-      <c r="F28" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="G28" s="9" t="s">
+      <c r="F28" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="G28" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="H28" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="I28" s="9"/>
-      <c r="J28" s="9"/>
-      <c r="K28" s="9"/>
-      <c r="L28" s="9"/>
-      <c r="M28" s="9"/>
-      <c r="N28" s="9"/>
-      <c r="O28" s="9"/>
-      <c r="P28" s="9" t="s">
+      <c r="H28" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="I28" s="13"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="13"/>
+      <c r="M28" s="13"/>
+      <c r="N28" s="13"/>
+      <c r="O28" s="13"/>
+      <c r="P28" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="Q28" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="R28" s="9"/>
-      <c r="S28" s="9"/>
-      <c r="T28" s="9"/>
+      <c r="Q28" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="R28" s="13"/>
+      <c r="S28" s="13"/>
+      <c r="T28" s="13"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A29" s="13">
+      <c r="A29" s="17">
         <v>13020022</v>
       </c>
-      <c r="B29" s="13" t="s">
+      <c r="B29" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="C29" s="13">
+      <c r="C29" s="17">
         <v>3</v>
       </c>
-      <c r="D29" s="9">
+      <c r="D29" s="13">
         <v>5</v>
       </c>
-      <c r="E29" s="9">
+      <c r="E29" s="13">
         <v>13010004</v>
       </c>
-      <c r="F29" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="G29" s="9" t="s">
+      <c r="F29" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="G29" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="H29" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="I29" s="9"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="9"/>
-      <c r="L29" s="9"/>
-      <c r="M29" s="9"/>
-      <c r="N29" s="9"/>
-      <c r="O29" s="9"/>
-      <c r="P29" s="9" t="s">
+      <c r="H29" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="I29" s="13"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="13"/>
+      <c r="M29" s="13"/>
+      <c r="N29" s="13"/>
+      <c r="O29" s="13"/>
+      <c r="P29" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="Q29" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="R29" s="9"/>
-      <c r="S29" s="9"/>
-      <c r="T29" s="9"/>
+      <c r="Q29" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="R29" s="13"/>
+      <c r="S29" s="13"/>
+      <c r="T29" s="13"/>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A30" s="13">
+      <c r="A30" s="17">
         <v>13020023</v>
       </c>
-      <c r="B30" s="13" t="s">
+      <c r="B30" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="C30" s="13">
+      <c r="C30" s="17">
         <v>3</v>
       </c>
-      <c r="D30" s="9">
+      <c r="D30" s="13">
         <v>5</v>
       </c>
-      <c r="E30" s="9">
+      <c r="E30" s="13">
         <v>13010004</v>
       </c>
-      <c r="F30" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="G30" s="9" t="s">
+      <c r="F30" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="G30" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="H30" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="I30" s="9"/>
-      <c r="J30" s="9"/>
-      <c r="K30" s="9"/>
-      <c r="L30" s="9"/>
-      <c r="M30" s="9"/>
-      <c r="N30" s="9"/>
-      <c r="O30" s="9"/>
-      <c r="P30" s="9" t="s">
+      <c r="H30" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="I30" s="13"/>
+      <c r="J30" s="13"/>
+      <c r="K30" s="13"/>
+      <c r="L30" s="13"/>
+      <c r="M30" s="13"/>
+      <c r="N30" s="13"/>
+      <c r="O30" s="13"/>
+      <c r="P30" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Q30" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="R30" s="9"/>
-      <c r="S30" s="9"/>
-      <c r="T30" s="9"/>
+      <c r="Q30" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="R30" s="13"/>
+      <c r="S30" s="13"/>
+      <c r="T30" s="13"/>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A31" s="18">
         <v>13020031</v>
       </c>
-      <c r="B31" s="13" t="s">
-        <v>190</v>
+      <c r="B31" s="17" t="s">
+        <v>189</v>
       </c>
       <c r="C31" s="18">
         <v>3</v>
@@ -4052,7 +4063,9 @@
       </c>
       <c r="F31" s="19"/>
       <c r="G31" s="19"/>
-      <c r="H31" s="19"/>
+      <c r="H31" s="19" t="s">
+        <v>201</v>
+      </c>
       <c r="I31" s="19"/>
       <c r="J31" s="19"/>
       <c r="K31" s="19"/>
@@ -4060,11 +4073,11 @@
       <c r="M31" s="19"/>
       <c r="N31" s="19"/>
       <c r="O31" s="19"/>
-      <c r="P31" s="9" t="s">
-        <v>191</v>
+      <c r="P31" s="13" t="s">
+        <v>190</v>
       </c>
       <c r="Q31" s="19" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="R31" s="19"/>
       <c r="S31" s="19"/>
@@ -4074,8 +4087,8 @@
       <c r="A32" s="18">
         <v>13020032</v>
       </c>
-      <c r="B32" s="13" t="s">
-        <v>192</v>
+      <c r="B32" s="17" t="s">
+        <v>191</v>
       </c>
       <c r="C32" s="18">
         <v>3</v>
@@ -4088,7 +4101,9 @@
       </c>
       <c r="F32" s="19"/>
       <c r="G32" s="19"/>
-      <c r="H32" s="19"/>
+      <c r="H32" s="19" t="s">
+        <v>202</v>
+      </c>
       <c r="I32" s="19"/>
       <c r="J32" s="19"/>
       <c r="K32" s="19"/>
@@ -4096,11 +4111,11 @@
       <c r="M32" s="19"/>
       <c r="N32" s="19"/>
       <c r="O32" s="19"/>
-      <c r="P32" s="9" t="s">
-        <v>191</v>
+      <c r="P32" s="13" t="s">
+        <v>190</v>
       </c>
       <c r="Q32" s="19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="R32" s="19"/>
       <c r="S32" s="19"/>
@@ -4110,8 +4125,8 @@
       <c r="A33" s="18">
         <v>13020033</v>
       </c>
-      <c r="B33" s="13" t="s">
-        <v>193</v>
+      <c r="B33" s="17" t="s">
+        <v>192</v>
       </c>
       <c r="C33" s="18">
         <v>3</v>
@@ -4124,7 +4139,9 @@
       </c>
       <c r="F33" s="19"/>
       <c r="G33" s="19"/>
-      <c r="H33" s="19"/>
+      <c r="H33" s="19" t="s">
+        <v>203</v>
+      </c>
       <c r="I33" s="19"/>
       <c r="J33" s="19"/>
       <c r="K33" s="19"/>
@@ -4132,11 +4149,11 @@
       <c r="M33" s="19"/>
       <c r="N33" s="19"/>
       <c r="O33" s="19"/>
-      <c r="P33" s="9" t="s">
-        <v>191</v>
+      <c r="P33" s="13" t="s">
+        <v>190</v>
       </c>
       <c r="Q33" s="19" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="R33" s="20"/>
       <c r="S33" s="20"/>
@@ -4146,8 +4163,8 @@
       <c r="A34" s="18">
         <v>13020034</v>
       </c>
-      <c r="B34" s="13" t="s">
-        <v>194</v>
+      <c r="B34" s="17" t="s">
+        <v>193</v>
       </c>
       <c r="C34" s="18">
         <v>3</v>
@@ -4160,7 +4177,9 @@
       </c>
       <c r="F34" s="19"/>
       <c r="G34" s="19"/>
-      <c r="H34" s="19"/>
+      <c r="H34" s="19" t="s">
+        <v>204</v>
+      </c>
       <c r="I34" s="19"/>
       <c r="J34" s="19"/>
       <c r="K34" s="19"/>
@@ -4168,11 +4187,11 @@
       <c r="M34" s="19"/>
       <c r="N34" s="19"/>
       <c r="O34" s="19"/>
-      <c r="P34" s="9" t="s">
-        <v>191</v>
+      <c r="P34" s="13" t="s">
+        <v>190</v>
       </c>
       <c r="Q34" s="19" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="R34" s="20"/>
       <c r="S34" s="20"/>
@@ -4182,8 +4201,8 @@
       <c r="A35" s="18">
         <v>13020035</v>
       </c>
-      <c r="B35" s="13" t="s">
-        <v>195</v>
+      <c r="B35" s="17" t="s">
+        <v>194</v>
       </c>
       <c r="C35" s="18">
         <v>3</v>
@@ -4196,7 +4215,9 @@
       </c>
       <c r="F35" s="19"/>
       <c r="G35" s="19"/>
-      <c r="H35" s="19"/>
+      <c r="H35" s="19" t="s">
+        <v>205</v>
+      </c>
       <c r="I35" s="19"/>
       <c r="J35" s="19"/>
       <c r="K35" s="19"/>
@@ -4204,11 +4225,11 @@
       <c r="M35" s="19"/>
       <c r="N35" s="19"/>
       <c r="O35" s="19"/>
-      <c r="P35" s="9" t="s">
-        <v>191</v>
+      <c r="P35" s="13" t="s">
+        <v>190</v>
       </c>
       <c r="Q35" s="19" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="R35" s="20"/>
       <c r="S35" s="20"/>
@@ -4217,17 +4238,17 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="I4:N35">
-    <cfRule type="cellIs" dxfId="27" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4">
-    <cfRule type="cellIs" dxfId="26" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4:H35">
-    <cfRule type="containsBlanks" dxfId="25" priority="5">
+    <cfRule type="containsBlanks" dxfId="23" priority="5">
       <formula>LEN(TRIM(F4))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
add a new event spinbox
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Scene.xlsx
+++ b/ConfigData/Xlsx/Scene.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Scene" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -347,10 +347,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>met;30|treasure;25</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>类型</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -533,10 +529,6 @@
     <t>viliage3</t>
   </si>
   <si>
-    <t>hiddeway;35</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>forestfire;10|crystalball;35</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -673,10 +665,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>met;30|lighthouse;60|floatbottle;50</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>orehole;1|stone;2|sandflow;2</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -771,10 +759,6 @@
     <t>trees;8</t>
   </si>
   <si>
-    <t>wishwell;20</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>crystalball;55|wishwell;20</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -788,6 +772,22 @@
   </si>
   <si>
     <t>met;30|goblinhome;30|gamecook;20|wishwell;20</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|lighthouse;60|floatbottle;50|spinbox;30</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|treasure;25|spinbox;30</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>wishwell;20|spinbox;30</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>hiddeway;35|spinbox;35</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -2613,7 +2613,7 @@
   <dimension ref="A1:T35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2643,13 +2643,13 @@
         <v>16</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>30</v>
@@ -2658,7 +2658,7 @@
         <v>90</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>50</v>
@@ -2705,13 +2705,13 @@
         <v>14</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>13</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>87</v>
@@ -2767,13 +2767,13 @@
         <v>21</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>22</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>29</v>
@@ -2782,7 +2782,7 @@
         <v>92</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I3" s="11" t="s">
         <v>51</v>
@@ -2841,7 +2841,7 @@
         <v>89</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="H4" s="13"/>
       <c r="I4" s="13">
@@ -2854,7 +2854,7 @@
       <c r="N4" s="13"/>
       <c r="O4" s="13"/>
       <c r="P4" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Q4" s="13" t="s">
         <v>28</v>
@@ -2886,10 +2886,10 @@
         <v>13010001</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H5" s="13"/>
       <c r="I5" s="13">
@@ -2938,10 +2938,10 @@
         <v>13010006</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H6" s="13"/>
       <c r="I6" s="13">
@@ -2976,7 +2976,7 @@
         <v>13010005</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C7" s="13">
         <v>2</v>
@@ -2988,10 +2988,10 @@
         <v>13010006</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="H7" s="13"/>
       <c r="I7" s="13">
@@ -3006,7 +3006,7 @@
       <c r="N7" s="13"/>
       <c r="O7" s="13"/>
       <c r="P7" s="13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="Q7" s="13" t="s">
         <v>36</v>
@@ -3048,7 +3048,7 @@
       <c r="N8" s="13"/>
       <c r="O8" s="13"/>
       <c r="P8" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="Q8" s="13" t="s">
         <v>32</v>
@@ -3080,10 +3080,10 @@
         <v>13010006</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="H9" s="13"/>
       <c r="I9" s="13">
@@ -3100,7 +3100,7 @@
       <c r="N9" s="13"/>
       <c r="O9" s="13"/>
       <c r="P9" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Q9" s="13" t="s">
         <v>34</v>
@@ -3132,10 +3132,10 @@
         <v>13010006</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G10" s="21" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="H10" s="13"/>
       <c r="I10" s="13">
@@ -3152,10 +3152,10 @@
       <c r="N10" s="13"/>
       <c r="O10" s="13"/>
       <c r="P10" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="Q10" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="R10" s="13" t="s">
         <v>74</v>
@@ -3184,10 +3184,10 @@
         <v>13010006</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="G11" s="13" t="s">
-        <v>175</v>
+        <v>181</v>
+      </c>
+      <c r="G11" s="21" t="s">
+        <v>204</v>
       </c>
       <c r="H11" s="13"/>
       <c r="I11" s="13">
@@ -3202,7 +3202,7 @@
       </c>
       <c r="O11" s="13"/>
       <c r="P11" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="Q11" s="13" t="s">
         <v>38</v>
@@ -3234,10 +3234,10 @@
         <v>13010006</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H12" s="13"/>
       <c r="I12" s="13">
@@ -3252,7 +3252,7 @@
       <c r="N12" s="13"/>
       <c r="O12" s="13"/>
       <c r="P12" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Q12" s="13" t="s">
         <v>39</v>
@@ -3284,10 +3284,10 @@
         <v>13010006</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H13" s="13"/>
       <c r="I13" s="13">
@@ -3300,7 +3300,7 @@
       <c r="N13" s="13"/>
       <c r="O13" s="13"/>
       <c r="P13" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Q13" s="13" t="s">
         <v>33</v>
@@ -3332,10 +3332,10 @@
         <v>13010006</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H14" s="13"/>
       <c r="I14" s="13">
@@ -3348,7 +3348,7 @@
       <c r="N14" s="13"/>
       <c r="O14" s="13"/>
       <c r="P14" s="13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Q14" s="13" t="s">
         <v>37</v>
@@ -3380,10 +3380,10 @@
         <v>13010006</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H15" s="13"/>
       <c r="I15" s="13">
@@ -3400,7 +3400,7 @@
       </c>
       <c r="O15" s="13"/>
       <c r="P15" s="13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Q15" s="13" t="s">
         <v>40</v>
@@ -3420,7 +3420,7 @@
         <v>13010015</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C16" s="15">
         <v>2</v>
@@ -3432,10 +3432,10 @@
         <v>13010006</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G16" s="13" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H16" s="13"/>
       <c r="I16" s="15">
@@ -3448,10 +3448,10 @@
       <c r="N16" s="15"/>
       <c r="O16" s="15"/>
       <c r="P16" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q16" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="R16" s="15"/>
       <c r="S16" s="15"/>
@@ -3484,7 +3484,7 @@
       <c r="N17" s="13"/>
       <c r="O17" s="13"/>
       <c r="P17" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="Q17" s="13" t="s">
         <v>47</v>
@@ -3516,10 +3516,10 @@
         <v>13010101</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H18" s="13"/>
       <c r="I18" s="13">
@@ -3534,7 +3534,7 @@
       <c r="N18" s="13"/>
       <c r="O18" s="13"/>
       <c r="P18" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="Q18" s="13" t="s">
         <v>44</v>
@@ -3566,10 +3566,10 @@
         <v>13010101</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>176</v>
-      </c>
-      <c r="G19" s="13" t="s">
-        <v>93</v>
+        <v>173</v>
+      </c>
+      <c r="G19" s="21" t="s">
+        <v>205</v>
       </c>
       <c r="H19" s="13"/>
       <c r="I19" s="13">
@@ -3582,10 +3582,10 @@
       <c r="N19" s="13"/>
       <c r="O19" s="13"/>
       <c r="P19" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q19" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="R19" s="13" t="s">
         <v>68</v>
@@ -3614,10 +3614,10 @@
         <v>13010101</v>
       </c>
       <c r="F20" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G20" s="13" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H20" s="13"/>
       <c r="I20" s="13">
@@ -3632,7 +3632,7 @@
       <c r="N20" s="13"/>
       <c r="O20" s="13"/>
       <c r="P20" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q20" s="13" t="s">
         <v>46</v>
@@ -3667,7 +3667,7 @@
         <v>88</v>
       </c>
       <c r="G21" s="13" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H21" s="13"/>
       <c r="I21" s="13"/>
@@ -3678,7 +3678,7 @@
       <c r="N21" s="13"/>
       <c r="O21" s="13"/>
       <c r="P21" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="Q21" s="13" t="s">
         <v>48</v>
@@ -3698,7 +3698,7 @@
         <v>13010106</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C22" s="13">
         <v>2</v>
@@ -3710,10 +3710,10 @@
         <v>13010016</v>
       </c>
       <c r="F22" s="13" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G22" s="13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="H22" s="13"/>
       <c r="I22" s="13">
@@ -3728,7 +3728,7 @@
       </c>
       <c r="O22" s="13"/>
       <c r="P22" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="Q22" s="13" t="s">
         <v>43</v>
@@ -3748,7 +3748,7 @@
         <v>13020001</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C23" s="17">
         <v>3</v>
@@ -3760,11 +3760,11 @@
         <v>13010002</v>
       </c>
       <c r="F23" s="13" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G23" s="13"/>
       <c r="H23" s="13" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="I23" s="13"/>
       <c r="J23" s="13"/>
@@ -3774,10 +3774,10 @@
       <c r="N23" s="13"/>
       <c r="O23" s="13"/>
       <c r="P23" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Q23" s="13" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="R23" s="13"/>
       <c r="S23" s="13"/>
@@ -3788,7 +3788,7 @@
         <v>13020002</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C24" s="17">
         <v>3</v>
@@ -3810,10 +3810,10 @@
       <c r="N24" s="13"/>
       <c r="O24" s="13"/>
       <c r="P24" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="Q24" s="13" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="R24" s="13"/>
       <c r="S24" s="13"/>
@@ -3824,7 +3824,7 @@
         <v>13020011</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C25" s="17">
         <v>3</v>
@@ -3836,10 +3836,10 @@
         <v>13010007</v>
       </c>
       <c r="F25" s="13" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="G25" s="21" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="H25" s="13"/>
       <c r="I25" s="13"/>
@@ -3850,10 +3850,10 @@
       <c r="N25" s="13"/>
       <c r="O25" s="13"/>
       <c r="P25" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Q25" s="13" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="R25" s="13"/>
       <c r="S25" s="13"/>
@@ -3864,7 +3864,7 @@
         <v>13020012</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C26" s="17">
         <v>3</v>
@@ -3876,7 +3876,7 @@
         <v>13010007</v>
       </c>
       <c r="F26" s="13" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G26" s="13"/>
       <c r="H26" s="13"/>
@@ -3888,10 +3888,10 @@
       <c r="N26" s="13"/>
       <c r="O26" s="13"/>
       <c r="P26" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="Q26" s="13" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="R26" s="13"/>
       <c r="S26" s="13"/>
@@ -3902,7 +3902,7 @@
         <v>13020013</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C27" s="17">
         <v>3</v>
@@ -3924,10 +3924,10 @@
       <c r="N27" s="13"/>
       <c r="O27" s="13"/>
       <c r="P27" s="13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="Q27" s="13" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="R27" s="13"/>
       <c r="S27" s="13"/>
@@ -3938,7 +3938,7 @@
         <v>13020021</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C28" s="17">
         <v>3</v>
@@ -3950,13 +3950,13 @@
         <v>13010004</v>
       </c>
       <c r="F28" s="13" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G28" s="21" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="H28" s="13" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="I28" s="13"/>
       <c r="J28" s="13"/>
@@ -3966,10 +3966,10 @@
       <c r="N28" s="13"/>
       <c r="O28" s="13"/>
       <c r="P28" s="13" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="Q28" s="13" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="R28" s="13"/>
       <c r="S28" s="13"/>
@@ -3980,7 +3980,7 @@
         <v>13020022</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C29" s="17">
         <v>3</v>
@@ -3992,13 +3992,13 @@
         <v>13010004</v>
       </c>
       <c r="F29" s="13" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G29" s="21" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="H29" s="13" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I29" s="13"/>
       <c r="J29" s="13"/>
@@ -4008,10 +4008,10 @@
       <c r="N29" s="13"/>
       <c r="O29" s="13"/>
       <c r="P29" s="13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q29" s="13" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="R29" s="13"/>
       <c r="S29" s="13"/>
@@ -4022,7 +4022,7 @@
         <v>13020023</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C30" s="17">
         <v>3</v>
@@ -4034,13 +4034,13 @@
         <v>13010004</v>
       </c>
       <c r="F30" s="13" t="s">
-        <v>161</v>
-      </c>
-      <c r="G30" s="13" t="s">
-        <v>140</v>
+        <v>159</v>
+      </c>
+      <c r="G30" s="21" t="s">
+        <v>207</v>
       </c>
       <c r="H30" s="13" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I30" s="13"/>
       <c r="J30" s="13"/>
@@ -4050,10 +4050,10 @@
       <c r="N30" s="13"/>
       <c r="O30" s="13"/>
       <c r="P30" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q30" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="R30" s="13"/>
       <c r="S30" s="13"/>
@@ -4064,7 +4064,7 @@
         <v>13020031</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C31" s="18">
         <v>3</v>
@@ -4078,7 +4078,7 @@
       <c r="F31" s="19"/>
       <c r="G31" s="19"/>
       <c r="H31" s="19" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="I31" s="19"/>
       <c r="J31" s="19"/>
@@ -4088,10 +4088,10 @@
       <c r="N31" s="19"/>
       <c r="O31" s="19"/>
       <c r="P31" s="13" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="Q31" s="19" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="R31" s="19"/>
       <c r="S31" s="19"/>
@@ -4102,7 +4102,7 @@
         <v>13020032</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C32" s="18">
         <v>3</v>
@@ -4116,7 +4116,7 @@
       <c r="F32" s="19"/>
       <c r="G32" s="19"/>
       <c r="H32" s="19" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="I32" s="19"/>
       <c r="J32" s="19"/>
@@ -4126,10 +4126,10 @@
       <c r="N32" s="19"/>
       <c r="O32" s="19"/>
       <c r="P32" s="13" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="Q32" s="19" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="R32" s="19"/>
       <c r="S32" s="19"/>
@@ -4140,7 +4140,7 @@
         <v>13020033</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C33" s="18">
         <v>3</v>
@@ -4154,7 +4154,7 @@
       <c r="F33" s="19"/>
       <c r="G33" s="19"/>
       <c r="H33" s="19" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="I33" s="19"/>
       <c r="J33" s="19"/>
@@ -4164,10 +4164,10 @@
       <c r="N33" s="19"/>
       <c r="O33" s="19"/>
       <c r="P33" s="13" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="Q33" s="19" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="R33" s="20"/>
       <c r="S33" s="20"/>
@@ -4178,7 +4178,7 @@
         <v>13020034</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C34" s="18">
         <v>3</v>
@@ -4192,7 +4192,7 @@
       <c r="F34" s="19"/>
       <c r="G34" s="19"/>
       <c r="H34" s="19" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="I34" s="19"/>
       <c r="J34" s="19"/>
@@ -4202,10 +4202,10 @@
       <c r="N34" s="19"/>
       <c r="O34" s="19"/>
       <c r="P34" s="13" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="Q34" s="19" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="R34" s="20"/>
       <c r="S34" s="20"/>
@@ -4216,7 +4216,7 @@
         <v>13020035</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C35" s="18">
         <v>3</v>
@@ -4230,7 +4230,7 @@
       <c r="F35" s="19"/>
       <c r="G35" s="19"/>
       <c r="H35" s="19" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="I35" s="19"/>
       <c r="J35" s="19"/>
@@ -4240,10 +4240,10 @@
       <c r="N35" s="19"/>
       <c r="O35" s="19"/>
       <c r="P35" s="13" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="Q35" s="19" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="R35" s="20"/>
       <c r="S35" s="20"/>

</xml_diff>

<commit_message>
finish the function resmerchant
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Scene.xlsx
+++ b/ConfigData/Xlsx/Scene.xlsx
@@ -192,10 +192,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>激活传送门</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>QPortal</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -775,19 +771,23 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>met;30|lighthouse;60|floatbottle;50|spinbox;30</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|treasure;25|spinbox;30</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>wishwell;20|spinbox;30</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>hiddeway;35|spinbox;35</t>
+    <t>激活传送</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|lighthouse;60|floatbottle;50</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|treasure;25</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>hiddeway;35</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>wishwell;20</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1518,18 +1518,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
@@ -1580,6 +1568,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -2613,1641 +2613,1641 @@
   <dimension ref="A1:T35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="11.125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="10.625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="5.125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="4.375" style="5" customWidth="1"/>
-    <col min="5" max="5" width="9" style="5" customWidth="1"/>
-    <col min="6" max="6" width="52.875" style="5" customWidth="1"/>
-    <col min="7" max="7" width="23.625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="50.875" style="5" customWidth="1"/>
-    <col min="9" max="14" width="3.125" style="5" customWidth="1"/>
-    <col min="15" max="15" width="6.625" style="5" customWidth="1"/>
-    <col min="16" max="16" width="9.75" style="5" customWidth="1"/>
-    <col min="17" max="17" width="9.5" style="5" customWidth="1"/>
-    <col min="18" max="18" width="7.25" style="5" customWidth="1"/>
-    <col min="19" max="20" width="6" style="5" customWidth="1"/>
-    <col min="21" max="16384" width="9" style="5"/>
+    <col min="1" max="1" width="11.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="5.125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="4.375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9" style="1" customWidth="1"/>
+    <col min="6" max="6" width="52.875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="23.625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="50.875" style="1" customWidth="1"/>
+    <col min="9" max="14" width="3.125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="6.625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="9.75" style="1" customWidth="1"/>
+    <col min="17" max="17" width="9.5" style="1" customWidth="1"/>
+    <col min="18" max="18" width="7.25" style="1" customWidth="1"/>
+    <col min="19" max="20" width="6" style="1" customWidth="1"/>
+    <col min="21" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="E1" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="F1" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="J1" s="3" t="s">
+      <c r="G1" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="K1" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="M1" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="N1" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="R1" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="S1" s="2" t="s">
+      <c r="R1" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="S1" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="T1" s="21" t="s">
         <v>84</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="D2" s="7" t="s">
+      <c r="C2" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="I2" s="8" t="s">
+      <c r="E2" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="L2" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="M2" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="N2" s="8" t="s">
+      <c r="N2" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="O2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="7" t="s">
+      <c r="P2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="Q2" s="7" t="s">
+      <c r="Q2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="R2" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="S2" s="7" t="s">
+      <c r="R2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="S2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="T2" s="9" t="s">
+      <c r="T2" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="D3" s="10" t="s">
+      <c r="C3" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="F3" s="10" t="s">
+      <c r="E3" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="I3" s="11" t="s">
+      <c r="G3" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="J3" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="J3" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="K3" s="11" t="s">
+      <c r="K3" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="L3" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="L3" s="11" t="s">
+      <c r="M3" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="M3" s="11" t="s">
+      <c r="N3" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="N3" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="O3" s="10" t="s">
+      <c r="O3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="P3" s="10" t="s">
+      <c r="P3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="Q3" s="10" t="s">
+      <c r="Q3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="R3" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="S3" s="10" t="s">
+      <c r="R3" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="S3" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="T3" s="6" t="s">
         <v>62</v>
-      </c>
-      <c r="T3" s="10" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A4" s="12">
+      <c r="A4" s="8">
         <v>13010001</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C4" s="9">
         <v>2</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="9">
         <v>1</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="9">
         <v>13010001</v>
       </c>
-      <c r="F4" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>202</v>
-      </c>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13">
+      <c r="F4" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9">
         <v>1</v>
       </c>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q4" s="13" t="s">
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q4" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="R4" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="S4" s="13">
+      <c r="R4" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="S4" s="9">
         <v>1348</v>
       </c>
-      <c r="T4" s="13">
+      <c r="T4" s="9">
         <v>611</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A5" s="12">
+      <c r="A5" s="8">
         <v>13010002</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="9">
         <v>2</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="9">
         <v>2</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="9">
         <v>13010001</v>
       </c>
-      <c r="F5" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="G5" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13">
+      <c r="F5" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9">
         <v>1</v>
       </c>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13">
+      <c r="J5" s="9"/>
+      <c r="K5" s="9">
         <v>1</v>
       </c>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13">
+      <c r="L5" s="9"/>
+      <c r="M5" s="9">
         <v>1</v>
       </c>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13" t="s">
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="Q5" s="13" t="s">
+      <c r="Q5" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="R5" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="S5" s="13">
+      <c r="R5" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="S5" s="9">
         <v>1279</v>
       </c>
-      <c r="T5" s="13">
+      <c r="T5" s="9">
         <v>571</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A6" s="12">
+      <c r="A6" s="8">
         <v>13010004</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="9">
         <v>2</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="9">
         <v>5</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="9">
         <v>13010006</v>
       </c>
-      <c r="F6" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="G6" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13">
+      <c r="F6" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9">
         <v>1</v>
       </c>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13">
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9">
         <v>1</v>
       </c>
-      <c r="M6" s="13"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="13"/>
-      <c r="P6" s="13" t="s">
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="Q6" s="13" t="s">
+      <c r="Q6" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="R6" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="S6" s="13">
+      <c r="R6" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="S6" s="9">
         <v>1148</v>
       </c>
-      <c r="T6" s="13">
+      <c r="T6" s="9">
         <v>351</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A7" s="12">
+      <c r="A7" s="8">
         <v>13010005</v>
       </c>
-      <c r="B7" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="C7" s="13">
+      <c r="B7" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="C7" s="9">
         <v>2</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="9">
         <v>8</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="9">
         <v>13010006</v>
       </c>
-      <c r="F7" s="13" t="s">
-        <v>175</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13">
+      <c r="F7" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9">
         <v>1</v>
       </c>
-      <c r="J7" s="13">
+      <c r="J7" s="9">
         <v>1</v>
       </c>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
-      <c r="P7" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q7" s="13" t="s">
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q7" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="R7" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="S7" s="13">
+      <c r="R7" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="S7" s="9">
         <v>1386</v>
       </c>
-      <c r="T7" s="13">
+      <c r="T7" s="9">
         <v>339</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A8" s="12">
+      <c r="A8" s="8">
         <v>13010006</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="9">
         <v>1</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="9">
         <v>3</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="9">
         <v>13010006</v>
       </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="13"/>
-      <c r="P8" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q8" s="13" t="s">
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q8" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="R8" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="S8" s="13">
+      <c r="R8" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="S8" s="9">
         <v>1232</v>
       </c>
-      <c r="T8" s="13">
+      <c r="T8" s="9">
         <v>506</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A9" s="12">
+      <c r="A9" s="8">
         <v>13010007</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="9">
         <v>2</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="9">
         <v>7</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="9">
         <v>13010006</v>
       </c>
-      <c r="F9" s="13" t="s">
-        <v>179</v>
-      </c>
-      <c r="G9" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13">
+      <c r="F9" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9">
         <v>1</v>
       </c>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13">
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9">
         <v>1</v>
       </c>
-      <c r="M9" s="13">
+      <c r="M9" s="9">
         <v>1</v>
       </c>
-      <c r="N9" s="13"/>
-      <c r="O9" s="13"/>
-      <c r="P9" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="Q9" s="13" t="s">
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q9" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="R9" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="S9" s="13">
+      <c r="R9" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="S9" s="9">
         <v>1431</v>
       </c>
-      <c r="T9" s="13">
+      <c r="T9" s="9">
         <v>440</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A10" s="12">
+      <c r="A10" s="8">
         <v>13010009</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="9">
         <v>2</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="9">
         <v>4</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="9">
         <v>13010006</v>
       </c>
-      <c r="F10" s="13" t="s">
-        <v>172</v>
-      </c>
-      <c r="G10" s="21" t="s">
-        <v>203</v>
-      </c>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13">
+      <c r="F10" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9">
         <v>1</v>
       </c>
-      <c r="J10" s="13">
+      <c r="J10" s="9">
         <v>1</v>
       </c>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13">
+      <c r="K10" s="9"/>
+      <c r="L10" s="9">
         <v>1</v>
       </c>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="13"/>
-      <c r="P10" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="Q10" s="13" t="s">
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="R10" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="S10" s="13">
+      <c r="Q10" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="R10" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="S10" s="9">
         <v>1332</v>
       </c>
-      <c r="T10" s="13">
+      <c r="T10" s="9">
         <v>484</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A11" s="12">
+      <c r="A11" s="8">
         <v>13010010</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="13">
+      <c r="C11" s="9">
         <v>2</v>
       </c>
-      <c r="D11" s="13">
+      <c r="D11" s="9">
         <v>10</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E11" s="9">
         <v>13010006</v>
       </c>
-      <c r="F11" s="13" t="s">
-        <v>181</v>
-      </c>
-      <c r="G11" s="21" t="s">
+      <c r="F11" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="G11" s="17" t="s">
         <v>204</v>
       </c>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13">
+      <c r="H11" s="9"/>
+      <c r="I11" s="9">
         <v>1</v>
       </c>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="13">
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9">
         <v>1</v>
       </c>
-      <c r="O11" s="13"/>
-      <c r="P11" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="Q11" s="13" t="s">
+      <c r="O11" s="9"/>
+      <c r="P11" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q11" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="R11" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="S11" s="13">
+      <c r="R11" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="S11" s="9">
         <v>1441</v>
       </c>
-      <c r="T11" s="13">
+      <c r="T11" s="9">
         <v>527</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A12" s="12">
+      <c r="A12" s="8">
         <v>13010011</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="13">
+      <c r="C12" s="9">
         <v>2</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="9">
         <v>12</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E12" s="9">
         <v>13010006</v>
       </c>
-      <c r="F12" s="13" t="s">
-        <v>180</v>
-      </c>
-      <c r="G12" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13">
+      <c r="F12" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9">
         <v>1</v>
       </c>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13">
+      <c r="J12" s="9"/>
+      <c r="K12" s="9">
         <v>1</v>
       </c>
-      <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
-      <c r="N12" s="13"/>
-      <c r="O12" s="13"/>
-      <c r="P12" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q12" s="13" t="s">
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q12" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="R12" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="S12" s="13">
+      <c r="R12" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="S12" s="9">
         <v>1574</v>
       </c>
-      <c r="T12" s="13">
+      <c r="T12" s="9">
         <v>373</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A13" s="12">
+      <c r="A13" s="8">
         <v>13010012</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="13">
+      <c r="C13" s="9">
         <v>2</v>
       </c>
-      <c r="D13" s="13">
+      <c r="D13" s="9">
         <v>3</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E13" s="9">
         <v>13010006</v>
       </c>
-      <c r="F13" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="G13" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13">
+      <c r="F13" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9">
         <v>1</v>
       </c>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="13"/>
-      <c r="O13" s="13"/>
-      <c r="P13" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q13" s="13" t="s">
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q13" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="R13" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="S13" s="13">
+      <c r="R13" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="S13" s="9">
         <v>1251</v>
       </c>
-      <c r="T13" s="13">
+      <c r="T13" s="9">
         <v>432</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A14" s="12">
+      <c r="A14" s="8">
         <v>13010013</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="13">
+      <c r="C14" s="9">
         <v>2</v>
       </c>
-      <c r="D14" s="13">
+      <c r="D14" s="9">
         <v>6</v>
       </c>
-      <c r="E14" s="13">
+      <c r="E14" s="9">
         <v>13010006</v>
       </c>
-      <c r="F14" s="13" t="s">
-        <v>162</v>
-      </c>
-      <c r="G14" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13">
+      <c r="F14" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9">
         <v>1</v>
       </c>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="13"/>
-      <c r="N14" s="13"/>
-      <c r="O14" s="13"/>
-      <c r="P14" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q14" s="13" t="s">
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q14" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="R14" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="S14" s="13">
+      <c r="R14" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="S14" s="9">
         <v>1250</v>
       </c>
-      <c r="T14" s="13">
+      <c r="T14" s="9">
         <v>338</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A15" s="12">
+      <c r="A15" s="8">
         <v>13010014</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="13">
+      <c r="C15" s="9">
         <v>2</v>
       </c>
-      <c r="D15" s="13">
+      <c r="D15" s="9">
         <v>14</v>
       </c>
-      <c r="E15" s="13">
+      <c r="E15" s="9">
         <v>13010006</v>
       </c>
-      <c r="F15" s="13" t="s">
-        <v>174</v>
-      </c>
-      <c r="G15" s="13" t="s">
-        <v>178</v>
-      </c>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13">
+      <c r="F15" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9">
         <v>1</v>
       </c>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="13">
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9">
         <v>1</v>
       </c>
-      <c r="N15" s="13">
+      <c r="N15" s="9">
         <v>1</v>
       </c>
-      <c r="O15" s="13"/>
-      <c r="P15" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q15" s="13" t="s">
+      <c r="O15" s="9"/>
+      <c r="P15" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q15" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="R15" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="S15" s="13">
+      <c r="R15" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="S15" s="9">
         <v>1550</v>
       </c>
-      <c r="T15" s="13">
+      <c r="T15" s="9">
         <v>505</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A16" s="12">
+      <c r="A16" s="8">
         <v>13010015</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="C16" s="11">
+        <v>2</v>
+      </c>
+      <c r="D16" s="11">
+        <v>6</v>
+      </c>
+      <c r="E16" s="9">
+        <v>13010006</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="H16" s="9"/>
+      <c r="I16" s="11">
+        <v>1</v>
+      </c>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="11"/>
+      <c r="P16" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="C16" s="15">
-        <v>2</v>
-      </c>
-      <c r="D16" s="15">
-        <v>6</v>
-      </c>
-      <c r="E16" s="13">
-        <v>13010006</v>
-      </c>
-      <c r="F16" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="G16" s="13" t="s">
-        <v>171</v>
-      </c>
-      <c r="H16" s="13"/>
-      <c r="I16" s="15">
-        <v>1</v>
-      </c>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="15"/>
-      <c r="O16" s="15"/>
-      <c r="P16" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="Q16" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="R16" s="15"/>
-      <c r="S16" s="15"/>
-      <c r="T16" s="15"/>
+      <c r="Q16" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="R16" s="11"/>
+      <c r="S16" s="11"/>
+      <c r="T16" s="11"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A17" s="16">
+      <c r="A17" s="12">
         <v>13010101</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="13">
+      <c r="C17" s="9">
         <v>1</v>
       </c>
-      <c r="D17" s="13">
+      <c r="D17" s="9">
         <v>16</v>
       </c>
-      <c r="E17" s="13">
+      <c r="E17" s="9">
         <v>13010101</v>
       </c>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
-      <c r="N17" s="13"/>
-      <c r="O17" s="13"/>
-      <c r="P17" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="Q17" s="13" t="s">
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q17" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="R17" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="S17" s="13">
+      <c r="R17" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="S17" s="9">
         <v>919</v>
       </c>
-      <c r="T17" s="13">
+      <c r="T17" s="9">
         <v>534</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A18" s="16">
+      <c r="A18" s="12">
         <v>13010102</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="13">
+      <c r="C18" s="9">
         <v>2</v>
       </c>
-      <c r="D18" s="13">
+      <c r="D18" s="9">
         <v>16</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E18" s="9">
         <v>13010101</v>
       </c>
-      <c r="F18" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="G18" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13">
+      <c r="F18" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9">
         <v>1</v>
       </c>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="13">
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9">
         <v>1</v>
       </c>
-      <c r="M18" s="13"/>
-      <c r="N18" s="13"/>
-      <c r="O18" s="13"/>
-      <c r="P18" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="Q18" s="13" t="s">
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q18" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="R18" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="S18" s="13">
+      <c r="R18" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="S18" s="9">
         <v>1040</v>
       </c>
-      <c r="T18" s="13">
+      <c r="T18" s="9">
         <v>538</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A19" s="16">
+      <c r="A19" s="12">
         <v>13010103</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="13">
+      <c r="C19" s="9">
         <v>2</v>
       </c>
-      <c r="D19" s="13">
+      <c r="D19" s="9">
         <v>19</v>
       </c>
-      <c r="E19" s="13">
+      <c r="E19" s="9">
         <v>13010101</v>
       </c>
-      <c r="F19" s="13" t="s">
-        <v>173</v>
-      </c>
-      <c r="G19" s="21" t="s">
+      <c r="F19" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="G19" s="17" t="s">
         <v>205</v>
       </c>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13">
+      <c r="H19" s="9"/>
+      <c r="I19" s="9">
         <v>1</v>
       </c>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
-      <c r="N19" s="13"/>
-      <c r="O19" s="13"/>
-      <c r="P19" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="Q19" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="R19" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="S19" s="13">
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q19" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="R19" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="S19" s="9">
         <v>1213</v>
       </c>
-      <c r="T19" s="13">
+      <c r="T19" s="9">
         <v>655</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A20" s="16">
+      <c r="A20" s="12">
         <v>13010104</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="13">
+      <c r="C20" s="9">
         <v>2</v>
       </c>
-      <c r="D20" s="13">
+      <c r="D20" s="9">
         <v>18</v>
       </c>
-      <c r="E20" s="13">
+      <c r="E20" s="9">
         <v>13010101</v>
       </c>
-      <c r="F20" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="G20" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13">
+      <c r="F20" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9">
         <v>1</v>
       </c>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13">
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9">
         <v>1</v>
       </c>
-      <c r="N20" s="13"/>
-      <c r="O20" s="13"/>
-      <c r="P20" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="Q20" s="13" t="s">
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q20" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="R20" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="S20" s="13">
+      <c r="R20" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="S20" s="9">
         <v>1149</v>
       </c>
-      <c r="T20" s="13">
+      <c r="T20" s="9">
         <v>584</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A21" s="16">
+      <c r="A21" s="12">
         <v>13010105</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="13">
+      <c r="C21" s="9">
         <v>2</v>
       </c>
-      <c r="D21" s="13">
+      <c r="D21" s="9">
         <v>20</v>
       </c>
-      <c r="E21" s="13">
+      <c r="E21" s="9">
         <v>13010101</v>
       </c>
-      <c r="F21" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="G21" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="13"/>
-      <c r="N21" s="13"/>
-      <c r="O21" s="13"/>
-      <c r="P21" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q21" s="13" t="s">
+      <c r="F21" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q21" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="R21" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="S21" s="13">
+      <c r="R21" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="S21" s="9">
         <v>840</v>
       </c>
-      <c r="T21" s="13">
+      <c r="T21" s="9">
         <v>444</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A22" s="16">
+      <c r="A22" s="12">
         <v>13010106</v>
       </c>
-      <c r="B22" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="C22" s="13">
+      <c r="B22" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="C22" s="9">
         <v>2</v>
       </c>
-      <c r="D22" s="13">
+      <c r="D22" s="9">
         <v>15</v>
       </c>
-      <c r="E22" s="13">
+      <c r="E22" s="9">
         <v>13010016</v>
       </c>
-      <c r="F22" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="G22" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13">
+      <c r="F22" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9">
         <v>1</v>
       </c>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="13">
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9">
         <v>1</v>
       </c>
-      <c r="O22" s="13"/>
-      <c r="P22" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q22" s="13" t="s">
+      <c r="O22" s="9"/>
+      <c r="P22" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q22" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="R22" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="S22" s="13">
+      <c r="R22" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="S22" s="9">
         <v>1067</v>
       </c>
-      <c r="T22" s="13">
+      <c r="T22" s="9">
         <v>445</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A23" s="17">
+      <c r="A23" s="13">
         <v>13020001</v>
       </c>
-      <c r="B23" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="C23" s="17">
+      <c r="B23" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="C23" s="13">
         <v>3</v>
       </c>
-      <c r="D23" s="13">
+      <c r="D23" s="9">
         <v>3</v>
       </c>
-      <c r="E23" s="13">
+      <c r="E23" s="9">
         <v>13010002</v>
       </c>
-      <c r="F23" s="13" t="s">
-        <v>150</v>
-      </c>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13" t="s">
+      <c r="F23" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
-      <c r="N23" s="13"/>
-      <c r="O23" s="13"/>
-      <c r="P23" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="Q23" s="13" t="s">
-        <v>163</v>
-      </c>
-      <c r="R23" s="13"/>
-      <c r="S23" s="13"/>
-      <c r="T23" s="13"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q23" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="R23" s="9"/>
+      <c r="S23" s="9"/>
+      <c r="T23" s="9"/>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A24" s="17">
+      <c r="A24" s="13">
         <v>13020002</v>
       </c>
-      <c r="B24" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="C24" s="17">
+      <c r="B24" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="C24" s="13">
         <v>3</v>
       </c>
-      <c r="D24" s="13">
+      <c r="D24" s="9">
         <v>3</v>
       </c>
-      <c r="E24" s="13">
+      <c r="E24" s="9">
         <v>13010002</v>
       </c>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="13"/>
-      <c r="L24" s="13"/>
-      <c r="M24" s="13"/>
-      <c r="N24" s="13"/>
-      <c r="O24" s="13"/>
-      <c r="P24" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="Q24" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="R24" s="13"/>
-      <c r="S24" s="13"/>
-      <c r="T24" s="13"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q24" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="R24" s="9"/>
+      <c r="S24" s="9"/>
+      <c r="T24" s="9"/>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A25" s="17">
+      <c r="A25" s="13">
         <v>13020011</v>
       </c>
-      <c r="B25" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="C25" s="17">
+      <c r="B25" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="C25" s="13">
         <v>3</v>
       </c>
-      <c r="D25" s="13">
+      <c r="D25" s="9">
         <v>8</v>
       </c>
-      <c r="E25" s="13">
+      <c r="E25" s="9">
         <v>13010007</v>
       </c>
-      <c r="F25" s="13" t="s">
-        <v>176</v>
-      </c>
-      <c r="G25" s="21" t="s">
-        <v>206</v>
-      </c>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="13"/>
-      <c r="N25" s="13"/>
-      <c r="O25" s="13"/>
-      <c r="P25" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="Q25" s="13" t="s">
-        <v>165</v>
-      </c>
-      <c r="R25" s="13"/>
-      <c r="S25" s="13"/>
-      <c r="T25" s="13"/>
+      <c r="F25" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="G25" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q25" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="R25" s="9"/>
+      <c r="S25" s="9"/>
+      <c r="T25" s="9"/>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A26" s="17">
+      <c r="A26" s="13">
         <v>13020012</v>
       </c>
-      <c r="B26" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="C26" s="17">
+      <c r="B26" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="C26" s="13">
         <v>3</v>
       </c>
-      <c r="D26" s="13">
+      <c r="D26" s="9">
         <v>8</v>
       </c>
-      <c r="E26" s="13">
+      <c r="E26" s="9">
         <v>13010007</v>
       </c>
-      <c r="F26" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="13"/>
-      <c r="K26" s="13"/>
-      <c r="L26" s="13"/>
-      <c r="M26" s="13"/>
-      <c r="N26" s="13"/>
-      <c r="O26" s="13"/>
-      <c r="P26" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="Q26" s="13" t="s">
-        <v>166</v>
-      </c>
-      <c r="R26" s="13"/>
-      <c r="S26" s="13"/>
-      <c r="T26" s="13"/>
+      <c r="F26" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="9"/>
+      <c r="M26" s="9"/>
+      <c r="N26" s="9"/>
+      <c r="O26" s="9"/>
+      <c r="P26" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q26" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="R26" s="9"/>
+      <c r="S26" s="9"/>
+      <c r="T26" s="9"/>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A27" s="17">
+      <c r="A27" s="13">
         <v>13020013</v>
       </c>
-      <c r="B27" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="C27" s="17">
+      <c r="B27" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="C27" s="13">
         <v>3</v>
       </c>
-      <c r="D27" s="13">
+      <c r="D27" s="9">
         <v>8</v>
       </c>
-      <c r="E27" s="13">
+      <c r="E27" s="9">
         <v>13010007</v>
       </c>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="13"/>
-      <c r="K27" s="13"/>
-      <c r="L27" s="13"/>
-      <c r="M27" s="13"/>
-      <c r="N27" s="13"/>
-      <c r="O27" s="13"/>
-      <c r="P27" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q27" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="R27" s="13"/>
-      <c r="S27" s="13"/>
-      <c r="T27" s="13"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="9"/>
+      <c r="M27" s="9"/>
+      <c r="N27" s="9"/>
+      <c r="O27" s="9"/>
+      <c r="P27" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q27" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="R27" s="9"/>
+      <c r="S27" s="9"/>
+      <c r="T27" s="9"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A28" s="17">
+      <c r="A28" s="13">
         <v>13020021</v>
       </c>
-      <c r="B28" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="C28" s="17">
+      <c r="B28" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="C28" s="13">
         <v>3</v>
       </c>
-      <c r="D28" s="13">
+      <c r="D28" s="9">
         <v>5</v>
       </c>
-      <c r="E28" s="13">
+      <c r="E28" s="9">
         <v>13010004</v>
       </c>
-      <c r="F28" s="13" t="s">
-        <v>161</v>
-      </c>
-      <c r="G28" s="21" t="s">
-        <v>200</v>
-      </c>
-      <c r="H28" s="13" t="s">
-        <v>194</v>
-      </c>
-      <c r="I28" s="13"/>
-      <c r="J28" s="13"/>
-      <c r="K28" s="13"/>
-      <c r="L28" s="13"/>
-      <c r="M28" s="13"/>
-      <c r="N28" s="13"/>
-      <c r="O28" s="13"/>
-      <c r="P28" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="Q28" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="R28" s="13"/>
-      <c r="S28" s="13"/>
-      <c r="T28" s="13"/>
+      <c r="F28" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="G28" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="H28" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="9"/>
+      <c r="O28" s="9"/>
+      <c r="P28" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q28" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="R28" s="9"/>
+      <c r="S28" s="9"/>
+      <c r="T28" s="9"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A29" s="17">
+      <c r="A29" s="13">
         <v>13020022</v>
       </c>
-      <c r="B29" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="C29" s="17">
+      <c r="B29" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="C29" s="13">
         <v>3</v>
       </c>
-      <c r="D29" s="13">
+      <c r="D29" s="9">
         <v>5</v>
       </c>
-      <c r="E29" s="13">
+      <c r="E29" s="9">
         <v>13010004</v>
       </c>
-      <c r="F29" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="G29" s="21" t="s">
-        <v>201</v>
-      </c>
-      <c r="H29" s="13" t="s">
+      <c r="F29" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="I29" s="13"/>
-      <c r="J29" s="13"/>
-      <c r="K29" s="13"/>
-      <c r="L29" s="13"/>
-      <c r="M29" s="13"/>
-      <c r="N29" s="13"/>
-      <c r="O29" s="13"/>
-      <c r="P29" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="Q29" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="R29" s="13"/>
-      <c r="S29" s="13"/>
-      <c r="T29" s="13"/>
+      <c r="G29" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="H29" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="9"/>
+      <c r="M29" s="9"/>
+      <c r="N29" s="9"/>
+      <c r="O29" s="9"/>
+      <c r="P29" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q29" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="R29" s="9"/>
+      <c r="S29" s="9"/>
+      <c r="T29" s="9"/>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A30" s="17">
+      <c r="A30" s="13">
         <v>13020023</v>
       </c>
-      <c r="B30" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="C30" s="17">
+      <c r="B30" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="C30" s="13">
         <v>3</v>
       </c>
-      <c r="D30" s="13">
+      <c r="D30" s="9">
         <v>5</v>
       </c>
-      <c r="E30" s="13">
+      <c r="E30" s="9">
         <v>13010004</v>
       </c>
-      <c r="F30" s="13" t="s">
-        <v>159</v>
-      </c>
-      <c r="G30" s="21" t="s">
-        <v>207</v>
-      </c>
-      <c r="H30" s="13" t="s">
-        <v>156</v>
-      </c>
-      <c r="I30" s="13"/>
-      <c r="J30" s="13"/>
-      <c r="K30" s="13"/>
-      <c r="L30" s="13"/>
-      <c r="M30" s="13"/>
-      <c r="N30" s="13"/>
-      <c r="O30" s="13"/>
-      <c r="P30" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="Q30" s="13" t="s">
-        <v>170</v>
-      </c>
-      <c r="R30" s="13"/>
-      <c r="S30" s="13"/>
-      <c r="T30" s="13"/>
+      <c r="F30" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="G30" s="17" t="s">
+        <v>206</v>
+      </c>
+      <c r="H30" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="9"/>
+      <c r="M30" s="9"/>
+      <c r="N30" s="9"/>
+      <c r="O30" s="9"/>
+      <c r="P30" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q30" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="R30" s="9"/>
+      <c r="S30" s="9"/>
+      <c r="T30" s="9"/>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A31" s="18">
+      <c r="A31" s="14">
         <v>13020031</v>
       </c>
-      <c r="B31" s="17" t="s">
+      <c r="B31" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="C31" s="14">
+        <v>3</v>
+      </c>
+      <c r="D31" s="15">
+        <v>10</v>
+      </c>
+      <c r="E31" s="15">
+        <v>13010005</v>
+      </c>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="I31" s="15"/>
+      <c r="J31" s="15"/>
+      <c r="K31" s="15"/>
+      <c r="L31" s="15"/>
+      <c r="M31" s="15"/>
+      <c r="N31" s="15"/>
+      <c r="O31" s="15"/>
+      <c r="P31" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="C31" s="18">
-        <v>3</v>
-      </c>
-      <c r="D31" s="19">
-        <v>10</v>
-      </c>
-      <c r="E31" s="19">
-        <v>13010005</v>
-      </c>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
-      <c r="H31" s="19" t="s">
-        <v>195</v>
-      </c>
-      <c r="I31" s="19"/>
-      <c r="J31" s="19"/>
-      <c r="K31" s="19"/>
-      <c r="L31" s="19"/>
-      <c r="M31" s="19"/>
-      <c r="N31" s="19"/>
-      <c r="O31" s="19"/>
-      <c r="P31" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="Q31" s="19" t="s">
-        <v>189</v>
-      </c>
-      <c r="R31" s="19"/>
-      <c r="S31" s="19"/>
-      <c r="T31" s="19"/>
+      <c r="Q31" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="R31" s="15"/>
+      <c r="S31" s="15"/>
+      <c r="T31" s="15"/>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A32" s="18">
+      <c r="A32" s="14">
         <v>13020032</v>
       </c>
-      <c r="B32" s="17" t="s">
-        <v>185</v>
-      </c>
-      <c r="C32" s="18">
+      <c r="B32" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="C32" s="14">
         <v>3</v>
       </c>
-      <c r="D32" s="19">
+      <c r="D32" s="15">
         <v>10</v>
       </c>
-      <c r="E32" s="19">
+      <c r="E32" s="15">
         <v>13010005</v>
       </c>
-      <c r="F32" s="19"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="19" t="s">
-        <v>196</v>
-      </c>
-      <c r="I32" s="19"/>
-      <c r="J32" s="19"/>
-      <c r="K32" s="19"/>
-      <c r="L32" s="19"/>
-      <c r="M32" s="19"/>
-      <c r="N32" s="19"/>
-      <c r="O32" s="19"/>
-      <c r="P32" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="Q32" s="19" t="s">
-        <v>190</v>
-      </c>
-      <c r="R32" s="19"/>
-      <c r="S32" s="19"/>
-      <c r="T32" s="19"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="I32" s="15"/>
+      <c r="J32" s="15"/>
+      <c r="K32" s="15"/>
+      <c r="L32" s="15"/>
+      <c r="M32" s="15"/>
+      <c r="N32" s="15"/>
+      <c r="O32" s="15"/>
+      <c r="P32" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q32" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="R32" s="15"/>
+      <c r="S32" s="15"/>
+      <c r="T32" s="15"/>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A33" s="18">
+      <c r="A33" s="14">
         <v>13020033</v>
       </c>
-      <c r="B33" s="17" t="s">
-        <v>186</v>
-      </c>
-      <c r="C33" s="18">
+      <c r="B33" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="C33" s="14">
         <v>3</v>
       </c>
-      <c r="D33" s="19">
+      <c r="D33" s="15">
         <v>10</v>
       </c>
-      <c r="E33" s="19">
+      <c r="E33" s="15">
         <v>13010005</v>
       </c>
-      <c r="F33" s="19"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="19" t="s">
-        <v>197</v>
-      </c>
-      <c r="I33" s="19"/>
-      <c r="J33" s="19"/>
-      <c r="K33" s="19"/>
-      <c r="L33" s="19"/>
-      <c r="M33" s="19"/>
-      <c r="N33" s="19"/>
-      <c r="O33" s="19"/>
-      <c r="P33" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="Q33" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="R33" s="20"/>
-      <c r="S33" s="20"/>
-      <c r="T33" s="20"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="I33" s="15"/>
+      <c r="J33" s="15"/>
+      <c r="K33" s="15"/>
+      <c r="L33" s="15"/>
+      <c r="M33" s="15"/>
+      <c r="N33" s="15"/>
+      <c r="O33" s="15"/>
+      <c r="P33" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q33" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="R33" s="16"/>
+      <c r="S33" s="16"/>
+      <c r="T33" s="16"/>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A34" s="18">
+      <c r="A34" s="14">
         <v>13020034</v>
       </c>
-      <c r="B34" s="17" t="s">
-        <v>187</v>
-      </c>
-      <c r="C34" s="18">
+      <c r="B34" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="C34" s="14">
         <v>3</v>
       </c>
-      <c r="D34" s="19">
+      <c r="D34" s="15">
         <v>10</v>
       </c>
-      <c r="E34" s="19">
+      <c r="E34" s="15">
         <v>13010005</v>
       </c>
-      <c r="F34" s="19"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="19" t="s">
-        <v>198</v>
-      </c>
-      <c r="I34" s="19"/>
-      <c r="J34" s="19"/>
-      <c r="K34" s="19"/>
-      <c r="L34" s="19"/>
-      <c r="M34" s="19"/>
-      <c r="N34" s="19"/>
-      <c r="O34" s="19"/>
-      <c r="P34" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="Q34" s="19" t="s">
-        <v>192</v>
-      </c>
-      <c r="R34" s="20"/>
-      <c r="S34" s="20"/>
-      <c r="T34" s="20"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="I34" s="15"/>
+      <c r="J34" s="15"/>
+      <c r="K34" s="15"/>
+      <c r="L34" s="15"/>
+      <c r="M34" s="15"/>
+      <c r="N34" s="15"/>
+      <c r="O34" s="15"/>
+      <c r="P34" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q34" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="R34" s="16"/>
+      <c r="S34" s="16"/>
+      <c r="T34" s="16"/>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A35" s="18">
+      <c r="A35" s="14">
         <v>13020035</v>
       </c>
-      <c r="B35" s="17" t="s">
-        <v>188</v>
-      </c>
-      <c r="C35" s="18">
+      <c r="B35" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="C35" s="14">
         <v>3</v>
       </c>
-      <c r="D35" s="19">
+      <c r="D35" s="15">
         <v>10</v>
       </c>
-      <c r="E35" s="19">
+      <c r="E35" s="15">
         <v>13010005</v>
       </c>
-      <c r="F35" s="19"/>
-      <c r="G35" s="19"/>
-      <c r="H35" s="19" t="s">
-        <v>199</v>
-      </c>
-      <c r="I35" s="19"/>
-      <c r="J35" s="19"/>
-      <c r="K35" s="19"/>
-      <c r="L35" s="19"/>
-      <c r="M35" s="19"/>
-      <c r="N35" s="19"/>
-      <c r="O35" s="19"/>
-      <c r="P35" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="Q35" s="19" t="s">
-        <v>193</v>
-      </c>
-      <c r="R35" s="20"/>
-      <c r="S35" s="20"/>
-      <c r="T35" s="20"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="I35" s="15"/>
+      <c r="J35" s="15"/>
+      <c r="K35" s="15"/>
+      <c r="L35" s="15"/>
+      <c r="M35" s="15"/>
+      <c r="N35" s="15"/>
+      <c r="O35" s="15"/>
+      <c r="P35" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q35" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="R35" s="16"/>
+      <c r="S35" s="16"/>
+      <c r="T35" s="16"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>

<commit_message>
support wheel and res config
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Scene.xlsx
+++ b/ConfigData/Xlsx/Scene.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="Scene" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="213">
   <si>
     <t>村外小屋</t>
   </si>
@@ -788,13 +788,32 @@
   </si>
   <si>
     <t>wishwell;20</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>转盘</t>
+  </si>
+  <si>
+    <t>期货</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QWheel</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QRes</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1514,7 +1533,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1580,6 +1599,9 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1626,7 +1648,7 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="28">
     <dxf>
       <font>
         <b val="0"/>
@@ -1776,6 +1798,64 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -2258,32 +2338,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A3:T35" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21" tableBorderDxfId="20">
-  <autoFilter ref="A3:T35" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState ref="A4:T27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:V35" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23" tableBorderDxfId="22">
+  <autoFilter ref="A3:V35"/>
+  <sortState ref="A4:V27">
     <sortCondition ref="A3:A27"/>
   </sortState>
-  <tableColumns count="20">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="18"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Type" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Level" dataDxfId="16"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="ReviveScene" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Quest" dataDxfId="14"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="QuestRandom" dataDxfId="13"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="QuestDungeon" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="QPortal" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="QCardChange" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="QPiece" dataDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="QMerchant" dataDxfId="8"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="QDoctor" dataDxfId="7"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="QAngel" dataDxfId="6"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Func" dataDxfId="5"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Url" dataDxfId="4"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="TilePath" dataDxfId="3"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Icon" dataDxfId="2"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="IconX" dataDxfId="1"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="IconY" dataDxfId="0"/>
+  <tableColumns count="22">
+    <tableColumn id="1" name="Id" dataDxfId="21"/>
+    <tableColumn id="2" name="Name" dataDxfId="20"/>
+    <tableColumn id="18" name="Type" dataDxfId="19"/>
+    <tableColumn id="3" name="Level" dataDxfId="18"/>
+    <tableColumn id="20" name="ReviveScene" dataDxfId="17"/>
+    <tableColumn id="4" name="Quest" dataDxfId="16"/>
+    <tableColumn id="17" name="QuestRandom" dataDxfId="15"/>
+    <tableColumn id="19" name="QuestDungeon" dataDxfId="14"/>
+    <tableColumn id="5" name="QPortal" dataDxfId="13"/>
+    <tableColumn id="6" name="QCardChange" dataDxfId="12"/>
+    <tableColumn id="7" name="QPiece" dataDxfId="11"/>
+    <tableColumn id="8" name="QMerchant" dataDxfId="10"/>
+    <tableColumn id="9" name="QDoctor" dataDxfId="9"/>
+    <tableColumn id="10" name="QAngel" dataDxfId="8"/>
+    <tableColumn id="21" name="QWheel" dataDxfId="7"/>
+    <tableColumn id="22" name="QRes" dataDxfId="6"/>
+    <tableColumn id="11" name="Func" dataDxfId="5"/>
+    <tableColumn id="12" name="Url" dataDxfId="4"/>
+    <tableColumn id="13" name="TilePath" dataDxfId="3"/>
+    <tableColumn id="14" name="Icon" dataDxfId="2"/>
+    <tableColumn id="15" name="IconX" dataDxfId="1"/>
+    <tableColumn id="16" name="IconY" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2609,11 +2691,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2626,16 +2708,16 @@
     <col min="6" max="6" width="52.875" style="1" customWidth="1"/>
     <col min="7" max="7" width="23.625" style="1" customWidth="1"/>
     <col min="8" max="8" width="50.875" style="1" customWidth="1"/>
-    <col min="9" max="14" width="3.125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="6.625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="9.75" style="1" customWidth="1"/>
-    <col min="17" max="17" width="9.5" style="1" customWidth="1"/>
-    <col min="18" max="18" width="7.25" style="1" customWidth="1"/>
-    <col min="19" max="20" width="6" style="1" customWidth="1"/>
-    <col min="21" max="16384" width="9" style="1"/>
+    <col min="9" max="16" width="3.125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="6.625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="9.75" style="1" customWidth="1"/>
+    <col min="19" max="19" width="9.5" style="1" customWidth="1"/>
+    <col min="20" max="20" width="7.25" style="1" customWidth="1"/>
+    <col min="21" max="22" width="6" style="1" customWidth="1"/>
+    <col min="23" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="60" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:22" ht="60" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="18" t="s">
         <v>15</v>
       </c>
@@ -2678,26 +2760,32 @@
       <c r="N1" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="O1" s="19" t="s">
+      <c r="O1" s="20" t="s">
+        <v>208</v>
+      </c>
+      <c r="P1" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="Q1" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="P1" s="19" t="s">
+      <c r="R1" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="Q1" s="19" t="s">
+      <c r="S1" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="R1" s="19" t="s">
+      <c r="T1" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="S1" s="19" t="s">
+      <c r="U1" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="T1" s="21" t="s">
+      <c r="V1" s="21" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -2740,26 +2828,32 @@
       <c r="N2" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="O2" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="Q2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="U2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="T2" s="5" t="s">
+      <c r="V2" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
         <v>20</v>
       </c>
@@ -2802,26 +2896,32 @@
       <c r="N3" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="O3" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="P3" s="22" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="R3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="S3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="T3" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="S3" s="6" t="s">
+      <c r="U3" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="T3" s="6" t="s">
+      <c r="V3" s="6" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A4" s="8">
         <v>13010001</v>
       </c>
@@ -2853,23 +2953,25 @@
       <c r="M4" s="9"/>
       <c r="N4" s="9"/>
       <c r="O4" s="9"/>
-      <c r="P4" s="9" t="s">
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="Q4" s="9" t="s">
+      <c r="S4" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="R4" s="9" t="s">
+      <c r="T4" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="S4" s="9">
+      <c r="U4" s="9">
         <v>1348</v>
       </c>
-      <c r="T4" s="9">
+      <c r="V4" s="9">
         <v>611</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A5" s="8">
         <v>13010002</v>
       </c>
@@ -2905,23 +3007,25 @@
       </c>
       <c r="N5" s="9"/>
       <c r="O5" s="9"/>
-      <c r="P5" s="9" t="s">
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="Q5" s="9" t="s">
+      <c r="S5" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="R5" s="9" t="s">
+      <c r="T5" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="S5" s="9">
+      <c r="U5" s="9">
         <v>1279</v>
       </c>
-      <c r="T5" s="9">
+      <c r="V5" s="9">
         <v>571</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A6" s="8">
         <v>13010004</v>
       </c>
@@ -2955,23 +3059,25 @@
       <c r="M6" s="9"/>
       <c r="N6" s="9"/>
       <c r="O6" s="9"/>
-      <c r="P6" s="9" t="s">
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="Q6" s="9" t="s">
+      <c r="S6" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="R6" s="9" t="s">
+      <c r="T6" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="S6" s="9">
+      <c r="U6" s="9">
         <v>1148</v>
       </c>
-      <c r="T6" s="9">
+      <c r="V6" s="9">
         <v>351</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A7" s="8">
         <v>13010005</v>
       </c>
@@ -3005,23 +3111,25 @@
       <c r="M7" s="9"/>
       <c r="N7" s="9"/>
       <c r="O7" s="9"/>
-      <c r="P7" s="9" t="s">
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="Q7" s="9" t="s">
+      <c r="S7" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="R7" s="9" t="s">
+      <c r="T7" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="S7" s="9">
+      <c r="U7" s="9">
         <v>1386</v>
       </c>
-      <c r="T7" s="9">
+      <c r="V7" s="9">
         <v>339</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A8" s="8">
         <v>13010006</v>
       </c>
@@ -3047,23 +3155,25 @@
       <c r="M8" s="9"/>
       <c r="N8" s="9"/>
       <c r="O8" s="9"/>
-      <c r="P8" s="9" t="s">
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="Q8" s="9" t="s">
+      <c r="S8" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="R8" s="9" t="s">
+      <c r="T8" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="S8" s="9">
+      <c r="U8" s="9">
         <v>1232</v>
       </c>
-      <c r="T8" s="9">
+      <c r="V8" s="9">
         <v>506</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A9" s="8">
         <v>13010007</v>
       </c>
@@ -3091,31 +3201,33 @@
       </c>
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
-      <c r="L9" s="9">
-        <v>1</v>
-      </c>
+      <c r="L9" s="9"/>
       <c r="M9" s="9">
         <v>1</v>
       </c>
       <c r="N9" s="9"/>
       <c r="O9" s="9"/>
-      <c r="P9" s="9" t="s">
+      <c r="P9" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="Q9" s="9" t="s">
+      <c r="S9" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="R9" s="9" t="s">
+      <c r="T9" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="S9" s="9">
+      <c r="U9" s="9">
         <v>1431</v>
       </c>
-      <c r="T9" s="9">
+      <c r="V9" s="9">
         <v>440</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A10" s="8">
         <v>13010009</v>
       </c>
@@ -3151,23 +3263,25 @@
       <c r="M10" s="9"/>
       <c r="N10" s="9"/>
       <c r="O10" s="9"/>
-      <c r="P10" s="9" t="s">
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="Q10" s="9" t="s">
+      <c r="S10" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="R10" s="9" t="s">
+      <c r="T10" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="S10" s="9">
+      <c r="U10" s="9">
         <v>1332</v>
       </c>
-      <c r="T10" s="9">
+      <c r="V10" s="9">
         <v>484</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A11" s="8">
         <v>13010010</v>
       </c>
@@ -3200,24 +3314,28 @@
       <c r="N11" s="9">
         <v>1</v>
       </c>
-      <c r="O11" s="9"/>
-      <c r="P11" s="9" t="s">
+      <c r="O11" s="9">
+        <v>1</v>
+      </c>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="Q11" s="9" t="s">
+      <c r="S11" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="R11" s="9" t="s">
+      <c r="T11" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="S11" s="9">
+      <c r="U11" s="9">
         <v>1441</v>
       </c>
-      <c r="T11" s="9">
+      <c r="V11" s="9">
         <v>527</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A12" s="8">
         <v>13010011</v>
       </c>
@@ -3251,23 +3369,27 @@
       <c r="M12" s="9"/>
       <c r="N12" s="9"/>
       <c r="O12" s="9"/>
-      <c r="P12" s="9" t="s">
+      <c r="P12" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="Q12" s="9" t="s">
+      <c r="S12" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="R12" s="9" t="s">
+      <c r="T12" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="S12" s="9">
+      <c r="U12" s="9">
         <v>1574</v>
       </c>
-      <c r="T12" s="9">
+      <c r="V12" s="9">
         <v>373</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A13" s="8">
         <v>13010012</v>
       </c>
@@ -3299,23 +3421,25 @@
       <c r="M13" s="9"/>
       <c r="N13" s="9"/>
       <c r="O13" s="9"/>
-      <c r="P13" s="9" t="s">
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="Q13" s="9" t="s">
+      <c r="S13" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="R13" s="9" t="s">
+      <c r="T13" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="S13" s="9">
+      <c r="U13" s="9">
         <v>1251</v>
       </c>
-      <c r="T13" s="9">
+      <c r="V13" s="9">
         <v>432</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A14" s="8">
         <v>13010013</v>
       </c>
@@ -3346,24 +3470,28 @@
       <c r="L14" s="9"/>
       <c r="M14" s="9"/>
       <c r="N14" s="9"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="9" t="s">
+      <c r="O14" s="9">
+        <v>1</v>
+      </c>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="Q14" s="9" t="s">
+      <c r="S14" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="R14" s="9" t="s">
+      <c r="T14" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="S14" s="9">
+      <c r="U14" s="9">
         <v>1250</v>
       </c>
-      <c r="T14" s="9">
+      <c r="V14" s="9">
         <v>338</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A15" s="8">
         <v>13010014</v>
       </c>
@@ -3399,23 +3527,25 @@
         <v>1</v>
       </c>
       <c r="O15" s="9"/>
-      <c r="P15" s="9" t="s">
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="Q15" s="9" t="s">
+      <c r="S15" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="R15" s="9" t="s">
+      <c r="T15" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="S15" s="9">
+      <c r="U15" s="9">
         <v>1550</v>
       </c>
-      <c r="T15" s="9">
+      <c r="V15" s="9">
         <v>505</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A16" s="8">
         <v>13010015</v>
       </c>
@@ -3447,17 +3577,19 @@
       <c r="M16" s="11"/>
       <c r="N16" s="11"/>
       <c r="O16" s="11"/>
-      <c r="P16" s="11" t="s">
+      <c r="P16" s="11"/>
+      <c r="Q16" s="11"/>
+      <c r="R16" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="Q16" s="11" t="s">
+      <c r="S16" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="R16" s="11"/>
-      <c r="S16" s="11"/>
       <c r="T16" s="11"/>
+      <c r="U16" s="11"/>
+      <c r="V16" s="11"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A17" s="12">
         <v>13010101</v>
       </c>
@@ -3483,23 +3615,25 @@
       <c r="M17" s="9"/>
       <c r="N17" s="9"/>
       <c r="O17" s="9"/>
-      <c r="P17" s="9" t="s">
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="Q17" s="9" t="s">
+      <c r="S17" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="R17" s="9" t="s">
+      <c r="T17" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="S17" s="9">
+      <c r="U17" s="9">
         <v>919</v>
       </c>
-      <c r="T17" s="9">
+      <c r="V17" s="9">
         <v>534</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A18" s="12">
         <v>13010102</v>
       </c>
@@ -3533,23 +3667,25 @@
       <c r="M18" s="9"/>
       <c r="N18" s="9"/>
       <c r="O18" s="9"/>
-      <c r="P18" s="9" t="s">
+      <c r="P18" s="9"/>
+      <c r="Q18" s="9"/>
+      <c r="R18" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="Q18" s="9" t="s">
+      <c r="S18" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="R18" s="9" t="s">
+      <c r="T18" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="S18" s="9">
+      <c r="U18" s="9">
         <v>1040</v>
       </c>
-      <c r="T18" s="9">
+      <c r="V18" s="9">
         <v>538</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A19" s="12">
         <v>13010103</v>
       </c>
@@ -3581,23 +3717,25 @@
       <c r="M19" s="9"/>
       <c r="N19" s="9"/>
       <c r="O19" s="9"/>
-      <c r="P19" s="9" t="s">
+      <c r="P19" s="9"/>
+      <c r="Q19" s="9"/>
+      <c r="R19" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="Q19" s="9" t="s">
+      <c r="S19" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="R19" s="9" t="s">
+      <c r="T19" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="S19" s="9">
+      <c r="U19" s="9">
         <v>1213</v>
       </c>
-      <c r="T19" s="9">
+      <c r="V19" s="9">
         <v>655</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A20" s="12">
         <v>13010104</v>
       </c>
@@ -3631,23 +3769,25 @@
       </c>
       <c r="N20" s="9"/>
       <c r="O20" s="9"/>
-      <c r="P20" s="9" t="s">
+      <c r="P20" s="9"/>
+      <c r="Q20" s="9"/>
+      <c r="R20" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="Q20" s="9" t="s">
+      <c r="S20" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="R20" s="9" t="s">
+      <c r="T20" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="S20" s="9">
+      <c r="U20" s="9">
         <v>1149</v>
       </c>
-      <c r="T20" s="9">
+      <c r="V20" s="9">
         <v>584</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A21" s="12">
         <v>13010105</v>
       </c>
@@ -3677,23 +3817,25 @@
       <c r="M21" s="9"/>
       <c r="N21" s="9"/>
       <c r="O21" s="9"/>
-      <c r="P21" s="9" t="s">
+      <c r="P21" s="9"/>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="Q21" s="9" t="s">
+      <c r="S21" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="R21" s="9" t="s">
+      <c r="T21" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="S21" s="9">
+      <c r="U21" s="9">
         <v>840</v>
       </c>
-      <c r="T21" s="9">
+      <c r="V21" s="9">
         <v>444</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A22" s="12">
         <v>13010106</v>
       </c>
@@ -3727,23 +3869,25 @@
         <v>1</v>
       </c>
       <c r="O22" s="9"/>
-      <c r="P22" s="9" t="s">
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="Q22" s="9" t="s">
+      <c r="S22" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="R22" s="9" t="s">
+      <c r="T22" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="S22" s="9">
+      <c r="U22" s="9">
         <v>1067</v>
       </c>
-      <c r="T22" s="9">
+      <c r="V22" s="9">
         <v>445</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A23" s="13">
         <v>13020001</v>
       </c>
@@ -3773,17 +3917,19 @@
       <c r="M23" s="9"/>
       <c r="N23" s="9"/>
       <c r="O23" s="9"/>
-      <c r="P23" s="9" t="s">
+      <c r="P23" s="9"/>
+      <c r="Q23" s="9"/>
+      <c r="R23" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="Q23" s="9" t="s">
+      <c r="S23" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="R23" s="9"/>
-      <c r="S23" s="9"/>
       <c r="T23" s="9"/>
+      <c r="U23" s="9"/>
+      <c r="V23" s="9"/>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A24" s="13">
         <v>13020002</v>
       </c>
@@ -3809,17 +3955,19 @@
       <c r="M24" s="9"/>
       <c r="N24" s="9"/>
       <c r="O24" s="9"/>
-      <c r="P24" s="9" t="s">
+      <c r="P24" s="9"/>
+      <c r="Q24" s="9"/>
+      <c r="R24" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="Q24" s="9" t="s">
+      <c r="S24" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="R24" s="9"/>
-      <c r="S24" s="9"/>
       <c r="T24" s="9"/>
+      <c r="U24" s="9"/>
+      <c r="V24" s="9"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A25" s="13">
         <v>13020011</v>
       </c>
@@ -3849,17 +3997,19 @@
       <c r="M25" s="9"/>
       <c r="N25" s="9"/>
       <c r="O25" s="9"/>
-      <c r="P25" s="9" t="s">
+      <c r="P25" s="9"/>
+      <c r="Q25" s="9"/>
+      <c r="R25" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="Q25" s="9" t="s">
+      <c r="S25" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="R25" s="9"/>
-      <c r="S25" s="9"/>
       <c r="T25" s="9"/>
+      <c r="U25" s="9"/>
+      <c r="V25" s="9"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A26" s="13">
         <v>13020012</v>
       </c>
@@ -3887,17 +4037,19 @@
       <c r="M26" s="9"/>
       <c r="N26" s="9"/>
       <c r="O26" s="9"/>
-      <c r="P26" s="9" t="s">
+      <c r="P26" s="9"/>
+      <c r="Q26" s="9"/>
+      <c r="R26" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="Q26" s="9" t="s">
+      <c r="S26" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="R26" s="9"/>
-      <c r="S26" s="9"/>
       <c r="T26" s="9"/>
+      <c r="U26" s="9"/>
+      <c r="V26" s="9"/>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A27" s="13">
         <v>13020013</v>
       </c>
@@ -3923,17 +4075,19 @@
       <c r="M27" s="9"/>
       <c r="N27" s="9"/>
       <c r="O27" s="9"/>
-      <c r="P27" s="9" t="s">
+      <c r="P27" s="9"/>
+      <c r="Q27" s="9"/>
+      <c r="R27" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="Q27" s="9" t="s">
+      <c r="S27" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="R27" s="9"/>
-      <c r="S27" s="9"/>
       <c r="T27" s="9"/>
+      <c r="U27" s="9"/>
+      <c r="V27" s="9"/>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A28" s="13">
         <v>13020021</v>
       </c>
@@ -3965,17 +4119,19 @@
       <c r="M28" s="9"/>
       <c r="N28" s="9"/>
       <c r="O28" s="9"/>
-      <c r="P28" s="9" t="s">
+      <c r="P28" s="9"/>
+      <c r="Q28" s="9"/>
+      <c r="R28" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="Q28" s="9" t="s">
+      <c r="S28" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="R28" s="9"/>
-      <c r="S28" s="9"/>
       <c r="T28" s="9"/>
+      <c r="U28" s="9"/>
+      <c r="V28" s="9"/>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A29" s="13">
         <v>13020022</v>
       </c>
@@ -4007,17 +4163,19 @@
       <c r="M29" s="9"/>
       <c r="N29" s="9"/>
       <c r="O29" s="9"/>
-      <c r="P29" s="9" t="s">
+      <c r="P29" s="9"/>
+      <c r="Q29" s="9"/>
+      <c r="R29" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="Q29" s="9" t="s">
+      <c r="S29" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="R29" s="9"/>
-      <c r="S29" s="9"/>
       <c r="T29" s="9"/>
+      <c r="U29" s="9"/>
+      <c r="V29" s="9"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A30" s="13">
         <v>13020023</v>
       </c>
@@ -4049,17 +4207,19 @@
       <c r="M30" s="9"/>
       <c r="N30" s="9"/>
       <c r="O30" s="9"/>
-      <c r="P30" s="9" t="s">
+      <c r="P30" s="9"/>
+      <c r="Q30" s="9"/>
+      <c r="R30" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="Q30" s="9" t="s">
+      <c r="S30" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="R30" s="9"/>
-      <c r="S30" s="9"/>
       <c r="T30" s="9"/>
+      <c r="U30" s="9"/>
+      <c r="V30" s="9"/>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A31" s="14">
         <v>13020031</v>
       </c>
@@ -4087,17 +4247,19 @@
       <c r="M31" s="15"/>
       <c r="N31" s="15"/>
       <c r="O31" s="15"/>
-      <c r="P31" s="9" t="s">
+      <c r="P31" s="15"/>
+      <c r="Q31" s="15"/>
+      <c r="R31" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="Q31" s="15" t="s">
+      <c r="S31" s="15" t="s">
         <v>188</v>
       </c>
-      <c r="R31" s="15"/>
-      <c r="S31" s="15"/>
       <c r="T31" s="15"/>
+      <c r="U31" s="15"/>
+      <c r="V31" s="15"/>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A32" s="14">
         <v>13020032</v>
       </c>
@@ -4125,17 +4287,19 @@
       <c r="M32" s="15"/>
       <c r="N32" s="15"/>
       <c r="O32" s="15"/>
-      <c r="P32" s="9" t="s">
+      <c r="P32" s="15"/>
+      <c r="Q32" s="15"/>
+      <c r="R32" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="Q32" s="15" t="s">
+      <c r="S32" s="15" t="s">
         <v>189</v>
       </c>
-      <c r="R32" s="15"/>
-      <c r="S32" s="15"/>
       <c r="T32" s="15"/>
+      <c r="U32" s="15"/>
+      <c r="V32" s="15"/>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A33" s="14">
         <v>13020033</v>
       </c>
@@ -4163,17 +4327,19 @@
       <c r="M33" s="15"/>
       <c r="N33" s="15"/>
       <c r="O33" s="15"/>
-      <c r="P33" s="9" t="s">
+      <c r="P33" s="15"/>
+      <c r="Q33" s="15"/>
+      <c r="R33" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="Q33" s="15" t="s">
+      <c r="S33" s="15" t="s">
         <v>190</v>
       </c>
-      <c r="R33" s="16"/>
-      <c r="S33" s="16"/>
       <c r="T33" s="16"/>
+      <c r="U33" s="16"/>
+      <c r="V33" s="16"/>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A34" s="14">
         <v>13020034</v>
       </c>
@@ -4201,17 +4367,19 @@
       <c r="M34" s="15"/>
       <c r="N34" s="15"/>
       <c r="O34" s="15"/>
-      <c r="P34" s="9" t="s">
+      <c r="P34" s="15"/>
+      <c r="Q34" s="15"/>
+      <c r="R34" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="Q34" s="15" t="s">
+      <c r="S34" s="15" t="s">
         <v>191</v>
       </c>
-      <c r="R34" s="16"/>
-      <c r="S34" s="16"/>
       <c r="T34" s="16"/>
+      <c r="U34" s="16"/>
+      <c r="V34" s="16"/>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A35" s="14">
         <v>13020035</v>
       </c>
@@ -4239,30 +4407,32 @@
       <c r="M35" s="15"/>
       <c r="N35" s="15"/>
       <c r="O35" s="15"/>
-      <c r="P35" s="9" t="s">
+      <c r="P35" s="15"/>
+      <c r="Q35" s="15"/>
+      <c r="R35" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="Q35" s="15" t="s">
+      <c r="S35" s="15" t="s">
         <v>192</v>
       </c>
-      <c r="R35" s="16"/>
-      <c r="S35" s="16"/>
       <c r="T35" s="16"/>
+      <c r="U35" s="16"/>
+      <c r="V35" s="16"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="I4:N35">
-    <cfRule type="cellIs" dxfId="25" priority="4" operator="equal">
+  <conditionalFormatting sqref="I4:P35">
+    <cfRule type="cellIs" dxfId="27" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4">
-    <cfRule type="cellIs" dxfId="24" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4:H35">
-    <cfRule type="containsBlanks" dxfId="23" priority="5">
+    <cfRule type="containsBlanks" dxfId="25" priority="5">
       <formula>LEN(TRIM(F4))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
add some new map icons
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Scene.xlsx
+++ b/ConfigData/Xlsx/Scene.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="235">
   <si>
     <t>村外小屋</t>
   </si>
@@ -807,6 +807,86 @@
   </si>
   <si>
     <t>woodviliage</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>风悦石林北</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>风悦石林南</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>fyslb</t>
+  </si>
+  <si>
+    <t>fysln</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>石林迷窟</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>slmk</t>
+  </si>
+  <si>
+    <t>hmgd</t>
+  </si>
+  <si>
+    <t>bszx</t>
+  </si>
+  <si>
+    <t>html</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>hdyz</t>
+  </si>
+  <si>
+    <t>lshj</t>
+  </si>
+  <si>
+    <t>wxzd</t>
+  </si>
+  <si>
+    <t>ljhna</t>
+  </si>
+  <si>
+    <t>hsk</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>维述儿火山</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>卡夫金字塔</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>顿河南岸</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>流沙幻境</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>断臂角</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>鲁高因</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>库斯特树林</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>日落古道</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1030,7 +1110,6 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -1533,59 +1612,8 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="38" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="39" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1600,7 +1628,55 @@
     <xf numFmtId="0" fontId="19" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="255" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="38" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="39" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="39" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1649,6 +1725,27 @@
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="28">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2303,27 +2400,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2338,34 +2414,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A3:V35" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23" tableBorderDxfId="22">
-  <autoFilter ref="A3:V35" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState ref="A4:V27">
-    <sortCondition ref="A3:A27"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A3:V46" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26" tableBorderDxfId="25">
+  <autoFilter ref="A3:V46" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState ref="A4:V38">
+    <sortCondition ref="A3:A38"/>
   </sortState>
   <tableColumns count="22">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="20"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Type" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Level" dataDxfId="18"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="ReviveScene" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Quest" dataDxfId="16"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="QuestRandom" dataDxfId="15"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="QuestDungeon" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="QPortal" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="QCardChange" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="QPiece" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="QMerchant" dataDxfId="10"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="QDoctor" dataDxfId="9"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="QAngel" dataDxfId="8"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="QWheel" dataDxfId="7"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="QRes" dataDxfId="6"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Func" dataDxfId="5"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Url" dataDxfId="4"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="TilePath" dataDxfId="3"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Icon" dataDxfId="2"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="IconX" dataDxfId="1"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="IconY" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="23"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Type" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Level" dataDxfId="21"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="ReviveScene" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Quest" dataDxfId="19"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="QuestRandom" dataDxfId="18"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="QuestDungeon" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="QPortal" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="QCardChange" dataDxfId="15"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="QPiece" dataDxfId="14"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="QMerchant" dataDxfId="13"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="QDoctor" dataDxfId="12"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="QAngel" dataDxfId="11"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="QWheel" dataDxfId="10"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="QRes" dataDxfId="9"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Func" dataDxfId="8"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Url" dataDxfId="7"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="TilePath" dataDxfId="6"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Icon" dataDxfId="5"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="IconX" dataDxfId="4"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="IconY" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2692,1634 +2768,1660 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V35"/>
+  <dimension ref="A1:V46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="11.125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="5.125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="4.375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9" style="1" customWidth="1"/>
-    <col min="6" max="6" width="52.875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="23.625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="50.875" style="1" customWidth="1"/>
-    <col min="9" max="16" width="3.125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="6.625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="9.75" style="1" customWidth="1"/>
-    <col min="19" max="19" width="9.5" style="1" customWidth="1"/>
-    <col min="20" max="20" width="7.25" style="1" customWidth="1"/>
-    <col min="21" max="22" width="6" style="1" customWidth="1"/>
-    <col min="23" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="11.125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="10.625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="5.125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="4.375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="9" style="5" customWidth="1"/>
+    <col min="6" max="6" width="52.875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="23.625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="50.875" style="5" customWidth="1"/>
+    <col min="9" max="16" width="3.125" style="5" customWidth="1"/>
+    <col min="17" max="17" width="6.625" style="5" customWidth="1"/>
+    <col min="18" max="18" width="9.75" style="5" customWidth="1"/>
+    <col min="19" max="19" width="9.5" style="5" customWidth="1"/>
+    <col min="20" max="20" width="7.25" style="5" customWidth="1"/>
+    <col min="21" max="22" width="6" style="5" customWidth="1"/>
+    <col min="23" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="60" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="H1" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="J1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="K1" s="20" t="s">
+      <c r="K1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="L1" s="20" t="s">
+      <c r="L1" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="M1" s="20" t="s">
+      <c r="M1" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="N1" s="20" t="s">
+      <c r="N1" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="O1" s="20" t="s">
+      <c r="O1" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="P1" s="20" t="s">
+      <c r="P1" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="Q1" s="19" t="s">
+      <c r="Q1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="R1" s="19" t="s">
+      <c r="R1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="S1" s="19" t="s">
+      <c r="S1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="T1" s="19" t="s">
+      <c r="T1" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="U1" s="19" t="s">
+      <c r="U1" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="V1" s="21" t="s">
+      <c r="V1" s="4" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="N2" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="O2" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="P2" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="Q2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="R2" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="S2" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="T2" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="U2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="V2" s="5" t="s">
+      <c r="V2" s="9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J3" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="K3" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="L3" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="M3" s="7" t="s">
+      <c r="M3" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="N3" s="7" t="s">
+      <c r="N3" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="O3" s="22" t="s">
+      <c r="O3" s="11" t="s">
         <v>210</v>
       </c>
-      <c r="P3" s="22" t="s">
+      <c r="P3" s="11" t="s">
         <v>211</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="Q3" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="R3" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="S3" s="6" t="s">
+      <c r="S3" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="T3" s="6" t="s">
+      <c r="T3" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="U3" s="6" t="s">
+      <c r="U3" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="V3" s="6" t="s">
+      <c r="V3" s="10" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A4" s="8">
+      <c r="A4" s="12">
         <v>13010001</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="13">
         <v>2</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="13">
         <v>1</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="13">
         <v>13010001</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="14" t="s">
         <v>200</v>
       </c>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9">
+      <c r="H4" s="13"/>
+      <c r="I4" s="13">
         <v>1</v>
       </c>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9"/>
-      <c r="Q4" s="9"/>
-      <c r="R4" s="9" t="s">
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="13"/>
+      <c r="Q4" s="13"/>
+      <c r="R4" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="S4" s="9" t="s">
+      <c r="S4" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="T4" s="9" t="s">
+      <c r="T4" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="U4" s="9">
+      <c r="U4" s="13">
         <v>1348</v>
       </c>
-      <c r="V4" s="9">
+      <c r="V4" s="13">
         <v>611</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A5" s="8">
+      <c r="A5" s="12">
         <v>13010002</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="13">
         <v>2</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="13">
         <v>2</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="13">
         <v>13010001</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9">
+      <c r="H5" s="13"/>
+      <c r="I5" s="13">
         <v>1</v>
       </c>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9">
+      <c r="J5" s="13"/>
+      <c r="K5" s="13">
         <v>1</v>
       </c>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9">
+      <c r="L5" s="13"/>
+      <c r="M5" s="13">
         <v>1</v>
       </c>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="9"/>
-      <c r="Q5" s="9"/>
-      <c r="R5" s="9" t="s">
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="13"/>
+      <c r="R5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="S5" s="9" t="s">
+      <c r="S5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="T5" s="9" t="s">
+      <c r="T5" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="U5" s="9">
+      <c r="U5" s="13">
         <v>1279</v>
       </c>
-      <c r="V5" s="9">
+      <c r="V5" s="13">
         <v>571</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A6" s="8">
+      <c r="A6" s="12">
         <v>13010004</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="13">
         <v>2</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="13">
         <v>5</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="13">
         <v>13010006</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9">
+      <c r="H6" s="13"/>
+      <c r="I6" s="13">
         <v>1</v>
       </c>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9">
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13">
         <v>1</v>
       </c>
-      <c r="M6" s="9"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="9"/>
-      <c r="Q6" s="9"/>
-      <c r="R6" s="9" t="s">
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="S6" s="9" t="s">
+      <c r="S6" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="T6" s="9" t="s">
+      <c r="T6" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="U6" s="9">
+      <c r="U6" s="13">
         <v>1148</v>
       </c>
-      <c r="V6" s="9">
+      <c r="V6" s="13">
         <v>351</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A7" s="8">
+      <c r="A7" s="12">
         <v>13010005</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="13">
         <v>2</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="13">
         <v>8</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="13">
         <v>13010006</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="13" t="s">
         <v>173</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9">
+      <c r="H7" s="13"/>
+      <c r="I7" s="13">
         <v>1</v>
       </c>
-      <c r="J7" s="9">
+      <c r="J7" s="13">
         <v>1</v>
       </c>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="9"/>
-      <c r="Q7" s="9"/>
-      <c r="R7" s="9" t="s">
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="13"/>
+      <c r="R7" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="S7" s="9" t="s">
+      <c r="S7" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="T7" s="9" t="s">
+      <c r="T7" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="U7" s="9">
+      <c r="U7" s="13">
         <v>1386</v>
       </c>
-      <c r="V7" s="9">
+      <c r="V7" s="13">
         <v>339</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A8" s="8">
+      <c r="A8" s="12">
         <v>13010006</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="13">
         <v>1</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="13">
         <v>3</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="13">
         <v>13010006</v>
       </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
-      <c r="P8" s="9"/>
-      <c r="Q8" s="9"/>
-      <c r="R8" s="9" t="s">
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="13"/>
+      <c r="R8" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="S8" s="9" t="s">
+      <c r="S8" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="T8" s="9" t="s">
+      <c r="T8" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="U8" s="9">
+      <c r="U8" s="13">
         <v>1232</v>
       </c>
-      <c r="V8" s="9">
+      <c r="V8" s="13">
         <v>506</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A9" s="8">
+      <c r="A9" s="12">
         <v>13010007</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="13">
         <v>2</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="13">
         <v>7</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="13">
         <v>13010006</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G9" s="13" t="s">
         <v>175</v>
       </c>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9">
+      <c r="H9" s="13"/>
+      <c r="I9" s="13">
         <v>1</v>
       </c>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9">
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13">
         <v>1</v>
       </c>
-      <c r="N9" s="9"/>
-      <c r="O9" s="9"/>
-      <c r="P9" s="9">
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13">
         <v>1</v>
       </c>
-      <c r="Q9" s="9"/>
-      <c r="R9" s="9" t="s">
+      <c r="Q9" s="13"/>
+      <c r="R9" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="S9" s="9" t="s">
+      <c r="S9" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="T9" s="9" t="s">
+      <c r="T9" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="U9" s="9">
+      <c r="U9" s="13">
         <v>1431</v>
       </c>
-      <c r="V9" s="9">
+      <c r="V9" s="13">
         <v>440</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A10" s="8">
+      <c r="A10" s="12">
         <v>13010009</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="13">
         <v>2</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="13">
         <v>4</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="13">
         <v>13010006</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="13" t="s">
         <v>170</v>
       </c>
-      <c r="G10" s="17" t="s">
+      <c r="G10" s="13" t="s">
         <v>201</v>
       </c>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9">
+      <c r="H10" s="13"/>
+      <c r="I10" s="13">
         <v>1</v>
       </c>
-      <c r="J10" s="9">
+      <c r="J10" s="13">
         <v>1</v>
       </c>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9">
+      <c r="K10" s="13"/>
+      <c r="L10" s="13">
         <v>1</v>
       </c>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="9"/>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="9" t="s">
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="13"/>
+      <c r="R10" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="S10" s="9" t="s">
+      <c r="S10" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="T10" s="9" t="s">
+      <c r="T10" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="U10" s="9">
+      <c r="U10" s="13">
         <v>1332</v>
       </c>
-      <c r="V10" s="9">
+      <c r="V10" s="13">
         <v>484</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A11" s="8">
+      <c r="A11" s="12">
         <v>13010010</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="13">
         <v>2</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="13">
         <v>13010006</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="13" t="s">
         <v>179</v>
       </c>
-      <c r="G11" s="17" t="s">
+      <c r="G11" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9">
+      <c r="H11" s="13"/>
+      <c r="I11" s="13">
         <v>1</v>
       </c>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="9">
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13">
         <v>1</v>
       </c>
-      <c r="O11" s="9">
+      <c r="O11" s="13">
         <v>1</v>
       </c>
-      <c r="P11" s="9"/>
-      <c r="Q11" s="9"/>
-      <c r="R11" s="9" t="s">
+      <c r="P11" s="13"/>
+      <c r="Q11" s="13"/>
+      <c r="R11" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="S11" s="9" t="s">
+      <c r="S11" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="T11" s="9" t="s">
+      <c r="T11" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="U11" s="9">
+      <c r="U11" s="13">
         <v>1441</v>
       </c>
-      <c r="V11" s="9">
+      <c r="V11" s="13">
         <v>527</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A12" s="8">
+      <c r="A12" s="12">
         <v>13010011</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="13">
         <v>2</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="13">
         <v>12</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="13">
         <v>13010006</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F12" s="13" t="s">
         <v>178</v>
       </c>
-      <c r="G12" s="9" t="s">
+      <c r="G12" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9">
+      <c r="H12" s="13"/>
+      <c r="I12" s="13">
         <v>1</v>
       </c>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9">
+      <c r="J12" s="13"/>
+      <c r="K12" s="13">
         <v>1</v>
       </c>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="9">
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="13"/>
+      <c r="P12" s="13">
         <v>1</v>
       </c>
-      <c r="Q12" s="9"/>
-      <c r="R12" s="9" t="s">
+      <c r="Q12" s="13"/>
+      <c r="R12" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="S12" s="9" t="s">
+      <c r="S12" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="T12" s="9" t="s">
+      <c r="T12" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="U12" s="9">
+      <c r="U12" s="13">
         <v>1574</v>
       </c>
-      <c r="V12" s="9">
+      <c r="V12" s="13">
         <v>373</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A13" s="8">
+      <c r="A13" s="12">
         <v>13010012</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="13">
         <v>2</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="13">
         <v>3</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="13">
         <v>13010006</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="F13" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="G13" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9">
+      <c r="H13" s="13"/>
+      <c r="I13" s="13">
         <v>1</v>
       </c>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="9"/>
-      <c r="Q13" s="9"/>
-      <c r="R13" s="9" t="s">
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
+      <c r="P13" s="13"/>
+      <c r="Q13" s="13"/>
+      <c r="R13" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="S13" s="9" t="s">
+      <c r="S13" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="T13" s="9" t="s">
+      <c r="T13" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="U13" s="9">
+      <c r="U13" s="13">
         <v>1251</v>
       </c>
-      <c r="V13" s="9">
+      <c r="V13" s="13">
         <v>432</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A14" s="8">
+      <c r="A14" s="12">
         <v>13010013</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="13">
         <v>2</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="13">
         <v>6</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="13">
         <v>13010006</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="F14" s="13" t="s">
         <v>160</v>
       </c>
-      <c r="G14" s="9" t="s">
+      <c r="G14" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9">
+      <c r="H14" s="13"/>
+      <c r="I14" s="13">
         <v>1</v>
       </c>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="9">
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13">
         <v>1</v>
       </c>
-      <c r="P14" s="9"/>
-      <c r="Q14" s="9"/>
-      <c r="R14" s="9" t="s">
+      <c r="P14" s="13"/>
+      <c r="Q14" s="13"/>
+      <c r="R14" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="S14" s="9" t="s">
+      <c r="S14" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="T14" s="9" t="s">
+      <c r="T14" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="U14" s="9">
+      <c r="U14" s="13">
         <v>1250</v>
       </c>
-      <c r="V14" s="9">
+      <c r="V14" s="13">
         <v>338</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A15" s="8">
+      <c r="A15" s="12">
         <v>13010014</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="13">
         <v>2</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="13">
         <v>14</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="13">
         <v>13010006</v>
       </c>
-      <c r="F15" s="9" t="s">
+      <c r="F15" s="13" t="s">
         <v>172</v>
       </c>
-      <c r="G15" s="9" t="s">
+      <c r="G15" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9">
+      <c r="H15" s="13"/>
+      <c r="I15" s="13">
         <v>1</v>
       </c>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="9"/>
-      <c r="M15" s="9">
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13">
         <v>1</v>
       </c>
-      <c r="N15" s="9">
+      <c r="N15" s="13">
         <v>1</v>
       </c>
-      <c r="O15" s="9"/>
-      <c r="P15" s="9"/>
-      <c r="Q15" s="9"/>
-      <c r="R15" s="9" t="s">
+      <c r="O15" s="13"/>
+      <c r="P15" s="13"/>
+      <c r="Q15" s="13"/>
+      <c r="R15" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="S15" s="9" t="s">
+      <c r="S15" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="T15" s="9" t="s">
+      <c r="T15" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="U15" s="9">
+      <c r="U15" s="13">
         <v>1550</v>
       </c>
-      <c r="V15" s="9">
+      <c r="V15" s="13">
         <v>505</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A16" s="8">
+      <c r="A16" s="12">
         <v>13010015</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="C16" s="11">
+      <c r="C16" s="15">
         <v>2</v>
       </c>
-      <c r="D16" s="11">
+      <c r="D16" s="15">
         <v>6</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="13">
         <v>13010006</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="F16" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="G16" s="9" t="s">
+      <c r="G16" s="13" t="s">
         <v>169</v>
       </c>
-      <c r="H16" s="9"/>
-      <c r="I16" s="11">
+      <c r="H16" s="13"/>
+      <c r="I16" s="15">
         <v>1</v>
       </c>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="11"/>
-      <c r="N16" s="11"/>
-      <c r="O16" s="11"/>
-      <c r="P16" s="11"/>
-      <c r="Q16" s="11"/>
-      <c r="R16" s="11" t="s">
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="15"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="15"/>
+      <c r="O16" s="15"/>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="15"/>
+      <c r="R16" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="S16" s="11" t="s">
+      <c r="S16" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="T16" s="11"/>
-      <c r="U16" s="11"/>
-      <c r="V16" s="11"/>
+      <c r="T16" s="15"/>
+      <c r="U16" s="15"/>
+      <c r="V16" s="15"/>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A17" s="12">
+      <c r="A17" s="16">
         <v>13010101</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17" s="13">
         <v>1</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D17" s="13">
         <v>16</v>
       </c>
-      <c r="E17" s="9">
+      <c r="E17" s="13">
         <v>13010101</v>
       </c>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="9"/>
-      <c r="P17" s="9"/>
-      <c r="Q17" s="9"/>
-      <c r="R17" s="17" t="s">
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="13"/>
+      <c r="O17" s="13"/>
+      <c r="P17" s="13"/>
+      <c r="Q17" s="13"/>
+      <c r="R17" s="13" t="s">
         <v>212</v>
       </c>
-      <c r="S17" s="9" t="s">
+      <c r="S17" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="T17" s="9" t="s">
+      <c r="T17" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="U17" s="9">
-        <v>919</v>
-      </c>
-      <c r="V17" s="9">
-        <v>534</v>
+      <c r="U17" s="13">
+        <v>894</v>
+      </c>
+      <c r="V17" s="13">
+        <v>509</v>
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A18" s="12">
+      <c r="A18" s="16">
         <v>13010102</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C18" s="13">
         <v>2</v>
       </c>
-      <c r="D18" s="9">
+      <c r="D18" s="13">
         <v>16</v>
       </c>
-      <c r="E18" s="9">
+      <c r="E18" s="13">
         <v>13010101</v>
       </c>
-      <c r="F18" s="9" t="s">
+      <c r="F18" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="G18" s="9" t="s">
+      <c r="G18" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9">
+      <c r="H18" s="13"/>
+      <c r="I18" s="13">
         <v>1</v>
       </c>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9">
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13">
         <v>1</v>
       </c>
-      <c r="M18" s="9"/>
-      <c r="N18" s="9"/>
-      <c r="O18" s="9"/>
-      <c r="P18" s="9"/>
-      <c r="Q18" s="9"/>
-      <c r="R18" s="9" t="s">
+      <c r="M18" s="13"/>
+      <c r="N18" s="13"/>
+      <c r="O18" s="13"/>
+      <c r="P18" s="13"/>
+      <c r="Q18" s="13"/>
+      <c r="R18" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="S18" s="9" t="s">
+      <c r="S18" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="T18" s="9" t="s">
+      <c r="T18" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="U18" s="9">
+      <c r="U18" s="13">
         <v>1040</v>
       </c>
-      <c r="V18" s="9">
+      <c r="V18" s="13">
         <v>538</v>
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A19" s="12">
+      <c r="A19" s="16">
         <v>13010103</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C19" s="13">
         <v>2</v>
       </c>
-      <c r="D19" s="9">
+      <c r="D19" s="13">
         <v>19</v>
       </c>
-      <c r="E19" s="9">
+      <c r="E19" s="13">
         <v>13010101</v>
       </c>
-      <c r="F19" s="9" t="s">
+      <c r="F19" s="13" t="s">
         <v>171</v>
       </c>
-      <c r="G19" s="17" t="s">
+      <c r="G19" s="13" t="s">
         <v>204</v>
       </c>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9">
+      <c r="H19" s="13"/>
+      <c r="I19" s="13">
         <v>1</v>
       </c>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="9"/>
-      <c r="O19" s="9"/>
-      <c r="P19" s="9"/>
-      <c r="Q19" s="9"/>
-      <c r="R19" s="9" t="s">
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="13"/>
+      <c r="P19" s="13"/>
+      <c r="Q19" s="13"/>
+      <c r="R19" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="S19" s="9" t="s">
+      <c r="S19" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="T19" s="9" t="s">
+      <c r="T19" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="U19" s="9">
+      <c r="U19" s="13">
         <v>1213</v>
       </c>
-      <c r="V19" s="9">
+      <c r="V19" s="13">
         <v>655</v>
       </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A20" s="12">
+      <c r="A20" s="16">
         <v>13010104</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C20" s="13">
         <v>2</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20" s="13">
         <v>18</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E20" s="13">
         <v>13010101</v>
       </c>
-      <c r="F20" s="9" t="s">
+      <c r="F20" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="G20" s="9" t="s">
+      <c r="G20" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9">
+      <c r="H20" s="13"/>
+      <c r="I20" s="13">
         <v>1</v>
       </c>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9">
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13">
         <v>1</v>
       </c>
-      <c r="N20" s="9"/>
-      <c r="O20" s="9"/>
-      <c r="P20" s="9"/>
-      <c r="Q20" s="9"/>
-      <c r="R20" s="9" t="s">
+      <c r="N20" s="13"/>
+      <c r="O20" s="13"/>
+      <c r="P20" s="13"/>
+      <c r="Q20" s="13"/>
+      <c r="R20" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="S20" s="9" t="s">
+      <c r="S20" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="T20" s="9" t="s">
+      <c r="T20" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="U20" s="9">
+      <c r="U20" s="13">
         <v>1149</v>
       </c>
-      <c r="V20" s="9">
+      <c r="V20" s="13">
         <v>584</v>
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A21" s="12">
+      <c r="A21" s="16">
         <v>13010105</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="9">
+      <c r="C21" s="13">
         <v>2</v>
       </c>
-      <c r="D21" s="9">
+      <c r="D21" s="13">
         <v>20</v>
       </c>
-      <c r="E21" s="9">
+      <c r="E21" s="13">
         <v>13010101</v>
       </c>
-      <c r="F21" s="9" t="s">
+      <c r="F21" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="G21" s="9" t="s">
+      <c r="G21" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
-      <c r="L21" s="9"/>
-      <c r="M21" s="9"/>
-      <c r="N21" s="9"/>
-      <c r="O21" s="9"/>
-      <c r="P21" s="9"/>
-      <c r="Q21" s="9"/>
-      <c r="R21" s="9" t="s">
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="13"/>
+      <c r="O21" s="13"/>
+      <c r="P21" s="13"/>
+      <c r="Q21" s="13"/>
+      <c r="R21" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="S21" s="9" t="s">
+      <c r="S21" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="T21" s="9" t="s">
+      <c r="T21" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="U21" s="9">
+      <c r="U21" s="13">
         <v>840</v>
       </c>
-      <c r="V21" s="9">
+      <c r="V21" s="13">
         <v>444</v>
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A22" s="12">
+      <c r="A22" s="16">
         <v>13010106</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="C22" s="9">
+      <c r="C22" s="13">
         <v>2</v>
       </c>
-      <c r="D22" s="9">
+      <c r="D22" s="13">
         <v>15</v>
       </c>
-      <c r="E22" s="9">
+      <c r="E22" s="13">
         <v>13010016</v>
       </c>
-      <c r="F22" s="9" t="s">
+      <c r="F22" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="G22" s="9" t="s">
+      <c r="G22" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9">
+      <c r="H22" s="13"/>
+      <c r="I22" s="13">
         <v>1</v>
       </c>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
-      <c r="L22" s="9"/>
-      <c r="M22" s="9"/>
-      <c r="N22" s="9">
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="13">
         <v>1</v>
       </c>
-      <c r="O22" s="9"/>
-      <c r="P22" s="9"/>
-      <c r="Q22" s="9"/>
-      <c r="R22" s="9" t="s">
+      <c r="O22" s="13"/>
+      <c r="P22" s="13"/>
+      <c r="Q22" s="13"/>
+      <c r="R22" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="S22" s="9" t="s">
+      <c r="S22" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="T22" s="9" t="s">
+      <c r="T22" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="U22" s="9">
+      <c r="U22" s="13">
         <v>1067</v>
       </c>
-      <c r="V22" s="9">
+      <c r="V22" s="13">
         <v>445</v>
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A23" s="13">
-        <v>13020001</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="C23" s="13">
-        <v>3</v>
-      </c>
-      <c r="D23" s="9">
-        <v>3</v>
-      </c>
-      <c r="E23" s="9">
-        <v>13010002</v>
-      </c>
-      <c r="F23" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
-      <c r="L23" s="9"/>
-      <c r="M23" s="9"/>
-      <c r="N23" s="9"/>
-      <c r="O23" s="9"/>
-      <c r="P23" s="9"/>
-      <c r="Q23" s="9"/>
-      <c r="R23" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="S23" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="T23" s="9"/>
-      <c r="U23" s="9"/>
-      <c r="V23" s="9"/>
+      <c r="A23" s="16">
+        <v>13010107</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>213</v>
+      </c>
+      <c r="C23" s="15">
+        <v>2</v>
+      </c>
+      <c r="D23" s="15">
+        <v>15</v>
+      </c>
+      <c r="E23" s="15">
+        <v>13010101</v>
+      </c>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="15"/>
+      <c r="O23" s="15"/>
+      <c r="P23" s="15"/>
+      <c r="Q23" s="15"/>
+      <c r="R23" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="S23" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="T23" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="U23" s="15">
+        <v>974</v>
+      </c>
+      <c r="V23" s="15">
+        <v>594</v>
+      </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A24" s="13">
-        <v>13020002</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="C24" s="13">
-        <v>3</v>
-      </c>
-      <c r="D24" s="9">
-        <v>3</v>
-      </c>
-      <c r="E24" s="9">
-        <v>13010002</v>
-      </c>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="9"/>
-      <c r="M24" s="9"/>
-      <c r="N24" s="9"/>
-      <c r="O24" s="9"/>
-      <c r="P24" s="9"/>
-      <c r="Q24" s="9"/>
-      <c r="R24" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="S24" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="T24" s="9"/>
-      <c r="U24" s="9"/>
-      <c r="V24" s="9"/>
+      <c r="A24" s="16">
+        <v>13010108</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>214</v>
+      </c>
+      <c r="C24" s="15">
+        <v>2</v>
+      </c>
+      <c r="D24" s="15">
+        <v>15</v>
+      </c>
+      <c r="E24" s="15">
+        <v>13010101</v>
+      </c>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="15"/>
+      <c r="M24" s="15"/>
+      <c r="N24" s="15"/>
+      <c r="O24" s="15"/>
+      <c r="P24" s="15"/>
+      <c r="Q24" s="15"/>
+      <c r="R24" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="S24" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="T24" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="U24" s="15">
+        <v>1080</v>
+      </c>
+      <c r="V24" s="15">
+        <v>720</v>
+      </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A25" s="13">
-        <v>13020011</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="C25" s="13">
-        <v>3</v>
-      </c>
-      <c r="D25" s="9">
-        <v>8</v>
-      </c>
-      <c r="E25" s="9">
-        <v>13010007</v>
-      </c>
-      <c r="F25" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="G25" s="17" t="s">
-        <v>206</v>
-      </c>
-      <c r="H25" s="9"/>
-      <c r="I25" s="9"/>
-      <c r="J25" s="9"/>
-      <c r="K25" s="9"/>
-      <c r="L25" s="9"/>
-      <c r="M25" s="9"/>
-      <c r="N25" s="9"/>
-      <c r="O25" s="9"/>
-      <c r="P25" s="9"/>
-      <c r="Q25" s="9"/>
-      <c r="R25" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="S25" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="T25" s="9"/>
-      <c r="U25" s="9"/>
-      <c r="V25" s="9"/>
+      <c r="A25" s="16">
+        <v>13010109</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>234</v>
+      </c>
+      <c r="C25" s="15">
+        <v>2</v>
+      </c>
+      <c r="D25" s="15">
+        <v>15</v>
+      </c>
+      <c r="E25" s="15">
+        <v>13010101</v>
+      </c>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="15"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="15"/>
+      <c r="L25" s="15"/>
+      <c r="M25" s="15"/>
+      <c r="N25" s="15"/>
+      <c r="O25" s="15"/>
+      <c r="P25" s="15"/>
+      <c r="Q25" s="15"/>
+      <c r="R25" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="S25" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="T25" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="U25" s="15">
+        <v>894</v>
+      </c>
+      <c r="V25" s="15">
+        <v>679</v>
+      </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A26" s="13">
-        <v>13020012</v>
-      </c>
-      <c r="B26" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="C26" s="13">
-        <v>3</v>
-      </c>
-      <c r="D26" s="9">
-        <v>8</v>
-      </c>
-      <c r="E26" s="9">
-        <v>13010007</v>
-      </c>
-      <c r="F26" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
-      <c r="J26" s="9"/>
-      <c r="K26" s="9"/>
-      <c r="L26" s="9"/>
-      <c r="M26" s="9"/>
-      <c r="N26" s="9"/>
-      <c r="O26" s="9"/>
-      <c r="P26" s="9"/>
-      <c r="Q26" s="9"/>
-      <c r="R26" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="S26" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="T26" s="9"/>
-      <c r="U26" s="9"/>
-      <c r="V26" s="9"/>
+      <c r="A26" s="16">
+        <v>13010110</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="C26" s="15">
+        <v>2</v>
+      </c>
+      <c r="D26" s="15">
+        <v>15</v>
+      </c>
+      <c r="E26" s="15">
+        <v>13010101</v>
+      </c>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="15"/>
+      <c r="K26" s="15"/>
+      <c r="L26" s="15"/>
+      <c r="M26" s="15"/>
+      <c r="N26" s="15"/>
+      <c r="O26" s="15"/>
+      <c r="P26" s="15"/>
+      <c r="Q26" s="15"/>
+      <c r="R26" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="S26" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="T26" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="U26" s="15">
+        <v>1074</v>
+      </c>
+      <c r="V26" s="15">
+        <v>630</v>
+      </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A27" s="13">
-        <v>13020013</v>
-      </c>
-      <c r="B27" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="C27" s="13">
-        <v>3</v>
-      </c>
-      <c r="D27" s="9">
-        <v>8</v>
-      </c>
-      <c r="E27" s="9">
-        <v>13010007</v>
-      </c>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="9"/>
-      <c r="L27" s="9"/>
-      <c r="M27" s="9"/>
-      <c r="N27" s="9"/>
-      <c r="O27" s="9"/>
-      <c r="P27" s="9"/>
-      <c r="Q27" s="9"/>
-      <c r="R27" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="S27" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="T27" s="9"/>
-      <c r="U27" s="9"/>
-      <c r="V27" s="9"/>
+      <c r="A27" s="16">
+        <v>13010111</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="C27" s="15">
+        <v>2</v>
+      </c>
+      <c r="D27" s="15">
+        <v>15</v>
+      </c>
+      <c r="E27" s="15">
+        <v>13010101</v>
+      </c>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="18"/>
+      <c r="L27" s="18"/>
+      <c r="M27" s="18"/>
+      <c r="N27" s="18"/>
+      <c r="O27" s="15"/>
+      <c r="P27" s="15"/>
+      <c r="Q27" s="18"/>
+      <c r="R27" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="S27" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="T27" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="U27" s="18">
+        <v>850</v>
+      </c>
+      <c r="V27" s="18">
+        <v>589</v>
+      </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A28" s="13">
-        <v>13020021</v>
-      </c>
-      <c r="B28" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C28" s="13">
-        <v>3</v>
-      </c>
-      <c r="D28" s="9">
-        <v>5</v>
-      </c>
-      <c r="E28" s="9">
-        <v>13010004</v>
-      </c>
-      <c r="F28" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="G28" s="17" t="s">
-        <v>198</v>
-      </c>
-      <c r="H28" s="9" t="s">
-        <v>192</v>
-      </c>
-      <c r="I28" s="9"/>
-      <c r="J28" s="9"/>
-      <c r="K28" s="9"/>
-      <c r="L28" s="9"/>
-      <c r="M28" s="9"/>
-      <c r="N28" s="9"/>
-      <c r="O28" s="9"/>
-      <c r="P28" s="9"/>
-      <c r="Q28" s="9"/>
-      <c r="R28" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="S28" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="T28" s="9"/>
-      <c r="U28" s="9"/>
-      <c r="V28" s="9"/>
+      <c r="A28" s="16">
+        <v>13010112</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>231</v>
+      </c>
+      <c r="C28" s="15">
+        <v>2</v>
+      </c>
+      <c r="D28" s="15">
+        <v>15</v>
+      </c>
+      <c r="E28" s="15">
+        <v>13010101</v>
+      </c>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="18"/>
+      <c r="L28" s="18"/>
+      <c r="M28" s="18"/>
+      <c r="N28" s="18"/>
+      <c r="O28" s="15"/>
+      <c r="P28" s="15"/>
+      <c r="Q28" s="18"/>
+      <c r="R28" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="S28" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="T28" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="U28" s="15">
+        <v>984</v>
+      </c>
+      <c r="V28" s="15">
+        <v>734</v>
+      </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A29" s="13">
-        <v>13020022</v>
-      </c>
-      <c r="B29" s="13" t="s">
-        <v>133</v>
-      </c>
-      <c r="C29" s="13">
-        <v>3</v>
-      </c>
-      <c r="D29" s="9">
-        <v>5</v>
-      </c>
-      <c r="E29" s="9">
-        <v>13010004</v>
-      </c>
-      <c r="F29" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="G29" s="17" t="s">
-        <v>199</v>
-      </c>
-      <c r="H29" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="I29" s="9"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="9"/>
-      <c r="L29" s="9"/>
-      <c r="M29" s="9"/>
-      <c r="N29" s="9"/>
-      <c r="O29" s="9"/>
-      <c r="P29" s="9"/>
-      <c r="Q29" s="9"/>
-      <c r="R29" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="S29" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="T29" s="9"/>
-      <c r="U29" s="9"/>
-      <c r="V29" s="9"/>
+      <c r="A29" s="16">
+        <v>13010113</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="C29" s="15">
+        <v>2</v>
+      </c>
+      <c r="D29" s="15">
+        <v>15</v>
+      </c>
+      <c r="E29" s="15">
+        <v>13010101</v>
+      </c>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="18"/>
+      <c r="I29" s="18"/>
+      <c r="J29" s="18"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="18"/>
+      <c r="M29" s="18"/>
+      <c r="N29" s="18"/>
+      <c r="O29" s="15"/>
+      <c r="P29" s="15"/>
+      <c r="Q29" s="18"/>
+      <c r="R29" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="S29" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="T29" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="U29" s="5">
+        <v>807</v>
+      </c>
+      <c r="V29" s="5">
+        <v>720</v>
+      </c>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A30" s="13">
-        <v>13020023</v>
-      </c>
-      <c r="B30" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="C30" s="13">
-        <v>3</v>
-      </c>
-      <c r="D30" s="9">
-        <v>5</v>
-      </c>
-      <c r="E30" s="9">
-        <v>13010004</v>
-      </c>
-      <c r="F30" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="G30" s="17" t="s">
-        <v>205</v>
-      </c>
-      <c r="H30" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="I30" s="9"/>
-      <c r="J30" s="9"/>
-      <c r="K30" s="9"/>
-      <c r="L30" s="9"/>
-      <c r="M30" s="9"/>
-      <c r="N30" s="9"/>
-      <c r="O30" s="9"/>
-      <c r="P30" s="9"/>
-      <c r="Q30" s="9"/>
-      <c r="R30" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="S30" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="T30" s="9"/>
-      <c r="U30" s="9"/>
-      <c r="V30" s="9"/>
+      <c r="A30" s="16">
+        <v>13010114</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="C30" s="15">
+        <v>2</v>
+      </c>
+      <c r="D30" s="15">
+        <v>15</v>
+      </c>
+      <c r="E30" s="15">
+        <v>13010101</v>
+      </c>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="18"/>
+      <c r="I30" s="18"/>
+      <c r="J30" s="18"/>
+      <c r="K30" s="18"/>
+      <c r="L30" s="18"/>
+      <c r="M30" s="18"/>
+      <c r="N30" s="18"/>
+      <c r="O30" s="15"/>
+      <c r="P30" s="15"/>
+      <c r="Q30" s="18"/>
+      <c r="R30" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="S30" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="T30" s="18" t="s">
+        <v>223</v>
+      </c>
+      <c r="U30" s="5">
+        <v>717</v>
+      </c>
+      <c r="V30" s="5">
+        <v>655</v>
+      </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A31" s="14">
-        <v>13020031</v>
-      </c>
-      <c r="B31" s="13" t="s">
-        <v>181</v>
-      </c>
-      <c r="C31" s="14">
-        <v>3</v>
+      <c r="A31" s="16">
+        <v>13010115</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="C31" s="15">
+        <v>2</v>
       </c>
       <c r="D31" s="15">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E31" s="15">
-        <v>13010005</v>
-      </c>
-      <c r="F31" s="15"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="15" t="s">
-        <v>193</v>
-      </c>
-      <c r="I31" s="15"/>
-      <c r="J31" s="15"/>
-      <c r="K31" s="15"/>
-      <c r="L31" s="15"/>
-      <c r="M31" s="15"/>
-      <c r="N31" s="15"/>
+        <v>13010101</v>
+      </c>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="18"/>
+      <c r="I31" s="18"/>
+      <c r="J31" s="18"/>
+      <c r="K31" s="18"/>
+      <c r="L31" s="18"/>
+      <c r="M31" s="18"/>
+      <c r="N31" s="18"/>
       <c r="O31" s="15"/>
       <c r="P31" s="15"/>
-      <c r="Q31" s="15"/>
-      <c r="R31" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="S31" s="15" t="s">
-        <v>187</v>
-      </c>
-      <c r="T31" s="15"/>
-      <c r="U31" s="15"/>
-      <c r="V31" s="15"/>
+      <c r="Q31" s="18"/>
+      <c r="R31" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="S31" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="T31" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="U31" s="5">
+        <v>637</v>
+      </c>
+      <c r="V31" s="5">
+        <v>735</v>
+      </c>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A32" s="14">
-        <v>13020032</v>
-      </c>
-      <c r="B32" s="13" t="s">
-        <v>183</v>
-      </c>
-      <c r="C32" s="14">
-        <v>3</v>
+      <c r="A32" s="16">
+        <v>13010116</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="C32" s="15">
+        <v>2</v>
       </c>
       <c r="D32" s="15">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E32" s="15">
-        <v>13010005</v>
-      </c>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="15" t="s">
-        <v>194</v>
-      </c>
-      <c r="I32" s="15"/>
-      <c r="J32" s="15"/>
-      <c r="K32" s="15"/>
-      <c r="L32" s="15"/>
-      <c r="M32" s="15"/>
-      <c r="N32" s="15"/>
+        <v>13010101</v>
+      </c>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
+      <c r="I32" s="18"/>
+      <c r="J32" s="18"/>
+      <c r="K32" s="18"/>
+      <c r="L32" s="18"/>
+      <c r="M32" s="18"/>
+      <c r="N32" s="18"/>
       <c r="O32" s="15"/>
       <c r="P32" s="15"/>
-      <c r="Q32" s="15"/>
-      <c r="R32" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="S32" s="15" t="s">
-        <v>188</v>
-      </c>
-      <c r="T32" s="15"/>
-      <c r="U32" s="15"/>
-      <c r="V32" s="15"/>
+      <c r="Q32" s="18"/>
+      <c r="R32" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="S32" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="T32" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="U32" s="5">
+        <v>682</v>
+      </c>
+      <c r="V32" s="5">
+        <v>545</v>
+      </c>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A33" s="14">
-        <v>13020033</v>
-      </c>
-      <c r="B33" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="C33" s="14">
-        <v>3</v>
+      <c r="A33" s="16">
+        <v>13010117</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>227</v>
+      </c>
+      <c r="C33" s="15">
+        <v>2</v>
       </c>
       <c r="D33" s="15">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E33" s="15">
-        <v>13010005</v>
+        <v>13010101</v>
       </c>
       <c r="F33" s="15"/>
       <c r="G33" s="15"/>
-      <c r="H33" s="15" t="s">
-        <v>195</v>
-      </c>
+      <c r="H33" s="15"/>
       <c r="I33" s="15"/>
       <c r="J33" s="15"/>
       <c r="K33" s="15"/>
@@ -4329,110 +4431,568 @@
       <c r="O33" s="15"/>
       <c r="P33" s="15"/>
       <c r="Q33" s="15"/>
-      <c r="R33" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="S33" s="15" t="s">
-        <v>189</v>
-      </c>
-      <c r="T33" s="16"/>
-      <c r="U33" s="16"/>
-      <c r="V33" s="16"/>
+      <c r="R33" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="S33" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="T33" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="U33" s="5">
+        <v>737</v>
+      </c>
+      <c r="V33" s="5">
+        <v>785</v>
+      </c>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A34" s="14">
-        <v>13020034</v>
-      </c>
-      <c r="B34" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="C34" s="14">
+      <c r="A34" s="19">
+        <v>13020001</v>
+      </c>
+      <c r="B34" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="C34" s="19">
         <v>3</v>
       </c>
-      <c r="D34" s="15">
-        <v>10</v>
-      </c>
-      <c r="E34" s="15">
-        <v>13010005</v>
-      </c>
-      <c r="F34" s="15"/>
-      <c r="G34" s="15"/>
-      <c r="H34" s="15" t="s">
-        <v>196</v>
-      </c>
-      <c r="I34" s="15"/>
-      <c r="J34" s="15"/>
-      <c r="K34" s="15"/>
-      <c r="L34" s="15"/>
-      <c r="M34" s="15"/>
-      <c r="N34" s="15"/>
-      <c r="O34" s="15"/>
-      <c r="P34" s="15"/>
-      <c r="Q34" s="15"/>
-      <c r="R34" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="S34" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="T34" s="16"/>
-      <c r="U34" s="16"/>
-      <c r="V34" s="16"/>
+      <c r="D34" s="13">
+        <v>3</v>
+      </c>
+      <c r="E34" s="13">
+        <v>13010002</v>
+      </c>
+      <c r="F34" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="I34" s="13"/>
+      <c r="J34" s="13"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="13"/>
+      <c r="M34" s="13"/>
+      <c r="N34" s="13"/>
+      <c r="O34" s="13"/>
+      <c r="P34" s="13"/>
+      <c r="Q34" s="13"/>
+      <c r="R34" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="S34" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="T34" s="13"/>
+      <c r="U34" s="13"/>
+      <c r="V34" s="13"/>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A35" s="14">
+      <c r="A35" s="19">
+        <v>13020002</v>
+      </c>
+      <c r="B35" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="C35" s="19">
+        <v>3</v>
+      </c>
+      <c r="D35" s="13">
+        <v>3</v>
+      </c>
+      <c r="E35" s="13">
+        <v>13010002</v>
+      </c>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="13"/>
+      <c r="K35" s="13"/>
+      <c r="L35" s="13"/>
+      <c r="M35" s="13"/>
+      <c r="N35" s="13"/>
+      <c r="O35" s="13"/>
+      <c r="P35" s="13"/>
+      <c r="Q35" s="13"/>
+      <c r="R35" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="S35" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="T35" s="13"/>
+      <c r="U35" s="13"/>
+      <c r="V35" s="13"/>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.15">
+      <c r="A36" s="19">
+        <v>13020011</v>
+      </c>
+      <c r="B36" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="C36" s="19">
+        <v>3</v>
+      </c>
+      <c r="D36" s="13">
+        <v>8</v>
+      </c>
+      <c r="E36" s="13">
+        <v>13010007</v>
+      </c>
+      <c r="F36" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="G36" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="H36" s="13"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="13"/>
+      <c r="K36" s="13"/>
+      <c r="L36" s="13"/>
+      <c r="M36" s="13"/>
+      <c r="N36" s="13"/>
+      <c r="O36" s="13"/>
+      <c r="P36" s="13"/>
+      <c r="Q36" s="13"/>
+      <c r="R36" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="S36" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="T36" s="13"/>
+      <c r="U36" s="13"/>
+      <c r="V36" s="13"/>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.15">
+      <c r="A37" s="19">
+        <v>13020012</v>
+      </c>
+      <c r="B37" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="C37" s="19">
+        <v>3</v>
+      </c>
+      <c r="D37" s="13">
+        <v>8</v>
+      </c>
+      <c r="E37" s="13">
+        <v>13010007</v>
+      </c>
+      <c r="F37" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="13"/>
+      <c r="K37" s="13"/>
+      <c r="L37" s="13"/>
+      <c r="M37" s="13"/>
+      <c r="N37" s="13"/>
+      <c r="O37" s="13"/>
+      <c r="P37" s="13"/>
+      <c r="Q37" s="13"/>
+      <c r="R37" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="S37" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="T37" s="13"/>
+      <c r="U37" s="13"/>
+      <c r="V37" s="13"/>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.15">
+      <c r="A38" s="19">
+        <v>13020013</v>
+      </c>
+      <c r="B38" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="C38" s="19">
+        <v>3</v>
+      </c>
+      <c r="D38" s="13">
+        <v>8</v>
+      </c>
+      <c r="E38" s="13">
+        <v>13010007</v>
+      </c>
+      <c r="F38" s="13"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
+      <c r="I38" s="13"/>
+      <c r="J38" s="13"/>
+      <c r="K38" s="13"/>
+      <c r="L38" s="13"/>
+      <c r="M38" s="13"/>
+      <c r="N38" s="13"/>
+      <c r="O38" s="13"/>
+      <c r="P38" s="13"/>
+      <c r="Q38" s="13"/>
+      <c r="R38" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="S38" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="T38" s="13"/>
+      <c r="U38" s="13"/>
+      <c r="V38" s="13"/>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.15">
+      <c r="A39" s="19">
+        <v>13020021</v>
+      </c>
+      <c r="B39" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="C39" s="19">
+        <v>3</v>
+      </c>
+      <c r="D39" s="13">
+        <v>5</v>
+      </c>
+      <c r="E39" s="13">
+        <v>13010004</v>
+      </c>
+      <c r="F39" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="G39" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="H39" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="I39" s="13"/>
+      <c r="J39" s="13"/>
+      <c r="K39" s="13"/>
+      <c r="L39" s="13"/>
+      <c r="M39" s="13"/>
+      <c r="N39" s="13"/>
+      <c r="O39" s="13"/>
+      <c r="P39" s="13"/>
+      <c r="Q39" s="13"/>
+      <c r="R39" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="S39" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="T39" s="13"/>
+      <c r="U39" s="13"/>
+      <c r="V39" s="13"/>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.15">
+      <c r="A40" s="19">
+        <v>13020022</v>
+      </c>
+      <c r="B40" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="C40" s="19">
+        <v>3</v>
+      </c>
+      <c r="D40" s="13">
+        <v>5</v>
+      </c>
+      <c r="E40" s="13">
+        <v>13010004</v>
+      </c>
+      <c r="F40" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="G40" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="H40" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="I40" s="13"/>
+      <c r="J40" s="13"/>
+      <c r="K40" s="13"/>
+      <c r="L40" s="13"/>
+      <c r="M40" s="13"/>
+      <c r="N40" s="13"/>
+      <c r="O40" s="13"/>
+      <c r="P40" s="13"/>
+      <c r="Q40" s="13"/>
+      <c r="R40" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="S40" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="T40" s="13"/>
+      <c r="U40" s="13"/>
+      <c r="V40" s="13"/>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.15">
+      <c r="A41" s="19">
+        <v>13020023</v>
+      </c>
+      <c r="B41" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="C41" s="19">
+        <v>3</v>
+      </c>
+      <c r="D41" s="13">
+        <v>5</v>
+      </c>
+      <c r="E41" s="13">
+        <v>13010004</v>
+      </c>
+      <c r="F41" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="G41" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="H41" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="I41" s="13"/>
+      <c r="J41" s="13"/>
+      <c r="K41" s="13"/>
+      <c r="L41" s="13"/>
+      <c r="M41" s="13"/>
+      <c r="N41" s="13"/>
+      <c r="O41" s="13"/>
+      <c r="P41" s="13"/>
+      <c r="Q41" s="13"/>
+      <c r="R41" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="S41" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="T41" s="13"/>
+      <c r="U41" s="13"/>
+      <c r="V41" s="13"/>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.15">
+      <c r="A42" s="20">
+        <v>13020031</v>
+      </c>
+      <c r="B42" s="19" t="s">
+        <v>181</v>
+      </c>
+      <c r="C42" s="20">
+        <v>3</v>
+      </c>
+      <c r="D42" s="15">
+        <v>10</v>
+      </c>
+      <c r="E42" s="15">
+        <v>13010005</v>
+      </c>
+      <c r="F42" s="15"/>
+      <c r="G42" s="15"/>
+      <c r="H42" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="I42" s="15"/>
+      <c r="J42" s="15"/>
+      <c r="K42" s="15"/>
+      <c r="L42" s="15"/>
+      <c r="M42" s="15"/>
+      <c r="N42" s="15"/>
+      <c r="O42" s="15"/>
+      <c r="P42" s="15"/>
+      <c r="Q42" s="15"/>
+      <c r="R42" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="S42" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="T42" s="15"/>
+      <c r="U42" s="15"/>
+      <c r="V42" s="15"/>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.15">
+      <c r="A43" s="20">
+        <v>13020032</v>
+      </c>
+      <c r="B43" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="C43" s="20">
+        <v>3</v>
+      </c>
+      <c r="D43" s="15">
+        <v>10</v>
+      </c>
+      <c r="E43" s="15">
+        <v>13010005</v>
+      </c>
+      <c r="F43" s="15"/>
+      <c r="G43" s="15"/>
+      <c r="H43" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="I43" s="15"/>
+      <c r="J43" s="15"/>
+      <c r="K43" s="15"/>
+      <c r="L43" s="15"/>
+      <c r="M43" s="15"/>
+      <c r="N43" s="15"/>
+      <c r="O43" s="15"/>
+      <c r="P43" s="15"/>
+      <c r="Q43" s="15"/>
+      <c r="R43" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="S43" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="T43" s="15"/>
+      <c r="U43" s="15"/>
+      <c r="V43" s="15"/>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.15">
+      <c r="A44" s="20">
+        <v>13020033</v>
+      </c>
+      <c r="B44" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="C44" s="20">
+        <v>3</v>
+      </c>
+      <c r="D44" s="15">
+        <v>10</v>
+      </c>
+      <c r="E44" s="15">
+        <v>13010005</v>
+      </c>
+      <c r="F44" s="15"/>
+      <c r="G44" s="15"/>
+      <c r="H44" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="I44" s="15"/>
+      <c r="J44" s="15"/>
+      <c r="K44" s="15"/>
+      <c r="L44" s="15"/>
+      <c r="M44" s="15"/>
+      <c r="N44" s="15"/>
+      <c r="O44" s="15"/>
+      <c r="P44" s="15"/>
+      <c r="Q44" s="15"/>
+      <c r="R44" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="S44" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="T44" s="21"/>
+      <c r="U44" s="21"/>
+      <c r="V44" s="21"/>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.15">
+      <c r="A45" s="20">
+        <v>13020034</v>
+      </c>
+      <c r="B45" s="19" t="s">
+        <v>185</v>
+      </c>
+      <c r="C45" s="20">
+        <v>3</v>
+      </c>
+      <c r="D45" s="15">
+        <v>10</v>
+      </c>
+      <c r="E45" s="15">
+        <v>13010005</v>
+      </c>
+      <c r="F45" s="15"/>
+      <c r="G45" s="15"/>
+      <c r="H45" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="I45" s="15"/>
+      <c r="J45" s="15"/>
+      <c r="K45" s="15"/>
+      <c r="L45" s="15"/>
+      <c r="M45" s="15"/>
+      <c r="N45" s="15"/>
+      <c r="O45" s="15"/>
+      <c r="P45" s="15"/>
+      <c r="Q45" s="15"/>
+      <c r="R45" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="S45" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="T45" s="21"/>
+      <c r="U45" s="21"/>
+      <c r="V45" s="21"/>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.15">
+      <c r="A46" s="20">
         <v>13020035</v>
       </c>
-      <c r="B35" s="13" t="s">
+      <c r="B46" s="19" t="s">
         <v>186</v>
       </c>
-      <c r="C35" s="14">
+      <c r="C46" s="20">
         <v>3</v>
       </c>
-      <c r="D35" s="15">
+      <c r="D46" s="15">
         <v>10</v>
       </c>
-      <c r="E35" s="15">
+      <c r="E46" s="15">
         <v>13010005</v>
       </c>
-      <c r="F35" s="15"/>
-      <c r="G35" s="15"/>
-      <c r="H35" s="15" t="s">
+      <c r="F46" s="15"/>
+      <c r="G46" s="15"/>
+      <c r="H46" s="15" t="s">
         <v>197</v>
       </c>
-      <c r="I35" s="15"/>
-      <c r="J35" s="15"/>
-      <c r="K35" s="15"/>
-      <c r="L35" s="15"/>
-      <c r="M35" s="15"/>
-      <c r="N35" s="15"/>
-      <c r="O35" s="15"/>
-      <c r="P35" s="15"/>
-      <c r="Q35" s="15"/>
-      <c r="R35" s="9" t="s">
+      <c r="I46" s="15"/>
+      <c r="J46" s="15"/>
+      <c r="K46" s="15"/>
+      <c r="L46" s="15"/>
+      <c r="M46" s="15"/>
+      <c r="N46" s="15"/>
+      <c r="O46" s="15"/>
+      <c r="P46" s="15"/>
+      <c r="Q46" s="15"/>
+      <c r="R46" s="13" t="s">
         <v>182</v>
       </c>
-      <c r="S35" s="15" t="s">
+      <c r="S46" s="15" t="s">
         <v>191</v>
       </c>
-      <c r="T35" s="16"/>
-      <c r="U35" s="16"/>
-      <c r="V35" s="16"/>
+      <c r="T46" s="21"/>
+      <c r="U46" s="21"/>
+      <c r="V46" s="21"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="I4:P35">
-    <cfRule type="cellIs" dxfId="27" priority="4" operator="equal">
+  <conditionalFormatting sqref="I4:P46">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4">
-    <cfRule type="cellIs" dxfId="26" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F4:H35">
-    <cfRule type="containsBlanks" dxfId="25" priority="5">
+  <conditionalFormatting sqref="F4:H46">
+    <cfRule type="containsBlanks" dxfId="0" priority="5">
       <formula>LEN(TRIM(F4))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
add some scene images
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Scene.xlsx
+++ b/ConfigData/Xlsx/Scene.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="Scene" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="240">
   <si>
     <t>村外小屋</t>
   </si>
@@ -887,13 +887,30 @@
   </si>
   <si>
     <t>日落古道</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>lugaoyin</t>
+  </si>
+  <si>
+    <t>sunfallroad</t>
+  </si>
+  <si>
+    <t>kusttree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">armcape </t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>sandflow</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1612,7 +1629,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1677,6 +1694,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1725,27 +1745,6 @@
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="28">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2400,8 +2399,97 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2414,34 +2502,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A3:V46" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26" tableBorderDxfId="25">
-  <autoFilter ref="A3:V46" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:V46" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23" tableBorderDxfId="22">
+  <autoFilter ref="A3:V46"/>
   <sortState ref="A4:V38">
     <sortCondition ref="A3:A38"/>
   </sortState>
   <tableColumns count="22">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="23"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Type" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Level" dataDxfId="21"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="ReviveScene" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Quest" dataDxfId="19"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="QuestRandom" dataDxfId="18"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="QuestDungeon" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="QPortal" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="QCardChange" dataDxfId="15"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="QPiece" dataDxfId="14"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="QMerchant" dataDxfId="13"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="QDoctor" dataDxfId="12"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="QAngel" dataDxfId="11"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="QWheel" dataDxfId="10"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="QRes" dataDxfId="9"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Func" dataDxfId="8"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Url" dataDxfId="7"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="TilePath" dataDxfId="6"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Icon" dataDxfId="5"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="IconX" dataDxfId="4"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="IconY" dataDxfId="3"/>
+    <tableColumn id="1" name="Id" dataDxfId="21"/>
+    <tableColumn id="2" name="Name" dataDxfId="20"/>
+    <tableColumn id="18" name="Type" dataDxfId="19"/>
+    <tableColumn id="3" name="Level" dataDxfId="18"/>
+    <tableColumn id="20" name="ReviveScene" dataDxfId="17"/>
+    <tableColumn id="4" name="Quest" dataDxfId="16"/>
+    <tableColumn id="17" name="QuestRandom" dataDxfId="15"/>
+    <tableColumn id="19" name="QuestDungeon" dataDxfId="14"/>
+    <tableColumn id="5" name="QPortal" dataDxfId="13"/>
+    <tableColumn id="6" name="QCardChange" dataDxfId="12"/>
+    <tableColumn id="7" name="QPiece" dataDxfId="11"/>
+    <tableColumn id="8" name="QMerchant" dataDxfId="10"/>
+    <tableColumn id="9" name="QDoctor" dataDxfId="9"/>
+    <tableColumn id="10" name="QAngel" dataDxfId="8"/>
+    <tableColumn id="21" name="QWheel" dataDxfId="7"/>
+    <tableColumn id="22" name="QRes" dataDxfId="6"/>
+    <tableColumn id="11" name="Func" dataDxfId="5"/>
+    <tableColumn id="12" name="Url" dataDxfId="4"/>
+    <tableColumn id="13" name="TilePath" dataDxfId="3"/>
+    <tableColumn id="14" name="Icon" dataDxfId="2"/>
+    <tableColumn id="15" name="IconX" dataDxfId="1"/>
+    <tableColumn id="16" name="IconY" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2455,7 +2543,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="C7EDCC"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -2767,11 +2855,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2783,7 +2871,7 @@
     <col min="5" max="5" width="9" style="5" customWidth="1"/>
     <col min="6" max="6" width="52.875" style="5" customWidth="1"/>
     <col min="7" max="7" width="23.625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="50.875" style="5" customWidth="1"/>
+    <col min="8" max="8" width="43.5" style="5" customWidth="1"/>
     <col min="9" max="16" width="3.125" style="5" customWidth="1"/>
     <col min="17" max="17" width="6.625" style="5" customWidth="1"/>
     <col min="18" max="18" width="9.75" style="5" customWidth="1"/>
@@ -4080,7 +4168,7 @@
       <c r="P25" s="15"/>
       <c r="Q25" s="15"/>
       <c r="R25" s="13" t="s">
-        <v>104</v>
+        <v>236</v>
       </c>
       <c r="S25" s="13" t="s">
         <v>43</v>
@@ -4168,7 +4256,7 @@
       <c r="P27" s="15"/>
       <c r="Q27" s="18"/>
       <c r="R27" s="13" t="s">
-        <v>104</v>
+        <v>237</v>
       </c>
       <c r="S27" s="13" t="s">
         <v>43</v>
@@ -4211,8 +4299,8 @@
       <c r="O28" s="15"/>
       <c r="P28" s="15"/>
       <c r="Q28" s="18"/>
-      <c r="R28" s="13" t="s">
-        <v>104</v>
+      <c r="R28" s="22" t="s">
+        <v>238</v>
       </c>
       <c r="S28" s="13" t="s">
         <v>43</v>
@@ -4256,7 +4344,7 @@
       <c r="P29" s="15"/>
       <c r="Q29" s="18"/>
       <c r="R29" s="13" t="s">
-        <v>104</v>
+        <v>235</v>
       </c>
       <c r="S29" s="13" t="s">
         <v>43</v>
@@ -4299,8 +4387,8 @@
       <c r="O30" s="15"/>
       <c r="P30" s="15"/>
       <c r="Q30" s="18"/>
-      <c r="R30" s="13" t="s">
-        <v>104</v>
+      <c r="R30" s="22" t="s">
+        <v>239</v>
       </c>
       <c r="S30" s="13" t="s">
         <v>43</v>
@@ -4982,17 +5070,17 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="I4:P46">
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4:H46">
-    <cfRule type="containsBlanks" dxfId="0" priority="5">
+    <cfRule type="containsBlanks" dxfId="25" priority="5">
       <formula>LEN(TRIM(F4))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
add some new scenes
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Scene.xlsx
+++ b/ConfigData/Xlsx/Scene.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="246">
   <si>
     <t>村外小屋</t>
   </si>
@@ -899,11 +899,30 @@
     <t>kusttree</t>
   </si>
   <si>
-    <t xml:space="preserve">armcape </t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>sandflow</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>danriversouth</t>
+  </si>
+  <si>
+    <t>windstonenorth</t>
+  </si>
+  <si>
+    <t>windstonesouth</t>
+  </si>
+  <si>
+    <t>windstonehole</t>
+  </si>
+  <si>
+    <t>vocano</t>
+  </si>
+  <si>
+    <t>pyramid</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>armcape</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -2858,8 +2877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R23" sqref="R23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4080,7 +4099,7 @@
       <c r="P23" s="15"/>
       <c r="Q23" s="15"/>
       <c r="R23" s="13" t="s">
-        <v>104</v>
+        <v>240</v>
       </c>
       <c r="S23" s="13" t="s">
         <v>43</v>
@@ -4124,7 +4143,7 @@
       <c r="P24" s="15"/>
       <c r="Q24" s="15"/>
       <c r="R24" s="13" t="s">
-        <v>104</v>
+        <v>241</v>
       </c>
       <c r="S24" s="13" t="s">
         <v>43</v>
@@ -4212,7 +4231,7 @@
       <c r="P26" s="15"/>
       <c r="Q26" s="15"/>
       <c r="R26" s="13" t="s">
-        <v>104</v>
+        <v>242</v>
       </c>
       <c r="S26" s="13" t="s">
         <v>43</v>
@@ -4300,7 +4319,7 @@
       <c r="P28" s="15"/>
       <c r="Q28" s="18"/>
       <c r="R28" s="22" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="S28" s="13" t="s">
         <v>43</v>
@@ -4388,7 +4407,7 @@
       <c r="P30" s="15"/>
       <c r="Q30" s="18"/>
       <c r="R30" s="22" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="S30" s="13" t="s">
         <v>43</v>
@@ -4431,8 +4450,8 @@
       <c r="O31" s="15"/>
       <c r="P31" s="15"/>
       <c r="Q31" s="18"/>
-      <c r="R31" s="13" t="s">
-        <v>104</v>
+      <c r="R31" s="22" t="s">
+        <v>244</v>
       </c>
       <c r="S31" s="13" t="s">
         <v>43</v>
@@ -4476,7 +4495,7 @@
       <c r="P32" s="15"/>
       <c r="Q32" s="18"/>
       <c r="R32" s="13" t="s">
-        <v>104</v>
+        <v>239</v>
       </c>
       <c r="S32" s="13" t="s">
         <v>43</v>
@@ -4520,7 +4539,7 @@
       <c r="P33" s="15"/>
       <c r="Q33" s="15"/>
       <c r="R33" s="13" t="s">
-        <v>104</v>
+        <v>243</v>
       </c>
       <c r="S33" s="13" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
add the scene scripts
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Scene.xlsx
+++ b/ConfigData/Xlsx/Scene.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18528"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="245">
   <si>
     <t>村外小屋</t>
   </si>
@@ -167,9 +167,6 @@
   <si>
     <t>月光林地</t>
     <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>gerdin</t>
   </si>
   <si>
     <t>fogvalley</t>
@@ -2441,74 +2438,6 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2562,7 +2491,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="C7EDCC"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -2877,8 +2806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R23" sqref="R23"/>
+    <sheetView tabSelected="1" topLeftCell="G16" workbookViewId="0">
+      <selection activeCell="S22" sqref="S22:S33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2908,46 +2837,46 @@
         <v>16</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>30</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="J1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="K1" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="L1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="N1" s="3" t="s">
-        <v>60</v>
-      </c>
       <c r="O1" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>207</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>208</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>18</v>
@@ -2959,13 +2888,13 @@
         <v>27</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="U1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="V1" s="4" t="s">
         <v>83</v>
-      </c>
-      <c r="V1" s="4" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.15">
@@ -2976,46 +2905,46 @@
         <v>14</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>13</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O2" s="8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="P2" s="8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Q2" s="7" t="s">
         <v>14</v>
@@ -3027,7 +2956,7 @@
         <v>26</v>
       </c>
       <c r="T2" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="U2" s="7" t="s">
         <v>13</v>
@@ -3044,46 +2973,46 @@
         <v>21</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>22</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>29</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I3" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="J3" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="J3" s="11" t="s">
-        <v>51</v>
-      </c>
       <c r="K3" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="L3" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="L3" s="11" t="s">
+      <c r="M3" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="M3" s="11" t="s">
+      <c r="N3" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="N3" s="11" t="s">
-        <v>57</v>
-      </c>
       <c r="O3" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="P3" s="11" t="s">
         <v>210</v>
-      </c>
-      <c r="P3" s="11" t="s">
-        <v>211</v>
       </c>
       <c r="Q3" s="10" t="s">
         <v>23</v>
@@ -3095,13 +3024,13 @@
         <v>25</v>
       </c>
       <c r="T3" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="U3" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="V3" s="10" t="s">
         <v>61</v>
-      </c>
-      <c r="V3" s="10" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.15">
@@ -3121,10 +3050,10 @@
         <v>13010001</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H4" s="13"/>
       <c r="I4" s="13">
@@ -3139,13 +3068,13 @@
       <c r="P4" s="13"/>
       <c r="Q4" s="13"/>
       <c r="R4" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="S4" s="13" t="s">
         <v>28</v>
       </c>
       <c r="T4" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="U4" s="13">
         <v>1348</v>
@@ -3171,10 +3100,10 @@
         <v>13010001</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H5" s="13"/>
       <c r="I5" s="13">
@@ -3199,7 +3128,7 @@
         <v>31</v>
       </c>
       <c r="T5" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="U5" s="13">
         <v>1279</v>
@@ -3225,10 +3154,10 @@
         <v>13010006</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H6" s="13"/>
       <c r="I6" s="13">
@@ -3251,7 +3180,7 @@
         <v>35</v>
       </c>
       <c r="T6" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="U6" s="13">
         <v>1148</v>
@@ -3265,7 +3194,7 @@
         <v>13010005</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C7" s="13">
         <v>2</v>
@@ -3277,10 +3206,10 @@
         <v>13010006</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H7" s="13"/>
       <c r="I7" s="13">
@@ -3297,13 +3226,13 @@
       <c r="P7" s="13"/>
       <c r="Q7" s="13"/>
       <c r="R7" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="S7" s="13" t="s">
         <v>36</v>
       </c>
       <c r="T7" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="U7" s="13">
         <v>1386</v>
@@ -3341,13 +3270,13 @@
       <c r="P8" s="13"/>
       <c r="Q8" s="13"/>
       <c r="R8" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="S8" s="13" t="s">
         <v>32</v>
       </c>
       <c r="T8" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="U8" s="13">
         <v>1232</v>
@@ -3373,10 +3302,10 @@
         <v>13010006</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H9" s="13"/>
       <c r="I9" s="13">
@@ -3395,13 +3324,13 @@
       </c>
       <c r="Q9" s="13"/>
       <c r="R9" s="13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="S9" s="13" t="s">
         <v>34</v>
       </c>
       <c r="T9" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="U9" s="13">
         <v>1431</v>
@@ -3427,10 +3356,10 @@
         <v>13010006</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H10" s="13"/>
       <c r="I10" s="13">
@@ -3449,13 +3378,13 @@
       <c r="P10" s="13"/>
       <c r="Q10" s="13"/>
       <c r="R10" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="S10" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="T10" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="U10" s="13">
         <v>1332</v>
@@ -3481,10 +3410,10 @@
         <v>13010006</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H11" s="13"/>
       <c r="I11" s="13">
@@ -3503,13 +3432,13 @@
       <c r="P11" s="13"/>
       <c r="Q11" s="13"/>
       <c r="R11" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="S11" s="13" t="s">
         <v>38</v>
       </c>
       <c r="T11" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="U11" s="13">
         <v>1441</v>
@@ -3535,10 +3464,10 @@
         <v>13010006</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H12" s="13"/>
       <c r="I12" s="13">
@@ -3557,13 +3486,13 @@
       </c>
       <c r="Q12" s="13"/>
       <c r="R12" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S12" s="13" t="s">
         <v>39</v>
       </c>
       <c r="T12" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="U12" s="13">
         <v>1574</v>
@@ -3589,10 +3518,10 @@
         <v>13010006</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H13" s="13"/>
       <c r="I13" s="13">
@@ -3607,13 +3536,13 @@
       <c r="P13" s="13"/>
       <c r="Q13" s="13"/>
       <c r="R13" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="S13" s="13" t="s">
         <v>33</v>
       </c>
       <c r="T13" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="U13" s="13">
         <v>1251</v>
@@ -3639,10 +3568,10 @@
         <v>13010006</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H14" s="13"/>
       <c r="I14" s="13">
@@ -3659,13 +3588,13 @@
       <c r="P14" s="13"/>
       <c r="Q14" s="13"/>
       <c r="R14" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="S14" s="13" t="s">
         <v>37</v>
       </c>
       <c r="T14" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="U14" s="13">
         <v>1250</v>
@@ -3691,10 +3620,10 @@
         <v>13010006</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H15" s="13"/>
       <c r="I15" s="13">
@@ -3713,13 +3642,13 @@
       <c r="P15" s="13"/>
       <c r="Q15" s="13"/>
       <c r="R15" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="S15" s="13" t="s">
         <v>40</v>
       </c>
       <c r="T15" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="U15" s="13">
         <v>1550</v>
@@ -3733,7 +3662,7 @@
         <v>13010015</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C16" s="15">
         <v>2</v>
@@ -3745,10 +3674,10 @@
         <v>13010006</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G16" s="13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H16" s="13"/>
       <c r="I16" s="15">
@@ -3763,10 +3692,10 @@
       <c r="P16" s="15"/>
       <c r="Q16" s="15"/>
       <c r="R16" s="15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="S16" s="15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="T16" s="15"/>
       <c r="U16" s="15"/>
@@ -3801,13 +3730,13 @@
       <c r="P17" s="13"/>
       <c r="Q17" s="13"/>
       <c r="R17" s="13" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="S17" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="T17" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="U17" s="13">
         <v>894</v>
@@ -3833,10 +3762,10 @@
         <v>13010101</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H18" s="13"/>
       <c r="I18" s="13">
@@ -3853,13 +3782,13 @@
       <c r="P18" s="13"/>
       <c r="Q18" s="13"/>
       <c r="R18" s="13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S18" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T18" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="U18" s="13">
         <v>1040</v>
@@ -3873,7 +3802,7 @@
         <v>13010103</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C19" s="13">
         <v>2</v>
@@ -3885,10 +3814,10 @@
         <v>13010101</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G19" s="13" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H19" s="13"/>
       <c r="I19" s="13">
@@ -3903,13 +3832,13 @@
       <c r="P19" s="13"/>
       <c r="Q19" s="13"/>
       <c r="R19" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="S19" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="T19" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="U19" s="13">
         <v>1213</v>
@@ -3935,10 +3864,10 @@
         <v>13010101</v>
       </c>
       <c r="F20" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G20" s="13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H20" s="13"/>
       <c r="I20" s="13">
@@ -3955,13 +3884,13 @@
       <c r="P20" s="13"/>
       <c r="Q20" s="13"/>
       <c r="R20" s="13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="S20" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="T20" s="13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="U20" s="13">
         <v>1149</v>
@@ -3987,10 +3916,10 @@
         <v>13010101</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G21" s="13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H21" s="13"/>
       <c r="I21" s="13"/>
@@ -4003,13 +3932,13 @@
       <c r="P21" s="13"/>
       <c r="Q21" s="13"/>
       <c r="R21" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="S21" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="T21" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="U21" s="13">
         <v>840</v>
@@ -4023,7 +3952,7 @@
         <v>13010106</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C22" s="13">
         <v>2</v>
@@ -4035,10 +3964,10 @@
         <v>13010016</v>
       </c>
       <c r="F22" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G22" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H22" s="13"/>
       <c r="I22" s="13">
@@ -4055,13 +3984,13 @@
       <c r="P22" s="13"/>
       <c r="Q22" s="13"/>
       <c r="R22" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="S22" s="13" t="s">
-        <v>43</v>
+        <v>103</v>
       </c>
       <c r="T22" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="U22" s="13">
         <v>1067</v>
@@ -4075,7 +4004,7 @@
         <v>13010107</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C23" s="15">
         <v>2</v>
@@ -4099,13 +4028,13 @@
       <c r="P23" s="15"/>
       <c r="Q23" s="15"/>
       <c r="R23" s="13" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="S23" s="13" t="s">
-        <v>43</v>
+        <v>239</v>
       </c>
       <c r="T23" s="15" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="U23" s="15">
         <v>974</v>
@@ -4119,7 +4048,7 @@
         <v>13010108</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C24" s="15">
         <v>2</v>
@@ -4143,13 +4072,13 @@
       <c r="P24" s="15"/>
       <c r="Q24" s="15"/>
       <c r="R24" s="13" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="S24" s="13" t="s">
-        <v>43</v>
+        <v>240</v>
       </c>
       <c r="T24" s="15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="U24" s="15">
         <v>1080</v>
@@ -4163,7 +4092,7 @@
         <v>13010109</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C25" s="15">
         <v>2</v>
@@ -4187,13 +4116,13 @@
       <c r="P25" s="15"/>
       <c r="Q25" s="15"/>
       <c r="R25" s="13" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="S25" s="13" t="s">
-        <v>43</v>
+        <v>235</v>
       </c>
       <c r="T25" s="15" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="U25" s="15">
         <v>894</v>
@@ -4207,7 +4136,7 @@
         <v>13010110</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C26" s="15">
         <v>2</v>
@@ -4231,13 +4160,13 @@
       <c r="P26" s="15"/>
       <c r="Q26" s="15"/>
       <c r="R26" s="13" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="S26" s="13" t="s">
-        <v>43</v>
+        <v>241</v>
       </c>
       <c r="T26" s="15" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="U26" s="15">
         <v>1074</v>
@@ -4251,7 +4180,7 @@
         <v>13010111</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C27" s="15">
         <v>2</v>
@@ -4275,13 +4204,13 @@
       <c r="P27" s="15"/>
       <c r="Q27" s="18"/>
       <c r="R27" s="13" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="S27" s="13" t="s">
-        <v>43</v>
+        <v>236</v>
       </c>
       <c r="T27" s="13" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="U27" s="18">
         <v>850</v>
@@ -4295,7 +4224,7 @@
         <v>13010112</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C28" s="15">
         <v>2</v>
@@ -4319,13 +4248,13 @@
       <c r="P28" s="15"/>
       <c r="Q28" s="18"/>
       <c r="R28" s="22" t="s">
-        <v>245</v>
-      </c>
-      <c r="S28" s="13" t="s">
-        <v>43</v>
+        <v>244</v>
+      </c>
+      <c r="S28" s="22" t="s">
+        <v>244</v>
       </c>
       <c r="T28" s="18" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="U28" s="15">
         <v>984</v>
@@ -4339,7 +4268,7 @@
         <v>13010113</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C29" s="15">
         <v>2</v>
@@ -4363,13 +4292,13 @@
       <c r="P29" s="15"/>
       <c r="Q29" s="18"/>
       <c r="R29" s="13" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="S29" s="13" t="s">
-        <v>43</v>
+        <v>234</v>
       </c>
       <c r="T29" s="18" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="U29" s="5">
         <v>807</v>
@@ -4383,7 +4312,7 @@
         <v>13010114</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C30" s="15">
         <v>2</v>
@@ -4407,13 +4336,13 @@
       <c r="P30" s="15"/>
       <c r="Q30" s="18"/>
       <c r="R30" s="22" t="s">
-        <v>238</v>
-      </c>
-      <c r="S30" s="13" t="s">
-        <v>43</v>
+        <v>237</v>
+      </c>
+      <c r="S30" s="22" t="s">
+        <v>237</v>
       </c>
       <c r="T30" s="18" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="U30" s="5">
         <v>717</v>
@@ -4427,7 +4356,7 @@
         <v>13010115</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C31" s="15">
         <v>2</v>
@@ -4451,13 +4380,13 @@
       <c r="P31" s="15"/>
       <c r="Q31" s="18"/>
       <c r="R31" s="22" t="s">
-        <v>244</v>
-      </c>
-      <c r="S31" s="13" t="s">
-        <v>43</v>
+        <v>243</v>
+      </c>
+      <c r="S31" s="22" t="s">
+        <v>243</v>
       </c>
       <c r="T31" s="18" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="U31" s="5">
         <v>637</v>
@@ -4471,7 +4400,7 @@
         <v>13010116</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C32" s="15">
         <v>2</v>
@@ -4495,13 +4424,13 @@
       <c r="P32" s="15"/>
       <c r="Q32" s="18"/>
       <c r="R32" s="13" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="S32" s="13" t="s">
-        <v>43</v>
+        <v>238</v>
       </c>
       <c r="T32" s="18" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="U32" s="5">
         <v>682</v>
@@ -4515,7 +4444,7 @@
         <v>13010117</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C33" s="15">
         <v>2</v>
@@ -4539,13 +4468,13 @@
       <c r="P33" s="15"/>
       <c r="Q33" s="15"/>
       <c r="R33" s="13" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="S33" s="13" t="s">
-        <v>43</v>
+        <v>242</v>
       </c>
       <c r="T33" s="13" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="U33" s="5">
         <v>737</v>
@@ -4559,7 +4488,7 @@
         <v>13020001</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C34" s="19">
         <v>3</v>
@@ -4571,11 +4500,11 @@
         <v>13010002</v>
       </c>
       <c r="F34" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G34" s="13"/>
       <c r="H34" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I34" s="13"/>
       <c r="J34" s="13"/>
@@ -4587,10 +4516,10 @@
       <c r="P34" s="13"/>
       <c r="Q34" s="13"/>
       <c r="R34" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="S34" s="13" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="T34" s="13"/>
       <c r="U34" s="13"/>
@@ -4601,7 +4530,7 @@
         <v>13020002</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C35" s="19">
         <v>3</v>
@@ -4625,10 +4554,10 @@
       <c r="P35" s="13"/>
       <c r="Q35" s="13"/>
       <c r="R35" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="S35" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="T35" s="13"/>
       <c r="U35" s="13"/>
@@ -4639,7 +4568,7 @@
         <v>13020011</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C36" s="19">
         <v>3</v>
@@ -4651,10 +4580,10 @@
         <v>13010007</v>
       </c>
       <c r="F36" s="13" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G36" s="13" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H36" s="13"/>
       <c r="I36" s="13"/>
@@ -4667,10 +4596,10 @@
       <c r="P36" s="13"/>
       <c r="Q36" s="13"/>
       <c r="R36" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="S36" s="13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="T36" s="13"/>
       <c r="U36" s="13"/>
@@ -4681,7 +4610,7 @@
         <v>13020012</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C37" s="19">
         <v>3</v>
@@ -4693,7 +4622,7 @@
         <v>13010007</v>
       </c>
       <c r="F37" s="13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G37" s="13"/>
       <c r="H37" s="13"/>
@@ -4707,10 +4636,10 @@
       <c r="P37" s="13"/>
       <c r="Q37" s="13"/>
       <c r="R37" s="13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="S37" s="13" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="T37" s="13"/>
       <c r="U37" s="13"/>
@@ -4721,7 +4650,7 @@
         <v>13020013</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C38" s="19">
         <v>3</v>
@@ -4745,10 +4674,10 @@
       <c r="P38" s="13"/>
       <c r="Q38" s="13"/>
       <c r="R38" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="S38" s="13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="T38" s="13"/>
       <c r="U38" s="13"/>
@@ -4759,7 +4688,7 @@
         <v>13020021</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C39" s="19">
         <v>3</v>
@@ -4771,13 +4700,13 @@
         <v>13010004</v>
       </c>
       <c r="F39" s="13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G39" s="13" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H39" s="13" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I39" s="13"/>
       <c r="J39" s="13"/>
@@ -4789,10 +4718,10 @@
       <c r="P39" s="13"/>
       <c r="Q39" s="13"/>
       <c r="R39" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="S39" s="13" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="T39" s="13"/>
       <c r="U39" s="13"/>
@@ -4803,7 +4732,7 @@
         <v>13020022</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C40" s="19">
         <v>3</v>
@@ -4815,13 +4744,13 @@
         <v>13010004</v>
       </c>
       <c r="F40" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G40" s="13" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H40" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I40" s="13"/>
       <c r="J40" s="13"/>
@@ -4833,10 +4762,10 @@
       <c r="P40" s="13"/>
       <c r="Q40" s="13"/>
       <c r="R40" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="S40" s="13" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="T40" s="13"/>
       <c r="U40" s="13"/>
@@ -4847,7 +4776,7 @@
         <v>13020023</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C41" s="19">
         <v>3</v>
@@ -4859,13 +4788,13 @@
         <v>13010004</v>
       </c>
       <c r="F41" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G41" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H41" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I41" s="13"/>
       <c r="J41" s="13"/>
@@ -4877,10 +4806,10 @@
       <c r="P41" s="13"/>
       <c r="Q41" s="13"/>
       <c r="R41" s="13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="S41" s="13" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="T41" s="13"/>
       <c r="U41" s="13"/>
@@ -4891,7 +4820,7 @@
         <v>13020031</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C42" s="20">
         <v>3</v>
@@ -4905,7 +4834,7 @@
       <c r="F42" s="15"/>
       <c r="G42" s="15"/>
       <c r="H42" s="15" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I42" s="15"/>
       <c r="J42" s="15"/>
@@ -4917,10 +4846,10 @@
       <c r="P42" s="15"/>
       <c r="Q42" s="15"/>
       <c r="R42" s="13" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="S42" s="15" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="T42" s="15"/>
       <c r="U42" s="15"/>
@@ -4931,7 +4860,7 @@
         <v>13020032</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C43" s="20">
         <v>3</v>
@@ -4945,7 +4874,7 @@
       <c r="F43" s="15"/>
       <c r="G43" s="15"/>
       <c r="H43" s="15" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I43" s="15"/>
       <c r="J43" s="15"/>
@@ -4957,10 +4886,10 @@
       <c r="P43" s="15"/>
       <c r="Q43" s="15"/>
       <c r="R43" s="13" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="S43" s="15" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="T43" s="15"/>
       <c r="U43" s="15"/>
@@ -4971,7 +4900,7 @@
         <v>13020033</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C44" s="20">
         <v>3</v>
@@ -4985,7 +4914,7 @@
       <c r="F44" s="15"/>
       <c r="G44" s="15"/>
       <c r="H44" s="15" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I44" s="15"/>
       <c r="J44" s="15"/>
@@ -4997,10 +4926,10 @@
       <c r="P44" s="15"/>
       <c r="Q44" s="15"/>
       <c r="R44" s="13" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="S44" s="15" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="T44" s="21"/>
       <c r="U44" s="21"/>
@@ -5011,7 +4940,7 @@
         <v>13020034</v>
       </c>
       <c r="B45" s="19" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C45" s="20">
         <v>3</v>
@@ -5025,7 +4954,7 @@
       <c r="F45" s="15"/>
       <c r="G45" s="15"/>
       <c r="H45" s="15" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I45" s="15"/>
       <c r="J45" s="15"/>
@@ -5037,10 +4966,10 @@
       <c r="P45" s="15"/>
       <c r="Q45" s="15"/>
       <c r="R45" s="13" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="S45" s="15" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="T45" s="21"/>
       <c r="U45" s="21"/>
@@ -5051,7 +4980,7 @@
         <v>13020035</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C46" s="20">
         <v>3</v>
@@ -5065,7 +4994,7 @@
       <c r="F46" s="15"/>
       <c r="G46" s="15"/>
       <c r="H46" s="15" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I46" s="15"/>
       <c r="J46" s="15"/>
@@ -5077,10 +5006,10 @@
       <c r="P46" s="15"/>
       <c r="Q46" s="15"/>
       <c r="R46" s="13" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="S46" s="15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="T46" s="21"/>
       <c r="U46" s="21"/>

</xml_diff>

<commit_message>
new distinct setting for game
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Scene.xlsx
+++ b/ConfigData/Xlsx/Scene.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="251">
   <si>
     <t>村外小屋</t>
   </si>
@@ -920,6 +920,29 @@
   </si>
   <si>
     <t>armcape</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>图标背景色</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>IconColor</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Green</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yellow</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>LawnGreen</t>
+  </si>
+  <si>
+    <t>LightBlue</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1147,7 +1170,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="40">
+  <fills count="42">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1365,7 +1388,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1645,7 +1680,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1694,25 +1729,43 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="39" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="39" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="20" fillId="40" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="41" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1760,7 +1813,55 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="29">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2415,27 +2516,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2450,34 +2530,35 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:V46" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23" tableBorderDxfId="22">
-  <autoFilter ref="A3:V46"/>
-  <sortState ref="A4:V38">
-    <sortCondition ref="A3:A38"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:W46" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27" tableBorderDxfId="26">
+  <autoFilter ref="A3:W46"/>
+  <sortState ref="A4:W46">
+    <sortCondition ref="A3:A46"/>
   </sortState>
-  <tableColumns count="22">
-    <tableColumn id="1" name="Id" dataDxfId="21"/>
-    <tableColumn id="2" name="Name" dataDxfId="20"/>
-    <tableColumn id="18" name="Type" dataDxfId="19"/>
-    <tableColumn id="3" name="Level" dataDxfId="18"/>
-    <tableColumn id="20" name="ReviveScene" dataDxfId="17"/>
-    <tableColumn id="4" name="Quest" dataDxfId="16"/>
-    <tableColumn id="17" name="QuestRandom" dataDxfId="15"/>
-    <tableColumn id="19" name="QuestDungeon" dataDxfId="14"/>
-    <tableColumn id="5" name="QPortal" dataDxfId="13"/>
-    <tableColumn id="6" name="QCardChange" dataDxfId="12"/>
-    <tableColumn id="7" name="QPiece" dataDxfId="11"/>
-    <tableColumn id="8" name="QMerchant" dataDxfId="10"/>
-    <tableColumn id="9" name="QDoctor" dataDxfId="9"/>
-    <tableColumn id="10" name="QAngel" dataDxfId="8"/>
-    <tableColumn id="21" name="QWheel" dataDxfId="7"/>
-    <tableColumn id="22" name="QRes" dataDxfId="6"/>
-    <tableColumn id="11" name="Func" dataDxfId="5"/>
-    <tableColumn id="12" name="Url" dataDxfId="4"/>
-    <tableColumn id="13" name="TilePath" dataDxfId="3"/>
-    <tableColumn id="14" name="Icon" dataDxfId="2"/>
-    <tableColumn id="15" name="IconX" dataDxfId="1"/>
-    <tableColumn id="16" name="IconY" dataDxfId="0"/>
+  <tableColumns count="23">
+    <tableColumn id="1" name="Id" dataDxfId="25"/>
+    <tableColumn id="2" name="Name" dataDxfId="24"/>
+    <tableColumn id="18" name="Type" dataDxfId="23"/>
+    <tableColumn id="3" name="Level" dataDxfId="22"/>
+    <tableColumn id="20" name="ReviveScene" dataDxfId="21"/>
+    <tableColumn id="4" name="Quest" dataDxfId="20"/>
+    <tableColumn id="17" name="QuestRandom" dataDxfId="19"/>
+    <tableColumn id="19" name="QuestDungeon" dataDxfId="18"/>
+    <tableColumn id="5" name="QPortal" dataDxfId="17"/>
+    <tableColumn id="6" name="QCardChange" dataDxfId="16"/>
+    <tableColumn id="7" name="QPiece" dataDxfId="15"/>
+    <tableColumn id="8" name="QMerchant" dataDxfId="14"/>
+    <tableColumn id="9" name="QDoctor" dataDxfId="13"/>
+    <tableColumn id="10" name="QAngel" dataDxfId="12"/>
+    <tableColumn id="21" name="QWheel" dataDxfId="11"/>
+    <tableColumn id="22" name="QRes" dataDxfId="10"/>
+    <tableColumn id="11" name="Func" dataDxfId="9"/>
+    <tableColumn id="12" name="Url" dataDxfId="8"/>
+    <tableColumn id="13" name="TilePath" dataDxfId="7"/>
+    <tableColumn id="14" name="Icon" dataDxfId="6"/>
+    <tableColumn id="15" name="IconX" dataDxfId="5"/>
+    <tableColumn id="16" name="IconY" dataDxfId="4"/>
+    <tableColumn id="24" name="IconColor" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2804,10 +2885,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V46"/>
+  <dimension ref="A1:W46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G16" workbookViewId="0">
-      <selection activeCell="S22" sqref="S22:S33"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2825,11 +2906,11 @@
     <col min="18" max="18" width="9.75" style="5" customWidth="1"/>
     <col min="19" max="19" width="9.5" style="5" customWidth="1"/>
     <col min="20" max="20" width="7.25" style="5" customWidth="1"/>
-    <col min="21" max="22" width="6" style="5" customWidth="1"/>
-    <col min="23" max="16384" width="9" style="5"/>
+    <col min="21" max="23" width="6" style="5" customWidth="1"/>
+    <col min="24" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="60" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:23" ht="60" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -2896,8 +2977,11 @@
       <c r="V1" s="4" t="s">
         <v>83</v>
       </c>
+      <c r="W1" s="4" t="s">
+        <v>245</v>
+      </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
         <v>13</v>
       </c>
@@ -2964,8 +3048,11 @@
       <c r="V2" s="9" t="s">
         <v>13</v>
       </c>
+      <c r="W2" s="9" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A3" s="10" t="s">
         <v>20</v>
       </c>
@@ -3032,8 +3119,11 @@
       <c r="V3" s="10" t="s">
         <v>61</v>
       </c>
+      <c r="W3" s="23" t="s">
+        <v>246</v>
+      </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A4" s="12">
         <v>13010001</v>
       </c>
@@ -3082,8 +3172,11 @@
       <c r="V4" s="13">
         <v>611</v>
       </c>
+      <c r="W4" s="24" t="s">
+        <v>249</v>
+      </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A5" s="12">
         <v>13010002</v>
       </c>
@@ -3136,28 +3229,31 @@
       <c r="V5" s="13">
         <v>571</v>
       </c>
+      <c r="W5" s="24" t="s">
+        <v>249</v>
+      </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A6" s="12">
-        <v>13010004</v>
+        <v>13010003</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C6" s="13">
         <v>2</v>
       </c>
       <c r="D6" s="13">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E6" s="13">
         <v>13010006</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="H6" s="13"/>
       <c r="I6" s="13">
@@ -3165,103 +3261,115 @@
       </c>
       <c r="J6" s="13"/>
       <c r="K6" s="13"/>
-      <c r="L6" s="13">
-        <v>1</v>
-      </c>
+      <c r="L6" s="13"/>
       <c r="M6" s="13"/>
       <c r="N6" s="13"/>
       <c r="O6" s="13"/>
       <c r="P6" s="13"/>
       <c r="Q6" s="13"/>
       <c r="R6" s="13" t="s">
-        <v>35</v>
+        <v>108</v>
       </c>
       <c r="S6" s="13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="T6" s="13" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="U6" s="13">
-        <v>1148</v>
+        <v>1251</v>
       </c>
       <c r="V6" s="13">
-        <v>351</v>
+        <v>432</v>
+      </c>
+      <c r="W6" s="24" t="s">
+        <v>249</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A7" s="12">
-        <v>13010005</v>
+        <v>13010004</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>179</v>
+        <v>2</v>
       </c>
       <c r="C7" s="13">
         <v>2</v>
       </c>
       <c r="D7" s="13">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E7" s="13">
         <v>13010006</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="H7" s="13"/>
       <c r="I7" s="13">
         <v>1</v>
       </c>
-      <c r="J7" s="13">
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13">
         <v>1</v>
       </c>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
       <c r="M7" s="13"/>
       <c r="N7" s="13"/>
       <c r="O7" s="13"/>
       <c r="P7" s="13"/>
       <c r="Q7" s="13"/>
       <c r="R7" s="13" t="s">
-        <v>100</v>
+        <v>35</v>
       </c>
       <c r="S7" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="T7" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="U7" s="13">
-        <v>1386</v>
+        <v>1148</v>
       </c>
       <c r="V7" s="13">
-        <v>339</v>
+        <v>351</v>
+      </c>
+      <c r="W7" s="24" t="s">
+        <v>249</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A8" s="12">
-        <v>13010006</v>
+        <v>13010005</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>3</v>
+        <v>179</v>
       </c>
       <c r="C8" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8" s="13">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E8" s="13">
         <v>13010006</v>
       </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="F8" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>157</v>
+      </c>
       <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
+      <c r="I8" s="13">
+        <v>1</v>
+      </c>
+      <c r="J8" s="13">
+        <v>1</v>
+      </c>
       <c r="K8" s="13"/>
       <c r="L8" s="13"/>
       <c r="M8" s="13"/>
@@ -3270,150 +3378,149 @@
       <c r="P8" s="13"/>
       <c r="Q8" s="13"/>
       <c r="R8" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="S8" s="13" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="T8" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="U8" s="13">
-        <v>1232</v>
+        <v>1386</v>
       </c>
       <c r="V8" s="13">
-        <v>506</v>
+        <v>339</v>
+      </c>
+      <c r="W8" s="24" t="s">
+        <v>249</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A9" s="12">
-        <v>13010007</v>
+        <v>13010006</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C9" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D9" s="13">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E9" s="13">
         <v>13010006</v>
       </c>
-      <c r="F9" s="13" t="s">
-        <v>176</v>
-      </c>
-      <c r="G9" s="13" t="s">
-        <v>174</v>
-      </c>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
       <c r="H9" s="13"/>
-      <c r="I9" s="13">
-        <v>1</v>
-      </c>
+      <c r="I9" s="13"/>
       <c r="J9" s="13"/>
       <c r="K9" s="13"/>
       <c r="L9" s="13"/>
-      <c r="M9" s="13">
-        <v>1</v>
-      </c>
+      <c r="M9" s="13"/>
       <c r="N9" s="13"/>
       <c r="O9" s="13"/>
-      <c r="P9" s="13">
-        <v>1</v>
-      </c>
+      <c r="P9" s="13"/>
       <c r="Q9" s="13"/>
       <c r="R9" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="S9" s="13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="T9" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="U9" s="13">
-        <v>1431</v>
+        <v>1232</v>
       </c>
       <c r="V9" s="13">
-        <v>440</v>
+        <v>506</v>
+      </c>
+      <c r="W9" s="24" t="s">
+        <v>249</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A10" s="12">
-        <v>13010009</v>
+        <v>13010007</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10" s="13">
         <v>2</v>
       </c>
       <c r="D10" s="13">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E10" s="13">
         <v>13010006</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>200</v>
+        <v>174</v>
       </c>
       <c r="H10" s="13"/>
       <c r="I10" s="13">
         <v>1</v>
       </c>
-      <c r="J10" s="13">
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13">
         <v>1</v>
       </c>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13">
-        <v>1</v>
-      </c>
-      <c r="M10" s="13"/>
       <c r="N10" s="13"/>
       <c r="O10" s="13"/>
-      <c r="P10" s="13"/>
+      <c r="P10" s="13">
+        <v>1</v>
+      </c>
       <c r="Q10" s="13"/>
       <c r="R10" s="13" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="S10" s="13" t="s">
-        <v>104</v>
+        <v>34</v>
       </c>
       <c r="T10" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="U10" s="13">
-        <v>1332</v>
+        <v>1431</v>
       </c>
       <c r="V10" s="13">
-        <v>484</v>
+        <v>440</v>
+      </c>
+      <c r="W10" s="24" t="s">
+        <v>249</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A11" s="12">
-        <v>13010010</v>
+        <v>13010008</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C11" s="13">
         <v>2</v>
       </c>
       <c r="D11" s="13">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E11" s="13">
         <v>13010006</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>178</v>
+        <v>159</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>202</v>
+        <v>141</v>
       </c>
       <c r="H11" s="13"/>
       <c r="I11" s="13">
@@ -3423,207 +3530,203 @@
       <c r="K11" s="13"/>
       <c r="L11" s="13"/>
       <c r="M11" s="13"/>
-      <c r="N11" s="13">
-        <v>1</v>
-      </c>
+      <c r="N11" s="13"/>
       <c r="O11" s="13">
         <v>1</v>
       </c>
       <c r="P11" s="13"/>
       <c r="Q11" s="13"/>
       <c r="R11" s="13" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="S11" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="T11" s="13" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="U11" s="13">
-        <v>1441</v>
+        <v>1250</v>
       </c>
       <c r="V11" s="13">
-        <v>527</v>
+        <v>338</v>
+      </c>
+      <c r="W11" s="24" t="s">
+        <v>249</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A12" s="12">
-        <v>13010011</v>
+        <v>13010009</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C12" s="13">
         <v>2</v>
       </c>
       <c r="D12" s="13">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E12" s="13">
         <v>13010006</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>138</v>
+        <v>200</v>
       </c>
       <c r="H12" s="13"/>
       <c r="I12" s="13">
         <v>1</v>
       </c>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13">
+      <c r="J12" s="13">
         <v>1</v>
       </c>
-      <c r="L12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13">
+        <v>1</v>
+      </c>
       <c r="M12" s="13"/>
       <c r="N12" s="13"/>
       <c r="O12" s="13"/>
-      <c r="P12" s="13">
-        <v>1</v>
-      </c>
+      <c r="P12" s="13"/>
       <c r="Q12" s="13"/>
       <c r="R12" s="13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="S12" s="13" t="s">
-        <v>39</v>
+        <v>104</v>
       </c>
       <c r="T12" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="U12" s="13">
-        <v>1574</v>
+        <v>1332</v>
       </c>
       <c r="V12" s="13">
-        <v>373</v>
+        <v>484</v>
+      </c>
+      <c r="W12" s="24" t="s">
+        <v>249</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A13" s="12">
-        <v>13010012</v>
+        <v>13010010</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="13">
+        <v>128</v>
+      </c>
+      <c r="C13" s="15">
         <v>2</v>
       </c>
-      <c r="D13" s="13">
-        <v>3</v>
+      <c r="D13" s="15">
+        <v>6</v>
       </c>
       <c r="E13" s="13">
         <v>13010006</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>140</v>
+        <v>168</v>
       </c>
       <c r="H13" s="13"/>
-      <c r="I13" s="13">
+      <c r="I13" s="15">
         <v>1</v>
       </c>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="13"/>
-      <c r="O13" s="13"/>
-      <c r="P13" s="13"/>
-      <c r="Q13" s="13"/>
-      <c r="R13" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="S13" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="T13" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="U13" s="13">
-        <v>1251</v>
-      </c>
-      <c r="V13" s="13">
-        <v>432</v>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="S13" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="T13" s="15"/>
+      <c r="U13" s="15"/>
+      <c r="V13" s="15"/>
+      <c r="W13" s="24" t="s">
+        <v>249</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A14" s="12">
-        <v>13010013</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>9</v>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A14" s="27">
+        <v>13010101</v>
+      </c>
+      <c r="B14" s="27" t="s">
+        <v>12</v>
       </c>
       <c r="C14" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D14" s="13">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="E14" s="13">
-        <v>13010006</v>
-      </c>
-      <c r="F14" s="13" t="s">
-        <v>159</v>
-      </c>
-      <c r="G14" s="13" t="s">
-        <v>141</v>
-      </c>
+        <v>13010101</v>
+      </c>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
       <c r="H14" s="13"/>
-      <c r="I14" s="13">
-        <v>1</v>
-      </c>
+      <c r="I14" s="13"/>
       <c r="J14" s="13"/>
       <c r="K14" s="13"/>
       <c r="L14" s="13"/>
       <c r="M14" s="13"/>
       <c r="N14" s="13"/>
-      <c r="O14" s="13">
-        <v>1</v>
-      </c>
+      <c r="O14" s="13"/>
       <c r="P14" s="13"/>
       <c r="Q14" s="13"/>
       <c r="R14" s="13" t="s">
-        <v>109</v>
+        <v>211</v>
       </c>
       <c r="S14" s="13" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="T14" s="13" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="U14" s="13">
-        <v>1250</v>
+        <v>894</v>
       </c>
       <c r="V14" s="13">
-        <v>338</v>
+        <v>509</v>
+      </c>
+      <c r="W14" s="24" t="s">
+        <v>247</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A15" s="12">
-        <v>13010014</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>10</v>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A15" s="27">
+        <v>13010102</v>
+      </c>
+      <c r="B15" s="27" t="s">
+        <v>11</v>
       </c>
       <c r="C15" s="13">
         <v>2</v>
       </c>
       <c r="D15" s="13">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E15" s="13">
-        <v>13010006</v>
+        <v>13010101</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>171</v>
+        <v>95</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>175</v>
+        <v>121</v>
       </c>
       <c r="H15" s="13"/>
       <c r="I15" s="13">
@@ -3631,193 +3734,213 @@
       </c>
       <c r="J15" s="13"/>
       <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="13">
+      <c r="L15" s="13">
         <v>1</v>
       </c>
-      <c r="N15" s="13">
-        <v>1</v>
-      </c>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
       <c r="O15" s="13"/>
       <c r="P15" s="13"/>
       <c r="Q15" s="13"/>
       <c r="R15" s="13" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="S15" s="13" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="T15" s="13" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="U15" s="13">
-        <v>1550</v>
+        <v>1040</v>
       </c>
       <c r="V15" s="13">
-        <v>505</v>
+        <v>538</v>
+      </c>
+      <c r="W15" s="24" t="s">
+        <v>247</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A16" s="12">
-        <v>13010015</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="C16" s="15">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A16" s="27">
+        <v>13010103</v>
+      </c>
+      <c r="B16" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="13">
         <v>2</v>
       </c>
-      <c r="D16" s="15">
-        <v>6</v>
+      <c r="D16" s="13">
+        <v>19</v>
       </c>
       <c r="E16" s="13">
-        <v>13010006</v>
+        <v>13010101</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>152</v>
+        <v>170</v>
       </c>
       <c r="G16" s="13" t="s">
-        <v>168</v>
+        <v>203</v>
       </c>
       <c r="H16" s="13"/>
-      <c r="I16" s="15">
+      <c r="I16" s="13">
         <v>1</v>
       </c>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="15"/>
-      <c r="O16" s="15"/>
-      <c r="P16" s="15"/>
-      <c r="Q16" s="15"/>
-      <c r="R16" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="S16" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="T16" s="15"/>
-      <c r="U16" s="15"/>
-      <c r="V16" s="15"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="13"/>
+      <c r="O16" s="13"/>
+      <c r="P16" s="13"/>
+      <c r="Q16" s="13"/>
+      <c r="R16" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="S16" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="T16" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="U16" s="13">
+        <v>1213</v>
+      </c>
+      <c r="V16" s="13">
+        <v>655</v>
+      </c>
+      <c r="W16" s="24" t="s">
+        <v>247</v>
+      </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A17" s="16">
-        <v>13010101</v>
-      </c>
-      <c r="B17" s="16" t="s">
-        <v>12</v>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A17" s="27">
+        <v>13010104</v>
+      </c>
+      <c r="B17" s="27" t="s">
+        <v>41</v>
       </c>
       <c r="C17" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D17" s="13">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E17" s="13">
         <v>13010101</v>
       </c>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
+      <c r="F17" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>137</v>
+      </c>
       <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
+      <c r="I17" s="13">
+        <v>1</v>
+      </c>
       <c r="J17" s="13"/>
       <c r="K17" s="13"/>
       <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
+      <c r="M17" s="13">
+        <v>1</v>
+      </c>
       <c r="N17" s="13"/>
       <c r="O17" s="13"/>
       <c r="P17" s="13"/>
       <c r="Q17" s="13"/>
       <c r="R17" s="13" t="s">
-        <v>211</v>
+        <v>112</v>
       </c>
       <c r="S17" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="T17" s="13" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="U17" s="13">
-        <v>894</v>
+        <v>1149</v>
       </c>
       <c r="V17" s="13">
-        <v>509</v>
+        <v>584</v>
+      </c>
+      <c r="W17" s="24" t="s">
+        <v>247</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A18" s="16">
-        <v>13010102</v>
-      </c>
-      <c r="B18" s="16" t="s">
-        <v>11</v>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A18" s="27">
+        <v>13010105</v>
+      </c>
+      <c r="B18" s="27" t="s">
+        <v>42</v>
       </c>
       <c r="C18" s="13">
         <v>2</v>
       </c>
       <c r="D18" s="13">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E18" s="13">
         <v>13010101</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>121</v>
+        <v>142</v>
       </c>
       <c r="H18" s="13"/>
-      <c r="I18" s="13">
-        <v>1</v>
-      </c>
+      <c r="I18" s="13"/>
       <c r="J18" s="13"/>
       <c r="K18" s="13"/>
-      <c r="L18" s="13">
-        <v>1</v>
-      </c>
+      <c r="L18" s="13"/>
       <c r="M18" s="13"/>
       <c r="N18" s="13"/>
       <c r="O18" s="13"/>
       <c r="P18" s="13"/>
       <c r="Q18" s="13"/>
       <c r="R18" s="13" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="S18" s="13" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="T18" s="13" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="U18" s="13">
-        <v>1040</v>
+        <v>840</v>
       </c>
       <c r="V18" s="13">
-        <v>538</v>
+        <v>444</v>
+      </c>
+      <c r="W18" s="24" t="s">
+        <v>247</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A19" s="16">
-        <v>13010103</v>
-      </c>
-      <c r="B19" s="16" t="s">
-        <v>44</v>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A19" s="27">
+        <v>13010106</v>
+      </c>
+      <c r="B19" s="27" t="s">
+        <v>130</v>
       </c>
       <c r="C19" s="13">
         <v>2</v>
       </c>
       <c r="D19" s="13">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E19" s="13">
-        <v>13010101</v>
+        <v>13010016</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>170</v>
+        <v>148</v>
       </c>
       <c r="G19" s="13" t="s">
-        <v>203</v>
+        <v>143</v>
       </c>
       <c r="H19" s="13"/>
       <c r="I19" s="13">
@@ -3827,183 +3950,177 @@
       <c r="K19" s="13"/>
       <c r="L19" s="13"/>
       <c r="M19" s="13"/>
-      <c r="N19" s="13"/>
+      <c r="N19" s="13">
+        <v>1</v>
+      </c>
       <c r="O19" s="13"/>
       <c r="P19" s="13"/>
       <c r="Q19" s="13"/>
       <c r="R19" s="13" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="S19" s="13" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="T19" s="13" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="U19" s="13">
-        <v>1213</v>
+        <v>1067</v>
       </c>
       <c r="V19" s="13">
-        <v>655</v>
+        <v>445</v>
+      </c>
+      <c r="W19" s="24" t="s">
+        <v>247</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A20" s="16">
-        <v>13010104</v>
-      </c>
-      <c r="B20" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" s="13">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A20" s="27">
+        <v>13010107</v>
+      </c>
+      <c r="B20" s="27" t="s">
+        <v>232</v>
+      </c>
+      <c r="C20" s="15">
         <v>2</v>
       </c>
-      <c r="D20" s="13">
-        <v>18</v>
-      </c>
-      <c r="E20" s="13">
+      <c r="D20" s="15">
+        <v>15</v>
+      </c>
+      <c r="E20" s="15">
         <v>13010101</v>
       </c>
-      <c r="F20" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="G20" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13">
-        <v>1</v>
-      </c>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13">
-        <v>1</v>
-      </c>
-      <c r="N20" s="13"/>
-      <c r="O20" s="13"/>
-      <c r="P20" s="13"/>
-      <c r="Q20" s="13"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
+      <c r="L20" s="16"/>
+      <c r="M20" s="16"/>
+      <c r="N20" s="16"/>
+      <c r="O20" s="15"/>
+      <c r="P20" s="15"/>
+      <c r="Q20" s="16"/>
       <c r="R20" s="13" t="s">
-        <v>112</v>
+        <v>236</v>
       </c>
       <c r="S20" s="13" t="s">
-        <v>45</v>
+        <v>236</v>
       </c>
       <c r="T20" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="U20" s="13">
-        <v>1149</v>
-      </c>
-      <c r="V20" s="13">
-        <v>584</v>
+        <v>220</v>
+      </c>
+      <c r="U20" s="16">
+        <v>850</v>
+      </c>
+      <c r="V20" s="16">
+        <v>589</v>
+      </c>
+      <c r="W20" s="24" t="s">
+        <v>247</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A21" s="16">
-        <v>13010105</v>
-      </c>
-      <c r="B21" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" s="13">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A21" s="27">
+        <v>13010108</v>
+      </c>
+      <c r="B21" s="27" t="s">
+        <v>228</v>
+      </c>
+      <c r="C21" s="15">
         <v>2</v>
       </c>
-      <c r="D21" s="13">
-        <v>20</v>
-      </c>
-      <c r="E21" s="13">
+      <c r="D21" s="15">
+        <v>15</v>
+      </c>
+      <c r="E21" s="15">
         <v>13010101</v>
       </c>
-      <c r="F21" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="G21" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="13"/>
-      <c r="N21" s="13"/>
-      <c r="O21" s="13"/>
-      <c r="P21" s="13"/>
-      <c r="Q21" s="13"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
+      <c r="L21" s="16"/>
+      <c r="M21" s="16"/>
+      <c r="N21" s="16"/>
+      <c r="O21" s="15"/>
+      <c r="P21" s="15"/>
+      <c r="Q21" s="16"/>
       <c r="R21" s="13" t="s">
-        <v>113</v>
+        <v>238</v>
       </c>
       <c r="S21" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="T21" s="13" t="s">
-        <v>81</v>
+        <v>238</v>
+      </c>
+      <c r="T21" s="16" t="s">
+        <v>224</v>
       </c>
       <c r="U21" s="13">
-        <v>840</v>
+        <v>682</v>
       </c>
       <c r="V21" s="13">
-        <v>444</v>
+        <v>545</v>
+      </c>
+      <c r="W21" s="24" t="s">
+        <v>247</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A22" s="16">
-        <v>13010106</v>
-      </c>
-      <c r="B22" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="C22" s="13">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A22" s="25">
+        <v>13010201</v>
+      </c>
+      <c r="B22" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="C22" s="15">
         <v>2</v>
       </c>
-      <c r="D22" s="13">
+      <c r="D22" s="15">
         <v>15</v>
       </c>
-      <c r="E22" s="13">
-        <v>13010016</v>
-      </c>
-      <c r="F22" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="G22" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13">
-        <v>1</v>
-      </c>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="13">
-        <v>1</v>
-      </c>
-      <c r="O22" s="13"/>
-      <c r="P22" s="13"/>
-      <c r="Q22" s="13"/>
+      <c r="E22" s="15">
+        <v>13010201</v>
+      </c>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="16"/>
+      <c r="L22" s="16"/>
+      <c r="M22" s="16"/>
+      <c r="N22" s="16"/>
+      <c r="O22" s="15"/>
+      <c r="P22" s="15"/>
+      <c r="Q22" s="16"/>
       <c r="R22" s="13" t="s">
-        <v>103</v>
+        <v>234</v>
       </c>
       <c r="S22" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="T22" s="13" t="s">
-        <v>71</v>
+        <v>234</v>
+      </c>
+      <c r="T22" s="16" t="s">
+        <v>221</v>
       </c>
       <c r="U22" s="13">
-        <v>1067</v>
+        <v>807</v>
       </c>
       <c r="V22" s="13">
-        <v>445</v>
+        <v>720</v>
+      </c>
+      <c r="W22" s="24" t="s">
+        <v>248</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A23" s="16">
-        <v>13010107</v>
-      </c>
-      <c r="B23" s="16" t="s">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A23" s="25">
+        <v>13010202</v>
+      </c>
+      <c r="B23" s="25" t="s">
         <v>212</v>
       </c>
       <c r="C23" s="15">
@@ -4013,7 +4130,7 @@
         <v>15</v>
       </c>
       <c r="E23" s="15">
-        <v>13010101</v>
+        <v>13010201</v>
       </c>
       <c r="F23" s="15"/>
       <c r="G23" s="15"/>
@@ -4042,12 +4159,15 @@
       <c r="V23" s="15">
         <v>594</v>
       </c>
+      <c r="W23" s="24" t="s">
+        <v>248</v>
+      </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A24" s="16">
-        <v>13010108</v>
-      </c>
-      <c r="B24" s="16" t="s">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A24" s="25">
+        <v>13010203</v>
+      </c>
+      <c r="B24" s="25" t="s">
         <v>213</v>
       </c>
       <c r="C24" s="15">
@@ -4057,7 +4177,7 @@
         <v>15</v>
       </c>
       <c r="E24" s="15">
-        <v>13010101</v>
+        <v>13010201</v>
       </c>
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
@@ -4086,13 +4206,16 @@
       <c r="V24" s="15">
         <v>720</v>
       </c>
+      <c r="W24" s="24" t="s">
+        <v>248</v>
+      </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A25" s="16">
-        <v>13010109</v>
-      </c>
-      <c r="B25" s="17" t="s">
-        <v>233</v>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A25" s="25">
+        <v>13010204</v>
+      </c>
+      <c r="B25" s="26" t="s">
+        <v>216</v>
       </c>
       <c r="C25" s="15">
         <v>2</v>
@@ -4101,7 +4224,7 @@
         <v>15</v>
       </c>
       <c r="E25" s="15">
-        <v>13010101</v>
+        <v>13010201</v>
       </c>
       <c r="F25" s="15"/>
       <c r="G25" s="15"/>
@@ -4116,27 +4239,30 @@
       <c r="P25" s="15"/>
       <c r="Q25" s="15"/>
       <c r="R25" s="13" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="S25" s="13" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="T25" s="15" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="U25" s="15">
-        <v>894</v>
+        <v>1074</v>
       </c>
       <c r="V25" s="15">
-        <v>679</v>
+        <v>630</v>
+      </c>
+      <c r="W25" s="24" t="s">
+        <v>248</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A26" s="16">
-        <v>13010110</v>
-      </c>
-      <c r="B26" s="17" t="s">
-        <v>216</v>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A26" s="25">
+        <v>13010205</v>
+      </c>
+      <c r="B26" s="25" t="s">
+        <v>229</v>
       </c>
       <c r="C26" s="15">
         <v>2</v>
@@ -4145,42 +4271,45 @@
         <v>15</v>
       </c>
       <c r="E26" s="15">
-        <v>13010101</v>
-      </c>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="15"/>
-      <c r="I26" s="15"/>
-      <c r="J26" s="15"/>
-      <c r="K26" s="15"/>
-      <c r="L26" s="15"/>
-      <c r="M26" s="15"/>
-      <c r="N26" s="15"/>
+        <v>13010201</v>
+      </c>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="16"/>
+      <c r="L26" s="16"/>
+      <c r="M26" s="16"/>
+      <c r="N26" s="16"/>
       <c r="O26" s="15"/>
       <c r="P26" s="15"/>
-      <c r="Q26" s="15"/>
-      <c r="R26" s="13" t="s">
-        <v>241</v>
-      </c>
-      <c r="S26" s="13" t="s">
-        <v>241</v>
-      </c>
-      <c r="T26" s="15" t="s">
-        <v>217</v>
-      </c>
-      <c r="U26" s="15">
-        <v>1074</v>
-      </c>
-      <c r="V26" s="15">
-        <v>630</v>
+      <c r="Q26" s="16"/>
+      <c r="R26" s="20" t="s">
+        <v>237</v>
+      </c>
+      <c r="S26" s="20" t="s">
+        <v>237</v>
+      </c>
+      <c r="T26" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="U26" s="13">
+        <v>717</v>
+      </c>
+      <c r="V26" s="13">
+        <v>655</v>
+      </c>
+      <c r="W26" s="24" t="s">
+        <v>248</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A27" s="16">
-        <v>13010111</v>
-      </c>
-      <c r="B27" s="16" t="s">
-        <v>232</v>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A27" s="25">
+        <v>13010206</v>
+      </c>
+      <c r="B27" s="25" t="s">
+        <v>227</v>
       </c>
       <c r="C27" s="15">
         <v>2</v>
@@ -4189,42 +4318,45 @@
         <v>15</v>
       </c>
       <c r="E27" s="15">
-        <v>13010101</v>
-      </c>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
-      <c r="K27" s="18"/>
-      <c r="L27" s="18"/>
-      <c r="M27" s="18"/>
-      <c r="N27" s="18"/>
+        <v>13010201</v>
+      </c>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16"/>
+      <c r="N27" s="16"/>
       <c r="O27" s="15"/>
       <c r="P27" s="15"/>
-      <c r="Q27" s="18"/>
-      <c r="R27" s="13" t="s">
-        <v>236</v>
-      </c>
-      <c r="S27" s="13" t="s">
-        <v>236</v>
-      </c>
-      <c r="T27" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="U27" s="18">
-        <v>850</v>
-      </c>
-      <c r="V27" s="18">
-        <v>589</v>
+      <c r="Q27" s="16"/>
+      <c r="R27" s="20" t="s">
+        <v>243</v>
+      </c>
+      <c r="S27" s="20" t="s">
+        <v>243</v>
+      </c>
+      <c r="T27" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="U27" s="13">
+        <v>637</v>
+      </c>
+      <c r="V27" s="13">
+        <v>735</v>
+      </c>
+      <c r="W27" s="24" t="s">
+        <v>248</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A28" s="16">
-        <v>13010112</v>
-      </c>
-      <c r="B28" s="16" t="s">
-        <v>230</v>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A28" s="25">
+        <v>13010207</v>
+      </c>
+      <c r="B28" s="25" t="s">
+        <v>226</v>
       </c>
       <c r="C28" s="15">
         <v>2</v>
@@ -4233,42 +4365,45 @@
         <v>15</v>
       </c>
       <c r="E28" s="15">
-        <v>13010101</v>
-      </c>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="18"/>
-      <c r="J28" s="18"/>
-      <c r="K28" s="18"/>
-      <c r="L28" s="18"/>
-      <c r="M28" s="18"/>
-      <c r="N28" s="18"/>
+        <v>13010201</v>
+      </c>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="15"/>
+      <c r="K28" s="15"/>
+      <c r="L28" s="15"/>
+      <c r="M28" s="15"/>
+      <c r="N28" s="15"/>
       <c r="O28" s="15"/>
       <c r="P28" s="15"/>
-      <c r="Q28" s="18"/>
-      <c r="R28" s="22" t="s">
-        <v>244</v>
-      </c>
-      <c r="S28" s="22" t="s">
-        <v>244</v>
-      </c>
-      <c r="T28" s="18" t="s">
-        <v>219</v>
-      </c>
-      <c r="U28" s="15">
-        <v>984</v>
-      </c>
-      <c r="V28" s="15">
-        <v>734</v>
+      <c r="Q28" s="15"/>
+      <c r="R28" s="13" t="s">
+        <v>242</v>
+      </c>
+      <c r="S28" s="13" t="s">
+        <v>242</v>
+      </c>
+      <c r="T28" s="13" t="s">
+        <v>225</v>
+      </c>
+      <c r="U28" s="13">
+        <v>737</v>
+      </c>
+      <c r="V28" s="13">
+        <v>785</v>
+      </c>
+      <c r="W28" s="24" t="s">
+        <v>248</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A29" s="16">
-        <v>13010113</v>
-      </c>
-      <c r="B29" s="16" t="s">
-        <v>231</v>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A29" s="25">
+        <v>13010208</v>
+      </c>
+      <c r="B29" s="26" t="s">
+        <v>233</v>
       </c>
       <c r="C29" s="15">
         <v>2</v>
@@ -4277,42 +4412,45 @@
         <v>15</v>
       </c>
       <c r="E29" s="15">
-        <v>13010101</v>
-      </c>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
-      <c r="H29" s="18"/>
-      <c r="I29" s="18"/>
-      <c r="J29" s="18"/>
-      <c r="K29" s="18"/>
-      <c r="L29" s="18"/>
-      <c r="M29" s="18"/>
-      <c r="N29" s="18"/>
+        <v>13010201</v>
+      </c>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="15"/>
+      <c r="J29" s="15"/>
+      <c r="K29" s="15"/>
+      <c r="L29" s="15"/>
+      <c r="M29" s="15"/>
+      <c r="N29" s="15"/>
       <c r="O29" s="15"/>
       <c r="P29" s="15"/>
-      <c r="Q29" s="18"/>
+      <c r="Q29" s="15"/>
       <c r="R29" s="13" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="S29" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="T29" s="18" t="s">
-        <v>221</v>
-      </c>
-      <c r="U29" s="5">
-        <v>807</v>
-      </c>
-      <c r="V29" s="5">
-        <v>720</v>
+        <v>235</v>
+      </c>
+      <c r="T29" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="U29" s="19">
+        <v>894</v>
+      </c>
+      <c r="V29" s="19">
+        <v>679</v>
+      </c>
+      <c r="W29" s="24" t="s">
+        <v>248</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A30" s="16">
-        <v>13010114</v>
-      </c>
-      <c r="B30" s="16" t="s">
-        <v>229</v>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A30" s="25">
+        <v>13010209</v>
+      </c>
+      <c r="B30" s="25" t="s">
+        <v>230</v>
       </c>
       <c r="C30" s="15">
         <v>2</v>
@@ -4321,176 +4459,218 @@
         <v>15</v>
       </c>
       <c r="E30" s="15">
-        <v>13010101</v>
-      </c>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
-      <c r="H30" s="18"/>
-      <c r="I30" s="18"/>
-      <c r="J30" s="18"/>
-      <c r="K30" s="18"/>
-      <c r="L30" s="18"/>
-      <c r="M30" s="18"/>
-      <c r="N30" s="18"/>
+        <v>13010201</v>
+      </c>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="16"/>
+      <c r="K30" s="16"/>
+      <c r="L30" s="16"/>
+      <c r="M30" s="16"/>
+      <c r="N30" s="16"/>
       <c r="O30" s="15"/>
       <c r="P30" s="15"/>
-      <c r="Q30" s="18"/>
-      <c r="R30" s="22" t="s">
-        <v>237</v>
-      </c>
-      <c r="S30" s="22" t="s">
-        <v>237</v>
-      </c>
-      <c r="T30" s="18" t="s">
-        <v>222</v>
-      </c>
-      <c r="U30" s="5">
-        <v>717</v>
-      </c>
-      <c r="V30" s="5">
-        <v>655</v>
+      <c r="Q30" s="16"/>
+      <c r="R30" s="20" t="s">
+        <v>244</v>
+      </c>
+      <c r="S30" s="20" t="s">
+        <v>244</v>
+      </c>
+      <c r="T30" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="U30" s="19">
+        <v>984</v>
+      </c>
+      <c r="V30" s="19">
+        <v>734</v>
+      </c>
+      <c r="W30" s="24" t="s">
+        <v>248</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A31" s="16">
-        <v>13010115</v>
-      </c>
-      <c r="B31" s="16" t="s">
-        <v>227</v>
-      </c>
-      <c r="C31" s="15">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A31" s="28">
+        <v>13010301</v>
+      </c>
+      <c r="B31" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" s="13">
         <v>2</v>
       </c>
-      <c r="D31" s="15">
-        <v>15</v>
-      </c>
-      <c r="E31" s="15">
-        <v>13010101</v>
-      </c>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
-      <c r="H31" s="18"/>
-      <c r="I31" s="18"/>
-      <c r="J31" s="18"/>
-      <c r="K31" s="18"/>
-      <c r="L31" s="18"/>
-      <c r="M31" s="18"/>
-      <c r="N31" s="18"/>
-      <c r="O31" s="15"/>
-      <c r="P31" s="15"/>
-      <c r="Q31" s="18"/>
-      <c r="R31" s="22" t="s">
-        <v>243</v>
-      </c>
-      <c r="S31" s="22" t="s">
-        <v>243</v>
-      </c>
-      <c r="T31" s="18" t="s">
-        <v>223</v>
-      </c>
-      <c r="U31" s="5">
-        <v>637</v>
-      </c>
-      <c r="V31" s="5">
-        <v>735</v>
+      <c r="D31" s="13">
+        <v>14</v>
+      </c>
+      <c r="E31" s="13">
+        <v>13010006</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="G31" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13">
+        <v>1</v>
+      </c>
+      <c r="J31" s="13"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13"/>
+      <c r="M31" s="13">
+        <v>1</v>
+      </c>
+      <c r="N31" s="13">
+        <v>1</v>
+      </c>
+      <c r="O31" s="13"/>
+      <c r="P31" s="13"/>
+      <c r="Q31" s="13"/>
+      <c r="R31" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="S31" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="T31" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="U31" s="21">
+        <v>1550</v>
+      </c>
+      <c r="V31" s="21">
+        <v>505</v>
+      </c>
+      <c r="W31" s="24" t="s">
+        <v>250</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A32" s="16">
-        <v>13010116</v>
-      </c>
-      <c r="B32" s="16" t="s">
-        <v>228</v>
-      </c>
-      <c r="C32" s="15">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A32" s="28">
+        <v>13010302</v>
+      </c>
+      <c r="B32" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" s="13">
         <v>2</v>
       </c>
-      <c r="D32" s="15">
-        <v>15</v>
-      </c>
-      <c r="E32" s="15">
-        <v>13010101</v>
-      </c>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="18"/>
-      <c r="I32" s="18"/>
-      <c r="J32" s="18"/>
-      <c r="K32" s="18"/>
-      <c r="L32" s="18"/>
-      <c r="M32" s="18"/>
-      <c r="N32" s="18"/>
-      <c r="O32" s="15"/>
-      <c r="P32" s="15"/>
-      <c r="Q32" s="18"/>
+      <c r="D32" s="13">
+        <v>10</v>
+      </c>
+      <c r="E32" s="13">
+        <v>13010006</v>
+      </c>
+      <c r="F32" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="G32" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="H32" s="13"/>
+      <c r="I32" s="13">
+        <v>1</v>
+      </c>
+      <c r="J32" s="13"/>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="13"/>
+      <c r="N32" s="13">
+        <v>1</v>
+      </c>
+      <c r="O32" s="13">
+        <v>1</v>
+      </c>
+      <c r="P32" s="13"/>
+      <c r="Q32" s="13"/>
       <c r="R32" s="13" t="s">
-        <v>238</v>
+        <v>106</v>
       </c>
       <c r="S32" s="13" t="s">
-        <v>238</v>
-      </c>
-      <c r="T32" s="18" t="s">
-        <v>224</v>
-      </c>
-      <c r="U32" s="5">
-        <v>682</v>
-      </c>
-      <c r="V32" s="5">
-        <v>545</v>
+        <v>38</v>
+      </c>
+      <c r="T32" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="U32" s="21">
+        <v>1441</v>
+      </c>
+      <c r="V32" s="21">
+        <v>527</v>
+      </c>
+      <c r="W32" s="24" t="s">
+        <v>250</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A33" s="16">
-        <v>13010117</v>
-      </c>
-      <c r="B33" s="16" t="s">
-        <v>226</v>
-      </c>
-      <c r="C33" s="15">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A33" s="28">
+        <v>13010303</v>
+      </c>
+      <c r="B33" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" s="13">
         <v>2</v>
       </c>
-      <c r="D33" s="15">
-        <v>15</v>
-      </c>
-      <c r="E33" s="15">
-        <v>13010101</v>
-      </c>
-      <c r="F33" s="15"/>
-      <c r="G33" s="15"/>
-      <c r="H33" s="15"/>
-      <c r="I33" s="15"/>
-      <c r="J33" s="15"/>
-      <c r="K33" s="15"/>
-      <c r="L33" s="15"/>
-      <c r="M33" s="15"/>
-      <c r="N33" s="15"/>
-      <c r="O33" s="15"/>
-      <c r="P33" s="15"/>
-      <c r="Q33" s="15"/>
+      <c r="D33" s="13">
+        <v>12</v>
+      </c>
+      <c r="E33" s="13">
+        <v>13010006</v>
+      </c>
+      <c r="F33" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="G33" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13">
+        <v>1</v>
+      </c>
+      <c r="J33" s="13"/>
+      <c r="K33" s="13">
+        <v>1</v>
+      </c>
+      <c r="L33" s="13"/>
+      <c r="M33" s="13"/>
+      <c r="N33" s="13"/>
+      <c r="O33" s="13"/>
+      <c r="P33" s="13">
+        <v>1</v>
+      </c>
+      <c r="Q33" s="13"/>
       <c r="R33" s="13" t="s">
-        <v>242</v>
+        <v>107</v>
       </c>
       <c r="S33" s="13" t="s">
-        <v>242</v>
+        <v>39</v>
       </c>
       <c r="T33" s="13" t="s">
-        <v>225</v>
-      </c>
-      <c r="U33" s="5">
-        <v>737</v>
-      </c>
-      <c r="V33" s="5">
-        <v>785</v>
+        <v>74</v>
+      </c>
+      <c r="U33" s="21">
+        <v>1574</v>
+      </c>
+      <c r="V33" s="21">
+        <v>373</v>
+      </c>
+      <c r="W33" s="24" t="s">
+        <v>250</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A34" s="19">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A34" s="17">
         <v>13020001</v>
       </c>
-      <c r="B34" s="19" t="s">
+      <c r="B34" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="C34" s="19">
+      <c r="C34" s="17">
         <v>3</v>
       </c>
       <c r="D34" s="13">
@@ -4524,15 +4704,16 @@
       <c r="T34" s="13"/>
       <c r="U34" s="13"/>
       <c r="V34" s="13"/>
+      <c r="W34" s="22"/>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A35" s="19">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A35" s="17">
         <v>13020002</v>
       </c>
-      <c r="B35" s="19" t="s">
+      <c r="B35" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="C35" s="19">
+      <c r="C35" s="17">
         <v>3</v>
       </c>
       <c r="D35" s="13">
@@ -4562,15 +4743,16 @@
       <c r="T35" s="13"/>
       <c r="U35" s="13"/>
       <c r="V35" s="13"/>
+      <c r="W35" s="22"/>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A36" s="19">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A36" s="17">
         <v>13020011</v>
       </c>
-      <c r="B36" s="19" t="s">
+      <c r="B36" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="C36" s="19">
+      <c r="C36" s="17">
         <v>3</v>
       </c>
       <c r="D36" s="13">
@@ -4604,15 +4786,16 @@
       <c r="T36" s="13"/>
       <c r="U36" s="13"/>
       <c r="V36" s="13"/>
+      <c r="W36" s="22"/>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A37" s="19">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A37" s="17">
         <v>13020012</v>
       </c>
-      <c r="B37" s="19" t="s">
+      <c r="B37" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="C37" s="19">
+      <c r="C37" s="17">
         <v>3</v>
       </c>
       <c r="D37" s="13">
@@ -4644,15 +4827,16 @@
       <c r="T37" s="13"/>
       <c r="U37" s="13"/>
       <c r="V37" s="13"/>
+      <c r="W37" s="22"/>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A38" s="19">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A38" s="17">
         <v>13020013</v>
       </c>
-      <c r="B38" s="19" t="s">
+      <c r="B38" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="C38" s="19">
+      <c r="C38" s="17">
         <v>3</v>
       </c>
       <c r="D38" s="13">
@@ -4682,15 +4866,16 @@
       <c r="T38" s="13"/>
       <c r="U38" s="13"/>
       <c r="V38" s="13"/>
+      <c r="W38" s="22"/>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A39" s="19">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A39" s="17">
         <v>13020021</v>
       </c>
-      <c r="B39" s="19" t="s">
+      <c r="B39" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="C39" s="19">
+      <c r="C39" s="17">
         <v>3</v>
       </c>
       <c r="D39" s="13">
@@ -4726,15 +4911,16 @@
       <c r="T39" s="13"/>
       <c r="U39" s="13"/>
       <c r="V39" s="13"/>
+      <c r="W39" s="22"/>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A40" s="19">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A40" s="17">
         <v>13020022</v>
       </c>
-      <c r="B40" s="19" t="s">
+      <c r="B40" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="C40" s="19">
+      <c r="C40" s="17">
         <v>3</v>
       </c>
       <c r="D40" s="13">
@@ -4770,15 +4956,16 @@
       <c r="T40" s="13"/>
       <c r="U40" s="13"/>
       <c r="V40" s="13"/>
+      <c r="W40" s="22"/>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A41" s="19">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A41" s="17">
         <v>13020023</v>
       </c>
-      <c r="B41" s="19" t="s">
+      <c r="B41" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="C41" s="19">
+      <c r="C41" s="17">
         <v>3</v>
       </c>
       <c r="D41" s="13">
@@ -4814,15 +5001,16 @@
       <c r="T41" s="13"/>
       <c r="U41" s="13"/>
       <c r="V41" s="13"/>
+      <c r="W41" s="22"/>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A42" s="20">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A42" s="18">
         <v>13020031</v>
       </c>
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="17" t="s">
         <v>180</v>
       </c>
-      <c r="C42" s="20">
+      <c r="C42" s="18">
         <v>3</v>
       </c>
       <c r="D42" s="15">
@@ -4854,15 +5042,16 @@
       <c r="T42" s="15"/>
       <c r="U42" s="15"/>
       <c r="V42" s="15"/>
+      <c r="W42" s="22"/>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A43" s="20">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A43" s="18">
         <v>13020032</v>
       </c>
-      <c r="B43" s="19" t="s">
+      <c r="B43" s="17" t="s">
         <v>182</v>
       </c>
-      <c r="C43" s="20">
+      <c r="C43" s="18">
         <v>3</v>
       </c>
       <c r="D43" s="15">
@@ -4894,15 +5083,16 @@
       <c r="T43" s="15"/>
       <c r="U43" s="15"/>
       <c r="V43" s="15"/>
+      <c r="W43" s="22"/>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A44" s="20">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A44" s="18">
         <v>13020033</v>
       </c>
-      <c r="B44" s="19" t="s">
+      <c r="B44" s="17" t="s">
         <v>183</v>
       </c>
-      <c r="C44" s="20">
+      <c r="C44" s="18">
         <v>3</v>
       </c>
       <c r="D44" s="15">
@@ -4931,18 +5121,19 @@
       <c r="S44" s="15" t="s">
         <v>188</v>
       </c>
-      <c r="T44" s="21"/>
-      <c r="U44" s="21"/>
-      <c r="V44" s="21"/>
+      <c r="T44" s="19"/>
+      <c r="U44" s="19"/>
+      <c r="V44" s="19"/>
+      <c r="W44" s="22"/>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A45" s="20">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A45" s="18">
         <v>13020034</v>
       </c>
-      <c r="B45" s="19" t="s">
+      <c r="B45" s="17" t="s">
         <v>184</v>
       </c>
-      <c r="C45" s="20">
+      <c r="C45" s="18">
         <v>3</v>
       </c>
       <c r="D45" s="15">
@@ -4971,18 +5162,19 @@
       <c r="S45" s="15" t="s">
         <v>189</v>
       </c>
-      <c r="T45" s="21"/>
-      <c r="U45" s="21"/>
-      <c r="V45" s="21"/>
+      <c r="T45" s="19"/>
+      <c r="U45" s="19"/>
+      <c r="V45" s="19"/>
+      <c r="W45" s="22"/>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A46" s="20">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A46" s="18">
         <v>13020035</v>
       </c>
-      <c r="B46" s="19" t="s">
+      <c r="B46" s="17" t="s">
         <v>185</v>
       </c>
-      <c r="C46" s="20">
+      <c r="C46" s="18">
         <v>3</v>
       </c>
       <c r="D46" s="15">
@@ -5011,24 +5203,25 @@
       <c r="S46" s="15" t="s">
         <v>190</v>
       </c>
-      <c r="T46" s="21"/>
-      <c r="U46" s="21"/>
-      <c r="V46" s="21"/>
+      <c r="T46" s="19"/>
+      <c r="U46" s="19"/>
+      <c r="V46" s="19"/>
+      <c r="W46" s="22"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="I4:P46">
-    <cfRule type="cellIs" dxfId="27" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4">
-    <cfRule type="cellIs" dxfId="26" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4:H46">
-    <cfRule type="containsBlanks" dxfId="25" priority="5">
+    <cfRule type="containsBlanks" dxfId="1" priority="5">
       <formula>LEN(TRIM(F4))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
add a Sector des for scene
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Scene.xlsx
+++ b/ConfigData/Xlsx/Scene.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="258">
   <si>
     <t>村外小屋</t>
   </si>
@@ -943,6 +943,34 @@
   </si>
   <si>
     <t>LightBlue</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>所属</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>沙地</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>湾区</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>谷地</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sector</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>湖区</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1813,7 +1841,7 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="29">
+  <dxfs count="30">
     <dxf>
       <font>
         <b val="0"/>
@@ -1840,27 +1868,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -2393,6 +2400,41 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -2516,6 +2558,27 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2530,34 +2593,35 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:W46" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27" tableBorderDxfId="26">
-  <autoFilter ref="A3:W46"/>
-  <sortState ref="A4:W46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:X46" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25" tableBorderDxfId="24">
+  <autoFilter ref="A3:X46"/>
+  <sortState ref="A4:X46">
     <sortCondition ref="A3:A46"/>
   </sortState>
-  <tableColumns count="23">
-    <tableColumn id="1" name="Id" dataDxfId="25"/>
-    <tableColumn id="2" name="Name" dataDxfId="24"/>
-    <tableColumn id="18" name="Type" dataDxfId="23"/>
-    <tableColumn id="3" name="Level" dataDxfId="22"/>
-    <tableColumn id="20" name="ReviveScene" dataDxfId="21"/>
-    <tableColumn id="4" name="Quest" dataDxfId="20"/>
-    <tableColumn id="17" name="QuestRandom" dataDxfId="19"/>
-    <tableColumn id="19" name="QuestDungeon" dataDxfId="18"/>
-    <tableColumn id="5" name="QPortal" dataDxfId="17"/>
-    <tableColumn id="6" name="QCardChange" dataDxfId="16"/>
-    <tableColumn id="7" name="QPiece" dataDxfId="15"/>
-    <tableColumn id="8" name="QMerchant" dataDxfId="14"/>
-    <tableColumn id="9" name="QDoctor" dataDxfId="13"/>
-    <tableColumn id="10" name="QAngel" dataDxfId="12"/>
-    <tableColumn id="21" name="QWheel" dataDxfId="11"/>
-    <tableColumn id="22" name="QRes" dataDxfId="10"/>
-    <tableColumn id="11" name="Func" dataDxfId="9"/>
-    <tableColumn id="12" name="Url" dataDxfId="8"/>
-    <tableColumn id="13" name="TilePath" dataDxfId="7"/>
-    <tableColumn id="14" name="Icon" dataDxfId="6"/>
-    <tableColumn id="15" name="IconX" dataDxfId="5"/>
-    <tableColumn id="16" name="IconY" dataDxfId="4"/>
+  <tableColumns count="24">
+    <tableColumn id="1" name="Id" dataDxfId="23"/>
+    <tableColumn id="2" name="Name" dataDxfId="22"/>
+    <tableColumn id="18" name="Type" dataDxfId="21"/>
+    <tableColumn id="25" name="Sector" dataDxfId="20"/>
+    <tableColumn id="3" name="Level" dataDxfId="19"/>
+    <tableColumn id="20" name="ReviveScene" dataDxfId="18"/>
+    <tableColumn id="4" name="Quest" dataDxfId="17"/>
+    <tableColumn id="17" name="QuestRandom" dataDxfId="16"/>
+    <tableColumn id="19" name="QuestDungeon" dataDxfId="15"/>
+    <tableColumn id="5" name="QPortal" dataDxfId="14"/>
+    <tableColumn id="6" name="QCardChange" dataDxfId="13"/>
+    <tableColumn id="7" name="QPiece" dataDxfId="12"/>
+    <tableColumn id="8" name="QMerchant" dataDxfId="11"/>
+    <tableColumn id="9" name="QDoctor" dataDxfId="10"/>
+    <tableColumn id="10" name="QAngel" dataDxfId="9"/>
+    <tableColumn id="21" name="QWheel" dataDxfId="8"/>
+    <tableColumn id="22" name="QRes" dataDxfId="7"/>
+    <tableColumn id="11" name="Func" dataDxfId="6"/>
+    <tableColumn id="12" name="Url" dataDxfId="5"/>
+    <tableColumn id="13" name="TilePath" dataDxfId="4"/>
+    <tableColumn id="14" name="Icon" dataDxfId="3"/>
+    <tableColumn id="15" name="IconX" dataDxfId="2"/>
+    <tableColumn id="16" name="IconY" dataDxfId="1"/>
     <tableColumn id="24" name="IconColor" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2885,10 +2949,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W46"/>
+  <dimension ref="A1:X46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2896,21 +2960,22 @@
     <col min="1" max="1" width="11.125" style="5" customWidth="1"/>
     <col min="2" max="2" width="10.625" style="5" customWidth="1"/>
     <col min="3" max="3" width="5.125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="4.375" style="5" customWidth="1"/>
-    <col min="5" max="5" width="9" style="5" customWidth="1"/>
-    <col min="6" max="6" width="52.875" style="5" customWidth="1"/>
-    <col min="7" max="7" width="23.625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="43.5" style="5" customWidth="1"/>
-    <col min="9" max="16" width="3.125" style="5" customWidth="1"/>
-    <col min="17" max="17" width="6.625" style="5" customWidth="1"/>
-    <col min="18" max="18" width="9.75" style="5" customWidth="1"/>
-    <col min="19" max="19" width="9.5" style="5" customWidth="1"/>
-    <col min="20" max="20" width="7.25" style="5" customWidth="1"/>
-    <col min="21" max="23" width="6" style="5" customWidth="1"/>
-    <col min="24" max="16384" width="9" style="5"/>
+    <col min="4" max="4" width="5.375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="4.375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="9" style="5" customWidth="1"/>
+    <col min="7" max="7" width="52.875" style="5" customWidth="1"/>
+    <col min="8" max="8" width="23.625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="43.5" style="5" customWidth="1"/>
+    <col min="10" max="17" width="3.125" style="5" customWidth="1"/>
+    <col min="18" max="18" width="6.625" style="5" customWidth="1"/>
+    <col min="19" max="19" width="9.75" style="5" customWidth="1"/>
+    <col min="20" max="20" width="9.5" style="5" customWidth="1"/>
+    <col min="21" max="21" width="7.25" style="5" customWidth="1"/>
+    <col min="22" max="24" width="6" style="5" customWidth="1"/>
+    <col min="25" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="60" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:24" ht="60" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -2921,67 +2986,70 @@
         <v>91</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
         <v>13</v>
       </c>
@@ -2992,22 +3060,22 @@
         <v>92</v>
       </c>
       <c r="D2" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="F2" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="I2" s="7" t="s">
         <v>85</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>48</v>
       </c>
       <c r="J2" s="8" t="s">
         <v>48</v>
@@ -3025,34 +3093,37 @@
         <v>48</v>
       </c>
       <c r="O2" s="8" t="s">
-        <v>208</v>
+        <v>48</v>
       </c>
       <c r="P2" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="Q2" s="7" t="s">
+      <c r="Q2" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="R2" s="7" t="s">
         <v>14</v>
-      </c>
-      <c r="R2" s="7" t="s">
-        <v>26</v>
       </c>
       <c r="S2" s="7" t="s">
         <v>26</v>
       </c>
       <c r="T2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="U2" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="U2" s="7" t="s">
+      <c r="V2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="V2" s="9" t="s">
+      <c r="W2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="W2" s="9" t="s">
+      <c r="X2" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A3" s="10" t="s">
         <v>20</v>
       </c>
@@ -3062,68 +3133,71 @@
       <c r="C3" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="23" t="s">
+        <v>256</v>
+      </c>
+      <c r="E3" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="F3" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="G3" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="H3" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="I3" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="J3" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="K3" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="L3" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="L3" s="11" t="s">
+      <c r="M3" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="M3" s="11" t="s">
+      <c r="N3" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="N3" s="11" t="s">
+      <c r="O3" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="O3" s="11" t="s">
+      <c r="P3" s="11" t="s">
         <v>209</v>
       </c>
-      <c r="P3" s="11" t="s">
+      <c r="Q3" s="11" t="s">
         <v>210</v>
       </c>
-      <c r="Q3" s="10" t="s">
+      <c r="R3" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="R3" s="10" t="s">
+      <c r="S3" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="S3" s="10" t="s">
+      <c r="T3" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="T3" s="10" t="s">
+      <c r="U3" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="U3" s="10" t="s">
+      <c r="V3" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="V3" s="10" t="s">
+      <c r="W3" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="W3" s="23" t="s">
+      <c r="X3" s="23" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A4" s="12">
         <v>13010001</v>
       </c>
@@ -3133,23 +3207,25 @@
       <c r="C4" s="13">
         <v>2</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="20" t="s">
+        <v>255</v>
+      </c>
+      <c r="E4" s="13">
         <v>1</v>
       </c>
-      <c r="E4" s="13">
+      <c r="F4" s="13">
         <v>13010001</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="G4" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="H4" s="14" t="s">
         <v>199</v>
       </c>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13">
+      <c r="I4" s="13"/>
+      <c r="J4" s="13">
         <v>1</v>
       </c>
-      <c r="J4" s="13"/>
       <c r="K4" s="13"/>
       <c r="L4" s="13"/>
       <c r="M4" s="13"/>
@@ -3157,26 +3233,27 @@
       <c r="O4" s="13"/>
       <c r="P4" s="13"/>
       <c r="Q4" s="13"/>
-      <c r="R4" s="13" t="s">
+      <c r="R4" s="13"/>
+      <c r="S4" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="S4" s="13" t="s">
+      <c r="T4" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="T4" s="13" t="s">
+      <c r="U4" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="U4" s="13">
+      <c r="V4" s="13">
         <v>1348</v>
       </c>
-      <c r="V4" s="13">
+      <c r="W4" s="13">
         <v>611</v>
       </c>
-      <c r="W4" s="24" t="s">
+      <c r="X4" s="24" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A5" s="12">
         <v>13010002</v>
       </c>
@@ -3186,54 +3263,57 @@
       <c r="C5" s="13">
         <v>2</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="20" t="s">
+        <v>255</v>
+      </c>
+      <c r="E5" s="13">
         <v>2</v>
       </c>
-      <c r="E5" s="13">
+      <c r="F5" s="13">
         <v>13010001</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="G5" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="H5" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13">
+      <c r="I5" s="13"/>
+      <c r="J5" s="13">
         <v>1</v>
       </c>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13">
+      <c r="K5" s="13"/>
+      <c r="L5" s="13">
         <v>1</v>
       </c>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13">
+      <c r="M5" s="13"/>
+      <c r="N5" s="13">
         <v>1</v>
       </c>
-      <c r="N5" s="13"/>
       <c r="O5" s="13"/>
       <c r="P5" s="13"/>
       <c r="Q5" s="13"/>
-      <c r="R5" s="13" t="s">
-        <v>31</v>
-      </c>
+      <c r="R5" s="13"/>
       <c r="S5" s="13" t="s">
         <v>31</v>
       </c>
       <c r="T5" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="U5" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="U5" s="13">
+      <c r="V5" s="13">
         <v>1279</v>
       </c>
-      <c r="V5" s="13">
+      <c r="W5" s="13">
         <v>571</v>
       </c>
-      <c r="W5" s="24" t="s">
+      <c r="X5" s="24" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A6" s="12">
         <v>13010003</v>
       </c>
@@ -3243,23 +3323,25 @@
       <c r="C6" s="13">
         <v>2</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="20" t="s">
+        <v>255</v>
+      </c>
+      <c r="E6" s="13">
         <v>3</v>
       </c>
-      <c r="E6" s="13">
+      <c r="F6" s="13">
         <v>13010006</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="G6" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="H6" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13">
+      <c r="I6" s="13"/>
+      <c r="J6" s="13">
         <v>1</v>
       </c>
-      <c r="J6" s="13"/>
       <c r="K6" s="13"/>
       <c r="L6" s="13"/>
       <c r="M6" s="13"/>
@@ -3267,26 +3349,27 @@
       <c r="O6" s="13"/>
       <c r="P6" s="13"/>
       <c r="Q6" s="13"/>
-      <c r="R6" s="13" t="s">
+      <c r="R6" s="13"/>
+      <c r="S6" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="S6" s="13" t="s">
+      <c r="T6" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="T6" s="13" t="s">
+      <c r="U6" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="U6" s="13">
+      <c r="V6" s="13">
         <v>1251</v>
       </c>
-      <c r="V6" s="13">
+      <c r="W6" s="13">
         <v>432</v>
       </c>
-      <c r="W6" s="24" t="s">
+      <c r="X6" s="24" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A7" s="12">
         <v>13010004</v>
       </c>
@@ -3296,52 +3379,55 @@
       <c r="C7" s="13">
         <v>2</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="20" t="s">
+        <v>255</v>
+      </c>
+      <c r="E7" s="13">
         <v>5</v>
       </c>
-      <c r="E7" s="13">
+      <c r="F7" s="13">
         <v>13010006</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="G7" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="H7" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13">
+      <c r="I7" s="13"/>
+      <c r="J7" s="13">
         <v>1</v>
       </c>
-      <c r="J7" s="13"/>
       <c r="K7" s="13"/>
-      <c r="L7" s="13">
+      <c r="L7" s="13"/>
+      <c r="M7" s="13">
         <v>1</v>
       </c>
-      <c r="M7" s="13"/>
       <c r="N7" s="13"/>
       <c r="O7" s="13"/>
       <c r="P7" s="13"/>
       <c r="Q7" s="13"/>
-      <c r="R7" s="13" t="s">
-        <v>35</v>
-      </c>
+      <c r="R7" s="13"/>
       <c r="S7" s="13" t="s">
         <v>35</v>
       </c>
       <c r="T7" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="U7" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="U7" s="13">
+      <c r="V7" s="13">
         <v>1148</v>
       </c>
-      <c r="V7" s="13">
+      <c r="W7" s="13">
         <v>351</v>
       </c>
-      <c r="W7" s="24" t="s">
+      <c r="X7" s="24" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A8" s="12">
         <v>13010005</v>
       </c>
@@ -3351,52 +3437,55 @@
       <c r="C8" s="13">
         <v>2</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="20" t="s">
+        <v>255</v>
+      </c>
+      <c r="E8" s="13">
         <v>8</v>
       </c>
-      <c r="E8" s="13">
+      <c r="F8" s="13">
         <v>13010006</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="G8" s="13" t="s">
         <v>172</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="H8" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13">
-        <v>1</v>
-      </c>
+      <c r="I8" s="13"/>
       <c r="J8" s="13">
         <v>1</v>
       </c>
-      <c r="K8" s="13"/>
+      <c r="K8" s="13">
+        <v>1</v>
+      </c>
       <c r="L8" s="13"/>
       <c r="M8" s="13"/>
       <c r="N8" s="13"/>
       <c r="O8" s="13"/>
       <c r="P8" s="13"/>
       <c r="Q8" s="13"/>
-      <c r="R8" s="13" t="s">
+      <c r="R8" s="13"/>
+      <c r="S8" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="S8" s="13" t="s">
+      <c r="T8" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="T8" s="13" t="s">
+      <c r="U8" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="U8" s="13">
+      <c r="V8" s="13">
         <v>1386</v>
       </c>
-      <c r="V8" s="13">
+      <c r="W8" s="13">
         <v>339</v>
       </c>
-      <c r="W8" s="24" t="s">
+      <c r="X8" s="24" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A9" s="12">
         <v>13010006</v>
       </c>
@@ -3406,13 +3495,15 @@
       <c r="C9" s="13">
         <v>1</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="20" t="s">
+        <v>255</v>
+      </c>
+      <c r="E9" s="13">
         <v>3</v>
       </c>
-      <c r="E9" s="13">
+      <c r="F9" s="13">
         <v>13010006</v>
       </c>
-      <c r="F9" s="13"/>
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
       <c r="I9" s="13"/>
@@ -3424,26 +3515,27 @@
       <c r="O9" s="13"/>
       <c r="P9" s="13"/>
       <c r="Q9" s="13"/>
-      <c r="R9" s="13" t="s">
+      <c r="R9" s="13"/>
+      <c r="S9" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="S9" s="13" t="s">
+      <c r="T9" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="T9" s="13" t="s">
+      <c r="U9" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="U9" s="13">
+      <c r="V9" s="13">
         <v>1232</v>
       </c>
-      <c r="V9" s="13">
+      <c r="W9" s="13">
         <v>506</v>
       </c>
-      <c r="W9" s="24" t="s">
+      <c r="X9" s="24" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A10" s="12">
         <v>13010007</v>
       </c>
@@ -3453,54 +3545,57 @@
       <c r="C10" s="13">
         <v>2</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="20" t="s">
+        <v>255</v>
+      </c>
+      <c r="E10" s="13">
         <v>7</v>
       </c>
-      <c r="E10" s="13">
+      <c r="F10" s="13">
         <v>13010006</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="G10" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="G10" s="13" t="s">
+      <c r="H10" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13">
+      <c r="I10" s="13"/>
+      <c r="J10" s="13">
         <v>1</v>
       </c>
-      <c r="J10" s="13"/>
       <c r="K10" s="13"/>
       <c r="L10" s="13"/>
-      <c r="M10" s="13">
+      <c r="M10" s="13"/>
+      <c r="N10" s="13">
         <v>1</v>
       </c>
-      <c r="N10" s="13"/>
       <c r="O10" s="13"/>
-      <c r="P10" s="13">
+      <c r="P10" s="13"/>
+      <c r="Q10" s="13">
         <v>1</v>
       </c>
-      <c r="Q10" s="13"/>
-      <c r="R10" s="13" t="s">
+      <c r="R10" s="13"/>
+      <c r="S10" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="S10" s="13" t="s">
+      <c r="T10" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="T10" s="13" t="s">
+      <c r="U10" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="U10" s="13">
+      <c r="V10" s="13">
         <v>1431</v>
       </c>
-      <c r="V10" s="13">
+      <c r="W10" s="13">
         <v>440</v>
       </c>
-      <c r="W10" s="24" t="s">
+      <c r="X10" s="24" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A11" s="12">
         <v>13010008</v>
       </c>
@@ -3510,52 +3605,55 @@
       <c r="C11" s="13">
         <v>2</v>
       </c>
-      <c r="D11" s="13">
+      <c r="D11" s="20" t="s">
+        <v>255</v>
+      </c>
+      <c r="E11" s="13">
         <v>6</v>
       </c>
-      <c r="E11" s="13">
+      <c r="F11" s="13">
         <v>13010006</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="G11" s="13" t="s">
         <v>159</v>
       </c>
-      <c r="G11" s="13" t="s">
+      <c r="H11" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13">
+      <c r="I11" s="13"/>
+      <c r="J11" s="13">
         <v>1</v>
       </c>
-      <c r="J11" s="13"/>
       <c r="K11" s="13"/>
       <c r="L11" s="13"/>
       <c r="M11" s="13"/>
       <c r="N11" s="13"/>
-      <c r="O11" s="13">
+      <c r="O11" s="13"/>
+      <c r="P11" s="13">
         <v>1</v>
       </c>
-      <c r="P11" s="13"/>
       <c r="Q11" s="13"/>
-      <c r="R11" s="13" t="s">
+      <c r="R11" s="13"/>
+      <c r="S11" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="S11" s="13" t="s">
+      <c r="T11" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="T11" s="13" t="s">
+      <c r="U11" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="U11" s="13">
+      <c r="V11" s="13">
         <v>1250</v>
       </c>
-      <c r="V11" s="13">
+      <c r="W11" s="13">
         <v>338</v>
       </c>
-      <c r="W11" s="24" t="s">
+      <c r="X11" s="24" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A12" s="12">
         <v>13010009</v>
       </c>
@@ -3565,54 +3663,57 @@
       <c r="C12" s="13">
         <v>2</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="20" t="s">
+        <v>255</v>
+      </c>
+      <c r="E12" s="13">
         <v>4</v>
       </c>
-      <c r="E12" s="13">
+      <c r="F12" s="13">
         <v>13010006</v>
       </c>
-      <c r="F12" s="13" t="s">
+      <c r="G12" s="13" t="s">
         <v>169</v>
       </c>
-      <c r="G12" s="13" t="s">
+      <c r="H12" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13">
-        <v>1</v>
-      </c>
+      <c r="I12" s="13"/>
       <c r="J12" s="13">
         <v>1</v>
       </c>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13">
+      <c r="K12" s="13">
         <v>1</v>
       </c>
-      <c r="M12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13">
+        <v>1</v>
+      </c>
       <c r="N12" s="13"/>
       <c r="O12" s="13"/>
       <c r="P12" s="13"/>
       <c r="Q12" s="13"/>
-      <c r="R12" s="13" t="s">
+      <c r="R12" s="13"/>
+      <c r="S12" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="S12" s="13" t="s">
+      <c r="T12" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="T12" s="13" t="s">
+      <c r="U12" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="U12" s="13">
+      <c r="V12" s="13">
         <v>1332</v>
       </c>
-      <c r="V12" s="13">
+      <c r="W12" s="13">
         <v>484</v>
       </c>
-      <c r="W12" s="24" t="s">
+      <c r="X12" s="24" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A13" s="12">
         <v>13010010</v>
       </c>
@@ -3622,23 +3723,25 @@
       <c r="C13" s="15">
         <v>2</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="20" t="s">
+        <v>255</v>
+      </c>
+      <c r="E13" s="15">
         <v>6</v>
       </c>
-      <c r="E13" s="13">
+      <c r="F13" s="13">
         <v>13010006</v>
       </c>
-      <c r="F13" s="13" t="s">
+      <c r="G13" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="G13" s="13" t="s">
+      <c r="H13" s="13" t="s">
         <v>168</v>
       </c>
-      <c r="H13" s="13"/>
-      <c r="I13" s="15">
+      <c r="I13" s="13"/>
+      <c r="J13" s="15">
         <v>1</v>
       </c>
-      <c r="J13" s="15"/>
       <c r="K13" s="15"/>
       <c r="L13" s="15"/>
       <c r="M13" s="15"/>
@@ -3646,20 +3749,21 @@
       <c r="O13" s="15"/>
       <c r="P13" s="15"/>
       <c r="Q13" s="15"/>
-      <c r="R13" s="15" t="s">
-        <v>129</v>
-      </c>
+      <c r="R13" s="15"/>
       <c r="S13" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="T13" s="15"/>
+      <c r="T13" s="15" t="s">
+        <v>129</v>
+      </c>
       <c r="U13" s="15"/>
       <c r="V13" s="15"/>
-      <c r="W13" s="24" t="s">
+      <c r="W13" s="15"/>
+      <c r="X13" s="24" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A14" s="27">
         <v>13010101</v>
       </c>
@@ -3669,13 +3773,15 @@
       <c r="C14" s="13">
         <v>1</v>
       </c>
-      <c r="D14" s="13">
+      <c r="D14" s="20" t="s">
+        <v>257</v>
+      </c>
+      <c r="E14" s="13">
         <v>16</v>
       </c>
-      <c r="E14" s="13">
+      <c r="F14" s="13">
         <v>13010101</v>
       </c>
-      <c r="F14" s="13"/>
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
       <c r="I14" s="13"/>
@@ -3687,26 +3793,27 @@
       <c r="O14" s="13"/>
       <c r="P14" s="13"/>
       <c r="Q14" s="13"/>
-      <c r="R14" s="13" t="s">
+      <c r="R14" s="13"/>
+      <c r="S14" s="13" t="s">
         <v>211</v>
       </c>
-      <c r="S14" s="13" t="s">
+      <c r="T14" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="T14" s="13" t="s">
+      <c r="U14" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="U14" s="13">
+      <c r="V14" s="13">
         <v>894</v>
       </c>
-      <c r="V14" s="13">
+      <c r="W14" s="13">
         <v>509</v>
       </c>
-      <c r="W14" s="24" t="s">
+      <c r="X14" s="24" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A15" s="27">
         <v>13010102</v>
       </c>
@@ -3716,52 +3823,55 @@
       <c r="C15" s="13">
         <v>2</v>
       </c>
-      <c r="D15" s="13">
+      <c r="D15" s="20" t="s">
+        <v>257</v>
+      </c>
+      <c r="E15" s="13">
         <v>16</v>
       </c>
-      <c r="E15" s="13">
+      <c r="F15" s="13">
         <v>13010101</v>
       </c>
-      <c r="F15" s="13" t="s">
+      <c r="G15" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="G15" s="13" t="s">
+      <c r="H15" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13">
+      <c r="I15" s="13"/>
+      <c r="J15" s="13">
         <v>1</v>
       </c>
-      <c r="J15" s="13"/>
       <c r="K15" s="13"/>
-      <c r="L15" s="13">
+      <c r="L15" s="13"/>
+      <c r="M15" s="13">
         <v>1</v>
       </c>
-      <c r="M15" s="13"/>
       <c r="N15" s="13"/>
       <c r="O15" s="13"/>
       <c r="P15" s="13"/>
       <c r="Q15" s="13"/>
-      <c r="R15" s="13" t="s">
+      <c r="R15" s="13"/>
+      <c r="S15" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="S15" s="13" t="s">
+      <c r="T15" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="T15" s="13" t="s">
+      <c r="U15" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="U15" s="13">
+      <c r="V15" s="13">
         <v>1040</v>
       </c>
-      <c r="V15" s="13">
+      <c r="W15" s="13">
         <v>538</v>
       </c>
-      <c r="W15" s="24" t="s">
+      <c r="X15" s="24" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A16" s="27">
         <v>13010103</v>
       </c>
@@ -3771,23 +3881,25 @@
       <c r="C16" s="13">
         <v>2</v>
       </c>
-      <c r="D16" s="13">
+      <c r="D16" s="20" t="s">
+        <v>257</v>
+      </c>
+      <c r="E16" s="13">
         <v>19</v>
       </c>
-      <c r="E16" s="13">
+      <c r="F16" s="13">
         <v>13010101</v>
       </c>
-      <c r="F16" s="13" t="s">
+      <c r="G16" s="13" t="s">
         <v>170</v>
       </c>
-      <c r="G16" s="13" t="s">
+      <c r="H16" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13">
+      <c r="I16" s="13"/>
+      <c r="J16" s="13">
         <v>1</v>
       </c>
-      <c r="J16" s="13"/>
       <c r="K16" s="13"/>
       <c r="L16" s="13"/>
       <c r="M16" s="13"/>
@@ -3795,26 +3907,27 @@
       <c r="O16" s="13"/>
       <c r="P16" s="13"/>
       <c r="Q16" s="13"/>
-      <c r="R16" s="13" t="s">
-        <v>99</v>
-      </c>
+      <c r="R16" s="13"/>
       <c r="S16" s="13" t="s">
         <v>99</v>
       </c>
       <c r="T16" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="U16" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="U16" s="13">
+      <c r="V16" s="13">
         <v>1213</v>
       </c>
-      <c r="V16" s="13">
+      <c r="W16" s="13">
         <v>655</v>
       </c>
-      <c r="W16" s="24" t="s">
+      <c r="X16" s="24" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A17" s="27">
         <v>13010104</v>
       </c>
@@ -3824,52 +3937,55 @@
       <c r="C17" s="13">
         <v>2</v>
       </c>
-      <c r="D17" s="13">
+      <c r="D17" s="20" t="s">
+        <v>257</v>
+      </c>
+      <c r="E17" s="13">
         <v>18</v>
       </c>
-      <c r="E17" s="13">
+      <c r="F17" s="13">
         <v>13010101</v>
       </c>
-      <c r="F17" s="13" t="s">
+      <c r="G17" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="G17" s="13" t="s">
+      <c r="H17" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13">
+      <c r="I17" s="13"/>
+      <c r="J17" s="13">
         <v>1</v>
       </c>
-      <c r="J17" s="13"/>
       <c r="K17" s="13"/>
       <c r="L17" s="13"/>
-      <c r="M17" s="13">
+      <c r="M17" s="13"/>
+      <c r="N17" s="13">
         <v>1</v>
       </c>
-      <c r="N17" s="13"/>
       <c r="O17" s="13"/>
       <c r="P17" s="13"/>
       <c r="Q17" s="13"/>
-      <c r="R17" s="13" t="s">
+      <c r="R17" s="13"/>
+      <c r="S17" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="S17" s="13" t="s">
+      <c r="T17" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="T17" s="13" t="s">
+      <c r="U17" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="U17" s="13">
+      <c r="V17" s="13">
         <v>1149</v>
       </c>
-      <c r="V17" s="13">
+      <c r="W17" s="13">
         <v>584</v>
       </c>
-      <c r="W17" s="24" t="s">
+      <c r="X17" s="24" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A18" s="27">
         <v>13010105</v>
       </c>
@@ -3879,19 +3995,21 @@
       <c r="C18" s="13">
         <v>2</v>
       </c>
-      <c r="D18" s="13">
+      <c r="D18" s="20" t="s">
+        <v>257</v>
+      </c>
+      <c r="E18" s="13">
         <v>20</v>
       </c>
-      <c r="E18" s="13">
+      <c r="F18" s="13">
         <v>13010101</v>
       </c>
-      <c r="F18" s="13" t="s">
+      <c r="G18" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="G18" s="13" t="s">
+      <c r="H18" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="H18" s="13"/>
       <c r="I18" s="13"/>
       <c r="J18" s="13"/>
       <c r="K18" s="13"/>
@@ -3901,26 +4019,27 @@
       <c r="O18" s="13"/>
       <c r="P18" s="13"/>
       <c r="Q18" s="13"/>
-      <c r="R18" s="13" t="s">
+      <c r="R18" s="13"/>
+      <c r="S18" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="S18" s="13" t="s">
+      <c r="T18" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="T18" s="13" t="s">
+      <c r="U18" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="U18" s="13">
+      <c r="V18" s="13">
         <v>840</v>
       </c>
-      <c r="V18" s="13">
+      <c r="W18" s="13">
         <v>444</v>
       </c>
-      <c r="W18" s="24" t="s">
+      <c r="X18" s="24" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A19" s="27">
         <v>13010106</v>
       </c>
@@ -3930,52 +4049,55 @@
       <c r="C19" s="13">
         <v>2</v>
       </c>
-      <c r="D19" s="13">
+      <c r="D19" s="20" t="s">
+        <v>257</v>
+      </c>
+      <c r="E19" s="13">
         <v>15</v>
       </c>
-      <c r="E19" s="13">
+      <c r="F19" s="13">
         <v>13010016</v>
       </c>
-      <c r="F19" s="13" t="s">
+      <c r="G19" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="G19" s="13" t="s">
+      <c r="H19" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13">
+      <c r="I19" s="13"/>
+      <c r="J19" s="13">
         <v>1</v>
       </c>
-      <c r="J19" s="13"/>
       <c r="K19" s="13"/>
       <c r="L19" s="13"/>
       <c r="M19" s="13"/>
-      <c r="N19" s="13">
+      <c r="N19" s="13"/>
+      <c r="O19" s="13">
         <v>1</v>
       </c>
-      <c r="O19" s="13"/>
       <c r="P19" s="13"/>
       <c r="Q19" s="13"/>
-      <c r="R19" s="13" t="s">
-        <v>103</v>
-      </c>
+      <c r="R19" s="13"/>
       <c r="S19" s="13" t="s">
         <v>103</v>
       </c>
       <c r="T19" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="U19" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="U19" s="13">
+      <c r="V19" s="13">
         <v>1067</v>
       </c>
-      <c r="V19" s="13">
+      <c r="W19" s="13">
         <v>445</v>
       </c>
-      <c r="W19" s="24" t="s">
+      <c r="X19" s="24" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A20" s="27">
         <v>13010107</v>
       </c>
@@ -3985,13 +4107,15 @@
       <c r="C20" s="15">
         <v>2</v>
       </c>
-      <c r="D20" s="15">
+      <c r="D20" s="20" t="s">
+        <v>257</v>
+      </c>
+      <c r="E20" s="15">
         <v>15</v>
       </c>
-      <c r="E20" s="15">
+      <c r="F20" s="15">
         <v>13010101</v>
       </c>
-      <c r="F20" s="16"/>
       <c r="G20" s="16"/>
       <c r="H20" s="16"/>
       <c r="I20" s="16"/>
@@ -4000,29 +4124,30 @@
       <c r="L20" s="16"/>
       <c r="M20" s="16"/>
       <c r="N20" s="16"/>
-      <c r="O20" s="15"/>
+      <c r="O20" s="16"/>
       <c r="P20" s="15"/>
-      <c r="Q20" s="16"/>
-      <c r="R20" s="13" t="s">
-        <v>236</v>
-      </c>
+      <c r="Q20" s="15"/>
+      <c r="R20" s="16"/>
       <c r="S20" s="13" t="s">
         <v>236</v>
       </c>
       <c r="T20" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="U20" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="U20" s="16">
+      <c r="V20" s="16">
         <v>850</v>
       </c>
-      <c r="V20" s="16">
+      <c r="W20" s="16">
         <v>589</v>
       </c>
-      <c r="W20" s="24" t="s">
+      <c r="X20" s="24" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A21" s="27">
         <v>13010108</v>
       </c>
@@ -4032,13 +4157,15 @@
       <c r="C21" s="15">
         <v>2</v>
       </c>
-      <c r="D21" s="15">
+      <c r="D21" s="20" t="s">
+        <v>257</v>
+      </c>
+      <c r="E21" s="15">
         <v>15</v>
       </c>
-      <c r="E21" s="15">
+      <c r="F21" s="15">
         <v>13010101</v>
       </c>
-      <c r="F21" s="16"/>
       <c r="G21" s="16"/>
       <c r="H21" s="16"/>
       <c r="I21" s="16"/>
@@ -4047,29 +4174,30 @@
       <c r="L21" s="16"/>
       <c r="M21" s="16"/>
       <c r="N21" s="16"/>
-      <c r="O21" s="15"/>
+      <c r="O21" s="16"/>
       <c r="P21" s="15"/>
-      <c r="Q21" s="16"/>
-      <c r="R21" s="13" t="s">
-        <v>238</v>
-      </c>
+      <c r="Q21" s="15"/>
+      <c r="R21" s="16"/>
       <c r="S21" s="13" t="s">
         <v>238</v>
       </c>
-      <c r="T21" s="16" t="s">
+      <c r="T21" s="13" t="s">
+        <v>238</v>
+      </c>
+      <c r="U21" s="16" t="s">
         <v>224</v>
       </c>
-      <c r="U21" s="13">
+      <c r="V21" s="13">
         <v>682</v>
       </c>
-      <c r="V21" s="13">
+      <c r="W21" s="13">
         <v>545</v>
       </c>
-      <c r="W21" s="24" t="s">
+      <c r="X21" s="24" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A22" s="25">
         <v>13010201</v>
       </c>
@@ -4079,13 +4207,15 @@
       <c r="C22" s="15">
         <v>2</v>
       </c>
-      <c r="D22" s="15">
+      <c r="D22" s="15" t="s">
+        <v>253</v>
+      </c>
+      <c r="E22" s="15">
         <v>15</v>
       </c>
-      <c r="E22" s="15">
+      <c r="F22" s="15">
         <v>13010201</v>
       </c>
-      <c r="F22" s="16"/>
       <c r="G22" s="16"/>
       <c r="H22" s="16"/>
       <c r="I22" s="16"/>
@@ -4094,29 +4224,30 @@
       <c r="L22" s="16"/>
       <c r="M22" s="16"/>
       <c r="N22" s="16"/>
-      <c r="O22" s="15"/>
+      <c r="O22" s="16"/>
       <c r="P22" s="15"/>
-      <c r="Q22" s="16"/>
-      <c r="R22" s="13" t="s">
-        <v>234</v>
-      </c>
+      <c r="Q22" s="15"/>
+      <c r="R22" s="16"/>
       <c r="S22" s="13" t="s">
         <v>234</v>
       </c>
-      <c r="T22" s="16" t="s">
+      <c r="T22" s="13" t="s">
+        <v>234</v>
+      </c>
+      <c r="U22" s="16" t="s">
         <v>221</v>
       </c>
-      <c r="U22" s="13">
+      <c r="V22" s="13">
         <v>807</v>
       </c>
-      <c r="V22" s="13">
+      <c r="W22" s="13">
         <v>720</v>
       </c>
-      <c r="W22" s="24" t="s">
+      <c r="X22" s="24" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A23" s="25">
         <v>13010202</v>
       </c>
@@ -4126,13 +4257,15 @@
       <c r="C23" s="15">
         <v>2</v>
       </c>
-      <c r="D23" s="15">
+      <c r="D23" s="15" t="s">
+        <v>253</v>
+      </c>
+      <c r="E23" s="15">
         <v>15</v>
       </c>
-      <c r="E23" s="15">
+      <c r="F23" s="15">
         <v>13010201</v>
       </c>
-      <c r="F23" s="15"/>
       <c r="G23" s="15"/>
       <c r="H23" s="15"/>
       <c r="I23" s="15"/>
@@ -4144,26 +4277,27 @@
       <c r="O23" s="15"/>
       <c r="P23" s="15"/>
       <c r="Q23" s="15"/>
-      <c r="R23" s="13" t="s">
-        <v>239</v>
-      </c>
+      <c r="R23" s="15"/>
       <c r="S23" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="T23" s="15" t="s">
+      <c r="T23" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="U23" s="15" t="s">
         <v>214</v>
       </c>
-      <c r="U23" s="15">
+      <c r="V23" s="15">
         <v>974</v>
       </c>
-      <c r="V23" s="15">
+      <c r="W23" s="15">
         <v>594</v>
       </c>
-      <c r="W23" s="24" t="s">
+      <c r="X23" s="24" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A24" s="25">
         <v>13010203</v>
       </c>
@@ -4173,13 +4307,15 @@
       <c r="C24" s="15">
         <v>2</v>
       </c>
-      <c r="D24" s="15">
+      <c r="D24" s="15" t="s">
+        <v>253</v>
+      </c>
+      <c r="E24" s="15">
         <v>15</v>
       </c>
-      <c r="E24" s="15">
+      <c r="F24" s="15">
         <v>13010201</v>
       </c>
-      <c r="F24" s="15"/>
       <c r="G24" s="15"/>
       <c r="H24" s="15"/>
       <c r="I24" s="15"/>
@@ -4191,26 +4327,27 @@
       <c r="O24" s="15"/>
       <c r="P24" s="15"/>
       <c r="Q24" s="15"/>
-      <c r="R24" s="13" t="s">
-        <v>240</v>
-      </c>
+      <c r="R24" s="15"/>
       <c r="S24" s="13" t="s">
         <v>240</v>
       </c>
-      <c r="T24" s="15" t="s">
+      <c r="T24" s="13" t="s">
+        <v>240</v>
+      </c>
+      <c r="U24" s="15" t="s">
         <v>215</v>
       </c>
-      <c r="U24" s="15">
+      <c r="V24" s="15">
         <v>1080</v>
       </c>
-      <c r="V24" s="15">
+      <c r="W24" s="15">
         <v>720</v>
       </c>
-      <c r="W24" s="24" t="s">
+      <c r="X24" s="24" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A25" s="25">
         <v>13010204</v>
       </c>
@@ -4220,13 +4357,15 @@
       <c r="C25" s="15">
         <v>2</v>
       </c>
-      <c r="D25" s="15">
+      <c r="D25" s="15" t="s">
+        <v>253</v>
+      </c>
+      <c r="E25" s="15">
         <v>15</v>
       </c>
-      <c r="E25" s="15">
+      <c r="F25" s="15">
         <v>13010201</v>
       </c>
-      <c r="F25" s="15"/>
       <c r="G25" s="15"/>
       <c r="H25" s="15"/>
       <c r="I25" s="15"/>
@@ -4238,26 +4377,27 @@
       <c r="O25" s="15"/>
       <c r="P25" s="15"/>
       <c r="Q25" s="15"/>
-      <c r="R25" s="13" t="s">
-        <v>241</v>
-      </c>
+      <c r="R25" s="15"/>
       <c r="S25" s="13" t="s">
         <v>241</v>
       </c>
-      <c r="T25" s="15" t="s">
+      <c r="T25" s="13" t="s">
+        <v>241</v>
+      </c>
+      <c r="U25" s="15" t="s">
         <v>217</v>
       </c>
-      <c r="U25" s="15">
+      <c r="V25" s="15">
         <v>1074</v>
       </c>
-      <c r="V25" s="15">
+      <c r="W25" s="15">
         <v>630</v>
       </c>
-      <c r="W25" s="24" t="s">
+      <c r="X25" s="24" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A26" s="25">
         <v>13010205</v>
       </c>
@@ -4267,13 +4407,15 @@
       <c r="C26" s="15">
         <v>2</v>
       </c>
-      <c r="D26" s="15">
+      <c r="D26" s="15" t="s">
+        <v>253</v>
+      </c>
+      <c r="E26" s="15">
         <v>15</v>
       </c>
-      <c r="E26" s="15">
+      <c r="F26" s="15">
         <v>13010201</v>
       </c>
-      <c r="F26" s="16"/>
       <c r="G26" s="16"/>
       <c r="H26" s="16"/>
       <c r="I26" s="16"/>
@@ -4282,29 +4424,30 @@
       <c r="L26" s="16"/>
       <c r="M26" s="16"/>
       <c r="N26" s="16"/>
-      <c r="O26" s="15"/>
+      <c r="O26" s="16"/>
       <c r="P26" s="15"/>
-      <c r="Q26" s="16"/>
-      <c r="R26" s="20" t="s">
-        <v>237</v>
-      </c>
+      <c r="Q26" s="15"/>
+      <c r="R26" s="16"/>
       <c r="S26" s="20" t="s">
         <v>237</v>
       </c>
-      <c r="T26" s="16" t="s">
+      <c r="T26" s="20" t="s">
+        <v>237</v>
+      </c>
+      <c r="U26" s="16" t="s">
         <v>222</v>
       </c>
-      <c r="U26" s="13">
+      <c r="V26" s="13">
         <v>717</v>
       </c>
-      <c r="V26" s="13">
+      <c r="W26" s="13">
         <v>655</v>
       </c>
-      <c r="W26" s="24" t="s">
+      <c r="X26" s="24" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A27" s="25">
         <v>13010206</v>
       </c>
@@ -4314,13 +4457,15 @@
       <c r="C27" s="15">
         <v>2</v>
       </c>
-      <c r="D27" s="15">
+      <c r="D27" s="15" t="s">
+        <v>253</v>
+      </c>
+      <c r="E27" s="15">
         <v>15</v>
       </c>
-      <c r="E27" s="15">
+      <c r="F27" s="15">
         <v>13010201</v>
       </c>
-      <c r="F27" s="16"/>
       <c r="G27" s="16"/>
       <c r="H27" s="16"/>
       <c r="I27" s="16"/>
@@ -4329,29 +4474,30 @@
       <c r="L27" s="16"/>
       <c r="M27" s="16"/>
       <c r="N27" s="16"/>
-      <c r="O27" s="15"/>
+      <c r="O27" s="16"/>
       <c r="P27" s="15"/>
-      <c r="Q27" s="16"/>
-      <c r="R27" s="20" t="s">
-        <v>243</v>
-      </c>
+      <c r="Q27" s="15"/>
+      <c r="R27" s="16"/>
       <c r="S27" s="20" t="s">
         <v>243</v>
       </c>
-      <c r="T27" s="16" t="s">
+      <c r="T27" s="20" t="s">
+        <v>243</v>
+      </c>
+      <c r="U27" s="16" t="s">
         <v>223</v>
       </c>
-      <c r="U27" s="13">
+      <c r="V27" s="13">
         <v>637</v>
       </c>
-      <c r="V27" s="13">
+      <c r="W27" s="13">
         <v>735</v>
       </c>
-      <c r="W27" s="24" t="s">
+      <c r="X27" s="24" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A28" s="25">
         <v>13010207</v>
       </c>
@@ -4361,13 +4507,15 @@
       <c r="C28" s="15">
         <v>2</v>
       </c>
-      <c r="D28" s="15">
+      <c r="D28" s="15" t="s">
+        <v>253</v>
+      </c>
+      <c r="E28" s="15">
         <v>15</v>
       </c>
-      <c r="E28" s="15">
+      <c r="F28" s="15">
         <v>13010201</v>
       </c>
-      <c r="F28" s="15"/>
       <c r="G28" s="15"/>
       <c r="H28" s="15"/>
       <c r="I28" s="15"/>
@@ -4379,26 +4527,27 @@
       <c r="O28" s="15"/>
       <c r="P28" s="15"/>
       <c r="Q28" s="15"/>
-      <c r="R28" s="13" t="s">
-        <v>242</v>
-      </c>
+      <c r="R28" s="15"/>
       <c r="S28" s="13" t="s">
         <v>242</v>
       </c>
       <c r="T28" s="13" t="s">
+        <v>242</v>
+      </c>
+      <c r="U28" s="13" t="s">
         <v>225</v>
       </c>
-      <c r="U28" s="13">
+      <c r="V28" s="13">
         <v>737</v>
       </c>
-      <c r="V28" s="13">
+      <c r="W28" s="13">
         <v>785</v>
       </c>
-      <c r="W28" s="24" t="s">
+      <c r="X28" s="24" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A29" s="25">
         <v>13010208</v>
       </c>
@@ -4408,13 +4557,15 @@
       <c r="C29" s="15">
         <v>2</v>
       </c>
-      <c r="D29" s="15">
+      <c r="D29" s="15" t="s">
+        <v>253</v>
+      </c>
+      <c r="E29" s="15">
         <v>15</v>
       </c>
-      <c r="E29" s="15">
+      <c r="F29" s="15">
         <v>13010201</v>
       </c>
-      <c r="F29" s="15"/>
       <c r="G29" s="15"/>
       <c r="H29" s="15"/>
       <c r="I29" s="15"/>
@@ -4426,26 +4577,27 @@
       <c r="O29" s="15"/>
       <c r="P29" s="15"/>
       <c r="Q29" s="15"/>
-      <c r="R29" s="13" t="s">
-        <v>235</v>
-      </c>
+      <c r="R29" s="15"/>
       <c r="S29" s="13" t="s">
         <v>235</v>
       </c>
-      <c r="T29" s="15" t="s">
+      <c r="T29" s="13" t="s">
+        <v>235</v>
+      </c>
+      <c r="U29" s="15" t="s">
         <v>218</v>
       </c>
-      <c r="U29" s="19">
+      <c r="V29" s="19">
         <v>894</v>
       </c>
-      <c r="V29" s="19">
+      <c r="W29" s="19">
         <v>679</v>
       </c>
-      <c r="W29" s="24" t="s">
+      <c r="X29" s="24" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A30" s="25">
         <v>13010209</v>
       </c>
@@ -4455,13 +4607,15 @@
       <c r="C30" s="15">
         <v>2</v>
       </c>
-      <c r="D30" s="15">
+      <c r="D30" s="15" t="s">
+        <v>253</v>
+      </c>
+      <c r="E30" s="15">
         <v>15</v>
       </c>
-      <c r="E30" s="15">
+      <c r="F30" s="15">
         <v>13010201</v>
       </c>
-      <c r="F30" s="16"/>
       <c r="G30" s="16"/>
       <c r="H30" s="16"/>
       <c r="I30" s="16"/>
@@ -4470,29 +4624,30 @@
       <c r="L30" s="16"/>
       <c r="M30" s="16"/>
       <c r="N30" s="16"/>
-      <c r="O30" s="15"/>
+      <c r="O30" s="16"/>
       <c r="P30" s="15"/>
-      <c r="Q30" s="16"/>
-      <c r="R30" s="20" t="s">
-        <v>244</v>
-      </c>
+      <c r="Q30" s="15"/>
+      <c r="R30" s="16"/>
       <c r="S30" s="20" t="s">
         <v>244</v>
       </c>
-      <c r="T30" s="16" t="s">
+      <c r="T30" s="20" t="s">
+        <v>244</v>
+      </c>
+      <c r="U30" s="16" t="s">
         <v>219</v>
       </c>
-      <c r="U30" s="19">
+      <c r="V30" s="19">
         <v>984</v>
       </c>
-      <c r="V30" s="19">
+      <c r="W30" s="19">
         <v>734</v>
       </c>
-      <c r="W30" s="24" t="s">
+      <c r="X30" s="24" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A31" s="28">
         <v>13010301</v>
       </c>
@@ -4502,54 +4657,57 @@
       <c r="C31" s="13">
         <v>2</v>
       </c>
-      <c r="D31" s="13">
+      <c r="D31" s="20" t="s">
+        <v>254</v>
+      </c>
+      <c r="E31" s="13">
         <v>14</v>
       </c>
-      <c r="E31" s="13">
+      <c r="F31" s="13">
         <v>13010006</v>
       </c>
-      <c r="F31" s="13" t="s">
+      <c r="G31" s="13" t="s">
         <v>171</v>
       </c>
-      <c r="G31" s="13" t="s">
+      <c r="H31" s="13" t="s">
         <v>175</v>
       </c>
-      <c r="H31" s="13"/>
-      <c r="I31" s="13">
+      <c r="I31" s="13"/>
+      <c r="J31" s="13">
         <v>1</v>
       </c>
-      <c r="J31" s="13"/>
       <c r="K31" s="13"/>
       <c r="L31" s="13"/>
-      <c r="M31" s="13">
-        <v>1</v>
-      </c>
+      <c r="M31" s="13"/>
       <c r="N31" s="13">
         <v>1</v>
       </c>
-      <c r="O31" s="13"/>
+      <c r="O31" s="13">
+        <v>1</v>
+      </c>
       <c r="P31" s="13"/>
       <c r="Q31" s="13"/>
-      <c r="R31" s="13" t="s">
+      <c r="R31" s="13"/>
+      <c r="S31" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="S31" s="13" t="s">
+      <c r="T31" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="T31" s="13" t="s">
+      <c r="U31" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="U31" s="21">
+      <c r="V31" s="21">
         <v>1550</v>
       </c>
-      <c r="V31" s="21">
+      <c r="W31" s="21">
         <v>505</v>
       </c>
-      <c r="W31" s="24" t="s">
+      <c r="X31" s="24" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A32" s="28">
         <v>13010302</v>
       </c>
@@ -4559,54 +4717,57 @@
       <c r="C32" s="13">
         <v>2</v>
       </c>
-      <c r="D32" s="13">
+      <c r="D32" s="20" t="s">
+        <v>254</v>
+      </c>
+      <c r="E32" s="13">
         <v>10</v>
       </c>
-      <c r="E32" s="13">
+      <c r="F32" s="13">
         <v>13010006</v>
       </c>
-      <c r="F32" s="13" t="s">
+      <c r="G32" s="13" t="s">
         <v>178</v>
       </c>
-      <c r="G32" s="13" t="s">
+      <c r="H32" s="13" t="s">
         <v>202</v>
       </c>
-      <c r="H32" s="13"/>
-      <c r="I32" s="13">
+      <c r="I32" s="13"/>
+      <c r="J32" s="13">
         <v>1</v>
       </c>
-      <c r="J32" s="13"/>
       <c r="K32" s="13"/>
       <c r="L32" s="13"/>
       <c r="M32" s="13"/>
-      <c r="N32" s="13">
-        <v>1</v>
-      </c>
+      <c r="N32" s="13"/>
       <c r="O32" s="13">
         <v>1</v>
       </c>
-      <c r="P32" s="13"/>
+      <c r="P32" s="13">
+        <v>1</v>
+      </c>
       <c r="Q32" s="13"/>
-      <c r="R32" s="13" t="s">
+      <c r="R32" s="13"/>
+      <c r="S32" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="S32" s="13" t="s">
+      <c r="T32" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="T32" s="13" t="s">
+      <c r="U32" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="U32" s="21">
+      <c r="V32" s="21">
         <v>1441</v>
       </c>
-      <c r="V32" s="21">
+      <c r="W32" s="21">
         <v>527</v>
       </c>
-      <c r="W32" s="24" t="s">
+      <c r="X32" s="24" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A33" s="28">
         <v>13010303</v>
       </c>
@@ -4616,77 +4777,80 @@
       <c r="C33" s="13">
         <v>2</v>
       </c>
-      <c r="D33" s="13">
+      <c r="D33" s="20" t="s">
+        <v>254</v>
+      </c>
+      <c r="E33" s="13">
         <v>12</v>
       </c>
-      <c r="E33" s="13">
+      <c r="F33" s="13">
         <v>13010006</v>
       </c>
-      <c r="F33" s="13" t="s">
+      <c r="G33" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="G33" s="13" t="s">
+      <c r="H33" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="H33" s="13"/>
-      <c r="I33" s="13">
+      <c r="I33" s="13"/>
+      <c r="J33" s="13">
         <v>1</v>
       </c>
-      <c r="J33" s="13"/>
-      <c r="K33" s="13">
+      <c r="K33" s="13"/>
+      <c r="L33" s="13">
         <v>1</v>
       </c>
-      <c r="L33" s="13"/>
       <c r="M33" s="13"/>
       <c r="N33" s="13"/>
       <c r="O33" s="13"/>
-      <c r="P33" s="13">
+      <c r="P33" s="13"/>
+      <c r="Q33" s="13">
         <v>1</v>
       </c>
-      <c r="Q33" s="13"/>
-      <c r="R33" s="13" t="s">
+      <c r="R33" s="13"/>
+      <c r="S33" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="S33" s="13" t="s">
+      <c r="T33" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="T33" s="13" t="s">
+      <c r="U33" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="U33" s="21">
+      <c r="V33" s="21">
         <v>1574</v>
       </c>
-      <c r="V33" s="21">
+      <c r="W33" s="21">
         <v>373</v>
       </c>
-      <c r="W33" s="24" t="s">
+      <c r="X33" s="24" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A34" s="17">
         <v>13020001</v>
       </c>
       <c r="B34" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="C34" s="17">
+      <c r="C34" s="13">
         <v>3</v>
       </c>
-      <c r="D34" s="13">
+      <c r="D34" s="15"/>
+      <c r="E34" s="13">
         <v>3</v>
       </c>
-      <c r="E34" s="13">
+      <c r="F34" s="13">
         <v>13010002</v>
       </c>
-      <c r="F34" s="13" t="s">
+      <c r="G34" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="G34" s="13"/>
-      <c r="H34" s="13" t="s">
+      <c r="H34" s="13"/>
+      <c r="I34" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="I34" s="13"/>
       <c r="J34" s="13"/>
       <c r="K34" s="13"/>
       <c r="L34" s="13"/>
@@ -4695,34 +4859,35 @@
       <c r="O34" s="13"/>
       <c r="P34" s="13"/>
       <c r="Q34" s="13"/>
-      <c r="R34" s="13" t="s">
+      <c r="R34" s="13"/>
+      <c r="S34" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="S34" s="13" t="s">
+      <c r="T34" s="13" t="s">
         <v>160</v>
       </c>
-      <c r="T34" s="13"/>
       <c r="U34" s="13"/>
       <c r="V34" s="13"/>
-      <c r="W34" s="22"/>
+      <c r="W34" s="13"/>
+      <c r="X34" s="22"/>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A35" s="17">
         <v>13020002</v>
       </c>
       <c r="B35" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="C35" s="17">
+      <c r="C35" s="13">
         <v>3</v>
       </c>
-      <c r="D35" s="13">
+      <c r="D35" s="15"/>
+      <c r="E35" s="13">
         <v>3</v>
       </c>
-      <c r="E35" s="13">
+      <c r="F35" s="13">
         <v>13010002</v>
       </c>
-      <c r="F35" s="13"/>
       <c r="G35" s="13"/>
       <c r="H35" s="13"/>
       <c r="I35" s="13"/>
@@ -4734,40 +4899,41 @@
       <c r="O35" s="13"/>
       <c r="P35" s="13"/>
       <c r="Q35" s="13"/>
-      <c r="R35" s="13" t="s">
+      <c r="R35" s="13"/>
+      <c r="S35" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="S35" s="13" t="s">
+      <c r="T35" s="13" t="s">
         <v>161</v>
       </c>
-      <c r="T35" s="13"/>
       <c r="U35" s="13"/>
       <c r="V35" s="13"/>
-      <c r="W35" s="22"/>
+      <c r="W35" s="13"/>
+      <c r="X35" s="22"/>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A36" s="17">
         <v>13020011</v>
       </c>
       <c r="B36" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="C36" s="17">
+      <c r="C36" s="13">
         <v>3</v>
       </c>
-      <c r="D36" s="13">
+      <c r="D36" s="15"/>
+      <c r="E36" s="13">
         <v>8</v>
       </c>
-      <c r="E36" s="13">
+      <c r="F36" s="13">
         <v>13010007</v>
       </c>
-      <c r="F36" s="13" t="s">
+      <c r="G36" s="13" t="s">
         <v>173</v>
       </c>
-      <c r="G36" s="13" t="s">
+      <c r="H36" s="13" t="s">
         <v>205</v>
       </c>
-      <c r="H36" s="13"/>
       <c r="I36" s="13"/>
       <c r="J36" s="13"/>
       <c r="K36" s="13"/>
@@ -4777,37 +4943,38 @@
       <c r="O36" s="13"/>
       <c r="P36" s="13"/>
       <c r="Q36" s="13"/>
-      <c r="R36" s="13" t="s">
+      <c r="R36" s="13"/>
+      <c r="S36" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="S36" s="13" t="s">
+      <c r="T36" s="13" t="s">
         <v>162</v>
       </c>
-      <c r="T36" s="13"/>
       <c r="U36" s="13"/>
       <c r="V36" s="13"/>
-      <c r="W36" s="22"/>
+      <c r="W36" s="13"/>
+      <c r="X36" s="22"/>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A37" s="17">
         <v>13020012</v>
       </c>
       <c r="B37" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="C37" s="17">
+      <c r="C37" s="13">
         <v>3</v>
       </c>
-      <c r="D37" s="13">
+      <c r="D37" s="15"/>
+      <c r="E37" s="13">
         <v>8</v>
       </c>
-      <c r="E37" s="13">
+      <c r="F37" s="13">
         <v>13010007</v>
       </c>
-      <c r="F37" s="13" t="s">
+      <c r="G37" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="G37" s="13"/>
       <c r="H37" s="13"/>
       <c r="I37" s="13"/>
       <c r="J37" s="13"/>
@@ -4818,34 +4985,35 @@
       <c r="O37" s="13"/>
       <c r="P37" s="13"/>
       <c r="Q37" s="13"/>
-      <c r="R37" s="13" t="s">
+      <c r="R37" s="13"/>
+      <c r="S37" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="S37" s="13" t="s">
+      <c r="T37" s="13" t="s">
         <v>163</v>
       </c>
-      <c r="T37" s="13"/>
       <c r="U37" s="13"/>
       <c r="V37" s="13"/>
-      <c r="W37" s="22"/>
+      <c r="W37" s="13"/>
+      <c r="X37" s="22"/>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A38" s="17">
         <v>13020013</v>
       </c>
       <c r="B38" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="C38" s="17">
+      <c r="C38" s="13">
         <v>3</v>
       </c>
-      <c r="D38" s="13">
+      <c r="D38" s="15"/>
+      <c r="E38" s="13">
         <v>8</v>
       </c>
-      <c r="E38" s="13">
+      <c r="F38" s="13">
         <v>13010007</v>
       </c>
-      <c r="F38" s="13"/>
       <c r="G38" s="13"/>
       <c r="H38" s="13"/>
       <c r="I38" s="13"/>
@@ -4857,43 +5025,44 @@
       <c r="O38" s="13"/>
       <c r="P38" s="13"/>
       <c r="Q38" s="13"/>
-      <c r="R38" s="13" t="s">
+      <c r="R38" s="13"/>
+      <c r="S38" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="S38" s="13" t="s">
+      <c r="T38" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="T38" s="13"/>
       <c r="U38" s="13"/>
       <c r="V38" s="13"/>
-      <c r="W38" s="22"/>
+      <c r="W38" s="13"/>
+      <c r="X38" s="22"/>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A39" s="17">
         <v>13020021</v>
       </c>
       <c r="B39" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="C39" s="17">
+      <c r="C39" s="13">
         <v>3</v>
       </c>
-      <c r="D39" s="13">
+      <c r="D39" s="15"/>
+      <c r="E39" s="13">
         <v>5</v>
       </c>
-      <c r="E39" s="13">
+      <c r="F39" s="13">
         <v>13010004</v>
       </c>
-      <c r="F39" s="13" t="s">
+      <c r="G39" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="G39" s="13" t="s">
+      <c r="H39" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="H39" s="13" t="s">
+      <c r="I39" s="13" t="s">
         <v>191</v>
       </c>
-      <c r="I39" s="13"/>
       <c r="J39" s="13"/>
       <c r="K39" s="13"/>
       <c r="L39" s="13"/>
@@ -4902,43 +5071,44 @@
       <c r="O39" s="13"/>
       <c r="P39" s="13"/>
       <c r="Q39" s="13"/>
-      <c r="R39" s="13" t="s">
+      <c r="R39" s="13"/>
+      <c r="S39" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="S39" s="13" t="s">
+      <c r="T39" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="T39" s="13"/>
       <c r="U39" s="13"/>
       <c r="V39" s="13"/>
-      <c r="W39" s="22"/>
+      <c r="W39" s="13"/>
+      <c r="X39" s="22"/>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A40" s="17">
         <v>13020022</v>
       </c>
       <c r="B40" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="C40" s="17">
+      <c r="C40" s="13">
         <v>3</v>
       </c>
-      <c r="D40" s="13">
+      <c r="D40" s="15"/>
+      <c r="E40" s="13">
         <v>5</v>
       </c>
-      <c r="E40" s="13">
+      <c r="F40" s="13">
         <v>13010004</v>
       </c>
-      <c r="F40" s="13" t="s">
+      <c r="G40" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="G40" s="13" t="s">
+      <c r="H40" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="H40" s="13" t="s">
+      <c r="I40" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="I40" s="13"/>
       <c r="J40" s="13"/>
       <c r="K40" s="13"/>
       <c r="L40" s="13"/>
@@ -4947,43 +5117,44 @@
       <c r="O40" s="13"/>
       <c r="P40" s="13"/>
       <c r="Q40" s="13"/>
-      <c r="R40" s="13" t="s">
+      <c r="R40" s="13"/>
+      <c r="S40" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="S40" s="13" t="s">
+      <c r="T40" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="T40" s="13"/>
       <c r="U40" s="13"/>
       <c r="V40" s="13"/>
-      <c r="W40" s="22"/>
+      <c r="W40" s="13"/>
+      <c r="X40" s="22"/>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A41" s="17">
         <v>13020023</v>
       </c>
       <c r="B41" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="C41" s="17">
+      <c r="C41" s="13">
         <v>3</v>
       </c>
-      <c r="D41" s="13">
+      <c r="D41" s="15"/>
+      <c r="E41" s="13">
         <v>5</v>
       </c>
-      <c r="E41" s="13">
+      <c r="F41" s="13">
         <v>13010004</v>
       </c>
-      <c r="F41" s="13" t="s">
+      <c r="G41" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="G41" s="13" t="s">
+      <c r="H41" s="13" t="s">
         <v>204</v>
       </c>
-      <c r="H41" s="13" t="s">
+      <c r="I41" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="I41" s="13"/>
       <c r="J41" s="13"/>
       <c r="K41" s="13"/>
       <c r="L41" s="13"/>
@@ -4992,39 +5163,40 @@
       <c r="O41" s="13"/>
       <c r="P41" s="13"/>
       <c r="Q41" s="13"/>
-      <c r="R41" s="13" t="s">
+      <c r="R41" s="13"/>
+      <c r="S41" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="S41" s="13" t="s">
+      <c r="T41" s="13" t="s">
         <v>167</v>
       </c>
-      <c r="T41" s="13"/>
       <c r="U41" s="13"/>
       <c r="V41" s="13"/>
-      <c r="W41" s="22"/>
+      <c r="W41" s="13"/>
+      <c r="X41" s="22"/>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A42" s="18">
         <v>13020031</v>
       </c>
       <c r="B42" s="17" t="s">
         <v>180</v>
       </c>
-      <c r="C42" s="18">
+      <c r="C42" s="13">
         <v>3</v>
       </c>
-      <c r="D42" s="15">
+      <c r="D42" s="15"/>
+      <c r="E42" s="15">
         <v>10</v>
       </c>
-      <c r="E42" s="15">
+      <c r="F42" s="15">
         <v>13010005</v>
       </c>
-      <c r="F42" s="15"/>
       <c r="G42" s="15"/>
-      <c r="H42" s="15" t="s">
+      <c r="H42" s="15"/>
+      <c r="I42" s="15" t="s">
         <v>192</v>
       </c>
-      <c r="I42" s="15"/>
       <c r="J42" s="15"/>
       <c r="K42" s="15"/>
       <c r="L42" s="15"/>
@@ -5033,39 +5205,40 @@
       <c r="O42" s="15"/>
       <c r="P42" s="15"/>
       <c r="Q42" s="15"/>
-      <c r="R42" s="13" t="s">
+      <c r="R42" s="15"/>
+      <c r="S42" s="13" t="s">
         <v>181</v>
       </c>
-      <c r="S42" s="15" t="s">
+      <c r="T42" s="15" t="s">
         <v>186</v>
       </c>
-      <c r="T42" s="15"/>
       <c r="U42" s="15"/>
       <c r="V42" s="15"/>
-      <c r="W42" s="22"/>
+      <c r="W42" s="15"/>
+      <c r="X42" s="22"/>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A43" s="18">
         <v>13020032</v>
       </c>
       <c r="B43" s="17" t="s">
         <v>182</v>
       </c>
-      <c r="C43" s="18">
+      <c r="C43" s="13">
         <v>3</v>
       </c>
-      <c r="D43" s="15">
+      <c r="D43" s="15"/>
+      <c r="E43" s="15">
         <v>10</v>
       </c>
-      <c r="E43" s="15">
+      <c r="F43" s="15">
         <v>13010005</v>
       </c>
-      <c r="F43" s="15"/>
       <c r="G43" s="15"/>
-      <c r="H43" s="15" t="s">
+      <c r="H43" s="15"/>
+      <c r="I43" s="15" t="s">
         <v>193</v>
       </c>
-      <c r="I43" s="15"/>
       <c r="J43" s="15"/>
       <c r="K43" s="15"/>
       <c r="L43" s="15"/>
@@ -5074,39 +5247,40 @@
       <c r="O43" s="15"/>
       <c r="P43" s="15"/>
       <c r="Q43" s="15"/>
-      <c r="R43" s="13" t="s">
+      <c r="R43" s="15"/>
+      <c r="S43" s="13" t="s">
         <v>181</v>
       </c>
-      <c r="S43" s="15" t="s">
+      <c r="T43" s="15" t="s">
         <v>187</v>
       </c>
-      <c r="T43" s="15"/>
       <c r="U43" s="15"/>
       <c r="V43" s="15"/>
-      <c r="W43" s="22"/>
+      <c r="W43" s="15"/>
+      <c r="X43" s="22"/>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A44" s="18">
         <v>13020033</v>
       </c>
       <c r="B44" s="17" t="s">
         <v>183</v>
       </c>
-      <c r="C44" s="18">
+      <c r="C44" s="13">
         <v>3</v>
       </c>
-      <c r="D44" s="15">
+      <c r="D44" s="15"/>
+      <c r="E44" s="15">
         <v>10</v>
       </c>
-      <c r="E44" s="15">
+      <c r="F44" s="15">
         <v>13010005</v>
       </c>
-      <c r="F44" s="15"/>
       <c r="G44" s="15"/>
-      <c r="H44" s="15" t="s">
+      <c r="H44" s="15"/>
+      <c r="I44" s="15" t="s">
         <v>194</v>
       </c>
-      <c r="I44" s="15"/>
       <c r="J44" s="15"/>
       <c r="K44" s="15"/>
       <c r="L44" s="15"/>
@@ -5115,39 +5289,40 @@
       <c r="O44" s="15"/>
       <c r="P44" s="15"/>
       <c r="Q44" s="15"/>
-      <c r="R44" s="13" t="s">
+      <c r="R44" s="15"/>
+      <c r="S44" s="13" t="s">
         <v>181</v>
       </c>
-      <c r="S44" s="15" t="s">
+      <c r="T44" s="15" t="s">
         <v>188</v>
       </c>
-      <c r="T44" s="19"/>
       <c r="U44" s="19"/>
       <c r="V44" s="19"/>
-      <c r="W44" s="22"/>
+      <c r="W44" s="19"/>
+      <c r="X44" s="22"/>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A45" s="18">
         <v>13020034</v>
       </c>
       <c r="B45" s="17" t="s">
         <v>184</v>
       </c>
-      <c r="C45" s="18">
+      <c r="C45" s="13">
         <v>3</v>
       </c>
-      <c r="D45" s="15">
+      <c r="D45" s="15"/>
+      <c r="E45" s="15">
         <v>10</v>
       </c>
-      <c r="E45" s="15">
+      <c r="F45" s="15">
         <v>13010005</v>
       </c>
-      <c r="F45" s="15"/>
       <c r="G45" s="15"/>
-      <c r="H45" s="15" t="s">
+      <c r="H45" s="15"/>
+      <c r="I45" s="15" t="s">
         <v>195</v>
       </c>
-      <c r="I45" s="15"/>
       <c r="J45" s="15"/>
       <c r="K45" s="15"/>
       <c r="L45" s="15"/>
@@ -5156,39 +5331,40 @@
       <c r="O45" s="15"/>
       <c r="P45" s="15"/>
       <c r="Q45" s="15"/>
-      <c r="R45" s="13" t="s">
+      <c r="R45" s="15"/>
+      <c r="S45" s="13" t="s">
         <v>181</v>
       </c>
-      <c r="S45" s="15" t="s">
+      <c r="T45" s="15" t="s">
         <v>189</v>
       </c>
-      <c r="T45" s="19"/>
       <c r="U45" s="19"/>
       <c r="V45" s="19"/>
-      <c r="W45" s="22"/>
+      <c r="W45" s="19"/>
+      <c r="X45" s="22"/>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A46" s="18">
         <v>13020035</v>
       </c>
       <c r="B46" s="17" t="s">
         <v>185</v>
       </c>
-      <c r="C46" s="18">
+      <c r="C46" s="13">
         <v>3</v>
       </c>
-      <c r="D46" s="15">
+      <c r="D46" s="15"/>
+      <c r="E46" s="15">
         <v>10</v>
       </c>
-      <c r="E46" s="15">
+      <c r="F46" s="15">
         <v>13010005</v>
       </c>
-      <c r="F46" s="15"/>
       <c r="G46" s="15"/>
-      <c r="H46" s="15" t="s">
+      <c r="H46" s="15"/>
+      <c r="I46" s="15" t="s">
         <v>196</v>
       </c>
-      <c r="I46" s="15"/>
       <c r="J46" s="15"/>
       <c r="K46" s="15"/>
       <c r="L46" s="15"/>
@@ -5197,32 +5373,33 @@
       <c r="O46" s="15"/>
       <c r="P46" s="15"/>
       <c r="Q46" s="15"/>
-      <c r="R46" s="13" t="s">
+      <c r="R46" s="15"/>
+      <c r="S46" s="13" t="s">
         <v>181</v>
       </c>
-      <c r="S46" s="15" t="s">
+      <c r="T46" s="15" t="s">
         <v>190</v>
       </c>
-      <c r="T46" s="19"/>
       <c r="U46" s="19"/>
       <c r="V46" s="19"/>
-      <c r="W46" s="22"/>
+      <c r="W46" s="19"/>
+      <c r="X46" s="22"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="I4:P46">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+  <conditionalFormatting sqref="J4:Q46">
+    <cfRule type="cellIs" dxfId="29" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J4">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+  <conditionalFormatting sqref="K4">
+    <cfRule type="cellIs" dxfId="28" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F4:H46">
-    <cfRule type="containsBlanks" dxfId="1" priority="5">
-      <formula>LEN(TRIM(F4))=0</formula>
+  <conditionalFormatting sqref="G4:I46">
+    <cfRule type="containsBlanks" dxfId="27" priority="5">
+      <formula>LEN(TRIM(G4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add two new scenes
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Scene.xlsx
+++ b/ConfigData/Xlsx/Scene.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18528"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scene" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="262">
   <si>
     <t>村外小屋</t>
   </si>
@@ -971,13 +971,27 @@
   </si>
   <si>
     <t>湖区</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>顿河北岸</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ljhba</t>
+  </si>
+  <si>
+    <t>lypb</t>
+  </si>
+  <si>
+    <t>拉雅瀑布</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1708,7 +1722,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1794,6 +1808,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="41" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1842,6 +1859,27 @@
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="30">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2558,27 +2596,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2593,36 +2610,36 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:X46" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25" tableBorderDxfId="24">
-  <autoFilter ref="A3:X46"/>
-  <sortState ref="A4:X46">
-    <sortCondition ref="A3:A46"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A3:X48" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" tableBorderDxfId="27">
+  <autoFilter ref="A3:X48" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState ref="A4:X48">
+    <sortCondition ref="A3:A48"/>
   </sortState>
   <tableColumns count="24">
-    <tableColumn id="1" name="Id" dataDxfId="23"/>
-    <tableColumn id="2" name="Name" dataDxfId="22"/>
-    <tableColumn id="18" name="Type" dataDxfId="21"/>
-    <tableColumn id="25" name="Sector" dataDxfId="20"/>
-    <tableColumn id="3" name="Level" dataDxfId="19"/>
-    <tableColumn id="20" name="ReviveScene" dataDxfId="18"/>
-    <tableColumn id="4" name="Quest" dataDxfId="17"/>
-    <tableColumn id="17" name="QuestRandom" dataDxfId="16"/>
-    <tableColumn id="19" name="QuestDungeon" dataDxfId="15"/>
-    <tableColumn id="5" name="QPortal" dataDxfId="14"/>
-    <tableColumn id="6" name="QCardChange" dataDxfId="13"/>
-    <tableColumn id="7" name="QPiece" dataDxfId="12"/>
-    <tableColumn id="8" name="QMerchant" dataDxfId="11"/>
-    <tableColumn id="9" name="QDoctor" dataDxfId="10"/>
-    <tableColumn id="10" name="QAngel" dataDxfId="9"/>
-    <tableColumn id="21" name="QWheel" dataDxfId="8"/>
-    <tableColumn id="22" name="QRes" dataDxfId="7"/>
-    <tableColumn id="11" name="Func" dataDxfId="6"/>
-    <tableColumn id="12" name="Url" dataDxfId="5"/>
-    <tableColumn id="13" name="TilePath" dataDxfId="4"/>
-    <tableColumn id="14" name="Icon" dataDxfId="3"/>
-    <tableColumn id="15" name="IconX" dataDxfId="2"/>
-    <tableColumn id="16" name="IconY" dataDxfId="1"/>
-    <tableColumn id="24" name="IconColor" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="25"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Type" dataDxfId="24"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Sector" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Level" dataDxfId="22"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="ReviveScene" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Quest" dataDxfId="20"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="QuestRandom" dataDxfId="19"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="QuestDungeon" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="QPortal" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="QCardChange" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="QPiece" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="QMerchant" dataDxfId="14"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="QDoctor" dataDxfId="13"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="QAngel" dataDxfId="12"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="QWheel" dataDxfId="11"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="QRes" dataDxfId="10"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Func" dataDxfId="9"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Url" dataDxfId="8"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="TilePath" dataDxfId="7"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Icon" dataDxfId="6"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="IconX" dataDxfId="5"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="IconY" dataDxfId="4"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="IconColor" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2948,11 +2965,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:X48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="W22" sqref="W22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4198,23 +4215,23 @@
       </c>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A22" s="25">
-        <v>13010201</v>
-      </c>
-      <c r="B22" s="25" t="s">
-        <v>231</v>
+      <c r="A22" s="27">
+        <v>13010109</v>
+      </c>
+      <c r="B22" s="29" t="s">
+        <v>258</v>
       </c>
       <c r="C22" s="15">
         <v>2</v>
       </c>
-      <c r="D22" s="15" t="s">
-        <v>253</v>
+      <c r="D22" s="20" t="s">
+        <v>257</v>
       </c>
       <c r="E22" s="15">
         <v>15</v>
       </c>
       <c r="F22" s="15">
-        <v>13010201</v>
+        <v>13010101</v>
       </c>
       <c r="G22" s="16"/>
       <c r="H22" s="16"/>
@@ -4229,80 +4246,80 @@
       <c r="Q22" s="15"/>
       <c r="R22" s="16"/>
       <c r="S22" s="13" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="T22" s="13" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="U22" s="16" t="s">
-        <v>221</v>
-      </c>
-      <c r="V22" s="13">
-        <v>807</v>
-      </c>
-      <c r="W22" s="13">
-        <v>720</v>
+        <v>259</v>
+      </c>
+      <c r="V22" s="16">
+        <v>643</v>
+      </c>
+      <c r="W22" s="16">
+        <v>455</v>
       </c>
       <c r="X22" s="24" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A23" s="25">
-        <v>13010202</v>
-      </c>
-      <c r="B23" s="25" t="s">
-        <v>212</v>
+      <c r="A23" s="27">
+        <v>13010110</v>
+      </c>
+      <c r="B23" s="29" t="s">
+        <v>261</v>
       </c>
       <c r="C23" s="15">
         <v>2</v>
       </c>
-      <c r="D23" s="15" t="s">
-        <v>253</v>
+      <c r="D23" s="20" t="s">
+        <v>257</v>
       </c>
       <c r="E23" s="15">
         <v>15</v>
       </c>
       <c r="F23" s="15">
-        <v>13010201</v>
-      </c>
-      <c r="G23" s="15"/>
-      <c r="H23" s="15"/>
-      <c r="I23" s="15"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="15"/>
-      <c r="L23" s="15"/>
-      <c r="M23" s="15"/>
-      <c r="N23" s="15"/>
-      <c r="O23" s="15"/>
+        <v>13010101</v>
+      </c>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16"/>
+      <c r="L23" s="16"/>
+      <c r="M23" s="16"/>
+      <c r="N23" s="16"/>
+      <c r="O23" s="16"/>
       <c r="P23" s="15"/>
       <c r="Q23" s="15"/>
-      <c r="R23" s="15"/>
+      <c r="R23" s="16"/>
       <c r="S23" s="13" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="T23" s="13" t="s">
-        <v>239</v>
-      </c>
-      <c r="U23" s="15" t="s">
-        <v>214</v>
-      </c>
-      <c r="V23" s="15">
-        <v>974</v>
-      </c>
-      <c r="W23" s="15">
-        <v>594</v>
+        <v>238</v>
+      </c>
+      <c r="U23" s="16" t="s">
+        <v>260</v>
+      </c>
+      <c r="V23" s="16">
+        <v>720</v>
+      </c>
+      <c r="W23" s="16">
+        <v>375</v>
       </c>
       <c r="X23" s="24" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A24" s="25">
-        <v>13010203</v>
+        <v>13010201</v>
       </c>
       <c r="B24" s="25" t="s">
-        <v>213</v>
+        <v>231</v>
       </c>
       <c r="C24" s="15">
         <v>2</v>
@@ -4316,31 +4333,31 @@
       <c r="F24" s="15">
         <v>13010201</v>
       </c>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
-      <c r="O24" s="15"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="16"/>
+      <c r="L24" s="16"/>
+      <c r="M24" s="16"/>
+      <c r="N24" s="16"/>
+      <c r="O24" s="16"/>
       <c r="P24" s="15"/>
       <c r="Q24" s="15"/>
-      <c r="R24" s="15"/>
+      <c r="R24" s="16"/>
       <c r="S24" s="13" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="T24" s="13" t="s">
-        <v>240</v>
-      </c>
-      <c r="U24" s="15" t="s">
-        <v>215</v>
-      </c>
-      <c r="V24" s="15">
-        <v>1080</v>
-      </c>
-      <c r="W24" s="15">
+        <v>234</v>
+      </c>
+      <c r="U24" s="16" t="s">
+        <v>221</v>
+      </c>
+      <c r="V24" s="13">
+        <v>807</v>
+      </c>
+      <c r="W24" s="13">
         <v>720</v>
       </c>
       <c r="X24" s="24" t="s">
@@ -4349,10 +4366,10 @@
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A25" s="25">
-        <v>13010204</v>
-      </c>
-      <c r="B25" s="26" t="s">
-        <v>216</v>
+        <v>13010202</v>
+      </c>
+      <c r="B25" s="25" t="s">
+        <v>212</v>
       </c>
       <c r="C25" s="15">
         <v>2</v>
@@ -4379,19 +4396,19 @@
       <c r="Q25" s="15"/>
       <c r="R25" s="15"/>
       <c r="S25" s="13" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="T25" s="13" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="U25" s="15" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="V25" s="15">
-        <v>1074</v>
+        <v>974</v>
       </c>
       <c r="W25" s="15">
-        <v>630</v>
+        <v>594</v>
       </c>
       <c r="X25" s="24" t="s">
         <v>248</v>
@@ -4399,10 +4416,10 @@
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A26" s="25">
-        <v>13010205</v>
+        <v>13010203</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>229</v>
+        <v>213</v>
       </c>
       <c r="C26" s="15">
         <v>2</v>
@@ -4416,32 +4433,32 @@
       <c r="F26" s="15">
         <v>13010201</v>
       </c>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="16"/>
-      <c r="J26" s="16"/>
-      <c r="K26" s="16"/>
-      <c r="L26" s="16"/>
-      <c r="M26" s="16"/>
-      <c r="N26" s="16"/>
-      <c r="O26" s="16"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="15"/>
+      <c r="K26" s="15"/>
+      <c r="L26" s="15"/>
+      <c r="M26" s="15"/>
+      <c r="N26" s="15"/>
+      <c r="O26" s="15"/>
       <c r="P26" s="15"/>
       <c r="Q26" s="15"/>
-      <c r="R26" s="16"/>
-      <c r="S26" s="20" t="s">
-        <v>237</v>
-      </c>
-      <c r="T26" s="20" t="s">
-        <v>237</v>
-      </c>
-      <c r="U26" s="16" t="s">
-        <v>222</v>
-      </c>
-      <c r="V26" s="13">
-        <v>717</v>
-      </c>
-      <c r="W26" s="13">
-        <v>655</v>
+      <c r="R26" s="15"/>
+      <c r="S26" s="13" t="s">
+        <v>240</v>
+      </c>
+      <c r="T26" s="13" t="s">
+        <v>240</v>
+      </c>
+      <c r="U26" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="V26" s="15">
+        <v>1080</v>
+      </c>
+      <c r="W26" s="15">
+        <v>720</v>
       </c>
       <c r="X26" s="24" t="s">
         <v>248</v>
@@ -4449,10 +4466,10 @@
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A27" s="25">
-        <v>13010206</v>
-      </c>
-      <c r="B27" s="25" t="s">
-        <v>227</v>
+        <v>13010204</v>
+      </c>
+      <c r="B27" s="26" t="s">
+        <v>216</v>
       </c>
       <c r="C27" s="15">
         <v>2</v>
@@ -4466,32 +4483,32 @@
       <c r="F27" s="15">
         <v>13010201</v>
       </c>
-      <c r="G27" s="16"/>
-      <c r="H27" s="16"/>
-      <c r="I27" s="16"/>
-      <c r="J27" s="16"/>
-      <c r="K27" s="16"/>
-      <c r="L27" s="16"/>
-      <c r="M27" s="16"/>
-      <c r="N27" s="16"/>
-      <c r="O27" s="16"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="15"/>
+      <c r="J27" s="15"/>
+      <c r="K27" s="15"/>
+      <c r="L27" s="15"/>
+      <c r="M27" s="15"/>
+      <c r="N27" s="15"/>
+      <c r="O27" s="15"/>
       <c r="P27" s="15"/>
       <c r="Q27" s="15"/>
-      <c r="R27" s="16"/>
-      <c r="S27" s="20" t="s">
-        <v>243</v>
-      </c>
-      <c r="T27" s="20" t="s">
-        <v>243</v>
-      </c>
-      <c r="U27" s="16" t="s">
-        <v>223</v>
-      </c>
-      <c r="V27" s="13">
-        <v>637</v>
-      </c>
-      <c r="W27" s="13">
-        <v>735</v>
+      <c r="R27" s="15"/>
+      <c r="S27" s="13" t="s">
+        <v>241</v>
+      </c>
+      <c r="T27" s="13" t="s">
+        <v>241</v>
+      </c>
+      <c r="U27" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="V27" s="15">
+        <v>1074</v>
+      </c>
+      <c r="W27" s="15">
+        <v>630</v>
       </c>
       <c r="X27" s="24" t="s">
         <v>248</v>
@@ -4499,10 +4516,10 @@
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A28" s="25">
-        <v>13010207</v>
+        <v>13010205</v>
       </c>
       <c r="B28" s="25" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="C28" s="15">
         <v>2</v>
@@ -4516,32 +4533,32 @@
       <c r="F28" s="15">
         <v>13010201</v>
       </c>
-      <c r="G28" s="15"/>
-      <c r="H28" s="15"/>
-      <c r="I28" s="15"/>
-      <c r="J28" s="15"/>
-      <c r="K28" s="15"/>
-      <c r="L28" s="15"/>
-      <c r="M28" s="15"/>
-      <c r="N28" s="15"/>
-      <c r="O28" s="15"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="16"/>
+      <c r="K28" s="16"/>
+      <c r="L28" s="16"/>
+      <c r="M28" s="16"/>
+      <c r="N28" s="16"/>
+      <c r="O28" s="16"/>
       <c r="P28" s="15"/>
       <c r="Q28" s="15"/>
-      <c r="R28" s="15"/>
-      <c r="S28" s="13" t="s">
-        <v>242</v>
-      </c>
-      <c r="T28" s="13" t="s">
-        <v>242</v>
-      </c>
-      <c r="U28" s="13" t="s">
-        <v>225</v>
+      <c r="R28" s="16"/>
+      <c r="S28" s="20" t="s">
+        <v>237</v>
+      </c>
+      <c r="T28" s="20" t="s">
+        <v>237</v>
+      </c>
+      <c r="U28" s="16" t="s">
+        <v>222</v>
       </c>
       <c r="V28" s="13">
-        <v>737</v>
+        <v>717</v>
       </c>
       <c r="W28" s="13">
-        <v>785</v>
+        <v>655</v>
       </c>
       <c r="X28" s="24" t="s">
         <v>248</v>
@@ -4549,10 +4566,10 @@
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A29" s="25">
-        <v>13010208</v>
-      </c>
-      <c r="B29" s="26" t="s">
-        <v>233</v>
+        <v>13010206</v>
+      </c>
+      <c r="B29" s="25" t="s">
+        <v>227</v>
       </c>
       <c r="C29" s="15">
         <v>2</v>
@@ -4566,32 +4583,32 @@
       <c r="F29" s="15">
         <v>13010201</v>
       </c>
-      <c r="G29" s="15"/>
-      <c r="H29" s="15"/>
-      <c r="I29" s="15"/>
-      <c r="J29" s="15"/>
-      <c r="K29" s="15"/>
-      <c r="L29" s="15"/>
-      <c r="M29" s="15"/>
-      <c r="N29" s="15"/>
-      <c r="O29" s="15"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="16"/>
+      <c r="K29" s="16"/>
+      <c r="L29" s="16"/>
+      <c r="M29" s="16"/>
+      <c r="N29" s="16"/>
+      <c r="O29" s="16"/>
       <c r="P29" s="15"/>
       <c r="Q29" s="15"/>
-      <c r="R29" s="15"/>
-      <c r="S29" s="13" t="s">
-        <v>235</v>
-      </c>
-      <c r="T29" s="13" t="s">
-        <v>235</v>
-      </c>
-      <c r="U29" s="15" t="s">
-        <v>218</v>
-      </c>
-      <c r="V29" s="19">
-        <v>894</v>
-      </c>
-      <c r="W29" s="19">
-        <v>679</v>
+      <c r="R29" s="16"/>
+      <c r="S29" s="20" t="s">
+        <v>243</v>
+      </c>
+      <c r="T29" s="20" t="s">
+        <v>243</v>
+      </c>
+      <c r="U29" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="V29" s="13">
+        <v>637</v>
+      </c>
+      <c r="W29" s="13">
+        <v>735</v>
       </c>
       <c r="X29" s="24" t="s">
         <v>248</v>
@@ -4599,10 +4616,10 @@
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A30" s="25">
-        <v>13010209</v>
+        <v>13010207</v>
       </c>
       <c r="B30" s="25" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C30" s="15">
         <v>2</v>
@@ -4616,163 +4633,143 @@
       <c r="F30" s="15">
         <v>13010201</v>
       </c>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16"/>
-      <c r="I30" s="16"/>
-      <c r="J30" s="16"/>
-      <c r="K30" s="16"/>
-      <c r="L30" s="16"/>
-      <c r="M30" s="16"/>
-      <c r="N30" s="16"/>
-      <c r="O30" s="16"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="15"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="15"/>
+      <c r="M30" s="15"/>
+      <c r="N30" s="15"/>
+      <c r="O30" s="15"/>
       <c r="P30" s="15"/>
       <c r="Q30" s="15"/>
-      <c r="R30" s="16"/>
-      <c r="S30" s="20" t="s">
-        <v>244</v>
-      </c>
-      <c r="T30" s="20" t="s">
-        <v>244</v>
-      </c>
-      <c r="U30" s="16" t="s">
-        <v>219</v>
-      </c>
-      <c r="V30" s="19">
-        <v>984</v>
-      </c>
-      <c r="W30" s="19">
-        <v>734</v>
+      <c r="R30" s="15"/>
+      <c r="S30" s="13" t="s">
+        <v>242</v>
+      </c>
+      <c r="T30" s="13" t="s">
+        <v>242</v>
+      </c>
+      <c r="U30" s="13" t="s">
+        <v>225</v>
+      </c>
+      <c r="V30" s="13">
+        <v>737</v>
+      </c>
+      <c r="W30" s="13">
+        <v>785</v>
       </c>
       <c r="X30" s="24" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A31" s="28">
-        <v>13010301</v>
-      </c>
-      <c r="B31" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="C31" s="13">
+      <c r="A31" s="25">
+        <v>13010208</v>
+      </c>
+      <c r="B31" s="26" t="s">
+        <v>233</v>
+      </c>
+      <c r="C31" s="15">
         <v>2</v>
       </c>
-      <c r="D31" s="20" t="s">
-        <v>254</v>
-      </c>
-      <c r="E31" s="13">
-        <v>14</v>
-      </c>
-      <c r="F31" s="13">
-        <v>13010006</v>
-      </c>
-      <c r="G31" s="13" t="s">
-        <v>171</v>
-      </c>
-      <c r="H31" s="13" t="s">
-        <v>175</v>
-      </c>
-      <c r="I31" s="13"/>
-      <c r="J31" s="13">
-        <v>1</v>
-      </c>
-      <c r="K31" s="13"/>
-      <c r="L31" s="13"/>
-      <c r="M31" s="13"/>
-      <c r="N31" s="13">
-        <v>1</v>
-      </c>
-      <c r="O31" s="13">
-        <v>1</v>
-      </c>
-      <c r="P31" s="13"/>
-      <c r="Q31" s="13"/>
-      <c r="R31" s="13"/>
+      <c r="D31" s="15" t="s">
+        <v>253</v>
+      </c>
+      <c r="E31" s="15">
+        <v>15</v>
+      </c>
+      <c r="F31" s="15">
+        <v>13010201</v>
+      </c>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="15"/>
+      <c r="J31" s="15"/>
+      <c r="K31" s="15"/>
+      <c r="L31" s="15"/>
+      <c r="M31" s="15"/>
+      <c r="N31" s="15"/>
+      <c r="O31" s="15"/>
+      <c r="P31" s="15"/>
+      <c r="Q31" s="15"/>
+      <c r="R31" s="15"/>
       <c r="S31" s="13" t="s">
-        <v>110</v>
+        <v>235</v>
       </c>
       <c r="T31" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="U31" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="V31" s="21">
-        <v>1550</v>
-      </c>
-      <c r="W31" s="21">
-        <v>505</v>
+        <v>235</v>
+      </c>
+      <c r="U31" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="V31" s="19">
+        <v>894</v>
+      </c>
+      <c r="W31" s="19">
+        <v>679</v>
       </c>
       <c r="X31" s="24" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A32" s="28">
-        <v>13010302</v>
-      </c>
-      <c r="B32" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="C32" s="13">
+      <c r="A32" s="25">
+        <v>13010209</v>
+      </c>
+      <c r="B32" s="25" t="s">
+        <v>230</v>
+      </c>
+      <c r="C32" s="15">
         <v>2</v>
       </c>
-      <c r="D32" s="20" t="s">
-        <v>254</v>
-      </c>
-      <c r="E32" s="13">
-        <v>10</v>
-      </c>
-      <c r="F32" s="13">
-        <v>13010006</v>
-      </c>
-      <c r="G32" s="13" t="s">
-        <v>178</v>
-      </c>
-      <c r="H32" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="I32" s="13"/>
-      <c r="J32" s="13">
-        <v>1</v>
-      </c>
-      <c r="K32" s="13"/>
-      <c r="L32" s="13"/>
-      <c r="M32" s="13"/>
-      <c r="N32" s="13"/>
-      <c r="O32" s="13">
-        <v>1</v>
-      </c>
-      <c r="P32" s="13">
-        <v>1</v>
-      </c>
-      <c r="Q32" s="13"/>
-      <c r="R32" s="13"/>
-      <c r="S32" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="T32" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="U32" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="V32" s="21">
-        <v>1441</v>
-      </c>
-      <c r="W32" s="21">
-        <v>527</v>
+      <c r="D32" s="15" t="s">
+        <v>253</v>
+      </c>
+      <c r="E32" s="15">
+        <v>15</v>
+      </c>
+      <c r="F32" s="15">
+        <v>13010201</v>
+      </c>
+      <c r="G32" s="16"/>
+      <c r="H32" s="16"/>
+      <c r="I32" s="16"/>
+      <c r="J32" s="16"/>
+      <c r="K32" s="16"/>
+      <c r="L32" s="16"/>
+      <c r="M32" s="16"/>
+      <c r="N32" s="16"/>
+      <c r="O32" s="16"/>
+      <c r="P32" s="15"/>
+      <c r="Q32" s="15"/>
+      <c r="R32" s="16"/>
+      <c r="S32" s="20" t="s">
+        <v>244</v>
+      </c>
+      <c r="T32" s="20" t="s">
+        <v>244</v>
+      </c>
+      <c r="U32" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="V32" s="19">
+        <v>984</v>
+      </c>
+      <c r="W32" s="19">
+        <v>734</v>
       </c>
       <c r="X32" s="24" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A33" s="28">
-        <v>13010303</v>
+        <v>13010301</v>
       </c>
       <c r="B33" s="28" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C33" s="13">
         <v>2</v>
@@ -4781,160 +4778,196 @@
         <v>254</v>
       </c>
       <c r="E33" s="13">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F33" s="13">
         <v>13010006</v>
       </c>
       <c r="G33" s="13" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="H33" s="13" t="s">
-        <v>138</v>
+        <v>175</v>
       </c>
       <c r="I33" s="13"/>
       <c r="J33" s="13">
         <v>1</v>
       </c>
       <c r="K33" s="13"/>
-      <c r="L33" s="13">
+      <c r="L33" s="13"/>
+      <c r="M33" s="13"/>
+      <c r="N33" s="13">
         <v>1</v>
       </c>
-      <c r="M33" s="13"/>
-      <c r="N33" s="13"/>
-      <c r="O33" s="13"/>
+      <c r="O33" s="13">
+        <v>1</v>
+      </c>
       <c r="P33" s="13"/>
-      <c r="Q33" s="13">
-        <v>1</v>
-      </c>
+      <c r="Q33" s="13"/>
       <c r="R33" s="13"/>
       <c r="S33" s="13" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="T33" s="13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="U33" s="13" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="V33" s="21">
-        <v>1574</v>
+        <v>1550</v>
       </c>
       <c r="W33" s="21">
-        <v>373</v>
+        <v>505</v>
       </c>
       <c r="X33" s="24" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A34" s="17">
-        <v>13020001</v>
-      </c>
-      <c r="B34" s="17" t="s">
-        <v>96</v>
+      <c r="A34" s="28">
+        <v>13010302</v>
+      </c>
+      <c r="B34" s="28" t="s">
+        <v>6</v>
       </c>
       <c r="C34" s="13">
-        <v>3</v>
-      </c>
-      <c r="D34" s="15"/>
+        <v>2</v>
+      </c>
+      <c r="D34" s="20" t="s">
+        <v>254</v>
+      </c>
       <c r="E34" s="13">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F34" s="13">
-        <v>13010002</v>
+        <v>13010006</v>
       </c>
       <c r="G34" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="H34" s="13"/>
-      <c r="I34" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="J34" s="13"/>
+        <v>178</v>
+      </c>
+      <c r="H34" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="I34" s="13"/>
+      <c r="J34" s="13">
+        <v>1</v>
+      </c>
       <c r="K34" s="13"/>
       <c r="L34" s="13"/>
       <c r="M34" s="13"/>
       <c r="N34" s="13"/>
-      <c r="O34" s="13"/>
-      <c r="P34" s="13"/>
+      <c r="O34" s="13">
+        <v>1</v>
+      </c>
+      <c r="P34" s="13">
+        <v>1</v>
+      </c>
       <c r="Q34" s="13"/>
       <c r="R34" s="13"/>
       <c r="S34" s="13" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="T34" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="U34" s="13"/>
-      <c r="V34" s="13"/>
-      <c r="W34" s="13"/>
-      <c r="X34" s="22"/>
+        <v>38</v>
+      </c>
+      <c r="U34" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="V34" s="21">
+        <v>1441</v>
+      </c>
+      <c r="W34" s="21">
+        <v>527</v>
+      </c>
+      <c r="X34" s="24" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A35" s="17">
-        <v>13020002</v>
-      </c>
-      <c r="B35" s="17" t="s">
-        <v>97</v>
+      <c r="A35" s="28">
+        <v>13010303</v>
+      </c>
+      <c r="B35" s="28" t="s">
+        <v>7</v>
       </c>
       <c r="C35" s="13">
-        <v>3</v>
-      </c>
-      <c r="D35" s="15"/>
+        <v>2</v>
+      </c>
+      <c r="D35" s="20" t="s">
+        <v>254</v>
+      </c>
       <c r="E35" s="13">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F35" s="13">
-        <v>13010002</v>
-      </c>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
+        <v>13010006</v>
+      </c>
+      <c r="G35" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="H35" s="13" t="s">
+        <v>138</v>
+      </c>
       <c r="I35" s="13"/>
-      <c r="J35" s="13"/>
+      <c r="J35" s="13">
+        <v>1</v>
+      </c>
       <c r="K35" s="13"/>
-      <c r="L35" s="13"/>
+      <c r="L35" s="13">
+        <v>1</v>
+      </c>
       <c r="M35" s="13"/>
       <c r="N35" s="13"/>
       <c r="O35" s="13"/>
       <c r="P35" s="13"/>
-      <c r="Q35" s="13"/>
+      <c r="Q35" s="13">
+        <v>1</v>
+      </c>
       <c r="R35" s="13"/>
       <c r="S35" s="13" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="T35" s="13" t="s">
-        <v>161</v>
-      </c>
-      <c r="U35" s="13"/>
-      <c r="V35" s="13"/>
-      <c r="W35" s="13"/>
-      <c r="X35" s="22"/>
+        <v>39</v>
+      </c>
+      <c r="U35" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="V35" s="21">
+        <v>1574</v>
+      </c>
+      <c r="W35" s="21">
+        <v>373</v>
+      </c>
+      <c r="X35" s="24" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A36" s="17">
-        <v>13020011</v>
+        <v>13020001</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>125</v>
+        <v>96</v>
       </c>
       <c r="C36" s="13">
         <v>3</v>
       </c>
       <c r="D36" s="15"/>
       <c r="E36" s="13">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F36" s="13">
-        <v>13010007</v>
+        <v>13010002</v>
       </c>
       <c r="G36" s="13" t="s">
-        <v>173</v>
-      </c>
-      <c r="H36" s="13" t="s">
-        <v>205</v>
-      </c>
-      <c r="I36" s="13"/>
+        <v>147</v>
+      </c>
+      <c r="H36" s="13"/>
+      <c r="I36" s="13" t="s">
+        <v>146</v>
+      </c>
       <c r="J36" s="13"/>
       <c r="K36" s="13"/>
       <c r="L36" s="13"/>
@@ -4945,10 +4978,10 @@
       <c r="Q36" s="13"/>
       <c r="R36" s="13"/>
       <c r="S36" s="13" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="T36" s="13" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="U36" s="13"/>
       <c r="V36" s="13"/>
@@ -4957,24 +4990,22 @@
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A37" s="17">
-        <v>13020012</v>
+        <v>13020002</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>122</v>
+        <v>97</v>
       </c>
       <c r="C37" s="13">
         <v>3</v>
       </c>
       <c r="D37" s="15"/>
       <c r="E37" s="13">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F37" s="13">
-        <v>13010007</v>
-      </c>
-      <c r="G37" s="13" t="s">
-        <v>155</v>
-      </c>
+        <v>13010002</v>
+      </c>
+      <c r="G37" s="13"/>
       <c r="H37" s="13"/>
       <c r="I37" s="13"/>
       <c r="J37" s="13"/>
@@ -4987,10 +5018,10 @@
       <c r="Q37" s="13"/>
       <c r="R37" s="13"/>
       <c r="S37" s="13" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="T37" s="13" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="U37" s="13"/>
       <c r="V37" s="13"/>
@@ -4999,10 +5030,10 @@
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A38" s="17">
-        <v>13020013</v>
+        <v>13020011</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C38" s="13">
         <v>3</v>
@@ -5014,8 +5045,12 @@
       <c r="F38" s="13">
         <v>13010007</v>
       </c>
-      <c r="G38" s="13"/>
-      <c r="H38" s="13"/>
+      <c r="G38" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="H38" s="13" t="s">
+        <v>205</v>
+      </c>
       <c r="I38" s="13"/>
       <c r="J38" s="13"/>
       <c r="K38" s="13"/>
@@ -5027,10 +5062,10 @@
       <c r="Q38" s="13"/>
       <c r="R38" s="13"/>
       <c r="S38" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="T38" s="13" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="U38" s="13"/>
       <c r="V38" s="13"/>
@@ -5039,30 +5074,26 @@
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A39" s="17">
-        <v>13020021</v>
+        <v>13020012</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="C39" s="13">
         <v>3</v>
       </c>
       <c r="D39" s="15"/>
       <c r="E39" s="13">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F39" s="13">
-        <v>13010004</v>
+        <v>13010007</v>
       </c>
       <c r="G39" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="H39" s="13" t="s">
-        <v>197</v>
-      </c>
-      <c r="I39" s="13" t="s">
-        <v>191</v>
-      </c>
+        <v>155</v>
+      </c>
+      <c r="H39" s="13"/>
+      <c r="I39" s="13"/>
       <c r="J39" s="13"/>
       <c r="K39" s="13"/>
       <c r="L39" s="13"/>
@@ -5073,10 +5104,10 @@
       <c r="Q39" s="13"/>
       <c r="R39" s="13"/>
       <c r="S39" s="13" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
       <c r="T39" s="13" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="U39" s="13"/>
       <c r="V39" s="13"/>
@@ -5085,30 +5116,24 @@
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A40" s="17">
-        <v>13020022</v>
+        <v>13020013</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C40" s="13">
         <v>3</v>
       </c>
       <c r="D40" s="15"/>
       <c r="E40" s="13">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F40" s="13">
-        <v>13010004</v>
-      </c>
-      <c r="G40" s="13" t="s">
-        <v>150</v>
-      </c>
-      <c r="H40" s="13" t="s">
-        <v>198</v>
-      </c>
-      <c r="I40" s="13" t="s">
-        <v>149</v>
-      </c>
+        <v>13010007</v>
+      </c>
+      <c r="G40" s="13"/>
+      <c r="H40" s="13"/>
+      <c r="I40" s="13"/>
       <c r="J40" s="13"/>
       <c r="K40" s="13"/>
       <c r="L40" s="13"/>
@@ -5119,10 +5144,10 @@
       <c r="Q40" s="13"/>
       <c r="R40" s="13"/>
       <c r="S40" s="13" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="T40" s="13" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="U40" s="13"/>
       <c r="V40" s="13"/>
@@ -5131,10 +5156,10 @@
     </row>
     <row r="41" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A41" s="17">
-        <v>13020023</v>
+        <v>13020021</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C41" s="13">
         <v>3</v>
@@ -5147,13 +5172,13 @@
         <v>13010004</v>
       </c>
       <c r="G41" s="13" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="H41" s="13" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="I41" s="13" t="s">
-        <v>153</v>
+        <v>191</v>
       </c>
       <c r="J41" s="13"/>
       <c r="K41" s="13"/>
@@ -5165,10 +5190,10 @@
       <c r="Q41" s="13"/>
       <c r="R41" s="13"/>
       <c r="S41" s="13" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="T41" s="13" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="U41" s="13"/>
       <c r="V41" s="13"/>
@@ -5176,95 +5201,103 @@
       <c r="X41" s="22"/>
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A42" s="18">
-        <v>13020031</v>
+      <c r="A42" s="17">
+        <v>13020022</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>180</v>
+        <v>132</v>
       </c>
       <c r="C42" s="13">
         <v>3</v>
       </c>
       <c r="D42" s="15"/>
-      <c r="E42" s="15">
-        <v>10</v>
-      </c>
-      <c r="F42" s="15">
-        <v>13010005</v>
-      </c>
-      <c r="G42" s="15"/>
-      <c r="H42" s="15"/>
-      <c r="I42" s="15" t="s">
-        <v>192</v>
-      </c>
-      <c r="J42" s="15"/>
-      <c r="K42" s="15"/>
-      <c r="L42" s="15"/>
-      <c r="M42" s="15"/>
-      <c r="N42" s="15"/>
-      <c r="O42" s="15"/>
-      <c r="P42" s="15"/>
-      <c r="Q42" s="15"/>
-      <c r="R42" s="15"/>
+      <c r="E42" s="13">
+        <v>5</v>
+      </c>
+      <c r="F42" s="13">
+        <v>13010004</v>
+      </c>
+      <c r="G42" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="H42" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="I42" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="J42" s="13"/>
+      <c r="K42" s="13"/>
+      <c r="L42" s="13"/>
+      <c r="M42" s="13"/>
+      <c r="N42" s="13"/>
+      <c r="O42" s="13"/>
+      <c r="P42" s="13"/>
+      <c r="Q42" s="13"/>
+      <c r="R42" s="13"/>
       <c r="S42" s="13" t="s">
-        <v>181</v>
-      </c>
-      <c r="T42" s="15" t="s">
-        <v>186</v>
-      </c>
-      <c r="U42" s="15"/>
-      <c r="V42" s="15"/>
-      <c r="W42" s="15"/>
+        <v>134</v>
+      </c>
+      <c r="T42" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="U42" s="13"/>
+      <c r="V42" s="13"/>
+      <c r="W42" s="13"/>
       <c r="X42" s="22"/>
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A43" s="18">
-        <v>13020032</v>
+      <c r="A43" s="17">
+        <v>13020023</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>182</v>
+        <v>133</v>
       </c>
       <c r="C43" s="13">
         <v>3</v>
       </c>
       <c r="D43" s="15"/>
-      <c r="E43" s="15">
-        <v>10</v>
-      </c>
-      <c r="F43" s="15">
-        <v>13010005</v>
-      </c>
-      <c r="G43" s="15"/>
-      <c r="H43" s="15"/>
-      <c r="I43" s="15" t="s">
-        <v>193</v>
-      </c>
-      <c r="J43" s="15"/>
-      <c r="K43" s="15"/>
-      <c r="L43" s="15"/>
-      <c r="M43" s="15"/>
-      <c r="N43" s="15"/>
-      <c r="O43" s="15"/>
-      <c r="P43" s="15"/>
-      <c r="Q43" s="15"/>
-      <c r="R43" s="15"/>
+      <c r="E43" s="13">
+        <v>5</v>
+      </c>
+      <c r="F43" s="13">
+        <v>13010004</v>
+      </c>
+      <c r="G43" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="H43" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="I43" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="J43" s="13"/>
+      <c r="K43" s="13"/>
+      <c r="L43" s="13"/>
+      <c r="M43" s="13"/>
+      <c r="N43" s="13"/>
+      <c r="O43" s="13"/>
+      <c r="P43" s="13"/>
+      <c r="Q43" s="13"/>
+      <c r="R43" s="13"/>
       <c r="S43" s="13" t="s">
-        <v>181</v>
-      </c>
-      <c r="T43" s="15" t="s">
-        <v>187</v>
-      </c>
-      <c r="U43" s="15"/>
-      <c r="V43" s="15"/>
-      <c r="W43" s="15"/>
+        <v>135</v>
+      </c>
+      <c r="T43" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="U43" s="13"/>
+      <c r="V43" s="13"/>
+      <c r="W43" s="13"/>
       <c r="X43" s="22"/>
     </row>
     <row r="44" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A44" s="18">
-        <v>13020033</v>
+        <v>13020031</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C44" s="13">
         <v>3</v>
@@ -5279,7 +5312,7 @@
       <c r="G44" s="15"/>
       <c r="H44" s="15"/>
       <c r="I44" s="15" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="J44" s="15"/>
       <c r="K44" s="15"/>
@@ -5294,19 +5327,19 @@
         <v>181</v>
       </c>
       <c r="T44" s="15" t="s">
-        <v>188</v>
-      </c>
-      <c r="U44" s="19"/>
-      <c r="V44" s="19"/>
-      <c r="W44" s="19"/>
+        <v>186</v>
+      </c>
+      <c r="U44" s="15"/>
+      <c r="V44" s="15"/>
+      <c r="W44" s="15"/>
       <c r="X44" s="22"/>
     </row>
     <row r="45" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A45" s="18">
-        <v>13020034</v>
+        <v>13020032</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C45" s="13">
         <v>3</v>
@@ -5321,7 +5354,7 @@
       <c r="G45" s="15"/>
       <c r="H45" s="15"/>
       <c r="I45" s="15" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="J45" s="15"/>
       <c r="K45" s="15"/>
@@ -5336,19 +5369,19 @@
         <v>181</v>
       </c>
       <c r="T45" s="15" t="s">
-        <v>189</v>
-      </c>
-      <c r="U45" s="19"/>
-      <c r="V45" s="19"/>
-      <c r="W45" s="19"/>
+        <v>187</v>
+      </c>
+      <c r="U45" s="15"/>
+      <c r="V45" s="15"/>
+      <c r="W45" s="15"/>
       <c r="X45" s="22"/>
     </row>
     <row r="46" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A46" s="18">
-        <v>13020035</v>
+        <v>13020033</v>
       </c>
       <c r="B46" s="17" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C46" s="13">
         <v>3</v>
@@ -5363,7 +5396,7 @@
       <c r="G46" s="15"/>
       <c r="H46" s="15"/>
       <c r="I46" s="15" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="J46" s="15"/>
       <c r="K46" s="15"/>
@@ -5378,27 +5411,111 @@
         <v>181</v>
       </c>
       <c r="T46" s="15" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="U46" s="19"/>
       <c r="V46" s="19"/>
       <c r="W46" s="19"/>
       <c r="X46" s="22"/>
     </row>
+    <row r="47" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="A47" s="18">
+        <v>13020034</v>
+      </c>
+      <c r="B47" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="C47" s="13">
+        <v>3</v>
+      </c>
+      <c r="D47" s="15"/>
+      <c r="E47" s="15">
+        <v>10</v>
+      </c>
+      <c r="F47" s="15">
+        <v>13010005</v>
+      </c>
+      <c r="G47" s="15"/>
+      <c r="H47" s="15"/>
+      <c r="I47" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="J47" s="15"/>
+      <c r="K47" s="15"/>
+      <c r="L47" s="15"/>
+      <c r="M47" s="15"/>
+      <c r="N47" s="15"/>
+      <c r="O47" s="15"/>
+      <c r="P47" s="15"/>
+      <c r="Q47" s="15"/>
+      <c r="R47" s="15"/>
+      <c r="S47" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="T47" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="U47" s="19"/>
+      <c r="V47" s="19"/>
+      <c r="W47" s="19"/>
+      <c r="X47" s="22"/>
+    </row>
+    <row r="48" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="A48" s="18">
+        <v>13020035</v>
+      </c>
+      <c r="B48" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="C48" s="13">
+        <v>3</v>
+      </c>
+      <c r="D48" s="15"/>
+      <c r="E48" s="15">
+        <v>10</v>
+      </c>
+      <c r="F48" s="15">
+        <v>13010005</v>
+      </c>
+      <c r="G48" s="15"/>
+      <c r="H48" s="15"/>
+      <c r="I48" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="J48" s="15"/>
+      <c r="K48" s="15"/>
+      <c r="L48" s="15"/>
+      <c r="M48" s="15"/>
+      <c r="N48" s="15"/>
+      <c r="O48" s="15"/>
+      <c r="P48" s="15"/>
+      <c r="Q48" s="15"/>
+      <c r="R48" s="15"/>
+      <c r="S48" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="T48" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="U48" s="19"/>
+      <c r="V48" s="19"/>
+      <c r="W48" s="19"/>
+      <c r="X48" s="22"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="J4:Q46">
-    <cfRule type="cellIs" dxfId="29" priority="4" operator="equal">
+  <conditionalFormatting sqref="J4:Q48">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4">
-    <cfRule type="cellIs" dxfId="28" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4:I46">
-    <cfRule type="containsBlanks" dxfId="27" priority="5">
+  <conditionalFormatting sqref="G4:I48">
+    <cfRule type="containsBlanks" dxfId="0" priority="5">
       <formula>LEN(TRIM(G4))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
add a scene cell rate view on tips
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Scene.xlsx
+++ b/ConfigData/Xlsx/Scene.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18528"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="Scene" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="271">
   <si>
     <t>村外小屋</t>
   </si>
@@ -460,549 +460,572 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>古城大厅</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>persepalace1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>persepalace3</t>
+  </si>
+  <si>
+    <t>古城外围</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>古城大殿</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>persepalace2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>玲珑峰隧道</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>smallhillchanel</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>格丁湖</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>村落入口</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>村中心</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>议事厅</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>viliage2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>viliage3</t>
+  </si>
+  <si>
+    <t>forestfire;10|crystalball;35</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|lighthouse;60</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|goblinhome;40|lighthouse;70</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>wolfnest;2|gamegamble;1|fishpool;2|sewer;3|river;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>forestfire;35|witchhome;10</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|icedream;25|lighthouse;30</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|goblinhome;40</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trees;3|grave;1|portal;1|oldtree;1|manflower;1|gamerace;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>viliage1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trees;4|manflower;2|sandland;2|cliff;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>colorpool;1|barn;1|portal;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>poppyfield;1|fishpool;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>suntemple;2|potteryroom;2|honeyhome;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>barn;1|diarybook;1|weaponseller;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>river;2|stone;3|ruintown1;1|hiddeway;1|manflower;2|orehole;1|weaponseller;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>mushroom;1|torch;1|batcrowd;2|earthelement;1|snare;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>suntemple;2|grave;2|snare;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|treasure;25|witchhome;20|dyeseller;25</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>shadowprince;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>bossmanwang;1|stonedoor;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>goblinhome;50|gamemagicbook;15|stonedoor;20</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>sandflow;2|brokehouse;2|colordoor;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>coldwind;3|snowhill;2|snowmountain;2|ropeway;1|iceland;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dgforestmaze</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dgforestinner</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dgpersepalace1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dgpersepalace2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dgpersepalace3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dgviliage1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dgviliage2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dgviliage3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>underwater;40|earthcrack;60|stonedoor;15|cavefind1;60</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ruintown1;1|manflower;2|cornfield;1|honeyhome;3|poppyfield;1|river;2|insectstorm;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>orehole;1|stone;2|sandflow;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>river;2|fishpool;1|swamp;2|colordoor;1|corsair1;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>suntemple;2|shadowprince;1|colordoor;1|blockway;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>blockway;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|treasure;25|gamerobot;20|dyeseller;30|waterbeast;20</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|witchhome;30|waterbeast;20</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>portal;1|fishpool;1|grave;2|hiddeway;1|snare;2|starve;2|blockway;1|suntemple;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>fortune;1|colordoor;1|waternest;2|ruinpiece;3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>shell;2|waternest;3|sandflow;1|corsair1;1|ruinpiece;3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>布萨特高塔</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>高塔1层</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>tower</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>高塔2层</t>
+  </si>
+  <si>
+    <t>高塔3层</t>
+  </si>
+  <si>
+    <t>高塔4层</t>
+  </si>
+  <si>
+    <t>高塔5层</t>
+  </si>
+  <si>
+    <t>dgtower1</t>
+  </si>
+  <si>
+    <t>dgtower2</t>
+  </si>
+  <si>
+    <t>dgtower3</t>
+  </si>
+  <si>
+    <t>dgtower4</t>
+  </si>
+  <si>
+    <t>dgtower5</t>
+  </si>
+  <si>
+    <t>trees;4|sandland;2|potteryroom;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trees;4</t>
+  </si>
+  <si>
+    <t>trees;5</t>
+  </si>
+  <si>
+    <t>trees;6</t>
+  </si>
+  <si>
+    <t>trees;7</t>
+  </si>
+  <si>
+    <t>trees;8</t>
+  </si>
+  <si>
+    <t>crystalball;55|wishwell;20</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>crystalball;55|wishwell;20</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>strangeletter1;30|wishwell;30</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|goblinhome;30|gamecook;20|wishwell;20</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>激活传送</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|lighthouse;60|floatbottle;50</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>met;30|treasure;25</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>hiddeway;35</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>wishwell;20</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>转盘</t>
+  </si>
+  <si>
+    <t>期货</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QWheel</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QRes</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>woodviliage</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>风悦石林北</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>风悦石林南</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>fyslb</t>
+  </si>
+  <si>
+    <t>fysln</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>石林迷窟</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>slmk</t>
+  </si>
+  <si>
+    <t>hmgd</t>
+  </si>
+  <si>
+    <t>bszx</t>
+  </si>
+  <si>
+    <t>html</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>hdyz</t>
+  </si>
+  <si>
+    <t>lshj</t>
+  </si>
+  <si>
+    <t>wxzd</t>
+  </si>
+  <si>
+    <t>ljhna</t>
+  </si>
+  <si>
+    <t>hsk</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>维述儿火山</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>卡夫金字塔</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>顿河南岸</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>流沙幻境</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>断臂角</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>鲁高因</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>库斯特树林</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>日落古道</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>lugaoyin</t>
+  </si>
+  <si>
+    <t>sunfallroad</t>
+  </si>
+  <si>
+    <t>kusttree</t>
+  </si>
+  <si>
+    <t>sandflow</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>danriversouth</t>
+  </si>
+  <si>
+    <t>windstonenorth</t>
+  </si>
+  <si>
+    <t>windstonesouth</t>
+  </si>
+  <si>
+    <t>windstonehole</t>
+  </si>
+  <si>
+    <t>vocano</t>
+  </si>
+  <si>
+    <t>pyramid</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>armcape</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>图标背景色</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>IconColor</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Green</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yellow</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>LawnGreen</t>
+  </si>
+  <si>
+    <t>LightBlue</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>所属</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>沙地</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>湾区</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>谷地</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sector</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>湖区</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>顿河北岸</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ljhba</t>
+  </si>
+  <si>
+    <t>lypb</t>
+  </si>
+  <si>
+    <t>拉雅瀑布</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>danrivernorth</t>
+  </si>
+  <si>
+    <t>danrivernorth</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>waterfalllaya</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>met;30|goblinhome;30</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>古城大厅</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>persepalace1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>persepalace3</t>
-  </si>
-  <si>
-    <t>古城外围</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>古城大殿</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>persepalace2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>玲珑峰隧道</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>smallhillchanel</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>格丁湖</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>村落入口</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>村中心</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>议事厅</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>viliage2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>viliage3</t>
-  </si>
-  <si>
-    <t>forestfire;10|crystalball;35</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|lighthouse;60</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|goblinhome;40|lighthouse;70</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>wolfnest;2|gamegamble;1|fishpool;2|sewer;3|river;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>forestfire;35|witchhome;10</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|icedream;25|lighthouse;30</t>
-    <phoneticPr fontId="18" type="noConversion"/>
+    <t>met;30</t>
   </si>
   <si>
     <t>met;30|forestfire;20|witchhome;40</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>met;30|goblinhome;40</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>trees;3|grave;1|portal;1|oldtree;1|manflower;1|gamerace;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>viliage1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>trees;4|manflower;2|sandland;2|cliff;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>colorpool;1|barn;1|portal;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>poppyfield;1|fishpool;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>suntemple;2|potteryroom;2|honeyhome;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>barn;1|diarybook;1|weaponseller;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>river;2|stone;3|ruintown1;1|hiddeway;1|manflower;2|orehole;1|weaponseller;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>mushroom;1|torch;1|batcrowd;2|earthelement;1|snare;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>suntemple;2|grave;2|snare;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|treasure;25|witchhome;20|dyeseller;25</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>shadowprince;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>bossmanwang;1|stonedoor;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>goblinhome;50|gamemagicbook;15|stonedoor;20</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>sandflow;2|brokehouse;2|colordoor;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>coldwind;3|snowhill;2|snowmountain;2|ropeway;1|iceland;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>dgforestmaze</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>dgforestinner</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>dgpersepalace1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>dgpersepalace2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>dgpersepalace3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>dgviliage1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>dgviliage2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>dgviliage3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>underwater;40|earthcrack;60|stonedoor;15|cavefind1;60</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ruintown1;1|manflower;2|cornfield;1|honeyhome;3|poppyfield;1|river;2|insectstorm;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>orehole;1|stone;2|sandflow;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>river;2|fishpool;1|swamp;2|colordoor;1|corsair1;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>suntemple;2|shadowprince;1|colordoor;1|blockway;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>blockway;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|treasure;25|gamerobot;20|dyeseller;30|waterbeast;20</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|witchhome;30|waterbeast;20</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>portal;1|fishpool;1|grave;2|hiddeway;1|snare;2|starve;2|blockway;1|suntemple;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>fortune;1|colordoor;1|waternest;2|ruinpiece;3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>shell;2|waternest;3|sandflow;1|corsair1;1|ruinpiece;3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>布萨特高塔</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>高塔1层</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>tower</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>高塔2层</t>
-  </si>
-  <si>
-    <t>高塔3层</t>
-  </si>
-  <si>
-    <t>高塔4层</t>
-  </si>
-  <si>
-    <t>高塔5层</t>
-  </si>
-  <si>
-    <t>dgtower1</t>
-  </si>
-  <si>
-    <t>dgtower2</t>
-  </si>
-  <si>
-    <t>dgtower3</t>
-  </si>
-  <si>
-    <t>dgtower4</t>
-  </si>
-  <si>
-    <t>dgtower5</t>
-  </si>
-  <si>
-    <t>trees;4|sandland;2|potteryroom;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>trees;4</t>
-  </si>
-  <si>
-    <t>trees;5</t>
-  </si>
-  <si>
-    <t>trees;6</t>
-  </si>
-  <si>
-    <t>trees;7</t>
-  </si>
-  <si>
-    <t>trees;8</t>
-  </si>
-  <si>
-    <t>crystalball;55|wishwell;20</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>crystalball;55|wishwell;20</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>strangeletter1;30|wishwell;30</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|goblinhome;30|gamecook;20|wishwell;20</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>激活传送</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|lighthouse;60|floatbottle;50</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|treasure;25</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>hiddeway;35</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>wishwell;20</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>转盘</t>
-  </si>
-  <si>
-    <t>期货</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>QWheel</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>QRes</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>woodviliage</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>风悦石林北</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>风悦石林南</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>fyslb</t>
-  </si>
-  <si>
-    <t>fysln</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>石林迷窟</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>slmk</t>
-  </si>
-  <si>
-    <t>hmgd</t>
-  </si>
-  <si>
-    <t>bszx</t>
-  </si>
-  <si>
-    <t>html</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>hdyz</t>
-  </si>
-  <si>
-    <t>lshj</t>
-  </si>
-  <si>
-    <t>wxzd</t>
-  </si>
-  <si>
-    <t>ljhna</t>
-  </si>
-  <si>
-    <t>hsk</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>维述儿火山</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>卡夫金字塔</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>顿河南岸</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>流沙幻境</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>断臂角</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>鲁高因</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>库斯特树林</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>日落古道</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>lugaoyin</t>
-  </si>
-  <si>
-    <t>sunfallroad</t>
-  </si>
-  <si>
-    <t>kusttree</t>
-  </si>
-  <si>
-    <t>sandflow</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>danriversouth</t>
-  </si>
-  <si>
-    <t>windstonenorth</t>
-  </si>
-  <si>
-    <t>windstonesouth</t>
-  </si>
-  <si>
-    <t>windstonehole</t>
-  </si>
-  <si>
-    <t>vocano</t>
-  </si>
-  <si>
-    <t>pyramid</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>armcape</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>图标背景色</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>IconColor</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Green</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Yellow</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>LawnGreen</t>
-  </si>
-  <si>
-    <t>LightBlue</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>所属</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>沙地</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>湾区</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>谷地</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sector</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>湖区</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>顿河北岸</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ljhba</t>
-  </si>
-  <si>
-    <t>lypb</t>
-  </si>
-  <si>
-    <t>拉雅瀑布</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>danrivernorth</t>
-  </si>
-  <si>
-    <t>danrivernorth</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>waterfalllaya</t>
+    <t>forestfire;25</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>orehole;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>sandland;2|sandflow;5</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>sandland;2|sandflow;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>sandland;2|orehole;1|sandflow;1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2609,6 +2632,74 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2621,36 +2712,36 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A3:X48" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25" tableBorderDxfId="24">
-  <autoFilter ref="A3:X48" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:X48" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25" tableBorderDxfId="24">
+  <autoFilter ref="A3:X48"/>
   <sortState ref="A4:X48">
     <sortCondition ref="A3:A48"/>
   </sortState>
   <tableColumns count="24">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="22"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Type" dataDxfId="21"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Sector" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Level" dataDxfId="19"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="ReviveScene" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Quest" dataDxfId="17"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="QuestRandom" dataDxfId="16"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="QuestDungeon" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="QPortal" dataDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="QCardChange" dataDxfId="13"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="QPiece" dataDxfId="12"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="QMerchant" dataDxfId="11"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="QDoctor" dataDxfId="10"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="QAngel" dataDxfId="9"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="QWheel" dataDxfId="8"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="QRes" dataDxfId="7"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Func" dataDxfId="6"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Url" dataDxfId="5"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="TilePath" dataDxfId="4"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Icon" dataDxfId="3"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="IconX" dataDxfId="2"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="IconY" dataDxfId="1"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="IconColor" dataDxfId="0"/>
+    <tableColumn id="1" name="Id" dataDxfId="23"/>
+    <tableColumn id="2" name="Name" dataDxfId="22"/>
+    <tableColumn id="18" name="Type" dataDxfId="21"/>
+    <tableColumn id="25" name="Sector" dataDxfId="20"/>
+    <tableColumn id="3" name="Level" dataDxfId="19"/>
+    <tableColumn id="20" name="ReviveScene" dataDxfId="18"/>
+    <tableColumn id="4" name="Quest" dataDxfId="17"/>
+    <tableColumn id="17" name="QuestRandom" dataDxfId="16"/>
+    <tableColumn id="19" name="QuestDungeon" dataDxfId="15"/>
+    <tableColumn id="5" name="QPortal" dataDxfId="14"/>
+    <tableColumn id="6" name="QCardChange" dataDxfId="13"/>
+    <tableColumn id="7" name="QPiece" dataDxfId="12"/>
+    <tableColumn id="8" name="QMerchant" dataDxfId="11"/>
+    <tableColumn id="9" name="QDoctor" dataDxfId="10"/>
+    <tableColumn id="10" name="QAngel" dataDxfId="9"/>
+    <tableColumn id="21" name="QWheel" dataDxfId="8"/>
+    <tableColumn id="22" name="QRes" dataDxfId="7"/>
+    <tableColumn id="11" name="Func" dataDxfId="6"/>
+    <tableColumn id="12" name="Url" dataDxfId="5"/>
+    <tableColumn id="13" name="TilePath" dataDxfId="4"/>
+    <tableColumn id="14" name="Icon" dataDxfId="3"/>
+    <tableColumn id="15" name="IconX" dataDxfId="2"/>
+    <tableColumn id="16" name="IconY" dataDxfId="1"/>
+    <tableColumn id="24" name="IconColor" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2664,7 +2755,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="C7EDCC"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -2976,11 +3067,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3014,7 +3105,7 @@
         <v>91</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>17</v>
@@ -3032,7 +3123,7 @@
         <v>116</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>51</v>
@@ -3050,10 +3141,10 @@
         <v>59</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="R1" s="2" t="s">
         <v>18</v>
@@ -3074,7 +3165,7 @@
         <v>83</v>
       </c>
       <c r="X1" s="4" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.15">
@@ -3088,7 +3179,7 @@
         <v>92</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>13</v>
@@ -3124,10 +3215,10 @@
         <v>48</v>
       </c>
       <c r="P2" s="8" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="R2" s="7" t="s">
         <v>14</v>
@@ -3162,7 +3253,7 @@
         <v>93</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E3" s="10" t="s">
         <v>22</v>
@@ -3198,10 +3289,10 @@
         <v>56</v>
       </c>
       <c r="P3" s="11" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="Q3" s="11" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="R3" s="10" t="s">
         <v>23</v>
@@ -3222,7 +3313,7 @@
         <v>61</v>
       </c>
       <c r="X3" s="23" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.15">
@@ -3236,7 +3327,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E4" s="13">
         <v>1</v>
@@ -3248,7 +3339,7 @@
         <v>87</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="I4" s="13"/>
       <c r="J4" s="13">
@@ -3278,7 +3369,7 @@
         <v>611</v>
       </c>
       <c r="X4" s="24" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.15">
@@ -3292,7 +3383,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E5" s="13">
         <v>2</v>
@@ -3301,10 +3392,10 @@
         <v>13010001</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I5" s="13"/>
       <c r="J5" s="13">
@@ -3338,7 +3429,7 @@
         <v>571</v>
       </c>
       <c r="X5" s="24" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.15">
@@ -3352,7 +3443,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E6" s="13">
         <v>3</v>
@@ -3361,10 +3452,10 @@
         <v>13010006</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I6" s="13"/>
       <c r="J6" s="13">
@@ -3394,7 +3485,7 @@
         <v>432</v>
       </c>
       <c r="X6" s="24" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.15">
@@ -3408,7 +3499,7 @@
         <v>2</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E7" s="13">
         <v>5</v>
@@ -3417,10 +3508,10 @@
         <v>13010006</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I7" s="13"/>
       <c r="J7" s="13">
@@ -3452,7 +3543,7 @@
         <v>351</v>
       </c>
       <c r="X7" s="24" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.15">
@@ -3460,13 +3551,13 @@
         <v>13010005</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C8" s="13">
         <v>2</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E8" s="13">
         <v>8</v>
@@ -3475,10 +3566,10 @@
         <v>13010006</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="I8" s="13"/>
       <c r="J8" s="13">
@@ -3510,7 +3601,7 @@
         <v>339</v>
       </c>
       <c r="X8" s="24" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.15">
@@ -3524,7 +3615,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E9" s="13">
         <v>3</v>
@@ -3560,7 +3651,7 @@
         <v>506</v>
       </c>
       <c r="X9" s="24" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.15">
@@ -3574,7 +3665,7 @@
         <v>2</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E10" s="13">
         <v>7</v>
@@ -3583,10 +3674,10 @@
         <v>13010006</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="I10" s="13"/>
       <c r="J10" s="13">
@@ -3620,7 +3711,7 @@
         <v>440</v>
       </c>
       <c r="X10" s="24" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.15">
@@ -3634,7 +3725,7 @@
         <v>2</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E11" s="13">
         <v>6</v>
@@ -3643,10 +3734,10 @@
         <v>13010006</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I11" s="13"/>
       <c r="J11" s="13">
@@ -3678,7 +3769,7 @@
         <v>338</v>
       </c>
       <c r="X11" s="24" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.15">
@@ -3692,7 +3783,7 @@
         <v>2</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E12" s="13">
         <v>4</v>
@@ -3701,10 +3792,10 @@
         <v>13010006</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="I12" s="13"/>
       <c r="J12" s="13">
@@ -3738,7 +3829,7 @@
         <v>484</v>
       </c>
       <c r="X12" s="24" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.15">
@@ -3746,13 +3837,13 @@
         <v>13010010</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C13" s="15">
         <v>2</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E13" s="15">
         <v>6</v>
@@ -3761,10 +3852,10 @@
         <v>13010006</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I13" s="13"/>
       <c r="J13" s="15">
@@ -3779,16 +3870,16 @@
       <c r="Q13" s="15"/>
       <c r="R13" s="15"/>
       <c r="S13" s="15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="T13" s="15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="U13" s="15"/>
       <c r="V13" s="15"/>
       <c r="W13" s="15"/>
       <c r="X13" s="24" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.15">
@@ -3802,7 +3893,7 @@
         <v>1</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E14" s="13">
         <v>16</v>
@@ -3823,7 +3914,7 @@
       <c r="Q14" s="13"/>
       <c r="R14" s="13"/>
       <c r="S14" s="13" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="T14" s="13" t="s">
         <v>46</v>
@@ -3838,7 +3929,7 @@
         <v>509</v>
       </c>
       <c r="X14" s="24" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.15">
@@ -3852,7 +3943,7 @@
         <v>2</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E15" s="13">
         <v>16</v>
@@ -3863,8 +3954,8 @@
       <c r="G15" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="H15" s="13" t="s">
-        <v>121</v>
+      <c r="H15" s="20" t="s">
+        <v>263</v>
       </c>
       <c r="I15" s="13"/>
       <c r="J15" s="13">
@@ -3896,7 +3987,7 @@
         <v>538</v>
       </c>
       <c r="X15" s="24" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.15">
@@ -3910,7 +4001,7 @@
         <v>2</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E16" s="13">
         <v>19</v>
@@ -3919,10 +4010,10 @@
         <v>13010101</v>
       </c>
       <c r="G16" s="13" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="I16" s="13"/>
       <c r="J16" s="13">
@@ -3933,7 +4024,9 @@
       <c r="M16" s="13"/>
       <c r="N16" s="13"/>
       <c r="O16" s="13"/>
-      <c r="P16" s="13"/>
+      <c r="P16" s="13">
+        <v>1</v>
+      </c>
       <c r="Q16" s="13"/>
       <c r="R16" s="13"/>
       <c r="S16" s="13" t="s">
@@ -3952,7 +4045,7 @@
         <v>655</v>
       </c>
       <c r="X16" s="24" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.15">
@@ -3966,7 +4059,7 @@
         <v>2</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E17" s="13">
         <v>18</v>
@@ -3978,7 +4071,7 @@
         <v>94</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I17" s="13"/>
       <c r="J17" s="13">
@@ -4010,7 +4103,7 @@
         <v>584</v>
       </c>
       <c r="X17" s="24" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.15">
@@ -4024,7 +4117,7 @@
         <v>2</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E18" s="13">
         <v>20</v>
@@ -4035,12 +4128,16 @@
       <c r="G18" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="H18" s="13" t="s">
-        <v>142</v>
+      <c r="H18" s="20" t="s">
+        <v>265</v>
       </c>
       <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
+      <c r="J18" s="13">
+        <v>1</v>
+      </c>
+      <c r="K18" s="13">
+        <v>1</v>
+      </c>
       <c r="L18" s="13"/>
       <c r="M18" s="13"/>
       <c r="N18" s="13"/>
@@ -4064,7 +4161,7 @@
         <v>444</v>
       </c>
       <c r="X18" s="24" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.15">
@@ -4072,13 +4169,13 @@
         <v>13010106</v>
       </c>
       <c r="B19" s="27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C19" s="13">
         <v>2</v>
       </c>
       <c r="D19" s="20" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E19" s="13">
         <v>15</v>
@@ -4087,10 +4184,10 @@
         <v>13010016</v>
       </c>
       <c r="G19" s="13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="I19" s="13"/>
       <c r="J19" s="13">
@@ -4122,7 +4219,7 @@
         <v>445</v>
       </c>
       <c r="X19" s="24" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.15">
@@ -4130,13 +4227,13 @@
         <v>13010107</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C20" s="15">
         <v>2</v>
       </c>
       <c r="D20" s="20" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E20" s="15">
         <v>15</v>
@@ -4145,25 +4242,33 @@
         <v>13010101</v>
       </c>
       <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
+      <c r="H20" s="20" t="s">
+        <v>266</v>
+      </c>
       <c r="I20" s="16"/>
-      <c r="J20" s="16"/>
+      <c r="J20" s="13">
+        <v>1</v>
+      </c>
       <c r="K20" s="16"/>
       <c r="L20" s="16"/>
       <c r="M20" s="16"/>
-      <c r="N20" s="16"/>
+      <c r="N20" s="16">
+        <v>1</v>
+      </c>
       <c r="O20" s="16"/>
       <c r="P20" s="15"/>
-      <c r="Q20" s="15"/>
+      <c r="Q20" s="15">
+        <v>1</v>
+      </c>
       <c r="R20" s="16"/>
       <c r="S20" s="13" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="T20" s="13" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="U20" s="13" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="V20" s="16">
         <v>850</v>
@@ -4172,7 +4277,7 @@
         <v>589</v>
       </c>
       <c r="X20" s="24" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.15">
@@ -4180,13 +4285,13 @@
         <v>13010108</v>
       </c>
       <c r="B21" s="27" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C21" s="15">
         <v>2</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E21" s="15">
         <v>15</v>
@@ -4195,11 +4300,17 @@
         <v>13010101</v>
       </c>
       <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
+      <c r="H21" s="16" t="s">
+        <v>264</v>
+      </c>
       <c r="I21" s="16"/>
-      <c r="J21" s="16"/>
+      <c r="J21" s="13">
+        <v>1</v>
+      </c>
       <c r="K21" s="16"/>
-      <c r="L21" s="16"/>
+      <c r="L21" s="16">
+        <v>1</v>
+      </c>
       <c r="M21" s="16"/>
       <c r="N21" s="16"/>
       <c r="O21" s="16"/>
@@ -4207,13 +4318,13 @@
       <c r="Q21" s="15"/>
       <c r="R21" s="16"/>
       <c r="S21" s="13" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="T21" s="13" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="U21" s="16" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="V21" s="13">
         <v>682</v>
@@ -4222,7 +4333,7 @@
         <v>545</v>
       </c>
       <c r="X21" s="24" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.15">
@@ -4230,13 +4341,13 @@
         <v>13010109</v>
       </c>
       <c r="B22" s="29" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C22" s="15">
         <v>2</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E22" s="15">
         <v>15</v>
@@ -4245,11 +4356,17 @@
         <v>13010101</v>
       </c>
       <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
+      <c r="H22" s="16" t="s">
+        <v>264</v>
+      </c>
       <c r="I22" s="16"/>
-      <c r="J22" s="16"/>
+      <c r="J22" s="13">
+        <v>1</v>
+      </c>
       <c r="K22" s="16"/>
-      <c r="L22" s="16"/>
+      <c r="L22" s="16">
+        <v>1</v>
+      </c>
       <c r="M22" s="16"/>
       <c r="N22" s="16"/>
       <c r="O22" s="16"/>
@@ -4257,13 +4374,13 @@
       <c r="Q22" s="15"/>
       <c r="R22" s="16"/>
       <c r="S22" s="13" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="T22" s="20" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="U22" s="16" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="V22" s="16">
         <v>643</v>
@@ -4272,7 +4389,7 @@
         <v>455</v>
       </c>
       <c r="X22" s="24" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.15">
@@ -4280,13 +4397,13 @@
         <v>13010110</v>
       </c>
       <c r="B23" s="29" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C23" s="15">
         <v>2</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E23" s="15">
         <v>15</v>
@@ -4295,25 +4412,33 @@
         <v>13010101</v>
       </c>
       <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
+      <c r="H23" s="16" t="s">
+        <v>264</v>
+      </c>
       <c r="I23" s="16"/>
-      <c r="J23" s="16"/>
+      <c r="J23" s="13">
+        <v>1</v>
+      </c>
       <c r="K23" s="16"/>
       <c r="L23" s="16"/>
       <c r="M23" s="16"/>
       <c r="N23" s="16"/>
       <c r="O23" s="16"/>
-      <c r="P23" s="15"/>
-      <c r="Q23" s="15"/>
+      <c r="P23" s="15">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="15">
+        <v>1</v>
+      </c>
       <c r="R23" s="16"/>
       <c r="S23" s="20" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="T23" s="20" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="U23" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="V23" s="16">
         <v>720</v>
@@ -4322,7 +4447,7 @@
         <v>375</v>
       </c>
       <c r="X23" s="24" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.15">
@@ -4330,13 +4455,13 @@
         <v>13010201</v>
       </c>
       <c r="B24" s="25" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C24" s="15">
         <v>2</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E24" s="15">
         <v>15</v>
@@ -4357,13 +4482,13 @@
       <c r="Q24" s="15"/>
       <c r="R24" s="16"/>
       <c r="S24" s="13" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="T24" s="13" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="U24" s="16" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="V24" s="13">
         <v>807</v>
@@ -4372,7 +4497,7 @@
         <v>720</v>
       </c>
       <c r="X24" s="24" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.15">
@@ -4380,13 +4505,13 @@
         <v>13010202</v>
       </c>
       <c r="B25" s="25" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C25" s="15">
         <v>2</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E25" s="15">
         <v>15</v>
@@ -4394,12 +4519,20 @@
       <c r="F25" s="15">
         <v>13010201</v>
       </c>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15"/>
+      <c r="G25" s="15" t="s">
+        <v>270</v>
+      </c>
+      <c r="H25" s="15" t="s">
+        <v>264</v>
+      </c>
       <c r="I25" s="15"/>
-      <c r="J25" s="15"/>
+      <c r="J25" s="13">
+        <v>1</v>
+      </c>
       <c r="K25" s="15"/>
-      <c r="L25" s="15"/>
+      <c r="L25" s="15">
+        <v>1</v>
+      </c>
       <c r="M25" s="15"/>
       <c r="N25" s="15"/>
       <c r="O25" s="15"/>
@@ -4407,13 +4540,13 @@
       <c r="Q25" s="15"/>
       <c r="R25" s="15"/>
       <c r="S25" s="13" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="T25" s="13" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="U25" s="15" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="V25" s="15">
         <v>974</v>
@@ -4422,7 +4555,7 @@
         <v>594</v>
       </c>
       <c r="X25" s="24" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.15">
@@ -4430,13 +4563,13 @@
         <v>13010203</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C26" s="15">
         <v>2</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E26" s="15">
         <v>15</v>
@@ -4444,26 +4577,34 @@
       <c r="F26" s="15">
         <v>13010201</v>
       </c>
-      <c r="G26" s="15"/>
-      <c r="H26" s="15"/>
+      <c r="G26" s="15" t="s">
+        <v>269</v>
+      </c>
+      <c r="H26" s="15" t="s">
+        <v>264</v>
+      </c>
       <c r="I26" s="15"/>
-      <c r="J26" s="15"/>
+      <c r="J26" s="13">
+        <v>1</v>
+      </c>
       <c r="K26" s="15"/>
       <c r="L26" s="15"/>
       <c r="M26" s="15"/>
       <c r="N26" s="15"/>
       <c r="O26" s="15"/>
       <c r="P26" s="15"/>
-      <c r="Q26" s="15"/>
+      <c r="Q26" s="15">
+        <v>1</v>
+      </c>
       <c r="R26" s="15"/>
       <c r="S26" s="13" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="T26" s="13" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="U26" s="15" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="V26" s="15">
         <v>1080</v>
@@ -4472,7 +4613,7 @@
         <v>720</v>
       </c>
       <c r="X26" s="24" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.15">
@@ -4480,13 +4621,13 @@
         <v>13010204</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C27" s="15">
         <v>2</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E27" s="15">
         <v>15</v>
@@ -4497,23 +4638,27 @@
       <c r="G27" s="15"/>
       <c r="H27" s="15"/>
       <c r="I27" s="15"/>
-      <c r="J27" s="15"/>
+      <c r="J27" s="13">
+        <v>1</v>
+      </c>
       <c r="K27" s="15"/>
       <c r="L27" s="15"/>
       <c r="M27" s="15"/>
-      <c r="N27" s="15"/>
+      <c r="N27" s="15">
+        <v>1</v>
+      </c>
       <c r="O27" s="15"/>
       <c r="P27" s="15"/>
       <c r="Q27" s="15"/>
       <c r="R27" s="15"/>
       <c r="S27" s="13" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="T27" s="13" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="U27" s="15" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="V27" s="15">
         <v>1074</v>
@@ -4522,7 +4667,7 @@
         <v>630</v>
       </c>
       <c r="X27" s="24" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.15">
@@ -4530,13 +4675,13 @@
         <v>13010205</v>
       </c>
       <c r="B28" s="25" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C28" s="15">
         <v>2</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E28" s="15">
         <v>15</v>
@@ -4544,11 +4689,17 @@
       <c r="F28" s="15">
         <v>13010201</v>
       </c>
-      <c r="G28" s="16"/>
+      <c r="G28" s="15" t="s">
+        <v>268</v>
+      </c>
       <c r="H28" s="16"/>
       <c r="I28" s="16"/>
-      <c r="J28" s="16"/>
-      <c r="K28" s="16"/>
+      <c r="J28" s="13">
+        <v>1</v>
+      </c>
+      <c r="K28" s="16">
+        <v>1</v>
+      </c>
       <c r="L28" s="16"/>
       <c r="M28" s="16"/>
       <c r="N28" s="16"/>
@@ -4557,13 +4708,13 @@
       <c r="Q28" s="15"/>
       <c r="R28" s="16"/>
       <c r="S28" s="20" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="T28" s="20" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="U28" s="16" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="V28" s="13">
         <v>717</v>
@@ -4572,7 +4723,7 @@
         <v>655</v>
       </c>
       <c r="X28" s="24" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.15">
@@ -4580,13 +4731,13 @@
         <v>13010206</v>
       </c>
       <c r="B29" s="25" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C29" s="15">
         <v>2</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E29" s="15">
         <v>15</v>
@@ -4595,25 +4746,33 @@
         <v>13010201</v>
       </c>
       <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
+      <c r="H29" s="16" t="s">
+        <v>264</v>
+      </c>
       <c r="I29" s="16"/>
-      <c r="J29" s="16"/>
+      <c r="J29" s="13">
+        <v>1</v>
+      </c>
       <c r="K29" s="16"/>
       <c r="L29" s="16"/>
-      <c r="M29" s="16"/>
+      <c r="M29" s="16">
+        <v>1</v>
+      </c>
       <c r="N29" s="16"/>
-      <c r="O29" s="16"/>
+      <c r="O29" s="16">
+        <v>1</v>
+      </c>
       <c r="P29" s="15"/>
       <c r="Q29" s="15"/>
       <c r="R29" s="16"/>
       <c r="S29" s="20" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="T29" s="20" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="U29" s="16" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="V29" s="13">
         <v>637</v>
@@ -4622,7 +4781,7 @@
         <v>735</v>
       </c>
       <c r="X29" s="24" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.15">
@@ -4630,13 +4789,13 @@
         <v>13010207</v>
       </c>
       <c r="B30" s="25" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C30" s="15">
         <v>2</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E30" s="15">
         <v>15</v>
@@ -4645,25 +4804,31 @@
         <v>13010201</v>
       </c>
       <c r="G30" s="15"/>
-      <c r="H30" s="15"/>
+      <c r="H30" s="15" t="s">
+        <v>264</v>
+      </c>
       <c r="I30" s="15"/>
-      <c r="J30" s="15"/>
+      <c r="J30" s="13">
+        <v>1</v>
+      </c>
       <c r="K30" s="15"/>
       <c r="L30" s="15"/>
       <c r="M30" s="15"/>
       <c r="N30" s="15"/>
       <c r="O30" s="15"/>
       <c r="P30" s="15"/>
-      <c r="Q30" s="15"/>
+      <c r="Q30" s="15">
+        <v>1</v>
+      </c>
       <c r="R30" s="15"/>
       <c r="S30" s="13" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="T30" s="13" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="U30" s="13" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="V30" s="13">
         <v>737</v>
@@ -4672,7 +4837,7 @@
         <v>785</v>
       </c>
       <c r="X30" s="24" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.15">
@@ -4680,13 +4845,13 @@
         <v>13010208</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C31" s="15">
         <v>2</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E31" s="15">
         <v>15</v>
@@ -4695,25 +4860,33 @@
         <v>13010201</v>
       </c>
       <c r="G31" s="15"/>
-      <c r="H31" s="15"/>
+      <c r="H31" s="15" t="s">
+        <v>264</v>
+      </c>
       <c r="I31" s="15"/>
-      <c r="J31" s="15"/>
+      <c r="J31" s="13">
+        <v>1</v>
+      </c>
       <c r="K31" s="15"/>
-      <c r="L31" s="15"/>
-      <c r="M31" s="15"/>
+      <c r="L31" s="15">
+        <v>1</v>
+      </c>
+      <c r="M31" s="15">
+        <v>1</v>
+      </c>
       <c r="N31" s="15"/>
       <c r="O31" s="15"/>
       <c r="P31" s="15"/>
       <c r="Q31" s="15"/>
       <c r="R31" s="15"/>
       <c r="S31" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="T31" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="U31" s="15" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="V31" s="19">
         <v>894</v>
@@ -4722,7 +4895,7 @@
         <v>679</v>
       </c>
       <c r="X31" s="24" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.15">
@@ -4730,13 +4903,13 @@
         <v>13010209</v>
       </c>
       <c r="B32" s="25" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C32" s="15">
         <v>2</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E32" s="15">
         <v>15</v>
@@ -4744,26 +4917,34 @@
       <c r="F32" s="15">
         <v>13010201</v>
       </c>
-      <c r="G32" s="16"/>
-      <c r="H32" s="16"/>
+      <c r="G32" s="20" t="s">
+        <v>267</v>
+      </c>
+      <c r="H32" s="16" t="s">
+        <v>264</v>
+      </c>
       <c r="I32" s="16"/>
-      <c r="J32" s="16"/>
+      <c r="J32" s="13">
+        <v>1</v>
+      </c>
       <c r="K32" s="16"/>
       <c r="L32" s="16"/>
       <c r="M32" s="16"/>
       <c r="N32" s="16"/>
       <c r="O32" s="16"/>
-      <c r="P32" s="15"/>
+      <c r="P32" s="15">
+        <v>1</v>
+      </c>
       <c r="Q32" s="15"/>
       <c r="R32" s="16"/>
       <c r="S32" s="20" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="T32" s="20" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="U32" s="16" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="V32" s="19">
         <v>984</v>
@@ -4772,7 +4953,7 @@
         <v>734</v>
       </c>
       <c r="X32" s="24" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.15">
@@ -4786,7 +4967,7 @@
         <v>2</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E33" s="13">
         <v>14</v>
@@ -4795,10 +4976,10 @@
         <v>13010006</v>
       </c>
       <c r="G33" s="13" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H33" s="13" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I33" s="13"/>
       <c r="J33" s="13">
@@ -4832,7 +5013,7 @@
         <v>505</v>
       </c>
       <c r="X33" s="24" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.15">
@@ -4846,7 +5027,7 @@
         <v>2</v>
       </c>
       <c r="D34" s="20" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E34" s="13">
         <v>10</v>
@@ -4855,10 +5036,10 @@
         <v>13010006</v>
       </c>
       <c r="G34" s="13" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H34" s="13" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I34" s="13"/>
       <c r="J34" s="13">
@@ -4892,7 +5073,7 @@
         <v>527</v>
       </c>
       <c r="X34" s="24" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.15">
@@ -4906,7 +5087,7 @@
         <v>2</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E35" s="13">
         <v>12</v>
@@ -4915,10 +5096,10 @@
         <v>13010006</v>
       </c>
       <c r="G35" s="13" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H35" s="13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I35" s="13"/>
       <c r="J35" s="13">
@@ -4952,7 +5133,7 @@
         <v>373</v>
       </c>
       <c r="X35" s="24" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.15">
@@ -4973,11 +5154,11 @@
         <v>13010002</v>
       </c>
       <c r="G36" s="13" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H36" s="13"/>
       <c r="I36" s="13" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="J36" s="13"/>
       <c r="K36" s="13"/>
@@ -4992,7 +5173,7 @@
         <v>114</v>
       </c>
       <c r="T36" s="13" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="U36" s="13"/>
       <c r="V36" s="13"/>
@@ -5032,7 +5213,7 @@
         <v>115</v>
       </c>
       <c r="T37" s="13" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="U37" s="13"/>
       <c r="V37" s="13"/>
@@ -5044,7 +5225,7 @@
         <v>13020011</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C38" s="13">
         <v>3</v>
@@ -5057,10 +5238,10 @@
         <v>13010007</v>
       </c>
       <c r="G38" s="13" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H38" s="13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I38" s="13"/>
       <c r="J38" s="13"/>
@@ -5073,10 +5254,10 @@
       <c r="Q38" s="13"/>
       <c r="R38" s="13"/>
       <c r="S38" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="T38" s="13" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="U38" s="13"/>
       <c r="V38" s="13"/>
@@ -5088,7 +5269,7 @@
         <v>13020012</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C39" s="13">
         <v>3</v>
@@ -5101,7 +5282,7 @@
         <v>13010007</v>
       </c>
       <c r="G39" s="13" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H39" s="13"/>
       <c r="I39" s="13"/>
@@ -5115,10 +5296,10 @@
       <c r="Q39" s="13"/>
       <c r="R39" s="13"/>
       <c r="S39" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="T39" s="13" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="U39" s="13"/>
       <c r="V39" s="13"/>
@@ -5130,7 +5311,7 @@
         <v>13020013</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C40" s="13">
         <v>3</v>
@@ -5155,10 +5336,10 @@
       <c r="Q40" s="13"/>
       <c r="R40" s="13"/>
       <c r="S40" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="T40" s="13" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="U40" s="13"/>
       <c r="V40" s="13"/>
@@ -5170,7 +5351,7 @@
         <v>13020021</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C41" s="13">
         <v>3</v>
@@ -5183,13 +5364,13 @@
         <v>13010004</v>
       </c>
       <c r="G41" s="13" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H41" s="13" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="I41" s="13" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="J41" s="13"/>
       <c r="K41" s="13"/>
@@ -5201,10 +5382,10 @@
       <c r="Q41" s="13"/>
       <c r="R41" s="13"/>
       <c r="S41" s="13" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="T41" s="13" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="U41" s="13"/>
       <c r="V41" s="13"/>
@@ -5216,7 +5397,7 @@
         <v>13020022</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C42" s="13">
         <v>3</v>
@@ -5229,13 +5410,13 @@
         <v>13010004</v>
       </c>
       <c r="G42" s="13" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H42" s="13" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="I42" s="13" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="J42" s="13"/>
       <c r="K42" s="13"/>
@@ -5247,10 +5428,10 @@
       <c r="Q42" s="13"/>
       <c r="R42" s="13"/>
       <c r="S42" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="T42" s="13" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="U42" s="13"/>
       <c r="V42" s="13"/>
@@ -5262,7 +5443,7 @@
         <v>13020023</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C43" s="13">
         <v>3</v>
@@ -5275,13 +5456,13 @@
         <v>13010004</v>
       </c>
       <c r="G43" s="13" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H43" s="13" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="I43" s="13" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="J43" s="13"/>
       <c r="K43" s="13"/>
@@ -5293,10 +5474,10 @@
       <c r="Q43" s="13"/>
       <c r="R43" s="13"/>
       <c r="S43" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="T43" s="13" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="U43" s="13"/>
       <c r="V43" s="13"/>
@@ -5308,7 +5489,7 @@
         <v>13020031</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C44" s="13">
         <v>3</v>
@@ -5323,7 +5504,7 @@
       <c r="G44" s="15"/>
       <c r="H44" s="15"/>
       <c r="I44" s="15" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="J44" s="15"/>
       <c r="K44" s="15"/>
@@ -5335,10 +5516,10 @@
       <c r="Q44" s="15"/>
       <c r="R44" s="15"/>
       <c r="S44" s="13" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="T44" s="15" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="U44" s="15"/>
       <c r="V44" s="15"/>
@@ -5350,7 +5531,7 @@
         <v>13020032</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C45" s="13">
         <v>3</v>
@@ -5365,7 +5546,7 @@
       <c r="G45" s="15"/>
       <c r="H45" s="15"/>
       <c r="I45" s="15" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="J45" s="15"/>
       <c r="K45" s="15"/>
@@ -5377,10 +5558,10 @@
       <c r="Q45" s="15"/>
       <c r="R45" s="15"/>
       <c r="S45" s="13" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="T45" s="15" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="U45" s="15"/>
       <c r="V45" s="15"/>
@@ -5392,7 +5573,7 @@
         <v>13020033</v>
       </c>
       <c r="B46" s="17" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C46" s="13">
         <v>3</v>
@@ -5407,7 +5588,7 @@
       <c r="G46" s="15"/>
       <c r="H46" s="15"/>
       <c r="I46" s="15" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="J46" s="15"/>
       <c r="K46" s="15"/>
@@ -5419,10 +5600,10 @@
       <c r="Q46" s="15"/>
       <c r="R46" s="15"/>
       <c r="S46" s="13" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="T46" s="15" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="U46" s="19"/>
       <c r="V46" s="19"/>
@@ -5434,7 +5615,7 @@
         <v>13020034</v>
       </c>
       <c r="B47" s="17" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C47" s="13">
         <v>3</v>
@@ -5449,7 +5630,7 @@
       <c r="G47" s="15"/>
       <c r="H47" s="15"/>
       <c r="I47" s="15" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="J47" s="15"/>
       <c r="K47" s="15"/>
@@ -5461,10 +5642,10 @@
       <c r="Q47" s="15"/>
       <c r="R47" s="15"/>
       <c r="S47" s="13" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="T47" s="15" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="U47" s="19"/>
       <c r="V47" s="19"/>
@@ -5476,7 +5657,7 @@
         <v>13020035</v>
       </c>
       <c r="B48" s="17" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C48" s="13">
         <v>3</v>
@@ -5491,7 +5672,7 @@
       <c r="G48" s="15"/>
       <c r="H48" s="15"/>
       <c r="I48" s="15" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="J48" s="15"/>
       <c r="K48" s="15"/>
@@ -5503,10 +5684,10 @@
       <c r="Q48" s="15"/>
       <c r="R48" s="15"/>
       <c r="S48" s="13" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="T48" s="15" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="U48" s="19"/>
       <c r="V48" s="19"/>

</xml_diff>

<commit_message>
new engine to limit some sq appear once in a dungeon
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Scene.xlsx
+++ b/ConfigData/Xlsx/Scene.xlsx
@@ -562,10 +562,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>bossmanwang;1|stonedoor;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>goblinhome;50|gamemagicbook;15|stonedoor;20</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -1023,7 +1019,11 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>barn;1|diarybook;1|weaponseller;1|potteryroom;1</t>
+    <t>barn;1|diarybook;1|weaponseller;1|potteryroom;1|booststr;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>bossmanwang;1|stonedoor;1|boostagi;1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -2981,7 +2981,7 @@
   <dimension ref="A1:W48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3014,7 +3014,7 @@
         <v>91</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>17</v>
@@ -3029,7 +3029,7 @@
         <v>88</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>51</v>
@@ -3047,10 +3047,10 @@
         <v>59</v>
       </c>
       <c r="O1" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>190</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>191</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>18</v>
@@ -3071,7 +3071,7 @@
         <v>83</v>
       </c>
       <c r="W1" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.15">
@@ -3085,7 +3085,7 @@
         <v>92</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>13</v>
@@ -3118,10 +3118,10 @@
         <v>48</v>
       </c>
       <c r="O2" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="P2" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="Q2" s="7" t="s">
         <v>14</v>
@@ -3156,7 +3156,7 @@
         <v>93</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E3" s="10" t="s">
         <v>22</v>
@@ -3189,10 +3189,10 @@
         <v>56</v>
       </c>
       <c r="O3" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="P3" s="11" t="s">
         <v>193</v>
-      </c>
-      <c r="P3" s="11" t="s">
-        <v>194</v>
       </c>
       <c r="Q3" s="10" t="s">
         <v>23</v>
@@ -3213,7 +3213,7 @@
         <v>61</v>
       </c>
       <c r="W3" s="23" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.15">
@@ -3227,7 +3227,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E4" s="13">
         <v>1</v>
@@ -3239,7 +3239,7 @@
         <v>87</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I4" s="13">
         <v>1</v>
@@ -3268,7 +3268,7 @@
         <v>611</v>
       </c>
       <c r="W4" s="24" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.15">
@@ -3282,7 +3282,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E5" s="13">
         <v>2</v>
@@ -3327,7 +3327,7 @@
         <v>571</v>
       </c>
       <c r="W5" s="24" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.15">
@@ -3341,7 +3341,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E6" s="13">
         <v>3</v>
@@ -3382,7 +3382,7 @@
         <v>432</v>
       </c>
       <c r="W6" s="24" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.15">
@@ -3396,7 +3396,7 @@
         <v>2</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E7" s="13">
         <v>5</v>
@@ -3439,7 +3439,7 @@
         <v>351</v>
       </c>
       <c r="W7" s="24" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.15">
@@ -3447,13 +3447,13 @@
         <v>13010005</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C8" s="13">
         <v>2</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E8" s="13">
         <v>8</v>
@@ -3462,10 +3462,10 @@
         <v>13010006</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I8" s="13">
         <v>1</v>
@@ -3496,7 +3496,7 @@
         <v>339</v>
       </c>
       <c r="W8" s="24" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.15">
@@ -3510,7 +3510,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E9" s="13">
         <v>3</v>
@@ -3545,7 +3545,7 @@
         <v>506</v>
       </c>
       <c r="W9" s="24" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.15">
@@ -3559,7 +3559,7 @@
         <v>2</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E10" s="13">
         <v>7</v>
@@ -3568,10 +3568,10 @@
         <v>13010006</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I10" s="13">
         <v>1</v>
@@ -3604,7 +3604,7 @@
         <v>440</v>
       </c>
       <c r="W10" s="24" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.15">
@@ -3618,7 +3618,7 @@
         <v>2</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E11" s="13">
         <v>6</v>
@@ -3627,7 +3627,7 @@
         <v>13010006</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H11" s="13" t="s">
         <v>138</v>
@@ -3661,7 +3661,7 @@
         <v>338</v>
       </c>
       <c r="W11" s="24" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.15">
@@ -3675,7 +3675,7 @@
         <v>2</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E12" s="13">
         <v>4</v>
@@ -3684,10 +3684,10 @@
         <v>13010006</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I12" s="13">
         <v>1</v>
@@ -3720,7 +3720,7 @@
         <v>484</v>
       </c>
       <c r="W12" s="24" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.15">
@@ -3734,7 +3734,7 @@
         <v>2</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E13" s="15">
         <v>6</v>
@@ -3746,7 +3746,7 @@
         <v>144</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I13" s="15">
         <v>1</v>
@@ -3769,7 +3769,7 @@
       <c r="U13" s="15"/>
       <c r="V13" s="15"/>
       <c r="W13" s="24" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.15">
@@ -3783,7 +3783,7 @@
         <v>1</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E14" s="13">
         <v>16</v>
@@ -3803,7 +3803,7 @@
       <c r="P14" s="13"/>
       <c r="Q14" s="13"/>
       <c r="R14" s="13" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="S14" s="13" t="s">
         <v>46</v>
@@ -3818,7 +3818,7 @@
         <v>509</v>
       </c>
       <c r="W14" s="24" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.15">
@@ -3832,7 +3832,7 @@
         <v>2</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E15" s="13">
         <v>16</v>
@@ -3844,7 +3844,7 @@
         <v>95</v>
       </c>
       <c r="H15" s="20" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I15" s="13">
         <v>1</v>
@@ -3875,7 +3875,7 @@
         <v>538</v>
       </c>
       <c r="W15" s="24" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.15">
@@ -3889,7 +3889,7 @@
         <v>2</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E16" s="13">
         <v>19</v>
@@ -3898,10 +3898,10 @@
         <v>13010101</v>
       </c>
       <c r="G16" s="20" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="H16" s="20" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I16" s="13">
         <v>1</v>
@@ -3932,7 +3932,7 @@
         <v>655</v>
       </c>
       <c r="W16" s="24" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.15">
@@ -3946,7 +3946,7 @@
         <v>2</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E17" s="13">
         <v>18</v>
@@ -3989,7 +3989,7 @@
         <v>584</v>
       </c>
       <c r="W17" s="24" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.15">
@@ -4003,7 +4003,7 @@
         <v>2</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E18" s="13">
         <v>20</v>
@@ -4015,7 +4015,7 @@
         <v>86</v>
       </c>
       <c r="H18" s="20" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I18" s="13">
         <v>1</v>
@@ -4046,7 +4046,7 @@
         <v>444</v>
       </c>
       <c r="W18" s="24" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.15">
@@ -4060,7 +4060,7 @@
         <v>2</v>
       </c>
       <c r="D19" s="20" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E19" s="13">
         <v>15</v>
@@ -4069,7 +4069,7 @@
         <v>13010016</v>
       </c>
       <c r="G19" s="20" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="H19" s="13" t="s">
         <v>139</v>
@@ -4103,7 +4103,7 @@
         <v>445</v>
       </c>
       <c r="W19" s="24" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.15">
@@ -4111,13 +4111,13 @@
         <v>13010107</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C20" s="15">
         <v>2</v>
       </c>
       <c r="D20" s="20" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E20" s="15">
         <v>15</v>
@@ -4126,10 +4126,10 @@
         <v>13010101</v>
       </c>
       <c r="G20" s="20" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H20" s="20" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="I20" s="13">
         <v>1</v>
@@ -4147,13 +4147,13 @@
       </c>
       <c r="Q20" s="16"/>
       <c r="R20" s="13" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="S20" s="13" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="T20" s="13" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="U20" s="16">
         <v>850</v>
@@ -4162,7 +4162,7 @@
         <v>589</v>
       </c>
       <c r="W20" s="24" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.15">
@@ -4170,13 +4170,13 @@
         <v>13010108</v>
       </c>
       <c r="B21" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C21" s="15">
         <v>2</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E21" s="15">
         <v>15</v>
@@ -4185,10 +4185,10 @@
         <v>13010101</v>
       </c>
       <c r="G21" s="20" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H21" s="20" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I21" s="13">
         <v>1</v>
@@ -4204,13 +4204,13 @@
       <c r="P21" s="15"/>
       <c r="Q21" s="16"/>
       <c r="R21" s="13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="S21" s="13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="T21" s="16" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="U21" s="13">
         <v>682</v>
@@ -4219,7 +4219,7 @@
         <v>545</v>
       </c>
       <c r="W21" s="24" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.15">
@@ -4227,13 +4227,13 @@
         <v>13010109</v>
       </c>
       <c r="B22" s="29" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C22" s="15">
         <v>2</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E22" s="15">
         <v>15</v>
@@ -4242,10 +4242,10 @@
         <v>13010101</v>
       </c>
       <c r="G22" s="20" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H22" s="16" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I22" s="13">
         <v>1</v>
@@ -4261,13 +4261,13 @@
       <c r="P22" s="15"/>
       <c r="Q22" s="16"/>
       <c r="R22" s="13" t="s">
+        <v>245</v>
+      </c>
+      <c r="S22" s="20" t="s">
         <v>246</v>
       </c>
-      <c r="S22" s="20" t="s">
-        <v>247</v>
-      </c>
       <c r="T22" s="16" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="U22" s="16">
         <v>643</v>
@@ -4276,7 +4276,7 @@
         <v>455</v>
       </c>
       <c r="W22" s="24" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.15">
@@ -4284,13 +4284,13 @@
         <v>13010110</v>
       </c>
       <c r="B23" s="29" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C23" s="15">
         <v>2</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E23" s="15">
         <v>15</v>
@@ -4299,10 +4299,10 @@
         <v>13010101</v>
       </c>
       <c r="G23" s="20" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H23" s="16" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I23" s="13">
         <v>1</v>
@@ -4320,13 +4320,13 @@
       </c>
       <c r="Q23" s="16"/>
       <c r="R23" s="20" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="S23" s="20" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="T23" s="16" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="U23" s="16">
         <v>720</v>
@@ -4335,7 +4335,7 @@
         <v>375</v>
       </c>
       <c r="W23" s="24" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.15">
@@ -4343,13 +4343,13 @@
         <v>13010201</v>
       </c>
       <c r="B24" s="25" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C24" s="15">
         <v>2</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E24" s="15">
         <v>15</v>
@@ -4369,13 +4369,13 @@
       <c r="P24" s="15"/>
       <c r="Q24" s="16"/>
       <c r="R24" s="13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="S24" s="13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="T24" s="16" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="U24" s="13">
         <v>807</v>
@@ -4384,7 +4384,7 @@
         <v>720</v>
       </c>
       <c r="W24" s="24" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.15">
@@ -4392,13 +4392,13 @@
         <v>13010202</v>
       </c>
       <c r="B25" s="25" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C25" s="15">
         <v>2</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E25" s="15">
         <v>15</v>
@@ -4407,10 +4407,10 @@
         <v>13010201</v>
       </c>
       <c r="G25" s="15" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="H25" s="15" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I25" s="13">
         <v>1</v>
@@ -4426,13 +4426,13 @@
       <c r="P25" s="15"/>
       <c r="Q25" s="15"/>
       <c r="R25" s="13" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="S25" s="13" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="T25" s="15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="U25" s="15">
         <v>974</v>
@@ -4441,7 +4441,7 @@
         <v>594</v>
       </c>
       <c r="W25" s="24" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.15">
@@ -4449,13 +4449,13 @@
         <v>13010203</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C26" s="15">
         <v>2</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E26" s="15">
         <v>15</v>
@@ -4464,10 +4464,10 @@
         <v>13010201</v>
       </c>
       <c r="G26" s="15" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="H26" s="15" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I26" s="13">
         <v>1</v>
@@ -4483,13 +4483,13 @@
       </c>
       <c r="Q26" s="15"/>
       <c r="R26" s="13" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="S26" s="13" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="T26" s="15" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="U26" s="15">
         <v>1080</v>
@@ -4498,7 +4498,7 @@
         <v>720</v>
       </c>
       <c r="W26" s="24" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.15">
@@ -4506,13 +4506,13 @@
         <v>13010204</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C27" s="15">
         <v>2</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E27" s="15">
         <v>15</v>
@@ -4521,10 +4521,10 @@
         <v>13010201</v>
       </c>
       <c r="G27" s="15" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H27" s="15" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I27" s="13">
         <v>1</v>
@@ -4540,13 +4540,13 @@
       <c r="P27" s="15"/>
       <c r="Q27" s="15"/>
       <c r="R27" s="13" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S27" s="13" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="T27" s="15" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="U27" s="15">
         <v>1074</v>
@@ -4555,7 +4555,7 @@
         <v>630</v>
       </c>
       <c r="W27" s="24" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.15">
@@ -4563,13 +4563,13 @@
         <v>13010205</v>
       </c>
       <c r="B28" s="25" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C28" s="15">
         <v>2</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E28" s="15">
         <v>15</v>
@@ -4578,7 +4578,7 @@
         <v>13010201</v>
       </c>
       <c r="G28" s="15" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H28" s="16"/>
       <c r="I28" s="13">
@@ -4595,13 +4595,13 @@
       <c r="P28" s="15"/>
       <c r="Q28" s="16"/>
       <c r="R28" s="20" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="S28" s="20" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="T28" s="16" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="U28" s="13">
         <v>717</v>
@@ -4610,7 +4610,7 @@
         <v>655</v>
       </c>
       <c r="W28" s="24" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.15">
@@ -4618,13 +4618,13 @@
         <v>13010206</v>
       </c>
       <c r="B29" s="25" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C29" s="15">
         <v>2</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E29" s="15">
         <v>15</v>
@@ -4634,7 +4634,7 @@
       </c>
       <c r="G29" s="16"/>
       <c r="H29" s="20" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I29" s="13">
         <v>1</v>
@@ -4652,13 +4652,13 @@
       <c r="P29" s="15"/>
       <c r="Q29" s="16"/>
       <c r="R29" s="20" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="S29" s="20" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="T29" s="16" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="U29" s="13">
         <v>637</v>
@@ -4667,7 +4667,7 @@
         <v>735</v>
       </c>
       <c r="W29" s="24" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.15">
@@ -4675,13 +4675,13 @@
         <v>13010207</v>
       </c>
       <c r="B30" s="25" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C30" s="15">
         <v>2</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E30" s="15">
         <v>15</v>
@@ -4691,7 +4691,7 @@
       </c>
       <c r="G30" s="15"/>
       <c r="H30" s="15" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I30" s="13">
         <v>1</v>
@@ -4707,13 +4707,13 @@
       </c>
       <c r="Q30" s="15"/>
       <c r="R30" s="13" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="S30" s="13" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="T30" s="13" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="U30" s="13">
         <v>737</v>
@@ -4722,7 +4722,7 @@
         <v>785</v>
       </c>
       <c r="W30" s="24" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.15">
@@ -4730,13 +4730,13 @@
         <v>13010208</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C31" s="15">
         <v>2</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E31" s="15">
         <v>15</v>
@@ -4745,10 +4745,10 @@
         <v>13010201</v>
       </c>
       <c r="G31" s="15" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H31" s="15" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I31" s="13">
         <v>1</v>
@@ -4766,13 +4766,13 @@
       <c r="P31" s="15"/>
       <c r="Q31" s="15"/>
       <c r="R31" s="13" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="S31" s="13" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="T31" s="15" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="U31" s="19">
         <v>894</v>
@@ -4781,7 +4781,7 @@
         <v>679</v>
       </c>
       <c r="W31" s="24" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.15">
@@ -4789,13 +4789,13 @@
         <v>13010209</v>
       </c>
       <c r="B32" s="25" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C32" s="15">
         <v>2</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E32" s="15">
         <v>15</v>
@@ -4804,10 +4804,10 @@
         <v>13010201</v>
       </c>
       <c r="G32" s="20" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H32" s="20" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="I32" s="13">
         <v>1</v>
@@ -4823,13 +4823,13 @@
       <c r="P32" s="15"/>
       <c r="Q32" s="16"/>
       <c r="R32" s="20" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="S32" s="20" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="T32" s="16" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="U32" s="19">
         <v>984</v>
@@ -4838,7 +4838,7 @@
         <v>734</v>
       </c>
       <c r="W32" s="24" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.15">
@@ -4852,7 +4852,7 @@
         <v>2</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E33" s="13">
         <v>14</v>
@@ -4861,10 +4861,10 @@
         <v>13010006</v>
       </c>
       <c r="G33" s="13" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H33" s="13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I33" s="13">
         <v>1</v>
@@ -4897,7 +4897,7 @@
         <v>505</v>
       </c>
       <c r="W33" s="24" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.15">
@@ -4911,7 +4911,7 @@
         <v>2</v>
       </c>
       <c r="D34" s="20" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E34" s="13">
         <v>10</v>
@@ -4920,10 +4920,10 @@
         <v>13010006</v>
       </c>
       <c r="G34" s="13" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H34" s="13" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I34" s="13">
         <v>1</v>
@@ -4956,7 +4956,7 @@
         <v>527</v>
       </c>
       <c r="W34" s="24" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.15">
@@ -4970,7 +4970,7 @@
         <v>2</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E35" s="13">
         <v>12</v>
@@ -4979,7 +4979,7 @@
         <v>13010006</v>
       </c>
       <c r="G35" s="13" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H35" s="13" t="s">
         <v>135</v>
@@ -5015,7 +5015,7 @@
         <v>373</v>
       </c>
       <c r="W35" s="24" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.15">
@@ -5054,7 +5054,7 @@
         <v>114</v>
       </c>
       <c r="S36" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="T36" s="13"/>
       <c r="U36" s="13"/>
@@ -5080,7 +5080,7 @@
       </c>
       <c r="G37" s="13"/>
       <c r="H37" s="20" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="I37" s="13"/>
       <c r="J37" s="13"/>
@@ -5095,7 +5095,7 @@
         <v>115</v>
       </c>
       <c r="S37" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="T37" s="13"/>
       <c r="U37" s="13"/>
@@ -5120,10 +5120,10 @@
         <v>13010007</v>
       </c>
       <c r="G38" s="13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H38" s="13" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I38" s="13"/>
       <c r="J38" s="13"/>
@@ -5138,7 +5138,7 @@
         <v>120</v>
       </c>
       <c r="S38" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="T38" s="13"/>
       <c r="U38" s="13"/>
@@ -5179,7 +5179,7 @@
         <v>124</v>
       </c>
       <c r="S39" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="T39" s="13"/>
       <c r="U39" s="13"/>
@@ -5218,7 +5218,7 @@
         <v>121</v>
       </c>
       <c r="S40" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="T40" s="13"/>
       <c r="U40" s="13"/>
@@ -5243,10 +5243,10 @@
         <v>13010004</v>
       </c>
       <c r="G41" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H41" s="13" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I41" s="13"/>
       <c r="J41" s="13"/>
@@ -5261,7 +5261,7 @@
         <v>141</v>
       </c>
       <c r="S41" s="13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="T41" s="13"/>
       <c r="U41" s="13"/>
@@ -5286,10 +5286,10 @@
         <v>13010004</v>
       </c>
       <c r="G42" s="20" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="H42" s="13" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I42" s="13"/>
       <c r="J42" s="13"/>
@@ -5304,7 +5304,7 @@
         <v>131</v>
       </c>
       <c r="S42" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="T42" s="13"/>
       <c r="U42" s="13"/>
@@ -5328,11 +5328,11 @@
       <c r="F43" s="13">
         <v>13010004</v>
       </c>
-      <c r="G43" s="13" t="s">
-        <v>147</v>
+      <c r="G43" s="20" t="s">
+        <v>270</v>
       </c>
       <c r="H43" s="13" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I43" s="13"/>
       <c r="J43" s="13"/>
@@ -5347,7 +5347,7 @@
         <v>132</v>
       </c>
       <c r="S43" s="13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="T43" s="13"/>
       <c r="U43" s="13"/>
@@ -5359,7 +5359,7 @@
         <v>13020031</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C44" s="13">
         <v>3</v>
@@ -5383,10 +5383,10 @@
       <c r="P44" s="15"/>
       <c r="Q44" s="15"/>
       <c r="R44" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="S44" s="15" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="T44" s="15"/>
       <c r="U44" s="15"/>
@@ -5398,7 +5398,7 @@
         <v>13020032</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C45" s="13">
         <v>3</v>
@@ -5422,10 +5422,10 @@
       <c r="P45" s="15"/>
       <c r="Q45" s="15"/>
       <c r="R45" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="S45" s="15" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="T45" s="15"/>
       <c r="U45" s="15"/>
@@ -5437,7 +5437,7 @@
         <v>13020033</v>
       </c>
       <c r="B46" s="17" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C46" s="13">
         <v>3</v>
@@ -5461,10 +5461,10 @@
       <c r="P46" s="15"/>
       <c r="Q46" s="15"/>
       <c r="R46" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="S46" s="15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="T46" s="19"/>
       <c r="U46" s="19"/>
@@ -5476,7 +5476,7 @@
         <v>13020034</v>
       </c>
       <c r="B47" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C47" s="13">
         <v>3</v>
@@ -5500,10 +5500,10 @@
       <c r="P47" s="15"/>
       <c r="Q47" s="15"/>
       <c r="R47" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="S47" s="15" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="T47" s="19"/>
       <c r="U47" s="19"/>
@@ -5515,7 +5515,7 @@
         <v>13020035</v>
       </c>
       <c r="B48" s="17" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C48" s="13">
         <v>3</v>
@@ -5539,10 +5539,10 @@
       <c r="P48" s="15"/>
       <c r="Q48" s="15"/>
       <c r="R48" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="S48" s="15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="T48" s="19"/>
       <c r="U48" s="19"/>

</xml_diff>

<commit_message>
add a drop rate
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Scene.xlsx
+++ b/ConfigData/Xlsx/Scene.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="277">
   <si>
     <t>村外小屋</t>
   </si>
@@ -1020,6 +1020,34 @@
   </si>
   <si>
     <t>colorpool;1|barn;1|portal;1|zookeeper;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>温度</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Temperature</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>湿度</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Humitity</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>高度</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Altitude</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1248,7 +1276,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="42">
+  <fills count="46">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1482,6 +1510,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -1758,7 +1810,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1847,6 +1899,24 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="40" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="42" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="42" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="43" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="43" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="44" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1894,7 +1964,115 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="29">
+  <dxfs count="32">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2584,27 +2762,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2619,35 +2776,38 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A3:W48" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24" tableBorderDxfId="23">
-  <autoFilter ref="A3:W48" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState ref="A4:W48">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A3:Z48" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30" tableBorderDxfId="29">
+  <autoFilter ref="A3:Z48" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState ref="A4:Z48">
     <sortCondition ref="A3:A48"/>
   </sortState>
-  <tableColumns count="23">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="21"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Type" dataDxfId="20"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Sector" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Level" dataDxfId="18"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="ReviveScene" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Quest" dataDxfId="16"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="QuestRandom" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="QPortal" dataDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="QCardChange" dataDxfId="13"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="QPiece" dataDxfId="12"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="QMerchant" dataDxfId="11"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="QDoctor" dataDxfId="10"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="QAngel" dataDxfId="9"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="QWheel" dataDxfId="8"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="QRes" dataDxfId="7"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Func" dataDxfId="6"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Url" dataDxfId="5"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="TilePath" dataDxfId="4"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Icon" dataDxfId="3"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="IconX" dataDxfId="2"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="IconY" dataDxfId="1"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="IconColor" dataDxfId="0"/>
+  <tableColumns count="26">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="27"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Type" dataDxfId="26"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Sector" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Level" dataDxfId="24"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="ReviveScene" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Quest" dataDxfId="22"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="QuestRandom" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="QPortal" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="QCardChange" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="QPiece" dataDxfId="18"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="QMerchant" dataDxfId="17"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="QDoctor" dataDxfId="16"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="QAngel" dataDxfId="15"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="QWheel" dataDxfId="14"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="QRes" dataDxfId="13"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Func" dataDxfId="12"/>
+    <tableColumn id="19" xr3:uid="{C4DE9876-761E-4F8F-AC05-98A2EEB0890C}" name="Temperature" dataDxfId="5"/>
+    <tableColumn id="23" xr3:uid="{CCCD053A-EDF9-4438-A6AA-6422F20485C6}" name="Humitity" dataDxfId="4"/>
+    <tableColumn id="26" xr3:uid="{C17F5093-27F2-476C-8B65-5FE7F10D25E9}" name="Altitude" dataDxfId="0"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Url" dataDxfId="11"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="TilePath" dataDxfId="10"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Icon" dataDxfId="9"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="IconX" dataDxfId="8"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="IconY" dataDxfId="7"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="IconColor" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2974,10 +3134,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W48"/>
+  <dimension ref="A1:Z48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="R44" sqref="R44:T48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2992,14 +3152,15 @@
     <col min="8" max="8" width="23.625" style="5" customWidth="1"/>
     <col min="9" max="16" width="3.125" style="5" customWidth="1"/>
     <col min="17" max="17" width="6.625" style="5" customWidth="1"/>
-    <col min="18" max="18" width="9.75" style="5" customWidth="1"/>
-    <col min="19" max="19" width="9.5" style="5" customWidth="1"/>
-    <col min="20" max="20" width="7.25" style="5" customWidth="1"/>
-    <col min="21" max="23" width="6" style="5" customWidth="1"/>
-    <col min="24" max="16384" width="9" style="5"/>
+    <col min="18" max="20" width="4.125" style="5" customWidth="1"/>
+    <col min="21" max="21" width="9.75" style="5" customWidth="1"/>
+    <col min="22" max="22" width="9.5" style="5" customWidth="1"/>
+    <col min="23" max="23" width="7.25" style="5" customWidth="1"/>
+    <col min="24" max="26" width="6" style="5" customWidth="1"/>
+    <col min="27" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="60" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:26" ht="60" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -3051,26 +3212,35 @@
       <c r="Q1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="32" t="s">
+        <v>270</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="T1" s="30" t="s">
+        <v>275</v>
+      </c>
+      <c r="U1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
         <v>13</v>
       </c>
@@ -3122,26 +3292,35 @@
       <c r="Q2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="R2" s="7" t="s">
+      <c r="R2" s="33" t="s">
+        <v>271</v>
+      </c>
+      <c r="S2" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="T2" s="31" t="s">
+        <v>271</v>
+      </c>
+      <c r="U2" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="S2" s="7" t="s">
+      <c r="V2" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="T2" s="7" t="s">
+      <c r="W2" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="U2" s="7" t="s">
+      <c r="X2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="V2" s="9" t="s">
+      <c r="Y2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="W2" s="9" t="s">
+      <c r="Z2" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A3" s="10" t="s">
         <v>20</v>
       </c>
@@ -3193,26 +3372,35 @@
       <c r="Q3" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="R3" s="10" t="s">
+      <c r="R3" s="34" t="s">
+        <v>272</v>
+      </c>
+      <c r="S3" s="23" t="s">
+        <v>274</v>
+      </c>
+      <c r="T3" s="35" t="s">
+        <v>276</v>
+      </c>
+      <c r="U3" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="S3" s="10" t="s">
+      <c r="V3" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="T3" s="10" t="s">
+      <c r="W3" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="U3" s="10" t="s">
+      <c r="X3" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="V3" s="10" t="s">
+      <c r="Y3" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="W3" s="23" t="s">
+      <c r="Z3" s="23" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A4" s="12">
         <v>13010001</v>
       </c>
@@ -3248,26 +3436,35 @@
       <c r="O4" s="13"/>
       <c r="P4" s="13"/>
       <c r="Q4" s="13"/>
-      <c r="R4" s="13" t="s">
+      <c r="R4" s="13">
+        <v>3</v>
+      </c>
+      <c r="S4" s="13">
+        <v>2</v>
+      </c>
+      <c r="T4" s="13">
+        <v>2</v>
+      </c>
+      <c r="U4" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="S4" s="13" t="s">
+      <c r="V4" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="T4" s="13" t="s">
+      <c r="W4" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="U4" s="13">
+      <c r="X4" s="13">
         <v>1348</v>
       </c>
-      <c r="V4" s="13">
+      <c r="Y4" s="13">
         <v>611</v>
       </c>
-      <c r="W4" s="24" t="s">
+      <c r="Z4" s="24" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A5" s="12">
         <v>13010002</v>
       </c>
@@ -3307,26 +3504,35 @@
       <c r="O5" s="13"/>
       <c r="P5" s="13"/>
       <c r="Q5" s="13"/>
-      <c r="R5" s="13" t="s">
+      <c r="R5" s="13">
+        <v>2</v>
+      </c>
+      <c r="S5" s="13">
+        <v>3</v>
+      </c>
+      <c r="T5" s="13">
+        <v>2</v>
+      </c>
+      <c r="U5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="S5" s="13" t="s">
+      <c r="V5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="T5" s="13" t="s">
+      <c r="W5" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="U5" s="13">
+      <c r="X5" s="13">
         <v>1279</v>
       </c>
-      <c r="V5" s="13">
+      <c r="Y5" s="13">
         <v>571</v>
       </c>
-      <c r="W5" s="24" t="s">
+      <c r="Z5" s="24" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A6" s="12">
         <v>13010003</v>
       </c>
@@ -3362,26 +3568,35 @@
       <c r="O6" s="13"/>
       <c r="P6" s="13"/>
       <c r="Q6" s="13"/>
-      <c r="R6" s="13" t="s">
+      <c r="R6" s="13">
+        <v>3</v>
+      </c>
+      <c r="S6" s="13">
+        <v>3</v>
+      </c>
+      <c r="T6" s="13">
+        <v>2</v>
+      </c>
+      <c r="U6" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="S6" s="13" t="s">
+      <c r="V6" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="T6" s="13" t="s">
+      <c r="W6" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="U6" s="13">
+      <c r="X6" s="13">
         <v>1251</v>
       </c>
-      <c r="V6" s="13">
+      <c r="Y6" s="13">
         <v>432</v>
       </c>
-      <c r="W6" s="24" t="s">
+      <c r="Z6" s="24" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A7" s="12">
         <v>13010004</v>
       </c>
@@ -3419,26 +3634,35 @@
       <c r="O7" s="13"/>
       <c r="P7" s="13"/>
       <c r="Q7" s="13"/>
-      <c r="R7" s="13" t="s">
+      <c r="R7" s="13">
+        <v>3</v>
+      </c>
+      <c r="S7" s="13">
+        <v>2</v>
+      </c>
+      <c r="T7" s="13">
+        <v>1</v>
+      </c>
+      <c r="U7" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="S7" s="13" t="s">
+      <c r="V7" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="T7" s="13" t="s">
+      <c r="W7" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="U7" s="13">
+      <c r="X7" s="13">
         <v>1148</v>
       </c>
-      <c r="V7" s="13">
+      <c r="Y7" s="13">
         <v>351</v>
       </c>
-      <c r="W7" s="24" t="s">
+      <c r="Z7" s="24" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A8" s="12">
         <v>13010005</v>
       </c>
@@ -3476,26 +3700,35 @@
       <c r="O8" s="13"/>
       <c r="P8" s="13"/>
       <c r="Q8" s="13"/>
-      <c r="R8" s="13" t="s">
+      <c r="R8" s="13">
+        <v>2</v>
+      </c>
+      <c r="S8" s="13">
+        <v>2</v>
+      </c>
+      <c r="T8" s="13">
+        <v>5</v>
+      </c>
+      <c r="U8" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="S8" s="13" t="s">
+      <c r="V8" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="T8" s="13" t="s">
+      <c r="W8" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="U8" s="13">
+      <c r="X8" s="13">
         <v>1386</v>
       </c>
-      <c r="V8" s="13">
+      <c r="Y8" s="13">
         <v>339</v>
       </c>
-      <c r="W8" s="24" t="s">
+      <c r="Z8" s="24" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A9" s="12">
         <v>13010006</v>
       </c>
@@ -3525,26 +3758,35 @@
       <c r="O9" s="13"/>
       <c r="P9" s="13"/>
       <c r="Q9" s="13"/>
-      <c r="R9" s="13" t="s">
+      <c r="R9" s="13">
+        <v>3</v>
+      </c>
+      <c r="S9" s="13">
+        <v>3</v>
+      </c>
+      <c r="T9" s="13">
+        <v>2</v>
+      </c>
+      <c r="U9" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="S9" s="13" t="s">
+      <c r="V9" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="T9" s="13" t="s">
+      <c r="W9" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="U9" s="13">
+      <c r="X9" s="13">
         <v>1232</v>
       </c>
-      <c r="V9" s="13">
+      <c r="Y9" s="13">
         <v>506</v>
       </c>
-      <c r="W9" s="24" t="s">
+      <c r="Z9" s="24" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A10" s="12">
         <v>13010007</v>
       </c>
@@ -3584,26 +3826,35 @@
         <v>1</v>
       </c>
       <c r="Q10" s="13"/>
-      <c r="R10" s="13" t="s">
+      <c r="R10" s="13">
+        <v>2</v>
+      </c>
+      <c r="S10" s="13">
+        <v>4</v>
+      </c>
+      <c r="T10" s="13">
+        <v>2</v>
+      </c>
+      <c r="U10" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="S10" s="13" t="s">
+      <c r="V10" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="T10" s="13" t="s">
+      <c r="W10" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="U10" s="13">
+      <c r="X10" s="13">
         <v>1431</v>
       </c>
-      <c r="V10" s="13">
+      <c r="Y10" s="13">
         <v>440</v>
       </c>
-      <c r="W10" s="24" t="s">
+      <c r="Z10" s="24" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A11" s="12">
         <v>13010008</v>
       </c>
@@ -3641,26 +3892,35 @@
       </c>
       <c r="P11" s="13"/>
       <c r="Q11" s="13"/>
-      <c r="R11" s="13" t="s">
+      <c r="R11" s="13">
+        <v>1</v>
+      </c>
+      <c r="S11" s="13">
+        <v>3</v>
+      </c>
+      <c r="T11" s="13">
+        <v>5</v>
+      </c>
+      <c r="U11" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="S11" s="13" t="s">
+      <c r="V11" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="T11" s="13" t="s">
+      <c r="W11" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="U11" s="13">
+      <c r="X11" s="13">
         <v>1250</v>
       </c>
-      <c r="V11" s="13">
+      <c r="Y11" s="13">
         <v>338</v>
       </c>
-      <c r="W11" s="24" t="s">
+      <c r="Z11" s="24" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A12" s="12">
         <v>13010009</v>
       </c>
@@ -3700,26 +3960,35 @@
       <c r="O12" s="13"/>
       <c r="P12" s="13"/>
       <c r="Q12" s="13"/>
-      <c r="R12" s="13" t="s">
+      <c r="R12" s="13">
+        <v>3</v>
+      </c>
+      <c r="S12" s="13">
+        <v>3</v>
+      </c>
+      <c r="T12" s="13">
+        <v>2</v>
+      </c>
+      <c r="U12" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="S12" s="13" t="s">
+      <c r="V12" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="T12" s="13" t="s">
+      <c r="W12" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="U12" s="13">
+      <c r="X12" s="13">
         <v>1332</v>
       </c>
-      <c r="V12" s="13">
+      <c r="Y12" s="13">
         <v>484</v>
       </c>
-      <c r="W12" s="24" t="s">
+      <c r="Z12" s="24" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A13" s="12">
         <v>13010010</v>
       </c>
@@ -3755,20 +4024,29 @@
       <c r="O13" s="15"/>
       <c r="P13" s="15"/>
       <c r="Q13" s="15"/>
-      <c r="R13" s="15" t="s">
+      <c r="R13" s="13">
+        <v>2</v>
+      </c>
+      <c r="S13" s="13">
+        <v>2</v>
+      </c>
+      <c r="T13" s="13">
+        <v>3</v>
+      </c>
+      <c r="U13" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="S13" s="15" t="s">
+      <c r="V13" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="T13" s="15"/>
-      <c r="U13" s="15"/>
-      <c r="V13" s="15"/>
-      <c r="W13" s="24" t="s">
+      <c r="W13" s="15"/>
+      <c r="X13" s="15"/>
+      <c r="Y13" s="15"/>
+      <c r="Z13" s="24" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A14" s="27">
         <v>13010101</v>
       </c>
@@ -3798,26 +4076,35 @@
       <c r="O14" s="13"/>
       <c r="P14" s="13"/>
       <c r="Q14" s="13"/>
-      <c r="R14" s="13" t="s">
+      <c r="R14" s="13">
+        <v>2</v>
+      </c>
+      <c r="S14" s="13">
+        <v>3</v>
+      </c>
+      <c r="T14" s="13">
+        <v>2</v>
+      </c>
+      <c r="U14" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="S14" s="13" t="s">
+      <c r="V14" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="T14" s="13" t="s">
+      <c r="W14" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="U14" s="13">
+      <c r="X14" s="13">
         <v>894</v>
       </c>
-      <c r="V14" s="13">
+      <c r="Y14" s="13">
         <v>509</v>
       </c>
-      <c r="W14" s="24" t="s">
+      <c r="Z14" s="24" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A15" s="27">
         <v>13010102</v>
       </c>
@@ -3855,26 +4142,35 @@
       <c r="O15" s="13"/>
       <c r="P15" s="13"/>
       <c r="Q15" s="13"/>
-      <c r="R15" s="13" t="s">
+      <c r="R15" s="13">
+        <v>2</v>
+      </c>
+      <c r="S15" s="13">
+        <v>5</v>
+      </c>
+      <c r="T15" s="13">
+        <v>2</v>
+      </c>
+      <c r="U15" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="S15" s="13" t="s">
+      <c r="V15" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="T15" s="13" t="s">
+      <c r="W15" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="U15" s="13">
+      <c r="X15" s="13">
         <v>1040</v>
       </c>
-      <c r="V15" s="13">
+      <c r="Y15" s="13">
         <v>538</v>
       </c>
-      <c r="W15" s="24" t="s">
+      <c r="Z15" s="24" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A16" s="27">
         <v>13010103</v>
       </c>
@@ -3912,26 +4208,35 @@
       </c>
       <c r="P16" s="13"/>
       <c r="Q16" s="13"/>
-      <c r="R16" s="13" t="s">
+      <c r="R16" s="13">
+        <v>3</v>
+      </c>
+      <c r="S16" s="13">
+        <v>3</v>
+      </c>
+      <c r="T16" s="13">
+        <v>2</v>
+      </c>
+      <c r="U16" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="S16" s="13" t="s">
+      <c r="V16" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="T16" s="13" t="s">
+      <c r="W16" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="U16" s="13">
+      <c r="X16" s="13">
         <v>1213</v>
       </c>
-      <c r="V16" s="13">
+      <c r="Y16" s="13">
         <v>655</v>
       </c>
-      <c r="W16" s="24" t="s">
+      <c r="Z16" s="24" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A17" s="27">
         <v>13010104</v>
       </c>
@@ -3969,26 +4274,35 @@
       <c r="O17" s="13"/>
       <c r="P17" s="13"/>
       <c r="Q17" s="13"/>
-      <c r="R17" s="13" t="s">
+      <c r="R17" s="13">
+        <v>2</v>
+      </c>
+      <c r="S17" s="13">
+        <v>4</v>
+      </c>
+      <c r="T17" s="13">
+        <v>2</v>
+      </c>
+      <c r="U17" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="S17" s="13" t="s">
+      <c r="V17" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="T17" s="13" t="s">
+      <c r="W17" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="U17" s="13">
+      <c r="X17" s="13">
         <v>1149</v>
       </c>
-      <c r="V17" s="13">
+      <c r="Y17" s="13">
         <v>584</v>
       </c>
-      <c r="W17" s="24" t="s">
+      <c r="Z17" s="24" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A18" s="27">
         <v>13010105</v>
       </c>
@@ -4026,26 +4340,35 @@
       <c r="O18" s="13"/>
       <c r="P18" s="13"/>
       <c r="Q18" s="13"/>
-      <c r="R18" s="13" t="s">
+      <c r="R18" s="13">
+        <v>2</v>
+      </c>
+      <c r="S18" s="13">
+        <v>3</v>
+      </c>
+      <c r="T18" s="13">
+        <v>2</v>
+      </c>
+      <c r="U18" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="S18" s="13" t="s">
+      <c r="V18" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="T18" s="13" t="s">
+      <c r="W18" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="U18" s="13">
+      <c r="X18" s="13">
         <v>840</v>
       </c>
-      <c r="V18" s="13">
+      <c r="Y18" s="13">
         <v>444</v>
       </c>
-      <c r="W18" s="24" t="s">
+      <c r="Z18" s="24" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A19" s="27">
         <v>13010106</v>
       </c>
@@ -4083,26 +4406,35 @@
       <c r="O19" s="13"/>
       <c r="P19" s="13"/>
       <c r="Q19" s="13"/>
-      <c r="R19" s="13" t="s">
+      <c r="R19" s="13">
+        <v>3</v>
+      </c>
+      <c r="S19" s="13">
+        <v>4</v>
+      </c>
+      <c r="T19" s="13">
+        <v>2</v>
+      </c>
+      <c r="U19" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="S19" s="13" t="s">
+      <c r="V19" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="T19" s="13" t="s">
+      <c r="W19" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="U19" s="13">
+      <c r="X19" s="13">
         <v>1067</v>
       </c>
-      <c r="V19" s="13">
+      <c r="Y19" s="13">
         <v>445</v>
       </c>
-      <c r="W19" s="24" t="s">
+      <c r="Z19" s="24" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A20" s="27">
         <v>13010107</v>
       </c>
@@ -4142,26 +4474,35 @@
         <v>1</v>
       </c>
       <c r="Q20" s="16"/>
-      <c r="R20" s="13" t="s">
+      <c r="R20" s="13">
+        <v>3</v>
+      </c>
+      <c r="S20" s="13">
+        <v>3</v>
+      </c>
+      <c r="T20" s="13">
+        <v>2</v>
+      </c>
+      <c r="U20" s="13" t="s">
         <v>218</v>
       </c>
-      <c r="S20" s="13" t="s">
+      <c r="V20" s="13" t="s">
         <v>218</v>
       </c>
-      <c r="T20" s="13" t="s">
+      <c r="W20" s="13" t="s">
         <v>202</v>
       </c>
-      <c r="U20" s="16">
+      <c r="X20" s="16">
         <v>850</v>
       </c>
-      <c r="V20" s="16">
+      <c r="Y20" s="16">
         <v>589</v>
       </c>
-      <c r="W20" s="24" t="s">
+      <c r="Z20" s="24" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A21" s="27">
         <v>13010108</v>
       </c>
@@ -4199,26 +4540,35 @@
       <c r="O21" s="15"/>
       <c r="P21" s="15"/>
       <c r="Q21" s="16"/>
-      <c r="R21" s="13" t="s">
+      <c r="R21" s="13">
+        <v>3</v>
+      </c>
+      <c r="S21" s="13">
+        <v>3</v>
+      </c>
+      <c r="T21" s="13">
+        <v>3</v>
+      </c>
+      <c r="U21" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="S21" s="13" t="s">
+      <c r="V21" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="T21" s="16" t="s">
+      <c r="W21" s="16" t="s">
         <v>206</v>
       </c>
-      <c r="U21" s="13">
+      <c r="X21" s="13">
         <v>682</v>
       </c>
-      <c r="V21" s="13">
+      <c r="Y21" s="13">
         <v>545</v>
       </c>
-      <c r="W21" s="24" t="s">
+      <c r="Z21" s="24" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A22" s="27">
         <v>13010109</v>
       </c>
@@ -4256,26 +4606,35 @@
       <c r="O22" s="15"/>
       <c r="P22" s="15"/>
       <c r="Q22" s="16"/>
-      <c r="R22" s="13" t="s">
+      <c r="R22" s="13">
+        <v>3</v>
+      </c>
+      <c r="S22" s="13">
+        <v>3</v>
+      </c>
+      <c r="T22" s="13">
+        <v>3</v>
+      </c>
+      <c r="U22" s="13" t="s">
         <v>244</v>
       </c>
-      <c r="S22" s="20" t="s">
+      <c r="V22" s="20" t="s">
         <v>245</v>
       </c>
-      <c r="T22" s="16" t="s">
+      <c r="W22" s="16" t="s">
         <v>241</v>
       </c>
-      <c r="U22" s="16">
+      <c r="X22" s="16">
         <v>643</v>
       </c>
-      <c r="V22" s="16">
+      <c r="Y22" s="16">
         <v>455</v>
       </c>
-      <c r="W22" s="24" t="s">
+      <c r="Z22" s="24" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A23" s="27">
         <v>13010110</v>
       </c>
@@ -4315,26 +4674,35 @@
         <v>1</v>
       </c>
       <c r="Q23" s="16"/>
-      <c r="R23" s="20" t="s">
+      <c r="R23" s="13">
+        <v>2</v>
+      </c>
+      <c r="S23" s="13">
+        <v>4</v>
+      </c>
+      <c r="T23" s="13">
+        <v>3</v>
+      </c>
+      <c r="U23" s="20" t="s">
         <v>246</v>
       </c>
-      <c r="S23" s="20" t="s">
+      <c r="V23" s="20" t="s">
         <v>246</v>
       </c>
-      <c r="T23" s="16" t="s">
+      <c r="W23" s="16" t="s">
         <v>242</v>
       </c>
-      <c r="U23" s="16">
+      <c r="X23" s="16">
         <v>720</v>
       </c>
-      <c r="V23" s="16">
+      <c r="Y23" s="16">
         <v>375</v>
       </c>
-      <c r="W23" s="24" t="s">
+      <c r="Z23" s="24" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A24" s="25">
         <v>13010201</v>
       </c>
@@ -4364,26 +4732,35 @@
       <c r="O24" s="15"/>
       <c r="P24" s="15"/>
       <c r="Q24" s="16"/>
-      <c r="R24" s="13" t="s">
+      <c r="R24" s="13">
+        <v>4</v>
+      </c>
+      <c r="S24" s="13">
+        <v>2</v>
+      </c>
+      <c r="T24" s="13">
+        <v>2</v>
+      </c>
+      <c r="U24" s="13" t="s">
         <v>216</v>
       </c>
-      <c r="S24" s="13" t="s">
+      <c r="V24" s="13" t="s">
         <v>216</v>
       </c>
-      <c r="T24" s="16" t="s">
+      <c r="W24" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="U24" s="13">
+      <c r="X24" s="13">
         <v>807</v>
       </c>
-      <c r="V24" s="13">
+      <c r="Y24" s="13">
         <v>720</v>
       </c>
-      <c r="W24" s="24" t="s">
+      <c r="Z24" s="24" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A25" s="25">
         <v>13010202</v>
       </c>
@@ -4421,26 +4798,35 @@
       <c r="O25" s="15"/>
       <c r="P25" s="15"/>
       <c r="Q25" s="15"/>
-      <c r="R25" s="13" t="s">
+      <c r="R25" s="13">
+        <v>4</v>
+      </c>
+      <c r="S25" s="13">
+        <v>1</v>
+      </c>
+      <c r="T25" s="13">
+        <v>3</v>
+      </c>
+      <c r="U25" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="S25" s="13" t="s">
+      <c r="V25" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="T25" s="15" t="s">
+      <c r="W25" s="15" t="s">
         <v>196</v>
       </c>
-      <c r="U25" s="15">
+      <c r="X25" s="15">
         <v>974</v>
       </c>
-      <c r="V25" s="15">
+      <c r="Y25" s="15">
         <v>594</v>
       </c>
-      <c r="W25" s="24" t="s">
+      <c r="Z25" s="24" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A26" s="25">
         <v>13010203</v>
       </c>
@@ -4478,26 +4864,35 @@
         <v>1</v>
       </c>
       <c r="Q26" s="15"/>
-      <c r="R26" s="13" t="s">
+      <c r="R26" s="13">
+        <v>4</v>
+      </c>
+      <c r="S26" s="13">
+        <v>1</v>
+      </c>
+      <c r="T26" s="13">
+        <v>3</v>
+      </c>
+      <c r="U26" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="S26" s="13" t="s">
+      <c r="V26" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="T26" s="15" t="s">
+      <c r="W26" s="15" t="s">
         <v>197</v>
       </c>
-      <c r="U26" s="15">
+      <c r="X26" s="15">
         <v>1080</v>
       </c>
-      <c r="V26" s="15">
+      <c r="Y26" s="15">
         <v>720</v>
       </c>
-      <c r="W26" s="24" t="s">
+      <c r="Z26" s="24" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A27" s="25">
         <v>13010204</v>
       </c>
@@ -4535,26 +4930,35 @@
       <c r="O27" s="15"/>
       <c r="P27" s="15"/>
       <c r="Q27" s="15"/>
-      <c r="R27" s="13" t="s">
+      <c r="R27" s="13">
+        <v>4</v>
+      </c>
+      <c r="S27" s="13">
+        <v>1</v>
+      </c>
+      <c r="T27" s="13">
+        <v>3</v>
+      </c>
+      <c r="U27" s="13" t="s">
         <v>223</v>
       </c>
-      <c r="S27" s="13" t="s">
+      <c r="V27" s="13" t="s">
         <v>223</v>
       </c>
-      <c r="T27" s="15" t="s">
+      <c r="W27" s="15" t="s">
         <v>199</v>
       </c>
-      <c r="U27" s="15">
+      <c r="X27" s="15">
         <v>1074</v>
       </c>
-      <c r="V27" s="15">
+      <c r="Y27" s="15">
         <v>630</v>
       </c>
-      <c r="W27" s="24" t="s">
+      <c r="Z27" s="24" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A28" s="25">
         <v>13010205</v>
       </c>
@@ -4590,26 +4994,35 @@
       <c r="O28" s="15"/>
       <c r="P28" s="15"/>
       <c r="Q28" s="16"/>
-      <c r="R28" s="20" t="s">
+      <c r="R28" s="13">
+        <v>4</v>
+      </c>
+      <c r="S28" s="13">
+        <v>1</v>
+      </c>
+      <c r="T28" s="13">
+        <v>2</v>
+      </c>
+      <c r="U28" s="20" t="s">
         <v>219</v>
       </c>
-      <c r="S28" s="20" t="s">
+      <c r="V28" s="20" t="s">
         <v>219</v>
       </c>
-      <c r="T28" s="16" t="s">
+      <c r="W28" s="16" t="s">
         <v>204</v>
       </c>
-      <c r="U28" s="13">
+      <c r="X28" s="13">
         <v>717</v>
       </c>
-      <c r="V28" s="13">
+      <c r="Y28" s="13">
         <v>655</v>
       </c>
-      <c r="W28" s="24" t="s">
+      <c r="Z28" s="24" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A29" s="25">
         <v>13010206</v>
       </c>
@@ -4647,26 +5060,35 @@
       <c r="O29" s="15"/>
       <c r="P29" s="15"/>
       <c r="Q29" s="16"/>
-      <c r="R29" s="20" t="s">
+      <c r="R29" s="13">
+        <v>4</v>
+      </c>
+      <c r="S29" s="13">
+        <v>1</v>
+      </c>
+      <c r="T29" s="13">
+        <v>2</v>
+      </c>
+      <c r="U29" s="20" t="s">
         <v>225</v>
       </c>
-      <c r="S29" s="20" t="s">
+      <c r="V29" s="20" t="s">
         <v>225</v>
       </c>
-      <c r="T29" s="16" t="s">
+      <c r="W29" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="U29" s="13">
+      <c r="X29" s="13">
         <v>637</v>
       </c>
-      <c r="V29" s="13">
+      <c r="Y29" s="13">
         <v>735</v>
       </c>
-      <c r="W29" s="24" t="s">
+      <c r="Z29" s="24" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A30" s="25">
         <v>13010207</v>
       </c>
@@ -4702,26 +5124,35 @@
         <v>1</v>
       </c>
       <c r="Q30" s="15"/>
-      <c r="R30" s="13" t="s">
+      <c r="R30" s="13">
+        <v>5</v>
+      </c>
+      <c r="S30" s="13">
+        <v>1</v>
+      </c>
+      <c r="T30" s="13">
+        <v>4</v>
+      </c>
+      <c r="U30" s="13" t="s">
         <v>224</v>
       </c>
-      <c r="S30" s="13" t="s">
+      <c r="V30" s="13" t="s">
         <v>224</v>
       </c>
-      <c r="T30" s="13" t="s">
+      <c r="W30" s="13" t="s">
         <v>207</v>
       </c>
-      <c r="U30" s="13">
+      <c r="X30" s="13">
         <v>737</v>
       </c>
-      <c r="V30" s="13">
+      <c r="Y30" s="13">
         <v>785</v>
       </c>
-      <c r="W30" s="24" t="s">
+      <c r="Z30" s="24" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A31" s="25">
         <v>13010208</v>
       </c>
@@ -4761,26 +5192,35 @@
       <c r="O31" s="15"/>
       <c r="P31" s="15"/>
       <c r="Q31" s="15"/>
-      <c r="R31" s="13" t="s">
+      <c r="R31" s="13">
+        <v>4</v>
+      </c>
+      <c r="S31" s="13">
+        <v>1</v>
+      </c>
+      <c r="T31" s="13">
+        <v>2</v>
+      </c>
+      <c r="U31" s="13" t="s">
         <v>217</v>
       </c>
-      <c r="S31" s="13" t="s">
+      <c r="V31" s="13" t="s">
         <v>217</v>
       </c>
-      <c r="T31" s="15" t="s">
+      <c r="W31" s="15" t="s">
         <v>200</v>
       </c>
-      <c r="U31" s="19">
+      <c r="X31" s="19">
         <v>894</v>
       </c>
-      <c r="V31" s="19">
+      <c r="Y31" s="19">
         <v>679</v>
       </c>
-      <c r="W31" s="24" t="s">
+      <c r="Z31" s="24" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A32" s="25">
         <v>13010209</v>
       </c>
@@ -4818,26 +5258,35 @@
       </c>
       <c r="P32" s="15"/>
       <c r="Q32" s="16"/>
-      <c r="R32" s="20" t="s">
+      <c r="R32" s="13">
+        <v>4</v>
+      </c>
+      <c r="S32" s="13">
+        <v>2</v>
+      </c>
+      <c r="T32" s="13">
+        <v>2</v>
+      </c>
+      <c r="U32" s="20" t="s">
         <v>226</v>
       </c>
-      <c r="S32" s="20" t="s">
+      <c r="V32" s="20" t="s">
         <v>226</v>
       </c>
-      <c r="T32" s="16" t="s">
+      <c r="W32" s="16" t="s">
         <v>201</v>
       </c>
-      <c r="U32" s="19">
+      <c r="X32" s="19">
         <v>984</v>
       </c>
-      <c r="V32" s="19">
+      <c r="Y32" s="19">
         <v>734</v>
       </c>
-      <c r="W32" s="24" t="s">
+      <c r="Z32" s="24" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A33" s="28">
         <v>13010301</v>
       </c>
@@ -4877,26 +5326,35 @@
       <c r="O33" s="13"/>
       <c r="P33" s="13"/>
       <c r="Q33" s="13"/>
-      <c r="R33" s="13" t="s">
+      <c r="R33" s="13">
+        <v>3</v>
+      </c>
+      <c r="S33" s="13">
+        <v>3</v>
+      </c>
+      <c r="T33" s="13">
+        <v>1</v>
+      </c>
+      <c r="U33" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="S33" s="13" t="s">
+      <c r="V33" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="T33" s="13" t="s">
+      <c r="W33" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="U33" s="21">
+      <c r="X33" s="21">
         <v>1550</v>
       </c>
-      <c r="V33" s="21">
+      <c r="Y33" s="21">
         <v>505</v>
       </c>
-      <c r="W33" s="24" t="s">
+      <c r="Z33" s="24" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A34" s="28">
         <v>13010302</v>
       </c>
@@ -4936,26 +5394,35 @@
       </c>
       <c r="P34" s="13"/>
       <c r="Q34" s="13"/>
-      <c r="R34" s="13" t="s">
+      <c r="R34" s="13">
+        <v>4</v>
+      </c>
+      <c r="S34" s="13">
+        <v>3</v>
+      </c>
+      <c r="T34" s="13">
+        <v>1</v>
+      </c>
+      <c r="U34" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="S34" s="13" t="s">
+      <c r="V34" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="T34" s="13" t="s">
+      <c r="W34" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="U34" s="21">
+      <c r="X34" s="21">
         <v>1441</v>
       </c>
-      <c r="V34" s="21">
+      <c r="Y34" s="21">
         <v>527</v>
       </c>
-      <c r="W34" s="24" t="s">
+      <c r="Z34" s="24" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A35" s="28">
         <v>13010303</v>
       </c>
@@ -4995,26 +5462,35 @@
         <v>1</v>
       </c>
       <c r="Q35" s="13"/>
-      <c r="R35" s="13" t="s">
+      <c r="R35" s="13">
+        <v>3</v>
+      </c>
+      <c r="S35" s="13">
+        <v>3</v>
+      </c>
+      <c r="T35" s="13">
+        <v>2</v>
+      </c>
+      <c r="U35" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="S35" s="13" t="s">
+      <c r="V35" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="T35" s="13" t="s">
+      <c r="W35" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="U35" s="21">
+      <c r="X35" s="21">
         <v>1574</v>
       </c>
-      <c r="V35" s="21">
+      <c r="Y35" s="21">
         <v>373</v>
       </c>
-      <c r="W35" s="24" t="s">
+      <c r="Z35" s="24" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A36" s="17">
         <v>13020001</v>
       </c>
@@ -5046,18 +5522,27 @@
       <c r="O36" s="13"/>
       <c r="P36" s="13"/>
       <c r="Q36" s="13"/>
-      <c r="R36" s="13" t="s">
+      <c r="R36" s="13">
+        <v>2</v>
+      </c>
+      <c r="S36" s="13">
+        <v>3</v>
+      </c>
+      <c r="T36" s="13">
+        <v>2</v>
+      </c>
+      <c r="U36" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="S36" s="13" t="s">
+      <c r="V36" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="T36" s="13"/>
-      <c r="U36" s="13"/>
-      <c r="V36" s="13"/>
-      <c r="W36" s="22"/>
+      <c r="W36" s="13"/>
+      <c r="X36" s="13"/>
+      <c r="Y36" s="13"/>
+      <c r="Z36" s="22"/>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A37" s="17">
         <v>13020002</v>
       </c>
@@ -5085,18 +5570,27 @@
       <c r="O37" s="13"/>
       <c r="P37" s="13"/>
       <c r="Q37" s="13"/>
-      <c r="R37" s="13" t="s">
+      <c r="R37" s="13">
+        <v>2</v>
+      </c>
+      <c r="S37" s="13">
+        <v>3</v>
+      </c>
+      <c r="T37" s="13">
+        <v>2</v>
+      </c>
+      <c r="U37" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="S37" s="13" t="s">
+      <c r="V37" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="T37" s="13"/>
-      <c r="U37" s="13"/>
-      <c r="V37" s="13"/>
-      <c r="W37" s="22"/>
+      <c r="W37" s="13"/>
+      <c r="X37" s="13"/>
+      <c r="Y37" s="13"/>
+      <c r="Z37" s="22"/>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A38" s="17">
         <v>13020011</v>
       </c>
@@ -5128,18 +5622,27 @@
       <c r="O38" s="13"/>
       <c r="P38" s="13"/>
       <c r="Q38" s="13"/>
-      <c r="R38" s="13" t="s">
+      <c r="R38" s="13">
+        <v>2</v>
+      </c>
+      <c r="S38" s="13">
+        <v>4</v>
+      </c>
+      <c r="T38" s="13">
+        <v>2</v>
+      </c>
+      <c r="U38" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="S38" s="13" t="s">
+      <c r="V38" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="T38" s="13"/>
-      <c r="U38" s="13"/>
-      <c r="V38" s="13"/>
-      <c r="W38" s="22"/>
+      <c r="W38" s="13"/>
+      <c r="X38" s="13"/>
+      <c r="Y38" s="13"/>
+      <c r="Z38" s="22"/>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A39" s="17">
         <v>13020012</v>
       </c>
@@ -5169,18 +5672,27 @@
       <c r="O39" s="13"/>
       <c r="P39" s="13"/>
       <c r="Q39" s="13"/>
-      <c r="R39" s="13" t="s">
+      <c r="R39" s="13">
+        <v>2</v>
+      </c>
+      <c r="S39" s="13">
+        <v>4</v>
+      </c>
+      <c r="T39" s="13">
+        <v>2</v>
+      </c>
+      <c r="U39" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="S39" s="13" t="s">
+      <c r="V39" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="T39" s="13"/>
-      <c r="U39" s="13"/>
-      <c r="V39" s="13"/>
-      <c r="W39" s="22"/>
+      <c r="W39" s="13"/>
+      <c r="X39" s="13"/>
+      <c r="Y39" s="13"/>
+      <c r="Z39" s="22"/>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A40" s="17">
         <v>13020013</v>
       </c>
@@ -5208,18 +5720,27 @@
       <c r="O40" s="13"/>
       <c r="P40" s="13"/>
       <c r="Q40" s="13"/>
-      <c r="R40" s="13" t="s">
+      <c r="R40" s="13">
+        <v>2</v>
+      </c>
+      <c r="S40" s="13">
+        <v>4</v>
+      </c>
+      <c r="T40" s="13">
+        <v>2</v>
+      </c>
+      <c r="U40" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="S40" s="13" t="s">
+      <c r="V40" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="T40" s="13"/>
-      <c r="U40" s="13"/>
-      <c r="V40" s="13"/>
-      <c r="W40" s="22"/>
+      <c r="W40" s="13"/>
+      <c r="X40" s="13"/>
+      <c r="Y40" s="13"/>
+      <c r="Z40" s="22"/>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A41" s="17">
         <v>13020021</v>
       </c>
@@ -5251,18 +5772,27 @@
       <c r="O41" s="13"/>
       <c r="P41" s="13"/>
       <c r="Q41" s="13"/>
-      <c r="R41" s="13" t="s">
+      <c r="R41" s="13">
+        <v>3</v>
+      </c>
+      <c r="S41" s="13">
+        <v>3</v>
+      </c>
+      <c r="T41" s="13">
+        <v>1</v>
+      </c>
+      <c r="U41" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="S41" s="13" t="s">
+      <c r="V41" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="T41" s="13"/>
-      <c r="U41" s="13"/>
-      <c r="V41" s="13"/>
-      <c r="W41" s="22"/>
+      <c r="W41" s="13"/>
+      <c r="X41" s="13"/>
+      <c r="Y41" s="13"/>
+      <c r="Z41" s="22"/>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A42" s="17">
         <v>13020022</v>
       </c>
@@ -5294,18 +5824,27 @@
       <c r="O42" s="13"/>
       <c r="P42" s="13"/>
       <c r="Q42" s="13"/>
-      <c r="R42" s="13" t="s">
+      <c r="R42" s="13">
+        <v>3</v>
+      </c>
+      <c r="S42" s="13">
+        <v>3</v>
+      </c>
+      <c r="T42" s="13">
+        <v>1</v>
+      </c>
+      <c r="U42" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="S42" s="13" t="s">
+      <c r="V42" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="T42" s="13"/>
-      <c r="U42" s="13"/>
-      <c r="V42" s="13"/>
-      <c r="W42" s="22"/>
+      <c r="W42" s="13"/>
+      <c r="X42" s="13"/>
+      <c r="Y42" s="13"/>
+      <c r="Z42" s="22"/>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A43" s="17">
         <v>13020023</v>
       </c>
@@ -5337,18 +5876,27 @@
       <c r="O43" s="13"/>
       <c r="P43" s="13"/>
       <c r="Q43" s="13"/>
-      <c r="R43" s="13" t="s">
+      <c r="R43" s="13">
+        <v>3</v>
+      </c>
+      <c r="S43" s="13">
+        <v>3</v>
+      </c>
+      <c r="T43" s="13">
+        <v>1</v>
+      </c>
+      <c r="U43" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="S43" s="13" t="s">
+      <c r="V43" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="T43" s="13"/>
-      <c r="U43" s="13"/>
-      <c r="V43" s="13"/>
-      <c r="W43" s="22"/>
+      <c r="W43" s="13"/>
+      <c r="X43" s="13"/>
+      <c r="Y43" s="13"/>
+      <c r="Z43" s="22"/>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A44" s="18">
         <v>13020031</v>
       </c>
@@ -5376,18 +5924,27 @@
       <c r="O44" s="15"/>
       <c r="P44" s="15"/>
       <c r="Q44" s="15"/>
-      <c r="R44" s="13" t="s">
+      <c r="R44" s="13">
+        <v>2</v>
+      </c>
+      <c r="S44" s="13">
+        <v>2</v>
+      </c>
+      <c r="T44" s="13">
+        <v>5</v>
+      </c>
+      <c r="U44" s="13" t="s">
         <v>169</v>
       </c>
-      <c r="S44" s="15" t="s">
+      <c r="V44" s="15" t="s">
         <v>174</v>
       </c>
-      <c r="T44" s="15"/>
-      <c r="U44" s="15"/>
-      <c r="V44" s="15"/>
-      <c r="W44" s="22"/>
+      <c r="W44" s="15"/>
+      <c r="X44" s="15"/>
+      <c r="Y44" s="15"/>
+      <c r="Z44" s="22"/>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A45" s="18">
         <v>13020032</v>
       </c>
@@ -5415,18 +5972,27 @@
       <c r="O45" s="15"/>
       <c r="P45" s="15"/>
       <c r="Q45" s="15"/>
-      <c r="R45" s="13" t="s">
+      <c r="R45" s="13">
+        <v>2</v>
+      </c>
+      <c r="S45" s="13">
+        <v>2</v>
+      </c>
+      <c r="T45" s="13">
+        <v>5</v>
+      </c>
+      <c r="U45" s="13" t="s">
         <v>169</v>
       </c>
-      <c r="S45" s="15" t="s">
+      <c r="V45" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="T45" s="15"/>
-      <c r="U45" s="15"/>
-      <c r="V45" s="15"/>
-      <c r="W45" s="22"/>
+      <c r="W45" s="15"/>
+      <c r="X45" s="15"/>
+      <c r="Y45" s="15"/>
+      <c r="Z45" s="22"/>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A46" s="18">
         <v>13020033</v>
       </c>
@@ -5454,18 +6020,27 @@
       <c r="O46" s="15"/>
       <c r="P46" s="15"/>
       <c r="Q46" s="15"/>
-      <c r="R46" s="13" t="s">
+      <c r="R46" s="13">
+        <v>2</v>
+      </c>
+      <c r="S46" s="13">
+        <v>2</v>
+      </c>
+      <c r="T46" s="13">
+        <v>5</v>
+      </c>
+      <c r="U46" s="13" t="s">
         <v>169</v>
       </c>
-      <c r="S46" s="15" t="s">
+      <c r="V46" s="15" t="s">
         <v>176</v>
       </c>
-      <c r="T46" s="19"/>
-      <c r="U46" s="19"/>
-      <c r="V46" s="19"/>
-      <c r="W46" s="22"/>
+      <c r="W46" s="19"/>
+      <c r="X46" s="19"/>
+      <c r="Y46" s="19"/>
+      <c r="Z46" s="22"/>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A47" s="18">
         <v>13020034</v>
       </c>
@@ -5493,18 +6068,27 @@
       <c r="O47" s="15"/>
       <c r="P47" s="15"/>
       <c r="Q47" s="15"/>
-      <c r="R47" s="13" t="s">
+      <c r="R47" s="13">
+        <v>2</v>
+      </c>
+      <c r="S47" s="13">
+        <v>2</v>
+      </c>
+      <c r="T47" s="13">
+        <v>5</v>
+      </c>
+      <c r="U47" s="13" t="s">
         <v>169</v>
       </c>
-      <c r="S47" s="15" t="s">
+      <c r="V47" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="T47" s="19"/>
-      <c r="U47" s="19"/>
-      <c r="V47" s="19"/>
-      <c r="W47" s="22"/>
+      <c r="W47" s="19"/>
+      <c r="X47" s="19"/>
+      <c r="Y47" s="19"/>
+      <c r="Z47" s="22"/>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A48" s="18">
         <v>13020035</v>
       </c>
@@ -5532,31 +6116,40 @@
       <c r="O48" s="15"/>
       <c r="P48" s="15"/>
       <c r="Q48" s="15"/>
-      <c r="R48" s="13" t="s">
+      <c r="R48" s="13">
+        <v>2</v>
+      </c>
+      <c r="S48" s="13">
+        <v>2</v>
+      </c>
+      <c r="T48" s="13">
+        <v>5</v>
+      </c>
+      <c r="U48" s="13" t="s">
         <v>169</v>
       </c>
-      <c r="S48" s="15" t="s">
+      <c r="V48" s="15" t="s">
         <v>178</v>
       </c>
-      <c r="T48" s="19"/>
-      <c r="U48" s="19"/>
-      <c r="V48" s="19"/>
-      <c r="W48" s="22"/>
+      <c r="W48" s="19"/>
+      <c r="X48" s="19"/>
+      <c r="Y48" s="19"/>
+      <c r="Z48" s="22"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="I4:P48">
-    <cfRule type="cellIs" dxfId="28" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4">
-    <cfRule type="cellIs" dxfId="27" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:H48">
-    <cfRule type="containsBlanks" dxfId="26" priority="5">
+    <cfRule type="containsBlanks" dxfId="1" priority="5">
       <formula>LEN(TRIM(G4))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
let the collect quest be in scene format
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Scene.xlsx
+++ b/ConfigData/Xlsx/Scene.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="Scene" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="285">
   <si>
     <t>村外小屋</t>
   </si>
@@ -320,14 +320,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>trees;3|mushroom;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>sewer;3|river;2|fortune;1|oldtree;1|poppyfield;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>小概率任务</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -352,10 +344,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>mushroom;1|hiddeway;1|swamp;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>portal;3|sandflow;2|manflower;3</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -518,10 +506,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>wolfnest;2|gamegamble;1|fishpool;2|sewer;3|river;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>forestfire;35|witchhome;10</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -534,22 +518,10 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>trees;3|grave;1|portal;1|oldtree;1|manflower;1|gamerace;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>viliage1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>river;2|stone;3|ruintown1;1|hiddeway;1|manflower;2|orehole;1|weaponseller;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>mushroom;1|torch;1|batcrowd;2|earthelement;1|snare;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>met;30|treasure;25|witchhome;20|dyeseller;25</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -610,10 +582,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>river;2|fishpool;1|swamp;2|colordoor;1|corsair1;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>suntemple;2|shadowprince;1|colordoor;1|blockway;1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -630,10 +598,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>portal;1|fishpool;1|grave;2|hiddeway;1|snare;2|starve;2|blockway;1|suntemple;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>fortune;1|colordoor;1|waternest;2|ruinpiece;3</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -943,14 +907,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>orehole;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>mushroom;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>underwater;1|torch;1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -971,10 +927,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>oldtree;1|dyeseller;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>treasure;20</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -987,30 +939,14 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>oldtree;1|river;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>poppyfield;1|fishpool;2|river;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>manflower;2|dyeseller;1|poppyfield;1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>sandland;2|orehole;1|sandflow;1|stone;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>sandland;2|sandflow;1|stone;2</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>orehole;1|sandflow;2|stone;3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>bossmanwang;1|stonedoor;1|boostagi;1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -1048,13 +984,109 @@
   </si>
   <si>
     <t>Altitude</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QItemWood</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QItemOre</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QItemFish</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QItemDrug</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QItemMushroom</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>木材</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>矿石</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>鱼</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>草药</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>蘑菇</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>float</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>sewer;3|river;2|fortune;1|poppyfield;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trees;3|grave;1|portal;1|manflower;1|gamerace;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>river;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dyeseller;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>wolfnest;2|gamegamble;1|sewer;3|river;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>portal;1|grave;2|hiddeway;1|snare;2|starve;2|blockway;1|suntemple;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>poppyfield;1|river;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>river;2|swamp;2|colordoor;1|corsair1;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>river;2|stone;3|ruintown1;1|hiddeway;1|manflower;2|weaponseller;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>sandflow;2|stone;3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>torch;1|batcrowd;2|earthelement;1|snare;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>hiddeway;1|swamp;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trees;3</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1810,7 +1842,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1917,6 +1949,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1964,7 +1999,28 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="32">
+  <dxfs count="37">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1995,25 +2051,62 @@
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -2222,6 +2315,93 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -2764,6 +2944,74 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2776,38 +3024,43 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A3:Z48" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30" tableBorderDxfId="29">
-  <autoFilter ref="A3:Z48" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState ref="A4:Z48">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AE48" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35" tableBorderDxfId="34">
+  <autoFilter ref="A3:AE48"/>
+  <sortState ref="A4:AE48">
     <sortCondition ref="A3:A48"/>
   </sortState>
-  <tableColumns count="26">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="28"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="27"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Type" dataDxfId="26"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Sector" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Level" dataDxfId="24"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="ReviveScene" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Quest" dataDxfId="22"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="QuestRandom" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="QPortal" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="QCardChange" dataDxfId="19"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="QPiece" dataDxfId="18"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="QMerchant" dataDxfId="17"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="QDoctor" dataDxfId="16"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="QAngel" dataDxfId="15"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="QWheel" dataDxfId="14"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="QRes" dataDxfId="13"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Func" dataDxfId="12"/>
-    <tableColumn id="19" xr3:uid="{C4DE9876-761E-4F8F-AC05-98A2EEB0890C}" name="Temperature" dataDxfId="5"/>
-    <tableColumn id="23" xr3:uid="{CCCD053A-EDF9-4438-A6AA-6422F20485C6}" name="Humitity" dataDxfId="4"/>
-    <tableColumn id="26" xr3:uid="{C17F5093-27F2-476C-8B65-5FE7F10D25E9}" name="Altitude" dataDxfId="0"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Url" dataDxfId="11"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="TilePath" dataDxfId="10"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Icon" dataDxfId="9"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="IconX" dataDxfId="8"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="IconY" dataDxfId="7"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="IconColor" dataDxfId="6"/>
+  <tableColumns count="31">
+    <tableColumn id="1" name="Id" dataDxfId="33"/>
+    <tableColumn id="2" name="Name" dataDxfId="32"/>
+    <tableColumn id="18" name="Type" dataDxfId="31"/>
+    <tableColumn id="25" name="Sector" dataDxfId="30"/>
+    <tableColumn id="3" name="Level" dataDxfId="29"/>
+    <tableColumn id="20" name="ReviveScene" dataDxfId="28"/>
+    <tableColumn id="4" name="Quest" dataDxfId="27"/>
+    <tableColumn id="17" name="QuestRandom" dataDxfId="26"/>
+    <tableColumn id="5" name="QPortal" dataDxfId="25"/>
+    <tableColumn id="6" name="QCardChange" dataDxfId="24"/>
+    <tableColumn id="7" name="QPiece" dataDxfId="23"/>
+    <tableColumn id="8" name="QMerchant" dataDxfId="22"/>
+    <tableColumn id="9" name="QDoctor" dataDxfId="21"/>
+    <tableColumn id="10" name="QAngel" dataDxfId="20"/>
+    <tableColumn id="21" name="QWheel" dataDxfId="19"/>
+    <tableColumn id="22" name="QRes" dataDxfId="18"/>
+    <tableColumn id="27" name="QItemDrug" dataDxfId="5"/>
+    <tableColumn id="31" name="QItemFish" dataDxfId="4"/>
+    <tableColumn id="30" name="QItemOre" dataDxfId="6"/>
+    <tableColumn id="28" name="QItemMushroom" dataDxfId="7"/>
+    <tableColumn id="29" name="QItemWood" dataDxfId="3"/>
+    <tableColumn id="11" name="Func" dataDxfId="17"/>
+    <tableColumn id="19" name="Temperature" dataDxfId="16"/>
+    <tableColumn id="23" name="Humitity" dataDxfId="15"/>
+    <tableColumn id="26" name="Altitude" dataDxfId="14"/>
+    <tableColumn id="12" name="Url" dataDxfId="13"/>
+    <tableColumn id="13" name="TilePath" dataDxfId="12"/>
+    <tableColumn id="14" name="Icon" dataDxfId="11"/>
+    <tableColumn id="15" name="IconX" dataDxfId="10"/>
+    <tableColumn id="16" name="IconY" dataDxfId="9"/>
+    <tableColumn id="24" name="IconColor" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2821,7 +3074,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="C7EDCC"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -3133,11 +3386,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z48"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AE48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="R44" sqref="R44:T48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T23" sqref="T23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3151,16 +3404,22 @@
     <col min="7" max="7" width="52.875" style="5" customWidth="1"/>
     <col min="8" max="8" width="23.625" style="5" customWidth="1"/>
     <col min="9" max="16" width="3.125" style="5" customWidth="1"/>
-    <col min="17" max="17" width="6.625" style="5" customWidth="1"/>
-    <col min="18" max="20" width="4.125" style="5" customWidth="1"/>
-    <col min="21" max="21" width="9.75" style="5" customWidth="1"/>
-    <col min="22" max="22" width="9.5" style="5" customWidth="1"/>
-    <col min="23" max="23" width="7.25" style="5" customWidth="1"/>
-    <col min="24" max="26" width="6" style="5" customWidth="1"/>
-    <col min="27" max="16384" width="9" style="5"/>
+    <col min="17" max="18" width="3.25" style="5" customWidth="1"/>
+    <col min="19" max="19" width="3.25" customWidth="1"/>
+    <col min="20" max="20" width="3.25" style="5" customWidth="1"/>
+    <col min="21" max="21" width="3.25" customWidth="1"/>
+    <col min="22" max="22" width="3.125" style="5" customWidth="1"/>
+    <col min="24" max="24" width="3.125" style="5" customWidth="1"/>
+    <col min="25" max="25" width="6.625" style="5" customWidth="1"/>
+    <col min="26" max="28" width="4.125" style="5" customWidth="1"/>
+    <col min="29" max="29" width="9.75" style="5" customWidth="1"/>
+    <col min="30" max="30" width="9.5" style="5" customWidth="1"/>
+    <col min="31" max="31" width="7.25" style="5" customWidth="1"/>
+    <col min="32" max="34" width="6" style="5" customWidth="1"/>
+    <col min="35" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="60" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:31" ht="60" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -3168,25 +3427,25 @@
         <v>16</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>17</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>30</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>51</v>
@@ -3204,43 +3463,58 @@
         <v>59</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="Q1" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="V1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="R1" s="32" t="s">
-        <v>270</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="T1" s="30" t="s">
-        <v>275</v>
-      </c>
-      <c r="U1" s="2" t="s">
+      <c r="W1" s="32" t="s">
+        <v>254</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="Y1" s="30" t="s">
+        <v>259</v>
+      </c>
+      <c r="Z1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="Z1" s="4" t="s">
-        <v>227</v>
+      <c r="AE1" s="4" t="s">
+        <v>218</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
         <v>13</v>
       </c>
@@ -3248,22 +3522,22 @@
         <v>14</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>85</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I2" s="8" t="s">
         <v>48</v>
@@ -3284,43 +3558,58 @@
         <v>48</v>
       </c>
       <c r="O2" s="8" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="P2" s="8" t="s">
-        <v>190</v>
-      </c>
-      <c r="Q2" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q2" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="R2" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="S2" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="T2" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="U2" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="V2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="R2" s="33" t="s">
-        <v>271</v>
-      </c>
-      <c r="S2" s="7" t="s">
-        <v>271</v>
-      </c>
-      <c r="T2" s="31" t="s">
-        <v>271</v>
-      </c>
-      <c r="U2" s="7" t="s">
+      <c r="W2" s="33" t="s">
+        <v>255</v>
+      </c>
+      <c r="X2" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="Y2" s="31" t="s">
+        <v>255</v>
+      </c>
+      <c r="Z2" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="V2" s="7" t="s">
+      <c r="AA2" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="W2" s="7" t="s">
+      <c r="AB2" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="X2" s="7" t="s">
+      <c r="AC2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="Y2" s="9" t="s">
+      <c r="AD2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="Z2" s="9" t="s">
+      <c r="AE2" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A3" s="10" t="s">
         <v>20</v>
       </c>
@@ -3328,22 +3617,22 @@
         <v>21</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="E3" s="10" t="s">
         <v>22</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G3" s="10" t="s">
         <v>29</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I3" s="11" t="s">
         <v>49</v>
@@ -3364,43 +3653,58 @@
         <v>56</v>
       </c>
       <c r="O3" s="11" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="P3" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="Q3" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q3" s="36" t="s">
+        <v>264</v>
+      </c>
+      <c r="R3" s="36" t="s">
+        <v>263</v>
+      </c>
+      <c r="S3" s="36" t="s">
+        <v>262</v>
+      </c>
+      <c r="T3" s="36" t="s">
+        <v>265</v>
+      </c>
+      <c r="U3" s="36" t="s">
+        <v>261</v>
+      </c>
+      <c r="V3" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="R3" s="34" t="s">
-        <v>272</v>
-      </c>
-      <c r="S3" s="23" t="s">
-        <v>274</v>
-      </c>
-      <c r="T3" s="35" t="s">
-        <v>276</v>
-      </c>
-      <c r="U3" s="10" t="s">
+      <c r="W3" s="34" t="s">
+        <v>256</v>
+      </c>
+      <c r="X3" s="23" t="s">
+        <v>258</v>
+      </c>
+      <c r="Y3" s="35" t="s">
+        <v>260</v>
+      </c>
+      <c r="Z3" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="V3" s="10" t="s">
+      <c r="AA3" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="W3" s="10" t="s">
+      <c r="AB3" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="X3" s="10" t="s">
+      <c r="AC3" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="Y3" s="10" t="s">
+      <c r="AD3" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="Z3" s="23" t="s">
-        <v>228</v>
+      <c r="AE3" s="23" t="s">
+        <v>219</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A4" s="12">
         <v>13010001</v>
       </c>
@@ -3411,7 +3715,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="E4" s="13">
         <v>1</v>
@@ -3419,11 +3723,11 @@
       <c r="F4" s="13">
         <v>13010001</v>
       </c>
-      <c r="G4" s="13" t="s">
-        <v>87</v>
+      <c r="G4" s="20" t="s">
+        <v>272</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="I4" s="13">
         <v>1</v>
@@ -3436,35 +3740,42 @@
       <c r="O4" s="13"/>
       <c r="P4" s="13"/>
       <c r="Q4" s="13"/>
-      <c r="R4" s="13">
+      <c r="R4" s="13"/>
+      <c r="S4" s="13"/>
+      <c r="T4" s="13"/>
+      <c r="U4" s="13">
+        <v>1</v>
+      </c>
+      <c r="V4" s="13"/>
+      <c r="W4" s="13">
         <v>3</v>
       </c>
-      <c r="S4" s="13">
-        <v>2</v>
-      </c>
-      <c r="T4" s="13">
-        <v>2</v>
-      </c>
-      <c r="U4" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="V4" s="13" t="s">
+      <c r="X4" s="13">
+        <v>2</v>
+      </c>
+      <c r="Y4" s="13">
+        <v>2</v>
+      </c>
+      <c r="Z4" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="AA4" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="W4" s="13" t="s">
+      <c r="AB4" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="X4" s="13">
+      <c r="AC4" s="13">
         <v>1348</v>
       </c>
-      <c r="Y4" s="13">
+      <c r="AD4" s="13">
         <v>611</v>
       </c>
-      <c r="Z4" s="24" t="s">
-        <v>231</v>
+      <c r="AE4" s="24" t="s">
+        <v>222</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A5" s="12">
         <v>13010002</v>
       </c>
@@ -3475,7 +3786,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="E5" s="13">
         <v>2</v>
@@ -3483,11 +3794,11 @@
       <c r="F5" s="13">
         <v>13010001</v>
       </c>
-      <c r="G5" s="13" t="s">
-        <v>136</v>
+      <c r="G5" s="20" t="s">
+        <v>276</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="I5" s="13">
         <v>1</v>
@@ -3505,34 +3816,43 @@
       <c r="P5" s="13"/>
       <c r="Q5" s="13"/>
       <c r="R5" s="13">
-        <v>2</v>
-      </c>
-      <c r="S5" s="13">
+        <v>1</v>
+      </c>
+      <c r="S5" s="13"/>
+      <c r="T5" s="13"/>
+      <c r="U5" s="13">
+        <v>1</v>
+      </c>
+      <c r="V5" s="13"/>
+      <c r="W5" s="13">
+        <v>2</v>
+      </c>
+      <c r="X5" s="13">
         <v>3</v>
       </c>
-      <c r="T5" s="13">
-        <v>2</v>
-      </c>
-      <c r="U5" s="13" t="s">
+      <c r="Y5" s="13">
+        <v>2</v>
+      </c>
+      <c r="Z5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="V5" s="13" t="s">
+      <c r="AA5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="W5" s="13" t="s">
+      <c r="AB5" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="X5" s="13">
+      <c r="AC5" s="13">
         <v>1279</v>
       </c>
-      <c r="Y5" s="13">
+      <c r="AD5" s="13">
         <v>571</v>
       </c>
-      <c r="Z5" s="24" t="s">
-        <v>231</v>
+      <c r="AE5" s="24" t="s">
+        <v>222</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A6" s="12">
         <v>13010003</v>
       </c>
@@ -3543,7 +3863,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="E6" s="13">
         <v>3</v>
@@ -3551,11 +3871,11 @@
       <c r="F6" s="13">
         <v>13010006</v>
       </c>
-      <c r="G6" s="13" t="s">
-        <v>140</v>
+      <c r="G6" s="20" t="s">
+        <v>273</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I6" s="13">
         <v>1</v>
@@ -3568,35 +3888,40 @@
       <c r="O6" s="13"/>
       <c r="P6" s="13"/>
       <c r="Q6" s="13"/>
-      <c r="R6" s="13">
+      <c r="R6" s="13"/>
+      <c r="S6" s="13"/>
+      <c r="T6" s="13"/>
+      <c r="U6" s="13"/>
+      <c r="V6" s="13"/>
+      <c r="W6" s="13">
         <v>3</v>
       </c>
-      <c r="S6" s="13">
+      <c r="X6" s="13">
         <v>3</v>
       </c>
-      <c r="T6" s="13">
-        <v>2</v>
-      </c>
-      <c r="U6" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="V6" s="13" t="s">
+      <c r="Y6" s="13">
+        <v>2</v>
+      </c>
+      <c r="Z6" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="AA6" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="W6" s="13" t="s">
+      <c r="AB6" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="X6" s="13">
+      <c r="AC6" s="13">
         <v>1251</v>
       </c>
-      <c r="Y6" s="13">
+      <c r="AD6" s="13">
         <v>432</v>
       </c>
-      <c r="Z6" s="24" t="s">
-        <v>231</v>
+      <c r="AE6" s="24" t="s">
+        <v>222</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A7" s="12">
         <v>13010004</v>
       </c>
@@ -3607,7 +3932,7 @@
         <v>2</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="E7" s="13">
         <v>5</v>
@@ -3615,11 +3940,11 @@
       <c r="F7" s="13">
         <v>13010006</v>
       </c>
-      <c r="G7" s="13" t="s">
-        <v>142</v>
+      <c r="G7" s="20" t="s">
+        <v>280</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="I7" s="13">
         <v>1</v>
@@ -3634,46 +3959,53 @@
       <c r="O7" s="13"/>
       <c r="P7" s="13"/>
       <c r="Q7" s="13"/>
-      <c r="R7" s="13">
+      <c r="R7" s="13"/>
+      <c r="S7" s="13">
+        <v>1</v>
+      </c>
+      <c r="T7" s="13"/>
+      <c r="U7" s="13"/>
+      <c r="V7" s="13"/>
+      <c r="W7" s="13">
         <v>3</v>
       </c>
-      <c r="S7" s="13">
-        <v>2</v>
-      </c>
-      <c r="T7" s="13">
-        <v>1</v>
-      </c>
-      <c r="U7" s="13" t="s">
+      <c r="X7" s="13">
+        <v>2</v>
+      </c>
+      <c r="Y7" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="V7" s="13" t="s">
+      <c r="AA7" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="W7" s="13" t="s">
+      <c r="AB7" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="X7" s="13">
+      <c r="AC7" s="13">
         <v>1148</v>
       </c>
-      <c r="Y7" s="13">
+      <c r="AD7" s="13">
         <v>351</v>
       </c>
-      <c r="Z7" s="24" t="s">
-        <v>231</v>
+      <c r="AE7" s="24" t="s">
+        <v>222</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A8" s="12">
         <v>13010005</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="C8" s="13">
         <v>2</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="E8" s="13">
         <v>8</v>
@@ -3682,10 +4014,10 @@
         <v>13010006</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="I8" s="13">
         <v>1</v>
@@ -3700,35 +4032,40 @@
       <c r="O8" s="13"/>
       <c r="P8" s="13"/>
       <c r="Q8" s="13"/>
-      <c r="R8" s="13">
-        <v>2</v>
-      </c>
-      <c r="S8" s="13">
-        <v>2</v>
-      </c>
-      <c r="T8" s="13">
+      <c r="R8" s="13"/>
+      <c r="S8" s="13"/>
+      <c r="T8" s="13"/>
+      <c r="U8" s="13"/>
+      <c r="V8" s="13"/>
+      <c r="W8" s="13">
+        <v>2</v>
+      </c>
+      <c r="X8" s="13">
+        <v>2</v>
+      </c>
+      <c r="Y8" s="13">
         <v>5</v>
       </c>
-      <c r="U8" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="V8" s="13" t="s">
+      <c r="Z8" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="AA8" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="W8" s="13" t="s">
+      <c r="AB8" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="X8" s="13">
+      <c r="AC8" s="13">
         <v>1386</v>
       </c>
-      <c r="Y8" s="13">
+      <c r="AD8" s="13">
         <v>339</v>
       </c>
-      <c r="Z8" s="24" t="s">
-        <v>231</v>
+      <c r="AE8" s="24" t="s">
+        <v>222</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A9" s="12">
         <v>13010006</v>
       </c>
@@ -3739,7 +4076,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="E9" s="13">
         <v>3</v>
@@ -3758,35 +4095,40 @@
       <c r="O9" s="13"/>
       <c r="P9" s="13"/>
       <c r="Q9" s="13"/>
-      <c r="R9" s="13">
+      <c r="R9" s="13"/>
+      <c r="S9" s="13"/>
+      <c r="T9" s="13"/>
+      <c r="U9" s="13"/>
+      <c r="V9" s="13"/>
+      <c r="W9" s="13">
         <v>3</v>
       </c>
-      <c r="S9" s="13">
+      <c r="X9" s="13">
         <v>3</v>
       </c>
-      <c r="T9" s="13">
-        <v>2</v>
-      </c>
-      <c r="U9" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="V9" s="13" t="s">
+      <c r="Y9" s="13">
+        <v>2</v>
+      </c>
+      <c r="Z9" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="AA9" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="W9" s="13" t="s">
+      <c r="AB9" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="X9" s="13">
+      <c r="AC9" s="13">
         <v>1232</v>
       </c>
-      <c r="Y9" s="13">
+      <c r="AD9" s="13">
         <v>506</v>
       </c>
-      <c r="Z9" s="24" t="s">
-        <v>231</v>
+      <c r="AE9" s="24" t="s">
+        <v>222</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A10" s="12">
         <v>13010007</v>
       </c>
@@ -3797,7 +4139,7 @@
         <v>2</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="E10" s="13">
         <v>7</v>
@@ -3805,11 +4147,11 @@
       <c r="F10" s="13">
         <v>13010006</v>
       </c>
-      <c r="G10" s="13" t="s">
-        <v>164</v>
+      <c r="G10" s="20" t="s">
+        <v>277</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="I10" s="13">
         <v>1</v>
@@ -3827,34 +4169,41 @@
       </c>
       <c r="Q10" s="13"/>
       <c r="R10" s="13">
-        <v>2</v>
-      </c>
-      <c r="S10" s="13">
+        <v>1</v>
+      </c>
+      <c r="S10" s="13"/>
+      <c r="T10" s="13"/>
+      <c r="U10" s="13"/>
+      <c r="V10" s="13"/>
+      <c r="W10" s="13">
+        <v>2</v>
+      </c>
+      <c r="X10" s="13">
         <v>4</v>
       </c>
-      <c r="T10" s="13">
-        <v>2</v>
-      </c>
-      <c r="U10" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="V10" s="13" t="s">
+      <c r="Y10" s="13">
+        <v>2</v>
+      </c>
+      <c r="Z10" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA10" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="W10" s="13" t="s">
+      <c r="AB10" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="X10" s="13">
+      <c r="AC10" s="13">
         <v>1431</v>
       </c>
-      <c r="Y10" s="13">
+      <c r="AD10" s="13">
         <v>440</v>
       </c>
-      <c r="Z10" s="24" t="s">
-        <v>231</v>
+      <c r="AE10" s="24" t="s">
+        <v>222</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A11" s="12">
         <v>13010008</v>
       </c>
@@ -3865,7 +4214,7 @@
         <v>2</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="E11" s="13">
         <v>6</v>
@@ -3874,10 +4223,10 @@
         <v>13010006</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="I11" s="13">
         <v>1</v>
@@ -3892,35 +4241,40 @@
       </c>
       <c r="P11" s="13"/>
       <c r="Q11" s="13"/>
-      <c r="R11" s="13">
-        <v>1</v>
-      </c>
-      <c r="S11" s="13">
+      <c r="R11" s="13"/>
+      <c r="S11" s="13"/>
+      <c r="T11" s="13"/>
+      <c r="U11" s="13"/>
+      <c r="V11" s="13"/>
+      <c r="W11" s="13">
+        <v>1</v>
+      </c>
+      <c r="X11" s="13">
         <v>3</v>
       </c>
-      <c r="T11" s="13">
+      <c r="Y11" s="13">
         <v>5</v>
       </c>
-      <c r="U11" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="V11" s="13" t="s">
+      <c r="Z11" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="AA11" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="W11" s="13" t="s">
+      <c r="AB11" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="X11" s="13">
+      <c r="AC11" s="13">
         <v>1250</v>
       </c>
-      <c r="Y11" s="13">
+      <c r="AD11" s="13">
         <v>338</v>
       </c>
-      <c r="Z11" s="24" t="s">
-        <v>231</v>
+      <c r="AE11" s="24" t="s">
+        <v>222</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A12" s="12">
         <v>13010009</v>
       </c>
@@ -3931,7 +4285,7 @@
         <v>2</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="E12" s="13">
         <v>4</v>
@@ -3940,10 +4294,10 @@
         <v>13010006</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="I12" s="13">
         <v>1</v>
@@ -3960,46 +4314,51 @@
       <c r="O12" s="13"/>
       <c r="P12" s="13"/>
       <c r="Q12" s="13"/>
-      <c r="R12" s="13">
+      <c r="R12" s="13"/>
+      <c r="S12" s="13"/>
+      <c r="T12" s="13"/>
+      <c r="U12" s="13"/>
+      <c r="V12" s="13"/>
+      <c r="W12" s="13">
         <v>3</v>
       </c>
-      <c r="S12" s="13">
+      <c r="X12" s="13">
         <v>3</v>
       </c>
-      <c r="T12" s="13">
-        <v>2</v>
-      </c>
-      <c r="U12" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="V12" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="W12" s="13" t="s">
+      <c r="Y12" s="13">
+        <v>2</v>
+      </c>
+      <c r="Z12" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="AA12" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="AB12" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="X12" s="13">
+      <c r="AC12" s="13">
         <v>1332</v>
       </c>
-      <c r="Y12" s="13">
+      <c r="AD12" s="13">
         <v>484</v>
       </c>
-      <c r="Z12" s="24" t="s">
-        <v>231</v>
+      <c r="AE12" s="24" t="s">
+        <v>222</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A13" s="12">
         <v>13010010</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C13" s="15">
         <v>2</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="E13" s="15">
         <v>6</v>
@@ -4008,10 +4367,10 @@
         <v>13010006</v>
       </c>
       <c r="G13" s="20" t="s">
-        <v>143</v>
+        <v>282</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="I13" s="15">
         <v>1</v>
@@ -4024,29 +4383,36 @@
       <c r="O13" s="15"/>
       <c r="P13" s="15"/>
       <c r="Q13" s="15"/>
-      <c r="R13" s="13">
-        <v>2</v>
-      </c>
-      <c r="S13" s="13">
-        <v>2</v>
-      </c>
-      <c r="T13" s="13">
+      <c r="R13" s="15"/>
+      <c r="S13" s="15"/>
+      <c r="T13" s="15">
+        <v>1</v>
+      </c>
+      <c r="U13" s="15"/>
+      <c r="V13" s="15"/>
+      <c r="W13" s="13">
+        <v>2</v>
+      </c>
+      <c r="X13" s="13">
+        <v>2</v>
+      </c>
+      <c r="Y13" s="13">
         <v>3</v>
       </c>
-      <c r="U13" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="V13" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="W13" s="15"/>
-      <c r="X13" s="15"/>
-      <c r="Y13" s="15"/>
-      <c r="Z13" s="24" t="s">
-        <v>231</v>
+      <c r="Z13" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="AA13" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="AB13" s="15"/>
+      <c r="AC13" s="15"/>
+      <c r="AD13" s="15"/>
+      <c r="AE13" s="24" t="s">
+        <v>222</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A14" s="27">
         <v>13010101</v>
       </c>
@@ -4057,7 +4423,7 @@
         <v>1</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="E14" s="13">
         <v>16</v>
@@ -4076,35 +4442,40 @@
       <c r="O14" s="13"/>
       <c r="P14" s="13"/>
       <c r="Q14" s="13"/>
-      <c r="R14" s="13">
-        <v>2</v>
-      </c>
-      <c r="S14" s="13">
+      <c r="R14" s="13"/>
+      <c r="S14" s="13"/>
+      <c r="T14" s="13"/>
+      <c r="U14" s="13"/>
+      <c r="V14" s="13"/>
+      <c r="W14" s="13">
+        <v>2</v>
+      </c>
+      <c r="X14" s="13">
         <v>3</v>
       </c>
-      <c r="T14" s="13">
-        <v>2</v>
-      </c>
-      <c r="U14" s="13" t="s">
-        <v>193</v>
-      </c>
-      <c r="V14" s="13" t="s">
+      <c r="Y14" s="13">
+        <v>2</v>
+      </c>
+      <c r="Z14" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="AA14" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="W14" s="13" t="s">
+      <c r="AB14" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="X14" s="13">
+      <c r="AC14" s="13">
         <v>894</v>
       </c>
-      <c r="Y14" s="13">
+      <c r="AD14" s="13">
         <v>509</v>
       </c>
-      <c r="Z14" s="24" t="s">
-        <v>229</v>
+      <c r="AE14" s="24" t="s">
+        <v>220</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A15" s="27">
         <v>13010102</v>
       </c>
@@ -4115,7 +4486,7 @@
         <v>2</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="E15" s="13">
         <v>16</v>
@@ -4124,10 +4495,10 @@
         <v>13010101</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="H15" s="20" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="I15" s="13">
         <v>1</v>
@@ -4142,35 +4513,40 @@
       <c r="O15" s="13"/>
       <c r="P15" s="13"/>
       <c r="Q15" s="13"/>
-      <c r="R15" s="13">
-        <v>2</v>
-      </c>
-      <c r="S15" s="13">
+      <c r="R15" s="13"/>
+      <c r="S15" s="13"/>
+      <c r="T15" s="13"/>
+      <c r="U15" s="13"/>
+      <c r="V15" s="13"/>
+      <c r="W15" s="13">
+        <v>2</v>
+      </c>
+      <c r="X15" s="13">
         <v>5</v>
       </c>
-      <c r="T15" s="13">
-        <v>2</v>
-      </c>
-      <c r="U15" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="V15" s="13" t="s">
+      <c r="Y15" s="13">
+        <v>2</v>
+      </c>
+      <c r="Z15" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="AA15" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="W15" s="13" t="s">
+      <c r="AB15" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="X15" s="13">
+      <c r="AC15" s="13">
         <v>1040</v>
       </c>
-      <c r="Y15" s="13">
+      <c r="AD15" s="13">
         <v>538</v>
       </c>
-      <c r="Z15" s="24" t="s">
-        <v>229</v>
+      <c r="AE15" s="24" t="s">
+        <v>220</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A16" s="27">
         <v>13010103</v>
       </c>
@@ -4181,7 +4557,7 @@
         <v>2</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="E16" s="13">
         <v>19</v>
@@ -4190,10 +4566,10 @@
         <v>13010101</v>
       </c>
       <c r="G16" s="20" t="s">
-        <v>266</v>
+        <v>281</v>
       </c>
       <c r="H16" s="20" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="I16" s="13">
         <v>1</v>
@@ -4208,35 +4584,42 @@
       </c>
       <c r="P16" s="13"/>
       <c r="Q16" s="13"/>
-      <c r="R16" s="13">
+      <c r="R16" s="13"/>
+      <c r="S16" s="13">
+        <v>1</v>
+      </c>
+      <c r="T16" s="13"/>
+      <c r="U16" s="13"/>
+      <c r="V16" s="13"/>
+      <c r="W16" s="13">
         <v>3</v>
       </c>
-      <c r="S16" s="13">
+      <c r="X16" s="13">
         <v>3</v>
       </c>
-      <c r="T16" s="13">
-        <v>2</v>
-      </c>
-      <c r="U16" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="V16" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="W16" s="13" t="s">
+      <c r="Y16" s="13">
+        <v>2</v>
+      </c>
+      <c r="Z16" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="AA16" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="AB16" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="X16" s="13">
+      <c r="AC16" s="13">
         <v>1213</v>
       </c>
-      <c r="Y16" s="13">
+      <c r="AD16" s="13">
         <v>655</v>
       </c>
-      <c r="Z16" s="24" t="s">
-        <v>229</v>
+      <c r="AE16" s="24" t="s">
+        <v>220</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A17" s="27">
         <v>13010104</v>
       </c>
@@ -4247,7 +4630,7 @@
         <v>2</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="E17" s="13">
         <v>18</v>
@@ -4255,11 +4638,11 @@
       <c r="F17" s="13">
         <v>13010101</v>
       </c>
-      <c r="G17" s="13" t="s">
-        <v>94</v>
+      <c r="G17" s="20" t="s">
+        <v>283</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="I17" s="13">
         <v>1</v>
@@ -4274,35 +4657,42 @@
       <c r="O17" s="13"/>
       <c r="P17" s="13"/>
       <c r="Q17" s="13"/>
-      <c r="R17" s="13">
-        <v>2</v>
-      </c>
-      <c r="S17" s="13">
+      <c r="R17" s="13"/>
+      <c r="S17" s="13"/>
+      <c r="T17" s="13">
+        <v>1</v>
+      </c>
+      <c r="U17" s="13"/>
+      <c r="V17" s="13"/>
+      <c r="W17" s="13">
+        <v>2</v>
+      </c>
+      <c r="X17" s="13">
         <v>4</v>
       </c>
-      <c r="T17" s="13">
-        <v>2</v>
-      </c>
-      <c r="U17" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="V17" s="13" t="s">
+      <c r="Y17" s="13">
+        <v>2</v>
+      </c>
+      <c r="Z17" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="AA17" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="W17" s="13" t="s">
+      <c r="AB17" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="X17" s="13">
+      <c r="AC17" s="13">
         <v>1149</v>
       </c>
-      <c r="Y17" s="13">
+      <c r="AD17" s="13">
         <v>584</v>
       </c>
-      <c r="Z17" s="24" t="s">
-        <v>229</v>
+      <c r="AE17" s="24" t="s">
+        <v>220</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A18" s="27">
         <v>13010105</v>
       </c>
@@ -4313,7 +4703,7 @@
         <v>2</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="E18" s="13">
         <v>20</v>
@@ -4321,11 +4711,11 @@
       <c r="F18" s="13">
         <v>13010101</v>
       </c>
-      <c r="G18" s="13" t="s">
-        <v>86</v>
+      <c r="G18" s="20" t="s">
+        <v>284</v>
       </c>
       <c r="H18" s="20" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="I18" s="13">
         <v>1</v>
@@ -4340,46 +4730,53 @@
       <c r="O18" s="13"/>
       <c r="P18" s="13"/>
       <c r="Q18" s="13"/>
-      <c r="R18" s="13">
-        <v>2</v>
-      </c>
-      <c r="S18" s="13">
+      <c r="R18" s="13"/>
+      <c r="S18" s="13"/>
+      <c r="T18" s="13">
+        <v>1</v>
+      </c>
+      <c r="U18" s="13"/>
+      <c r="V18" s="13"/>
+      <c r="W18" s="13">
+        <v>2</v>
+      </c>
+      <c r="X18" s="13">
         <v>3</v>
       </c>
-      <c r="T18" s="13">
-        <v>2</v>
-      </c>
-      <c r="U18" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="V18" s="13" t="s">
+      <c r="Y18" s="13">
+        <v>2</v>
+      </c>
+      <c r="Z18" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="AA18" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="W18" s="13" t="s">
+      <c r="AB18" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="X18" s="13">
+      <c r="AC18" s="13">
         <v>840</v>
       </c>
-      <c r="Y18" s="13">
+      <c r="AD18" s="13">
         <v>444</v>
       </c>
-      <c r="Z18" s="24" t="s">
-        <v>229</v>
+      <c r="AE18" s="24" t="s">
+        <v>220</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A19" s="27">
         <v>13010106</v>
       </c>
       <c r="B19" s="27" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C19" s="13">
         <v>2</v>
       </c>
       <c r="D19" s="20" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="E19" s="13">
         <v>15</v>
@@ -4388,10 +4785,10 @@
         <v>13010016</v>
       </c>
       <c r="G19" s="20" t="s">
-        <v>262</v>
+        <v>278</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="I19" s="13">
         <v>1</v>
@@ -4407,45 +4804,52 @@
       <c r="P19" s="13"/>
       <c r="Q19" s="13"/>
       <c r="R19" s="13">
+        <v>1</v>
+      </c>
+      <c r="S19" s="13"/>
+      <c r="T19" s="13"/>
+      <c r="U19" s="13"/>
+      <c r="V19" s="13"/>
+      <c r="W19" s="13">
         <v>3</v>
       </c>
-      <c r="S19" s="13">
+      <c r="X19" s="13">
         <v>4</v>
       </c>
-      <c r="T19" s="13">
-        <v>2</v>
-      </c>
-      <c r="U19" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="V19" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="W19" s="13" t="s">
+      <c r="Y19" s="13">
+        <v>2</v>
+      </c>
+      <c r="Z19" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA19" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB19" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="X19" s="13">
+      <c r="AC19" s="13">
         <v>1067</v>
       </c>
-      <c r="Y19" s="13">
+      <c r="AD19" s="13">
         <v>445</v>
       </c>
-      <c r="Z19" s="24" t="s">
-        <v>229</v>
+      <c r="AE19" s="24" t="s">
+        <v>220</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A20" s="27">
         <v>13010107</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="C20" s="15">
         <v>2</v>
       </c>
       <c r="D20" s="20" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="E20" s="15">
         <v>15</v>
@@ -4454,10 +4858,10 @@
         <v>13010101</v>
       </c>
       <c r="G20" s="20" t="s">
-        <v>261</v>
+        <v>274</v>
       </c>
       <c r="H20" s="20" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="I20" s="13">
         <v>1</v>
@@ -4473,47 +4877,54 @@
       <c r="P20" s="15">
         <v>1</v>
       </c>
-      <c r="Q20" s="16"/>
-      <c r="R20" s="13">
+      <c r="Q20" s="15"/>
+      <c r="R20" s="15"/>
+      <c r="S20" s="15"/>
+      <c r="T20" s="15"/>
+      <c r="U20" s="15">
+        <v>1</v>
+      </c>
+      <c r="V20" s="16"/>
+      <c r="W20" s="13">
         <v>3</v>
       </c>
-      <c r="S20" s="13">
+      <c r="X20" s="13">
         <v>3</v>
       </c>
-      <c r="T20" s="13">
-        <v>2</v>
-      </c>
-      <c r="U20" s="13" t="s">
-        <v>218</v>
-      </c>
-      <c r="V20" s="13" t="s">
-        <v>218</v>
-      </c>
-      <c r="W20" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="X20" s="16">
+      <c r="Y20" s="13">
+        <v>2</v>
+      </c>
+      <c r="Z20" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="AA20" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="AB20" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="AC20" s="16">
         <v>850</v>
       </c>
-      <c r="Y20" s="16">
+      <c r="AD20" s="16">
         <v>589</v>
       </c>
-      <c r="Z20" s="24" t="s">
-        <v>229</v>
+      <c r="AE20" s="24" t="s">
+        <v>220</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A21" s="27">
         <v>13010108</v>
       </c>
       <c r="B21" s="27" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="C21" s="15">
         <v>2</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="E21" s="15">
         <v>15</v>
@@ -4522,10 +4933,10 @@
         <v>13010101</v>
       </c>
       <c r="G21" s="20" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
       <c r="H21" s="20" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="I21" s="13">
         <v>1</v>
@@ -4539,47 +4950,52 @@
       <c r="N21" s="16"/>
       <c r="O21" s="15"/>
       <c r="P21" s="15"/>
-      <c r="Q21" s="16"/>
-      <c r="R21" s="13">
+      <c r="Q21" s="15"/>
+      <c r="R21" s="15"/>
+      <c r="S21" s="15"/>
+      <c r="T21" s="15"/>
+      <c r="U21" s="15"/>
+      <c r="V21" s="16"/>
+      <c r="W21" s="13">
         <v>3</v>
       </c>
-      <c r="S21" s="13">
+      <c r="X21" s="13">
         <v>3</v>
       </c>
-      <c r="T21" s="13">
+      <c r="Y21" s="13">
         <v>3</v>
       </c>
-      <c r="U21" s="13" t="s">
+      <c r="Z21" s="13" t="s">
+        <v>211</v>
+      </c>
+      <c r="AA21" s="13" t="s">
+        <v>211</v>
+      </c>
+      <c r="AB21" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="AC21" s="13">
+        <v>682</v>
+      </c>
+      <c r="AD21" s="13">
+        <v>545</v>
+      </c>
+      <c r="AE21" s="24" t="s">
         <v>220</v>
       </c>
-      <c r="V21" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="W21" s="16" t="s">
-        <v>206</v>
-      </c>
-      <c r="X21" s="13">
-        <v>682</v>
-      </c>
-      <c r="Y21" s="13">
-        <v>545</v>
-      </c>
-      <c r="Z21" s="24" t="s">
-        <v>229</v>
-      </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A22" s="27">
         <v>13010109</v>
       </c>
       <c r="B22" s="29" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="C22" s="15">
         <v>2</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="E22" s="15">
         <v>15</v>
@@ -4588,10 +5004,10 @@
         <v>13010101</v>
       </c>
       <c r="G22" s="20" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
       <c r="H22" s="16" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="I22" s="13">
         <v>1</v>
@@ -4605,47 +5021,52 @@
       <c r="N22" s="16"/>
       <c r="O22" s="15"/>
       <c r="P22" s="15"/>
-      <c r="Q22" s="16"/>
-      <c r="R22" s="13">
+      <c r="Q22" s="15"/>
+      <c r="R22" s="15"/>
+      <c r="S22" s="15"/>
+      <c r="T22" s="15"/>
+      <c r="U22" s="15"/>
+      <c r="V22" s="16"/>
+      <c r="W22" s="13">
         <v>3</v>
       </c>
-      <c r="S22" s="13">
+      <c r="X22" s="13">
         <v>3</v>
       </c>
-      <c r="T22" s="13">
+      <c r="Y22" s="13">
         <v>3</v>
       </c>
-      <c r="U22" s="13" t="s">
-        <v>244</v>
-      </c>
-      <c r="V22" s="20" t="s">
-        <v>245</v>
-      </c>
-      <c r="W22" s="16" t="s">
-        <v>241</v>
-      </c>
-      <c r="X22" s="16">
+      <c r="Z22" s="13" t="s">
+        <v>235</v>
+      </c>
+      <c r="AA22" s="20" t="s">
+        <v>236</v>
+      </c>
+      <c r="AB22" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="AC22" s="16">
         <v>643</v>
       </c>
-      <c r="Y22" s="16">
+      <c r="AD22" s="16">
         <v>455</v>
       </c>
-      <c r="Z22" s="24" t="s">
-        <v>229</v>
+      <c r="AE22" s="24" t="s">
+        <v>220</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A23" s="27">
         <v>13010110</v>
       </c>
       <c r="B23" s="29" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="C23" s="15">
         <v>2</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="E23" s="15">
         <v>15</v>
@@ -4653,11 +5074,9 @@
       <c r="F23" s="15">
         <v>13010101</v>
       </c>
-      <c r="G23" s="20" t="s">
-        <v>251</v>
-      </c>
+      <c r="G23" s="20"/>
       <c r="H23" s="16" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="I23" s="13">
         <v>1</v>
@@ -4673,47 +5092,54 @@
       <c r="P23" s="15">
         <v>1</v>
       </c>
-      <c r="Q23" s="16"/>
-      <c r="R23" s="13">
-        <v>2</v>
-      </c>
-      <c r="S23" s="13">
+      <c r="Q23" s="15"/>
+      <c r="R23" s="15"/>
+      <c r="S23" s="15"/>
+      <c r="T23" s="15">
+        <v>1</v>
+      </c>
+      <c r="U23" s="15"/>
+      <c r="V23" s="16"/>
+      <c r="W23" s="13">
+        <v>2</v>
+      </c>
+      <c r="X23" s="13">
         <v>4</v>
       </c>
-      <c r="T23" s="13">
+      <c r="Y23" s="13">
         <v>3</v>
       </c>
-      <c r="U23" s="20" t="s">
-        <v>246</v>
-      </c>
-      <c r="V23" s="20" t="s">
-        <v>246</v>
-      </c>
-      <c r="W23" s="16" t="s">
-        <v>242</v>
-      </c>
-      <c r="X23" s="16">
+      <c r="Z23" s="20" t="s">
+        <v>237</v>
+      </c>
+      <c r="AA23" s="20" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB23" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="AC23" s="16">
         <v>720</v>
       </c>
-      <c r="Y23" s="16">
+      <c r="AD23" s="16">
         <v>375</v>
       </c>
-      <c r="Z23" s="24" t="s">
-        <v>229</v>
+      <c r="AE23" s="24" t="s">
+        <v>220</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A24" s="25">
         <v>13010201</v>
       </c>
       <c r="B24" s="25" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="C24" s="15">
         <v>2</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="E24" s="15">
         <v>15</v>
@@ -4731,47 +5157,52 @@
       <c r="N24" s="16"/>
       <c r="O24" s="15"/>
       <c r="P24" s="15"/>
-      <c r="Q24" s="16"/>
-      <c r="R24" s="13">
+      <c r="Q24" s="15"/>
+      <c r="R24" s="15"/>
+      <c r="S24" s="15"/>
+      <c r="T24" s="15"/>
+      <c r="U24" s="15"/>
+      <c r="V24" s="16"/>
+      <c r="W24" s="13">
         <v>4</v>
       </c>
-      <c r="S24" s="13">
-        <v>2</v>
-      </c>
-      <c r="T24" s="13">
-        <v>2</v>
-      </c>
-      <c r="U24" s="13" t="s">
-        <v>216</v>
-      </c>
-      <c r="V24" s="13" t="s">
-        <v>216</v>
-      </c>
-      <c r="W24" s="16" t="s">
-        <v>203</v>
-      </c>
       <c r="X24" s="13">
+        <v>2</v>
+      </c>
+      <c r="Y24" s="13">
+        <v>2</v>
+      </c>
+      <c r="Z24" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="AA24" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="AB24" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="AC24" s="13">
         <v>807</v>
       </c>
-      <c r="Y24" s="13">
+      <c r="AD24" s="13">
         <v>720</v>
       </c>
-      <c r="Z24" s="24" t="s">
-        <v>230</v>
+      <c r="AE24" s="24" t="s">
+        <v>221</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A25" s="25">
         <v>13010202</v>
       </c>
       <c r="B25" s="25" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="C25" s="15">
         <v>2</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="E25" s="15">
         <v>15</v>
@@ -4780,10 +5211,10 @@
         <v>13010201</v>
       </c>
       <c r="G25" s="15" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="H25" s="15" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="I25" s="13">
         <v>1</v>
@@ -4798,46 +5229,53 @@
       <c r="O25" s="15"/>
       <c r="P25" s="15"/>
       <c r="Q25" s="15"/>
-      <c r="R25" s="13">
+      <c r="R25" s="15"/>
+      <c r="S25" s="15">
+        <v>1</v>
+      </c>
+      <c r="T25" s="15"/>
+      <c r="U25" s="15"/>
+      <c r="V25" s="15"/>
+      <c r="W25" s="13">
         <v>4</v>
       </c>
-      <c r="S25" s="13">
-        <v>1</v>
-      </c>
-      <c r="T25" s="13">
+      <c r="X25" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y25" s="13">
         <v>3</v>
       </c>
-      <c r="U25" s="13" t="s">
+      <c r="Z25" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="AA25" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="AB25" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="AC25" s="15">
+        <v>974</v>
+      </c>
+      <c r="AD25" s="15">
+        <v>594</v>
+      </c>
+      <c r="AE25" s="24" t="s">
         <v>221</v>
       </c>
-      <c r="V25" s="13" t="s">
-        <v>221</v>
-      </c>
-      <c r="W25" s="15" t="s">
-        <v>196</v>
-      </c>
-      <c r="X25" s="15">
-        <v>974</v>
-      </c>
-      <c r="Y25" s="15">
-        <v>594</v>
-      </c>
-      <c r="Z25" s="24" t="s">
-        <v>230</v>
-      </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A26" s="25">
         <v>13010203</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="C26" s="15">
         <v>2</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="E26" s="15">
         <v>15</v>
@@ -4846,10 +5284,10 @@
         <v>13010201</v>
       </c>
       <c r="G26" s="15" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
       <c r="H26" s="15" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="I26" s="13">
         <v>1</v>
@@ -4864,46 +5302,51 @@
         <v>1</v>
       </c>
       <c r="Q26" s="15"/>
-      <c r="R26" s="13">
+      <c r="R26" s="15"/>
+      <c r="S26" s="15"/>
+      <c r="T26" s="15"/>
+      <c r="U26" s="15"/>
+      <c r="V26" s="15"/>
+      <c r="W26" s="13">
         <v>4</v>
       </c>
-      <c r="S26" s="13">
-        <v>1</v>
-      </c>
-      <c r="T26" s="13">
+      <c r="X26" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y26" s="13">
         <v>3</v>
       </c>
-      <c r="U26" s="13" t="s">
-        <v>222</v>
-      </c>
-      <c r="V26" s="13" t="s">
-        <v>222</v>
-      </c>
-      <c r="W26" s="15" t="s">
-        <v>197</v>
-      </c>
-      <c r="X26" s="15">
+      <c r="Z26" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="AA26" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="AB26" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="AC26" s="15">
         <v>1080</v>
       </c>
-      <c r="Y26" s="15">
+      <c r="AD26" s="15">
         <v>720</v>
       </c>
-      <c r="Z26" s="24" t="s">
-        <v>230</v>
+      <c r="AE26" s="24" t="s">
+        <v>221</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A27" s="25">
         <v>13010204</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="C27" s="15">
         <v>2</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="E27" s="15">
         <v>15</v>
@@ -4912,10 +5355,10 @@
         <v>13010201</v>
       </c>
       <c r="G27" s="15" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="H27" s="15" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
       <c r="I27" s="13">
         <v>1</v>
@@ -4930,46 +5373,51 @@
       <c r="O27" s="15"/>
       <c r="P27" s="15"/>
       <c r="Q27" s="15"/>
-      <c r="R27" s="13">
+      <c r="R27" s="15"/>
+      <c r="S27" s="15"/>
+      <c r="T27" s="15"/>
+      <c r="U27" s="15"/>
+      <c r="V27" s="15"/>
+      <c r="W27" s="13">
         <v>4</v>
       </c>
-      <c r="S27" s="13">
-        <v>1</v>
-      </c>
-      <c r="T27" s="13">
+      <c r="X27" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y27" s="13">
         <v>3</v>
       </c>
-      <c r="U27" s="13" t="s">
-        <v>223</v>
-      </c>
-      <c r="V27" s="13" t="s">
-        <v>223</v>
-      </c>
-      <c r="W27" s="15" t="s">
-        <v>199</v>
-      </c>
-      <c r="X27" s="15">
+      <c r="Z27" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="AA27" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="AB27" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="AC27" s="15">
         <v>1074</v>
       </c>
-      <c r="Y27" s="15">
+      <c r="AD27" s="15">
         <v>630</v>
       </c>
-      <c r="Z27" s="24" t="s">
-        <v>230</v>
+      <c r="AE27" s="24" t="s">
+        <v>221</v>
       </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A28" s="25">
         <v>13010205</v>
       </c>
       <c r="B28" s="25" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="C28" s="15">
         <v>2</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="E28" s="15">
         <v>15</v>
@@ -4978,7 +5426,7 @@
         <v>13010201</v>
       </c>
       <c r="G28" s="15" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="H28" s="16"/>
       <c r="I28" s="13">
@@ -4993,47 +5441,52 @@
       <c r="N28" s="16"/>
       <c r="O28" s="15"/>
       <c r="P28" s="15"/>
-      <c r="Q28" s="16"/>
-      <c r="R28" s="13">
+      <c r="Q28" s="15"/>
+      <c r="R28" s="15"/>
+      <c r="S28" s="15"/>
+      <c r="T28" s="15"/>
+      <c r="U28" s="15"/>
+      <c r="V28" s="16"/>
+      <c r="W28" s="13">
         <v>4</v>
       </c>
-      <c r="S28" s="13">
-        <v>1</v>
-      </c>
-      <c r="T28" s="13">
-        <v>2</v>
-      </c>
-      <c r="U28" s="20" t="s">
-        <v>219</v>
-      </c>
-      <c r="V28" s="20" t="s">
-        <v>219</v>
-      </c>
-      <c r="W28" s="16" t="s">
-        <v>204</v>
-      </c>
       <c r="X28" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y28" s="13">
+        <v>2</v>
+      </c>
+      <c r="Z28" s="20" t="s">
+        <v>210</v>
+      </c>
+      <c r="AA28" s="20" t="s">
+        <v>210</v>
+      </c>
+      <c r="AB28" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="AC28" s="13">
         <v>717</v>
       </c>
-      <c r="Y28" s="13">
+      <c r="AD28" s="13">
         <v>655</v>
       </c>
-      <c r="Z28" s="24" t="s">
-        <v>230</v>
+      <c r="AE28" s="24" t="s">
+        <v>221</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A29" s="25">
         <v>13010206</v>
       </c>
       <c r="B29" s="25" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="C29" s="15">
         <v>2</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="E29" s="15">
         <v>15</v>
@@ -5043,7 +5496,7 @@
       </c>
       <c r="G29" s="16"/>
       <c r="H29" s="20" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="I29" s="13">
         <v>1</v>
@@ -5059,47 +5512,52 @@
       </c>
       <c r="O29" s="15"/>
       <c r="P29" s="15"/>
-      <c r="Q29" s="16"/>
-      <c r="R29" s="13">
+      <c r="Q29" s="15"/>
+      <c r="R29" s="15"/>
+      <c r="S29" s="15"/>
+      <c r="T29" s="15"/>
+      <c r="U29" s="15"/>
+      <c r="V29" s="16"/>
+      <c r="W29" s="13">
         <v>4</v>
       </c>
-      <c r="S29" s="13">
-        <v>1</v>
-      </c>
-      <c r="T29" s="13">
-        <v>2</v>
-      </c>
-      <c r="U29" s="20" t="s">
-        <v>225</v>
-      </c>
-      <c r="V29" s="20" t="s">
-        <v>225</v>
-      </c>
-      <c r="W29" s="16" t="s">
-        <v>205</v>
-      </c>
       <c r="X29" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y29" s="13">
+        <v>2</v>
+      </c>
+      <c r="Z29" s="20" t="s">
+        <v>216</v>
+      </c>
+      <c r="AA29" s="20" t="s">
+        <v>216</v>
+      </c>
+      <c r="AB29" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="AC29" s="13">
         <v>637</v>
       </c>
-      <c r="Y29" s="13">
+      <c r="AD29" s="13">
         <v>735</v>
       </c>
-      <c r="Z29" s="24" t="s">
-        <v>230</v>
+      <c r="AE29" s="24" t="s">
+        <v>221</v>
       </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A30" s="25">
         <v>13010207</v>
       </c>
       <c r="B30" s="25" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="C30" s="15">
         <v>2</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="E30" s="15">
         <v>15</v>
@@ -5109,7 +5567,7 @@
       </c>
       <c r="G30" s="15"/>
       <c r="H30" s="15" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="I30" s="13">
         <v>1</v>
@@ -5124,46 +5582,51 @@
         <v>1</v>
       </c>
       <c r="Q30" s="15"/>
-      <c r="R30" s="13">
+      <c r="R30" s="15"/>
+      <c r="S30" s="15"/>
+      <c r="T30" s="15"/>
+      <c r="U30" s="15"/>
+      <c r="V30" s="15"/>
+      <c r="W30" s="13">
         <v>5</v>
       </c>
-      <c r="S30" s="13">
-        <v>1</v>
-      </c>
-      <c r="T30" s="13">
+      <c r="X30" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y30" s="13">
         <v>4</v>
       </c>
-      <c r="U30" s="13" t="s">
-        <v>224</v>
-      </c>
-      <c r="V30" s="13" t="s">
-        <v>224</v>
-      </c>
-      <c r="W30" s="13" t="s">
-        <v>207</v>
-      </c>
-      <c r="X30" s="13">
+      <c r="Z30" s="13" t="s">
+        <v>215</v>
+      </c>
+      <c r="AA30" s="13" t="s">
+        <v>215</v>
+      </c>
+      <c r="AB30" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="AC30" s="13">
         <v>737</v>
       </c>
-      <c r="Y30" s="13">
+      <c r="AD30" s="13">
         <v>785</v>
       </c>
-      <c r="Z30" s="24" t="s">
-        <v>230</v>
+      <c r="AE30" s="24" t="s">
+        <v>221</v>
       </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A31" s="25">
         <v>13010208</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="C31" s="15">
         <v>2</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="E31" s="15">
         <v>15</v>
@@ -5172,10 +5635,10 @@
         <v>13010201</v>
       </c>
       <c r="G31" s="15" t="s">
-        <v>257</v>
+        <v>275</v>
       </c>
       <c r="H31" s="15" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="I31" s="13">
         <v>1</v>
@@ -5192,46 +5655,53 @@
       <c r="O31" s="15"/>
       <c r="P31" s="15"/>
       <c r="Q31" s="15"/>
-      <c r="R31" s="13">
+      <c r="R31" s="15"/>
+      <c r="S31" s="15"/>
+      <c r="T31" s="15"/>
+      <c r="U31" s="15">
+        <v>1</v>
+      </c>
+      <c r="V31" s="15"/>
+      <c r="W31" s="13">
         <v>4</v>
       </c>
-      <c r="S31" s="13">
-        <v>1</v>
-      </c>
-      <c r="T31" s="13">
-        <v>2</v>
-      </c>
-      <c r="U31" s="13" t="s">
-        <v>217</v>
-      </c>
-      <c r="V31" s="13" t="s">
-        <v>217</v>
-      </c>
-      <c r="W31" s="15" t="s">
-        <v>200</v>
-      </c>
-      <c r="X31" s="19">
+      <c r="X31" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y31" s="13">
+        <v>2</v>
+      </c>
+      <c r="Z31" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="AA31" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="AB31" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="AC31" s="19">
         <v>894</v>
       </c>
-      <c r="Y31" s="19">
+      <c r="AD31" s="19">
         <v>679</v>
       </c>
-      <c r="Z31" s="24" t="s">
-        <v>230</v>
+      <c r="AE31" s="24" t="s">
+        <v>221</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A32" s="25">
         <v>13010209</v>
       </c>
       <c r="B32" s="25" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="C32" s="15">
         <v>2</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="E32" s="15">
         <v>15</v>
@@ -5239,11 +5709,9 @@
       <c r="F32" s="15">
         <v>13010201</v>
       </c>
-      <c r="G32" s="20" t="s">
-        <v>250</v>
-      </c>
+      <c r="G32" s="20"/>
       <c r="H32" s="20" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="I32" s="13">
         <v>1</v>
@@ -5257,36 +5725,43 @@
         <v>1</v>
       </c>
       <c r="P32" s="15"/>
-      <c r="Q32" s="16"/>
-      <c r="R32" s="13">
+      <c r="Q32" s="15"/>
+      <c r="R32" s="15"/>
+      <c r="S32" s="15">
+        <v>1</v>
+      </c>
+      <c r="T32" s="15"/>
+      <c r="U32" s="15"/>
+      <c r="V32" s="16"/>
+      <c r="W32" s="13">
         <v>4</v>
       </c>
-      <c r="S32" s="13">
-        <v>2</v>
-      </c>
-      <c r="T32" s="13">
-        <v>2</v>
-      </c>
-      <c r="U32" s="20" t="s">
-        <v>226</v>
-      </c>
-      <c r="V32" s="20" t="s">
-        <v>226</v>
-      </c>
-      <c r="W32" s="16" t="s">
-        <v>201</v>
-      </c>
-      <c r="X32" s="19">
+      <c r="X32" s="13">
+        <v>2</v>
+      </c>
+      <c r="Y32" s="13">
+        <v>2</v>
+      </c>
+      <c r="Z32" s="20" t="s">
+        <v>217</v>
+      </c>
+      <c r="AA32" s="20" t="s">
+        <v>217</v>
+      </c>
+      <c r="AB32" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="AC32" s="19">
         <v>984</v>
       </c>
-      <c r="Y32" s="19">
+      <c r="AD32" s="19">
         <v>734</v>
       </c>
-      <c r="Z32" s="24" t="s">
-        <v>230</v>
+      <c r="AE32" s="24" t="s">
+        <v>221</v>
       </c>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A33" s="28">
         <v>13010301</v>
       </c>
@@ -5297,7 +5772,7 @@
         <v>2</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="E33" s="13">
         <v>14</v>
@@ -5305,11 +5780,11 @@
       <c r="F33" s="13">
         <v>13010006</v>
       </c>
-      <c r="G33" s="13" t="s">
-        <v>159</v>
+      <c r="G33" s="20" t="s">
+        <v>279</v>
       </c>
       <c r="H33" s="13" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="I33" s="13">
         <v>1</v>
@@ -5327,34 +5802,41 @@
       <c r="P33" s="13"/>
       <c r="Q33" s="13"/>
       <c r="R33" s="13">
+        <v>1</v>
+      </c>
+      <c r="S33" s="13"/>
+      <c r="T33" s="13"/>
+      <c r="U33" s="13"/>
+      <c r="V33" s="13"/>
+      <c r="W33" s="13">
         <v>3</v>
       </c>
-      <c r="S33" s="13">
+      <c r="X33" s="13">
         <v>3</v>
       </c>
-      <c r="T33" s="13">
-        <v>1</v>
-      </c>
-      <c r="U33" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="V33" s="13" t="s">
+      <c r="Y33" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z33" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="AA33" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="W33" s="13" t="s">
+      <c r="AB33" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="X33" s="21">
+      <c r="AC33" s="21">
         <v>1550</v>
       </c>
-      <c r="Y33" s="21">
+      <c r="AD33" s="21">
         <v>505</v>
       </c>
-      <c r="Z33" s="24" t="s">
-        <v>232</v>
+      <c r="AE33" s="24" t="s">
+        <v>223</v>
       </c>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A34" s="28">
         <v>13010302</v>
       </c>
@@ -5365,7 +5847,7 @@
         <v>2</v>
       </c>
       <c r="D34" s="20" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="E34" s="13">
         <v>10</v>
@@ -5374,10 +5856,10 @@
         <v>13010006</v>
       </c>
       <c r="G34" s="13" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="H34" s="13" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="I34" s="13">
         <v>1</v>
@@ -5394,35 +5876,40 @@
       </c>
       <c r="P34" s="13"/>
       <c r="Q34" s="13"/>
-      <c r="R34" s="13">
+      <c r="R34" s="13"/>
+      <c r="S34" s="13"/>
+      <c r="T34" s="13"/>
+      <c r="U34" s="13"/>
+      <c r="V34" s="13"/>
+      <c r="W34" s="13">
         <v>4</v>
       </c>
-      <c r="S34" s="13">
+      <c r="X34" s="13">
         <v>3</v>
       </c>
-      <c r="T34" s="13">
-        <v>1</v>
-      </c>
-      <c r="U34" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="V34" s="13" t="s">
+      <c r="Y34" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z34" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="AA34" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="W34" s="13" t="s">
+      <c r="AB34" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="X34" s="21">
+      <c r="AC34" s="21">
         <v>1441</v>
       </c>
-      <c r="Y34" s="21">
+      <c r="AD34" s="21">
         <v>527</v>
       </c>
-      <c r="Z34" s="24" t="s">
-        <v>232</v>
+      <c r="AE34" s="24" t="s">
+        <v>223</v>
       </c>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A35" s="28">
         <v>13010303</v>
       </c>
@@ -5433,7 +5920,7 @@
         <v>2</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="E35" s="13">
         <v>12</v>
@@ -5442,10 +5929,10 @@
         <v>13010006</v>
       </c>
       <c r="G35" s="13" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="H35" s="13" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="I35" s="13">
         <v>1</v>
@@ -5462,40 +5949,45 @@
         <v>1</v>
       </c>
       <c r="Q35" s="13"/>
-      <c r="R35" s="13">
+      <c r="R35" s="13"/>
+      <c r="S35" s="13"/>
+      <c r="T35" s="13"/>
+      <c r="U35" s="13"/>
+      <c r="V35" s="13"/>
+      <c r="W35" s="13">
         <v>3</v>
       </c>
-      <c r="S35" s="13">
+      <c r="X35" s="13">
         <v>3</v>
       </c>
-      <c r="T35" s="13">
-        <v>2</v>
-      </c>
-      <c r="U35" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="V35" s="13" t="s">
+      <c r="Y35" s="13">
+        <v>2</v>
+      </c>
+      <c r="Z35" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="AA35" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="W35" s="13" t="s">
+      <c r="AB35" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="X35" s="21">
+      <c r="AC35" s="21">
         <v>1574</v>
       </c>
-      <c r="Y35" s="21">
+      <c r="AD35" s="21">
         <v>373</v>
       </c>
-      <c r="Z35" s="24" t="s">
-        <v>232</v>
+      <c r="AE35" s="24" t="s">
+        <v>223</v>
       </c>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A36" s="17">
         <v>13020001</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C36" s="13">
         <v>3</v>
@@ -5508,7 +6000,7 @@
         <v>13010002</v>
       </c>
       <c r="G36" s="20" t="s">
-        <v>269</v>
+        <v>253</v>
       </c>
       <c r="H36" s="13"/>
       <c r="I36" s="13"/>
@@ -5522,32 +6014,37 @@
       <c r="O36" s="13"/>
       <c r="P36" s="13"/>
       <c r="Q36" s="13"/>
-      <c r="R36" s="13">
-        <v>2</v>
-      </c>
-      <c r="S36" s="13">
+      <c r="R36" s="13"/>
+      <c r="S36" s="13"/>
+      <c r="T36" s="13"/>
+      <c r="U36" s="13"/>
+      <c r="V36" s="13"/>
+      <c r="W36" s="13">
+        <v>2</v>
+      </c>
+      <c r="X36" s="13">
         <v>3</v>
       </c>
-      <c r="T36" s="13">
-        <v>2</v>
-      </c>
-      <c r="U36" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="V36" s="13" t="s">
-        <v>149</v>
-      </c>
-      <c r="W36" s="13"/>
-      <c r="X36" s="13"/>
-      <c r="Y36" s="13"/>
-      <c r="Z36" s="22"/>
+      <c r="Y36" s="13">
+        <v>2</v>
+      </c>
+      <c r="Z36" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="AA36" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="AB36" s="13"/>
+      <c r="AC36" s="13"/>
+      <c r="AD36" s="13"/>
+      <c r="AE36" s="22"/>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A37" s="17">
         <v>13020002</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C37" s="13">
         <v>3</v>
@@ -5570,32 +6067,37 @@
       <c r="O37" s="13"/>
       <c r="P37" s="13"/>
       <c r="Q37" s="13"/>
-      <c r="R37" s="13">
-        <v>2</v>
-      </c>
-      <c r="S37" s="13">
+      <c r="R37" s="13"/>
+      <c r="S37" s="13"/>
+      <c r="T37" s="13"/>
+      <c r="U37" s="13"/>
+      <c r="V37" s="13"/>
+      <c r="W37" s="13">
+        <v>2</v>
+      </c>
+      <c r="X37" s="13">
         <v>3</v>
       </c>
-      <c r="T37" s="13">
-        <v>2</v>
-      </c>
-      <c r="U37" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="V37" s="13" t="s">
-        <v>150</v>
-      </c>
-      <c r="W37" s="13"/>
-      <c r="X37" s="13"/>
-      <c r="Y37" s="13"/>
-      <c r="Z37" s="22"/>
+      <c r="Y37" s="13">
+        <v>2</v>
+      </c>
+      <c r="Z37" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA37" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="AB37" s="13"/>
+      <c r="AC37" s="13"/>
+      <c r="AD37" s="13"/>
+      <c r="AE37" s="22"/>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A38" s="17">
         <v>13020011</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C38" s="13">
         <v>3</v>
@@ -5608,10 +6110,10 @@
         <v>13010007</v>
       </c>
       <c r="G38" s="13" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="H38" s="13" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="I38" s="13"/>
       <c r="J38" s="13"/>
@@ -5622,32 +6124,37 @@
       <c r="O38" s="13"/>
       <c r="P38" s="13"/>
       <c r="Q38" s="13"/>
-      <c r="R38" s="13">
-        <v>2</v>
-      </c>
-      <c r="S38" s="13">
+      <c r="R38" s="13"/>
+      <c r="S38" s="13"/>
+      <c r="T38" s="13"/>
+      <c r="U38" s="13"/>
+      <c r="V38" s="13"/>
+      <c r="W38" s="13">
+        <v>2</v>
+      </c>
+      <c r="X38" s="13">
         <v>4</v>
       </c>
-      <c r="T38" s="13">
-        <v>2</v>
-      </c>
-      <c r="U38" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="V38" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="W38" s="13"/>
-      <c r="X38" s="13"/>
-      <c r="Y38" s="13"/>
-      <c r="Z38" s="22"/>
+      <c r="Y38" s="13">
+        <v>2</v>
+      </c>
+      <c r="Z38" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA38" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="AB38" s="13"/>
+      <c r="AC38" s="13"/>
+      <c r="AD38" s="13"/>
+      <c r="AE38" s="22"/>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A39" s="17">
         <v>13020012</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C39" s="13">
         <v>3</v>
@@ -5660,7 +6167,7 @@
         <v>13010007</v>
       </c>
       <c r="G39" s="13" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="H39" s="13"/>
       <c r="I39" s="13"/>
@@ -5672,32 +6179,37 @@
       <c r="O39" s="13"/>
       <c r="P39" s="13"/>
       <c r="Q39" s="13"/>
-      <c r="R39" s="13">
-        <v>2</v>
-      </c>
-      <c r="S39" s="13">
+      <c r="R39" s="13"/>
+      <c r="S39" s="13"/>
+      <c r="T39" s="13"/>
+      <c r="U39" s="13"/>
+      <c r="V39" s="13"/>
+      <c r="W39" s="13">
+        <v>2</v>
+      </c>
+      <c r="X39" s="13">
         <v>4</v>
       </c>
-      <c r="T39" s="13">
-        <v>2</v>
-      </c>
-      <c r="U39" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="V39" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="W39" s="13"/>
-      <c r="X39" s="13"/>
-      <c r="Y39" s="13"/>
-      <c r="Z39" s="22"/>
+      <c r="Y39" s="13">
+        <v>2</v>
+      </c>
+      <c r="Z39" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="AA39" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="AB39" s="13"/>
+      <c r="AC39" s="13"/>
+      <c r="AD39" s="13"/>
+      <c r="AE39" s="22"/>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A40" s="17">
         <v>13020013</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C40" s="13">
         <v>3</v>
@@ -5720,32 +6232,37 @@
       <c r="O40" s="13"/>
       <c r="P40" s="13"/>
       <c r="Q40" s="13"/>
-      <c r="R40" s="13">
-        <v>2</v>
-      </c>
-      <c r="S40" s="13">
+      <c r="R40" s="13"/>
+      <c r="S40" s="13"/>
+      <c r="T40" s="13"/>
+      <c r="U40" s="13"/>
+      <c r="V40" s="13"/>
+      <c r="W40" s="13">
+        <v>2</v>
+      </c>
+      <c r="X40" s="13">
         <v>4</v>
       </c>
-      <c r="T40" s="13">
-        <v>2</v>
-      </c>
-      <c r="U40" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="V40" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="W40" s="13"/>
-      <c r="X40" s="13"/>
-      <c r="Y40" s="13"/>
-      <c r="Z40" s="22"/>
+      <c r="Y40" s="13">
+        <v>2</v>
+      </c>
+      <c r="Z40" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="AA40" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="AB40" s="13"/>
+      <c r="AC40" s="13"/>
+      <c r="AD40" s="13"/>
+      <c r="AE40" s="22"/>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A41" s="17">
         <v>13020021</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C41" s="13">
         <v>3</v>
@@ -5758,10 +6275,10 @@
         <v>13010004</v>
       </c>
       <c r="G41" s="13" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="H41" s="13" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="I41" s="13"/>
       <c r="J41" s="13"/>
@@ -5772,32 +6289,37 @@
       <c r="O41" s="13"/>
       <c r="P41" s="13"/>
       <c r="Q41" s="13"/>
-      <c r="R41" s="13">
+      <c r="R41" s="13"/>
+      <c r="S41" s="13"/>
+      <c r="T41" s="13"/>
+      <c r="U41" s="13"/>
+      <c r="V41" s="13"/>
+      <c r="W41" s="13">
         <v>3</v>
       </c>
-      <c r="S41" s="13">
+      <c r="X41" s="13">
         <v>3</v>
       </c>
-      <c r="T41" s="13">
-        <v>1</v>
-      </c>
-      <c r="U41" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="V41" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="W41" s="13"/>
-      <c r="X41" s="13"/>
-      <c r="Y41" s="13"/>
-      <c r="Z41" s="22"/>
+      <c r="Y41" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z41" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="AA41" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="AB41" s="13"/>
+      <c r="AC41" s="13"/>
+      <c r="AD41" s="13"/>
+      <c r="AE41" s="22"/>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A42" s="17">
         <v>13020022</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C42" s="13">
         <v>3</v>
@@ -5810,10 +6332,10 @@
         <v>13010004</v>
       </c>
       <c r="G42" s="20" t="s">
-        <v>268</v>
+        <v>252</v>
       </c>
       <c r="H42" s="13" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="I42" s="13"/>
       <c r="J42" s="13"/>
@@ -5824,32 +6346,37 @@
       <c r="O42" s="13"/>
       <c r="P42" s="13"/>
       <c r="Q42" s="13"/>
-      <c r="R42" s="13">
+      <c r="R42" s="13"/>
+      <c r="S42" s="13"/>
+      <c r="T42" s="13"/>
+      <c r="U42" s="13"/>
+      <c r="V42" s="13"/>
+      <c r="W42" s="13">
         <v>3</v>
       </c>
-      <c r="S42" s="13">
+      <c r="X42" s="13">
         <v>3</v>
       </c>
-      <c r="T42" s="13">
-        <v>1</v>
-      </c>
-      <c r="U42" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="V42" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="W42" s="13"/>
-      <c r="X42" s="13"/>
-      <c r="Y42" s="13"/>
-      <c r="Z42" s="22"/>
+      <c r="Y42" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z42" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="AA42" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="AB42" s="13"/>
+      <c r="AC42" s="13"/>
+      <c r="AD42" s="13"/>
+      <c r="AE42" s="22"/>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A43" s="17">
         <v>13020023</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C43" s="13">
         <v>3</v>
@@ -5862,10 +6389,10 @@
         <v>13010004</v>
       </c>
       <c r="G43" s="20" t="s">
-        <v>267</v>
+        <v>251</v>
       </c>
       <c r="H43" s="13" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="I43" s="13"/>
       <c r="J43" s="13"/>
@@ -5876,32 +6403,37 @@
       <c r="O43" s="13"/>
       <c r="P43" s="13"/>
       <c r="Q43" s="13"/>
-      <c r="R43" s="13">
+      <c r="R43" s="13"/>
+      <c r="S43" s="13"/>
+      <c r="T43" s="13"/>
+      <c r="U43" s="13"/>
+      <c r="V43" s="13"/>
+      <c r="W43" s="13">
         <v>3</v>
       </c>
-      <c r="S43" s="13">
+      <c r="X43" s="13">
         <v>3</v>
       </c>
-      <c r="T43" s="13">
-        <v>1</v>
-      </c>
-      <c r="U43" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="V43" s="13" t="s">
-        <v>156</v>
-      </c>
-      <c r="W43" s="13"/>
-      <c r="X43" s="13"/>
-      <c r="Y43" s="13"/>
-      <c r="Z43" s="22"/>
+      <c r="Y43" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z43" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="AA43" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="AB43" s="13"/>
+      <c r="AC43" s="13"/>
+      <c r="AD43" s="13"/>
+      <c r="AE43" s="22"/>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A44" s="18">
         <v>13020031</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="C44" s="13">
         <v>3</v>
@@ -5924,32 +6456,37 @@
       <c r="O44" s="15"/>
       <c r="P44" s="15"/>
       <c r="Q44" s="15"/>
-      <c r="R44" s="13">
-        <v>2</v>
-      </c>
-      <c r="S44" s="13">
-        <v>2</v>
-      </c>
-      <c r="T44" s="13">
+      <c r="R44" s="15"/>
+      <c r="S44" s="15"/>
+      <c r="T44" s="15"/>
+      <c r="U44" s="15"/>
+      <c r="V44" s="15"/>
+      <c r="W44" s="13">
+        <v>2</v>
+      </c>
+      <c r="X44" s="13">
+        <v>2</v>
+      </c>
+      <c r="Y44" s="13">
         <v>5</v>
       </c>
-      <c r="U44" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="V44" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="W44" s="15"/>
-      <c r="X44" s="15"/>
-      <c r="Y44" s="15"/>
-      <c r="Z44" s="22"/>
+      <c r="Z44" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA44" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="AB44" s="15"/>
+      <c r="AC44" s="15"/>
+      <c r="AD44" s="15"/>
+      <c r="AE44" s="22"/>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A45" s="18">
         <v>13020032</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="C45" s="13">
         <v>3</v>
@@ -5972,32 +6509,37 @@
       <c r="O45" s="15"/>
       <c r="P45" s="15"/>
       <c r="Q45" s="15"/>
-      <c r="R45" s="13">
-        <v>2</v>
-      </c>
-      <c r="S45" s="13">
-        <v>2</v>
-      </c>
-      <c r="T45" s="13">
+      <c r="R45" s="15"/>
+      <c r="S45" s="15"/>
+      <c r="T45" s="15"/>
+      <c r="U45" s="15"/>
+      <c r="V45" s="15"/>
+      <c r="W45" s="13">
+        <v>2</v>
+      </c>
+      <c r="X45" s="13">
+        <v>2</v>
+      </c>
+      <c r="Y45" s="13">
         <v>5</v>
       </c>
-      <c r="U45" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="V45" s="15" t="s">
-        <v>175</v>
-      </c>
-      <c r="W45" s="15"/>
-      <c r="X45" s="15"/>
-      <c r="Y45" s="15"/>
-      <c r="Z45" s="22"/>
+      <c r="Z45" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA45" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="AB45" s="15"/>
+      <c r="AC45" s="15"/>
+      <c r="AD45" s="15"/>
+      <c r="AE45" s="22"/>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A46" s="18">
         <v>13020033</v>
       </c>
       <c r="B46" s="17" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="C46" s="13">
         <v>3</v>
@@ -6020,32 +6562,37 @@
       <c r="O46" s="15"/>
       <c r="P46" s="15"/>
       <c r="Q46" s="15"/>
-      <c r="R46" s="13">
-        <v>2</v>
-      </c>
-      <c r="S46" s="13">
-        <v>2</v>
-      </c>
-      <c r="T46" s="13">
+      <c r="R46" s="15"/>
+      <c r="S46" s="15"/>
+      <c r="T46" s="15"/>
+      <c r="U46" s="15"/>
+      <c r="V46" s="15"/>
+      <c r="W46" s="13">
+        <v>2</v>
+      </c>
+      <c r="X46" s="13">
+        <v>2</v>
+      </c>
+      <c r="Y46" s="13">
         <v>5</v>
       </c>
-      <c r="U46" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="V46" s="15" t="s">
-        <v>176</v>
-      </c>
-      <c r="W46" s="19"/>
-      <c r="X46" s="19"/>
-      <c r="Y46" s="19"/>
-      <c r="Z46" s="22"/>
+      <c r="Z46" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA46" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="AB46" s="19"/>
+      <c r="AC46" s="19"/>
+      <c r="AD46" s="19"/>
+      <c r="AE46" s="22"/>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A47" s="18">
         <v>13020034</v>
       </c>
       <c r="B47" s="17" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C47" s="13">
         <v>3</v>
@@ -6068,32 +6615,37 @@
       <c r="O47" s="15"/>
       <c r="P47" s="15"/>
       <c r="Q47" s="15"/>
-      <c r="R47" s="13">
-        <v>2</v>
-      </c>
-      <c r="S47" s="13">
-        <v>2</v>
-      </c>
-      <c r="T47" s="13">
+      <c r="R47" s="15"/>
+      <c r="S47" s="15"/>
+      <c r="T47" s="15"/>
+      <c r="U47" s="15"/>
+      <c r="V47" s="15"/>
+      <c r="W47" s="13">
+        <v>2</v>
+      </c>
+      <c r="X47" s="13">
+        <v>2</v>
+      </c>
+      <c r="Y47" s="13">
         <v>5</v>
       </c>
-      <c r="U47" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="V47" s="15" t="s">
-        <v>177</v>
-      </c>
-      <c r="W47" s="19"/>
-      <c r="X47" s="19"/>
-      <c r="Y47" s="19"/>
-      <c r="Z47" s="22"/>
+      <c r="Z47" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA47" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="AB47" s="19"/>
+      <c r="AC47" s="19"/>
+      <c r="AD47" s="19"/>
+      <c r="AE47" s="22"/>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A48" s="18">
         <v>13020035</v>
       </c>
       <c r="B48" s="17" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="C48" s="13">
         <v>3</v>
@@ -6116,40 +6668,45 @@
       <c r="O48" s="15"/>
       <c r="P48" s="15"/>
       <c r="Q48" s="15"/>
-      <c r="R48" s="13">
-        <v>2</v>
-      </c>
-      <c r="S48" s="13">
-        <v>2</v>
-      </c>
-      <c r="T48" s="13">
+      <c r="R48" s="15"/>
+      <c r="S48" s="15"/>
+      <c r="T48" s="15"/>
+      <c r="U48" s="15"/>
+      <c r="V48" s="15"/>
+      <c r="W48" s="13">
+        <v>2</v>
+      </c>
+      <c r="X48" s="13">
+        <v>2</v>
+      </c>
+      <c r="Y48" s="13">
         <v>5</v>
       </c>
-      <c r="U48" s="13" t="s">
+      <c r="Z48" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA48" s="15" t="s">
         <v>169</v>
       </c>
-      <c r="V48" s="15" t="s">
-        <v>178</v>
-      </c>
-      <c r="W48" s="19"/>
-      <c r="X48" s="19"/>
-      <c r="Y48" s="19"/>
-      <c r="Z48" s="22"/>
+      <c r="AB48" s="19"/>
+      <c r="AC48" s="19"/>
+      <c r="AD48" s="19"/>
+      <c r="AE48" s="22"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="I4:P48">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+  <conditionalFormatting sqref="I4:U48">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:H48">
-    <cfRule type="containsBlanks" dxfId="1" priority="5">
+    <cfRule type="containsBlanks" dxfId="0" priority="5">
       <formula>LEN(TRIM(G4))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
fix the scene quest data
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Scene.xlsx
+++ b/ConfigData/Xlsx/Scene.xlsx
@@ -1020,10 +1020,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>float</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>sewer;3|river;2|fortune;1|poppyfield;1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -1073,6 +1069,10 @@
   </si>
   <si>
     <t>trees;3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>double</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1993,27 +1993,6 @@
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="36">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2908,6 +2887,27 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -2990,42 +2990,42 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AD48" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34" tableBorderDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AD48" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31" tableBorderDxfId="30">
   <autoFilter ref="A3:AD48"/>
   <sortState ref="A4:AD48">
     <sortCondition ref="A3:A48"/>
   </sortState>
   <tableColumns count="30">
-    <tableColumn id="1" name="Id" dataDxfId="32"/>
-    <tableColumn id="2" name="Name" dataDxfId="31"/>
-    <tableColumn id="18" name="Type" dataDxfId="30"/>
-    <tableColumn id="25" name="Sector" dataDxfId="29"/>
-    <tableColumn id="3" name="Level" dataDxfId="28"/>
-    <tableColumn id="20" name="ReviveScene" dataDxfId="27"/>
-    <tableColumn id="4" name="Quest" dataDxfId="26"/>
-    <tableColumn id="17" name="QuestRandom" dataDxfId="25"/>
-    <tableColumn id="5" name="QPortal" dataDxfId="24"/>
-    <tableColumn id="6" name="QCardChange" dataDxfId="23"/>
-    <tableColumn id="7" name="QPiece" dataDxfId="22"/>
-    <tableColumn id="8" name="QMerchant" dataDxfId="21"/>
-    <tableColumn id="9" name="QDoctor" dataDxfId="20"/>
-    <tableColumn id="10" name="QAngel" dataDxfId="19"/>
-    <tableColumn id="21" name="QWheel" dataDxfId="18"/>
-    <tableColumn id="22" name="QRes" dataDxfId="17"/>
-    <tableColumn id="27" name="QItemDrug" dataDxfId="16"/>
-    <tableColumn id="31" name="QItemFish" dataDxfId="15"/>
-    <tableColumn id="30" name="QItemOre" dataDxfId="14"/>
-    <tableColumn id="28" name="QItemMushroom" dataDxfId="13"/>
-    <tableColumn id="29" name="QItemWood" dataDxfId="12"/>
-    <tableColumn id="19" name="Temperature" dataDxfId="11"/>
-    <tableColumn id="23" name="Humitity" dataDxfId="10"/>
-    <tableColumn id="26" name="Altitude" dataDxfId="9"/>
-    <tableColumn id="12" name="Url" dataDxfId="8"/>
-    <tableColumn id="13" name="TilePath" dataDxfId="7"/>
-    <tableColumn id="14" name="Icon" dataDxfId="6"/>
-    <tableColumn id="15" name="IconX" dataDxfId="5"/>
-    <tableColumn id="16" name="IconY" dataDxfId="4"/>
-    <tableColumn id="24" name="IconColor" dataDxfId="3"/>
+    <tableColumn id="1" name="Id" dataDxfId="29"/>
+    <tableColumn id="2" name="Name" dataDxfId="28"/>
+    <tableColumn id="18" name="Type" dataDxfId="27"/>
+    <tableColumn id="25" name="Sector" dataDxfId="26"/>
+    <tableColumn id="3" name="Level" dataDxfId="25"/>
+    <tableColumn id="20" name="ReviveScene" dataDxfId="24"/>
+    <tableColumn id="4" name="Quest" dataDxfId="23"/>
+    <tableColumn id="17" name="QuestRandom" dataDxfId="22"/>
+    <tableColumn id="5" name="QPortal" dataDxfId="21"/>
+    <tableColumn id="6" name="QCardChange" dataDxfId="20"/>
+    <tableColumn id="7" name="QPiece" dataDxfId="19"/>
+    <tableColumn id="8" name="QMerchant" dataDxfId="18"/>
+    <tableColumn id="9" name="QDoctor" dataDxfId="17"/>
+    <tableColumn id="10" name="QAngel" dataDxfId="16"/>
+    <tableColumn id="21" name="QWheel" dataDxfId="15"/>
+    <tableColumn id="22" name="QRes" dataDxfId="14"/>
+    <tableColumn id="27" name="QItemDrug" dataDxfId="13"/>
+    <tableColumn id="31" name="QItemFish" dataDxfId="12"/>
+    <tableColumn id="30" name="QItemOre" dataDxfId="11"/>
+    <tableColumn id="28" name="QItemMushroom" dataDxfId="10"/>
+    <tableColumn id="29" name="QItemWood" dataDxfId="9"/>
+    <tableColumn id="19" name="Temperature" dataDxfId="8"/>
+    <tableColumn id="23" name="Humitity" dataDxfId="7"/>
+    <tableColumn id="26" name="Altitude" dataDxfId="6"/>
+    <tableColumn id="12" name="Url" dataDxfId="5"/>
+    <tableColumn id="13" name="TilePath" dataDxfId="4"/>
+    <tableColumn id="14" name="Icon" dataDxfId="3"/>
+    <tableColumn id="15" name="IconX" dataDxfId="2"/>
+    <tableColumn id="16" name="IconY" dataDxfId="1"/>
+    <tableColumn id="24" name="IconColor" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3355,7 +3355,7 @@
   <dimension ref="A1:AD48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB4" sqref="AB4"/>
+      <selection activeCell="Q2" sqref="Q2:U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3524,19 +3524,19 @@
         <v>179</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>269</v>
+        <v>282</v>
       </c>
       <c r="R2" s="8" t="s">
-        <v>269</v>
+        <v>282</v>
       </c>
       <c r="S2" s="8" t="s">
-        <v>269</v>
+        <v>282</v>
       </c>
       <c r="T2" s="8" t="s">
-        <v>269</v>
+        <v>282</v>
       </c>
       <c r="U2" s="8" t="s">
-        <v>269</v>
+        <v>282</v>
       </c>
       <c r="V2" s="33" t="s">
         <v>253</v>
@@ -3678,7 +3678,7 @@
         <v>13010001</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="H4" s="14" t="s">
         <v>170</v>
@@ -3752,7 +3752,7 @@
         <v>13010001</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="H5" s="13" t="s">
         <v>128</v>
@@ -3832,7 +3832,7 @@
         <v>13010006</v>
       </c>
       <c r="G6" s="20" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="H6" s="13" t="s">
         <v>131</v>
@@ -3904,7 +3904,7 @@
         <v>13010006</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="H7" s="13" t="s">
         <v>135</v>
@@ -4116,7 +4116,7 @@
         <v>13010006</v>
       </c>
       <c r="G10" s="20" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="H10" s="13" t="s">
         <v>152</v>
@@ -4348,7 +4348,7 @@
         <v>13010006</v>
       </c>
       <c r="G13" s="20" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H13" s="13" t="s">
         <v>148</v>
@@ -4556,7 +4556,7 @@
         <v>13010101</v>
       </c>
       <c r="G16" s="20" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="H16" s="20" t="s">
         <v>174</v>
@@ -4632,7 +4632,7 @@
         <v>13010101</v>
       </c>
       <c r="G17" s="20" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="H17" s="13" t="s">
         <v>129</v>
@@ -4708,7 +4708,7 @@
         <v>13010101</v>
       </c>
       <c r="G18" s="20" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H18" s="20" t="s">
         <v>238</v>
@@ -4784,7 +4784,7 @@
         <v>13010016</v>
       </c>
       <c r="G19" s="20" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H19" s="13" t="s">
         <v>133</v>
@@ -4862,7 +4862,7 @@
         <v>13010101</v>
       </c>
       <c r="G20" s="20" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="H20" s="20" t="s">
         <v>241</v>
@@ -5674,7 +5674,7 @@
         <v>13010201</v>
       </c>
       <c r="G31" s="15" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="H31" s="15" t="s">
         <v>237</v>
@@ -5824,7 +5824,7 @@
         <v>13010006</v>
       </c>
       <c r="G33" s="20" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="H33" s="13" t="s">
         <v>153</v>
@@ -6771,17 +6771,17 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="I4:U48">
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:H48">
-    <cfRule type="containsBlanks" dxfId="0" priority="5">
+    <cfRule type="containsBlanks" dxfId="33" priority="5">
       <formula>LEN(TRIM(G4))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
support differ bgm on differ scene
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Scene.xlsx
+++ b/ConfigData/Xlsx/Scene.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="278">
   <si>
     <t>村外小屋</t>
   </si>
@@ -1035,13 +1035,31 @@
   <si>
     <t>RegionId</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>背景音乐</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>BGM</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SCN001</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SCN002</t>
+  </si>
+  <si>
+    <t>SCN003</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1256,6 +1274,15 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
@@ -1796,7 +1823,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1900,6 +1927,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1947,28 +1977,7 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="35">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="36">
     <dxf>
       <font>
         <b val="0"/>
@@ -1984,19 +1993,8 @@
         <color theme="1"/>
         <name val="宋体"/>
         <family val="3"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -2707,6 +2705,35 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -2830,76 +2857,29 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2912,41 +2892,42 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AC48" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33" tableBorderDxfId="32">
-  <autoFilter ref="A3:AC48"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AD48" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31" tableBorderDxfId="30">
+  <autoFilter ref="A3:AD48"/>
   <sortState ref="A4:AC48">
     <sortCondition ref="A3:A48"/>
   </sortState>
-  <tableColumns count="29">
-    <tableColumn id="1" name="Id" dataDxfId="31"/>
-    <tableColumn id="2" name="Name" dataDxfId="30"/>
-    <tableColumn id="18" name="Type" dataDxfId="29"/>
-    <tableColumn id="11" name="RegionId" dataDxfId="3"/>
-    <tableColumn id="3" name="Level" dataDxfId="28"/>
-    <tableColumn id="20" name="ReviveScene" dataDxfId="27"/>
-    <tableColumn id="4" name="Quest" dataDxfId="26"/>
-    <tableColumn id="17" name="QuestRandom" dataDxfId="25"/>
-    <tableColumn id="5" name="QPortal" dataDxfId="24"/>
-    <tableColumn id="6" name="QCardChange" dataDxfId="23"/>
-    <tableColumn id="7" name="QPiece" dataDxfId="22"/>
-    <tableColumn id="8" name="QMerchant" dataDxfId="21"/>
-    <tableColumn id="9" name="QDoctor" dataDxfId="20"/>
-    <tableColumn id="10" name="QAngel" dataDxfId="19"/>
-    <tableColumn id="21" name="QWheel" dataDxfId="18"/>
-    <tableColumn id="22" name="QRes" dataDxfId="17"/>
-    <tableColumn id="27" name="QItemDrug" dataDxfId="16"/>
-    <tableColumn id="31" name="QItemFish" dataDxfId="15"/>
-    <tableColumn id="30" name="QItemOre" dataDxfId="14"/>
-    <tableColumn id="28" name="QItemMushroom" dataDxfId="13"/>
-    <tableColumn id="29" name="QItemWood" dataDxfId="12"/>
-    <tableColumn id="19" name="Temperature" dataDxfId="11"/>
-    <tableColumn id="23" name="Humitity" dataDxfId="10"/>
-    <tableColumn id="26" name="Altitude" dataDxfId="9"/>
-    <tableColumn id="12" name="Url" dataDxfId="8"/>
-    <tableColumn id="13" name="TilePath" dataDxfId="7"/>
-    <tableColumn id="14" name="Icon" dataDxfId="6"/>
-    <tableColumn id="15" name="IconX" dataDxfId="5"/>
-    <tableColumn id="16" name="IconY" dataDxfId="4"/>
+  <tableColumns count="30">
+    <tableColumn id="1" name="Id" dataDxfId="29"/>
+    <tableColumn id="2" name="Name" dataDxfId="28"/>
+    <tableColumn id="18" name="Type" dataDxfId="27"/>
+    <tableColumn id="11" name="RegionId" dataDxfId="26"/>
+    <tableColumn id="3" name="Level" dataDxfId="25"/>
+    <tableColumn id="20" name="ReviveScene" dataDxfId="24"/>
+    <tableColumn id="4" name="Quest" dataDxfId="23"/>
+    <tableColumn id="17" name="QuestRandom" dataDxfId="22"/>
+    <tableColumn id="5" name="QPortal" dataDxfId="21"/>
+    <tableColumn id="6" name="QCardChange" dataDxfId="20"/>
+    <tableColumn id="7" name="QPiece" dataDxfId="19"/>
+    <tableColumn id="8" name="QMerchant" dataDxfId="18"/>
+    <tableColumn id="9" name="QDoctor" dataDxfId="17"/>
+    <tableColumn id="10" name="QAngel" dataDxfId="16"/>
+    <tableColumn id="21" name="QWheel" dataDxfId="15"/>
+    <tableColumn id="22" name="QRes" dataDxfId="14"/>
+    <tableColumn id="27" name="QItemDrug" dataDxfId="13"/>
+    <tableColumn id="31" name="QItemFish" dataDxfId="12"/>
+    <tableColumn id="30" name="QItemOre" dataDxfId="11"/>
+    <tableColumn id="28" name="QItemMushroom" dataDxfId="10"/>
+    <tableColumn id="29" name="QItemWood" dataDxfId="9"/>
+    <tableColumn id="19" name="Temperature" dataDxfId="8"/>
+    <tableColumn id="23" name="Humitity" dataDxfId="7"/>
+    <tableColumn id="26" name="Altitude" dataDxfId="6"/>
+    <tableColumn id="12" name="Url" dataDxfId="5"/>
+    <tableColumn id="13" name="TilePath" dataDxfId="4"/>
+    <tableColumn id="14" name="Icon" dataDxfId="3"/>
+    <tableColumn id="15" name="IconX" dataDxfId="2"/>
+    <tableColumn id="16" name="IconY" dataDxfId="1"/>
+    <tableColumn id="24" name="BGM" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2960,7 +2941,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="C7EDCC"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -3273,10 +3254,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC48"/>
+  <dimension ref="A1:AD48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y9" sqref="Y9"/>
+    <sheetView tabSelected="1" topLeftCell="H28" workbookViewId="0">
+      <selection activeCell="AD36" sqref="AD36:AD48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3298,11 +3279,12 @@
     <col min="23" max="24" width="3.625" style="5" customWidth="1"/>
     <col min="25" max="27" width="7.75" style="5" customWidth="1"/>
     <col min="28" max="29" width="5.375" style="5" customWidth="1"/>
-    <col min="30" max="32" width="6" style="5" customWidth="1"/>
+    <col min="30" max="30" width="9.625" style="5" customWidth="1"/>
+    <col min="31" max="32" width="6" style="5" customWidth="1"/>
     <col min="33" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="60" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:30" ht="60" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -3390,8 +3372,11 @@
       <c r="AC1" s="4" t="s">
         <v>81</v>
       </c>
+      <c r="AD1" s="4" t="s">
+        <v>273</v>
+      </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
         <v>13</v>
       </c>
@@ -3479,8 +3464,11 @@
       <c r="AC2" s="9" t="s">
         <v>13</v>
       </c>
+      <c r="AD2" s="9" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A3" s="10" t="s">
         <v>19</v>
       </c>
@@ -3568,8 +3556,11 @@
       <c r="AC3" s="10" t="s">
         <v>59</v>
       </c>
+      <c r="AD3" s="35" t="s">
+        <v>274</v>
+      </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A4" s="12">
         <v>13010001</v>
       </c>
@@ -3639,8 +3630,11 @@
       <c r="AC4" s="13">
         <v>611</v>
       </c>
+      <c r="AD4" s="19" t="s">
+        <v>276</v>
+      </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A5" s="12">
         <v>13010002</v>
       </c>
@@ -3716,8 +3710,11 @@
       <c r="AC5" s="13">
         <v>571</v>
       </c>
+      <c r="AD5" s="19" t="s">
+        <v>275</v>
+      </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A6" s="12">
         <v>13010003</v>
       </c>
@@ -3785,8 +3782,11 @@
       <c r="AC6" s="13">
         <v>432</v>
       </c>
+      <c r="AD6" s="19" t="s">
+        <v>275</v>
+      </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A7" s="12">
         <v>13010004</v>
       </c>
@@ -3858,8 +3858,11 @@
       <c r="AC7" s="13">
         <v>351</v>
       </c>
+      <c r="AD7" s="19" t="s">
+        <v>275</v>
+      </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A8" s="12">
         <v>13010005</v>
       </c>
@@ -3929,8 +3932,11 @@
       <c r="AC8" s="13">
         <v>339</v>
       </c>
+      <c r="AD8" s="19" t="s">
+        <v>275</v>
+      </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A9" s="12">
         <v>13010006</v>
       </c>
@@ -3988,8 +3994,11 @@
       <c r="AC9" s="13">
         <v>506</v>
       </c>
+      <c r="AD9" s="19" t="s">
+        <v>276</v>
+      </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A10" s="12">
         <v>13010007</v>
       </c>
@@ -4061,8 +4070,11 @@
       <c r="AC10" s="13">
         <v>440</v>
       </c>
+      <c r="AD10" s="19" t="s">
+        <v>275</v>
+      </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A11" s="12">
         <v>13010008</v>
       </c>
@@ -4134,8 +4146,11 @@
       <c r="AC11" s="13">
         <v>338</v>
       </c>
+      <c r="AD11" s="19" t="s">
+        <v>275</v>
+      </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A12" s="12">
         <v>13010009</v>
       </c>
@@ -4211,8 +4226,11 @@
       <c r="AC12" s="13">
         <v>484</v>
       </c>
+      <c r="AD12" s="19" t="s">
+        <v>275</v>
+      </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A13" s="12">
         <v>13010010</v>
       </c>
@@ -4276,8 +4294,11 @@
       <c r="AA13" s="15"/>
       <c r="AB13" s="15"/>
       <c r="AC13" s="15"/>
+      <c r="AD13" s="19" t="s">
+        <v>275</v>
+      </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A14" s="25">
         <v>13010101</v>
       </c>
@@ -4335,8 +4356,11 @@
       <c r="AC14" s="13">
         <v>509</v>
       </c>
+      <c r="AD14" s="19" t="s">
+        <v>275</v>
+      </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A15" s="25">
         <v>13010102</v>
       </c>
@@ -4410,8 +4434,11 @@
       <c r="AC15" s="13">
         <v>538</v>
       </c>
+      <c r="AD15" s="19" t="s">
+        <v>275</v>
+      </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A16" s="25">
         <v>13010103</v>
       </c>
@@ -4483,8 +4510,11 @@
       <c r="AC16" s="13">
         <v>655</v>
       </c>
+      <c r="AD16" s="19" t="s">
+        <v>275</v>
+      </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A17" s="25">
         <v>13010104</v>
       </c>
@@ -4556,8 +4586,11 @@
       <c r="AC17" s="13">
         <v>584</v>
       </c>
+      <c r="AD17" s="19" t="s">
+        <v>275</v>
+      </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A18" s="25">
         <v>13010105</v>
       </c>
@@ -4629,8 +4662,11 @@
       <c r="AC18" s="13">
         <v>444</v>
       </c>
+      <c r="AD18" s="19" t="s">
+        <v>275</v>
+      </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A19" s="25">
         <v>13010106</v>
       </c>
@@ -4704,8 +4740,11 @@
       <c r="AC19" s="13">
         <v>445</v>
       </c>
+      <c r="AD19" s="19" t="s">
+        <v>275</v>
+      </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A20" s="25">
         <v>13010107</v>
       </c>
@@ -4781,8 +4820,11 @@
       <c r="AC20" s="16">
         <v>589</v>
       </c>
+      <c r="AD20" s="19" t="s">
+        <v>275</v>
+      </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A21" s="25">
         <v>13010108</v>
       </c>
@@ -4854,8 +4896,11 @@
       <c r="AC21" s="13">
         <v>545</v>
       </c>
+      <c r="AD21" s="19" t="s">
+        <v>275</v>
+      </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A22" s="25">
         <v>13010109</v>
       </c>
@@ -4927,8 +4972,11 @@
       <c r="AC22" s="16">
         <v>455</v>
       </c>
+      <c r="AD22" s="19" t="s">
+        <v>275</v>
+      </c>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A23" s="25">
         <v>13010110</v>
       </c>
@@ -5002,8 +5050,11 @@
       <c r="AC23" s="16">
         <v>375</v>
       </c>
+      <c r="AD23" s="19" t="s">
+        <v>275</v>
+      </c>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A24" s="23">
         <v>13010201</v>
       </c>
@@ -5061,8 +5112,11 @@
       <c r="AC24" s="13">
         <v>720</v>
       </c>
+      <c r="AD24" s="19" t="s">
+        <v>275</v>
+      </c>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A25" s="23">
         <v>13010202</v>
       </c>
@@ -5132,8 +5186,11 @@
       <c r="AC25" s="15">
         <v>594</v>
       </c>
+      <c r="AD25" s="19" t="s">
+        <v>275</v>
+      </c>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A26" s="23">
         <v>13010203</v>
       </c>
@@ -5205,8 +5262,11 @@
       <c r="AC26" s="15">
         <v>720</v>
       </c>
+      <c r="AD26" s="19" t="s">
+        <v>275</v>
+      </c>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A27" s="23">
         <v>13010204</v>
       </c>
@@ -5278,8 +5338,11 @@
       <c r="AC27" s="15">
         <v>630</v>
       </c>
+      <c r="AD27" s="19" t="s">
+        <v>275</v>
+      </c>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A28" s="23">
         <v>13010205</v>
       </c>
@@ -5347,8 +5410,11 @@
       <c r="AC28" s="13">
         <v>655</v>
       </c>
+      <c r="AD28" s="19" t="s">
+        <v>275</v>
+      </c>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A29" s="23">
         <v>13010206</v>
       </c>
@@ -5414,8 +5480,11 @@
       <c r="AC29" s="13">
         <v>735</v>
       </c>
+      <c r="AD29" s="19" t="s">
+        <v>275</v>
+      </c>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A30" s="23">
         <v>13010207</v>
       </c>
@@ -5483,8 +5552,11 @@
       <c r="AC30" s="13">
         <v>785</v>
       </c>
+      <c r="AD30" s="19" t="s">
+        <v>275</v>
+      </c>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A31" s="23">
         <v>13010208</v>
       </c>
@@ -5558,8 +5630,11 @@
       <c r="AC31" s="19">
         <v>679</v>
       </c>
+      <c r="AD31" s="19" t="s">
+        <v>275</v>
+      </c>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A32" s="23">
         <v>13010209</v>
       </c>
@@ -5627,8 +5702,11 @@
       <c r="AC32" s="19">
         <v>734</v>
       </c>
+      <c r="AD32" s="19" t="s">
+        <v>275</v>
+      </c>
     </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A33" s="26">
         <v>13010301</v>
       </c>
@@ -5700,8 +5778,11 @@
       <c r="AC33" s="21">
         <v>505</v>
       </c>
+      <c r="AD33" s="19" t="s">
+        <v>275</v>
+      </c>
     </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A34" s="26">
         <v>13010302</v>
       </c>
@@ -5773,8 +5854,11 @@
       <c r="AC34" s="21">
         <v>527</v>
       </c>
+      <c r="AD34" s="19" t="s">
+        <v>275</v>
+      </c>
     </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A35" s="26">
         <v>13010303</v>
       </c>
@@ -5850,8 +5934,11 @@
       <c r="AC35" s="21">
         <v>373</v>
       </c>
+      <c r="AD35" s="19" t="s">
+        <v>275</v>
+      </c>
     </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A36" s="17">
         <v>13020001</v>
       </c>
@@ -5913,8 +6000,11 @@
       <c r="AA36" s="13"/>
       <c r="AB36" s="13"/>
       <c r="AC36" s="13"/>
+      <c r="AD36" s="19" t="s">
+        <v>277</v>
+      </c>
     </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A37" s="17">
         <v>13020002</v>
       </c>
@@ -5972,8 +6062,11 @@
       <c r="AA37" s="13"/>
       <c r="AB37" s="13"/>
       <c r="AC37" s="13"/>
+      <c r="AD37" s="19" t="s">
+        <v>277</v>
+      </c>
     </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A38" s="17">
         <v>13020011</v>
       </c>
@@ -6033,8 +6126,11 @@
       <c r="AA38" s="13"/>
       <c r="AB38" s="13"/>
       <c r="AC38" s="13"/>
+      <c r="AD38" s="19" t="s">
+        <v>277</v>
+      </c>
     </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A39" s="17">
         <v>13020012</v>
       </c>
@@ -6090,8 +6186,11 @@
       <c r="AA39" s="13"/>
       <c r="AB39" s="13"/>
       <c r="AC39" s="13"/>
+      <c r="AD39" s="19" t="s">
+        <v>277</v>
+      </c>
     </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A40" s="17">
         <v>13020013</v>
       </c>
@@ -6143,8 +6242,11 @@
       <c r="AA40" s="13"/>
       <c r="AB40" s="13"/>
       <c r="AC40" s="13"/>
+      <c r="AD40" s="19" t="s">
+        <v>277</v>
+      </c>
     </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A41" s="17">
         <v>13020021</v>
       </c>
@@ -6206,8 +6308,11 @@
       <c r="AA41" s="13"/>
       <c r="AB41" s="13"/>
       <c r="AC41" s="13"/>
+      <c r="AD41" s="19" t="s">
+        <v>277</v>
+      </c>
     </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A42" s="17">
         <v>13020022</v>
       </c>
@@ -6269,8 +6374,11 @@
       <c r="AA42" s="13"/>
       <c r="AB42" s="13"/>
       <c r="AC42" s="13"/>
+      <c r="AD42" s="19" t="s">
+        <v>277</v>
+      </c>
     </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A43" s="17">
         <v>13020023</v>
       </c>
@@ -6330,8 +6438,11 @@
       <c r="AA43" s="13"/>
       <c r="AB43" s="13"/>
       <c r="AC43" s="13"/>
+      <c r="AD43" s="19" t="s">
+        <v>277</v>
+      </c>
     </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A44" s="18">
         <v>13020031</v>
       </c>
@@ -6383,8 +6494,11 @@
       <c r="AA44" s="15"/>
       <c r="AB44" s="15"/>
       <c r="AC44" s="15"/>
+      <c r="AD44" s="19" t="s">
+        <v>277</v>
+      </c>
     </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A45" s="18">
         <v>13020032</v>
       </c>
@@ -6436,8 +6550,11 @@
       <c r="AA45" s="15"/>
       <c r="AB45" s="15"/>
       <c r="AC45" s="15"/>
+      <c r="AD45" s="19" t="s">
+        <v>277</v>
+      </c>
     </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A46" s="18">
         <v>13020033</v>
       </c>
@@ -6489,8 +6606,11 @@
       <c r="AA46" s="19"/>
       <c r="AB46" s="19"/>
       <c r="AC46" s="19"/>
+      <c r="AD46" s="19" t="s">
+        <v>277</v>
+      </c>
     </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A47" s="18">
         <v>13020034</v>
       </c>
@@ -6542,8 +6662,11 @@
       <c r="AA47" s="19"/>
       <c r="AB47" s="19"/>
       <c r="AC47" s="19"/>
+      <c r="AD47" s="19" t="s">
+        <v>277</v>
+      </c>
     </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A48" s="18">
         <v>13020035</v>
       </c>
@@ -6595,21 +6718,24 @@
       <c r="AA48" s="19"/>
       <c r="AB48" s="19"/>
       <c r="AC48" s="19"/>
+      <c r="AD48" s="19" t="s">
+        <v>277</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="I4:U48">
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:H48">
-    <cfRule type="containsBlanks" dxfId="0" priority="5">
+    <cfRule type="containsBlanks" dxfId="33" priority="5">
       <formula>LEN(TRIM(G4))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
rate quest check logic update
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Scene.xlsx
+++ b/ConfigData/Xlsx/Scene.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="Scene" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="274">
   <si>
     <t>村外小屋</t>
   </si>
@@ -487,46 +487,14 @@
     <t>viliage3</t>
   </si>
   <si>
-    <t>forestfire;10|crystalball;35</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|lighthouse;60</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|goblinhome;40|lighthouse;70</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>forestfire;35|witchhome;10</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|icedream;25|lighthouse;30</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|goblinhome;40</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>viliage1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>met;30|treasure;25|witchhome;20|dyeseller;25</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>shadowprince;1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>goblinhome;50|gamemagicbook;15|stonedoor;20</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>sandflow;2|brokehouse;2|colordoor;1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -567,10 +535,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>underwater;40|earthcrack;60|stonedoor;15|cavefind1;60</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>ruintown1;1|manflower;2|cornfield;1|honeyhome;3|poppyfield;1|river;2|insectstorm;1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -583,14 +547,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>met;30|treasure;25|gamerobot;20|dyeseller;30|waterbeast;20</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|witchhome;30|waterbeast;20</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>fortune;1|colordoor;1|waternest;2|ruinpiece;3</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -638,42 +594,10 @@
     <t>dgtower5</t>
   </si>
   <si>
-    <t>crystalball;55|wishwell;20</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>crystalball;55|wishwell;20</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>strangeletter1;30|wishwell;30</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|goblinhome;30|gamecook;20|wishwell;20</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>激活传送</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>met;30|lighthouse;60|floatbottle;50</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|treasure;25</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>hiddeway;35</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>wishwell;20</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>转盘</t>
   </si>
   <si>
@@ -838,41 +762,10 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>met;30|goblinhome;30</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30</t>
-  </si>
-  <si>
-    <t>met;30|forestfire;20|witchhome;40</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>underwater;1|torch;1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>met;30</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>forestfire;25|wishwell;20</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|wishwell;20</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>met;30|stonedoor;25</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>treasure;20</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>sandland;2|sandflow;5|weaponseller;1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -889,10 +782,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>bossmanwang;1|stonedoor;1|boostagi;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>barn;1|diarybook;1|weaponseller;1|potteryroom;1|booststr;1|thief1;1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -1053,6 +942,79 @@
   </si>
   <si>
     <t>SCN003</t>
+  </si>
+  <si>
+    <t>strangeletter1|wishwell</t>
+  </si>
+  <si>
+    <t>forestfire|crystalball</t>
+  </si>
+  <si>
+    <t>forestfire|witchhome</t>
+  </si>
+  <si>
+    <t>met|treasure|witchhome|dyeseller</t>
+  </si>
+  <si>
+    <t>goblinhome|gamemagicbook|stonedoor</t>
+  </si>
+  <si>
+    <t>met|treasure|gamerobot|dyeseller|waterbeast</t>
+  </si>
+  <si>
+    <t>met|icedream|lighthouse</t>
+  </si>
+  <si>
+    <t>met|goblinhome|gamecook|wishwell</t>
+  </si>
+  <si>
+    <t>underwater|earthcrack|stonedoor|cavefind1</t>
+  </si>
+  <si>
+    <t>met|goblinhome</t>
+  </si>
+  <si>
+    <t>met|treasure</t>
+  </si>
+  <si>
+    <t>met|lighthouse</t>
+  </si>
+  <si>
+    <t>met|forestfire|witchhome</t>
+  </si>
+  <si>
+    <t>forestfire|wishwell</t>
+  </si>
+  <si>
+    <t>met</t>
+  </si>
+  <si>
+    <t>treasure</t>
+  </si>
+  <si>
+    <t>met|stonedoor</t>
+  </si>
+  <si>
+    <t>met|wishwell</t>
+  </si>
+  <si>
+    <t>met|witchhome|waterbeast</t>
+  </si>
+  <si>
+    <t>met|lighthouse|floatbottle</t>
+  </si>
+  <si>
+    <t>met|goblinhome|lighthouse</t>
+  </si>
+  <si>
+    <t>wishwell</t>
+  </si>
+  <si>
+    <t>crystalball|wishwell</t>
+  </si>
+  <si>
+    <t>bossmanwang;1|stonedoor;1|boostagi;1|hiddeway;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -3256,8 +3218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q99" sqref="Q99"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3295,7 +3257,7 @@
         <v>87</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>270</v>
+        <v>242</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>17</v>
@@ -3310,7 +3272,7 @@
         <v>84</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>49</v>
@@ -3328,34 +3290,34 @@
         <v>57</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>178</v>
+        <v>159</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>253</v>
+        <v>225</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>252</v>
+        <v>224</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>251</v>
+        <v>223</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>254</v>
+        <v>226</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>250</v>
+        <v>222</v>
       </c>
       <c r="V1" s="30" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>241</v>
+        <v>213</v>
       </c>
       <c r="X1" s="28" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
       <c r="Y1" s="2" t="s">
         <v>18</v>
@@ -3373,7 +3335,7 @@
         <v>81</v>
       </c>
       <c r="AD1" s="4" t="s">
-        <v>273</v>
+        <v>245</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.15">
@@ -3387,7 +3349,7 @@
         <v>88</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>271</v>
+        <v>243</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>13</v>
@@ -3420,34 +3382,34 @@
         <v>46</v>
       </c>
       <c r="O2" s="8" t="s">
-        <v>179</v>
+        <v>160</v>
       </c>
       <c r="P2" s="8" t="s">
-        <v>179</v>
+        <v>160</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>268</v>
+        <v>240</v>
       </c>
       <c r="R2" s="8" t="s">
-        <v>268</v>
+        <v>240</v>
       </c>
       <c r="S2" s="8" t="s">
-        <v>268</v>
+        <v>240</v>
       </c>
       <c r="T2" s="8" t="s">
-        <v>268</v>
+        <v>240</v>
       </c>
       <c r="U2" s="8" t="s">
-        <v>268</v>
+        <v>240</v>
       </c>
       <c r="V2" s="31" t="s">
-        <v>239</v>
+        <v>211</v>
       </c>
       <c r="W2" s="7" t="s">
-        <v>239</v>
+        <v>211</v>
       </c>
       <c r="X2" s="29" t="s">
-        <v>239</v>
+        <v>211</v>
       </c>
       <c r="Y2" s="7" t="s">
         <v>24</v>
@@ -3479,7 +3441,7 @@
         <v>89</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>272</v>
+        <v>244</v>
       </c>
       <c r="E3" s="10" t="s">
         <v>21</v>
@@ -3490,7 +3452,7 @@
       <c r="G3" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="22" t="s">
         <v>86</v>
       </c>
       <c r="I3" s="11" t="s">
@@ -3512,34 +3474,34 @@
         <v>54</v>
       </c>
       <c r="O3" s="11" t="s">
-        <v>180</v>
+        <v>161</v>
       </c>
       <c r="P3" s="11" t="s">
-        <v>181</v>
+        <v>162</v>
       </c>
       <c r="Q3" s="34" t="s">
-        <v>248</v>
+        <v>220</v>
       </c>
       <c r="R3" s="34" t="s">
-        <v>247</v>
+        <v>219</v>
       </c>
       <c r="S3" s="34" t="s">
-        <v>246</v>
+        <v>218</v>
       </c>
       <c r="T3" s="34" t="s">
-        <v>249</v>
+        <v>221</v>
       </c>
       <c r="U3" s="34" t="s">
-        <v>245</v>
+        <v>217</v>
       </c>
       <c r="V3" s="32" t="s">
-        <v>240</v>
+        <v>212</v>
       </c>
       <c r="W3" s="22" t="s">
-        <v>242</v>
+        <v>214</v>
       </c>
       <c r="X3" s="33" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
       <c r="Y3" s="10" t="s">
         <v>22</v>
@@ -3557,7 +3519,7 @@
         <v>59</v>
       </c>
       <c r="AD3" s="35" t="s">
-        <v>274</v>
+        <v>246</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.15">
@@ -3580,10 +3542,10 @@
         <v>13010001</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>255</v>
+        <v>227</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>170</v>
+        <v>250</v>
       </c>
       <c r="I4" s="13">
         <v>1</v>
@@ -3631,7 +3593,7 @@
         <v>611</v>
       </c>
       <c r="AD4" s="19" t="s">
-        <v>276</v>
+        <v>248</v>
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.15">
@@ -3654,10 +3616,10 @@
         <v>13010001</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>259</v>
+        <v>231</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>128</v>
+        <v>251</v>
       </c>
       <c r="I5" s="13">
         <v>1</v>
@@ -3711,7 +3673,7 @@
         <v>571</v>
       </c>
       <c r="AD5" s="19" t="s">
-        <v>275</v>
+        <v>247</v>
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.15">
@@ -3734,10 +3696,10 @@
         <v>13010006</v>
       </c>
       <c r="G6" s="20" t="s">
-        <v>256</v>
+        <v>228</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>131</v>
+        <v>252</v>
       </c>
       <c r="I6" s="13">
         <v>1</v>
@@ -3783,7 +3745,7 @@
         <v>432</v>
       </c>
       <c r="AD6" s="19" t="s">
-        <v>275</v>
+        <v>247</v>
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.15">
@@ -3806,10 +3768,10 @@
         <v>13010006</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>263</v>
+        <v>235</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>135</v>
+        <v>253</v>
       </c>
       <c r="I7" s="13">
         <v>1</v>
@@ -3859,7 +3821,7 @@
         <v>351</v>
       </c>
       <c r="AD7" s="19" t="s">
-        <v>275</v>
+        <v>247</v>
       </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.15">
@@ -3867,7 +3829,7 @@
         <v>13010005</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="C8" s="13">
         <v>2</v>
@@ -3882,10 +3844,10 @@
         <v>13010006</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>137</v>
+        <v>254</v>
       </c>
       <c r="I8" s="13">
         <v>1</v>
@@ -3933,7 +3895,7 @@
         <v>339</v>
       </c>
       <c r="AD8" s="19" t="s">
-        <v>275</v>
+        <v>247</v>
       </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.15">
@@ -3995,7 +3957,7 @@
         <v>506</v>
       </c>
       <c r="AD9" s="19" t="s">
-        <v>276</v>
+        <v>248</v>
       </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.15">
@@ -4018,10 +3980,10 @@
         <v>13010006</v>
       </c>
       <c r="G10" s="20" t="s">
-        <v>260</v>
+        <v>232</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>152</v>
+        <v>255</v>
       </c>
       <c r="I10" s="13">
         <v>1</v>
@@ -4071,7 +4033,7 @@
         <v>440</v>
       </c>
       <c r="AD10" s="19" t="s">
-        <v>275</v>
+        <v>247</v>
       </c>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.15">
@@ -4094,10 +4056,10 @@
         <v>13010006</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>132</v>
+        <v>256</v>
       </c>
       <c r="I11" s="13">
         <v>1</v>
@@ -4147,7 +4109,7 @@
         <v>338</v>
       </c>
       <c r="AD11" s="19" t="s">
-        <v>275</v>
+        <v>247</v>
       </c>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.15">
@@ -4170,10 +4132,10 @@
         <v>13010006</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>171</v>
+        <v>257</v>
       </c>
       <c r="I12" s="13">
         <v>1</v>
@@ -4227,7 +4189,7 @@
         <v>484</v>
       </c>
       <c r="AD12" s="19" t="s">
-        <v>275</v>
+        <v>247</v>
       </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.15">
@@ -4250,10 +4212,10 @@
         <v>13010006</v>
       </c>
       <c r="G13" s="20" t="s">
-        <v>265</v>
+        <v>237</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>148</v>
+        <v>258</v>
       </c>
       <c r="I13" s="15">
         <v>1</v>
@@ -4295,7 +4257,7 @@
       <c r="AB13" s="15"/>
       <c r="AC13" s="15"/>
       <c r="AD13" s="19" t="s">
-        <v>275</v>
+        <v>247</v>
       </c>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.15">
@@ -4342,7 +4304,7 @@
         <v>2</v>
       </c>
       <c r="Y14" s="13" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
       <c r="Z14" s="13" t="s">
         <v>44</v>
@@ -4357,7 +4319,7 @@
         <v>509</v>
       </c>
       <c r="AD14" s="19" t="s">
-        <v>275</v>
+        <v>247</v>
       </c>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.15">
@@ -4383,7 +4345,7 @@
         <v>90</v>
       </c>
       <c r="H15" s="20" t="s">
-        <v>223</v>
+        <v>259</v>
       </c>
       <c r="I15" s="13">
         <v>1</v>
@@ -4435,7 +4397,7 @@
         <v>538</v>
       </c>
       <c r="AD15" s="19" t="s">
-        <v>275</v>
+        <v>247</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.15">
@@ -4458,10 +4420,10 @@
         <v>13010101</v>
       </c>
       <c r="G16" s="20" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="H16" s="20" t="s">
-        <v>174</v>
+        <v>260</v>
       </c>
       <c r="I16" s="13">
         <v>1</v>
@@ -4511,7 +4473,7 @@
         <v>655</v>
       </c>
       <c r="AD16" s="19" t="s">
-        <v>275</v>
+        <v>247</v>
       </c>
     </row>
     <row r="17" spans="1:30" x14ac:dyDescent="0.15">
@@ -4534,10 +4496,10 @@
         <v>13010101</v>
       </c>
       <c r="G17" s="20" t="s">
-        <v>266</v>
+        <v>238</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>129</v>
+        <v>261</v>
       </c>
       <c r="I17" s="13">
         <v>1</v>
@@ -4587,7 +4549,7 @@
         <v>584</v>
       </c>
       <c r="AD17" s="19" t="s">
-        <v>275</v>
+        <v>247</v>
       </c>
     </row>
     <row r="18" spans="1:30" x14ac:dyDescent="0.15">
@@ -4610,10 +4572,10 @@
         <v>13010101</v>
       </c>
       <c r="G18" s="20" t="s">
-        <v>267</v>
+        <v>239</v>
       </c>
       <c r="H18" s="20" t="s">
-        <v>225</v>
+        <v>262</v>
       </c>
       <c r="I18" s="13">
         <v>1</v>
@@ -4663,7 +4625,7 @@
         <v>444</v>
       </c>
       <c r="AD18" s="19" t="s">
-        <v>275</v>
+        <v>247</v>
       </c>
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.15">
@@ -4686,10 +4648,10 @@
         <v>13010016</v>
       </c>
       <c r="G19" s="20" t="s">
-        <v>261</v>
+        <v>233</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>133</v>
+        <v>259</v>
       </c>
       <c r="I19" s="13">
         <v>1</v>
@@ -4741,7 +4703,7 @@
         <v>445</v>
       </c>
       <c r="AD19" s="19" t="s">
-        <v>275</v>
+        <v>247</v>
       </c>
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.15">
@@ -4749,7 +4711,7 @@
         <v>13010107</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>203</v>
+        <v>184</v>
       </c>
       <c r="C20" s="15">
         <v>2</v>
@@ -4764,10 +4726,10 @@
         <v>13010101</v>
       </c>
       <c r="G20" s="20" t="s">
-        <v>257</v>
+        <v>229</v>
       </c>
       <c r="H20" s="20" t="s">
-        <v>228</v>
+        <v>263</v>
       </c>
       <c r="I20" s="13">
         <v>1</v>
@@ -4806,13 +4768,13 @@
         <v>2</v>
       </c>
       <c r="Y20" s="13" t="s">
-        <v>207</v>
+        <v>188</v>
       </c>
       <c r="Z20" s="13" t="s">
-        <v>207</v>
+        <v>188</v>
       </c>
       <c r="AA20" s="13" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
       <c r="AB20" s="16">
         <v>850</v>
@@ -4821,7 +4783,7 @@
         <v>589</v>
       </c>
       <c r="AD20" s="19" t="s">
-        <v>275</v>
+        <v>247</v>
       </c>
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.15">
@@ -4829,7 +4791,7 @@
         <v>13010108</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>199</v>
+        <v>180</v>
       </c>
       <c r="C21" s="15">
         <v>2</v>
@@ -4844,10 +4806,10 @@
         <v>13010101</v>
       </c>
       <c r="G21" s="20" t="s">
-        <v>234</v>
+        <v>207</v>
       </c>
       <c r="H21" s="20" t="s">
-        <v>227</v>
+        <v>264</v>
       </c>
       <c r="I21" s="13">
         <v>1</v>
@@ -4882,13 +4844,13 @@
         <v>3</v>
       </c>
       <c r="Y21" s="13" t="s">
-        <v>209</v>
+        <v>190</v>
       </c>
       <c r="Z21" s="13" t="s">
-        <v>209</v>
+        <v>190</v>
       </c>
       <c r="AA21" s="16" t="s">
-        <v>195</v>
+        <v>176</v>
       </c>
       <c r="AB21" s="13">
         <v>682</v>
@@ -4897,7 +4859,7 @@
         <v>545</v>
       </c>
       <c r="AD21" s="19" t="s">
-        <v>275</v>
+        <v>247</v>
       </c>
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.15">
@@ -4905,7 +4867,7 @@
         <v>13010109</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>216</v>
+        <v>197</v>
       </c>
       <c r="C22" s="15">
         <v>2</v>
@@ -4920,10 +4882,10 @@
         <v>13010101</v>
       </c>
       <c r="G22" s="20" t="s">
-        <v>233</v>
+        <v>206</v>
       </c>
       <c r="H22" s="16" t="s">
-        <v>224</v>
+        <v>264</v>
       </c>
       <c r="I22" s="13">
         <v>1</v>
@@ -4958,13 +4920,13 @@
         <v>3</v>
       </c>
       <c r="Y22" s="13" t="s">
-        <v>220</v>
+        <v>201</v>
       </c>
       <c r="Z22" s="20" t="s">
-        <v>221</v>
+        <v>202</v>
       </c>
       <c r="AA22" s="16" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="AB22" s="16">
         <v>643</v>
@@ -4973,7 +4935,7 @@
         <v>455</v>
       </c>
       <c r="AD22" s="19" t="s">
-        <v>275</v>
+        <v>247</v>
       </c>
     </row>
     <row r="23" spans="1:30" x14ac:dyDescent="0.15">
@@ -4981,7 +4943,7 @@
         <v>13010110</v>
       </c>
       <c r="B23" s="27" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="C23" s="15">
         <v>2</v>
@@ -4997,7 +4959,7 @@
       </c>
       <c r="G23" s="20"/>
       <c r="H23" s="16" t="s">
-        <v>224</v>
+        <v>264</v>
       </c>
       <c r="I23" s="13">
         <v>1</v>
@@ -5036,13 +4998,13 @@
         <v>3</v>
       </c>
       <c r="Y23" s="20" t="s">
-        <v>222</v>
+        <v>203</v>
       </c>
       <c r="Z23" s="20" t="s">
-        <v>222</v>
+        <v>203</v>
       </c>
       <c r="AA23" s="16" t="s">
-        <v>218</v>
+        <v>199</v>
       </c>
       <c r="AB23" s="16">
         <v>720</v>
@@ -5051,7 +5013,7 @@
         <v>375</v>
       </c>
       <c r="AD23" s="19" t="s">
-        <v>275</v>
+        <v>247</v>
       </c>
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.15">
@@ -5059,7 +5021,7 @@
         <v>13010201</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>202</v>
+        <v>183</v>
       </c>
       <c r="C24" s="15">
         <v>2</v>
@@ -5098,13 +5060,13 @@
         <v>2</v>
       </c>
       <c r="Y24" s="13" t="s">
-        <v>205</v>
+        <v>186</v>
       </c>
       <c r="Z24" s="13" t="s">
-        <v>205</v>
+        <v>186</v>
       </c>
       <c r="AA24" s="16" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
       <c r="AB24" s="13">
         <v>807</v>
@@ -5113,7 +5075,7 @@
         <v>720</v>
       </c>
       <c r="AD24" s="19" t="s">
-        <v>275</v>
+        <v>247</v>
       </c>
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.15">
@@ -5121,7 +5083,7 @@
         <v>13010202</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="C25" s="15">
         <v>2</v>
@@ -5136,10 +5098,10 @@
         <v>13010201</v>
       </c>
       <c r="G25" s="15" t="s">
-        <v>235</v>
+        <v>208</v>
       </c>
       <c r="H25" s="15" t="s">
-        <v>224</v>
+        <v>264</v>
       </c>
       <c r="I25" s="13">
         <v>1</v>
@@ -5172,13 +5134,13 @@
         <v>3</v>
       </c>
       <c r="Y25" s="13" t="s">
-        <v>210</v>
+        <v>191</v>
       </c>
       <c r="Z25" s="13" t="s">
-        <v>210</v>
+        <v>191</v>
       </c>
       <c r="AA25" s="15" t="s">
-        <v>185</v>
+        <v>166</v>
       </c>
       <c r="AB25" s="15">
         <v>974</v>
@@ -5187,7 +5149,7 @@
         <v>594</v>
       </c>
       <c r="AD25" s="19" t="s">
-        <v>275</v>
+        <v>247</v>
       </c>
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.15">
@@ -5195,7 +5157,7 @@
         <v>13010203</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
       <c r="C26" s="15">
         <v>2</v>
@@ -5210,10 +5172,10 @@
         <v>13010201</v>
       </c>
       <c r="G26" s="15" t="s">
-        <v>235</v>
+        <v>208</v>
       </c>
       <c r="H26" s="15" t="s">
-        <v>224</v>
+        <v>264</v>
       </c>
       <c r="I26" s="13">
         <v>1</v>
@@ -5248,13 +5210,13 @@
         <v>3</v>
       </c>
       <c r="Y26" s="13" t="s">
-        <v>211</v>
+        <v>192</v>
       </c>
       <c r="Z26" s="13" t="s">
-        <v>211</v>
+        <v>192</v>
       </c>
       <c r="AA26" s="15" t="s">
-        <v>186</v>
+        <v>167</v>
       </c>
       <c r="AB26" s="15">
         <v>1080</v>
@@ -5263,7 +5225,7 @@
         <v>720</v>
       </c>
       <c r="AD26" s="19" t="s">
-        <v>275</v>
+        <v>247</v>
       </c>
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.15">
@@ -5271,7 +5233,7 @@
         <v>13010204</v>
       </c>
       <c r="B27" s="24" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
       <c r="C27" s="15">
         <v>2</v>
@@ -5286,10 +5248,10 @@
         <v>13010201</v>
       </c>
       <c r="G27" s="15" t="s">
-        <v>226</v>
+        <v>204</v>
       </c>
       <c r="H27" s="15" t="s">
-        <v>231</v>
+        <v>265</v>
       </c>
       <c r="I27" s="13">
         <v>1</v>
@@ -5324,13 +5286,13 @@
         <v>3</v>
       </c>
       <c r="Y27" s="13" t="s">
-        <v>212</v>
+        <v>193</v>
       </c>
       <c r="Z27" s="13" t="s">
-        <v>212</v>
+        <v>193</v>
       </c>
       <c r="AA27" s="15" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="AB27" s="15">
         <v>1074</v>
@@ -5339,7 +5301,7 @@
         <v>630</v>
       </c>
       <c r="AD27" s="19" t="s">
-        <v>275</v>
+        <v>247</v>
       </c>
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.15">
@@ -5347,7 +5309,7 @@
         <v>13010205</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>200</v>
+        <v>181</v>
       </c>
       <c r="C28" s="15">
         <v>2</v>
@@ -5362,7 +5324,7 @@
         <v>13010201</v>
       </c>
       <c r="G28" s="15" t="s">
-        <v>232</v>
+        <v>205</v>
       </c>
       <c r="H28" s="16"/>
       <c r="I28" s="13">
@@ -5396,13 +5358,13 @@
         <v>2</v>
       </c>
       <c r="Y28" s="20" t="s">
-        <v>208</v>
+        <v>189</v>
       </c>
       <c r="Z28" s="20" t="s">
-        <v>208</v>
+        <v>189</v>
       </c>
       <c r="AA28" s="16" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="AB28" s="13">
         <v>717</v>
@@ -5411,7 +5373,7 @@
         <v>655</v>
       </c>
       <c r="AD28" s="19" t="s">
-        <v>275</v>
+        <v>247</v>
       </c>
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.15">
@@ -5419,7 +5381,7 @@
         <v>13010206</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>198</v>
+        <v>179</v>
       </c>
       <c r="C29" s="15">
         <v>2</v>
@@ -5435,7 +5397,7 @@
       </c>
       <c r="G29" s="16"/>
       <c r="H29" s="20" t="s">
-        <v>230</v>
+        <v>266</v>
       </c>
       <c r="I29" s="13">
         <v>1</v>
@@ -5466,13 +5428,13 @@
         <v>2</v>
       </c>
       <c r="Y29" s="20" t="s">
-        <v>214</v>
+        <v>195</v>
       </c>
       <c r="Z29" s="20" t="s">
-        <v>214</v>
+        <v>195</v>
       </c>
       <c r="AA29" s="16" t="s">
-        <v>194</v>
+        <v>175</v>
       </c>
       <c r="AB29" s="13">
         <v>637</v>
@@ -5481,7 +5443,7 @@
         <v>735</v>
       </c>
       <c r="AD29" s="19" t="s">
-        <v>275</v>
+        <v>247</v>
       </c>
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.15">
@@ -5489,7 +5451,7 @@
         <v>13010207</v>
       </c>
       <c r="B30" s="23" t="s">
-        <v>197</v>
+        <v>178</v>
       </c>
       <c r="C30" s="15">
         <v>2</v>
@@ -5505,7 +5467,7 @@
       </c>
       <c r="G30" s="15"/>
       <c r="H30" s="15" t="s">
-        <v>224</v>
+        <v>264</v>
       </c>
       <c r="I30" s="13">
         <v>1</v>
@@ -5538,13 +5500,13 @@
         <v>4</v>
       </c>
       <c r="Y30" s="13" t="s">
-        <v>213</v>
+        <v>194</v>
       </c>
       <c r="Z30" s="13" t="s">
-        <v>213</v>
+        <v>194</v>
       </c>
       <c r="AA30" s="13" t="s">
-        <v>196</v>
+        <v>177</v>
       </c>
       <c r="AB30" s="13">
         <v>737</v>
@@ -5553,7 +5515,7 @@
         <v>785</v>
       </c>
       <c r="AD30" s="19" t="s">
-        <v>275</v>
+        <v>247</v>
       </c>
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.15">
@@ -5561,7 +5523,7 @@
         <v>13010208</v>
       </c>
       <c r="B31" s="24" t="s">
-        <v>204</v>
+        <v>185</v>
       </c>
       <c r="C31" s="15">
         <v>2</v>
@@ -5576,10 +5538,10 @@
         <v>13010201</v>
       </c>
       <c r="G31" s="15" t="s">
-        <v>258</v>
+        <v>230</v>
       </c>
       <c r="H31" s="15" t="s">
-        <v>224</v>
+        <v>264</v>
       </c>
       <c r="I31" s="13">
         <v>1</v>
@@ -5616,13 +5578,13 @@
         <v>2</v>
       </c>
       <c r="Y31" s="13" t="s">
-        <v>206</v>
+        <v>187</v>
       </c>
       <c r="Z31" s="13" t="s">
-        <v>206</v>
+        <v>187</v>
       </c>
       <c r="AA31" s="15" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
       <c r="AB31" s="19">
         <v>894</v>
@@ -5631,7 +5593,7 @@
         <v>679</v>
       </c>
       <c r="AD31" s="19" t="s">
-        <v>275</v>
+        <v>247</v>
       </c>
     </row>
     <row r="32" spans="1:30" x14ac:dyDescent="0.15">
@@ -5639,7 +5601,7 @@
         <v>13010209</v>
       </c>
       <c r="B32" s="23" t="s">
-        <v>201</v>
+        <v>182</v>
       </c>
       <c r="C32" s="15">
         <v>2</v>
@@ -5655,7 +5617,7 @@
       </c>
       <c r="G32" s="20"/>
       <c r="H32" s="20" t="s">
-        <v>229</v>
+        <v>267</v>
       </c>
       <c r="I32" s="13">
         <v>1</v>
@@ -5688,13 +5650,13 @@
         <v>2</v>
       </c>
       <c r="Y32" s="20" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="Z32" s="20" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="AA32" s="16" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="AB32" s="19">
         <v>984</v>
@@ -5703,7 +5665,7 @@
         <v>734</v>
       </c>
       <c r="AD32" s="19" t="s">
-        <v>275</v>
+        <v>247</v>
       </c>
     </row>
     <row r="33" spans="1:30" x14ac:dyDescent="0.15">
@@ -5726,10 +5688,10 @@
         <v>13010006</v>
       </c>
       <c r="G33" s="20" t="s">
-        <v>262</v>
+        <v>234</v>
       </c>
       <c r="H33" s="13" t="s">
-        <v>153</v>
+        <v>268</v>
       </c>
       <c r="I33" s="13">
         <v>1</v>
@@ -5779,7 +5741,7 @@
         <v>505</v>
       </c>
       <c r="AD33" s="19" t="s">
-        <v>275</v>
+        <v>247</v>
       </c>
     </row>
     <row r="34" spans="1:30" x14ac:dyDescent="0.15">
@@ -5802,10 +5764,10 @@
         <v>13010006</v>
       </c>
       <c r="G34" s="13" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="H34" s="13" t="s">
-        <v>173</v>
+        <v>269</v>
       </c>
       <c r="I34" s="13">
         <v>1</v>
@@ -5855,7 +5817,7 @@
         <v>527</v>
       </c>
       <c r="AD34" s="19" t="s">
-        <v>275</v>
+        <v>247</v>
       </c>
     </row>
     <row r="35" spans="1:30" x14ac:dyDescent="0.15">
@@ -5878,10 +5840,10 @@
         <v>13010006</v>
       </c>
       <c r="G35" s="13" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="H35" s="13" t="s">
-        <v>130</v>
+        <v>270</v>
       </c>
       <c r="I35" s="13">
         <v>1</v>
@@ -5935,7 +5897,7 @@
         <v>373</v>
       </c>
       <c r="AD35" s="19" t="s">
-        <v>275</v>
+        <v>247</v>
       </c>
     </row>
     <row r="36" spans="1:30" x14ac:dyDescent="0.15">
@@ -5958,7 +5920,7 @@
         <v>13010002</v>
       </c>
       <c r="G36" s="20" t="s">
-        <v>269</v>
+        <v>241</v>
       </c>
       <c r="H36" s="13"/>
       <c r="I36" s="13"/>
@@ -5995,13 +5957,13 @@
         <v>109</v>
       </c>
       <c r="Z36" s="13" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="AA36" s="13"/>
       <c r="AB36" s="13"/>
       <c r="AC36" s="13"/>
       <c r="AD36" s="19" t="s">
-        <v>277</v>
+        <v>249</v>
       </c>
     </row>
     <row r="37" spans="1:30" x14ac:dyDescent="0.15">
@@ -6057,13 +6019,13 @@
         <v>110</v>
       </c>
       <c r="Z37" s="13" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="AA37" s="13"/>
       <c r="AB37" s="13"/>
       <c r="AC37" s="13"/>
       <c r="AD37" s="19" t="s">
-        <v>277</v>
+        <v>249</v>
       </c>
     </row>
     <row r="38" spans="1:30" x14ac:dyDescent="0.15">
@@ -6086,10 +6048,10 @@
         <v>13010007</v>
       </c>
       <c r="G38" s="13" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="H38" s="13" t="s">
-        <v>176</v>
+        <v>271</v>
       </c>
       <c r="I38" s="13"/>
       <c r="J38" s="13"/>
@@ -6121,13 +6083,13 @@
         <v>115</v>
       </c>
       <c r="Z38" s="13" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="AA38" s="13"/>
       <c r="AB38" s="13"/>
       <c r="AC38" s="13"/>
       <c r="AD38" s="19" t="s">
-        <v>277</v>
+        <v>249</v>
       </c>
     </row>
     <row r="39" spans="1:30" x14ac:dyDescent="0.15">
@@ -6150,7 +6112,7 @@
         <v>13010007</v>
       </c>
       <c r="G39" s="13" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="H39" s="13"/>
       <c r="I39" s="13"/>
@@ -6181,13 +6143,13 @@
         <v>119</v>
       </c>
       <c r="Z39" s="13" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="AA39" s="13"/>
       <c r="AB39" s="13"/>
       <c r="AC39" s="13"/>
       <c r="AD39" s="19" t="s">
-        <v>277</v>
+        <v>249</v>
       </c>
     </row>
     <row r="40" spans="1:30" x14ac:dyDescent="0.15">
@@ -6237,13 +6199,13 @@
         <v>116</v>
       </c>
       <c r="Z40" s="13" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="AA40" s="13"/>
       <c r="AB40" s="13"/>
       <c r="AC40" s="13"/>
       <c r="AD40" s="19" t="s">
-        <v>277</v>
+        <v>249</v>
       </c>
     </row>
     <row r="41" spans="1:30" x14ac:dyDescent="0.15">
@@ -6266,10 +6228,10 @@
         <v>13010004</v>
       </c>
       <c r="G41" s="13" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="H41" s="13" t="s">
-        <v>168</v>
+        <v>272</v>
       </c>
       <c r="I41" s="13"/>
       <c r="J41" s="13"/>
@@ -6300,16 +6262,16 @@
         <v>1</v>
       </c>
       <c r="Y41" s="13" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="Z41" s="13" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="AA41" s="13"/>
       <c r="AB41" s="13"/>
       <c r="AC41" s="13"/>
       <c r="AD41" s="19" t="s">
-        <v>277</v>
+        <v>249</v>
       </c>
     </row>
     <row r="42" spans="1:30" x14ac:dyDescent="0.15">
@@ -6332,10 +6294,10 @@
         <v>13010004</v>
       </c>
       <c r="G42" s="20" t="s">
-        <v>237</v>
+        <v>209</v>
       </c>
       <c r="H42" s="13" t="s">
-        <v>169</v>
+        <v>272</v>
       </c>
       <c r="I42" s="13"/>
       <c r="J42" s="13"/>
@@ -6369,13 +6331,13 @@
         <v>126</v>
       </c>
       <c r="Z42" s="13" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="AA42" s="13"/>
       <c r="AB42" s="13"/>
       <c r="AC42" s="13"/>
       <c r="AD42" s="19" t="s">
-        <v>277</v>
+        <v>249</v>
       </c>
     </row>
     <row r="43" spans="1:30" x14ac:dyDescent="0.15">
@@ -6398,11 +6360,9 @@
         <v>13010004</v>
       </c>
       <c r="G43" s="20" t="s">
-        <v>236</v>
-      </c>
-      <c r="H43" s="13" t="s">
-        <v>175</v>
-      </c>
+        <v>273</v>
+      </c>
+      <c r="H43" s="13"/>
       <c r="I43" s="13"/>
       <c r="J43" s="13"/>
       <c r="K43" s="13"/>
@@ -6433,13 +6393,13 @@
         <v>127</v>
       </c>
       <c r="Z43" s="13" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="AA43" s="13"/>
       <c r="AB43" s="13"/>
       <c r="AC43" s="13"/>
       <c r="AD43" s="19" t="s">
-        <v>277</v>
+        <v>249</v>
       </c>
     </row>
     <row r="44" spans="1:30" x14ac:dyDescent="0.15">
@@ -6447,7 +6407,7 @@
         <v>13020031</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="C44" s="13">
         <v>3</v>
@@ -6486,16 +6446,16 @@
         <v>5</v>
       </c>
       <c r="Y44" s="13" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="Z44" s="15" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="AA44" s="15"/>
       <c r="AB44" s="15"/>
       <c r="AC44" s="15"/>
       <c r="AD44" s="19" t="s">
-        <v>277</v>
+        <v>249</v>
       </c>
     </row>
     <row r="45" spans="1:30" x14ac:dyDescent="0.15">
@@ -6503,7 +6463,7 @@
         <v>13020032</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="C45" s="13">
         <v>3</v>
@@ -6542,16 +6502,16 @@
         <v>5</v>
       </c>
       <c r="Y45" s="13" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="Z45" s="15" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="AA45" s="15"/>
       <c r="AB45" s="15"/>
       <c r="AC45" s="15"/>
       <c r="AD45" s="19" t="s">
-        <v>277</v>
+        <v>249</v>
       </c>
     </row>
     <row r="46" spans="1:30" x14ac:dyDescent="0.15">
@@ -6559,7 +6519,7 @@
         <v>13020033</v>
       </c>
       <c r="B46" s="17" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="C46" s="13">
         <v>3</v>
@@ -6598,16 +6558,16 @@
         <v>5</v>
       </c>
       <c r="Y46" s="13" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="Z46" s="15" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="AA46" s="19"/>
       <c r="AB46" s="19"/>
       <c r="AC46" s="19"/>
       <c r="AD46" s="19" t="s">
-        <v>277</v>
+        <v>249</v>
       </c>
     </row>
     <row r="47" spans="1:30" x14ac:dyDescent="0.15">
@@ -6615,7 +6575,7 @@
         <v>13020034</v>
       </c>
       <c r="B47" s="17" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="C47" s="13">
         <v>3</v>
@@ -6654,16 +6614,16 @@
         <v>5</v>
       </c>
       <c r="Y47" s="13" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="Z47" s="15" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="AA47" s="19"/>
       <c r="AB47" s="19"/>
       <c r="AC47" s="19"/>
       <c r="AD47" s="19" t="s">
-        <v>277</v>
+        <v>249</v>
       </c>
     </row>
     <row r="48" spans="1:30" x14ac:dyDescent="0.15">
@@ -6671,7 +6631,7 @@
         <v>13020035</v>
       </c>
       <c r="B48" s="17" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="C48" s="13">
         <v>3</v>
@@ -6710,16 +6670,16 @@
         <v>5</v>
       </c>
       <c r="Y48" s="13" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="Z48" s="15" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="AA48" s="19"/>
       <c r="AB48" s="19"/>
       <c r="AC48" s="19"/>
       <c r="AD48" s="19" t="s">
-        <v>277</v>
+        <v>249</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add a common battle event
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Scene.xlsx
+++ b/ConfigData/Xlsx/Scene.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{5E92439E-BB9A-4EFE-92FB-F085D9001CF0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9A0DC765-A1F8-4342-93C6-EC9363AAA22D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="282">
   <si>
     <t>村外小屋</t>
   </si>
@@ -1023,6 +1023,30 @@
   </si>
   <si>
     <t>SCN007</t>
+  </si>
+  <si>
+    <t>int[]</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>敌人列表</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>敌人数量</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QEnemy</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>EnemyIds</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1947,7 +1971,36 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="35">
+  <dxfs count="37">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1968,6 +2021,35 @@
           <bgColor theme="0" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -2833,41 +2915,43 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A3:AC48" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33" tableBorderDxfId="32">
-  <autoFilter ref="A3:AC48" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState ref="A4:AB48">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A3:AE48" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35" tableBorderDxfId="34">
+  <autoFilter ref="A3:AE48" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState ref="A4:AD48">
     <sortCondition ref="A3:A48"/>
   </sortState>
-  <tableColumns count="29">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="31"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="30"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Type" dataDxfId="29"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="RegionId" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Level" dataDxfId="27"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="ReviveScene" dataDxfId="26"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Quest" dataDxfId="25"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="QuestRandom" dataDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="QPortal" dataDxfId="23"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="QCardChange" dataDxfId="22"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="QPiece" dataDxfId="21"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="QMerchant" dataDxfId="20"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="QDoctor" dataDxfId="19"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="QAngel" dataDxfId="18"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="QRes" dataDxfId="17"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="QItemDrug" dataDxfId="16"/>
-    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="QItemFish" dataDxfId="15"/>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="QItemOre" dataDxfId="14"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="QItemMushroom" dataDxfId="13"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="QItemWood" dataDxfId="12"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Temperature" dataDxfId="11"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="Humitity" dataDxfId="10"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="Altitude" dataDxfId="9"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Url" dataDxfId="8"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="TilePath" dataDxfId="7"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Icon" dataDxfId="6"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="IconX" dataDxfId="5"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="IconY" dataDxfId="4"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="BGM" dataDxfId="3"/>
+  <tableColumns count="31">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="32"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Type" dataDxfId="31"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="RegionId" dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Level" dataDxfId="29"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="ReviveScene" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Quest" dataDxfId="27"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="QuestRandom" dataDxfId="26"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="QPortal" dataDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="QCardChange" dataDxfId="24"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="QPiece" dataDxfId="23"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="QMerchant" dataDxfId="22"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="QDoctor" dataDxfId="21"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="QAngel" dataDxfId="20"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="QRes" dataDxfId="19"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="QItemDrug" dataDxfId="18"/>
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="QItemFish" dataDxfId="17"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="QItemOre" dataDxfId="16"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="QItemMushroom" dataDxfId="15"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="QItemWood" dataDxfId="14"/>
+    <tableColumn id="32" xr3:uid="{A83B2B25-5C5C-426D-A301-0017A60CEB0A}" name="QEnemy" dataDxfId="0"/>
+    <tableColumn id="25" xr3:uid="{52509577-5139-4AB6-BDC1-0A628B9D6BD7}" name="EnemyIds" dataDxfId="4"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Temperature" dataDxfId="13"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="Humitity" dataDxfId="12"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="Altitude" dataDxfId="11"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Url" dataDxfId="10"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="TilePath" dataDxfId="9"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Icon" dataDxfId="8"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="IconX" dataDxfId="7"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="IconY" dataDxfId="6"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="BGM" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3194,10 +3278,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC48"/>
+  <dimension ref="A1:AE48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3214,17 +3298,18 @@
     <col min="16" max="17" width="3.75" style="5" customWidth="1"/>
     <col min="18" max="18" width="3.75" customWidth="1"/>
     <col min="19" max="19" width="3.75" style="5" customWidth="1"/>
-    <col min="20" max="20" width="3.75" customWidth="1"/>
-    <col min="21" max="21" width="3.625" customWidth="1"/>
-    <col min="22" max="23" width="3.625" style="5" customWidth="1"/>
-    <col min="24" max="26" width="7.75" style="5" customWidth="1"/>
-    <col min="27" max="28" width="5.375" style="5" customWidth="1"/>
-    <col min="29" max="29" width="9.625" style="5" customWidth="1"/>
-    <col min="30" max="31" width="6" style="5" customWidth="1"/>
-    <col min="32" max="16384" width="9" style="5"/>
+    <col min="20" max="21" width="3.75" customWidth="1"/>
+    <col min="22" max="22" width="12.75" style="5" customWidth="1"/>
+    <col min="23" max="23" width="3.625" customWidth="1"/>
+    <col min="24" max="25" width="3.625" style="5" customWidth="1"/>
+    <col min="26" max="28" width="7.75" style="5" customWidth="1"/>
+    <col min="29" max="30" width="5.375" style="5" customWidth="1"/>
+    <col min="31" max="31" width="9.625" style="5" customWidth="1"/>
+    <col min="32" max="33" width="6" style="5" customWidth="1"/>
+    <col min="34" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="60" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:31" ht="60" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -3285,35 +3370,41 @@
       <c r="T1" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="U1" s="30" t="s">
+      <c r="U1" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="V1" s="28" t="s">
+        <v>277</v>
+      </c>
+      <c r="W1" s="30" t="s">
         <v>208</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="W1" s="28" t="s">
+      <c r="Y1" s="28" t="s">
         <v>213</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AE1" s="4" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
         <v>13</v>
       </c>
@@ -3374,35 +3465,41 @@
       <c r="T2" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="U2" s="31" t="s">
+      <c r="U2" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="V2" s="29" t="s">
+        <v>276</v>
+      </c>
+      <c r="W2" s="31" t="s">
         <v>209</v>
       </c>
-      <c r="V2" s="7" t="s">
+      <c r="X2" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="W2" s="29" t="s">
+      <c r="Y2" s="29" t="s">
         <v>209</v>
       </c>
-      <c r="X2" s="7" t="s">
+      <c r="Z2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="Y2" s="7" t="s">
+      <c r="AA2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="Z2" s="7" t="s">
+      <c r="AB2" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="AA2" s="7" t="s">
+      <c r="AC2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="AB2" s="9" t="s">
+      <c r="AD2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="AC2" s="9" t="s">
+      <c r="AE2" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A3" s="10" t="s">
         <v>19</v>
       </c>
@@ -3430,7 +3527,7 @@
       <c r="I3" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="J3" s="34" t="s">
         <v>48</v>
       </c>
       <c r="K3" s="11" t="s">
@@ -3463,35 +3560,41 @@
       <c r="T3" s="34" t="s">
         <v>215</v>
       </c>
-      <c r="U3" s="32" t="s">
+      <c r="U3" s="34" t="s">
+        <v>280</v>
+      </c>
+      <c r="V3" s="33" t="s">
+        <v>281</v>
+      </c>
+      <c r="W3" s="32" t="s">
         <v>210</v>
       </c>
-      <c r="V3" s="22" t="s">
+      <c r="X3" s="22" t="s">
         <v>212</v>
       </c>
-      <c r="W3" s="33" t="s">
+      <c r="Y3" s="33" t="s">
         <v>214</v>
       </c>
-      <c r="X3" s="10" t="s">
+      <c r="Z3" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="Y3" s="10" t="s">
+      <c r="AA3" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="Z3" s="10" t="s">
+      <c r="AB3" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="AA3" s="10" t="s">
+      <c r="AC3" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="AB3" s="10" t="s">
+      <c r="AD3" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="AC3" s="35" t="s">
+      <c r="AE3" s="35" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A4" s="12">
         <v>13010001</v>
       </c>
@@ -3536,35 +3639,37 @@
       <c r="T4" s="13">
         <v>0.7</v>
       </c>
-      <c r="U4" s="13">
-        <v>3</v>
-      </c>
-      <c r="V4" s="13">
-        <v>2</v>
-      </c>
+      <c r="U4" s="13"/>
+      <c r="V4" s="13"/>
       <c r="W4" s="13">
-        <v>2</v>
-      </c>
-      <c r="X4" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="X4" s="13">
+        <v>2</v>
+      </c>
+      <c r="Y4" s="13">
+        <v>2</v>
+      </c>
+      <c r="Z4" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="Y4" s="13" t="s">
+      <c r="AA4" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="Z4" s="13" t="s">
+      <c r="AB4" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="AA4" s="13">
+      <c r="AC4" s="13">
         <v>1348</v>
       </c>
-      <c r="AB4" s="13">
+      <c r="AD4" s="13">
         <v>611</v>
       </c>
-      <c r="AC4" s="19" t="s">
+      <c r="AE4" s="19" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A5" s="12">
         <v>13010002</v>
       </c>
@@ -3616,34 +3721,40 @@
         <v>0.7</v>
       </c>
       <c r="U5" s="13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="V5" s="13">
-        <v>3</v>
+        <v>43000002</v>
       </c>
       <c r="W5" s="13">
         <v>2</v>
       </c>
-      <c r="X5" s="13" t="s">
+      <c r="X5" s="13">
+        <v>3</v>
+      </c>
+      <c r="Y5" s="13">
+        <v>2</v>
+      </c>
+      <c r="Z5" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="Y5" s="13" t="s">
+      <c r="AA5" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="Z5" s="13" t="s">
+      <c r="AB5" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="AA5" s="13">
+      <c r="AC5" s="13">
         <v>1279</v>
       </c>
-      <c r="AB5" s="13">
+      <c r="AD5" s="13">
         <v>571</v>
       </c>
-      <c r="AC5" s="19" t="s">
+      <c r="AE5" s="19" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A6" s="12">
         <v>13010003</v>
       </c>
@@ -3690,31 +3801,37 @@
         <v>3</v>
       </c>
       <c r="V6" s="13">
-        <v>3</v>
+        <v>43000002</v>
       </c>
       <c r="W6" s="13">
-        <v>2</v>
-      </c>
-      <c r="X6" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="X6" s="13">
+        <v>3</v>
+      </c>
+      <c r="Y6" s="13">
+        <v>2</v>
+      </c>
+      <c r="Z6" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="Y6" s="13" t="s">
+      <c r="AA6" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="Z6" s="13" t="s">
+      <c r="AB6" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="AA6" s="13">
+      <c r="AC6" s="13">
         <v>1251</v>
       </c>
-      <c r="AB6" s="13">
+      <c r="AD6" s="13">
         <v>432</v>
       </c>
-      <c r="AC6" s="19" t="s">
+      <c r="AE6" s="19" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A7" s="12">
         <v>13010004</v>
       </c>
@@ -3762,34 +3879,40 @@
         <v>0.3</v>
       </c>
       <c r="U7" s="13">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="V7" s="13">
-        <v>2</v>
+        <v>43000002</v>
       </c>
       <c r="W7" s="13">
-        <v>1</v>
-      </c>
-      <c r="X7" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="X7" s="13">
+        <v>2</v>
+      </c>
+      <c r="Y7" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="Y7" s="13" t="s">
+      <c r="AA7" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="Z7" s="13" t="s">
+      <c r="AB7" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="AA7" s="13">
+      <c r="AC7" s="13">
         <v>1148</v>
       </c>
-      <c r="AB7" s="13">
+      <c r="AD7" s="13">
         <v>351</v>
       </c>
-      <c r="AC7" s="19" t="s">
+      <c r="AE7" s="19" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A8" s="12">
         <v>13010005</v>
       </c>
@@ -3838,31 +3961,37 @@
         <v>2</v>
       </c>
       <c r="V8" s="13">
-        <v>2</v>
+        <v>43000002</v>
       </c>
       <c r="W8" s="13">
+        <v>2</v>
+      </c>
+      <c r="X8" s="13">
+        <v>2</v>
+      </c>
+      <c r="Y8" s="13">
         <v>5</v>
       </c>
-      <c r="X8" s="13" t="s">
+      <c r="Z8" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="Y8" s="13" t="s">
+      <c r="AA8" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="Z8" s="13" t="s">
+      <c r="AB8" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="AA8" s="13">
+      <c r="AC8" s="13">
         <v>1386</v>
       </c>
-      <c r="AB8" s="13">
+      <c r="AD8" s="13">
         <v>339</v>
       </c>
-      <c r="AC8" s="19" t="s">
+      <c r="AE8" s="19" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A9" s="12">
         <v>13010006</v>
       </c>
@@ -3895,35 +4024,37 @@
       <c r="R9" s="13"/>
       <c r="S9" s="13"/>
       <c r="T9" s="13"/>
-      <c r="U9" s="13">
-        <v>3</v>
-      </c>
-      <c r="V9" s="13">
-        <v>3</v>
-      </c>
+      <c r="U9" s="13"/>
+      <c r="V9" s="13"/>
       <c r="W9" s="13">
-        <v>2</v>
-      </c>
-      <c r="X9" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="X9" s="13">
+        <v>3</v>
+      </c>
+      <c r="Y9" s="13">
+        <v>2</v>
+      </c>
+      <c r="Z9" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="Y9" s="13" t="s">
+      <c r="AA9" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="Z9" s="13" t="s">
+      <c r="AB9" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="AA9" s="13">
+      <c r="AC9" s="13">
         <v>1232</v>
       </c>
-      <c r="AB9" s="13">
+      <c r="AD9" s="13">
         <v>506</v>
       </c>
-      <c r="AC9" s="19" t="s">
+      <c r="AE9" s="19" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A10" s="12">
         <v>13010007</v>
       </c>
@@ -3971,34 +4102,40 @@
       <c r="S10" s="13"/>
       <c r="T10" s="13"/>
       <c r="U10" s="13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V10" s="13">
+        <v>43000002</v>
+      </c>
+      <c r="W10" s="13">
+        <v>2</v>
+      </c>
+      <c r="X10" s="13">
         <v>4</v>
       </c>
-      <c r="W10" s="13">
-        <v>2</v>
-      </c>
-      <c r="X10" s="13" t="s">
+      <c r="Y10" s="13">
+        <v>2</v>
+      </c>
+      <c r="Z10" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="Y10" s="13" t="s">
+      <c r="AA10" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="Z10" s="13" t="s">
+      <c r="AB10" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="AA10" s="13">
+      <c r="AC10" s="13">
         <v>1431</v>
       </c>
-      <c r="AB10" s="13">
+      <c r="AD10" s="13">
         <v>440</v>
       </c>
-      <c r="AC10" s="19" t="s">
+      <c r="AE10" s="19" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A11" s="12">
         <v>13010008</v>
       </c>
@@ -4044,34 +4181,40 @@
         <v>0.4</v>
       </c>
       <c r="U11" s="13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="V11" s="13">
-        <v>3</v>
+        <v>43000002</v>
       </c>
       <c r="W11" s="13">
+        <v>1</v>
+      </c>
+      <c r="X11" s="13">
+        <v>3</v>
+      </c>
+      <c r="Y11" s="13">
         <v>5</v>
       </c>
-      <c r="X11" s="13" t="s">
+      <c r="Z11" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="Y11" s="13" t="s">
+      <c r="AA11" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="Z11" s="13" t="s">
+      <c r="AB11" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="AA11" s="13">
+      <c r="AC11" s="13">
         <v>1250</v>
       </c>
-      <c r="AB11" s="13">
+      <c r="AD11" s="13">
         <v>338</v>
       </c>
-      <c r="AC11" s="19" t="s">
+      <c r="AE11" s="19" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A12" s="12">
         <v>13010009</v>
       </c>
@@ -4123,34 +4266,40 @@
         <v>0.3</v>
       </c>
       <c r="U12" s="13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="V12" s="13">
-        <v>3</v>
+        <v>43000002</v>
       </c>
       <c r="W12" s="13">
-        <v>2</v>
-      </c>
-      <c r="X12" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="X12" s="13">
+        <v>3</v>
+      </c>
+      <c r="Y12" s="13">
+        <v>2</v>
+      </c>
+      <c r="Z12" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="Y12" s="13" t="s">
+      <c r="AA12" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="Z12" s="13" t="s">
+      <c r="AB12" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="AA12" s="13">
+      <c r="AC12" s="13">
         <v>1332</v>
       </c>
-      <c r="AB12" s="13">
+      <c r="AD12" s="13">
         <v>484</v>
       </c>
-      <c r="AC12" s="19" t="s">
+      <c r="AE12" s="19" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A13" s="12">
         <v>13010010</v>
       </c>
@@ -4196,28 +4345,34 @@
       </c>
       <c r="T13" s="15"/>
       <c r="U13" s="13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V13" s="13">
-        <v>2</v>
+        <v>43000002</v>
       </c>
       <c r="W13" s="13">
-        <v>3</v>
-      </c>
-      <c r="X13" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="X13" s="13">
+        <v>2</v>
+      </c>
+      <c r="Y13" s="13">
+        <v>3</v>
+      </c>
+      <c r="Z13" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="Y13" s="15" t="s">
+      <c r="AA13" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="Z13" s="15"/>
-      <c r="AA13" s="15"/>
       <c r="AB13" s="15"/>
-      <c r="AC13" s="19" t="s">
+      <c r="AC13" s="15"/>
+      <c r="AD13" s="15"/>
+      <c r="AE13" s="19" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A14" s="25">
         <v>13010101</v>
       </c>
@@ -4250,35 +4405,37 @@
       <c r="R14" s="13"/>
       <c r="S14" s="13"/>
       <c r="T14" s="13"/>
-      <c r="U14" s="13">
-        <v>2</v>
-      </c>
-      <c r="V14" s="13">
-        <v>3</v>
-      </c>
+      <c r="U14" s="13"/>
+      <c r="V14" s="13"/>
       <c r="W14" s="13">
         <v>2</v>
       </c>
-      <c r="X14" s="13" t="s">
+      <c r="X14" s="13">
+        <v>3</v>
+      </c>
+      <c r="Y14" s="13">
+        <v>2</v>
+      </c>
+      <c r="Z14" s="13" t="s">
         <v>161</v>
       </c>
-      <c r="Y14" s="13" t="s">
+      <c r="AA14" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="Z14" s="13" t="s">
+      <c r="AB14" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="AA14" s="13">
+      <c r="AC14" s="13">
         <v>894</v>
       </c>
-      <c r="AB14" s="13">
+      <c r="AD14" s="13">
         <v>509</v>
       </c>
-      <c r="AC14" s="19" t="s">
+      <c r="AE14" s="19" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A15" s="25">
         <v>13010102</v>
       </c>
@@ -4331,31 +4488,37 @@
         <v>2</v>
       </c>
       <c r="V15" s="13">
+        <v>43000002</v>
+      </c>
+      <c r="W15" s="13">
+        <v>2</v>
+      </c>
+      <c r="X15" s="13">
         <v>5</v>
       </c>
-      <c r="W15" s="13">
-        <v>2</v>
-      </c>
-      <c r="X15" s="13" t="s">
+      <c r="Y15" s="13">
+        <v>2</v>
+      </c>
+      <c r="Z15" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="Y15" s="13" t="s">
+      <c r="AA15" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="Z15" s="13" t="s">
+      <c r="AB15" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="AA15" s="13">
+      <c r="AC15" s="13">
         <v>1040</v>
       </c>
-      <c r="AB15" s="13">
+      <c r="AD15" s="13">
         <v>538</v>
       </c>
-      <c r="AC15" s="19" t="s">
+      <c r="AE15" s="19" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A16" s="25">
         <v>13010103</v>
       </c>
@@ -4401,34 +4564,40 @@
         <v>0.3</v>
       </c>
       <c r="U16" s="13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V16" s="13">
-        <v>3</v>
+        <v>43000002</v>
       </c>
       <c r="W16" s="13">
-        <v>2</v>
-      </c>
-      <c r="X16" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="X16" s="13">
+        <v>3</v>
+      </c>
+      <c r="Y16" s="13">
+        <v>2</v>
+      </c>
+      <c r="Z16" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="Y16" s="13" t="s">
+      <c r="AA16" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="Z16" s="13" t="s">
+      <c r="AB16" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="AA16" s="13">
+      <c r="AC16" s="13">
         <v>1213</v>
       </c>
-      <c r="AB16" s="13">
+      <c r="AD16" s="13">
         <v>655</v>
       </c>
-      <c r="AC16" s="19" t="s">
+      <c r="AE16" s="19" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A17" s="25">
         <v>13010104</v>
       </c>
@@ -4479,31 +4648,37 @@
         <v>2</v>
       </c>
       <c r="V17" s="13">
+        <v>43000002</v>
+      </c>
+      <c r="W17" s="13">
+        <v>2</v>
+      </c>
+      <c r="X17" s="13">
         <v>4</v>
       </c>
-      <c r="W17" s="13">
-        <v>2</v>
-      </c>
-      <c r="X17" s="13" t="s">
+      <c r="Y17" s="13">
+        <v>2</v>
+      </c>
+      <c r="Z17" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="Y17" s="13" t="s">
+      <c r="AA17" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="Z17" s="13" t="s">
+      <c r="AB17" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="AA17" s="13">
+      <c r="AC17" s="13">
         <v>1149</v>
       </c>
-      <c r="AB17" s="13">
+      <c r="AD17" s="13">
         <v>584</v>
       </c>
-      <c r="AC17" s="19" t="s">
+      <c r="AE17" s="19" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A18" s="25">
         <v>13010105</v>
       </c>
@@ -4554,31 +4729,37 @@
         <v>2</v>
       </c>
       <c r="V18" s="13">
-        <v>3</v>
+        <v>43000002</v>
       </c>
       <c r="W18" s="13">
         <v>2</v>
       </c>
-      <c r="X18" s="13" t="s">
+      <c r="X18" s="13">
+        <v>3</v>
+      </c>
+      <c r="Y18" s="13">
+        <v>2</v>
+      </c>
+      <c r="Z18" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="Y18" s="13" t="s">
+      <c r="AA18" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="Z18" s="13" t="s">
+      <c r="AB18" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="AA18" s="13">
+      <c r="AC18" s="13">
         <v>840</v>
       </c>
-      <c r="AB18" s="13">
+      <c r="AD18" s="13">
         <v>444</v>
       </c>
-      <c r="AC18" s="19" t="s">
+      <c r="AE18" s="19" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A19" s="25">
         <v>13010106</v>
       </c>
@@ -4628,34 +4809,40 @@
         <v>0.4</v>
       </c>
       <c r="U19" s="13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V19" s="13">
+        <v>43000002</v>
+      </c>
+      <c r="W19" s="13">
+        <v>3</v>
+      </c>
+      <c r="X19" s="13">
         <v>4</v>
       </c>
-      <c r="W19" s="13">
-        <v>2</v>
-      </c>
-      <c r="X19" s="13" t="s">
+      <c r="Y19" s="13">
+        <v>2</v>
+      </c>
+      <c r="Z19" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="Y19" s="13" t="s">
+      <c r="AA19" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="Z19" s="13" t="s">
+      <c r="AB19" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="AA19" s="13">
+      <c r="AC19" s="13">
         <v>1067</v>
       </c>
-      <c r="AB19" s="13">
+      <c r="AD19" s="13">
         <v>445</v>
       </c>
-      <c r="AC19" s="19" t="s">
+      <c r="AE19" s="19" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A20" s="25">
         <v>13010107</v>
       </c>
@@ -4707,34 +4894,40 @@
         <v>0.8</v>
       </c>
       <c r="U20" s="13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V20" s="13">
-        <v>3</v>
+        <v>43000002</v>
       </c>
       <c r="W20" s="13">
-        <v>2</v>
-      </c>
-      <c r="X20" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="X20" s="13">
+        <v>3</v>
+      </c>
+      <c r="Y20" s="13">
+        <v>2</v>
+      </c>
+      <c r="Z20" s="13" t="s">
         <v>186</v>
       </c>
-      <c r="Y20" s="13" t="s">
+      <c r="AA20" s="13" t="s">
         <v>186</v>
       </c>
-      <c r="Z20" s="13" t="s">
+      <c r="AB20" s="13" t="s">
         <v>170</v>
       </c>
-      <c r="AA20" s="16">
+      <c r="AC20" s="16">
         <v>850</v>
       </c>
-      <c r="AB20" s="16">
+      <c r="AD20" s="16">
         <v>589</v>
       </c>
-      <c r="AC20" s="19" t="s">
+      <c r="AE20" s="19" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A21" s="25">
         <v>13010108</v>
       </c>
@@ -4782,34 +4975,40 @@
         <v>0.8</v>
       </c>
       <c r="U21" s="13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V21" s="13">
-        <v>3</v>
+        <v>43000002</v>
       </c>
       <c r="W21" s="13">
         <v>3</v>
       </c>
-      <c r="X21" s="13" t="s">
+      <c r="X21" s="13">
+        <v>3</v>
+      </c>
+      <c r="Y21" s="13">
+        <v>3</v>
+      </c>
+      <c r="Z21" s="13" t="s">
         <v>188</v>
       </c>
-      <c r="Y21" s="13" t="s">
+      <c r="AA21" s="13" t="s">
         <v>188</v>
       </c>
-      <c r="Z21" s="16" t="s">
+      <c r="AB21" s="16" t="s">
         <v>174</v>
       </c>
-      <c r="AA21" s="13">
+      <c r="AC21" s="13">
         <v>682</v>
       </c>
-      <c r="AB21" s="13">
+      <c r="AD21" s="13">
         <v>545</v>
       </c>
-      <c r="AC21" s="19" t="s">
+      <c r="AE21" s="19" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A22" s="25">
         <v>13010109</v>
       </c>
@@ -4857,34 +5056,40 @@
       </c>
       <c r="T22" s="15"/>
       <c r="U22" s="13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V22" s="13">
-        <v>3</v>
+        <v>43000002</v>
       </c>
       <c r="W22" s="13">
         <v>3</v>
       </c>
-      <c r="X22" s="13" t="s">
+      <c r="X22" s="13">
+        <v>3</v>
+      </c>
+      <c r="Y22" s="13">
+        <v>3</v>
+      </c>
+      <c r="Z22" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="Y22" s="20" t="s">
+      <c r="AA22" s="20" t="s">
         <v>200</v>
       </c>
-      <c r="Z22" s="16" t="s">
+      <c r="AB22" s="16" t="s">
         <v>196</v>
       </c>
-      <c r="AA22" s="16">
+      <c r="AC22" s="16">
         <v>643</v>
       </c>
-      <c r="AB22" s="16">
+      <c r="AD22" s="16">
         <v>455</v>
       </c>
-      <c r="AC22" s="19" t="s">
+      <c r="AE22" s="19" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A23" s="25">
         <v>13010110</v>
       </c>
@@ -4935,31 +5140,37 @@
         <v>2</v>
       </c>
       <c r="V23" s="13">
+        <v>43000002</v>
+      </c>
+      <c r="W23" s="13">
+        <v>2</v>
+      </c>
+      <c r="X23" s="13">
         <v>4</v>
       </c>
-      <c r="W23" s="13">
-        <v>3</v>
-      </c>
-      <c r="X23" s="20" t="s">
+      <c r="Y23" s="13">
+        <v>3</v>
+      </c>
+      <c r="Z23" s="20" t="s">
         <v>201</v>
       </c>
-      <c r="Y23" s="20" t="s">
+      <c r="AA23" s="20" t="s">
         <v>201</v>
       </c>
-      <c r="Z23" s="16" t="s">
+      <c r="AB23" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="AA23" s="16">
+      <c r="AC23" s="16">
         <v>720</v>
       </c>
-      <c r="AB23" s="16">
+      <c r="AD23" s="16">
         <v>375</v>
       </c>
-      <c r="AC23" s="19" t="s">
+      <c r="AE23" s="19" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A24" s="23">
         <v>13010201</v>
       </c>
@@ -4992,35 +5203,37 @@
       <c r="R24" s="15"/>
       <c r="S24" s="15"/>
       <c r="T24" s="15"/>
-      <c r="U24" s="13">
+      <c r="U24" s="15"/>
+      <c r="V24" s="13"/>
+      <c r="W24" s="13">
         <v>4</v>
       </c>
-      <c r="V24" s="13">
-        <v>2</v>
-      </c>
-      <c r="W24" s="13">
-        <v>2</v>
-      </c>
-      <c r="X24" s="13" t="s">
+      <c r="X24" s="13">
+        <v>2</v>
+      </c>
+      <c r="Y24" s="13">
+        <v>2</v>
+      </c>
+      <c r="Z24" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="Y24" s="13" t="s">
+      <c r="AA24" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="Z24" s="16" t="s">
+      <c r="AB24" s="16" t="s">
         <v>171</v>
       </c>
-      <c r="AA24" s="13">
+      <c r="AC24" s="13">
         <v>807</v>
       </c>
-      <c r="AB24" s="13">
+      <c r="AD24" s="13">
         <v>720</v>
       </c>
-      <c r="AC24" s="19" t="s">
+      <c r="AE24" s="19" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A25" s="23">
         <v>13010202</v>
       </c>
@@ -5066,34 +5279,40 @@
         <v>0.3</v>
       </c>
       <c r="U25" s="13">
+        <v>2</v>
+      </c>
+      <c r="V25" s="13">
+        <v>43000002</v>
+      </c>
+      <c r="W25" s="13">
         <v>4</v>
       </c>
-      <c r="V25" s="13">
-        <v>1</v>
-      </c>
-      <c r="W25" s="13">
-        <v>3</v>
-      </c>
-      <c r="X25" s="13" t="s">
+      <c r="X25" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y25" s="13">
+        <v>3</v>
+      </c>
+      <c r="Z25" s="13" t="s">
         <v>189</v>
       </c>
-      <c r="Y25" s="13" t="s">
+      <c r="AA25" s="13" t="s">
         <v>189</v>
       </c>
-      <c r="Z25" s="15" t="s">
+      <c r="AB25" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="AA25" s="15">
+      <c r="AC25" s="15">
         <v>974</v>
       </c>
-      <c r="AB25" s="15">
+      <c r="AD25" s="15">
         <v>594</v>
       </c>
-      <c r="AC25" s="19" t="s">
+      <c r="AE25" s="19" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A26" s="23">
         <v>13010203</v>
       </c>
@@ -5141,34 +5360,40 @@
         <v>0.2</v>
       </c>
       <c r="U26" s="13">
+        <v>2</v>
+      </c>
+      <c r="V26" s="13">
+        <v>43000002</v>
+      </c>
+      <c r="W26" s="13">
         <v>4</v>
       </c>
-      <c r="V26" s="13">
-        <v>1</v>
-      </c>
-      <c r="W26" s="13">
-        <v>3</v>
-      </c>
-      <c r="X26" s="13" t="s">
+      <c r="X26" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y26" s="13">
+        <v>3</v>
+      </c>
+      <c r="Z26" s="13" t="s">
         <v>190</v>
       </c>
-      <c r="Y26" s="13" t="s">
+      <c r="AA26" s="13" t="s">
         <v>190</v>
       </c>
-      <c r="Z26" s="15" t="s">
+      <c r="AB26" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="AA26" s="15">
+      <c r="AC26" s="15">
         <v>1080</v>
       </c>
-      <c r="AB26" s="15">
+      <c r="AD26" s="15">
         <v>720</v>
       </c>
-      <c r="AC26" s="19" t="s">
+      <c r="AE26" s="19" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A27" s="23">
         <v>13010204</v>
       </c>
@@ -5216,34 +5441,40 @@
       </c>
       <c r="T27" s="15"/>
       <c r="U27" s="13">
+        <v>2</v>
+      </c>
+      <c r="V27" s="13">
+        <v>43000002</v>
+      </c>
+      <c r="W27" s="13">
         <v>4</v>
       </c>
-      <c r="V27" s="13">
-        <v>1</v>
-      </c>
-      <c r="W27" s="13">
-        <v>3</v>
-      </c>
-      <c r="X27" s="13" t="s">
+      <c r="X27" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y27" s="13">
+        <v>3</v>
+      </c>
+      <c r="Z27" s="13" t="s">
         <v>191</v>
       </c>
-      <c r="Y27" s="13" t="s">
+      <c r="AA27" s="13" t="s">
         <v>191</v>
       </c>
-      <c r="Z27" s="15" t="s">
+      <c r="AB27" s="15" t="s">
         <v>167</v>
       </c>
-      <c r="AA27" s="15">
+      <c r="AC27" s="15">
         <v>1074</v>
       </c>
-      <c r="AB27" s="15">
+      <c r="AD27" s="15">
         <v>630</v>
       </c>
-      <c r="AC27" s="19" t="s">
+      <c r="AE27" s="19" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A28" s="23">
         <v>13010205</v>
       </c>
@@ -5287,34 +5518,40 @@
         <v>0.3</v>
       </c>
       <c r="U28" s="13">
+        <v>2</v>
+      </c>
+      <c r="V28" s="13">
+        <v>43000002</v>
+      </c>
+      <c r="W28" s="13">
         <v>4</v>
       </c>
-      <c r="V28" s="13">
-        <v>1</v>
-      </c>
-      <c r="W28" s="13">
-        <v>2</v>
-      </c>
-      <c r="X28" s="20" t="s">
+      <c r="X28" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y28" s="13">
+        <v>2</v>
+      </c>
+      <c r="Z28" s="20" t="s">
         <v>187</v>
       </c>
-      <c r="Y28" s="20" t="s">
+      <c r="AA28" s="20" t="s">
         <v>187</v>
       </c>
-      <c r="Z28" s="16" t="s">
+      <c r="AB28" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="AA28" s="13">
+      <c r="AC28" s="13">
         <v>717</v>
       </c>
-      <c r="AB28" s="13">
+      <c r="AD28" s="13">
         <v>655</v>
       </c>
-      <c r="AC28" s="19" t="s">
+      <c r="AE28" s="19" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A29" s="23">
         <v>13010206</v>
       </c>
@@ -5356,34 +5593,40 @@
       <c r="S29" s="15"/>
       <c r="T29" s="15"/>
       <c r="U29" s="13">
+        <v>2</v>
+      </c>
+      <c r="V29" s="13">
+        <v>43000002</v>
+      </c>
+      <c r="W29" s="13">
         <v>4</v>
       </c>
-      <c r="V29" s="13">
-        <v>1</v>
-      </c>
-      <c r="W29" s="13">
-        <v>2</v>
-      </c>
-      <c r="X29" s="20" t="s">
+      <c r="X29" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y29" s="13">
+        <v>2</v>
+      </c>
+      <c r="Z29" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="Y29" s="20" t="s">
+      <c r="AA29" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="Z29" s="16" t="s">
+      <c r="AB29" s="16" t="s">
         <v>173</v>
       </c>
-      <c r="AA29" s="13">
+      <c r="AC29" s="13">
         <v>637</v>
       </c>
-      <c r="AB29" s="13">
+      <c r="AD29" s="13">
         <v>735</v>
       </c>
-      <c r="AC29" s="19" t="s">
+      <c r="AE29" s="19" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A30" s="23">
         <v>13010207</v>
       </c>
@@ -5427,34 +5670,40 @@
         <v>0.4</v>
       </c>
       <c r="U30" s="13">
+        <v>2</v>
+      </c>
+      <c r="V30" s="13">
+        <v>43000002</v>
+      </c>
+      <c r="W30" s="13">
         <v>5</v>
       </c>
-      <c r="V30" s="13">
-        <v>1</v>
-      </c>
-      <c r="W30" s="13">
+      <c r="X30" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y30" s="13">
         <v>4</v>
       </c>
-      <c r="X30" s="13" t="s">
+      <c r="Z30" s="13" t="s">
         <v>192</v>
       </c>
-      <c r="Y30" s="13" t="s">
+      <c r="AA30" s="13" t="s">
         <v>192</v>
       </c>
-      <c r="Z30" s="13" t="s">
+      <c r="AB30" s="13" t="s">
         <v>175</v>
       </c>
-      <c r="AA30" s="13">
+      <c r="AC30" s="13">
         <v>737</v>
       </c>
-      <c r="AB30" s="13">
+      <c r="AD30" s="13">
         <v>785</v>
       </c>
-      <c r="AC30" s="19" t="s">
+      <c r="AE30" s="19" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A31" s="23">
         <v>13010208</v>
       </c>
@@ -5504,34 +5753,40 @@
         <v>0.5</v>
       </c>
       <c r="U31" s="13">
+        <v>2</v>
+      </c>
+      <c r="V31" s="13">
+        <v>43000002</v>
+      </c>
+      <c r="W31" s="13">
         <v>4</v>
       </c>
-      <c r="V31" s="13">
-        <v>1</v>
-      </c>
-      <c r="W31" s="13">
-        <v>2</v>
-      </c>
-      <c r="X31" s="13" t="s">
+      <c r="X31" s="13">
+        <v>1</v>
+      </c>
+      <c r="Y31" s="13">
+        <v>2</v>
+      </c>
+      <c r="Z31" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="Y31" s="13" t="s">
+      <c r="AA31" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="Z31" s="15" t="s">
+      <c r="AB31" s="15" t="s">
         <v>168</v>
       </c>
-      <c r="AA31" s="19">
+      <c r="AC31" s="19">
         <v>894</v>
       </c>
-      <c r="AB31" s="19">
+      <c r="AD31" s="19">
         <v>679</v>
       </c>
-      <c r="AC31" s="19" t="s">
+      <c r="AE31" s="19" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A32" s="23">
         <v>13010209</v>
       </c>
@@ -5573,34 +5828,40 @@
       <c r="S32" s="15"/>
       <c r="T32" s="15"/>
       <c r="U32" s="13">
+        <v>2</v>
+      </c>
+      <c r="V32" s="13">
+        <v>43000002</v>
+      </c>
+      <c r="W32" s="13">
         <v>4</v>
       </c>
-      <c r="V32" s="13">
-        <v>2</v>
-      </c>
-      <c r="W32" s="13">
-        <v>2</v>
-      </c>
-      <c r="X32" s="20" t="s">
+      <c r="X32" s="13">
+        <v>2</v>
+      </c>
+      <c r="Y32" s="13">
+        <v>2</v>
+      </c>
+      <c r="Z32" s="20" t="s">
         <v>194</v>
       </c>
-      <c r="Y32" s="20" t="s">
+      <c r="AA32" s="20" t="s">
         <v>194</v>
       </c>
-      <c r="Z32" s="16" t="s">
+      <c r="AB32" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="AA32" s="19">
+      <c r="AC32" s="19">
         <v>984</v>
       </c>
-      <c r="AB32" s="19">
+      <c r="AD32" s="19">
         <v>734</v>
       </c>
-      <c r="AC32" s="19" t="s">
+      <c r="AE32" s="19" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A33" s="26">
         <v>13010301</v>
       </c>
@@ -5648,34 +5909,40 @@
         <v>0.3</v>
       </c>
       <c r="U33" s="13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V33" s="13">
-        <v>3</v>
+        <v>43000002</v>
       </c>
       <c r="W33" s="13">
-        <v>1</v>
-      </c>
-      <c r="X33" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="X33" s="13">
+        <v>3</v>
+      </c>
+      <c r="Y33" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z33" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="Y33" s="13" t="s">
+      <c r="AA33" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="Z33" s="13" t="s">
+      <c r="AB33" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="AA33" s="21">
+      <c r="AC33" s="21">
         <v>1550</v>
       </c>
-      <c r="AB33" s="21">
+      <c r="AD33" s="21">
         <v>505</v>
       </c>
-      <c r="AC33" s="19" t="s">
+      <c r="AE33" s="19" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A34" s="26">
         <v>13010302</v>
       </c>
@@ -5721,34 +5988,40 @@
         <v>0.3</v>
       </c>
       <c r="U34" s="13">
+        <v>2</v>
+      </c>
+      <c r="V34" s="13">
+        <v>43000002</v>
+      </c>
+      <c r="W34" s="13">
         <v>4</v>
       </c>
-      <c r="V34" s="13">
-        <v>3</v>
-      </c>
-      <c r="W34" s="13">
-        <v>1</v>
-      </c>
-      <c r="X34" s="13" t="s">
+      <c r="X34" s="13">
+        <v>3</v>
+      </c>
+      <c r="Y34" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z34" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="Y34" s="13" t="s">
+      <c r="AA34" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="Z34" s="13" t="s">
+      <c r="AB34" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="AA34" s="21">
+      <c r="AC34" s="21">
         <v>1441</v>
       </c>
-      <c r="AB34" s="21">
+      <c r="AD34" s="21">
         <v>527</v>
       </c>
-      <c r="AC34" s="19" t="s">
+      <c r="AE34" s="19" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A35" s="26">
         <v>13010303</v>
       </c>
@@ -5800,34 +6073,40 @@
         <v>0.8</v>
       </c>
       <c r="U35" s="13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V35" s="13">
-        <v>3</v>
+        <v>43000002</v>
       </c>
       <c r="W35" s="13">
-        <v>2</v>
-      </c>
-      <c r="X35" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="X35" s="13">
+        <v>3</v>
+      </c>
+      <c r="Y35" s="13">
+        <v>2</v>
+      </c>
+      <c r="Z35" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="Y35" s="13" t="s">
+      <c r="AA35" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="Z35" s="13" t="s">
+      <c r="AB35" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="AA35" s="21">
+      <c r="AC35" s="21">
         <v>1574</v>
       </c>
-      <c r="AB35" s="21">
+      <c r="AD35" s="21">
         <v>373</v>
       </c>
-      <c r="AC35" s="19" t="s">
+      <c r="AE35" s="19" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A36" s="17">
         <v>13020001</v>
       </c>
@@ -5870,29 +6149,31 @@
         <v>0.3</v>
       </c>
       <c r="T36" s="13"/>
-      <c r="U36" s="13">
-        <v>2</v>
-      </c>
-      <c r="V36" s="13">
-        <v>3</v>
-      </c>
+      <c r="U36" s="13"/>
+      <c r="V36" s="13"/>
       <c r="W36" s="13">
         <v>2</v>
       </c>
-      <c r="X36" s="13" t="s">
+      <c r="X36" s="13">
+        <v>3</v>
+      </c>
+      <c r="Y36" s="13">
+        <v>2</v>
+      </c>
+      <c r="Z36" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="Y36" s="13" t="s">
+      <c r="AA36" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="Z36" s="13"/>
-      <c r="AA36" s="13"/>
       <c r="AB36" s="13"/>
-      <c r="AC36" s="19" t="s">
+      <c r="AC36" s="13"/>
+      <c r="AD36" s="13"/>
+      <c r="AE36" s="19" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A37" s="17">
         <v>13020002</v>
       </c>
@@ -5931,29 +6212,31 @@
       <c r="T37" s="13">
         <v>0.2</v>
       </c>
-      <c r="U37" s="13">
-        <v>2</v>
-      </c>
-      <c r="V37" s="13">
-        <v>3</v>
-      </c>
+      <c r="U37" s="13"/>
+      <c r="V37" s="13"/>
       <c r="W37" s="13">
         <v>2</v>
       </c>
-      <c r="X37" s="13" t="s">
+      <c r="X37" s="13">
+        <v>3</v>
+      </c>
+      <c r="Y37" s="13">
+        <v>2</v>
+      </c>
+      <c r="Z37" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="Y37" s="13" t="s">
+      <c r="AA37" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="Z37" s="13"/>
-      <c r="AA37" s="13"/>
       <c r="AB37" s="13"/>
-      <c r="AC37" s="19" t="s">
+      <c r="AC37" s="13"/>
+      <c r="AD37" s="13"/>
+      <c r="AE37" s="19" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A38" s="17">
         <v>13020011</v>
       </c>
@@ -5994,29 +6277,31 @@
         <v>0.2</v>
       </c>
       <c r="T38" s="13"/>
-      <c r="U38" s="13">
-        <v>2</v>
-      </c>
-      <c r="V38" s="13">
+      <c r="U38" s="13"/>
+      <c r="V38" s="13"/>
+      <c r="W38" s="13">
+        <v>2</v>
+      </c>
+      <c r="X38" s="13">
         <v>4</v>
       </c>
-      <c r="W38" s="13">
-        <v>2</v>
-      </c>
-      <c r="X38" s="13" t="s">
+      <c r="Y38" s="13">
+        <v>2</v>
+      </c>
+      <c r="Z38" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="Y38" s="13" t="s">
+      <c r="AA38" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="Z38" s="13"/>
-      <c r="AA38" s="13"/>
       <c r="AB38" s="13"/>
-      <c r="AC38" s="19" t="s">
+      <c r="AC38" s="13"/>
+      <c r="AD38" s="13"/>
+      <c r="AE38" s="19" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A39" s="17">
         <v>13020012</v>
       </c>
@@ -6053,29 +6338,31 @@
       <c r="T39" s="13">
         <v>0.3</v>
       </c>
-      <c r="U39" s="13">
-        <v>2</v>
-      </c>
-      <c r="V39" s="13">
+      <c r="U39" s="13"/>
+      <c r="V39" s="13"/>
+      <c r="W39" s="13">
+        <v>2</v>
+      </c>
+      <c r="X39" s="13">
         <v>4</v>
       </c>
-      <c r="W39" s="13">
-        <v>2</v>
-      </c>
-      <c r="X39" s="13" t="s">
+      <c r="Y39" s="13">
+        <v>2</v>
+      </c>
+      <c r="Z39" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="Y39" s="13" t="s">
+      <c r="AA39" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="Z39" s="13"/>
-      <c r="AA39" s="13"/>
       <c r="AB39" s="13"/>
-      <c r="AC39" s="19" t="s">
+      <c r="AC39" s="13"/>
+      <c r="AD39" s="13"/>
+      <c r="AE39" s="19" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A40" s="17">
         <v>13020013</v>
       </c>
@@ -6108,29 +6395,31 @@
       <c r="R40" s="13"/>
       <c r="S40" s="13"/>
       <c r="T40" s="13"/>
-      <c r="U40" s="13">
-        <v>2</v>
-      </c>
-      <c r="V40" s="13">
+      <c r="U40" s="13"/>
+      <c r="V40" s="13"/>
+      <c r="W40" s="13">
+        <v>2</v>
+      </c>
+      <c r="X40" s="13">
         <v>4</v>
       </c>
-      <c r="W40" s="13">
-        <v>2</v>
-      </c>
-      <c r="X40" s="13" t="s">
+      <c r="Y40" s="13">
+        <v>2</v>
+      </c>
+      <c r="Z40" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="Y40" s="13" t="s">
+      <c r="AA40" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="Z40" s="13"/>
-      <c r="AA40" s="13"/>
       <c r="AB40" s="13"/>
-      <c r="AC40" s="19" t="s">
+      <c r="AC40" s="13"/>
+      <c r="AD40" s="13"/>
+      <c r="AE40" s="19" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A41" s="17">
         <v>13020021</v>
       </c>
@@ -6173,29 +6462,31 @@
       <c r="T41" s="13">
         <v>0.4</v>
       </c>
-      <c r="U41" s="13">
-        <v>3</v>
-      </c>
-      <c r="V41" s="13">
-        <v>3</v>
-      </c>
+      <c r="U41" s="13"/>
+      <c r="V41" s="13"/>
       <c r="W41" s="13">
-        <v>1</v>
-      </c>
-      <c r="X41" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="X41" s="13">
+        <v>3</v>
+      </c>
+      <c r="Y41" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z41" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="Y41" s="13" t="s">
+      <c r="AA41" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="Z41" s="13"/>
-      <c r="AA41" s="13"/>
       <c r="AB41" s="13"/>
-      <c r="AC41" s="19" t="s">
+      <c r="AC41" s="13"/>
+      <c r="AD41" s="13"/>
+      <c r="AE41" s="19" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A42" s="17">
         <v>13020022</v>
       </c>
@@ -6238,29 +6529,31 @@
       <c r="T42" s="13">
         <v>0.2</v>
       </c>
-      <c r="U42" s="13">
-        <v>3</v>
-      </c>
-      <c r="V42" s="13">
-        <v>3</v>
-      </c>
+      <c r="U42" s="13"/>
+      <c r="V42" s="13"/>
       <c r="W42" s="13">
-        <v>1</v>
-      </c>
-      <c r="X42" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="X42" s="13">
+        <v>3</v>
+      </c>
+      <c r="Y42" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z42" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="Y42" s="13" t="s">
+      <c r="AA42" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="Z42" s="13"/>
-      <c r="AA42" s="13"/>
       <c r="AB42" s="13"/>
-      <c r="AC42" s="19" t="s">
+      <c r="AC42" s="13"/>
+      <c r="AD42" s="13"/>
+      <c r="AE42" s="19" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A43" s="17">
         <v>13020023</v>
       </c>
@@ -6299,29 +6592,31 @@
       <c r="T43" s="13">
         <v>0.2</v>
       </c>
-      <c r="U43" s="13">
-        <v>3</v>
-      </c>
-      <c r="V43" s="13">
-        <v>3</v>
-      </c>
+      <c r="U43" s="13"/>
+      <c r="V43" s="13"/>
       <c r="W43" s="13">
-        <v>1</v>
-      </c>
-      <c r="X43" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="X43" s="13">
+        <v>3</v>
+      </c>
+      <c r="Y43" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z43" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="Y43" s="13" t="s">
+      <c r="AA43" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Z43" s="13"/>
-      <c r="AA43" s="13"/>
       <c r="AB43" s="13"/>
-      <c r="AC43" s="19" t="s">
+      <c r="AC43" s="13"/>
+      <c r="AD43" s="13"/>
+      <c r="AE43" s="19" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A44" s="18">
         <v>13020031</v>
       </c>
@@ -6354,29 +6649,31 @@
       <c r="R44" s="15"/>
       <c r="S44" s="15"/>
       <c r="T44" s="15"/>
-      <c r="U44" s="13">
-        <v>2</v>
-      </c>
-      <c r="V44" s="13">
-        <v>2</v>
-      </c>
+      <c r="U44" s="15"/>
+      <c r="V44" s="13"/>
       <c r="W44" s="13">
+        <v>2</v>
+      </c>
+      <c r="X44" s="13">
+        <v>2</v>
+      </c>
+      <c r="Y44" s="13">
         <v>5</v>
       </c>
-      <c r="X44" s="13" t="s">
+      <c r="Z44" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="Y44" s="15" t="s">
+      <c r="AA44" s="15" t="s">
         <v>152</v>
       </c>
-      <c r="Z44" s="15"/>
-      <c r="AA44" s="15"/>
       <c r="AB44" s="15"/>
-      <c r="AC44" s="19" t="s">
+      <c r="AC44" s="15"/>
+      <c r="AD44" s="15"/>
+      <c r="AE44" s="19" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A45" s="18">
         <v>13020032</v>
       </c>
@@ -6409,29 +6706,31 @@
       <c r="R45" s="15"/>
       <c r="S45" s="15"/>
       <c r="T45" s="15"/>
-      <c r="U45" s="13">
-        <v>2</v>
-      </c>
-      <c r="V45" s="13">
-        <v>2</v>
-      </c>
+      <c r="U45" s="15"/>
+      <c r="V45" s="13"/>
       <c r="W45" s="13">
+        <v>2</v>
+      </c>
+      <c r="X45" s="13">
+        <v>2</v>
+      </c>
+      <c r="Y45" s="13">
         <v>5</v>
       </c>
-      <c r="X45" s="13" t="s">
+      <c r="Z45" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="Y45" s="15" t="s">
+      <c r="AA45" s="15" t="s">
         <v>153</v>
       </c>
-      <c r="Z45" s="15"/>
-      <c r="AA45" s="15"/>
       <c r="AB45" s="15"/>
-      <c r="AC45" s="19" t="s">
+      <c r="AC45" s="15"/>
+      <c r="AD45" s="15"/>
+      <c r="AE45" s="19" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A46" s="18">
         <v>13020033</v>
       </c>
@@ -6464,29 +6763,31 @@
       <c r="R46" s="15"/>
       <c r="S46" s="15"/>
       <c r="T46" s="15"/>
-      <c r="U46" s="13">
-        <v>2</v>
-      </c>
-      <c r="V46" s="13">
-        <v>2</v>
-      </c>
+      <c r="U46" s="15"/>
+      <c r="V46" s="13"/>
       <c r="W46" s="13">
+        <v>2</v>
+      </c>
+      <c r="X46" s="13">
+        <v>2</v>
+      </c>
+      <c r="Y46" s="13">
         <v>5</v>
       </c>
-      <c r="X46" s="13" t="s">
+      <c r="Z46" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="Y46" s="15" t="s">
+      <c r="AA46" s="15" t="s">
         <v>154</v>
       </c>
-      <c r="Z46" s="19"/>
-      <c r="AA46" s="19"/>
       <c r="AB46" s="19"/>
-      <c r="AC46" s="19" t="s">
+      <c r="AC46" s="19"/>
+      <c r="AD46" s="19"/>
+      <c r="AE46" s="19" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A47" s="18">
         <v>13020034</v>
       </c>
@@ -6519,29 +6820,31 @@
       <c r="R47" s="15"/>
       <c r="S47" s="15"/>
       <c r="T47" s="15"/>
-      <c r="U47" s="13">
-        <v>2</v>
-      </c>
-      <c r="V47" s="13">
-        <v>2</v>
-      </c>
+      <c r="U47" s="15"/>
+      <c r="V47" s="13"/>
       <c r="W47" s="13">
+        <v>2</v>
+      </c>
+      <c r="X47" s="13">
+        <v>2</v>
+      </c>
+      <c r="Y47" s="13">
         <v>5</v>
       </c>
-      <c r="X47" s="13" t="s">
+      <c r="Z47" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="Y47" s="15" t="s">
+      <c r="AA47" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="Z47" s="19"/>
-      <c r="AA47" s="19"/>
       <c r="AB47" s="19"/>
-      <c r="AC47" s="19" t="s">
+      <c r="AC47" s="19"/>
+      <c r="AD47" s="19"/>
+      <c r="AE47" s="19" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A48" s="18">
         <v>13020035</v>
       </c>
@@ -6574,42 +6877,44 @@
       <c r="R48" s="15"/>
       <c r="S48" s="15"/>
       <c r="T48" s="15"/>
-      <c r="U48" s="13">
-        <v>2</v>
-      </c>
-      <c r="V48" s="13">
-        <v>2</v>
-      </c>
+      <c r="U48" s="15"/>
+      <c r="V48" s="13"/>
       <c r="W48" s="13">
+        <v>2</v>
+      </c>
+      <c r="X48" s="13">
+        <v>2</v>
+      </c>
+      <c r="Y48" s="13">
         <v>5</v>
       </c>
-      <c r="X48" s="13" t="s">
+      <c r="Z48" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="Y48" s="15" t="s">
+      <c r="AA48" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="Z48" s="19"/>
-      <c r="AA48" s="19"/>
       <c r="AB48" s="19"/>
-      <c r="AC48" s="19" t="s">
+      <c r="AC48" s="19"/>
+      <c r="AD48" s="19"/>
+      <c r="AE48" s="19" t="s">
         <v>247</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="I4:T48">
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+  <conditionalFormatting sqref="I4:V48">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:H48">
-    <cfRule type="containsBlanks" dxfId="0" priority="5">
+    <cfRule type="containsBlanks" dxfId="1" priority="5">
       <formula>LEN(TRIM(G4))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
new sq bg icon show rule
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Scene.xlsx
+++ b/ConfigData/Xlsx/Scene.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9A0DC765-A1F8-4342-93C6-EC9363AAA22D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{04E34B7F-EAFD-4242-ACCF-A1127399A33B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -500,10 +500,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>coldwind;3|snowhill;2|snowmountain;2|ropeway;1|iceland;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>dgforestmaze</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -536,10 +532,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>ruintown1;1|manflower;2|cornfield;1|honeyhome;3|poppyfield;1|river;2|insectstorm;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>suntemple;2|shadowprince;1|colordoor;1|blockway;1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -552,10 +544,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>shell;2|waternest;3|sandflow;1|corsair1;1|ruinpiece;3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>布萨特高塔</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -852,10 +840,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>trees;3|grave;1|portal;1|manflower;1|gamerace;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>river;2</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -864,14 +848,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>wolfnest;2|gamegamble;1|sewer;3|river;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>portal;1|grave;2|hiddeway;1|snare;2|starve;2|blockway;1|suntemple;2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>poppyfield;1|river;2</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -880,10 +856,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>river;2|stone;3|ruintown1;1|hiddeway;1|manflower;2|weaponseller;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>sandflow;2|stone;3</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -1046,6 +1018,34 @@
   </si>
   <si>
     <t>EnemyIds</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>wolfnest;2|gamegamble;1|river;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>trees;2|grave;1|portal;1|manflower;1|gamerace;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>river;1|stone;3|ruintown1;1|hiddeway;1|manflower;2|weaponseller;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>coldwind;2|snowhill;1|snowmountain;2|ropeway;1|iceland;2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ruintown1;1|manflower;2|cornfield;1|honeyhome;2|poppyfield;1|river;1|insectstorm;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>portal;1|grave;2|hiddeway;1|snare;1|starve;2|blockway;1|suntemple;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>shell;1|waternest;2|sandflow;1|corsair1;1|ruinpiece;3</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1987,85 +1987,6 @@
         <color theme="1"/>
         <name val="宋体"/>
         <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <family val="3"/>
         <scheme val="minor"/>
       </font>
     </dxf>
@@ -2191,6 +2112,64 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -2901,6 +2880,27 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2915,43 +2915,43 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A3:AE48" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35" tableBorderDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A3:AE48" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32" tableBorderDxfId="31">
   <autoFilter ref="A3:AE48" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState ref="A4:AD48">
     <sortCondition ref="A3:A48"/>
   </sortState>
   <tableColumns count="31">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="32"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Type" dataDxfId="31"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="RegionId" dataDxfId="30"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Level" dataDxfId="29"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="ReviveScene" dataDxfId="28"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Quest" dataDxfId="27"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="QuestRandom" dataDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="QPortal" dataDxfId="25"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="QCardChange" dataDxfId="24"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="QPiece" dataDxfId="23"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="QMerchant" dataDxfId="22"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="QDoctor" dataDxfId="21"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="QAngel" dataDxfId="20"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="QRes" dataDxfId="19"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="QItemDrug" dataDxfId="18"/>
-    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="QItemFish" dataDxfId="17"/>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="QItemOre" dataDxfId="16"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="QItemMushroom" dataDxfId="15"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="QItemWood" dataDxfId="14"/>
-    <tableColumn id="32" xr3:uid="{A83B2B25-5C5C-426D-A301-0017A60CEB0A}" name="QEnemy" dataDxfId="0"/>
-    <tableColumn id="25" xr3:uid="{52509577-5139-4AB6-BDC1-0A628B9D6BD7}" name="EnemyIds" dataDxfId="4"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Temperature" dataDxfId="13"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="Humitity" dataDxfId="12"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="Altitude" dataDxfId="11"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Url" dataDxfId="10"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="TilePath" dataDxfId="9"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Icon" dataDxfId="8"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="IconX" dataDxfId="7"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="IconY" dataDxfId="6"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="BGM" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="29"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Type" dataDxfId="28"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="RegionId" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Level" dataDxfId="26"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="ReviveScene" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Quest" dataDxfId="24"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="QuestRandom" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="QPortal" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="QCardChange" dataDxfId="21"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="QPiece" dataDxfId="20"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="QMerchant" dataDxfId="19"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="QDoctor" dataDxfId="18"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="QAngel" dataDxfId="17"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="QRes" dataDxfId="16"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="QItemDrug" dataDxfId="15"/>
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="QItemFish" dataDxfId="14"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="QItemOre" dataDxfId="13"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="QItemMushroom" dataDxfId="12"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="QItemWood" dataDxfId="11"/>
+    <tableColumn id="32" xr3:uid="{A83B2B25-5C5C-426D-A301-0017A60CEB0A}" name="QEnemy" dataDxfId="10"/>
+    <tableColumn id="25" xr3:uid="{52509577-5139-4AB6-BDC1-0A628B9D6BD7}" name="EnemyIds" dataDxfId="9"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Temperature" dataDxfId="8"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="Humitity" dataDxfId="7"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="Altitude" dataDxfId="6"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Url" dataDxfId="5"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="TilePath" dataDxfId="4"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Icon" dataDxfId="3"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="IconX" dataDxfId="2"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="IconY" dataDxfId="1"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="BGM" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3280,8 +3280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="U10" sqref="U10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="U29" sqref="U29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3320,7 +3320,7 @@
         <v>87</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>17</v>
@@ -3335,7 +3335,7 @@
         <v>84</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>49</v>
@@ -3353,37 +3353,37 @@
         <v>57</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="R1" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="S1" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="S1" s="3" t="s">
-        <v>224</v>
-      </c>
       <c r="T1" s="3" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="V1" s="28" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="W1" s="30" t="s">
+        <v>205</v>
+      </c>
+      <c r="X1" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="X1" s="2" t="s">
-        <v>211</v>
-      </c>
       <c r="Y1" s="28" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="Z1" s="2" t="s">
         <v>18</v>
@@ -3401,7 +3401,7 @@
         <v>81</v>
       </c>
       <c r="AE1" s="4" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.15">
@@ -3415,7 +3415,7 @@
         <v>88</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>13</v>
@@ -3448,37 +3448,37 @@
         <v>46</v>
       </c>
       <c r="O2" s="8" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="P2" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="R2" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="S2" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="T2" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="U2" s="8" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="V2" s="29" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="W2" s="31" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="X2" s="7" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="Y2" s="29" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="Z2" s="7" t="s">
         <v>24</v>
@@ -3510,7 +3510,7 @@
         <v>89</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="E3" s="10" t="s">
         <v>21</v>
@@ -3543,37 +3543,37 @@
         <v>54</v>
       </c>
       <c r="O3" s="11" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="P3" s="34" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="Q3" s="34" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="R3" s="34" t="s">
+        <v>213</v>
+      </c>
+      <c r="S3" s="34" t="s">
         <v>216</v>
       </c>
-      <c r="S3" s="34" t="s">
-        <v>219</v>
-      </c>
       <c r="T3" s="34" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="U3" s="34" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="V3" s="33" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="W3" s="32" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="X3" s="22" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="Y3" s="33" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="Z3" s="10" t="s">
         <v>22</v>
@@ -3591,7 +3591,7 @@
         <v>59</v>
       </c>
       <c r="AE3" s="35" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.15">
@@ -3614,10 +3614,10 @@
         <v>13010001</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="I4" s="13">
         <v>1</v>
@@ -3666,7 +3666,7 @@
         <v>611</v>
       </c>
       <c r="AE4" s="19" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.15">
@@ -3689,10 +3689,10 @@
         <v>13010001</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>229</v>
+        <v>275</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="I5" s="13">
         <v>1</v>
@@ -3751,7 +3751,7 @@
         <v>571</v>
       </c>
       <c r="AE5" s="19" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.15">
@@ -3774,10 +3774,10 @@
         <v>13010006</v>
       </c>
       <c r="G6" s="20" t="s">
-        <v>226</v>
+        <v>276</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="I6" s="13">
         <v>1</v>
@@ -3828,7 +3828,7 @@
         <v>432</v>
       </c>
       <c r="AE6" s="19" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.15">
@@ -3851,10 +3851,10 @@
         <v>13010006</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>233</v>
+        <v>277</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="I7" s="13">
         <v>1</v>
@@ -3879,7 +3879,7 @@
         <v>0.3</v>
       </c>
       <c r="U7" s="13">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="V7" s="13">
         <v>43000002</v>
@@ -3909,7 +3909,7 @@
         <v>351</v>
       </c>
       <c r="AE7" s="19" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.15">
@@ -3917,7 +3917,7 @@
         <v>13010005</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C8" s="13">
         <v>2</v>
@@ -3932,10 +3932,10 @@
         <v>13010006</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="I8" s="13">
         <v>1</v>
@@ -3957,12 +3957,8 @@
         <v>0.3</v>
       </c>
       <c r="T8" s="13"/>
-      <c r="U8" s="13">
-        <v>2</v>
-      </c>
-      <c r="V8" s="13">
-        <v>43000002</v>
-      </c>
+      <c r="U8" s="13"/>
+      <c r="V8" s="13"/>
       <c r="W8" s="13">
         <v>2</v>
       </c>
@@ -3988,7 +3984,7 @@
         <v>339</v>
       </c>
       <c r="AE8" s="19" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.15">
@@ -4051,7 +4047,7 @@
         <v>506</v>
       </c>
       <c r="AE9" s="19" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.15">
@@ -4074,10 +4070,10 @@
         <v>13010006</v>
       </c>
       <c r="G10" s="20" t="s">
-        <v>230</v>
+        <v>280</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="I10" s="13">
         <v>1</v>
@@ -4132,7 +4128,7 @@
         <v>440</v>
       </c>
       <c r="AE10" s="19" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.15">
@@ -4154,11 +4150,11 @@
       <c r="F11" s="13">
         <v>13010006</v>
       </c>
-      <c r="G11" s="13" t="s">
-        <v>131</v>
+      <c r="G11" s="20" t="s">
+        <v>278</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="I11" s="13">
         <v>1</v>
@@ -4211,7 +4207,7 @@
         <v>338</v>
       </c>
       <c r="AE11" s="19" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.15">
@@ -4233,11 +4229,11 @@
       <c r="F12" s="13">
         <v>13010006</v>
       </c>
-      <c r="G12" s="13" t="s">
-        <v>140</v>
+      <c r="G12" s="20" t="s">
+        <v>279</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="I12" s="13">
         <v>1</v>
@@ -4266,7 +4262,7 @@
         <v>0.3</v>
       </c>
       <c r="U12" s="13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V12" s="13">
         <v>43000002</v>
@@ -4296,7 +4292,7 @@
         <v>484</v>
       </c>
       <c r="AE12" s="19" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.15">
@@ -4319,10 +4315,10 @@
         <v>13010006</v>
       </c>
       <c r="G13" s="20" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="I13" s="15">
         <v>1</v>
@@ -4344,12 +4340,8 @@
         <v>0.7</v>
       </c>
       <c r="T13" s="15"/>
-      <c r="U13" s="13">
-        <v>3</v>
-      </c>
-      <c r="V13" s="13">
-        <v>43000002</v>
-      </c>
+      <c r="U13" s="13"/>
+      <c r="V13" s="13"/>
       <c r="W13" s="13">
         <v>2</v>
       </c>
@@ -4369,7 +4361,7 @@
       <c r="AC13" s="15"/>
       <c r="AD13" s="15"/>
       <c r="AE13" s="19" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.15">
@@ -4417,7 +4409,7 @@
         <v>2</v>
       </c>
       <c r="Z14" s="13" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="AA14" s="13" t="s">
         <v>44</v>
@@ -4432,7 +4424,7 @@
         <v>509</v>
       </c>
       <c r="AE14" s="19" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.15">
@@ -4458,7 +4450,7 @@
         <v>90</v>
       </c>
       <c r="H15" s="20" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="I15" s="13">
         <v>1</v>
@@ -4485,7 +4477,7 @@
         <v>0.5</v>
       </c>
       <c r="U15" s="13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V15" s="13">
         <v>43000002</v>
@@ -4515,7 +4507,7 @@
         <v>538</v>
       </c>
       <c r="AE15" s="19" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.15">
@@ -4538,10 +4530,10 @@
         <v>13010101</v>
       </c>
       <c r="G16" s="20" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="H16" s="20" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="I16" s="13">
         <v>1</v>
@@ -4564,7 +4556,7 @@
         <v>0.3</v>
       </c>
       <c r="U16" s="13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V16" s="13">
         <v>43000002</v>
@@ -4594,7 +4586,7 @@
         <v>655</v>
       </c>
       <c r="AE16" s="19" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.15">
@@ -4617,10 +4609,10 @@
         <v>13010101</v>
       </c>
       <c r="G17" s="20" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="I17" s="13">
         <v>1</v>
@@ -4675,7 +4667,7 @@
         <v>584</v>
       </c>
       <c r="AE17" s="19" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.15">
@@ -4698,10 +4690,10 @@
         <v>13010101</v>
       </c>
       <c r="G18" s="20" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="H18" s="20" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="I18" s="13">
         <v>1</v>
@@ -4726,7 +4718,7 @@
         <v>0.6</v>
       </c>
       <c r="U18" s="13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V18" s="13">
         <v>43000002</v>
@@ -4756,7 +4748,7 @@
         <v>444</v>
       </c>
       <c r="AE18" s="19" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.15">
@@ -4779,10 +4771,10 @@
         <v>13010016</v>
       </c>
       <c r="G19" s="20" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="I19" s="13">
         <v>1</v>
@@ -4809,7 +4801,7 @@
         <v>0.4</v>
       </c>
       <c r="U19" s="13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="V19" s="13">
         <v>43000002</v>
@@ -4839,7 +4831,7 @@
         <v>445</v>
       </c>
       <c r="AE19" s="19" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.15">
@@ -4847,7 +4839,7 @@
         <v>13010107</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C20" s="15">
         <v>2</v>
@@ -4862,10 +4854,10 @@
         <v>13010101</v>
       </c>
       <c r="G20" s="20" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="H20" s="20" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="I20" s="13">
         <v>1</v>
@@ -4894,7 +4886,7 @@
         <v>0.8</v>
       </c>
       <c r="U20" s="13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="V20" s="13">
         <v>43000002</v>
@@ -4909,13 +4901,13 @@
         <v>2</v>
       </c>
       <c r="Z20" s="13" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="AA20" s="13" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="AB20" s="13" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="AC20" s="16">
         <v>850</v>
@@ -4924,7 +4916,7 @@
         <v>589</v>
       </c>
       <c r="AE20" s="19" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.15">
@@ -4932,7 +4924,7 @@
         <v>13010108</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C21" s="15">
         <v>2</v>
@@ -4947,10 +4939,10 @@
         <v>13010101</v>
       </c>
       <c r="G21" s="20" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="H21" s="20" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="I21" s="13">
         <v>1</v>
@@ -4990,13 +4982,13 @@
         <v>3</v>
       </c>
       <c r="Z21" s="13" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="AA21" s="13" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="AB21" s="16" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="AC21" s="13">
         <v>682</v>
@@ -5005,7 +4997,7 @@
         <v>545</v>
       </c>
       <c r="AE21" s="19" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.15">
@@ -5013,7 +5005,7 @@
         <v>13010109</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C22" s="15">
         <v>2</v>
@@ -5028,10 +5020,10 @@
         <v>13010101</v>
       </c>
       <c r="G22" s="20" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="H22" s="16" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="I22" s="13">
         <v>1</v>
@@ -5056,7 +5048,7 @@
       </c>
       <c r="T22" s="15"/>
       <c r="U22" s="13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="V22" s="13">
         <v>43000002</v>
@@ -5071,13 +5063,13 @@
         <v>3</v>
       </c>
       <c r="Z22" s="13" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="AA22" s="20" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="AB22" s="16" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="AC22" s="16">
         <v>643</v>
@@ -5086,7 +5078,7 @@
         <v>455</v>
       </c>
       <c r="AE22" s="19" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.15">
@@ -5094,7 +5086,7 @@
         <v>13010110</v>
       </c>
       <c r="B23" s="27" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C23" s="15">
         <v>2</v>
@@ -5110,7 +5102,7 @@
       </c>
       <c r="G23" s="20"/>
       <c r="H23" s="16" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="I23" s="13">
         <v>1</v>
@@ -5137,7 +5129,7 @@
       </c>
       <c r="T23" s="15"/>
       <c r="U23" s="13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V23" s="13">
         <v>43000002</v>
@@ -5152,13 +5144,13 @@
         <v>3</v>
       </c>
       <c r="Z23" s="20" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="AA23" s="20" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="AB23" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="AC23" s="16">
         <v>720</v>
@@ -5167,7 +5159,7 @@
         <v>375</v>
       </c>
       <c r="AE23" s="19" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.15">
@@ -5175,7 +5167,7 @@
         <v>13010201</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C24" s="15">
         <v>1</v>
@@ -5215,13 +5207,13 @@
         <v>2</v>
       </c>
       <c r="Z24" s="13" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="AA24" s="13" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="AB24" s="16" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="AC24" s="13">
         <v>807</v>
@@ -5230,7 +5222,7 @@
         <v>720</v>
       </c>
       <c r="AE24" s="19" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.15">
@@ -5238,7 +5230,7 @@
         <v>13010202</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C25" s="15">
         <v>2</v>
@@ -5253,10 +5245,10 @@
         <v>13010201</v>
       </c>
       <c r="G25" s="15" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="H25" s="15" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="I25" s="13">
         <v>1</v>
@@ -5279,7 +5271,7 @@
         <v>0.3</v>
       </c>
       <c r="U25" s="13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V25" s="13">
         <v>43000002</v>
@@ -5294,13 +5286,13 @@
         <v>3</v>
       </c>
       <c r="Z25" s="13" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="AA25" s="13" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="AB25" s="15" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="AC25" s="15">
         <v>974</v>
@@ -5309,7 +5301,7 @@
         <v>594</v>
       </c>
       <c r="AE25" s="19" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.15">
@@ -5317,7 +5309,7 @@
         <v>13010203</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C26" s="15">
         <v>2</v>
@@ -5332,10 +5324,10 @@
         <v>13010201</v>
       </c>
       <c r="G26" s="15" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="H26" s="15" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="I26" s="13">
         <v>1</v>
@@ -5375,13 +5367,13 @@
         <v>3</v>
       </c>
       <c r="Z26" s="13" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="AA26" s="13" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="AB26" s="15" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="AC26" s="15">
         <v>1080</v>
@@ -5390,7 +5382,7 @@
         <v>720</v>
       </c>
       <c r="AE26" s="19" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.15">
@@ -5398,7 +5390,7 @@
         <v>13010204</v>
       </c>
       <c r="B27" s="24" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C27" s="15">
         <v>2</v>
@@ -5413,10 +5405,10 @@
         <v>13010201</v>
       </c>
       <c r="G27" s="15" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H27" s="15" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="I27" s="13">
         <v>1</v>
@@ -5441,7 +5433,7 @@
       </c>
       <c r="T27" s="15"/>
       <c r="U27" s="13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V27" s="13">
         <v>43000002</v>
@@ -5456,13 +5448,13 @@
         <v>3</v>
       </c>
       <c r="Z27" s="13" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="AA27" s="13" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="AB27" s="15" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="AC27" s="15">
         <v>1074</v>
@@ -5471,7 +5463,7 @@
         <v>630</v>
       </c>
       <c r="AE27" s="19" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.15">
@@ -5479,7 +5471,7 @@
         <v>13010205</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C28" s="15">
         <v>2</v>
@@ -5494,7 +5486,7 @@
         <v>13010201</v>
       </c>
       <c r="G28" s="15" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="H28" s="16"/>
       <c r="I28" s="13">
@@ -5518,7 +5510,7 @@
         <v>0.3</v>
       </c>
       <c r="U28" s="13">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="V28" s="13">
         <v>43000002</v>
@@ -5533,13 +5525,13 @@
         <v>2</v>
       </c>
       <c r="Z28" s="20" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="AA28" s="20" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="AB28" s="16" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="AC28" s="13">
         <v>717</v>
@@ -5548,7 +5540,7 @@
         <v>655</v>
       </c>
       <c r="AE28" s="19" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.15">
@@ -5556,7 +5548,7 @@
         <v>13010206</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C29" s="15">
         <v>2</v>
@@ -5572,7 +5564,7 @@
       </c>
       <c r="G29" s="16"/>
       <c r="H29" s="20" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="I29" s="13">
         <v>1</v>
@@ -5608,13 +5600,13 @@
         <v>2</v>
       </c>
       <c r="Z29" s="20" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="AA29" s="20" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="AB29" s="16" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="AC29" s="13">
         <v>637</v>
@@ -5623,7 +5615,7 @@
         <v>735</v>
       </c>
       <c r="AE29" s="19" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.15">
@@ -5631,7 +5623,7 @@
         <v>13010207</v>
       </c>
       <c r="B30" s="23" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C30" s="15">
         <v>2</v>
@@ -5647,7 +5639,7 @@
       </c>
       <c r="G30" s="15"/>
       <c r="H30" s="15" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="I30" s="13">
         <v>1</v>
@@ -5670,7 +5662,7 @@
         <v>0.4</v>
       </c>
       <c r="U30" s="13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V30" s="13">
         <v>43000002</v>
@@ -5685,13 +5677,13 @@
         <v>4</v>
       </c>
       <c r="Z30" s="13" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="AA30" s="13" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="AB30" s="13" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="AC30" s="13">
         <v>737</v>
@@ -5700,7 +5692,7 @@
         <v>785</v>
       </c>
       <c r="AE30" s="19" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.15">
@@ -5708,7 +5700,7 @@
         <v>13010208</v>
       </c>
       <c r="B31" s="24" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C31" s="15">
         <v>2</v>
@@ -5723,10 +5715,10 @@
         <v>13010201</v>
       </c>
       <c r="G31" s="15" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="H31" s="15" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="I31" s="13">
         <v>1</v>
@@ -5753,7 +5745,7 @@
         <v>0.5</v>
       </c>
       <c r="U31" s="13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="V31" s="13">
         <v>43000002</v>
@@ -5768,13 +5760,13 @@
         <v>2</v>
       </c>
       <c r="Z31" s="13" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="AA31" s="13" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="AB31" s="15" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="AC31" s="19">
         <v>894</v>
@@ -5783,7 +5775,7 @@
         <v>679</v>
       </c>
       <c r="AE31" s="19" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="32" spans="1:31" x14ac:dyDescent="0.15">
@@ -5791,7 +5783,7 @@
         <v>13010209</v>
       </c>
       <c r="B32" s="23" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C32" s="15">
         <v>2</v>
@@ -5807,7 +5799,7 @@
       </c>
       <c r="G32" s="20"/>
       <c r="H32" s="20" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="I32" s="13">
         <v>1</v>
@@ -5828,7 +5820,7 @@
       <c r="S32" s="15"/>
       <c r="T32" s="15"/>
       <c r="U32" s="13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V32" s="13">
         <v>43000002</v>
@@ -5843,13 +5835,13 @@
         <v>2</v>
       </c>
       <c r="Z32" s="20" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="AA32" s="20" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="AB32" s="16" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AC32" s="19">
         <v>984</v>
@@ -5858,7 +5850,7 @@
         <v>734</v>
       </c>
       <c r="AE32" s="19" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="33" spans="1:31" x14ac:dyDescent="0.15">
@@ -5881,10 +5873,10 @@
         <v>13010006</v>
       </c>
       <c r="G33" s="20" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="H33" s="13" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="I33" s="13">
         <v>1</v>
@@ -5939,7 +5931,7 @@
         <v>505</v>
       </c>
       <c r="AE33" s="19" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
     </row>
     <row r="34" spans="1:31" x14ac:dyDescent="0.15">
@@ -5961,11 +5953,11 @@
       <c r="F34" s="13">
         <v>13010006</v>
       </c>
-      <c r="G34" s="13" t="s">
-        <v>144</v>
+      <c r="G34" s="20" t="s">
+        <v>281</v>
       </c>
       <c r="H34" s="13" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="I34" s="13">
         <v>1</v>
@@ -5988,7 +5980,7 @@
         <v>0.3</v>
       </c>
       <c r="U34" s="13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V34" s="13">
         <v>43000002</v>
@@ -6018,7 +6010,7 @@
         <v>527</v>
       </c>
       <c r="AE34" s="19" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
     </row>
     <row r="35" spans="1:31" x14ac:dyDescent="0.15">
@@ -6041,10 +6033,10 @@
         <v>13010006</v>
       </c>
       <c r="G35" s="13" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H35" s="13" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="I35" s="13">
         <v>1</v>
@@ -6073,7 +6065,7 @@
         <v>0.8</v>
       </c>
       <c r="U35" s="13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="V35" s="13">
         <v>43000002</v>
@@ -6103,7 +6095,7 @@
         <v>373</v>
       </c>
       <c r="AE35" s="19" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
     </row>
     <row r="36" spans="1:31" x14ac:dyDescent="0.15">
@@ -6126,7 +6118,7 @@
         <v>13010002</v>
       </c>
       <c r="G36" s="20" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="H36" s="13"/>
       <c r="I36" s="13"/>
@@ -6164,13 +6156,13 @@
         <v>109</v>
       </c>
       <c r="AA36" s="13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AB36" s="13"/>
       <c r="AC36" s="13"/>
       <c r="AD36" s="13"/>
       <c r="AE36" s="19" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
     </row>
     <row r="37" spans="1:31" x14ac:dyDescent="0.15">
@@ -6227,13 +6219,13 @@
         <v>110</v>
       </c>
       <c r="AA37" s="13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AB37" s="13"/>
       <c r="AC37" s="13"/>
       <c r="AD37" s="13"/>
       <c r="AE37" s="19" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
     </row>
     <row r="38" spans="1:31" x14ac:dyDescent="0.15">
@@ -6256,10 +6248,10 @@
         <v>13010007</v>
       </c>
       <c r="G38" s="13" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H38" s="13" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="I38" s="13"/>
       <c r="J38" s="13"/>
@@ -6292,13 +6284,13 @@
         <v>115</v>
       </c>
       <c r="AA38" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AB38" s="13"/>
       <c r="AC38" s="13"/>
       <c r="AD38" s="13"/>
       <c r="AE38" s="19" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
     </row>
     <row r="39" spans="1:31" x14ac:dyDescent="0.15">
@@ -6353,13 +6345,13 @@
         <v>119</v>
       </c>
       <c r="AA39" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AB39" s="13"/>
       <c r="AC39" s="13"/>
       <c r="AD39" s="13"/>
       <c r="AE39" s="19" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
     </row>
     <row r="40" spans="1:31" x14ac:dyDescent="0.15">
@@ -6410,13 +6402,13 @@
         <v>116</v>
       </c>
       <c r="AA40" s="13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AB40" s="13"/>
       <c r="AC40" s="13"/>
       <c r="AD40" s="13"/>
       <c r="AE40" s="19" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
     </row>
     <row r="41" spans="1:31" x14ac:dyDescent="0.15">
@@ -6442,7 +6434,7 @@
         <v>130</v>
       </c>
       <c r="H41" s="13" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="I41" s="13"/>
       <c r="J41" s="13"/>
@@ -6477,13 +6469,13 @@
         <v>128</v>
       </c>
       <c r="AA41" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="AB41" s="13"/>
       <c r="AC41" s="13"/>
       <c r="AD41" s="13"/>
       <c r="AE41" s="19" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
     </row>
     <row r="42" spans="1:31" x14ac:dyDescent="0.15">
@@ -6506,10 +6498,10 @@
         <v>13010004</v>
       </c>
       <c r="G42" s="20" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="H42" s="13" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="I42" s="13"/>
       <c r="J42" s="13"/>
@@ -6544,13 +6536,13 @@
         <v>126</v>
       </c>
       <c r="AA42" s="13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AB42" s="13"/>
       <c r="AC42" s="13"/>
       <c r="AD42" s="13"/>
       <c r="AE42" s="19" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
     </row>
     <row r="43" spans="1:31" x14ac:dyDescent="0.15">
@@ -6573,7 +6565,7 @@
         <v>13010004</v>
       </c>
       <c r="G43" s="20" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="H43" s="13"/>
       <c r="I43" s="13"/>
@@ -6607,13 +6599,13 @@
         <v>127</v>
       </c>
       <c r="AA43" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AB43" s="13"/>
       <c r="AC43" s="13"/>
       <c r="AD43" s="13"/>
       <c r="AE43" s="19" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
     </row>
     <row r="44" spans="1:31" x14ac:dyDescent="0.15">
@@ -6621,7 +6613,7 @@
         <v>13020031</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C44" s="13">
         <v>3</v>
@@ -6661,16 +6653,16 @@
         <v>5</v>
       </c>
       <c r="Z44" s="13" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="AA44" s="15" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="AB44" s="15"/>
       <c r="AC44" s="15"/>
       <c r="AD44" s="15"/>
       <c r="AE44" s="19" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
     </row>
     <row r="45" spans="1:31" x14ac:dyDescent="0.15">
@@ -6678,7 +6670,7 @@
         <v>13020032</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C45" s="13">
         <v>3</v>
@@ -6718,16 +6710,16 @@
         <v>5</v>
       </c>
       <c r="Z45" s="13" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="AA45" s="15" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="AB45" s="15"/>
       <c r="AC45" s="15"/>
       <c r="AD45" s="15"/>
       <c r="AE45" s="19" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
     </row>
     <row r="46" spans="1:31" x14ac:dyDescent="0.15">
@@ -6735,7 +6727,7 @@
         <v>13020033</v>
       </c>
       <c r="B46" s="17" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C46" s="13">
         <v>3</v>
@@ -6775,16 +6767,16 @@
         <v>5</v>
       </c>
       <c r="Z46" s="13" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="AA46" s="15" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="AB46" s="19"/>
       <c r="AC46" s="19"/>
       <c r="AD46" s="19"/>
       <c r="AE46" s="19" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
     </row>
     <row r="47" spans="1:31" x14ac:dyDescent="0.15">
@@ -6792,7 +6784,7 @@
         <v>13020034</v>
       </c>
       <c r="B47" s="17" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C47" s="13">
         <v>3</v>
@@ -6832,16 +6824,16 @@
         <v>5</v>
       </c>
       <c r="Z47" s="13" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="AA47" s="15" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="AB47" s="19"/>
       <c r="AC47" s="19"/>
       <c r="AD47" s="19"/>
       <c r="AE47" s="19" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
     </row>
     <row r="48" spans="1:31" x14ac:dyDescent="0.15">
@@ -6849,7 +6841,7 @@
         <v>13020035</v>
       </c>
       <c r="B48" s="17" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C48" s="13">
         <v>3</v>
@@ -6889,32 +6881,32 @@
         <v>5</v>
       </c>
       <c r="Z48" s="13" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="AA48" s="15" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="AB48" s="19"/>
       <c r="AC48" s="19"/>
       <c r="AD48" s="19"/>
       <c r="AE48" s="19" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="I4:V48">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:H48">
-    <cfRule type="containsBlanks" dxfId="1" priority="5">
+    <cfRule type="containsBlanks" dxfId="34" priority="5">
       <formula>LEN(TRIM(G4))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
split the angel event
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Scene.xlsx
+++ b/ConfigData/Xlsx/Scene.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7D59F5AE-DFE3-485E-BB03-6FF8A0EB2F33}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="Scene" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="280">
   <si>
     <t>村外小屋</t>
   </si>
@@ -203,19 +202,11 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>QMerchant</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>QDoctor</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>QAngel</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>商人</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -1052,7 +1043,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1971,7 +1962,28 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="37">
+  <dxfs count="36">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2701,33 +2713,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2880,29 +2865,76 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2915,43 +2947,42 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A3:AE48" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32" tableBorderDxfId="31">
-  <autoFilter ref="A3:AE48" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState ref="A4:AD48">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AD48" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34" tableBorderDxfId="33">
+  <autoFilter ref="A3:AD48"/>
+  <sortState ref="A4:AC48">
     <sortCondition ref="A3:A48"/>
   </sortState>
-  <tableColumns count="31">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="30"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="29"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Type" dataDxfId="28"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="RegionId" dataDxfId="27"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Level" dataDxfId="26"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="ReviveScene" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Quest" dataDxfId="24"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="QuestRandom" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="QPortal" dataDxfId="22"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="QCardChange" dataDxfId="21"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="QPiece" dataDxfId="20"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="QMerchant" dataDxfId="19"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="QDoctor" dataDxfId="18"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="QAngel" dataDxfId="17"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="QRes" dataDxfId="16"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="QItemDrug" dataDxfId="15"/>
-    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="QItemFish" dataDxfId="14"/>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="QItemOre" dataDxfId="13"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="QItemMushroom" dataDxfId="12"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="QItemWood" dataDxfId="11"/>
-    <tableColumn id="32" xr3:uid="{A83B2B25-5C5C-426D-A301-0017A60CEB0A}" name="QEnemy" dataDxfId="10"/>
-    <tableColumn id="25" xr3:uid="{52509577-5139-4AB6-BDC1-0A628B9D6BD7}" name="EnemyIds" dataDxfId="9"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Temperature" dataDxfId="8"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="Humitity" dataDxfId="7"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="Altitude" dataDxfId="6"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Url" dataDxfId="5"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="TilePath" dataDxfId="4"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Icon" dataDxfId="3"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="IconX" dataDxfId="2"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="IconY" dataDxfId="1"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="BGM" dataDxfId="0"/>
+  <tableColumns count="30">
+    <tableColumn id="1" name="Id" dataDxfId="32"/>
+    <tableColumn id="2" name="Name" dataDxfId="31"/>
+    <tableColumn id="18" name="Type" dataDxfId="30"/>
+    <tableColumn id="11" name="RegionId" dataDxfId="29"/>
+    <tableColumn id="3" name="Level" dataDxfId="28"/>
+    <tableColumn id="20" name="ReviveScene" dataDxfId="27"/>
+    <tableColumn id="4" name="Quest" dataDxfId="26"/>
+    <tableColumn id="17" name="QuestRandom" dataDxfId="25"/>
+    <tableColumn id="5" name="QPortal" dataDxfId="24"/>
+    <tableColumn id="6" name="QCardChange" dataDxfId="23"/>
+    <tableColumn id="7" name="QPiece" dataDxfId="22"/>
+    <tableColumn id="9" name="QDoctor" dataDxfId="21"/>
+    <tableColumn id="10" name="QAngel" dataDxfId="20"/>
+    <tableColumn id="22" name="QRes" dataDxfId="19"/>
+    <tableColumn id="27" name="QItemDrug" dataDxfId="18"/>
+    <tableColumn id="31" name="QItemFish" dataDxfId="17"/>
+    <tableColumn id="30" name="QItemOre" dataDxfId="16"/>
+    <tableColumn id="28" name="QItemMushroom" dataDxfId="15"/>
+    <tableColumn id="29" name="QItemWood" dataDxfId="14"/>
+    <tableColumn id="32" name="QEnemy" dataDxfId="13"/>
+    <tableColumn id="25" name="EnemyIds" dataDxfId="12"/>
+    <tableColumn id="19" name="Temperature" dataDxfId="11"/>
+    <tableColumn id="23" name="Humitity" dataDxfId="10"/>
+    <tableColumn id="26" name="Altitude" dataDxfId="9"/>
+    <tableColumn id="12" name="Url" dataDxfId="8"/>
+    <tableColumn id="13" name="TilePath" dataDxfId="7"/>
+    <tableColumn id="14" name="Icon" dataDxfId="6"/>
+    <tableColumn id="15" name="IconX" dataDxfId="5"/>
+    <tableColumn id="16" name="IconY" dataDxfId="4"/>
+    <tableColumn id="24" name="BGM" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2965,7 +2996,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="C7EDCC"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -3277,11 +3308,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE48"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AD48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3294,22 +3325,22 @@
     <col min="6" max="6" width="9" style="5" customWidth="1"/>
     <col min="7" max="7" width="52.875" style="5" customWidth="1"/>
     <col min="8" max="8" width="23.625" style="5" customWidth="1"/>
-    <col min="9" max="15" width="3.125" style="5" customWidth="1"/>
-    <col min="16" max="17" width="3.75" style="5" customWidth="1"/>
-    <col min="18" max="18" width="3.75" customWidth="1"/>
-    <col min="19" max="19" width="3.75" style="5" customWidth="1"/>
-    <col min="20" max="21" width="3.75" customWidth="1"/>
-    <col min="22" max="22" width="12.75" style="5" customWidth="1"/>
-    <col min="23" max="23" width="3.625" customWidth="1"/>
-    <col min="24" max="25" width="3.625" style="5" customWidth="1"/>
-    <col min="26" max="28" width="7.75" style="5" customWidth="1"/>
-    <col min="29" max="30" width="5.375" style="5" customWidth="1"/>
-    <col min="31" max="31" width="9.625" style="5" customWidth="1"/>
-    <col min="32" max="33" width="6" style="5" customWidth="1"/>
-    <col min="34" max="16384" width="9" style="5"/>
+    <col min="9" max="14" width="3.125" style="5" customWidth="1"/>
+    <col min="15" max="16" width="3.75" style="5" customWidth="1"/>
+    <col min="17" max="17" width="3.75" customWidth="1"/>
+    <col min="18" max="18" width="3.75" style="5" customWidth="1"/>
+    <col min="19" max="20" width="3.75" customWidth="1"/>
+    <col min="21" max="21" width="12.75" style="5" customWidth="1"/>
+    <col min="22" max="22" width="3.625" customWidth="1"/>
+    <col min="23" max="24" width="3.625" style="5" customWidth="1"/>
+    <col min="25" max="27" width="7.75" style="5" customWidth="1"/>
+    <col min="28" max="29" width="5.375" style="5" customWidth="1"/>
+    <col min="30" max="30" width="9.625" style="5" customWidth="1"/>
+    <col min="31" max="32" width="6" style="5" customWidth="1"/>
+    <col min="33" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="60" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:30" ht="60" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -3317,25 +3348,25 @@
         <v>16</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>17</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>28</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>49</v>
@@ -3344,67 +3375,64 @@
         <v>50</v>
       </c>
       <c r="L1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="M1" s="3" t="s">
-        <v>56</v>
-      </c>
       <c r="N1" s="3" t="s">
-        <v>57</v>
+        <v>152</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>154</v>
+        <v>216</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="Q1" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="R1" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="R1" s="3" t="s">
-        <v>216</v>
-      </c>
       <c r="S1" s="3" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="V1" s="28" t="s">
-        <v>268</v>
-      </c>
-      <c r="W1" s="30" t="s">
-        <v>203</v>
-      </c>
-      <c r="X1" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="U1" s="28" t="s">
+        <v>266</v>
+      </c>
+      <c r="V1" s="30" t="s">
+        <v>201</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="X1" s="28" t="s">
         <v>206</v>
       </c>
-      <c r="Y1" s="28" t="s">
-        <v>208</v>
+      <c r="Y1" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="Z1" s="2" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="AA1" s="2" t="s">
-        <v>25</v>
+        <v>80</v>
       </c>
       <c r="AB1" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
+      </c>
+      <c r="AC1" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="AD1" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="AE1" s="4" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
         <v>13</v>
       </c>
@@ -3412,22 +3440,22 @@
         <v>14</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G2" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="H2" s="7" t="s">
         <v>83</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>85</v>
       </c>
       <c r="I2" s="8" t="s">
         <v>46</v>
@@ -3445,61 +3473,58 @@
         <v>46</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>46</v>
+        <v>153</v>
       </c>
       <c r="O2" s="8" t="s">
-        <v>155</v>
+        <v>227</v>
       </c>
       <c r="P2" s="8" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="R2" s="8" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="S2" s="8" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="T2" s="8" t="s">
-        <v>229</v>
-      </c>
-      <c r="U2" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="V2" s="29" t="s">
-        <v>267</v>
-      </c>
-      <c r="W2" s="31" t="s">
-        <v>204</v>
-      </c>
-      <c r="X2" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="Y2" s="29" t="s">
-        <v>204</v>
+        <v>268</v>
+      </c>
+      <c r="U2" s="29" t="s">
+        <v>265</v>
+      </c>
+      <c r="V2" s="31" t="s">
+        <v>202</v>
+      </c>
+      <c r="W2" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="X2" s="29" t="s">
+        <v>202</v>
+      </c>
+      <c r="Y2" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="Z2" s="7" t="s">
         <v>24</v>
       </c>
       <c r="AA2" s="7" t="s">
-        <v>24</v>
+        <v>59</v>
       </c>
       <c r="AB2" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="AC2" s="7" t="s">
         <v>13</v>
       </c>
+      <c r="AC2" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="AD2" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="AE2" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A3" s="10" t="s">
         <v>19</v>
       </c>
@@ -3507,22 +3532,22 @@
         <v>20</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E3" s="10" t="s">
         <v>21</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G3" s="10" t="s">
         <v>27</v>
       </c>
       <c r="H3" s="22" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I3" s="11" t="s">
         <v>47</v>
@@ -3540,61 +3565,58 @@
         <v>53</v>
       </c>
       <c r="N3" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="O3" s="11" t="s">
-        <v>156</v>
+        <v>154</v>
+      </c>
+      <c r="O3" s="34" t="s">
+        <v>211</v>
       </c>
       <c r="P3" s="34" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="Q3" s="34" t="s">
+        <v>209</v>
+      </c>
+      <c r="R3" s="34" t="s">
         <v>212</v>
       </c>
-      <c r="R3" s="34" t="s">
-        <v>211</v>
-      </c>
       <c r="S3" s="34" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="T3" s="34" t="s">
-        <v>210</v>
-      </c>
-      <c r="U3" s="34" t="s">
-        <v>271</v>
-      </c>
-      <c r="V3" s="33" t="s">
-        <v>272</v>
-      </c>
-      <c r="W3" s="32" t="s">
+        <v>269</v>
+      </c>
+      <c r="U3" s="33" t="s">
+        <v>270</v>
+      </c>
+      <c r="V3" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="W3" s="22" t="s">
         <v>205</v>
       </c>
-      <c r="X3" s="22" t="s">
+      <c r="X3" s="33" t="s">
         <v>207</v>
       </c>
-      <c r="Y3" s="33" t="s">
-        <v>209</v>
+      <c r="Y3" s="10" t="s">
+        <v>22</v>
       </c>
       <c r="Z3" s="10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="AA3" s="10" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="AB3" s="10" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="AC3" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="AD3" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="AE3" s="35" t="s">
-        <v>235</v>
+        <v>57</v>
+      </c>
+      <c r="AD3" s="35" t="s">
+        <v>233</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A4" s="12">
         <v>13010001</v>
       </c>
@@ -3614,10 +3636,10 @@
         <v>13010001</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I4" s="13">
         <v>1</v>
@@ -3627,49 +3649,48 @@
       <c r="L4" s="13"/>
       <c r="M4" s="13"/>
       <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13">
+      <c r="O4" s="13">
         <v>0.3</v>
       </c>
+      <c r="P4" s="13"/>
       <c r="Q4" s="13"/>
-      <c r="R4" s="13"/>
+      <c r="R4" s="13">
+        <v>0.5</v>
+      </c>
       <c r="S4" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="T4" s="13">
         <v>0.7</v>
       </c>
+      <c r="T4" s="13"/>
       <c r="U4" s="13"/>
-      <c r="V4" s="13"/>
+      <c r="V4" s="13">
+        <v>3</v>
+      </c>
       <c r="W4" s="13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="X4" s="13">
         <v>2</v>
       </c>
-      <c r="Y4" s="13">
-        <v>2</v>
+      <c r="Y4" s="13" t="s">
+        <v>91</v>
       </c>
       <c r="Z4" s="13" t="s">
-        <v>93</v>
+        <v>26</v>
       </c>
       <c r="AA4" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB4" s="13" t="s">
-        <v>62</v>
+        <v>60</v>
+      </c>
+      <c r="AB4" s="13">
+        <v>1348</v>
       </c>
       <c r="AC4" s="13">
-        <v>1348</v>
-      </c>
-      <c r="AD4" s="13">
         <v>611</v>
       </c>
-      <c r="AE4" s="19" t="s">
-        <v>237</v>
+      <c r="AD4" s="19" t="s">
+        <v>235</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A5" s="12">
         <v>13010002</v>
       </c>
@@ -3689,10 +3710,10 @@
         <v>13010001</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="I5" s="13">
         <v>1</v>
@@ -3701,60 +3722,59 @@
       <c r="K5" s="13">
         <v>1</v>
       </c>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13">
-        <v>1</v>
-      </c>
+      <c r="L5" s="13">
+        <v>1</v>
+      </c>
+      <c r="M5" s="13"/>
       <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
+      <c r="O5" s="13">
+        <v>0.3</v>
+      </c>
       <c r="P5" s="13">
+        <v>0.7</v>
+      </c>
+      <c r="Q5" s="13"/>
+      <c r="R5" s="13">
         <v>0.3</v>
       </c>
-      <c r="Q5" s="13">
+      <c r="S5" s="13">
         <v>0.7</v>
       </c>
-      <c r="R5" s="13"/>
-      <c r="S5" s="13">
-        <v>0.3</v>
-      </c>
       <c r="T5" s="13">
-        <v>0.7</v>
+        <v>4</v>
       </c>
       <c r="U5" s="13">
-        <v>4</v>
+        <v>43000002</v>
       </c>
       <c r="V5" s="13">
-        <v>43000002</v>
+        <v>2</v>
       </c>
       <c r="W5" s="13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="X5" s="13">
-        <v>3</v>
-      </c>
-      <c r="Y5" s="13">
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="Y5" s="13" t="s">
+        <v>29</v>
       </c>
       <c r="Z5" s="13" t="s">
         <v>29</v>
       </c>
       <c r="AA5" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="AB5" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
+      </c>
+      <c r="AB5" s="13">
+        <v>1279</v>
       </c>
       <c r="AC5" s="13">
-        <v>1279</v>
-      </c>
-      <c r="AD5" s="13">
         <v>571</v>
       </c>
-      <c r="AE5" s="19" t="s">
-        <v>236</v>
+      <c r="AD5" s="19" t="s">
+        <v>234</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A6" s="12">
         <v>13010003</v>
       </c>
@@ -3774,10 +3794,10 @@
         <v>13010006</v>
       </c>
       <c r="G6" s="20" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="I6" s="13">
         <v>1</v>
@@ -3787,51 +3807,50 @@
       <c r="L6" s="13"/>
       <c r="M6" s="13"/>
       <c r="N6" s="13"/>
-      <c r="O6" s="13"/>
+      <c r="O6" s="13">
+        <v>0.3</v>
+      </c>
       <c r="P6" s="13">
         <v>0.3</v>
       </c>
-      <c r="Q6" s="13">
-        <v>0.3</v>
-      </c>
+      <c r="Q6" s="13"/>
       <c r="R6" s="13"/>
       <c r="S6" s="13"/>
-      <c r="T6" s="13"/>
+      <c r="T6" s="13">
+        <v>3</v>
+      </c>
       <c r="U6" s="13">
-        <v>3</v>
+        <v>43000002</v>
       </c>
       <c r="V6" s="13">
-        <v>43000002</v>
+        <v>3</v>
       </c>
       <c r="W6" s="13">
         <v>3</v>
       </c>
       <c r="X6" s="13">
-        <v>3</v>
-      </c>
-      <c r="Y6" s="13">
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="Y6" s="13" t="s">
+        <v>101</v>
       </c>
       <c r="Z6" s="13" t="s">
-        <v>103</v>
+        <v>31</v>
       </c>
       <c r="AA6" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB6" s="13" t="s">
-        <v>73</v>
+        <v>71</v>
+      </c>
+      <c r="AB6" s="13">
+        <v>1251</v>
       </c>
       <c r="AC6" s="13">
-        <v>1251</v>
-      </c>
-      <c r="AD6" s="13">
         <v>432</v>
       </c>
-      <c r="AE6" s="19" t="s">
-        <v>264</v>
+      <c r="AD6" s="19" t="s">
+        <v>262</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A7" s="12">
         <v>13010004</v>
       </c>
@@ -3851,73 +3870,70 @@
         <v>13010006</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="I7" s="13">
         <v>1</v>
       </c>
       <c r="J7" s="13"/>
       <c r="K7" s="13"/>
-      <c r="L7" s="13">
-        <v>1</v>
-      </c>
+      <c r="L7" s="13"/>
       <c r="M7" s="13"/>
       <c r="N7" s="13"/>
       <c r="O7" s="13"/>
       <c r="P7" s="13"/>
-      <c r="Q7" s="13"/>
+      <c r="Q7" s="13">
+        <v>0.7</v>
+      </c>
       <c r="R7" s="13">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="S7" s="13">
         <v>0.3</v>
       </c>
       <c r="T7" s="13">
-        <v>0.3</v>
+        <v>4</v>
       </c>
       <c r="U7" s="13">
-        <v>4</v>
+        <v>43000002</v>
       </c>
       <c r="V7" s="13">
-        <v>43000002</v>
+        <v>3</v>
       </c>
       <c r="W7" s="13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="X7" s="13">
-        <v>2</v>
-      </c>
-      <c r="Y7" s="13">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="Y7" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="Z7" s="13" t="s">
         <v>33</v>
       </c>
       <c r="AA7" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB7" s="13" t="s">
-        <v>65</v>
+        <v>63</v>
+      </c>
+      <c r="AB7" s="13">
+        <v>1148</v>
       </c>
       <c r="AC7" s="13">
-        <v>1148</v>
-      </c>
-      <c r="AD7" s="13">
         <v>351</v>
       </c>
-      <c r="AE7" s="19" t="s">
-        <v>236</v>
+      <c r="AD7" s="19" t="s">
+        <v>234</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A8" s="12">
         <v>13010005</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C8" s="13">
         <v>2</v>
@@ -3932,10 +3948,10 @@
         <v>13010006</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="I8" s="13">
         <v>1</v>
@@ -3949,45 +3965,44 @@
       <c r="N8" s="13"/>
       <c r="O8" s="13"/>
       <c r="P8" s="13"/>
-      <c r="Q8" s="13"/>
+      <c r="Q8" s="13">
+        <v>0.3</v>
+      </c>
       <c r="R8" s="13">
         <v>0.3</v>
       </c>
-      <c r="S8" s="13">
-        <v>0.3</v>
-      </c>
+      <c r="S8" s="13"/>
       <c r="T8" s="13"/>
       <c r="U8" s="13"/>
-      <c r="V8" s="13"/>
+      <c r="V8" s="13">
+        <v>2</v>
+      </c>
       <c r="W8" s="13">
         <v>2</v>
       </c>
       <c r="X8" s="13">
-        <v>2</v>
-      </c>
-      <c r="Y8" s="13">
         <v>5</v>
       </c>
+      <c r="Y8" s="13" t="s">
+        <v>93</v>
+      </c>
       <c r="Z8" s="13" t="s">
-        <v>95</v>
+        <v>34</v>
       </c>
       <c r="AA8" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="AB8" s="13" t="s">
-        <v>66</v>
+        <v>64</v>
+      </c>
+      <c r="AB8" s="13">
+        <v>1386</v>
       </c>
       <c r="AC8" s="13">
-        <v>1386</v>
-      </c>
-      <c r="AD8" s="13">
         <v>339</v>
       </c>
-      <c r="AE8" s="19" t="s">
-        <v>236</v>
+      <c r="AD8" s="19" t="s">
+        <v>234</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A9" s="12">
         <v>13010006</v>
       </c>
@@ -4021,36 +4036,35 @@
       <c r="S9" s="13"/>
       <c r="T9" s="13"/>
       <c r="U9" s="13"/>
-      <c r="V9" s="13"/>
+      <c r="V9" s="13">
+        <v>3</v>
+      </c>
       <c r="W9" s="13">
         <v>3</v>
       </c>
       <c r="X9" s="13">
-        <v>3</v>
-      </c>
-      <c r="Y9" s="13">
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="Y9" s="13" t="s">
+        <v>94</v>
       </c>
       <c r="Z9" s="13" t="s">
-        <v>96</v>
+        <v>30</v>
       </c>
       <c r="AA9" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="AB9" s="13" t="s">
-        <v>67</v>
+        <v>65</v>
+      </c>
+      <c r="AB9" s="13">
+        <v>1232</v>
       </c>
       <c r="AC9" s="13">
-        <v>1232</v>
-      </c>
-      <c r="AD9" s="13">
         <v>506</v>
       </c>
-      <c r="AE9" s="19" t="s">
-        <v>237</v>
+      <c r="AD9" s="19" t="s">
+        <v>235</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A10" s="12">
         <v>13010007</v>
       </c>
@@ -4070,68 +4084,67 @@
         <v>13010006</v>
       </c>
       <c r="G10" s="20" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="I10" s="13">
         <v>1</v>
       </c>
       <c r="J10" s="13"/>
       <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13">
-        <v>1</v>
-      </c>
-      <c r="N10" s="13"/>
-      <c r="O10" s="13">
-        <v>1</v>
-      </c>
-      <c r="P10" s="13"/>
+      <c r="L10" s="13">
+        <v>1</v>
+      </c>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13">
+        <v>1</v>
+      </c>
+      <c r="O10" s="13"/>
+      <c r="P10" s="13">
+        <v>0.7</v>
+      </c>
       <c r="Q10" s="13">
-        <v>0.7</v>
-      </c>
-      <c r="R10" s="13">
         <v>0.2</v>
       </c>
+      <c r="R10" s="13"/>
       <c r="S10" s="13"/>
-      <c r="T10" s="13"/>
+      <c r="T10" s="13">
+        <v>3</v>
+      </c>
       <c r="U10" s="13">
-        <v>3</v>
+        <v>43000002</v>
       </c>
       <c r="V10" s="13">
-        <v>43000002</v>
+        <v>2</v>
       </c>
       <c r="W10" s="13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="X10" s="13">
-        <v>4</v>
-      </c>
-      <c r="Y10" s="13">
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="Y10" s="13" t="s">
+        <v>95</v>
       </c>
       <c r="Z10" s="13" t="s">
-        <v>97</v>
+        <v>32</v>
       </c>
       <c r="AA10" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB10" s="13" t="s">
-        <v>68</v>
+        <v>66</v>
+      </c>
+      <c r="AB10" s="13">
+        <v>1431</v>
       </c>
       <c r="AC10" s="13">
-        <v>1431</v>
-      </c>
-      <c r="AD10" s="13">
         <v>440</v>
       </c>
-      <c r="AE10" s="19" t="s">
-        <v>236</v>
+      <c r="AD10" s="19" t="s">
+        <v>234</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A11" s="12">
         <v>13010008</v>
       </c>
@@ -4151,10 +4164,10 @@
         <v>13010006</v>
       </c>
       <c r="G11" s="20" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="I11" s="13">
         <v>1</v>
@@ -4166,51 +4179,50 @@
       <c r="N11" s="13"/>
       <c r="O11" s="13"/>
       <c r="P11" s="13"/>
-      <c r="Q11" s="13"/>
+      <c r="Q11" s="13">
+        <v>0.4</v>
+      </c>
       <c r="R11" s="13">
+        <v>0.3</v>
+      </c>
+      <c r="S11" s="13">
         <v>0.4</v>
       </c>
-      <c r="S11" s="13">
-        <v>0.3</v>
-      </c>
       <c r="T11" s="13">
-        <v>0.4</v>
+        <v>3</v>
       </c>
       <c r="U11" s="13">
-        <v>3</v>
+        <v>43000002</v>
       </c>
       <c r="V11" s="13">
-        <v>43000002</v>
+        <v>1</v>
       </c>
       <c r="W11" s="13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="X11" s="13">
-        <v>3</v>
-      </c>
-      <c r="Y11" s="13">
         <v>5</v>
       </c>
+      <c r="Y11" s="13" t="s">
+        <v>102</v>
+      </c>
       <c r="Z11" s="13" t="s">
-        <v>104</v>
+        <v>35</v>
       </c>
       <c r="AA11" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB11" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
+      </c>
+      <c r="AB11" s="13">
+        <v>1250</v>
       </c>
       <c r="AC11" s="13">
-        <v>1250</v>
-      </c>
-      <c r="AD11" s="13">
         <v>338</v>
       </c>
-      <c r="AE11" s="19" t="s">
-        <v>266</v>
+      <c r="AD11" s="19" t="s">
+        <v>264</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A12" s="12">
         <v>13010009</v>
       </c>
@@ -4230,10 +4242,10 @@
         <v>13010006</v>
       </c>
       <c r="G12" s="20" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="I12" s="13">
         <v>1</v>
@@ -4242,16 +4254,16 @@
         <v>1</v>
       </c>
       <c r="K12" s="13"/>
-      <c r="L12" s="13">
-        <v>1</v>
-      </c>
+      <c r="L12" s="13"/>
       <c r="M12" s="13"/>
       <c r="N12" s="13"/>
-      <c r="O12" s="13"/>
-      <c r="P12" s="13">
+      <c r="O12" s="13">
         <v>0.3</v>
       </c>
-      <c r="Q12" s="13"/>
+      <c r="P12" s="13"/>
+      <c r="Q12" s="13">
+        <v>0.3</v>
+      </c>
       <c r="R12" s="13">
         <v>0.3</v>
       </c>
@@ -4259,48 +4271,45 @@
         <v>0.3</v>
       </c>
       <c r="T12" s="13">
-        <v>0.3</v>
+        <v>3</v>
       </c>
       <c r="U12" s="13">
-        <v>3</v>
+        <v>43000002</v>
       </c>
       <c r="V12" s="13">
-        <v>43000002</v>
+        <v>3</v>
       </c>
       <c r="W12" s="13">
         <v>3</v>
       </c>
       <c r="X12" s="13">
-        <v>3</v>
-      </c>
-      <c r="Y12" s="13">
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="Y12" s="13" t="s">
+        <v>98</v>
       </c>
       <c r="Z12" s="13" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="AA12" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="AB12" s="13" t="s">
-        <v>70</v>
+        <v>68</v>
+      </c>
+      <c r="AB12" s="13">
+        <v>1332</v>
       </c>
       <c r="AC12" s="13">
-        <v>1332</v>
-      </c>
-      <c r="AD12" s="13">
         <v>484</v>
       </c>
-      <c r="AE12" s="19" t="s">
-        <v>236</v>
+      <c r="AD12" s="19" t="s">
+        <v>234</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A13" s="12">
         <v>13010010</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C13" s="15">
         <v>2</v>
@@ -4315,10 +4324,10 @@
         <v>13010006</v>
       </c>
       <c r="G13" s="20" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="I13" s="15">
         <v>1</v>
@@ -4329,42 +4338,41 @@
       <c r="M13" s="15"/>
       <c r="N13" s="15"/>
       <c r="O13" s="15"/>
-      <c r="P13" s="15"/>
+      <c r="P13" s="15">
+        <v>0.6</v>
+      </c>
       <c r="Q13" s="15">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="R13" s="15">
         <v>0.7</v>
       </c>
-      <c r="S13" s="15">
-        <v>0.7</v>
-      </c>
-      <c r="T13" s="15"/>
+      <c r="S13" s="15"/>
+      <c r="T13" s="13"/>
       <c r="U13" s="13"/>
-      <c r="V13" s="13"/>
+      <c r="V13" s="13">
+        <v>2</v>
+      </c>
       <c r="W13" s="13">
         <v>2</v>
       </c>
       <c r="X13" s="13">
-        <v>2</v>
-      </c>
-      <c r="Y13" s="13">
-        <v>3</v>
+        <v>3</v>
+      </c>
+      <c r="Y13" s="15" t="s">
+        <v>119</v>
       </c>
       <c r="Z13" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="AA13" s="15" t="s">
-        <v>121</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="AA13" s="15"/>
       <c r="AB13" s="15"/>
       <c r="AC13" s="15"/>
-      <c r="AD13" s="15"/>
-      <c r="AE13" s="19" t="s">
-        <v>236</v>
+      <c r="AD13" s="19" t="s">
+        <v>234</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A14" s="25">
         <v>13010101</v>
       </c>
@@ -4398,36 +4406,35 @@
       <c r="S14" s="13"/>
       <c r="T14" s="13"/>
       <c r="U14" s="13"/>
-      <c r="V14" s="13"/>
+      <c r="V14" s="13">
+        <v>2</v>
+      </c>
       <c r="W14" s="13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="X14" s="13">
-        <v>3</v>
-      </c>
-      <c r="Y14" s="13">
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="Y14" s="13" t="s">
+        <v>155</v>
       </c>
       <c r="Z14" s="13" t="s">
-        <v>157</v>
+        <v>44</v>
       </c>
       <c r="AA14" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB14" s="13" t="s">
-        <v>77</v>
+        <v>75</v>
+      </c>
+      <c r="AB14" s="13">
+        <v>894</v>
       </c>
       <c r="AC14" s="13">
-        <v>894</v>
-      </c>
-      <c r="AD14" s="13">
         <v>509</v>
       </c>
-      <c r="AE14" s="19" t="s">
-        <v>265</v>
+      <c r="AD14" s="19" t="s">
+        <v>263</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A15" s="25">
         <v>13010102</v>
       </c>
@@ -4447,70 +4454,67 @@
         <v>13010101</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H15" s="20" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="I15" s="13">
         <v>1</v>
       </c>
       <c r="J15" s="13"/>
       <c r="K15" s="13"/>
-      <c r="L15" s="13">
-        <v>1</v>
-      </c>
+      <c r="L15" s="13"/>
       <c r="M15" s="13"/>
       <c r="N15" s="13"/>
-      <c r="O15" s="13"/>
+      <c r="O15" s="13">
+        <v>0.5</v>
+      </c>
       <c r="P15" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="Q15" s="13"/>
+      <c r="R15" s="13">
+        <v>0.7</v>
+      </c>
+      <c r="S15" s="13">
         <v>0.5</v>
       </c>
-      <c r="Q15" s="13">
-        <v>0.2</v>
-      </c>
-      <c r="R15" s="13"/>
-      <c r="S15" s="13">
-        <v>0.7</v>
-      </c>
       <c r="T15" s="13">
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="U15" s="13">
-        <v>3</v>
+        <v>43000002</v>
       </c>
       <c r="V15" s="13">
-        <v>43000002</v>
+        <v>2</v>
       </c>
       <c r="W15" s="13">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="X15" s="13">
-        <v>5</v>
-      </c>
-      <c r="Y15" s="13">
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="Y15" s="13" t="s">
+        <v>104</v>
       </c>
       <c r="Z15" s="13" t="s">
-        <v>106</v>
+        <v>41</v>
       </c>
       <c r="AA15" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB15" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
+      </c>
+      <c r="AB15" s="13">
+        <v>1040</v>
       </c>
       <c r="AC15" s="13">
-        <v>1040</v>
-      </c>
-      <c r="AD15" s="13">
         <v>538</v>
       </c>
-      <c r="AE15" s="19" t="s">
-        <v>265</v>
+      <c r="AD15" s="19" t="s">
+        <v>263</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A16" s="25">
         <v>13010103</v>
       </c>
@@ -4530,10 +4534,10 @@
         <v>13010101</v>
       </c>
       <c r="G16" s="20" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="H16" s="20" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="I16" s="13">
         <v>1</v>
@@ -4543,53 +4547,52 @@
       <c r="L16" s="13"/>
       <c r="M16" s="13"/>
       <c r="N16" s="13"/>
-      <c r="O16" s="13"/>
-      <c r="P16" s="13">
+      <c r="O16" s="13">
         <v>0.3</v>
       </c>
-      <c r="Q16" s="13"/>
-      <c r="R16" s="13">
+      <c r="P16" s="13"/>
+      <c r="Q16" s="13">
         <v>0.8</v>
       </c>
-      <c r="S16" s="13"/>
+      <c r="R16" s="13"/>
+      <c r="S16" s="13">
+        <v>0.3</v>
+      </c>
       <c r="T16" s="13">
-        <v>0.3</v>
+        <v>3</v>
       </c>
       <c r="U16" s="13">
-        <v>3</v>
+        <v>43000002</v>
       </c>
       <c r="V16" s="13">
-        <v>43000002</v>
+        <v>3</v>
       </c>
       <c r="W16" s="13">
         <v>3</v>
       </c>
       <c r="X16" s="13">
-        <v>3</v>
-      </c>
-      <c r="Y16" s="13">
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="Y16" s="13" t="s">
+        <v>92</v>
       </c>
       <c r="Z16" s="13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="AA16" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="AB16" s="13" t="s">
-        <v>64</v>
+        <v>62</v>
+      </c>
+      <c r="AB16" s="13">
+        <v>1213</v>
       </c>
       <c r="AC16" s="13">
-        <v>1213</v>
-      </c>
-      <c r="AD16" s="13">
         <v>655</v>
       </c>
-      <c r="AE16" s="19" t="s">
-        <v>264</v>
+      <c r="AD16" s="19" t="s">
+        <v>262</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A17" s="25">
         <v>13010104</v>
       </c>
@@ -4609,68 +4612,67 @@
         <v>13010101</v>
       </c>
       <c r="G17" s="20" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="I17" s="13">
         <v>1</v>
       </c>
       <c r="J17" s="13"/>
       <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13">
-        <v>1</v>
-      </c>
+      <c r="L17" s="13">
+        <v>1</v>
+      </c>
+      <c r="M17" s="13"/>
       <c r="N17" s="13"/>
       <c r="O17" s="13"/>
-      <c r="P17" s="13"/>
+      <c r="P17" s="13">
+        <v>0.7</v>
+      </c>
       <c r="Q17" s="13">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="R17" s="13">
-        <v>0.3</v>
-      </c>
-      <c r="S17" s="13">
         <v>0.5</v>
       </c>
-      <c r="T17" s="13"/>
+      <c r="S17" s="13"/>
+      <c r="T17" s="13">
+        <v>2</v>
+      </c>
       <c r="U17" s="13">
-        <v>2</v>
+        <v>43000002</v>
       </c>
       <c r="V17" s="13">
-        <v>43000002</v>
+        <v>2</v>
       </c>
       <c r="W17" s="13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="X17" s="13">
-        <v>4</v>
-      </c>
-      <c r="Y17" s="13">
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="Y17" s="13" t="s">
+        <v>105</v>
       </c>
       <c r="Z17" s="13" t="s">
-        <v>107</v>
+        <v>43</v>
       </c>
       <c r="AA17" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB17" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
+      </c>
+      <c r="AB17" s="13">
+        <v>1149</v>
       </c>
       <c r="AC17" s="13">
-        <v>1149</v>
-      </c>
-      <c r="AD17" s="13">
         <v>584</v>
       </c>
-      <c r="AE17" s="19" t="s">
-        <v>264</v>
+      <c r="AD17" s="19" t="s">
+        <v>262</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A18" s="25">
         <v>13010105</v>
       </c>
@@ -4690,10 +4692,10 @@
         <v>13010101</v>
       </c>
       <c r="G18" s="20" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H18" s="20" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="I18" s="13">
         <v>1</v>
@@ -4705,58 +4707,57 @@
       <c r="L18" s="13"/>
       <c r="M18" s="13"/>
       <c r="N18" s="13"/>
-      <c r="O18" s="13"/>
-      <c r="P18" s="13">
+      <c r="O18" s="13">
         <v>0.3</v>
       </c>
+      <c r="P18" s="13"/>
       <c r="Q18" s="13"/>
-      <c r="R18" s="13"/>
+      <c r="R18" s="13">
+        <v>0.7</v>
+      </c>
       <c r="S18" s="13">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="T18" s="13">
-        <v>0.6</v>
+        <v>3</v>
       </c>
       <c r="U18" s="13">
-        <v>3</v>
+        <v>43000002</v>
       </c>
       <c r="V18" s="13">
-        <v>43000002</v>
+        <v>2</v>
       </c>
       <c r="W18" s="13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="X18" s="13">
-        <v>3</v>
-      </c>
-      <c r="Y18" s="13">
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="Y18" s="13" t="s">
+        <v>106</v>
       </c>
       <c r="Z18" s="13" t="s">
-        <v>108</v>
+        <v>45</v>
       </c>
       <c r="AA18" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="AB18" s="13" t="s">
-        <v>79</v>
+        <v>77</v>
+      </c>
+      <c r="AB18" s="13">
+        <v>840</v>
       </c>
       <c r="AC18" s="13">
-        <v>840</v>
-      </c>
-      <c r="AD18" s="13">
         <v>444</v>
       </c>
-      <c r="AE18" s="19" t="s">
-        <v>265</v>
+      <c r="AD18" s="19" t="s">
+        <v>263</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A19" s="25">
         <v>13010106</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C19" s="13">
         <v>2</v>
@@ -4771,10 +4772,10 @@
         <v>13010016</v>
       </c>
       <c r="G19" s="20" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="I19" s="13">
         <v>1</v>
@@ -4783,63 +4784,60 @@
       <c r="K19" s="13"/>
       <c r="L19" s="13"/>
       <c r="M19" s="13"/>
-      <c r="N19" s="13">
-        <v>1</v>
-      </c>
-      <c r="O19" s="13"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="13">
+        <v>0.2</v>
+      </c>
       <c r="P19" s="13">
+        <v>0.8</v>
+      </c>
+      <c r="Q19" s="13"/>
+      <c r="R19" s="13">
         <v>0.2</v>
       </c>
-      <c r="Q19" s="13">
-        <v>0.8</v>
-      </c>
-      <c r="R19" s="13"/>
       <c r="S19" s="13">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="T19" s="13">
-        <v>0.4</v>
+        <v>4</v>
       </c>
       <c r="U19" s="13">
+        <v>43000002</v>
+      </c>
+      <c r="V19" s="13">
+        <v>3</v>
+      </c>
+      <c r="W19" s="13">
         <v>4</v>
       </c>
-      <c r="V19" s="13">
-        <v>43000002</v>
-      </c>
-      <c r="W19" s="13">
-        <v>3</v>
-      </c>
       <c r="X19" s="13">
-        <v>4</v>
-      </c>
-      <c r="Y19" s="13">
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="Y19" s="13" t="s">
+        <v>96</v>
       </c>
       <c r="Z19" s="13" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="AA19" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="AB19" s="13" t="s">
-        <v>69</v>
+        <v>67</v>
+      </c>
+      <c r="AB19" s="13">
+        <v>1067</v>
       </c>
       <c r="AC19" s="13">
-        <v>1067</v>
-      </c>
-      <c r="AD19" s="13">
         <v>445</v>
       </c>
-      <c r="AE19" s="19" t="s">
-        <v>265</v>
+      <c r="AD19" s="19" t="s">
+        <v>263</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A20" s="25">
         <v>13010107</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C20" s="15">
         <v>2</v>
@@ -4854,77 +4852,76 @@
         <v>13010101</v>
       </c>
       <c r="G20" s="20" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="H20" s="20" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="I20" s="13">
         <v>1</v>
       </c>
       <c r="J20" s="16"/>
       <c r="K20" s="16"/>
-      <c r="L20" s="16"/>
-      <c r="M20" s="16">
-        <v>1</v>
-      </c>
-      <c r="N20" s="16"/>
+      <c r="L20" s="16">
+        <v>1</v>
+      </c>
+      <c r="M20" s="16"/>
+      <c r="N20" s="15">
+        <v>1</v>
+      </c>
       <c r="O20" s="15">
-        <v>1</v>
-      </c>
-      <c r="P20" s="15">
         <v>0.3</v>
       </c>
-      <c r="Q20" s="15"/>
+      <c r="P20" s="15"/>
+      <c r="Q20" s="15">
+        <v>0.3</v>
+      </c>
       <c r="R20" s="15">
         <v>0.3</v>
       </c>
       <c r="S20" s="15">
-        <v>0.3</v>
-      </c>
-      <c r="T20" s="15">
         <v>0.8</v>
       </c>
+      <c r="T20" s="13">
+        <v>4</v>
+      </c>
       <c r="U20" s="13">
-        <v>4</v>
+        <v>43000002</v>
       </c>
       <c r="V20" s="13">
-        <v>43000002</v>
+        <v>3</v>
       </c>
       <c r="W20" s="13">
         <v>3</v>
       </c>
       <c r="X20" s="13">
-        <v>3</v>
-      </c>
-      <c r="Y20" s="13">
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="Y20" s="13" t="s">
+        <v>180</v>
       </c>
       <c r="Z20" s="13" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="AA20" s="13" t="s">
-        <v>182</v>
-      </c>
-      <c r="AB20" s="13" t="s">
-        <v>166</v>
+        <v>164</v>
+      </c>
+      <c r="AB20" s="16">
+        <v>850</v>
       </c>
       <c r="AC20" s="16">
-        <v>850</v>
-      </c>
-      <c r="AD20" s="16">
         <v>589</v>
       </c>
-      <c r="AE20" s="19" t="s">
-        <v>265</v>
+      <c r="AD20" s="19" t="s">
+        <v>263</v>
       </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A21" s="25">
         <v>13010108</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C21" s="15">
         <v>2</v>
@@ -4939,10 +4936,10 @@
         <v>13010101</v>
       </c>
       <c r="G21" s="20" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="H21" s="20" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="I21" s="13">
         <v>1</v>
@@ -4953,24 +4950,26 @@
       </c>
       <c r="L21" s="16"/>
       <c r="M21" s="16"/>
-      <c r="N21" s="16"/>
-      <c r="O21" s="15"/>
+      <c r="N21" s="15"/>
+      <c r="O21" s="15">
+        <v>0.1</v>
+      </c>
       <c r="P21" s="15">
-        <v>0.1</v>
-      </c>
-      <c r="Q21" s="15">
         <v>0.4</v>
       </c>
+      <c r="Q21" s="15"/>
       <c r="R21" s="15"/>
-      <c r="S21" s="15"/>
-      <c r="T21" s="15">
+      <c r="S21" s="15">
         <v>0.8</v>
       </c>
+      <c r="T21" s="13">
+        <v>2</v>
+      </c>
       <c r="U21" s="13">
-        <v>2</v>
+        <v>43000002</v>
       </c>
       <c r="V21" s="13">
-        <v>43000002</v>
+        <v>3</v>
       </c>
       <c r="W21" s="13">
         <v>3</v>
@@ -4978,34 +4977,31 @@
       <c r="X21" s="13">
         <v>3</v>
       </c>
-      <c r="Y21" s="13">
-        <v>3</v>
+      <c r="Y21" s="13" t="s">
+        <v>182</v>
       </c>
       <c r="Z21" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="AA21" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="AB21" s="16" t="s">
-        <v>170</v>
+        <v>182</v>
+      </c>
+      <c r="AA21" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="AB21" s="13">
+        <v>682</v>
       </c>
       <c r="AC21" s="13">
-        <v>682</v>
-      </c>
-      <c r="AD21" s="13">
         <v>545</v>
       </c>
-      <c r="AE21" s="19" t="s">
-        <v>266</v>
+      <c r="AD21" s="19" t="s">
+        <v>264</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A22" s="25">
         <v>13010109</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C22" s="15">
         <v>2</v>
@@ -5020,10 +5016,10 @@
         <v>13010101</v>
       </c>
       <c r="G22" s="20" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H22" s="16" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="I22" s="13">
         <v>1</v>
@@ -5034,24 +5030,26 @@
       </c>
       <c r="L22" s="16"/>
       <c r="M22" s="16"/>
-      <c r="N22" s="16"/>
-      <c r="O22" s="15"/>
+      <c r="N22" s="15"/>
+      <c r="O22" s="15">
+        <v>0.1</v>
+      </c>
       <c r="P22" s="15">
-        <v>0.1</v>
-      </c>
-      <c r="Q22" s="15">
         <v>0.4</v>
       </c>
-      <c r="R22" s="15"/>
-      <c r="S22" s="15">
+      <c r="Q22" s="15"/>
+      <c r="R22" s="15">
         <v>0.8</v>
       </c>
-      <c r="T22" s="15"/>
+      <c r="S22" s="15"/>
+      <c r="T22" s="13">
+        <v>4</v>
+      </c>
       <c r="U22" s="13">
-        <v>4</v>
+        <v>43000002</v>
       </c>
       <c r="V22" s="13">
-        <v>43000002</v>
+        <v>3</v>
       </c>
       <c r="W22" s="13">
         <v>3</v>
@@ -5059,34 +5057,31 @@
       <c r="X22" s="13">
         <v>3</v>
       </c>
-      <c r="Y22" s="13">
-        <v>3</v>
-      </c>
-      <c r="Z22" s="13" t="s">
-        <v>195</v>
-      </c>
-      <c r="AA22" s="20" t="s">
-        <v>196</v>
-      </c>
-      <c r="AB22" s="16" t="s">
-        <v>192</v>
+      <c r="Y22" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="Z22" s="20" t="s">
+        <v>194</v>
+      </c>
+      <c r="AA22" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="AB22" s="16">
+        <v>643</v>
       </c>
       <c r="AC22" s="16">
-        <v>643</v>
-      </c>
-      <c r="AD22" s="16">
         <v>455</v>
       </c>
-      <c r="AE22" s="19" t="s">
-        <v>266</v>
+      <c r="AD22" s="19" t="s">
+        <v>264</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A23" s="25">
         <v>13010110</v>
       </c>
       <c r="B23" s="27" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C23" s="15">
         <v>2</v>
@@ -5102,7 +5097,7 @@
       </c>
       <c r="G23" s="20"/>
       <c r="H23" s="16" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="I23" s="13">
         <v>1</v>
@@ -5111,63 +5106,62 @@
       <c r="K23" s="16"/>
       <c r="L23" s="16"/>
       <c r="M23" s="16"/>
-      <c r="N23" s="16"/>
+      <c r="N23" s="15">
+        <v>1</v>
+      </c>
       <c r="O23" s="15">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="P23" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="Q23" s="15">
         <v>0.2</v>
       </c>
-      <c r="Q23" s="15">
-        <v>0.8</v>
-      </c>
       <c r="R23" s="15">
-        <v>0.2</v>
-      </c>
-      <c r="S23" s="15">
         <v>0.5</v>
       </c>
-      <c r="T23" s="15"/>
+      <c r="S23" s="15"/>
+      <c r="T23" s="13">
+        <v>3</v>
+      </c>
       <c r="U23" s="13">
-        <v>3</v>
+        <v>43000002</v>
       </c>
       <c r="V23" s="13">
-        <v>43000002</v>
+        <v>2</v>
       </c>
       <c r="W23" s="13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="X23" s="13">
-        <v>4</v>
-      </c>
-      <c r="Y23" s="13">
-        <v>3</v>
+        <v>3</v>
+      </c>
+      <c r="Y23" s="20" t="s">
+        <v>195</v>
       </c>
       <c r="Z23" s="20" t="s">
-        <v>197</v>
-      </c>
-      <c r="AA23" s="20" t="s">
-        <v>197</v>
-      </c>
-      <c r="AB23" s="16" t="s">
-        <v>193</v>
+        <v>195</v>
+      </c>
+      <c r="AA23" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="AB23" s="16">
+        <v>720</v>
       </c>
       <c r="AC23" s="16">
-        <v>720</v>
-      </c>
-      <c r="AD23" s="16">
         <v>375</v>
       </c>
-      <c r="AE23" s="19" t="s">
-        <v>236</v>
+      <c r="AD23" s="19" t="s">
+        <v>234</v>
       </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A24" s="23">
         <v>13010201</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C24" s="15">
         <v>1</v>
@@ -5188,49 +5182,48 @@
       <c r="K24" s="16"/>
       <c r="L24" s="16"/>
       <c r="M24" s="16"/>
-      <c r="N24" s="16"/>
+      <c r="N24" s="15"/>
       <c r="O24" s="15"/>
       <c r="P24" s="15"/>
       <c r="Q24" s="15"/>
       <c r="R24" s="15"/>
       <c r="S24" s="15"/>
       <c r="T24" s="15"/>
-      <c r="U24" s="15"/>
-      <c r="V24" s="13"/>
+      <c r="U24" s="13"/>
+      <c r="V24" s="13">
+        <v>4</v>
+      </c>
       <c r="W24" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="X24" s="13">
         <v>2</v>
       </c>
-      <c r="Y24" s="13">
-        <v>2</v>
+      <c r="Y24" s="13" t="s">
+        <v>178</v>
       </c>
       <c r="Z24" s="13" t="s">
-        <v>180</v>
-      </c>
-      <c r="AA24" s="13" t="s">
-        <v>180</v>
-      </c>
-      <c r="AB24" s="16" t="s">
-        <v>167</v>
+        <v>178</v>
+      </c>
+      <c r="AA24" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="AB24" s="13">
+        <v>807</v>
       </c>
       <c r="AC24" s="13">
-        <v>807</v>
-      </c>
-      <c r="AD24" s="13">
         <v>720</v>
       </c>
-      <c r="AE24" s="19" t="s">
-        <v>263</v>
+      <c r="AD24" s="19" t="s">
+        <v>261</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A25" s="23">
         <v>13010202</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C25" s="15">
         <v>2</v>
@@ -5245,10 +5238,10 @@
         <v>13010201</v>
       </c>
       <c r="G25" s="15" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="H25" s="15" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="I25" s="13">
         <v>1</v>
@@ -5262,54 +5255,53 @@
       <c r="N25" s="15"/>
       <c r="O25" s="15"/>
       <c r="P25" s="15"/>
-      <c r="Q25" s="15"/>
-      <c r="R25" s="15">
+      <c r="Q25" s="15">
         <v>0.7</v>
       </c>
-      <c r="S25" s="15"/>
-      <c r="T25" s="15">
+      <c r="R25" s="15"/>
+      <c r="S25" s="15">
         <v>0.3</v>
       </c>
+      <c r="T25" s="13">
+        <v>3</v>
+      </c>
       <c r="U25" s="13">
-        <v>3</v>
+        <v>43000002</v>
       </c>
       <c r="V25" s="13">
-        <v>43000002</v>
+        <v>4</v>
       </c>
       <c r="W25" s="13">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="X25" s="13">
-        <v>1</v>
-      </c>
-      <c r="Y25" s="13">
-        <v>3</v>
+        <v>3</v>
+      </c>
+      <c r="Y25" s="13" t="s">
+        <v>183</v>
       </c>
       <c r="Z25" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="AA25" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="AB25" s="15" t="s">
-        <v>160</v>
+        <v>183</v>
+      </c>
+      <c r="AA25" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="AB25" s="15">
+        <v>974</v>
       </c>
       <c r="AC25" s="15">
-        <v>974</v>
-      </c>
-      <c r="AD25" s="15">
         <v>594</v>
       </c>
-      <c r="AE25" s="19" t="s">
-        <v>263</v>
+      <c r="AD25" s="19" t="s">
+        <v>261</v>
       </c>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A26" s="23">
         <v>13010203</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C26" s="15">
         <v>2</v>
@@ -5324,10 +5316,10 @@
         <v>13010201</v>
       </c>
       <c r="G26" s="15" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="H26" s="15" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="I26" s="13">
         <v>1</v>
@@ -5336,61 +5328,60 @@
       <c r="K26" s="15"/>
       <c r="L26" s="15"/>
       <c r="M26" s="15"/>
-      <c r="N26" s="15"/>
+      <c r="N26" s="15">
+        <v>1</v>
+      </c>
       <c r="O26" s="15">
-        <v>1</v>
-      </c>
-      <c r="P26" s="15">
         <v>0.2</v>
       </c>
-      <c r="Q26" s="15"/>
-      <c r="R26" s="15">
+      <c r="P26" s="15"/>
+      <c r="Q26" s="15">
         <v>0.5</v>
       </c>
-      <c r="S26" s="15"/>
-      <c r="T26" s="15">
+      <c r="R26" s="15"/>
+      <c r="S26" s="15">
         <v>0.2</v>
       </c>
+      <c r="T26" s="13">
+        <v>2</v>
+      </c>
       <c r="U26" s="13">
-        <v>2</v>
+        <v>43000002</v>
       </c>
       <c r="V26" s="13">
-        <v>43000002</v>
+        <v>4</v>
       </c>
       <c r="W26" s="13">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="X26" s="13">
-        <v>1</v>
-      </c>
-      <c r="Y26" s="13">
-        <v>3</v>
+        <v>3</v>
+      </c>
+      <c r="Y26" s="13" t="s">
+        <v>184</v>
       </c>
       <c r="Z26" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="AA26" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="AB26" s="15" t="s">
-        <v>161</v>
+        <v>184</v>
+      </c>
+      <c r="AA26" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="AB26" s="15">
+        <v>1080</v>
       </c>
       <c r="AC26" s="15">
-        <v>1080</v>
-      </c>
-      <c r="AD26" s="15">
         <v>720</v>
       </c>
-      <c r="AE26" s="19" t="s">
-        <v>263</v>
+      <c r="AD26" s="19" t="s">
+        <v>261</v>
       </c>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A27" s="23">
         <v>13010204</v>
       </c>
       <c r="B27" s="24" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C27" s="15">
         <v>2</v>
@@ -5405,73 +5396,72 @@
         <v>13010201</v>
       </c>
       <c r="G27" s="15" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="H27" s="15" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="I27" s="13">
         <v>1</v>
       </c>
       <c r="J27" s="15"/>
       <c r="K27" s="15"/>
-      <c r="L27" s="15"/>
-      <c r="M27" s="15">
-        <v>1</v>
-      </c>
+      <c r="L27" s="15">
+        <v>1</v>
+      </c>
+      <c r="M27" s="15"/>
       <c r="N27" s="15"/>
       <c r="O27" s="15"/>
-      <c r="P27" s="15"/>
+      <c r="P27" s="15">
+        <v>0.6</v>
+      </c>
       <c r="Q27" s="15">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="R27" s="15">
         <v>0.4</v>
       </c>
-      <c r="S27" s="15">
-        <v>0.4</v>
-      </c>
-      <c r="T27" s="15"/>
+      <c r="S27" s="15"/>
+      <c r="T27" s="13">
+        <v>3</v>
+      </c>
       <c r="U27" s="13">
-        <v>3</v>
+        <v>43000002</v>
       </c>
       <c r="V27" s="13">
-        <v>43000002</v>
+        <v>4</v>
       </c>
       <c r="W27" s="13">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="X27" s="13">
-        <v>1</v>
-      </c>
-      <c r="Y27" s="13">
-        <v>3</v>
+        <v>3</v>
+      </c>
+      <c r="Y27" s="13" t="s">
+        <v>185</v>
       </c>
       <c r="Z27" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="AA27" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="AB27" s="15" t="s">
-        <v>163</v>
+        <v>185</v>
+      </c>
+      <c r="AA27" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB27" s="15">
+        <v>1074</v>
       </c>
       <c r="AC27" s="15">
-        <v>1074</v>
-      </c>
-      <c r="AD27" s="15">
         <v>630</v>
       </c>
-      <c r="AE27" s="19" t="s">
-        <v>263</v>
+      <c r="AD27" s="19" t="s">
+        <v>261</v>
       </c>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A28" s="23">
         <v>13010205</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C28" s="15">
         <v>2</v>
@@ -5486,7 +5476,7 @@
         <v>13010201</v>
       </c>
       <c r="G28" s="15" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="H28" s="16"/>
       <c r="I28" s="13">
@@ -5498,57 +5488,56 @@
       <c r="K28" s="16"/>
       <c r="L28" s="16"/>
       <c r="M28" s="16"/>
-      <c r="N28" s="16"/>
-      <c r="O28" s="15"/>
-      <c r="P28" s="15">
+      <c r="N28" s="15"/>
+      <c r="O28" s="15">
         <v>0.3</v>
       </c>
+      <c r="P28" s="15"/>
       <c r="Q28" s="15"/>
       <c r="R28" s="15"/>
-      <c r="S28" s="15"/>
-      <c r="T28" s="15">
+      <c r="S28" s="15">
         <v>0.3</v>
       </c>
+      <c r="T28" s="13">
+        <v>5</v>
+      </c>
       <c r="U28" s="13">
-        <v>5</v>
+        <v>43000002</v>
       </c>
       <c r="V28" s="13">
-        <v>43000002</v>
+        <v>4</v>
       </c>
       <c r="W28" s="13">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="X28" s="13">
-        <v>1</v>
-      </c>
-      <c r="Y28" s="13">
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="Y28" s="20" t="s">
+        <v>181</v>
       </c>
       <c r="Z28" s="20" t="s">
-        <v>183</v>
-      </c>
-      <c r="AA28" s="20" t="s">
-        <v>183</v>
-      </c>
-      <c r="AB28" s="16" t="s">
-        <v>168</v>
+        <v>181</v>
+      </c>
+      <c r="AA28" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="AB28" s="13">
+        <v>717</v>
       </c>
       <c r="AC28" s="13">
-        <v>717</v>
-      </c>
-      <c r="AD28" s="13">
         <v>655</v>
       </c>
-      <c r="AE28" s="19" t="s">
-        <v>263</v>
+      <c r="AD28" s="19" t="s">
+        <v>261</v>
       </c>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A29" s="23">
         <v>13010206</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C29" s="15">
         <v>2</v>
@@ -5564,66 +5553,61 @@
       </c>
       <c r="G29" s="16"/>
       <c r="H29" s="20" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="I29" s="13">
         <v>1</v>
       </c>
       <c r="J29" s="16"/>
       <c r="K29" s="16"/>
-      <c r="L29" s="16">
-        <v>1</v>
-      </c>
+      <c r="L29" s="16"/>
       <c r="M29" s="16"/>
-      <c r="N29" s="16">
-        <v>1</v>
-      </c>
+      <c r="N29" s="15"/>
       <c r="O29" s="15"/>
       <c r="P29" s="15"/>
       <c r="Q29" s="15"/>
       <c r="R29" s="15"/>
       <c r="S29" s="15"/>
-      <c r="T29" s="15"/>
+      <c r="T29" s="13">
+        <v>2</v>
+      </c>
       <c r="U29" s="13">
-        <v>2</v>
+        <v>43000002</v>
       </c>
       <c r="V29" s="13">
-        <v>43000002</v>
+        <v>4</v>
       </c>
       <c r="W29" s="13">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="X29" s="13">
-        <v>1</v>
-      </c>
-      <c r="Y29" s="13">
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="Y29" s="20" t="s">
+        <v>187</v>
       </c>
       <c r="Z29" s="20" t="s">
-        <v>189</v>
-      </c>
-      <c r="AA29" s="20" t="s">
-        <v>189</v>
-      </c>
-      <c r="AB29" s="16" t="s">
-        <v>169</v>
+        <v>187</v>
+      </c>
+      <c r="AA29" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="AB29" s="13">
+        <v>637</v>
       </c>
       <c r="AC29" s="13">
-        <v>637</v>
-      </c>
-      <c r="AD29" s="13">
         <v>735</v>
       </c>
-      <c r="AE29" s="19" t="s">
-        <v>263</v>
+      <c r="AD29" s="19" t="s">
+        <v>261</v>
       </c>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A30" s="23">
         <v>13010207</v>
       </c>
       <c r="B30" s="23" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C30" s="15">
         <v>2</v>
@@ -5639,7 +5623,7 @@
       </c>
       <c r="G30" s="15"/>
       <c r="H30" s="15" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="I30" s="13">
         <v>1</v>
@@ -5648,59 +5632,58 @@
       <c r="K30" s="15"/>
       <c r="L30" s="15"/>
       <c r="M30" s="15"/>
-      <c r="N30" s="15"/>
+      <c r="N30" s="15">
+        <v>1</v>
+      </c>
       <c r="O30" s="15">
-        <v>1</v>
-      </c>
-      <c r="P30" s="15">
         <v>0.5</v>
       </c>
+      <c r="P30" s="15"/>
       <c r="Q30" s="15"/>
       <c r="R30" s="15"/>
-      <c r="S30" s="15"/>
-      <c r="T30" s="15">
+      <c r="S30" s="15">
         <v>0.4</v>
       </c>
+      <c r="T30" s="13">
+        <v>3</v>
+      </c>
       <c r="U30" s="13">
-        <v>3</v>
+        <v>43000002</v>
       </c>
       <c r="V30" s="13">
-        <v>43000002</v>
+        <v>5</v>
       </c>
       <c r="W30" s="13">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="X30" s="13">
-        <v>1</v>
-      </c>
-      <c r="Y30" s="13">
         <v>4</v>
       </c>
+      <c r="Y30" s="13" t="s">
+        <v>186</v>
+      </c>
       <c r="Z30" s="13" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="AA30" s="13" t="s">
-        <v>188</v>
-      </c>
-      <c r="AB30" s="13" t="s">
-        <v>171</v>
+        <v>169</v>
+      </c>
+      <c r="AB30" s="13">
+        <v>737</v>
       </c>
       <c r="AC30" s="13">
-        <v>737</v>
-      </c>
-      <c r="AD30" s="13">
         <v>785</v>
       </c>
-      <c r="AE30" s="19" t="s">
-        <v>263</v>
+      <c r="AD30" s="19" t="s">
+        <v>261</v>
       </c>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A31" s="23">
         <v>13010208</v>
       </c>
       <c r="B31" s="24" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C31" s="15">
         <v>2</v>
@@ -5715,10 +5698,10 @@
         <v>13010201</v>
       </c>
       <c r="G31" s="15" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="H31" s="15" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="I31" s="13">
         <v>1</v>
@@ -5727,63 +5710,60 @@
       <c r="K31" s="15">
         <v>1</v>
       </c>
-      <c r="L31" s="15">
-        <v>1</v>
-      </c>
+      <c r="L31" s="15"/>
       <c r="M31" s="15"/>
       <c r="N31" s="15"/>
       <c r="O31" s="15"/>
-      <c r="P31" s="15"/>
-      <c r="Q31" s="15">
+      <c r="P31" s="15">
         <v>0.2</v>
       </c>
-      <c r="R31" s="15"/>
+      <c r="Q31" s="15"/>
+      <c r="R31" s="15">
+        <v>0.1</v>
+      </c>
       <c r="S31" s="15">
-        <v>0.1</v>
-      </c>
-      <c r="T31" s="15">
         <v>0.5</v>
       </c>
+      <c r="T31" s="13">
+        <v>4</v>
+      </c>
       <c r="U31" s="13">
+        <v>43000002</v>
+      </c>
+      <c r="V31" s="13">
         <v>4</v>
       </c>
-      <c r="V31" s="13">
-        <v>43000002</v>
-      </c>
       <c r="W31" s="13">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="X31" s="13">
-        <v>1</v>
-      </c>
-      <c r="Y31" s="13">
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="Y31" s="13" t="s">
+        <v>179</v>
       </c>
       <c r="Z31" s="13" t="s">
-        <v>181</v>
-      </c>
-      <c r="AA31" s="13" t="s">
-        <v>181</v>
-      </c>
-      <c r="AB31" s="15" t="s">
-        <v>164</v>
+        <v>179</v>
+      </c>
+      <c r="AA31" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB31" s="19">
+        <v>894</v>
       </c>
       <c r="AC31" s="19">
-        <v>894</v>
-      </c>
-      <c r="AD31" s="19">
         <v>679</v>
       </c>
-      <c r="AE31" s="19" t="s">
-        <v>263</v>
+      <c r="AD31" s="19" t="s">
+        <v>261</v>
       </c>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A32" s="23">
         <v>13010209</v>
       </c>
       <c r="B32" s="23" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C32" s="15">
         <v>2</v>
@@ -5799,7 +5779,7 @@
       </c>
       <c r="G32" s="20"/>
       <c r="H32" s="20" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="I32" s="13">
         <v>1</v>
@@ -5808,52 +5788,51 @@
       <c r="K32" s="16"/>
       <c r="L32" s="16"/>
       <c r="M32" s="16"/>
-      <c r="N32" s="16"/>
-      <c r="O32" s="15"/>
-      <c r="P32" s="15">
+      <c r="N32" s="15"/>
+      <c r="O32" s="15">
         <v>0.3</v>
       </c>
-      <c r="Q32" s="15"/>
-      <c r="R32" s="15">
+      <c r="P32" s="15"/>
+      <c r="Q32" s="15">
         <v>0.7</v>
       </c>
+      <c r="R32" s="15"/>
       <c r="S32" s="15"/>
-      <c r="T32" s="15"/>
+      <c r="T32" s="13">
+        <v>3</v>
+      </c>
       <c r="U32" s="13">
-        <v>3</v>
+        <v>43000002</v>
       </c>
       <c r="V32" s="13">
-        <v>43000002</v>
+        <v>4</v>
       </c>
       <c r="W32" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="X32" s="13">
         <v>2</v>
       </c>
-      <c r="Y32" s="13">
-        <v>2</v>
+      <c r="Y32" s="20" t="s">
+        <v>188</v>
       </c>
       <c r="Z32" s="20" t="s">
-        <v>190</v>
-      </c>
-      <c r="AA32" s="20" t="s">
-        <v>190</v>
-      </c>
-      <c r="AB32" s="16" t="s">
-        <v>165</v>
+        <v>188</v>
+      </c>
+      <c r="AA32" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="AB32" s="19">
+        <v>984</v>
       </c>
       <c r="AC32" s="19">
-        <v>984</v>
-      </c>
-      <c r="AD32" s="19">
         <v>734</v>
       </c>
-      <c r="AE32" s="19" t="s">
-        <v>263</v>
+      <c r="AD32" s="19" t="s">
+        <v>261</v>
       </c>
     </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A33" s="26">
         <v>13010301</v>
       </c>
@@ -5873,68 +5852,65 @@
         <v>13010006</v>
       </c>
       <c r="G33" s="20" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="H33" s="13" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="I33" s="13">
         <v>1</v>
       </c>
       <c r="J33" s="13"/>
       <c r="K33" s="13"/>
-      <c r="L33" s="13"/>
-      <c r="M33" s="13">
-        <v>1</v>
-      </c>
-      <c r="N33" s="13">
-        <v>1</v>
-      </c>
+      <c r="L33" s="13">
+        <v>1</v>
+      </c>
+      <c r="M33" s="13"/>
+      <c r="N33" s="13"/>
       <c r="O33" s="13"/>
-      <c r="P33" s="13"/>
-      <c r="Q33" s="13">
+      <c r="P33" s="13">
         <v>0.8</v>
       </c>
+      <c r="Q33" s="13"/>
       <c r="R33" s="13"/>
-      <c r="S33" s="13"/>
+      <c r="S33" s="13">
+        <v>0.3</v>
+      </c>
       <c r="T33" s="13">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="U33" s="13">
-        <v>2</v>
+        <v>43000002</v>
       </c>
       <c r="V33" s="13">
-        <v>43000002</v>
+        <v>3</v>
       </c>
       <c r="W33" s="13">
         <v>3</v>
       </c>
       <c r="X33" s="13">
-        <v>3</v>
-      </c>
-      <c r="Y33" s="13">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="Y33" s="13" t="s">
+        <v>103</v>
       </c>
       <c r="Z33" s="13" t="s">
-        <v>105</v>
+        <v>38</v>
       </c>
       <c r="AA33" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB33" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
+      </c>
+      <c r="AB33" s="21">
+        <v>1550</v>
       </c>
       <c r="AC33" s="21">
-        <v>1550</v>
-      </c>
-      <c r="AD33" s="21">
         <v>505</v>
       </c>
-      <c r="AE33" s="19" t="s">
-        <v>236</v>
+      <c r="AD33" s="19" t="s">
+        <v>234</v>
       </c>
     </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A34" s="26">
         <v>13010302</v>
       </c>
@@ -5954,10 +5930,10 @@
         <v>13010006</v>
       </c>
       <c r="G34" s="20" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="H34" s="13" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="I34" s="13">
         <v>1</v>
@@ -5966,54 +5942,51 @@
       <c r="K34" s="13"/>
       <c r="L34" s="13"/>
       <c r="M34" s="13"/>
-      <c r="N34" s="13">
-        <v>1</v>
-      </c>
+      <c r="N34" s="13"/>
       <c r="O34" s="13"/>
-      <c r="P34" s="13"/>
-      <c r="Q34" s="13">
+      <c r="P34" s="13">
         <v>0.6</v>
       </c>
+      <c r="Q34" s="13"/>
       <c r="R34" s="13"/>
-      <c r="S34" s="13"/>
+      <c r="S34" s="13">
+        <v>0.3</v>
+      </c>
       <c r="T34" s="13">
-        <v>0.3</v>
+        <v>3</v>
       </c>
       <c r="U34" s="13">
-        <v>3</v>
+        <v>43000002</v>
       </c>
       <c r="V34" s="13">
-        <v>43000002</v>
+        <v>4</v>
       </c>
       <c r="W34" s="13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="X34" s="13">
-        <v>3</v>
-      </c>
-      <c r="Y34" s="13">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="Y34" s="13" t="s">
+        <v>99</v>
       </c>
       <c r="Z34" s="13" t="s">
-        <v>101</v>
+        <v>36</v>
       </c>
       <c r="AA34" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB34" s="13" t="s">
-        <v>71</v>
+        <v>69</v>
+      </c>
+      <c r="AB34" s="21">
+        <v>1441</v>
       </c>
       <c r="AC34" s="21">
-        <v>1441</v>
-      </c>
-      <c r="AD34" s="21">
         <v>527</v>
       </c>
-      <c r="AE34" s="19" t="s">
-        <v>236</v>
+      <c r="AD34" s="19" t="s">
+        <v>234</v>
       </c>
     </row>
-    <row r="35" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A35" s="26">
         <v>13010303</v>
       </c>
@@ -6033,10 +6006,10 @@
         <v>13010006</v>
       </c>
       <c r="G35" s="13" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H35" s="13" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="I35" s="13">
         <v>1</v>
@@ -6047,63 +6020,62 @@
       </c>
       <c r="L35" s="13"/>
       <c r="M35" s="13"/>
-      <c r="N35" s="13"/>
-      <c r="O35" s="13">
-        <v>1</v>
-      </c>
-      <c r="P35" s="13"/>
+      <c r="N35" s="13">
+        <v>1</v>
+      </c>
+      <c r="O35" s="13"/>
+      <c r="P35" s="13">
+        <v>0.2</v>
+      </c>
       <c r="Q35" s="13">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="R35" s="13">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="S35" s="13">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="T35" s="13">
-        <v>0.8</v>
+        <v>4</v>
       </c>
       <c r="U35" s="13">
-        <v>4</v>
+        <v>43000002</v>
       </c>
       <c r="V35" s="13">
-        <v>43000002</v>
+        <v>3</v>
       </c>
       <c r="W35" s="13">
         <v>3</v>
       </c>
       <c r="X35" s="13">
-        <v>3</v>
-      </c>
-      <c r="Y35" s="13">
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="Y35" s="13" t="s">
+        <v>100</v>
       </c>
       <c r="Z35" s="13" t="s">
-        <v>102</v>
+        <v>37</v>
       </c>
       <c r="AA35" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="AB35" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
+      </c>
+      <c r="AB35" s="21">
+        <v>1574</v>
       </c>
       <c r="AC35" s="21">
-        <v>1574</v>
-      </c>
-      <c r="AD35" s="21">
         <v>373</v>
       </c>
-      <c r="AE35" s="19" t="s">
-        <v>236</v>
+      <c r="AD35" s="19" t="s">
+        <v>234</v>
       </c>
     </row>
-    <row r="36" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A36" s="17">
         <v>13020001</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C36" s="13">
         <v>3</v>
@@ -6118,61 +6090,60 @@
         <v>13010002</v>
       </c>
       <c r="G36" s="20" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="H36" s="13"/>
       <c r="I36" s="13"/>
       <c r="J36" s="13"/>
       <c r="K36" s="13"/>
-      <c r="L36" s="13"/>
+      <c r="L36" s="13">
+        <v>1</v>
+      </c>
       <c r="M36" s="13"/>
-      <c r="N36" s="13">
-        <v>1</v>
-      </c>
-      <c r="O36" s="13"/>
+      <c r="N36" s="13"/>
+      <c r="O36" s="13">
+        <v>0.4</v>
+      </c>
       <c r="P36" s="13">
-        <v>0.4</v>
-      </c>
-      <c r="Q36" s="13">
         <v>0.3</v>
       </c>
-      <c r="R36" s="13"/>
-      <c r="S36" s="13">
+      <c r="Q36" s="13"/>
+      <c r="R36" s="13">
         <v>0.3</v>
       </c>
+      <c r="S36" s="13"/>
       <c r="T36" s="13"/>
-      <c r="U36" s="13"/>
+      <c r="U36" s="13">
+        <v>43000002</v>
+      </c>
       <c r="V36" s="13">
-        <v>43000002</v>
+        <v>2</v>
       </c>
       <c r="W36" s="13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="X36" s="13">
-        <v>3</v>
-      </c>
-      <c r="Y36" s="13">
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="Y36" s="13" t="s">
+        <v>107</v>
       </c>
       <c r="Z36" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="AA36" s="13" t="s">
-        <v>130</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="AA36" s="13"/>
       <c r="AB36" s="13"/>
       <c r="AC36" s="13"/>
-      <c r="AD36" s="13"/>
-      <c r="AE36" s="19" t="s">
-        <v>238</v>
+      <c r="AD36" s="19" t="s">
+        <v>236</v>
       </c>
     </row>
-    <row r="37" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A37" s="17">
         <v>13020002</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C37" s="13">
         <v>3</v>
@@ -6194,50 +6165,49 @@
       <c r="L37" s="13"/>
       <c r="M37" s="13"/>
       <c r="N37" s="13"/>
-      <c r="O37" s="13"/>
-      <c r="P37" s="13">
+      <c r="O37" s="13">
         <v>0.3</v>
       </c>
+      <c r="P37" s="13"/>
       <c r="Q37" s="13"/>
-      <c r="R37" s="13"/>
+      <c r="R37" s="13">
+        <v>0.2</v>
+      </c>
       <c r="S37" s="13">
         <v>0.2</v>
       </c>
-      <c r="T37" s="13">
-        <v>0.2</v>
-      </c>
-      <c r="U37" s="13"/>
+      <c r="T37" s="13"/>
+      <c r="U37" s="13">
+        <v>43000002</v>
+      </c>
       <c r="V37" s="13">
-        <v>43000002</v>
+        <v>2</v>
       </c>
       <c r="W37" s="13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="X37" s="13">
-        <v>3</v>
-      </c>
-      <c r="Y37" s="13">
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="Y37" s="13" t="s">
+        <v>108</v>
       </c>
       <c r="Z37" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="AA37" s="13" t="s">
-        <v>131</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="AA37" s="13"/>
       <c r="AB37" s="13"/>
       <c r="AC37" s="13"/>
-      <c r="AD37" s="13"/>
-      <c r="AE37" s="19" t="s">
-        <v>238</v>
+      <c r="AD37" s="19" t="s">
+        <v>236</v>
       </c>
     </row>
-    <row r="38" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A38" s="17">
         <v>13020011</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C38" s="13">
         <v>3</v>
@@ -6252,10 +6222,10 @@
         <v>13010007</v>
       </c>
       <c r="G38" s="13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H38" s="13" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I38" s="13"/>
       <c r="J38" s="13"/>
@@ -6263,48 +6233,47 @@
       <c r="L38" s="13"/>
       <c r="M38" s="13"/>
       <c r="N38" s="13"/>
-      <c r="O38" s="13"/>
-      <c r="P38" s="13">
+      <c r="O38" s="13">
         <v>0.3</v>
       </c>
+      <c r="P38" s="13"/>
       <c r="Q38" s="13"/>
-      <c r="R38" s="13"/>
-      <c r="S38" s="13">
+      <c r="R38" s="13">
         <v>0.2</v>
       </c>
+      <c r="S38" s="13"/>
       <c r="T38" s="13"/>
-      <c r="U38" s="13"/>
+      <c r="U38" s="13">
+        <v>43000002</v>
+      </c>
       <c r="V38" s="13">
-        <v>43000002</v>
+        <v>2</v>
       </c>
       <c r="W38" s="13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="X38" s="13">
-        <v>4</v>
-      </c>
-      <c r="Y38" s="13">
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="Y38" s="13" t="s">
+        <v>113</v>
       </c>
       <c r="Z38" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="AA38" s="13" t="s">
-        <v>132</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="AA38" s="13"/>
       <c r="AB38" s="13"/>
       <c r="AC38" s="13"/>
-      <c r="AD38" s="13"/>
-      <c r="AE38" s="19" t="s">
-        <v>238</v>
+      <c r="AD38" s="19" t="s">
+        <v>236</v>
       </c>
     </row>
-    <row r="39" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A39" s="17">
         <v>13020012</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C39" s="13">
         <v>3</v>
@@ -6319,7 +6288,7 @@
         <v>13010007</v>
       </c>
       <c r="G39" s="13" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H39" s="13"/>
       <c r="I39" s="13"/>
@@ -6332,42 +6301,41 @@
       <c r="P39" s="13"/>
       <c r="Q39" s="13"/>
       <c r="R39" s="13"/>
-      <c r="S39" s="13"/>
-      <c r="T39" s="13">
+      <c r="S39" s="13">
         <v>0.3</v>
       </c>
-      <c r="U39" s="13"/>
+      <c r="T39" s="13"/>
+      <c r="U39" s="13">
+        <v>43000002</v>
+      </c>
       <c r="V39" s="13">
-        <v>43000002</v>
+        <v>2</v>
       </c>
       <c r="W39" s="13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="X39" s="13">
-        <v>4</v>
-      </c>
-      <c r="Y39" s="13">
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="Y39" s="13" t="s">
+        <v>117</v>
       </c>
       <c r="Z39" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="AA39" s="13" t="s">
-        <v>133</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="AA39" s="13"/>
       <c r="AB39" s="13"/>
       <c r="AC39" s="13"/>
-      <c r="AD39" s="13"/>
-      <c r="AE39" s="19" t="s">
-        <v>238</v>
+      <c r="AD39" s="19" t="s">
+        <v>236</v>
       </c>
     </row>
-    <row r="40" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A40" s="17">
         <v>13020013</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C40" s="13">
         <v>3</v>
@@ -6395,38 +6363,37 @@
       <c r="R40" s="13"/>
       <c r="S40" s="13"/>
       <c r="T40" s="13"/>
-      <c r="U40" s="13"/>
+      <c r="U40" s="13">
+        <v>43000002</v>
+      </c>
       <c r="V40" s="13">
-        <v>43000002</v>
+        <v>2</v>
       </c>
       <c r="W40" s="13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="X40" s="13">
-        <v>4</v>
-      </c>
-      <c r="Y40" s="13">
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="Y40" s="13" t="s">
+        <v>114</v>
       </c>
       <c r="Z40" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="AA40" s="13" t="s">
-        <v>134</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="AA40" s="13"/>
       <c r="AB40" s="13"/>
       <c r="AC40" s="13"/>
-      <c r="AD40" s="13"/>
-      <c r="AE40" s="19" t="s">
-        <v>238</v>
+      <c r="AD40" s="19" t="s">
+        <v>236</v>
       </c>
     </row>
-    <row r="41" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A41" s="17">
         <v>13020021</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C41" s="13">
         <v>3</v>
@@ -6441,10 +6408,10 @@
         <v>13010004</v>
       </c>
       <c r="G41" s="20" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="H41" s="13" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="I41" s="13"/>
       <c r="J41" s="13"/>
@@ -6454,48 +6421,47 @@
       <c r="N41" s="13"/>
       <c r="O41" s="13"/>
       <c r="P41" s="13"/>
-      <c r="Q41" s="13"/>
+      <c r="Q41" s="13">
+        <v>0.2</v>
+      </c>
       <c r="R41" s="13">
         <v>0.2</v>
       </c>
       <c r="S41" s="13">
-        <v>0.2</v>
-      </c>
-      <c r="T41" s="13">
         <v>0.4</v>
       </c>
-      <c r="U41" s="13"/>
+      <c r="T41" s="13"/>
+      <c r="U41" s="13">
+        <v>43000002</v>
+      </c>
       <c r="V41" s="13">
-        <v>43000002</v>
+        <v>3</v>
       </c>
       <c r="W41" s="13">
         <v>3</v>
       </c>
       <c r="X41" s="13">
-        <v>3</v>
-      </c>
-      <c r="Y41" s="13">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="Y41" s="13" t="s">
+        <v>126</v>
       </c>
       <c r="Z41" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="AA41" s="13" t="s">
-        <v>135</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="AA41" s="13"/>
       <c r="AB41" s="13"/>
       <c r="AC41" s="13"/>
-      <c r="AD41" s="13"/>
-      <c r="AE41" s="19" t="s">
-        <v>238</v>
+      <c r="AD41" s="19" t="s">
+        <v>236</v>
       </c>
     </row>
-    <row r="42" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A42" s="17">
         <v>13020022</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C42" s="13">
         <v>3</v>
@@ -6510,10 +6476,10 @@
         <v>13010004</v>
       </c>
       <c r="G42" s="20" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="H42" s="13" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="I42" s="13"/>
       <c r="J42" s="13"/>
@@ -6522,49 +6488,48 @@
       <c r="M42" s="13"/>
       <c r="N42" s="13"/>
       <c r="O42" s="13"/>
-      <c r="P42" s="13"/>
-      <c r="Q42" s="13">
+      <c r="P42" s="13">
         <v>0.3</v>
       </c>
-      <c r="R42" s="13"/>
+      <c r="Q42" s="13"/>
+      <c r="R42" s="13">
+        <v>0.1</v>
+      </c>
       <c r="S42" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="T42" s="13">
         <v>0.2</v>
       </c>
-      <c r="U42" s="13"/>
+      <c r="T42" s="13"/>
+      <c r="U42" s="13">
+        <v>43000002</v>
+      </c>
       <c r="V42" s="13">
-        <v>43000002</v>
+        <v>3</v>
       </c>
       <c r="W42" s="13">
         <v>3</v>
       </c>
       <c r="X42" s="13">
-        <v>3</v>
-      </c>
-      <c r="Y42" s="13">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="Y42" s="13" t="s">
+        <v>124</v>
       </c>
       <c r="Z42" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="AA42" s="13" t="s">
-        <v>136</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="AA42" s="13"/>
       <c r="AB42" s="13"/>
       <c r="AC42" s="13"/>
-      <c r="AD42" s="13"/>
-      <c r="AE42" s="19" t="s">
-        <v>238</v>
+      <c r="AD42" s="19" t="s">
+        <v>236</v>
       </c>
     </row>
-    <row r="43" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A43" s="17">
         <v>13020023</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C43" s="13">
         <v>3</v>
@@ -6579,7 +6544,7 @@
         <v>13010004</v>
       </c>
       <c r="G43" s="20" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="H43" s="13"/>
       <c r="I43" s="13"/>
@@ -6589,47 +6554,46 @@
       <c r="M43" s="13"/>
       <c r="N43" s="13"/>
       <c r="O43" s="13"/>
-      <c r="P43" s="13"/>
-      <c r="Q43" s="13">
+      <c r="P43" s="13">
         <v>0.2</v>
       </c>
+      <c r="Q43" s="13"/>
       <c r="R43" s="13"/>
-      <c r="S43" s="13"/>
-      <c r="T43" s="13">
+      <c r="S43" s="13">
         <v>0.2</v>
       </c>
-      <c r="U43" s="13"/>
+      <c r="T43" s="13"/>
+      <c r="U43" s="13">
+        <v>43000002</v>
+      </c>
       <c r="V43" s="13">
-        <v>43000002</v>
+        <v>3</v>
       </c>
       <c r="W43" s="13">
         <v>3</v>
       </c>
       <c r="X43" s="13">
-        <v>3</v>
-      </c>
-      <c r="Y43" s="13">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="Y43" s="13" t="s">
+        <v>125</v>
       </c>
       <c r="Z43" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AA43" s="13" t="s">
-        <v>137</v>
-      </c>
+        <v>135</v>
+      </c>
+      <c r="AA43" s="13"/>
       <c r="AB43" s="13"/>
       <c r="AC43" s="13"/>
-      <c r="AD43" s="13"/>
-      <c r="AE43" s="19" t="s">
-        <v>238</v>
+      <c r="AD43" s="19" t="s">
+        <v>236</v>
       </c>
     </row>
-    <row r="44" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A44" s="18">
         <v>13020031</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C44" s="13">
         <v>3</v>
@@ -6657,38 +6621,37 @@
       <c r="R44" s="15"/>
       <c r="S44" s="15"/>
       <c r="T44" s="15"/>
-      <c r="U44" s="15"/>
+      <c r="U44" s="13">
+        <v>43000002</v>
+      </c>
       <c r="V44" s="13">
-        <v>43000002</v>
+        <v>2</v>
       </c>
       <c r="W44" s="13">
         <v>2</v>
       </c>
       <c r="X44" s="13">
-        <v>2</v>
-      </c>
-      <c r="Y44" s="13">
         <v>5</v>
       </c>
-      <c r="Z44" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="AA44" s="15" t="s">
-        <v>148</v>
-      </c>
+      <c r="Y44" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="Z44" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="AA44" s="15"/>
       <c r="AB44" s="15"/>
       <c r="AC44" s="15"/>
-      <c r="AD44" s="15"/>
-      <c r="AE44" s="19" t="s">
-        <v>238</v>
+      <c r="AD44" s="19" t="s">
+        <v>236</v>
       </c>
     </row>
-    <row r="45" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A45" s="18">
         <v>13020032</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C45" s="13">
         <v>3</v>
@@ -6716,38 +6679,37 @@
       <c r="R45" s="15"/>
       <c r="S45" s="15"/>
       <c r="T45" s="15"/>
-      <c r="U45" s="15"/>
+      <c r="U45" s="13">
+        <v>43000002</v>
+      </c>
       <c r="V45" s="13">
-        <v>43000002</v>
+        <v>2</v>
       </c>
       <c r="W45" s="13">
         <v>2</v>
       </c>
       <c r="X45" s="13">
-        <v>2</v>
-      </c>
-      <c r="Y45" s="13">
         <v>5</v>
       </c>
-      <c r="Z45" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="AA45" s="15" t="s">
-        <v>149</v>
-      </c>
+      <c r="Y45" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="Z45" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="AA45" s="15"/>
       <c r="AB45" s="15"/>
       <c r="AC45" s="15"/>
-      <c r="AD45" s="15"/>
-      <c r="AE45" s="19" t="s">
-        <v>238</v>
+      <c r="AD45" s="19" t="s">
+        <v>236</v>
       </c>
     </row>
-    <row r="46" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A46" s="18">
         <v>13020033</v>
       </c>
       <c r="B46" s="17" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C46" s="13">
         <v>3</v>
@@ -6775,38 +6737,37 @@
       <c r="R46" s="15"/>
       <c r="S46" s="15"/>
       <c r="T46" s="15"/>
-      <c r="U46" s="15"/>
+      <c r="U46" s="13">
+        <v>43000002</v>
+      </c>
       <c r="V46" s="13">
-        <v>43000002</v>
+        <v>2</v>
       </c>
       <c r="W46" s="13">
         <v>2</v>
       </c>
       <c r="X46" s="13">
-        <v>2</v>
-      </c>
-      <c r="Y46" s="13">
         <v>5</v>
       </c>
-      <c r="Z46" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="AA46" s="15" t="s">
-        <v>150</v>
-      </c>
+      <c r="Y46" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="Z46" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="AA46" s="19"/>
       <c r="AB46" s="19"/>
       <c r="AC46" s="19"/>
-      <c r="AD46" s="19"/>
-      <c r="AE46" s="19" t="s">
-        <v>238</v>
+      <c r="AD46" s="19" t="s">
+        <v>236</v>
       </c>
     </row>
-    <row r="47" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A47" s="18">
         <v>13020034</v>
       </c>
       <c r="B47" s="17" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C47" s="13">
         <v>3</v>
@@ -6834,38 +6795,37 @@
       <c r="R47" s="15"/>
       <c r="S47" s="15"/>
       <c r="T47" s="15"/>
-      <c r="U47" s="15"/>
+      <c r="U47" s="13">
+        <v>43000002</v>
+      </c>
       <c r="V47" s="13">
-        <v>43000002</v>
+        <v>2</v>
       </c>
       <c r="W47" s="13">
         <v>2</v>
       </c>
       <c r="X47" s="13">
-        <v>2</v>
-      </c>
-      <c r="Y47" s="13">
         <v>5</v>
       </c>
-      <c r="Z47" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="AA47" s="15" t="s">
-        <v>151</v>
-      </c>
+      <c r="Y47" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="Z47" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="AA47" s="19"/>
       <c r="AB47" s="19"/>
       <c r="AC47" s="19"/>
-      <c r="AD47" s="19"/>
-      <c r="AE47" s="19" t="s">
-        <v>238</v>
+      <c r="AD47" s="19" t="s">
+        <v>236</v>
       </c>
     </row>
-    <row r="48" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A48" s="18">
         <v>13020035</v>
       </c>
       <c r="B48" s="17" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C48" s="13">
         <v>3</v>
@@ -6893,46 +6853,45 @@
       <c r="R48" s="15"/>
       <c r="S48" s="15"/>
       <c r="T48" s="15"/>
-      <c r="U48" s="15"/>
+      <c r="U48" s="13">
+        <v>43000002</v>
+      </c>
       <c r="V48" s="13">
-        <v>43000002</v>
+        <v>2</v>
       </c>
       <c r="W48" s="13">
         <v>2</v>
       </c>
       <c r="X48" s="13">
-        <v>2</v>
-      </c>
-      <c r="Y48" s="13">
         <v>5</v>
       </c>
-      <c r="Z48" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="AA48" s="15" t="s">
-        <v>152</v>
-      </c>
+      <c r="Y48" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="Z48" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="AA48" s="19"/>
       <c r="AB48" s="19"/>
       <c r="AC48" s="19"/>
-      <c r="AD48" s="19"/>
-      <c r="AE48" s="19" t="s">
-        <v>238</v>
+      <c r="AD48" s="19" t="s">
+        <v>236</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="I4:V48">
-    <cfRule type="cellIs" dxfId="36" priority="4" operator="equal">
+  <conditionalFormatting sqref="I4:U48">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4">
-    <cfRule type="cellIs" dxfId="35" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:H48">
-    <cfRule type="containsBlanks" dxfId="34" priority="5">
+    <cfRule type="containsBlanks" dxfId="0" priority="5">
       <formula>LEN(TRIM(G4))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
merge some dungeon boost event
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Scene.xlsx
+++ b/ConfigData/Xlsx/Scene.xlsx
@@ -962,10 +962,6 @@
     <t>crystalball|wishwell</t>
   </si>
   <si>
-    <t>bossmanwang;1|stonedoor;1|boostagi;1|hiddeway;1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>SCN004</t>
   </si>
   <si>
@@ -1036,7 +1032,11 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>diarybook;1|potteryroom;1|booststr;1|thief1;1</t>
+    <t>diarybook;1|potteryroom;1|gym;1|thief1;1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>bossmanwang;1|stonedoor;1|gym;1|hiddeway;1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1963,27 +1963,6 @@
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="36">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2865,6 +2844,27 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -2947,42 +2947,42 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AD48" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34" tableBorderDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AD48" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31" tableBorderDxfId="30">
   <autoFilter ref="A3:AD48"/>
   <sortState ref="A4:AC48">
     <sortCondition ref="A3:A48"/>
   </sortState>
   <tableColumns count="30">
-    <tableColumn id="1" name="Id" dataDxfId="32"/>
-    <tableColumn id="2" name="Name" dataDxfId="31"/>
-    <tableColumn id="18" name="Type" dataDxfId="30"/>
-    <tableColumn id="11" name="RegionId" dataDxfId="29"/>
-    <tableColumn id="3" name="Level" dataDxfId="28"/>
-    <tableColumn id="20" name="ReviveScene" dataDxfId="27"/>
-    <tableColumn id="4" name="Quest" dataDxfId="26"/>
-    <tableColumn id="17" name="QuestRandom" dataDxfId="25"/>
-    <tableColumn id="5" name="QPortal" dataDxfId="24"/>
-    <tableColumn id="6" name="QCardChange" dataDxfId="23"/>
-    <tableColumn id="7" name="QPiece" dataDxfId="22"/>
-    <tableColumn id="9" name="QDoctor" dataDxfId="21"/>
-    <tableColumn id="10" name="QAngel" dataDxfId="20"/>
-    <tableColumn id="22" name="QRes" dataDxfId="19"/>
-    <tableColumn id="27" name="QItemDrug" dataDxfId="18"/>
-    <tableColumn id="31" name="QItemFish" dataDxfId="17"/>
-    <tableColumn id="30" name="QItemOre" dataDxfId="16"/>
-    <tableColumn id="28" name="QItemMushroom" dataDxfId="15"/>
-    <tableColumn id="29" name="QItemWood" dataDxfId="14"/>
-    <tableColumn id="32" name="QEnemy" dataDxfId="13"/>
-    <tableColumn id="25" name="EnemyIds" dataDxfId="12"/>
-    <tableColumn id="19" name="Temperature" dataDxfId="11"/>
-    <tableColumn id="23" name="Humitity" dataDxfId="10"/>
-    <tableColumn id="26" name="Altitude" dataDxfId="9"/>
-    <tableColumn id="12" name="Url" dataDxfId="8"/>
-    <tableColumn id="13" name="TilePath" dataDxfId="7"/>
-    <tableColumn id="14" name="Icon" dataDxfId="6"/>
-    <tableColumn id="15" name="IconX" dataDxfId="5"/>
-    <tableColumn id="16" name="IconY" dataDxfId="4"/>
-    <tableColumn id="24" name="BGM" dataDxfId="3"/>
+    <tableColumn id="1" name="Id" dataDxfId="29"/>
+    <tableColumn id="2" name="Name" dataDxfId="28"/>
+    <tableColumn id="18" name="Type" dataDxfId="27"/>
+    <tableColumn id="11" name="RegionId" dataDxfId="26"/>
+    <tableColumn id="3" name="Level" dataDxfId="25"/>
+    <tableColumn id="20" name="ReviveScene" dataDxfId="24"/>
+    <tableColumn id="4" name="Quest" dataDxfId="23"/>
+    <tableColumn id="17" name="QuestRandom" dataDxfId="22"/>
+    <tableColumn id="5" name="QPortal" dataDxfId="21"/>
+    <tableColumn id="6" name="QCardChange" dataDxfId="20"/>
+    <tableColumn id="7" name="QPiece" dataDxfId="19"/>
+    <tableColumn id="9" name="QDoctor" dataDxfId="18"/>
+    <tableColumn id="10" name="QAngel" dataDxfId="17"/>
+    <tableColumn id="22" name="QRes" dataDxfId="16"/>
+    <tableColumn id="27" name="QItemDrug" dataDxfId="15"/>
+    <tableColumn id="31" name="QItemFish" dataDxfId="14"/>
+    <tableColumn id="30" name="QItemOre" dataDxfId="13"/>
+    <tableColumn id="28" name="QItemMushroom" dataDxfId="12"/>
+    <tableColumn id="29" name="QItemWood" dataDxfId="11"/>
+    <tableColumn id="32" name="QEnemy" dataDxfId="10"/>
+    <tableColumn id="25" name="EnemyIds" dataDxfId="9"/>
+    <tableColumn id="19" name="Temperature" dataDxfId="8"/>
+    <tableColumn id="23" name="Humitity" dataDxfId="7"/>
+    <tableColumn id="26" name="Altitude" dataDxfId="6"/>
+    <tableColumn id="12" name="Url" dataDxfId="5"/>
+    <tableColumn id="13" name="TilePath" dataDxfId="4"/>
+    <tableColumn id="14" name="Icon" dataDxfId="3"/>
+    <tableColumn id="15" name="IconX" dataDxfId="2"/>
+    <tableColumn id="16" name="IconY" dataDxfId="1"/>
+    <tableColumn id="24" name="BGM" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3311,8 +3311,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3399,10 +3399,10 @@
         <v>213</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="U1" s="28" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="V1" s="30" t="s">
         <v>201</v>
@@ -3491,10 +3491,10 @@
         <v>227</v>
       </c>
       <c r="T2" s="8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="U2" s="29" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="V2" s="31" t="s">
         <v>202</v>
@@ -3583,10 +3583,10 @@
         <v>208</v>
       </c>
       <c r="T3" s="34" t="s">
+        <v>268</v>
+      </c>
+      <c r="U3" s="33" t="s">
         <v>269</v>
-      </c>
-      <c r="U3" s="33" t="s">
-        <v>270</v>
       </c>
       <c r="V3" s="32" t="s">
         <v>203</v>
@@ -3710,7 +3710,7 @@
         <v>13010001</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="H5" s="13" t="s">
         <v>238</v>
@@ -3794,7 +3794,7 @@
         <v>13010006</v>
       </c>
       <c r="G6" s="20" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="H6" s="13" t="s">
         <v>239</v>
@@ -3847,7 +3847,7 @@
         <v>432</v>
       </c>
       <c r="AD6" s="19" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.15">
@@ -3870,7 +3870,7 @@
         <v>13010006</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="H7" s="13" t="s">
         <v>240</v>
@@ -4084,7 +4084,7 @@
         <v>13010006</v>
       </c>
       <c r="G10" s="20" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H10" s="13" t="s">
         <v>242</v>
@@ -4164,7 +4164,7 @@
         <v>13010006</v>
       </c>
       <c r="G11" s="20" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="H11" s="13" t="s">
         <v>243</v>
@@ -4219,7 +4219,7 @@
         <v>338</v>
       </c>
       <c r="AD11" s="19" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.15">
@@ -4242,7 +4242,7 @@
         <v>13010006</v>
       </c>
       <c r="G12" s="20" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="H12" s="13" t="s">
         <v>244</v>
@@ -4431,7 +4431,7 @@
         <v>509</v>
       </c>
       <c r="AD14" s="19" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.15">
@@ -4511,7 +4511,7 @@
         <v>538</v>
       </c>
       <c r="AD15" s="19" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.15">
@@ -4589,7 +4589,7 @@
         <v>655</v>
       </c>
       <c r="AD16" s="19" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="17" spans="1:30" x14ac:dyDescent="0.15">
@@ -4669,7 +4669,7 @@
         <v>584</v>
       </c>
       <c r="AD17" s="19" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="18" spans="1:30" x14ac:dyDescent="0.15">
@@ -4749,7 +4749,7 @@
         <v>444</v>
       </c>
       <c r="AD18" s="19" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.15">
@@ -4829,7 +4829,7 @@
         <v>445</v>
       </c>
       <c r="AD19" s="19" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.15">
@@ -4913,7 +4913,7 @@
         <v>589</v>
       </c>
       <c r="AD20" s="19" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.15">
@@ -4993,7 +4993,7 @@
         <v>545</v>
       </c>
       <c r="AD21" s="19" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.15">
@@ -5073,7 +5073,7 @@
         <v>455</v>
       </c>
       <c r="AD22" s="19" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="23" spans="1:30" x14ac:dyDescent="0.15">
@@ -5215,7 +5215,7 @@
         <v>720</v>
       </c>
       <c r="AD24" s="19" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.15">
@@ -5293,7 +5293,7 @@
         <v>594</v>
       </c>
       <c r="AD25" s="19" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.15">
@@ -5373,7 +5373,7 @@
         <v>720</v>
       </c>
       <c r="AD26" s="19" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.15">
@@ -5453,7 +5453,7 @@
         <v>630</v>
       </c>
       <c r="AD27" s="19" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.15">
@@ -5529,7 +5529,7 @@
         <v>655</v>
       </c>
       <c r="AD28" s="19" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.15">
@@ -5599,7 +5599,7 @@
         <v>735</v>
       </c>
       <c r="AD29" s="19" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.15">
@@ -5675,7 +5675,7 @@
         <v>785</v>
       </c>
       <c r="AD30" s="19" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.15">
@@ -5755,7 +5755,7 @@
         <v>679</v>
       </c>
       <c r="AD31" s="19" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="32" spans="1:30" x14ac:dyDescent="0.15">
@@ -5829,7 +5829,7 @@
         <v>734</v>
       </c>
       <c r="AD32" s="19" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="33" spans="1:30" x14ac:dyDescent="0.15">
@@ -5930,7 +5930,7 @@
         <v>13010006</v>
       </c>
       <c r="G34" s="20" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="H34" s="13" t="s">
         <v>256</v>
@@ -6408,7 +6408,7 @@
         <v>13010004</v>
       </c>
       <c r="G41" s="20" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="H41" s="13" t="s">
         <v>259</v>
@@ -6476,7 +6476,7 @@
         <v>13010004</v>
       </c>
       <c r="G42" s="20" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="H42" s="13" t="s">
         <v>259</v>
@@ -6544,7 +6544,7 @@
         <v>13010004</v>
       </c>
       <c r="G43" s="20" t="s">
-        <v>260</v>
+        <v>279</v>
       </c>
       <c r="H43" s="13"/>
       <c r="I43" s="13"/>
@@ -6881,17 +6881,17 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="I4:U48">
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:H48">
-    <cfRule type="containsBlanks" dxfId="0" priority="5">
+    <cfRule type="containsBlanks" dxfId="33" priority="5">
       <formula>LEN(TRIM(G4))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>